<commit_message>
Appointments Module Update: Scenarios Updated: 1. All Type of Appointments (Visit,Video,Face2Face Phone, Card). 2. Cancel Appointment. 3. Past and Future Appointments verification. 4. Verify video invites.
By,
Patrick
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\INLOGIC\Framework_Inlogic\Demo-Inlogic_MMH\config\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Patrick-Codoid\INLOGIC_MMH_FRAMEWORK\New_Repo_Push\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="MMH" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t>KEY</t>
   </si>
@@ -142,12 +142,24 @@
   </si>
   <si>
     <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Video;9:00 AM;Book Face to Face;Dr Sam Entwistle</t>
+  </si>
+  <si>
+    <t>Cancelled;Dr Sam Entwistle;</t>
+  </si>
+  <si>
+    <t>APPOINTMENT_DETAILS_AFTER_CANCELLED</t>
+  </si>
+  <si>
+    <t>VIDEO_ICONS</t>
+  </si>
+  <si>
+    <t>Minimize;Close;Settings;Mute;Share Now;Video Off</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -494,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="B19" activeCellId="1" sqref="B27 B19"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -739,6 +751,28 @@
         <v>38</v>
       </c>
     </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>

<commit_message>
Appointments Module Update: Scenarios Updated: 1. Appointments Script Updated.
By,
Patrick
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>KEY</t>
   </si>
@@ -87,27 +87,9 @@
     <t>(NZD);4111111111111111;test;121</t>
   </si>
   <si>
-    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Video;9:00 AM;Book Video Appointment</t>
-  </si>
-  <si>
-    <t>Video;VM03Location</t>
-  </si>
-  <si>
-    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Video;9:00 AM;Book Face to Face</t>
-  </si>
-  <si>
-    <t>Visit;VM03Location;</t>
-  </si>
-  <si>
-    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Visit;9:00 AM;Dr Sam Entwistle</t>
-  </si>
-  <si>
     <t>Visit;VM03Location;Dr Sam Entwistle</t>
   </si>
   <si>
-    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Phone;9:00 AM;Dr Sam Entwistle;022;784512369</t>
-  </si>
-  <si>
     <t>Phone;VM03Location;Dr Sam Entwistle</t>
   </si>
   <si>
@@ -126,24 +108,12 @@
     <t>PHONE_APPOINTMENT_SUMMARY</t>
   </si>
   <si>
-    <t>Pending;Dr Sam Entwistle</t>
-  </si>
-  <si>
-    <t>Pending;Dr Sam Entwistle;</t>
-  </si>
-  <si>
     <t>APPOINTMENT_DETAILS_FOR_CANCEL</t>
   </si>
   <si>
     <t>Approved;Dr Sam Entwistle;</t>
   </si>
   <si>
-    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Video;9:00 AM;Book Video Appointment;Dr Sam Entwistle</t>
-  </si>
-  <si>
-    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Video;9:00 AM;Book Face to Face;Dr Sam Entwistle</t>
-  </si>
-  <si>
     <t>Cancelled;Dr Sam Entwistle;</t>
   </si>
   <si>
@@ -154,6 +124,45 @@
   </si>
   <si>
     <t>Minimize;Close;Settings;Mute;Share Now;Video Off</t>
+  </si>
+  <si>
+    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Visit;9:00 AM;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>Visit;VM03Location;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>Pending;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Video;9:00 AM;Book Video Appointment;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>Video;VM03Location;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Video;9:00 AM;Book Face to Face;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Phone;9:00 AM;Dr Sam Entwistle;022;784512369;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>Phone;VM03Location;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>Approved;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>Cancelled;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>FUTURE_DATE</t>
+  </si>
+  <si>
+    <t>AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>Video;VM03Location;Dr Sam Entwistle</t>
   </si>
 </sst>
 </file>
@@ -506,16 +515,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B19" activeCellId="1" sqref="B29 B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="69.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="141.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="157.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="125.140625" style="2" customWidth="1"/>
     <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
@@ -569,10 +578,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -580,197 +589,237 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>22</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>12</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>35</v>
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>26</v>
+        <v>15</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>21</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>41</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C31" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>44</v>
+      <c r="C32" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RRP Module Code Push
1. Total Nine Scenarios

By,
Patrick
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Patrick-Codoid\INLOGIC_MMH_FRAMEWORK\New_Repo_Push\config\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder (2)\Appointments_Updated\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="MMH" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
   <si>
     <t>KEY</t>
   </si>
@@ -163,18 +163,136 @@
   </si>
   <si>
     <t>Video;VM03Location;Dr Sam Entwistle</t>
+  </si>
+  <si>
+    <t>DATA FOR PATIENT TO COLLECT TO PRESCRIPTION</t>
+  </si>
+  <si>
+    <t>VM04Practice; Dr Tim ; Patient to Collect Script ; Next Day - Fee:;Panadol (Optizorb) 500mg Caplets;Repeat Medication Testing for PATIENT TO COLLECT</t>
+  </si>
+  <si>
+    <t>VERIFICATION DATA FOR PATIENT TO COLLECT PRESCRIPTION</t>
+  </si>
+  <si>
+    <t>VM04Practice;panadol (optizorb) 500mg caplets(paracetamol);pending;Next Day - Fee: NZ$12.00 (Incl. GST);Dr Tim</t>
+  </si>
+  <si>
+    <t>MORE INFO VERIFICATION DATA FOR PATIENT TO COLLECT PRESCRIPTION</t>
+  </si>
+  <si>
+    <t>Dr Tim ( VM04Practice );VM04Practice;Patient to Collect Script;Next Day - Fee: NZ$12.00 (Incl. GST);panadol (optizorb) 500mg caplets(paracetamol);Pending</t>
+  </si>
+  <si>
+    <t>DATA FOR SENT SCRIPT BY POST</t>
+  </si>
+  <si>
+    <t>VM04Location2;Tom Denver;Send Script by Post;Urgent/Same day - Fee:;Panadol (Optizorb) 500mg Caplets;Repeat Medication Testing for SENT SCRIPT BY POST</t>
+  </si>
+  <si>
+    <t>VERIFICATION DATA FOR SENT SCRIPT BY POST</t>
+  </si>
+  <si>
+    <t>VM04Practice;panadol (optizorb) 500mg caplets(paracetamol);pending;Urgent/Same day - Fee: NZ$45.00 (Incl. GST);TOM DENVER</t>
+  </si>
+  <si>
+    <t>MORE INFO VERIFICATION DATA FOR SENT SCRIPT BY POST</t>
+  </si>
+  <si>
+    <t>DATA FOR PRESCRIPTION BY SENT SCRIPT TO PHARMACY</t>
+  </si>
+  <si>
+    <t>VM04Practice;Kevin Peterson;Send Script to Pharmacy;Select from my saved list;Chemist Warehouse Auckland;48 Hours - Fee: NZ$;Panadol (Optizorb) 500mg Caplets;Repeat Medication Testing for Sent Script by Pharmacy;Chemist Warehouse Auckland</t>
+  </si>
+  <si>
+    <t>VERIFICATION DATA FOR SENT SCRIPT TO PHARMACY</t>
+  </si>
+  <si>
+    <t>VM04Practice;panadol (optizorb) 500mg caplets(paracetamol);pending;Chemist Warehouse Auckland - Lower Queen St;48 Hours - Fee: NZ$21.00 (Incl. GST);Kevin Peterson</t>
+  </si>
+  <si>
+    <t>MORE INFO DATA FOR PRESCRIPTION BY SENT SCRIPT TO PHARMACY</t>
+  </si>
+  <si>
+    <t>DATA FOR DELIVERY MEDS BY PHARMACY</t>
+  </si>
+  <si>
+    <t>VM04Practice;Kevin Peterson;Deliver Meds by Pharmacy;Select from my saved list;ZOOM Pharmacy home delivery;2: 456, demo;48 Hours - Fee: NZ$;Panadol (Optizorb) 500mg Caplets;Repeat Medication Testing for Delivery Meds by Pharmacy;ZOOM Pharmacy home delivery</t>
+  </si>
+  <si>
+    <t>VERIFICATION DATA FOR DELIVERY MEDS BY PHARMACY</t>
+  </si>
+  <si>
+    <t>VM04Practice;panadol (optizorb) 500mg caplets(paracetamol);pending;ZOOM Pharmacy home delivery;48 Hours - Fee: NZ$25.00 (Incl. GST);Kevin Peterson</t>
+  </si>
+  <si>
+    <t>MORE INFO DATA FOR DELIVERY MEDS BY PHARMACY</t>
+  </si>
+  <si>
+    <t>DATA MEDS PAY BY USING ONLINE CARD</t>
+  </si>
+  <si>
+    <t>VERIFICATION MEDS PAY BY USING ONLINE CARD</t>
+  </si>
+  <si>
+    <t>DATA MEDS PAY BY USING ONLINE A2A</t>
+  </si>
+  <si>
+    <t>VERIFICATION DATA FOR MEDS PAY BY USING A2A</t>
+  </si>
+  <si>
+    <t>CREDIT CARD DETAILS</t>
+  </si>
+  <si>
+    <t>CreditCard;4111111111111111;test;02;24;121</t>
+  </si>
+  <si>
+    <t>ACCOUNT TO ACCOUNT</t>
+  </si>
+  <si>
+    <t>Account2Account;AnzNZ;WindcaveA2ATest;Windcave1234;Payment Success</t>
+  </si>
+  <si>
+    <t>MEDICATION DETAILS FOR URGENCY</t>
+  </si>
+  <si>
+    <t>VM04Practice; Dr Tim ; Patient to Collect Script ;</t>
+  </si>
+  <si>
+    <t>URGENCY PRICE</t>
+  </si>
+  <si>
+    <t>Urgent/Same day - Fee: NZ$11.00 (Incl. GST);Next Day - Fee: NZ$12.00 (Incl. GST);48 Hours - Fee: NZ$13.00 (Incl. GST);72 Hours - Fee: NZ$14.00 (Incl. GST)</t>
+  </si>
+  <si>
+    <t>chrisc@mmh-demo.com</t>
+  </si>
+  <si>
+    <t>EMAIL FOR RRP</t>
+  </si>
+  <si>
+    <t>PASSWORD FOR RRP</t>
+  </si>
+  <si>
+    <t>https://beta.mmh-demo.com/home</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -196,16 +314,23 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
       <sz val="10"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -217,7 +342,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -225,19 +350,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="2"/>
@@ -515,311 +669,607 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="B19" activeCellId="1" sqref="B29 B19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="69.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="157.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="125.140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="69.54296875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="157.1796875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="125.1796875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14" thickBot="1">
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="1:3" ht="14" thickBot="1">
+      <c r="A38" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14" thickBot="1">
+      <c r="A39" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14" thickBot="1">
+      <c r="C40" s="7"/>
+    </row>
+    <row r="41" spans="1:3" ht="27.5" thickBot="1">
+      <c r="A41" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14" thickBot="1">
+      <c r="A42" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="27.5" thickBot="1">
+      <c r="A43" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14" thickBot="1">
+      <c r="A44" s="8"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="1:3" ht="14" thickBot="1">
+      <c r="A45" s="8"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:3" ht="27.5" thickBot="1">
+      <c r="A46" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="27.5" thickBot="1">
+      <c r="A47" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14" thickBot="1">
+      <c r="A48" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" ht="14" thickBot="1">
+      <c r="A49" s="8"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:3" ht="14" thickBot="1">
+      <c r="A50" s="8"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+    </row>
+    <row r="51" spans="1:3" ht="27.5" thickBot="1">
+      <c r="A51" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="27.5" thickBot="1">
+      <c r="A52" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15" thickBot="1">
+      <c r="A53" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+    </row>
+    <row r="54" spans="1:3" ht="14" thickBot="1">
+      <c r="A54" s="8"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+    </row>
+    <row r="55" spans="1:3" ht="14" thickBot="1">
+      <c r="A55" s="8"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:3" ht="41" thickBot="1">
+      <c r="A56" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="27.5" thickBot="1">
+      <c r="A57" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="14" thickBot="1">
+      <c r="A58" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+    </row>
+    <row r="59" spans="1:3" ht="14" thickBot="1">
+      <c r="A59" s="8"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+    </row>
+    <row r="60" spans="1:3" ht="14" thickBot="1">
+      <c r="A60" s="8"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+    </row>
+    <row r="61" spans="1:3" ht="41" thickBot="1">
+      <c r="A61" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="27.5" thickBot="1">
+      <c r="A62" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="14" thickBot="1">
+      <c r="A63" s="8"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+    </row>
+    <row r="64" spans="1:3" ht="14" thickBot="1">
+      <c r="A64" s="8"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+    </row>
+    <row r="65" spans="1:3" ht="41" thickBot="1">
+      <c r="A65" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="27.5" thickBot="1">
+      <c r="A66" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="14" thickBot="1">
+      <c r="A67" s="8"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+    </row>
+    <row r="68" spans="1:3" ht="14" thickBot="1">
+      <c r="A68" s="8"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+    </row>
+    <row r="69" spans="1:3" ht="14" thickBot="1">
+      <c r="A69" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="14" thickBot="1">
+      <c r="A70" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="14" thickBot="1">
+      <c r="A71" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="27.5" thickBot="1">
+      <c r="A72" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -830,8 +1280,12 @@
     <hyperlink ref="B2" r:id="rId4"/>
     <hyperlink ref="B3" r:id="rId5"/>
     <hyperlink ref="C3" r:id="rId6"/>
+    <hyperlink ref="B38" r:id="rId7" display="mailto:chrisc@mmh-demo.com"/>
+    <hyperlink ref="B39" r:id="rId8" display="mailto:Manage@123"/>
+    <hyperlink ref="C38" r:id="rId9" display="mailto:chrisc@mmh-demo.com"/>
+    <hyperlink ref="C39" r:id="rId10" display="mailto:Manage@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
27/06/22 Health Records Model Latest Update
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Patrick-Codoid\Naveen\Appointments_Updated\config\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
-  </bookViews>
   <sheets>
-    <sheet name="MMH" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="MMH" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="246">
   <si>
     <t>KEY</t>
   </si>
@@ -507,106 +499,142 @@
     <t>DATA_MY_ENTRIES_CLINIC_NOTES_1</t>
   </si>
   <si>
+    <t>25 Jun 2022;TestVisited;TestLocation</t>
+  </si>
+  <si>
     <t>18 May 2022;doctor;chennai</t>
   </si>
   <si>
     <t>DATA_MY_ENTRIES_INSIDE_CLINIC_NOTES_1</t>
   </si>
   <si>
+    <t>TestVisited;25 Jun 2022;TestLocation;Show this entry to my doctor;TestAdditional</t>
+  </si>
+  <si>
     <t>doctor;18 May 2022;chennai;Do not show this entry to my doctor;note testing</t>
   </si>
   <si>
     <t>DATA_MY_ENTRIES_PRESCRIPTIONS</t>
   </si>
   <si>
+    <t>25 Jun 2022;test;test</t>
+  </si>
+  <si>
     <t>26 May 2022;prescriptions test;tester</t>
   </si>
   <si>
     <t>DATA_MY_ENTRIES_INSIDE_PRESCRIPTIONS</t>
   </si>
   <si>
+    <t>test;testdose;25 Jun 2022;2;2 times per day;25 Jun 2022;25 Jun 2022;I took this in the past;Show this entry to my doctor;test</t>
+  </si>
+  <si>
     <t>prescriptions test;26 May 2022;2;2 times per day;26 May 2022;27 May 2022;I took this in the past;Show this entry to my doctor;tester</t>
   </si>
   <si>
     <t>DATA_MY_ENTRIES_ALLERGIES</t>
   </si>
   <si>
+    <t>23 Jun 2022;TestAllergy;High</t>
+  </si>
+  <si>
     <t>14 Jun 2022;Test01-KXVMJUHV;High</t>
   </si>
   <si>
     <t>DATA_MY_ENTRIES_INSIDE_ALLERGIES</t>
   </si>
   <si>
+    <t>TestAllergy;23 Jun 2022;Had this allergy in the past;Show this entry to my doctor;TestAdditional</t>
+  </si>
+  <si>
     <t>Test01-KXVMJUHV;14 Jun 2022;Had this allergy in the past;Show this entry to my doctor;Test02-Additional Information</t>
   </si>
   <si>
     <t>DATA_MY_ENTRIES_IMMUNISATIONS</t>
   </si>
   <si>
+    <t>25 Jun 2022;TestImmunisation</t>
+  </si>
+  <si>
     <t>27 May 2022;Cls Android</t>
   </si>
   <si>
-    <t>DATA_MY_ENTRIES_IMMUNISATIONS_1</t>
-  </si>
-  <si>
     <t>26 May 2022;Testt</t>
   </si>
   <si>
     <t>DATA_MY_ENTRIES_INSIDE_IMMUNISATIONS</t>
   </si>
   <si>
+    <t>TestImmunisation;25 Jun 2022;Show this entry to my doctor;TestAdditional</t>
+  </si>
+  <si>
     <t>Cls Android;27 May 2022;Show this entry to my doctor;Cls Android</t>
   </si>
   <si>
-    <t>DATA_MY_ENTRIES_INSIDE_IMMUNISATIONS_1</t>
-  </si>
-  <si>
     <t>Testt;26 May 2022;Show this entry to my doctor;Yes</t>
   </si>
   <si>
     <t>DATA_MY_ENTRIES_CLASSIFICATIONS</t>
   </si>
   <si>
+    <t>23 Jun 2022;TestCondition</t>
+  </si>
+  <si>
     <t>19 May 2022;ttee</t>
   </si>
   <si>
     <t>DATA_MY_ENTRIES_INSIDE_CLASSIFICATIONS</t>
   </si>
   <si>
+    <t>TestCondition;23/06/2022;25 Jun 2022;25 Jun 2022;Historic;Show this entry to my doctor;TestAdditional</t>
+  </si>
+  <si>
     <t xml:space="preserve">ttee;19/05/2022;20 May 2022;21 May 2022;Current;Show this entry to my doctor </t>
   </si>
   <si>
-    <t>RECALLS_REMAINDER_TABLEDATA</t>
+    <t>RECALLS_REMAINDER_TABLE_DATA</t>
+  </si>
+  <si>
+    <t>09 Nov 2021;Cervical Smear;CX;17 Dec 2021</t>
   </si>
   <si>
     <t>14 Jun 2022;Body Mass Index;BMI;07 Jun 2022</t>
   </si>
   <si>
-    <t>RECALLS_REMAINDER_ICONDATA</t>
+    <t>RECALLS_REMAINDER_ICON_DATA</t>
+  </si>
+  <si>
+    <t>17 Dec 2021;Daisy Daisy;VM03Location;Dr Tim</t>
   </si>
   <si>
     <t>Test doc :31/12/2021</t>
   </si>
   <si>
-    <t>RECALLS_TABLEDATA_1</t>
+    <t>RECALLS_TABLE_DATA_1</t>
+  </si>
+  <si>
+    <t>09 Nov 2021;Cervical Smear;MMH Email;VM03Location</t>
   </si>
   <si>
     <t>14 Jun 2022;Body Mass Index;MMH Email;VM03Location</t>
   </si>
   <si>
-    <t>RECALLS_ICONDATA_1</t>
+    <t>RECALLS_ICON_DATA_1</t>
+  </si>
+  <si>
+    <t>09/11/2021 06:53:01 PM;Cervical Smear;Auto Recall;17/12/2021 12:00:00 AM;MMH Email;Dr Tim;VM03Location</t>
   </si>
   <si>
     <t>14/06/2022 08:37:45 PM;Body Mass Index;note1;07/06/2022 12:00:00 AM;MMH Email;Dr Sam Entwistle;VM03Location</t>
   </si>
   <si>
-    <t>TESTRESULT_ICONDATA</t>
+    <t>TEST_RESULT_ICON_DATA</t>
   </si>
   <si>
     <t>Test, Patient;26-Jun-1995;A Mouse;01-Jun-2018</t>
   </si>
   <si>
-    <t>TESTRESULT_ICONDATA_1</t>
+    <t>TEST_RESULT_ICON_DATA_1</t>
   </si>
   <si>
     <t>TEST, Patient;26-Jun-1995;Donald Duck;24-Feb-2011</t>
@@ -684,12 +712,18 @@
     <t>DATA_MY_ENTRIES_COVID_IMMUNISATIONS</t>
   </si>
   <si>
+    <t>23 Jun 2022;Comirnaty, COVID-19 mRNA (Pfizer-BioNTech)</t>
+  </si>
+  <si>
     <t>19 May 2022;Comirnaty, COVID-19 mRNA (Pfizer-BioNTech);</t>
   </si>
   <si>
     <t>DATA_MY_ENTRIES_INSIDE_COVID_IMMUNISATIONS</t>
   </si>
   <si>
+    <t>Comirnaty, COVID-19 mRNA (Pfizer-BioNTech);COVID19 Comirnaty - 2;Test123;23 Jun 2022;Show this entry to my doctor;TestClinical</t>
+  </si>
+  <si>
     <t>Comirnaty, COVID-19 mRNA (Pfizer-BioNTech);COVID19 Comirnaty - 1;123456ghffb;19 May 2022;Show this entry to my doctor;TestEdit</t>
   </si>
   <si>
@@ -709,72 +743,86 @@
   </si>
   <si>
     <t>MMHtest.jpg</t>
+  </si>
+  <si>
+    <t>EMAIL_MMH</t>
+  </si>
+  <si>
+    <t>daisy@mmh-demo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="13">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Verdana"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Verdana"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -782,7 +830,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -791,14 +839,8 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="4">
+    <border/>
     <border>
       <left style="medium">
         <color rgb="FFCCCCCC"/>
@@ -812,7 +854,20 @@
       <bottom style="medium">
         <color rgb="FFCCCCCC"/>
       </bottom>
-      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -827,64 +882,85 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+  <cellXfs count="23">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="3" fillId="2" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1074,28 +1150,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="69.5703125" customWidth="1"/>
-    <col min="2" max="2" width="157.140625" customWidth="1"/>
-    <col min="3" max="3" width="125.140625" customWidth="1"/>
-    <col min="4" max="23" width="8.85546875" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="69.57"/>
+    <col customWidth="1" min="2" max="2" width="157.14"/>
+    <col customWidth="1" min="3" max="3" width="125.14"/>
+    <col customWidth="1" min="4" max="23" width="8.86"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="13.5" customHeight="1">
+    <row r="1" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1200,7 @@
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
     </row>
-    <row r="2" spans="1:23" ht="13.5" customHeight="1">
+    <row r="2" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1157,7 +1231,7 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
     </row>
-    <row r="3" spans="1:23" ht="13.5" customHeight="1">
+    <row r="3" ht="13.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1188,7 +1262,7 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="1:23" ht="13.5" customHeight="1">
+    <row r="4" ht="13.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1219,7 +1293,7 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
     </row>
-    <row r="5" spans="1:23" ht="13.5" customHeight="1">
+    <row r="5" ht="13.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1250,7 +1324,7 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
     </row>
-    <row r="6" spans="1:23" ht="13.5" customHeight="1">
+    <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1281,7 +1355,7 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
     </row>
-    <row r="7" spans="1:23" ht="13.5" customHeight="1">
+    <row r="7" ht="13.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1312,7 +1386,7 @@
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
     </row>
-    <row r="8" spans="1:23" ht="13.5" customHeight="1">
+    <row r="8" ht="13.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1341,7 +1415,7 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
     </row>
-    <row r="9" spans="1:23" ht="13.5" customHeight="1">
+    <row r="9" ht="13.5" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1366,7 +1440,7 @@
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:23" ht="13.5" customHeight="1">
+    <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1397,7 +1471,7 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:23" ht="13.5" customHeight="1">
+    <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1428,7 +1502,7 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:23" ht="13.5" customHeight="1">
+    <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1459,7 +1533,7 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:23" ht="13.5" customHeight="1">
+    <row r="13" ht="13.5" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1488,7 +1562,7 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:23" ht="13.5" customHeight="1">
+    <row r="14" ht="13.5" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1513,7 +1587,7 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:23" ht="13.5" customHeight="1">
+    <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1544,7 +1618,7 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:23" ht="13.5" customHeight="1">
+    <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -1575,7 +1649,7 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:23" ht="13.5" customHeight="1">
+    <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1606,7 +1680,7 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
     </row>
-    <row r="18" spans="1:23" ht="13.5" customHeight="1">
+    <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1635,7 +1709,7 @@
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
     </row>
-    <row r="19" spans="1:23" ht="13.5" customHeight="1">
+    <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1660,7 +1734,7 @@
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
     </row>
-    <row r="20" spans="1:23" ht="13.5" customHeight="1">
+    <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1691,7 +1765,7 @@
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
     </row>
-    <row r="21" spans="1:23" ht="13.5" customHeight="1">
+    <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -1722,7 +1796,7 @@
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
     </row>
-    <row r="22" spans="1:23" ht="13.5" customHeight="1">
+    <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1753,7 +1827,7 @@
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
     </row>
-    <row r="23" spans="1:23" ht="13.5" customHeight="1">
+    <row r="23" ht="13.5" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1782,7 +1856,7 @@
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
     </row>
-    <row r="24" spans="1:23" ht="13.5" customHeight="1">
+    <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1807,7 +1881,7 @@
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
     </row>
-    <row r="25" spans="1:23" ht="13.5" customHeight="1">
+    <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1838,7 +1912,7 @@
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
     </row>
-    <row r="26" spans="1:23" ht="13.5" customHeight="1">
+    <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1869,7 +1943,7 @@
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
     </row>
-    <row r="27" spans="1:23" ht="13.5" customHeight="1">
+    <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -1900,7 +1974,7 @@
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
     </row>
-    <row r="28" spans="1:23" ht="13.5" customHeight="1">
+    <row r="28" ht="13.5" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
@@ -1931,7 +2005,7 @@
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
     </row>
-    <row r="29" spans="1:23" ht="13.5" customHeight="1">
+    <row r="29" ht="13.5" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
@@ -1960,7 +2034,7 @@
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
     </row>
-    <row r="30" spans="1:23" ht="13.5" customHeight="1">
+    <row r="30" ht="13.5" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1985,7 +2059,7 @@
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
     </row>
-    <row r="31" spans="1:23" ht="13.5" customHeight="1">
+    <row r="31" ht="13.5" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -2016,7 +2090,7 @@
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
     </row>
-    <row r="32" spans="1:23" ht="13.5" customHeight="1">
+    <row r="32" ht="13.5" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2047,7 +2121,7 @@
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
     </row>
-    <row r="33" spans="1:23" ht="13.5" customHeight="1">
+    <row r="33" ht="13.5" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2072,7 +2146,7 @@
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
     </row>
-    <row r="34" spans="1:23" ht="13.5" customHeight="1">
+    <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
@@ -2103,7 +2177,7 @@
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
     </row>
-    <row r="35" spans="1:23" ht="13.5" customHeight="1">
+    <row r="35" ht="13.5" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2128,7 +2202,7 @@
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
     </row>
-    <row r="36" spans="1:23" ht="13.5" customHeight="1">
+    <row r="36" ht="13.5" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2153,7 +2227,7 @@
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
     </row>
-    <row r="37" spans="1:23" ht="13.5" customHeight="1">
+    <row r="37" ht="13.5" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2178,7 +2252,7 @@
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
     </row>
-    <row r="38" spans="1:23" ht="13.5" customHeight="1">
+    <row r="38" ht="13.5" customHeight="1">
       <c r="A38" s="5" t="s">
         <v>49</v>
       </c>
@@ -2209,7 +2283,7 @@
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
     </row>
-    <row r="39" spans="1:23" ht="13.5" customHeight="1">
+    <row r="39" ht="13.5" customHeight="1">
       <c r="A39" s="5" t="s">
         <v>51</v>
       </c>
@@ -2240,7 +2314,7 @@
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
     </row>
-    <row r="40" spans="1:23" ht="13.5" customHeight="1">
+    <row r="40" ht="13.5" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2265,7 +2339,7 @@
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
     </row>
-    <row r="41" spans="1:23" ht="13.5" customHeight="1">
+    <row r="41" ht="13.5" customHeight="1">
       <c r="A41" s="8" t="s">
         <v>52</v>
       </c>
@@ -2296,7 +2370,7 @@
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
     </row>
-    <row r="42" spans="1:23" ht="13.5" customHeight="1">
+    <row r="42" ht="13.5" customHeight="1">
       <c r="A42" s="8" t="s">
         <v>54</v>
       </c>
@@ -2327,7 +2401,7 @@
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
     </row>
-    <row r="43" spans="1:23" ht="13.5" customHeight="1">
+    <row r="43" ht="13.5" customHeight="1">
       <c r="A43" s="8" t="s">
         <v>56</v>
       </c>
@@ -2358,7 +2432,7 @@
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
     </row>
-    <row r="44" spans="1:23" ht="13.5" customHeight="1">
+    <row r="44" ht="13.5" customHeight="1">
       <c r="A44" s="8"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -2383,7 +2457,7 @@
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
     </row>
-    <row r="45" spans="1:23" ht="13.5" customHeight="1">
+    <row r="45" ht="13.5" customHeight="1">
       <c r="A45" s="8"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -2408,7 +2482,7 @@
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
     </row>
-    <row r="46" spans="1:23" ht="13.5" customHeight="1">
+    <row r="46" ht="13.5" customHeight="1">
       <c r="A46" s="8" t="s">
         <v>58</v>
       </c>
@@ -2439,7 +2513,7 @@
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
     </row>
-    <row r="47" spans="1:23" ht="13.5" customHeight="1">
+    <row r="47" ht="13.5" customHeight="1">
       <c r="A47" s="8" t="s">
         <v>60</v>
       </c>
@@ -2470,7 +2544,7 @@
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
     </row>
-    <row r="48" spans="1:23" ht="13.5" customHeight="1">
+    <row r="48" ht="13.5" customHeight="1">
       <c r="A48" s="8" t="s">
         <v>62</v>
       </c>
@@ -2497,7 +2571,7 @@
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
     </row>
-    <row r="49" spans="1:23" ht="13.5" customHeight="1">
+    <row r="49" ht="13.5" customHeight="1">
       <c r="A49" s="8"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -2522,7 +2596,7 @@
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
     </row>
-    <row r="50" spans="1:23" ht="13.5" customHeight="1">
+    <row r="50" ht="13.5" customHeight="1">
       <c r="A50" s="8"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -2547,7 +2621,7 @@
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
     </row>
-    <row r="51" spans="1:23" ht="13.5" customHeight="1">
+    <row r="51" ht="13.5" customHeight="1">
       <c r="A51" s="8" t="s">
         <v>63</v>
       </c>
@@ -2578,7 +2652,7 @@
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
     </row>
-    <row r="52" spans="1:23" ht="13.5" customHeight="1">
+    <row r="52" ht="13.5" customHeight="1">
       <c r="A52" s="8" t="s">
         <v>65</v>
       </c>
@@ -2609,7 +2683,7 @@
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
     </row>
-    <row r="53" spans="1:23" ht="13.5" customHeight="1">
+    <row r="53" ht="13.5" customHeight="1">
       <c r="A53" s="8" t="s">
         <v>67</v>
       </c>
@@ -2636,7 +2710,7 @@
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
     </row>
-    <row r="54" spans="1:23" ht="13.5" customHeight="1">
+    <row r="54" ht="13.5" customHeight="1">
       <c r="A54" s="8"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -2661,7 +2735,7 @@
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
     </row>
-    <row r="55" spans="1:23" ht="13.5" customHeight="1">
+    <row r="55" ht="13.5" customHeight="1">
       <c r="A55" s="8"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2686,7 +2760,7 @@
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
     </row>
-    <row r="56" spans="1:23" ht="13.5" customHeight="1">
+    <row r="56" ht="13.5" customHeight="1">
       <c r="A56" s="8" t="s">
         <v>68</v>
       </c>
@@ -2717,7 +2791,7 @@
       <c r="V56" s="1"/>
       <c r="W56" s="1"/>
     </row>
-    <row r="57" spans="1:23" ht="13.5" customHeight="1">
+    <row r="57" ht="13.5" customHeight="1">
       <c r="A57" s="8" t="s">
         <v>70</v>
       </c>
@@ -2748,7 +2822,7 @@
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
     </row>
-    <row r="58" spans="1:23" ht="13.5" customHeight="1">
+    <row r="58" ht="13.5" customHeight="1">
       <c r="A58" s="8" t="s">
         <v>72</v>
       </c>
@@ -2775,7 +2849,7 @@
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
     </row>
-    <row r="59" spans="1:23" ht="13.5" customHeight="1">
+    <row r="59" ht="13.5" customHeight="1">
       <c r="A59" s="8"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -2800,7 +2874,7 @@
       <c r="V59" s="1"/>
       <c r="W59" s="1"/>
     </row>
-    <row r="60" spans="1:23" ht="13.5" customHeight="1">
+    <row r="60" ht="13.5" customHeight="1">
       <c r="A60" s="8"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -2825,7 +2899,7 @@
       <c r="V60" s="1"/>
       <c r="W60" s="1"/>
     </row>
-    <row r="61" spans="1:23" ht="13.5" customHeight="1">
+    <row r="61" ht="13.5" customHeight="1">
       <c r="A61" s="8" t="s">
         <v>73</v>
       </c>
@@ -2856,7 +2930,7 @@
       <c r="V61" s="1"/>
       <c r="W61" s="1"/>
     </row>
-    <row r="62" spans="1:23" ht="13.5" customHeight="1">
+    <row r="62" ht="13.5" customHeight="1">
       <c r="A62" s="8" t="s">
         <v>74</v>
       </c>
@@ -2887,7 +2961,7 @@
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
     </row>
-    <row r="63" spans="1:23" ht="13.5" customHeight="1">
+    <row r="63" ht="13.5" customHeight="1">
       <c r="A63" s="8"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -2912,7 +2986,7 @@
       <c r="V63" s="1"/>
       <c r="W63" s="1"/>
     </row>
-    <row r="64" spans="1:23" ht="13.5" customHeight="1">
+    <row r="64" ht="13.5" customHeight="1">
       <c r="A64" s="8"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -2937,7 +3011,7 @@
       <c r="V64" s="1"/>
       <c r="W64" s="1"/>
     </row>
-    <row r="65" spans="1:23" ht="13.5" customHeight="1">
+    <row r="65" ht="13.5" customHeight="1">
       <c r="A65" s="8" t="s">
         <v>75</v>
       </c>
@@ -2968,7 +3042,7 @@
       <c r="V65" s="1"/>
       <c r="W65" s="1"/>
     </row>
-    <row r="66" spans="1:23" ht="13.5" customHeight="1">
+    <row r="66" ht="13.5" customHeight="1">
       <c r="A66" s="8" t="s">
         <v>76</v>
       </c>
@@ -2999,7 +3073,7 @@
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
     </row>
-    <row r="67" spans="1:23" ht="13.5" customHeight="1">
+    <row r="67" ht="13.5" customHeight="1">
       <c r="A67" s="8"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -3024,7 +3098,7 @@
       <c r="V67" s="1"/>
       <c r="W67" s="1"/>
     </row>
-    <row r="68" spans="1:23" ht="13.5" customHeight="1">
+    <row r="68" ht="13.5" customHeight="1">
       <c r="A68" s="8"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -3049,7 +3123,7 @@
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
     </row>
-    <row r="69" spans="1:23" ht="13.5" customHeight="1">
+    <row r="69" ht="13.5" customHeight="1">
       <c r="A69" s="8" t="s">
         <v>77</v>
       </c>
@@ -3080,7 +3154,7 @@
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
     </row>
-    <row r="70" spans="1:23" ht="13.5" customHeight="1">
+    <row r="70" ht="13.5" customHeight="1">
       <c r="A70" s="8" t="s">
         <v>79</v>
       </c>
@@ -3111,7 +3185,7 @@
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
     </row>
-    <row r="71" spans="1:23" ht="13.5" customHeight="1">
+    <row r="71" ht="13.5" customHeight="1">
       <c r="A71" s="8" t="s">
         <v>81</v>
       </c>
@@ -3142,7 +3216,7 @@
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
     </row>
-    <row r="72" spans="1:23" ht="13.5" customHeight="1">
+    <row r="72" ht="13.5" customHeight="1">
       <c r="A72" s="5" t="s">
         <v>83</v>
       </c>
@@ -3173,7 +3247,7 @@
       <c r="V72" s="1"/>
       <c r="W72" s="1"/>
     </row>
-    <row r="73" spans="1:23" ht="13.5" customHeight="1">
+    <row r="73" ht="13.5" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3198,7 +3272,7 @@
       <c r="V73" s="1"/>
       <c r="W73" s="1"/>
     </row>
-    <row r="74" spans="1:23" ht="13.5" customHeight="1">
+    <row r="74" ht="13.5" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3223,11 +3297,11 @@
       <c r="V74" s="1"/>
       <c r="W74" s="1"/>
     </row>
-    <row r="75" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A75" s="5" t="s">
+    <row r="75" ht="13.5" customHeight="1">
+      <c r="A75" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C75" s="6" t="s">
@@ -3254,11 +3328,11 @@
       <c r="V75" s="1"/>
       <c r="W75" s="1"/>
     </row>
-    <row r="76" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A76" s="5" t="s">
+    <row r="76" ht="13.5" customHeight="1">
+      <c r="A76" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C76" s="7" t="s">
@@ -3285,9 +3359,9 @@
       <c r="V76" s="1"/>
       <c r="W76" s="1"/>
     </row>
-    <row r="77" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
+    <row r="77" ht="13.5" customHeight="1">
+      <c r="A77" s="14"/>
+      <c r="B77" s="15"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -3310,14 +3384,14 @@
       <c r="V77" s="1"/>
       <c r="W77" s="1"/>
     </row>
-    <row r="78" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A78" s="10" t="s">
+    <row r="78" ht="13.5" customHeight="1">
+      <c r="A78" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="17" t="s">
         <v>88</v>
       </c>
       <c r="D78" s="1"/>
@@ -3341,14 +3415,14 @@
       <c r="V78" s="1"/>
       <c r="W78" s="1"/>
     </row>
-    <row r="79" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A79" s="12" t="s">
+    <row r="79" ht="13.5" customHeight="1">
+      <c r="A79" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B79" s="11" t="s">
+      <c r="B79" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C79" s="11" t="s">
+      <c r="C79" s="17" t="s">
         <v>90</v>
       </c>
       <c r="D79" s="1"/>
@@ -3372,14 +3446,14 @@
       <c r="V79" s="1"/>
       <c r="W79" s="1"/>
     </row>
-    <row r="80" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A80" s="12" t="s">
+    <row r="80" ht="13.5" customHeight="1">
+      <c r="A80" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="B80" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="C80" s="11" t="s">
+      <c r="C80" s="17" t="s">
         <v>92</v>
       </c>
       <c r="D80" s="1"/>
@@ -3403,14 +3477,14 @@
       <c r="V80" s="1"/>
       <c r="W80" s="1"/>
     </row>
-    <row r="81" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A81" s="12" t="s">
+    <row r="81" ht="13.5" customHeight="1">
+      <c r="A81" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="B81" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="C81" s="17" t="s">
         <v>94</v>
       </c>
       <c r="D81" s="1"/>
@@ -3434,14 +3508,14 @@
       <c r="V81" s="1"/>
       <c r="W81" s="1"/>
     </row>
-    <row r="82" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A82" s="12" t="s">
+    <row r="82" ht="13.5" customHeight="1">
+      <c r="A82" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B82" s="11" t="s">
+      <c r="B82" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C82" s="11" t="s">
+      <c r="C82" s="17" t="s">
         <v>96</v>
       </c>
       <c r="D82" s="1"/>
@@ -3465,14 +3539,14 @@
       <c r="V82" s="1"/>
       <c r="W82" s="1"/>
     </row>
-    <row r="83" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A83" s="12" t="s">
+    <row r="83" ht="13.5" customHeight="1">
+      <c r="A83" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="B83" s="11" t="s">
+      <c r="B83" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="C83" s="17" t="s">
         <v>98</v>
       </c>
       <c r="D83" s="1"/>
@@ -3496,14 +3570,14 @@
       <c r="V83" s="1"/>
       <c r="W83" s="1"/>
     </row>
-    <row r="84" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A84" s="12" t="s">
+    <row r="84" ht="13.5" customHeight="1">
+      <c r="A84" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B84" s="13" t="s">
+      <c r="B84" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C84" s="13" t="s">
+      <c r="C84" s="18" t="s">
         <v>100</v>
       </c>
       <c r="D84" s="1"/>
@@ -3527,14 +3601,14 @@
       <c r="V84" s="1"/>
       <c r="W84" s="1"/>
     </row>
-    <row r="85" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A85" s="12" t="s">
+    <row r="85" ht="13.5" customHeight="1">
+      <c r="A85" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B85" s="13" t="s">
+      <c r="B85" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C85" s="13" t="s">
+      <c r="C85" s="18" t="s">
         <v>102</v>
       </c>
       <c r="D85" s="1"/>
@@ -3558,14 +3632,14 @@
       <c r="V85" s="1"/>
       <c r="W85" s="1"/>
     </row>
-    <row r="86" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A86" s="12" t="s">
+    <row r="86" ht="13.5" customHeight="1">
+      <c r="A86" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B86" s="13" t="s">
+      <c r="B86" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C86" s="13" t="s">
+      <c r="C86" s="18" t="s">
         <v>104</v>
       </c>
       <c r="D86" s="1"/>
@@ -3589,14 +3663,14 @@
       <c r="V86" s="1"/>
       <c r="W86" s="1"/>
     </row>
-    <row r="87" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A87" s="12" t="s">
+    <row r="87" ht="13.5" customHeight="1">
+      <c r="A87" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B87" s="13" t="s">
+      <c r="B87" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C87" s="13" t="s">
+      <c r="C87" s="18" t="s">
         <v>106</v>
       </c>
       <c r="D87" s="1"/>
@@ -3620,14 +3694,14 @@
       <c r="V87" s="1"/>
       <c r="W87" s="1"/>
     </row>
-    <row r="88" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A88" s="12" t="s">
+    <row r="88" ht="13.5" customHeight="1">
+      <c r="A88" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B88" s="13" t="s">
+      <c r="B88" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C88" s="13" t="s">
+      <c r="C88" s="18" t="s">
         <v>108</v>
       </c>
       <c r="D88" s="1"/>
@@ -3651,14 +3725,14 @@
       <c r="V88" s="1"/>
       <c r="W88" s="1"/>
     </row>
-    <row r="89" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A89" s="12" t="s">
+    <row r="89" ht="13.5" customHeight="1">
+      <c r="A89" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B89" s="11" t="s">
+      <c r="B89" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C89" s="11" t="s">
+      <c r="C89" s="17" t="s">
         <v>110</v>
       </c>
       <c r="D89" s="1"/>
@@ -3682,14 +3756,14 @@
       <c r="V89" s="1"/>
       <c r="W89" s="1"/>
     </row>
-    <row r="90" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A90" s="12" t="s">
+    <row r="90" ht="13.5" customHeight="1">
+      <c r="A90" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B90" s="11" t="s">
+      <c r="B90" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C90" s="11" t="s">
+      <c r="C90" s="17" t="s">
         <v>112</v>
       </c>
       <c r="D90" s="1"/>
@@ -3713,14 +3787,14 @@
       <c r="V90" s="1"/>
       <c r="W90" s="1"/>
     </row>
-    <row r="91" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A91" s="12" t="s">
+    <row r="91" ht="13.5" customHeight="1">
+      <c r="A91" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B91" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="C91" s="11" t="s">
+      <c r="C91" s="17" t="s">
         <v>114</v>
       </c>
       <c r="D91" s="1"/>
@@ -3744,14 +3818,14 @@
       <c r="V91" s="1"/>
       <c r="W91" s="1"/>
     </row>
-    <row r="92" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A92" s="12" t="s">
+    <row r="92" ht="13.5" customHeight="1">
+      <c r="A92" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="B92" s="11" t="s">
+      <c r="B92" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C92" s="11" t="s">
+      <c r="C92" s="17" t="s">
         <v>116</v>
       </c>
       <c r="D92" s="1"/>
@@ -3775,14 +3849,14 @@
       <c r="V92" s="1"/>
       <c r="W92" s="1"/>
     </row>
-    <row r="93" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A93" s="12" t="s">
+    <row r="93" ht="13.5" customHeight="1">
+      <c r="A93" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B93" s="11" t="s">
+      <c r="B93" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C93" s="17" t="s">
         <v>118</v>
       </c>
       <c r="D93" s="1"/>
@@ -3806,14 +3880,14 @@
       <c r="V93" s="1"/>
       <c r="W93" s="1"/>
     </row>
-    <row r="94" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A94" s="12" t="s">
+    <row r="94" ht="13.5" customHeight="1">
+      <c r="A94" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="B94" s="13" t="s">
+      <c r="B94" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C94" s="13" t="s">
+      <c r="C94" s="18" t="s">
         <v>120</v>
       </c>
       <c r="D94" s="1"/>
@@ -3837,14 +3911,14 @@
       <c r="V94" s="1"/>
       <c r="W94" s="1"/>
     </row>
-    <row r="95" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A95" s="12" t="s">
+    <row r="95" ht="13.5" customHeight="1">
+      <c r="A95" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="B95" s="13" t="s">
+      <c r="B95" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C95" s="13" t="s">
+      <c r="C95" s="18" t="s">
         <v>122</v>
       </c>
       <c r="D95" s="1"/>
@@ -3868,14 +3942,14 @@
       <c r="V95" s="1"/>
       <c r="W95" s="1"/>
     </row>
-    <row r="96" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A96" s="12" t="s">
+    <row r="96" ht="13.5" customHeight="1">
+      <c r="A96" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B96" s="13" t="s">
+      <c r="B96" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C96" s="13" t="s">
+      <c r="C96" s="18" t="s">
         <v>124</v>
       </c>
       <c r="D96" s="1"/>
@@ -3899,14 +3973,14 @@
       <c r="V96" s="1"/>
       <c r="W96" s="1"/>
     </row>
-    <row r="97" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A97" s="12" t="s">
+    <row r="97" ht="13.5" customHeight="1">
+      <c r="A97" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="B97" s="14" t="s">
+      <c r="B97" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C97" s="14" t="s">
+      <c r="C97" s="20" t="s">
         <v>126</v>
       </c>
       <c r="D97" s="1"/>
@@ -3930,14 +4004,14 @@
       <c r="V97" s="1"/>
       <c r="W97" s="1"/>
     </row>
-    <row r="98" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A98" s="12" t="s">
+    <row r="98" ht="13.5" customHeight="1">
+      <c r="A98" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="B98" s="13" t="s">
+      <c r="B98" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="C98" s="13" t="s">
+      <c r="C98" s="18" t="s">
         <v>128</v>
       </c>
       <c r="D98" s="1"/>
@@ -3961,14 +4035,14 @@
       <c r="V98" s="1"/>
       <c r="W98" s="1"/>
     </row>
-    <row r="99" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A99" s="12" t="s">
+    <row r="99" ht="13.5" customHeight="1">
+      <c r="A99" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="B99" s="13" t="s">
+      <c r="B99" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="C99" s="13" t="s">
+      <c r="C99" s="18" t="s">
         <v>130</v>
       </c>
       <c r="D99" s="1"/>
@@ -3992,14 +4066,14 @@
       <c r="V99" s="1"/>
       <c r="W99" s="1"/>
     </row>
-    <row r="100" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A100" s="12" t="s">
+    <row r="100" ht="13.5" customHeight="1">
+      <c r="A100" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B100" s="14" t="s">
+      <c r="B100" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C100" s="14" t="s">
+      <c r="C100" s="20" t="s">
         <v>132</v>
       </c>
       <c r="D100" s="1"/>
@@ -4023,14 +4097,14 @@
       <c r="V100" s="1"/>
       <c r="W100" s="1"/>
     </row>
-    <row r="101" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A101" s="12" t="s">
+    <row r="101" ht="13.5" customHeight="1">
+      <c r="A101" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B101" s="13" t="s">
+      <c r="B101" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="C101" s="13" t="s">
+      <c r="C101" s="18" t="s">
         <v>134</v>
       </c>
       <c r="D101" s="1"/>
@@ -4054,14 +4128,14 @@
       <c r="V101" s="1"/>
       <c r="W101" s="1"/>
     </row>
-    <row r="102" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A102" s="15" t="s">
+    <row r="102" ht="13.5" customHeight="1">
+      <c r="A102" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="B102" s="11" t="s">
+      <c r="B102" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C102" s="11" t="s">
+      <c r="C102" s="17" t="s">
         <v>136</v>
       </c>
       <c r="D102" s="1"/>
@@ -4085,14 +4159,14 @@
       <c r="V102" s="1"/>
       <c r="W102" s="1"/>
     </row>
-    <row r="103" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A103" s="12" t="s">
+    <row r="103" ht="13.5" customHeight="1">
+      <c r="A103" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B103" s="11" t="s">
+      <c r="B103" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="C103" s="11" t="s">
+      <c r="C103" s="17" t="s">
         <v>138</v>
       </c>
       <c r="D103" s="1"/>
@@ -4116,14 +4190,14 @@
       <c r="V103" s="1"/>
       <c r="W103" s="1"/>
     </row>
-    <row r="104" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A104" s="15" t="s">
+    <row r="104" ht="13.5" customHeight="1">
+      <c r="A104" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="B104" s="11" t="s">
+      <c r="B104" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="C104" s="11" t="s">
+      <c r="C104" s="17" t="s">
         <v>140</v>
       </c>
       <c r="D104" s="1"/>
@@ -4147,14 +4221,14 @@
       <c r="V104" s="1"/>
       <c r="W104" s="1"/>
     </row>
-    <row r="105" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A105" s="12" t="s">
+    <row r="105" ht="13.5" customHeight="1">
+      <c r="A105" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B105" s="13" t="s">
+      <c r="B105" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="C105" s="18" t="s">
         <v>142</v>
       </c>
       <c r="D105" s="1"/>
@@ -4178,14 +4252,14 @@
       <c r="V105" s="1"/>
       <c r="W105" s="1"/>
     </row>
-    <row r="106" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A106" s="12" t="s">
+    <row r="106" ht="13.5" customHeight="1">
+      <c r="A106" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B106" s="14" t="s">
+      <c r="B106" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="C106" s="14" t="s">
+      <c r="C106" s="20" t="s">
         <v>144</v>
       </c>
       <c r="D106" s="1"/>
@@ -4209,14 +4283,14 @@
       <c r="V106" s="1"/>
       <c r="W106" s="1"/>
     </row>
-    <row r="107" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A107" s="12" t="s">
+    <row r="107" ht="13.5" customHeight="1">
+      <c r="A107" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B107" s="11" t="s">
+      <c r="B107" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="C107" s="11" t="s">
+      <c r="C107" s="17" t="s">
         <v>146</v>
       </c>
       <c r="D107" s="1"/>
@@ -4240,14 +4314,14 @@
       <c r="V107" s="1"/>
       <c r="W107" s="1"/>
     </row>
-    <row r="108" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A108" s="12" t="s">
+    <row r="108" ht="13.5" customHeight="1">
+      <c r="A108" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B108" s="11" t="s">
+      <c r="B108" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C108" s="11" t="s">
+      <c r="C108" s="17" t="s">
         <v>148</v>
       </c>
       <c r="D108" s="1"/>
@@ -4271,14 +4345,14 @@
       <c r="V108" s="1"/>
       <c r="W108" s="1"/>
     </row>
-    <row r="109" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A109" s="12" t="s">
+    <row r="109" ht="13.5" customHeight="1">
+      <c r="A109" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="B109" s="13" t="s">
+      <c r="B109" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="C109" s="13" t="s">
+      <c r="C109" s="18" t="s">
         <v>150</v>
       </c>
       <c r="D109" s="1"/>
@@ -4302,14 +4376,14 @@
       <c r="V109" s="1"/>
       <c r="W109" s="1"/>
     </row>
-    <row r="110" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A110" s="12" t="s">
+    <row r="110" ht="13.5" customHeight="1">
+      <c r="A110" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="B110" s="13" t="s">
+      <c r="B110" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="C110" s="13" t="s">
+      <c r="C110" s="18" t="s">
         <v>152</v>
       </c>
       <c r="D110" s="1"/>
@@ -4333,14 +4407,14 @@
       <c r="V110" s="1"/>
       <c r="W110" s="1"/>
     </row>
-    <row r="111" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A111" s="12" t="s">
+    <row r="111" ht="13.5" customHeight="1">
+      <c r="A111" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B111" s="14" t="s">
+      <c r="B111" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="C111" s="14" t="s">
+      <c r="C111" s="20" t="s">
         <v>154</v>
       </c>
       <c r="D111" s="1"/>
@@ -4364,14 +4438,14 @@
       <c r="V111" s="1"/>
       <c r="W111" s="1"/>
     </row>
-    <row r="112" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A112" s="12" t="s">
+    <row r="112" ht="13.5" customHeight="1">
+      <c r="A112" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="B112" s="11" t="s">
+      <c r="B112" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C112" s="11" t="s">
+      <c r="C112" s="17" t="s">
         <v>156</v>
       </c>
       <c r="D112" s="1"/>
@@ -4395,14 +4469,14 @@
       <c r="V112" s="1"/>
       <c r="W112" s="1"/>
     </row>
-    <row r="113" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A113" s="12" t="s">
+    <row r="113" ht="13.5" customHeight="1">
+      <c r="A113" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="B113" s="13" t="s">
+      <c r="B113" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="C113" s="13" t="s">
+      <c r="C113" s="18" t="s">
         <v>158</v>
       </c>
       <c r="D113" s="1"/>
@@ -4426,14 +4500,14 @@
       <c r="V113" s="1"/>
       <c r="W113" s="1"/>
     </row>
-    <row r="114" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A114" s="12" t="s">
+    <row r="114" ht="13.5" customHeight="1">
+      <c r="A114" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B114" s="11" t="s">
+      <c r="B114" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="C114" s="11" t="s">
+      <c r="C114" s="17" t="s">
         <v>160</v>
       </c>
       <c r="D114" s="1"/>
@@ -4457,15 +4531,15 @@
       <c r="V114" s="1"/>
       <c r="W114" s="1"/>
     </row>
-    <row r="115" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A115" s="13" t="s">
+    <row r="115" ht="13.5" customHeight="1">
+      <c r="A115" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="13" t="s">
+      <c r="B115" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="C115" s="13" t="s">
-        <v>162</v>
+      <c r="C115" s="18" t="s">
+        <v>163</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
@@ -4488,15 +4562,15 @@
       <c r="V115" s="1"/>
       <c r="W115" s="1"/>
     </row>
-    <row r="116" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A116" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="B116" s="11" t="s">
+    <row r="116" ht="13.5" customHeight="1">
+      <c r="A116" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="C116" s="11" t="s">
-        <v>164</v>
+      <c r="B116" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
@@ -4519,15 +4593,15 @@
       <c r="V116" s="1"/>
       <c r="W116" s="1"/>
     </row>
-    <row r="117" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A117" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="B117" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="C117" s="13" t="s">
-        <v>166</v>
+    <row r="117" ht="13.5" customHeight="1">
+      <c r="A117" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B117" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C117" s="18" t="s">
+        <v>169</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
@@ -4550,15 +4624,15 @@
       <c r="V117" s="1"/>
       <c r="W117" s="1"/>
     </row>
-    <row r="118" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A118" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="B118" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="C118" s="11" t="s">
-        <v>168</v>
+    <row r="118" ht="13.5" customHeight="1">
+      <c r="A118" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
@@ -4581,15 +4655,15 @@
       <c r="V118" s="1"/>
       <c r="W118" s="1"/>
     </row>
-    <row r="119" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A119" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="B119" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="C119" s="13" t="s">
-        <v>170</v>
+    <row r="119" ht="13.5" customHeight="1">
+      <c r="A119" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B119" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C119" s="18" t="s">
+        <v>175</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
@@ -4612,15 +4686,15 @@
       <c r="V119" s="1"/>
       <c r="W119" s="1"/>
     </row>
-    <row r="120" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A120" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="B120" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C120" s="16" t="s">
-        <v>172</v>
+    <row r="120" ht="13.5" customHeight="1">
+      <c r="A120" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B120" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C120" s="18" t="s">
+        <v>178</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
@@ -4643,15 +4717,15 @@
       <c r="V120" s="1"/>
       <c r="W120" s="1"/>
     </row>
-    <row r="121" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A121" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="B121" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="C121" s="13" t="s">
-        <v>174</v>
+    <row r="121" ht="13.5" customHeight="1">
+      <c r="A121" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B121" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C121" s="18" t="s">
+        <v>181</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -4674,15 +4748,11 @@
       <c r="V121" s="1"/>
       <c r="W121" s="1"/>
     </row>
-    <row r="122" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A122" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="B122" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="C122" s="13" t="s">
-        <v>176</v>
+    <row r="122" ht="13.5" customHeight="1">
+      <c r="A122" s="15"/>
+      <c r="B122" s="15"/>
+      <c r="C122" s="18" t="s">
+        <v>182</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
@@ -4705,15 +4775,15 @@
       <c r="V122" s="1"/>
       <c r="W122" s="1"/>
     </row>
-    <row r="123" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A123" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B123" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="C123" s="13" t="s">
-        <v>178</v>
+    <row r="123" ht="13.5" customHeight="1">
+      <c r="A123" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B123" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="C123" s="18" t="s">
+        <v>185</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
@@ -4736,15 +4806,11 @@
       <c r="V123" s="1"/>
       <c r="W123" s="1"/>
     </row>
-    <row r="124" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A124" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="B124" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="C124" s="13" t="s">
-        <v>180</v>
+    <row r="124" ht="13.5" customHeight="1">
+      <c r="A124" s="15"/>
+      <c r="B124" s="15"/>
+      <c r="C124" s="18" t="s">
+        <v>186</v>
       </c>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
@@ -4767,15 +4833,15 @@
       <c r="V124" s="1"/>
       <c r="W124" s="1"/>
     </row>
-    <row r="125" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A125" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="B125" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="C125" s="13" t="s">
-        <v>182</v>
+    <row r="125" ht="13.5" customHeight="1">
+      <c r="A125" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="B125" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C125" s="18" t="s">
+        <v>189</v>
       </c>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
@@ -4798,15 +4864,15 @@
       <c r="V125" s="1"/>
       <c r="W125" s="1"/>
     </row>
-    <row r="126" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A126" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="B126" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="C126" s="11" t="s">
-        <v>184</v>
+    <row r="126" ht="13.5" customHeight="1">
+      <c r="A126" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="B126" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="C126" s="17" t="s">
+        <v>192</v>
       </c>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
@@ -4829,15 +4895,15 @@
       <c r="V126" s="1"/>
       <c r="W126" s="1"/>
     </row>
-    <row r="127" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A127" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="B127" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="C127" s="13" t="s">
-        <v>186</v>
+    <row r="127" ht="13.5" customHeight="1">
+      <c r="A127" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="B127" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C127" s="18" t="s">
+        <v>195</v>
       </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
@@ -4860,15 +4926,15 @@
       <c r="V127" s="1"/>
       <c r="W127" s="1"/>
     </row>
-    <row r="128" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A128" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="B128" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="C128" s="13" t="s">
-        <v>188</v>
+    <row r="128" ht="13.5" customHeight="1">
+      <c r="A128" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B128" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="C128" s="18" t="s">
+        <v>198</v>
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
@@ -4891,15 +4957,15 @@
       <c r="V128" s="1"/>
       <c r="W128" s="1"/>
     </row>
-    <row r="129" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A129" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="B129" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="C129" s="13" t="s">
-        <v>190</v>
+    <row r="129" ht="13.5" customHeight="1">
+      <c r="A129" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B129" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C129" s="18" t="s">
+        <v>201</v>
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
@@ -4922,15 +4988,15 @@
       <c r="V129" s="1"/>
       <c r="W129" s="1"/>
     </row>
-    <row r="130" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A130" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="B130" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="C130" s="11" t="s">
-        <v>192</v>
+    <row r="130" ht="13.5" customHeight="1">
+      <c r="A130" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B130" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="C130" s="17" t="s">
+        <v>204</v>
       </c>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
@@ -4953,15 +5019,15 @@
       <c r="V130" s="1"/>
       <c r="W130" s="1"/>
     </row>
-    <row r="131" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A131" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="B131" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="C131" s="13" t="s">
-        <v>194</v>
+    <row r="131" ht="13.5" customHeight="1">
+      <c r="A131" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="B131" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C131" s="18" t="s">
+        <v>206</v>
       </c>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
@@ -4984,15 +5050,15 @@
       <c r="V131" s="1"/>
       <c r="W131" s="1"/>
     </row>
-    <row r="132" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A132" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="B132" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="C132" s="13" t="s">
-        <v>196</v>
+    <row r="132" ht="13.5" customHeight="1">
+      <c r="A132" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B132" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C132" s="18" t="s">
+        <v>208</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
@@ -5015,15 +5081,15 @@
       <c r="V132" s="1"/>
       <c r="W132" s="1"/>
     </row>
-    <row r="133" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A133" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="B133" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="C133" s="13" t="s">
-        <v>198</v>
+    <row r="133" ht="13.5" customHeight="1">
+      <c r="A133" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B133" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="C133" s="18" t="s">
+        <v>210</v>
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
@@ -5046,15 +5112,15 @@
       <c r="V133" s="1"/>
       <c r="W133" s="1"/>
     </row>
-    <row r="134" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A134" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="B134" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="C134" s="13" t="s">
-        <v>200</v>
+    <row r="134" ht="13.5" customHeight="1">
+      <c r="A134" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B134" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C134" s="18" t="s">
+        <v>212</v>
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
@@ -5077,15 +5143,15 @@
       <c r="V134" s="1"/>
       <c r="W134" s="1"/>
     </row>
-    <row r="135" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A135" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="B135" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="C135" s="13" t="s">
-        <v>202</v>
+    <row r="135" ht="13.5" customHeight="1">
+      <c r="A135" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B135" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="C135" s="18" t="s">
+        <v>214</v>
       </c>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
@@ -5108,15 +5174,15 @@
       <c r="V135" s="1"/>
       <c r="W135" s="1"/>
     </row>
-    <row r="136" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A136" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="B136" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="C136" s="13" t="s">
-        <v>204</v>
+    <row r="136" ht="13.5" customHeight="1">
+      <c r="A136" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B136" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C136" s="18" t="s">
+        <v>216</v>
       </c>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
@@ -5139,15 +5205,15 @@
       <c r="V136" s="1"/>
       <c r="W136" s="1"/>
     </row>
-    <row r="137" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A137" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="B137" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C137" s="13" t="s">
-        <v>206</v>
+    <row r="137" ht="13.5" customHeight="1">
+      <c r="A137" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B137" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C137" s="18" t="s">
+        <v>218</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
@@ -5170,10 +5236,10 @@
       <c r="V137" s="1"/>
       <c r="W137" s="1"/>
     </row>
-    <row r="138" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A138" s="13"/>
-      <c r="B138" s="13"/>
-      <c r="C138" s="13"/>
+    <row r="138" ht="13.5" customHeight="1">
+      <c r="A138" s="15"/>
+      <c r="B138" s="15"/>
+      <c r="C138" s="18"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -5195,15 +5261,15 @@
       <c r="V138" s="1"/>
       <c r="W138" s="1"/>
     </row>
-    <row r="139" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A139" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="B139" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="C139" s="13" t="s">
-        <v>208</v>
+    <row r="139" ht="13.5" customHeight="1">
+      <c r="A139" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="B139" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C139" s="18" t="s">
+        <v>220</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -5226,15 +5292,15 @@
       <c r="V139" s="1"/>
       <c r="W139" s="1"/>
     </row>
-    <row r="140" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A140" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="B140" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="C140" s="13" t="s">
-        <v>210</v>
+    <row r="140" ht="13.5" customHeight="1">
+      <c r="A140" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="B140" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="C140" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
@@ -5257,15 +5323,15 @@
       <c r="V140" s="1"/>
       <c r="W140" s="1"/>
     </row>
-    <row r="141" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A141" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="B141" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="C141" s="13" t="s">
-        <v>212</v>
+    <row r="141" ht="13.5" customHeight="1">
+      <c r="A141" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B141" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C141" s="18" t="s">
+        <v>224</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
@@ -5288,15 +5354,15 @@
       <c r="V141" s="1"/>
       <c r="W141" s="1"/>
     </row>
-    <row r="142" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A142" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="B142" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="C142" s="13" t="s">
-        <v>214</v>
+    <row r="142" ht="13.5" customHeight="1">
+      <c r="A142" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B142" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C142" s="18" t="s">
+        <v>226</v>
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
@@ -5319,15 +5385,15 @@
       <c r="V142" s="1"/>
       <c r="W142" s="1"/>
     </row>
-    <row r="143" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A143" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="B143" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="C143" s="13" t="s">
-        <v>216</v>
+    <row r="143" ht="13.5" customHeight="1">
+      <c r="A143" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B143" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C143" s="18" t="s">
+        <v>228</v>
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
@@ -5350,15 +5416,15 @@
       <c r="V143" s="1"/>
       <c r="W143" s="1"/>
     </row>
-    <row r="144" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A144" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="B144" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C144" s="13" t="s">
-        <v>217</v>
+    <row r="144" ht="13.5" customHeight="1">
+      <c r="A144" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="B144" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C144" s="18" t="s">
+        <v>229</v>
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
@@ -5381,15 +5447,15 @@
       <c r="V144" s="1"/>
       <c r="W144" s="1"/>
     </row>
-    <row r="145" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A145" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="B145" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="C145" s="13" t="s">
-        <v>214</v>
+    <row r="145" ht="13.5" customHeight="1">
+      <c r="A145" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B145" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C145" s="18" t="s">
+        <v>226</v>
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
@@ -5412,15 +5478,15 @@
       <c r="V145" s="1"/>
       <c r="W145" s="1"/>
     </row>
-    <row r="146" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A146" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="B146" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="C146" s="13" t="s">
-        <v>216</v>
+    <row r="146" ht="13.5" customHeight="1">
+      <c r="A146" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B146" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C146" s="18" t="s">
+        <v>228</v>
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
@@ -5443,15 +5509,15 @@
       <c r="V146" s="1"/>
       <c r="W146" s="1"/>
     </row>
-    <row r="147" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A147" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="B147" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="C147" s="13" t="s">
-        <v>219</v>
+    <row r="147" ht="13.5" customHeight="1">
+      <c r="A147" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="B147" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="C147" s="18" t="s">
+        <v>231</v>
       </c>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -5474,15 +5540,15 @@
       <c r="V147" s="1"/>
       <c r="W147" s="1"/>
     </row>
-    <row r="148" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A148" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B148" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="C148" s="13" t="s">
-        <v>221</v>
+    <row r="148" ht="13.5" customHeight="1">
+      <c r="A148" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B148" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C148" s="18" t="s">
+        <v>234</v>
       </c>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
@@ -5505,15 +5571,15 @@
       <c r="V148" s="1"/>
       <c r="W148" s="1"/>
     </row>
-    <row r="149" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A149" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="B149" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="C149" s="11" t="s">
-        <v>223</v>
+    <row r="149" ht="13.5" customHeight="1">
+      <c r="A149" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B149" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C149" s="17" t="s">
+        <v>237</v>
       </c>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
@@ -5536,15 +5602,15 @@
       <c r="V149" s="1"/>
       <c r="W149" s="1"/>
     </row>
-    <row r="150" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A150" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="B150" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="C150" s="13" t="s">
-        <v>225</v>
+    <row r="150" ht="13.5" customHeight="1">
+      <c r="A150" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B150" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C150" s="18" t="s">
+        <v>239</v>
       </c>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
@@ -5567,15 +5633,15 @@
       <c r="V150" s="1"/>
       <c r="W150" s="1"/>
     </row>
-    <row r="151" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A151" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="B151" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="C151" s="13" t="s">
-        <v>227</v>
+    <row r="151" ht="13.5" customHeight="1">
+      <c r="A151" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B151" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="C151" s="18" t="s">
+        <v>241</v>
       </c>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
@@ -5598,15 +5664,15 @@
       <c r="V151" s="1"/>
       <c r="W151" s="1"/>
     </row>
-    <row r="152" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A152" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="B152" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="C152" s="13" t="s">
-        <v>229</v>
+    <row r="152" ht="13.5" customHeight="1">
+      <c r="A152" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="B152" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C152" s="18" t="s">
+        <v>243</v>
       </c>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
@@ -5629,9 +5695,13 @@
       <c r="V152" s="1"/>
       <c r="W152" s="1"/>
     </row>
-    <row r="153" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A153" s="17"/>
-      <c r="B153" s="17"/>
+    <row r="153" ht="13.5" customHeight="1">
+      <c r="A153" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B153" s="22" t="s">
+        <v>245</v>
+      </c>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
@@ -5654,7 +5724,7 @@
       <c r="V153" s="1"/>
       <c r="W153" s="1"/>
     </row>
-    <row r="154" spans="1:23" ht="13.5" customHeight="1">
+    <row r="154" ht="13.5" customHeight="1">
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
@@ -5677,7 +5747,7 @@
       <c r="V154" s="1"/>
       <c r="W154" s="1"/>
     </row>
-    <row r="155" spans="1:23" ht="13.5" customHeight="1">
+    <row r="155" ht="13.5" customHeight="1">
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -5700,7 +5770,7 @@
       <c r="V155" s="1"/>
       <c r="W155" s="1"/>
     </row>
-    <row r="156" spans="1:23" ht="13.5" customHeight="1">
+    <row r="156" ht="13.5" customHeight="1">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -5725,7 +5795,7 @@
       <c r="V156" s="1"/>
       <c r="W156" s="1"/>
     </row>
-    <row r="157" spans="1:23" ht="13.5" customHeight="1">
+    <row r="157" ht="13.5" customHeight="1">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -5750,7 +5820,7 @@
       <c r="V157" s="1"/>
       <c r="W157" s="1"/>
     </row>
-    <row r="158" spans="1:23" ht="13.5" customHeight="1">
+    <row r="158" ht="13.5" customHeight="1">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -5775,7 +5845,7 @@
       <c r="V158" s="1"/>
       <c r="W158" s="1"/>
     </row>
-    <row r="159" spans="1:23" ht="13.5" customHeight="1">
+    <row r="159" ht="13.5" customHeight="1">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -5800,7 +5870,7 @@
       <c r="V159" s="1"/>
       <c r="W159" s="1"/>
     </row>
-    <row r="160" spans="1:23" ht="13.5" customHeight="1">
+    <row r="160" ht="13.5" customHeight="1">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -5825,7 +5895,7 @@
       <c r="V160" s="1"/>
       <c r="W160" s="1"/>
     </row>
-    <row r="161" spans="1:23" ht="13.5" customHeight="1">
+    <row r="161" ht="13.5" customHeight="1">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -5850,7 +5920,7 @@
       <c r="V161" s="1"/>
       <c r="W161" s="1"/>
     </row>
-    <row r="162" spans="1:23" ht="13.5" customHeight="1">
+    <row r="162" ht="13.5" customHeight="1">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -5875,7 +5945,7 @@
       <c r="V162" s="1"/>
       <c r="W162" s="1"/>
     </row>
-    <row r="163" spans="1:23" ht="13.5" customHeight="1">
+    <row r="163" ht="13.5" customHeight="1">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -5900,7 +5970,7 @@
       <c r="V163" s="1"/>
       <c r="W163" s="1"/>
     </row>
-    <row r="164" spans="1:23" ht="13.5" customHeight="1">
+    <row r="164" ht="13.5" customHeight="1">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -5925,7 +5995,7 @@
       <c r="V164" s="1"/>
       <c r="W164" s="1"/>
     </row>
-    <row r="165" spans="1:23" ht="13.5" customHeight="1">
+    <row r="165" ht="13.5" customHeight="1">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -5950,7 +6020,7 @@
       <c r="V165" s="1"/>
       <c r="W165" s="1"/>
     </row>
-    <row r="166" spans="1:23" ht="13.5" customHeight="1">
+    <row r="166" ht="13.5" customHeight="1">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -5975,7 +6045,7 @@
       <c r="V166" s="1"/>
       <c r="W166" s="1"/>
     </row>
-    <row r="167" spans="1:23" ht="13.5" customHeight="1">
+    <row r="167" ht="13.5" customHeight="1">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -6000,7 +6070,7 @@
       <c r="V167" s="1"/>
       <c r="W167" s="1"/>
     </row>
-    <row r="168" spans="1:23" ht="13.5" customHeight="1">
+    <row r="168" ht="13.5" customHeight="1">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -6025,7 +6095,7 @@
       <c r="V168" s="1"/>
       <c r="W168" s="1"/>
     </row>
-    <row r="169" spans="1:23" ht="13.5" customHeight="1">
+    <row r="169" ht="13.5" customHeight="1">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -6050,7 +6120,7 @@
       <c r="V169" s="1"/>
       <c r="W169" s="1"/>
     </row>
-    <row r="170" spans="1:23" ht="13.5" customHeight="1">
+    <row r="170" ht="13.5" customHeight="1">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -6075,7 +6145,7 @@
       <c r="V170" s="1"/>
       <c r="W170" s="1"/>
     </row>
-    <row r="171" spans="1:23" ht="13.5" customHeight="1">
+    <row r="171" ht="13.5" customHeight="1">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -6100,7 +6170,7 @@
       <c r="V171" s="1"/>
       <c r="W171" s="1"/>
     </row>
-    <row r="172" spans="1:23" ht="13.5" customHeight="1">
+    <row r="172" ht="13.5" customHeight="1">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -6125,7 +6195,7 @@
       <c r="V172" s="1"/>
       <c r="W172" s="1"/>
     </row>
-    <row r="173" spans="1:23" ht="13.5" customHeight="1">
+    <row r="173" ht="13.5" customHeight="1">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -6150,7 +6220,7 @@
       <c r="V173" s="1"/>
       <c r="W173" s="1"/>
     </row>
-    <row r="174" spans="1:23" ht="13.5" customHeight="1">
+    <row r="174" ht="13.5" customHeight="1">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -6175,7 +6245,7 @@
       <c r="V174" s="1"/>
       <c r="W174" s="1"/>
     </row>
-    <row r="175" spans="1:23" ht="13.5" customHeight="1">
+    <row r="175" ht="13.5" customHeight="1">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -6200,7 +6270,7 @@
       <c r="V175" s="1"/>
       <c r="W175" s="1"/>
     </row>
-    <row r="176" spans="1:23" ht="13.5" customHeight="1">
+    <row r="176" ht="13.5" customHeight="1">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -6225,7 +6295,7 @@
       <c r="V176" s="1"/>
       <c r="W176" s="1"/>
     </row>
-    <row r="177" spans="1:23" ht="13.5" customHeight="1">
+    <row r="177" ht="13.5" customHeight="1">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -6250,7 +6320,7 @@
       <c r="V177" s="1"/>
       <c r="W177" s="1"/>
     </row>
-    <row r="178" spans="1:23" ht="13.5" customHeight="1">
+    <row r="178" ht="13.5" customHeight="1">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -6275,7 +6345,7 @@
       <c r="V178" s="1"/>
       <c r="W178" s="1"/>
     </row>
-    <row r="179" spans="1:23" ht="13.5" customHeight="1">
+    <row r="179" ht="13.5" customHeight="1">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -6300,7 +6370,7 @@
       <c r="V179" s="1"/>
       <c r="W179" s="1"/>
     </row>
-    <row r="180" spans="1:23" ht="13.5" customHeight="1">
+    <row r="180" ht="13.5" customHeight="1">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -6325,7 +6395,7 @@
       <c r="V180" s="1"/>
       <c r="W180" s="1"/>
     </row>
-    <row r="181" spans="1:23" ht="13.5" customHeight="1">
+    <row r="181" ht="13.5" customHeight="1">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -6350,7 +6420,7 @@
       <c r="V181" s="1"/>
       <c r="W181" s="1"/>
     </row>
-    <row r="182" spans="1:23" ht="13.5" customHeight="1">
+    <row r="182" ht="13.5" customHeight="1">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -6375,7 +6445,7 @@
       <c r="V182" s="1"/>
       <c r="W182" s="1"/>
     </row>
-    <row r="183" spans="1:23" ht="13.5" customHeight="1">
+    <row r="183" ht="13.5" customHeight="1">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -6400,7 +6470,7 @@
       <c r="V183" s="1"/>
       <c r="W183" s="1"/>
     </row>
-    <row r="184" spans="1:23" ht="13.5" customHeight="1">
+    <row r="184" ht="13.5" customHeight="1">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -6425,7 +6495,7 @@
       <c r="V184" s="1"/>
       <c r="W184" s="1"/>
     </row>
-    <row r="185" spans="1:23" ht="13.5" customHeight="1">
+    <row r="185" ht="13.5" customHeight="1">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -6450,7 +6520,7 @@
       <c r="V185" s="1"/>
       <c r="W185" s="1"/>
     </row>
-    <row r="186" spans="1:23" ht="13.5" customHeight="1">
+    <row r="186" ht="13.5" customHeight="1">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -6475,7 +6545,7 @@
       <c r="V186" s="1"/>
       <c r="W186" s="1"/>
     </row>
-    <row r="187" spans="1:23" ht="13.5" customHeight="1">
+    <row r="187" ht="13.5" customHeight="1">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -6500,7 +6570,7 @@
       <c r="V187" s="1"/>
       <c r="W187" s="1"/>
     </row>
-    <row r="188" spans="1:23" ht="13.5" customHeight="1">
+    <row r="188" ht="13.5" customHeight="1">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -6525,7 +6595,7 @@
       <c r="V188" s="1"/>
       <c r="W188" s="1"/>
     </row>
-    <row r="189" spans="1:23" ht="13.5" customHeight="1">
+    <row r="189" ht="13.5" customHeight="1">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -6550,7 +6620,7 @@
       <c r="V189" s="1"/>
       <c r="W189" s="1"/>
     </row>
-    <row r="190" spans="1:23" ht="13.5" customHeight="1">
+    <row r="190" ht="13.5" customHeight="1">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -6575,7 +6645,7 @@
       <c r="V190" s="1"/>
       <c r="W190" s="1"/>
     </row>
-    <row r="191" spans="1:23" ht="13.5" customHeight="1">
+    <row r="191" ht="13.5" customHeight="1">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -6600,7 +6670,7 @@
       <c r="V191" s="1"/>
       <c r="W191" s="1"/>
     </row>
-    <row r="192" spans="1:23" ht="13.5" customHeight="1">
+    <row r="192" ht="13.5" customHeight="1">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -6625,7 +6695,7 @@
       <c r="V192" s="1"/>
       <c r="W192" s="1"/>
     </row>
-    <row r="193" spans="1:23" ht="13.5" customHeight="1">
+    <row r="193" ht="13.5" customHeight="1">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -6650,7 +6720,7 @@
       <c r="V193" s="1"/>
       <c r="W193" s="1"/>
     </row>
-    <row r="194" spans="1:23" ht="13.5" customHeight="1">
+    <row r="194" ht="13.5" customHeight="1">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -6675,7 +6745,7 @@
       <c r="V194" s="1"/>
       <c r="W194" s="1"/>
     </row>
-    <row r="195" spans="1:23" ht="13.5" customHeight="1">
+    <row r="195" ht="13.5" customHeight="1">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -6700,7 +6770,7 @@
       <c r="V195" s="1"/>
       <c r="W195" s="1"/>
     </row>
-    <row r="196" spans="1:23" ht="13.5" customHeight="1">
+    <row r="196" ht="13.5" customHeight="1">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -6725,7 +6795,7 @@
       <c r="V196" s="1"/>
       <c r="W196" s="1"/>
     </row>
-    <row r="197" spans="1:23" ht="13.5" customHeight="1">
+    <row r="197" ht="13.5" customHeight="1">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -6750,7 +6820,7 @@
       <c r="V197" s="1"/>
       <c r="W197" s="1"/>
     </row>
-    <row r="198" spans="1:23" ht="13.5" customHeight="1">
+    <row r="198" ht="13.5" customHeight="1">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -6775,7 +6845,7 @@
       <c r="V198" s="1"/>
       <c r="W198" s="1"/>
     </row>
-    <row r="199" spans="1:23" ht="13.5" customHeight="1">
+    <row r="199" ht="13.5" customHeight="1">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -6800,7 +6870,7 @@
       <c r="V199" s="1"/>
       <c r="W199" s="1"/>
     </row>
-    <row r="200" spans="1:23" ht="13.5" customHeight="1">
+    <row r="200" ht="13.5" customHeight="1">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -6825,7 +6895,7 @@
       <c r="V200" s="1"/>
       <c r="W200" s="1"/>
     </row>
-    <row r="201" spans="1:23" ht="13.5" customHeight="1">
+    <row r="201" ht="13.5" customHeight="1">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -6850,7 +6920,7 @@
       <c r="V201" s="1"/>
       <c r="W201" s="1"/>
     </row>
-    <row r="202" spans="1:23" ht="13.5" customHeight="1">
+    <row r="202" ht="13.5" customHeight="1">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -6875,7 +6945,7 @@
       <c r="V202" s="1"/>
       <c r="W202" s="1"/>
     </row>
-    <row r="203" spans="1:23" ht="13.5" customHeight="1">
+    <row r="203" ht="13.5" customHeight="1">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -6900,7 +6970,7 @@
       <c r="V203" s="1"/>
       <c r="W203" s="1"/>
     </row>
-    <row r="204" spans="1:23" ht="13.5" customHeight="1">
+    <row r="204" ht="13.5" customHeight="1">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -6925,7 +6995,7 @@
       <c r="V204" s="1"/>
       <c r="W204" s="1"/>
     </row>
-    <row r="205" spans="1:23" ht="13.5" customHeight="1">
+    <row r="205" ht="13.5" customHeight="1">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -6950,7 +7020,7 @@
       <c r="V205" s="1"/>
       <c r="W205" s="1"/>
     </row>
-    <row r="206" spans="1:23" ht="13.5" customHeight="1">
+    <row r="206" ht="13.5" customHeight="1">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -6975,7 +7045,7 @@
       <c r="V206" s="1"/>
       <c r="W206" s="1"/>
     </row>
-    <row r="207" spans="1:23" ht="13.5" customHeight="1">
+    <row r="207" ht="13.5" customHeight="1">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -7000,7 +7070,7 @@
       <c r="V207" s="1"/>
       <c r="W207" s="1"/>
     </row>
-    <row r="208" spans="1:23" ht="13.5" customHeight="1">
+    <row r="208" ht="13.5" customHeight="1">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -7025,7 +7095,7 @@
       <c r="V208" s="1"/>
       <c r="W208" s="1"/>
     </row>
-    <row r="209" spans="1:23" ht="13.5" customHeight="1">
+    <row r="209" ht="13.5" customHeight="1">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -7050,7 +7120,7 @@
       <c r="V209" s="1"/>
       <c r="W209" s="1"/>
     </row>
-    <row r="210" spans="1:23" ht="13.5" customHeight="1">
+    <row r="210" ht="13.5" customHeight="1">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -7075,7 +7145,7 @@
       <c r="V210" s="1"/>
       <c r="W210" s="1"/>
     </row>
-    <row r="211" spans="1:23" ht="13.5" customHeight="1">
+    <row r="211" ht="13.5" customHeight="1">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -7100,7 +7170,7 @@
       <c r="V211" s="1"/>
       <c r="W211" s="1"/>
     </row>
-    <row r="212" spans="1:23" ht="13.5" customHeight="1">
+    <row r="212" ht="13.5" customHeight="1">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -7125,7 +7195,7 @@
       <c r="V212" s="1"/>
       <c r="W212" s="1"/>
     </row>
-    <row r="213" spans="1:23" ht="13.5" customHeight="1">
+    <row r="213" ht="13.5" customHeight="1">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -7150,7 +7220,7 @@
       <c r="V213" s="1"/>
       <c r="W213" s="1"/>
     </row>
-    <row r="214" spans="1:23" ht="13.5" customHeight="1">
+    <row r="214" ht="13.5" customHeight="1">
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -7175,7 +7245,7 @@
       <c r="V214" s="1"/>
       <c r="W214" s="1"/>
     </row>
-    <row r="215" spans="1:23" ht="13.5" customHeight="1">
+    <row r="215" ht="13.5" customHeight="1">
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -7200,7 +7270,7 @@
       <c r="V215" s="1"/>
       <c r="W215" s="1"/>
     </row>
-    <row r="216" spans="1:23" ht="13.5" customHeight="1">
+    <row r="216" ht="13.5" customHeight="1">
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -7225,7 +7295,7 @@
       <c r="V216" s="1"/>
       <c r="W216" s="1"/>
     </row>
-    <row r="217" spans="1:23" ht="13.5" customHeight="1">
+    <row r="217" ht="13.5" customHeight="1">
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
@@ -7250,7 +7320,7 @@
       <c r="V217" s="1"/>
       <c r="W217" s="1"/>
     </row>
-    <row r="218" spans="1:23" ht="13.5" customHeight="1">
+    <row r="218" ht="13.5" customHeight="1">
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -7275,7 +7345,7 @@
       <c r="V218" s="1"/>
       <c r="W218" s="1"/>
     </row>
-    <row r="219" spans="1:23" ht="13.5" customHeight="1">
+    <row r="219" ht="13.5" customHeight="1">
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
@@ -7300,7 +7370,7 @@
       <c r="V219" s="1"/>
       <c r="W219" s="1"/>
     </row>
-    <row r="220" spans="1:23" ht="13.5" customHeight="1">
+    <row r="220" ht="13.5" customHeight="1">
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
@@ -7325,7 +7395,7 @@
       <c r="V220" s="1"/>
       <c r="W220" s="1"/>
     </row>
-    <row r="221" spans="1:23" ht="13.5" customHeight="1">
+    <row r="221" ht="13.5" customHeight="1">
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -7350,7 +7420,7 @@
       <c r="V221" s="1"/>
       <c r="W221" s="1"/>
     </row>
-    <row r="222" spans="1:23" ht="13.5" customHeight="1">
+    <row r="222" ht="13.5" customHeight="1">
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -7375,7 +7445,7 @@
       <c r="V222" s="1"/>
       <c r="W222" s="1"/>
     </row>
-    <row r="223" spans="1:23" ht="13.5" customHeight="1">
+    <row r="223" ht="13.5" customHeight="1">
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -7400,7 +7470,7 @@
       <c r="V223" s="1"/>
       <c r="W223" s="1"/>
     </row>
-    <row r="224" spans="1:23" ht="13.5" customHeight="1">
+    <row r="224" ht="13.5" customHeight="1">
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -7425,7 +7495,7 @@
       <c r="V224" s="1"/>
       <c r="W224" s="1"/>
     </row>
-    <row r="225" spans="1:23" ht="13.5" customHeight="1">
+    <row r="225" ht="13.5" customHeight="1">
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
@@ -7450,7 +7520,7 @@
       <c r="V225" s="1"/>
       <c r="W225" s="1"/>
     </row>
-    <row r="226" spans="1:23" ht="13.5" customHeight="1">
+    <row r="226" ht="13.5" customHeight="1">
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
@@ -7475,7 +7545,7 @@
       <c r="V226" s="1"/>
       <c r="W226" s="1"/>
     </row>
-    <row r="227" spans="1:23" ht="13.5" customHeight="1">
+    <row r="227" ht="13.5" customHeight="1">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
@@ -7500,7 +7570,7 @@
       <c r="V227" s="1"/>
       <c r="W227" s="1"/>
     </row>
-    <row r="228" spans="1:23" ht="13.5" customHeight="1">
+    <row r="228" ht="13.5" customHeight="1">
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -7525,7 +7595,7 @@
       <c r="V228" s="1"/>
       <c r="W228" s="1"/>
     </row>
-    <row r="229" spans="1:23" ht="13.5" customHeight="1">
+    <row r="229" ht="13.5" customHeight="1">
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
@@ -7550,7 +7620,7 @@
       <c r="V229" s="1"/>
       <c r="W229" s="1"/>
     </row>
-    <row r="230" spans="1:23" ht="13.5" customHeight="1">
+    <row r="230" ht="13.5" customHeight="1">
       <c r="A230" s="1"/>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
@@ -7575,7 +7645,7 @@
       <c r="V230" s="1"/>
       <c r="W230" s="1"/>
     </row>
-    <row r="231" spans="1:23" ht="13.5" customHeight="1">
+    <row r="231" ht="13.5" customHeight="1">
       <c r="A231" s="1"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
@@ -7600,7 +7670,7 @@
       <c r="V231" s="1"/>
       <c r="W231" s="1"/>
     </row>
-    <row r="232" spans="1:23" ht="13.5" customHeight="1">
+    <row r="232" ht="13.5" customHeight="1">
       <c r="A232" s="1"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
@@ -7625,7 +7695,7 @@
       <c r="V232" s="1"/>
       <c r="W232" s="1"/>
     </row>
-    <row r="233" spans="1:23" ht="13.5" customHeight="1">
+    <row r="233" ht="13.5" customHeight="1">
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
@@ -7650,7 +7720,7 @@
       <c r="V233" s="1"/>
       <c r="W233" s="1"/>
     </row>
-    <row r="234" spans="1:23" ht="13.5" customHeight="1">
+    <row r="234" ht="13.5" customHeight="1">
       <c r="A234" s="1"/>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
@@ -7675,7 +7745,7 @@
       <c r="V234" s="1"/>
       <c r="W234" s="1"/>
     </row>
-    <row r="235" spans="1:23" ht="13.5" customHeight="1">
+    <row r="235" ht="13.5" customHeight="1">
       <c r="A235" s="1"/>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
@@ -7700,7 +7770,7 @@
       <c r="V235" s="1"/>
       <c r="W235" s="1"/>
     </row>
-    <row r="236" spans="1:23" ht="13.5" customHeight="1">
+    <row r="236" ht="13.5" customHeight="1">
       <c r="A236" s="1"/>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
@@ -7725,7 +7795,7 @@
       <c r="V236" s="1"/>
       <c r="W236" s="1"/>
     </row>
-    <row r="237" spans="1:23" ht="13.5" customHeight="1">
+    <row r="237" ht="13.5" customHeight="1">
       <c r="A237" s="1"/>
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
@@ -7750,7 +7820,7 @@
       <c r="V237" s="1"/>
       <c r="W237" s="1"/>
     </row>
-    <row r="238" spans="1:23" ht="13.5" customHeight="1">
+    <row r="238" ht="13.5" customHeight="1">
       <c r="A238" s="1"/>
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
@@ -7775,7 +7845,7 @@
       <c r="V238" s="1"/>
       <c r="W238" s="1"/>
     </row>
-    <row r="239" spans="1:23" ht="13.5" customHeight="1">
+    <row r="239" ht="13.5" customHeight="1">
       <c r="A239" s="1"/>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
@@ -7800,7 +7870,7 @@
       <c r="V239" s="1"/>
       <c r="W239" s="1"/>
     </row>
-    <row r="240" spans="1:23" ht="13.5" customHeight="1">
+    <row r="240" ht="13.5" customHeight="1">
       <c r="A240" s="1"/>
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
@@ -7825,7 +7895,7 @@
       <c r="V240" s="1"/>
       <c r="W240" s="1"/>
     </row>
-    <row r="241" spans="1:23" ht="13.5" customHeight="1">
+    <row r="241" ht="13.5" customHeight="1">
       <c r="A241" s="1"/>
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
@@ -7850,7 +7920,7 @@
       <c r="V241" s="1"/>
       <c r="W241" s="1"/>
     </row>
-    <row r="242" spans="1:23" ht="13.5" customHeight="1">
+    <row r="242" ht="13.5" customHeight="1">
       <c r="A242" s="1"/>
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
@@ -7875,7 +7945,7 @@
       <c r="V242" s="1"/>
       <c r="W242" s="1"/>
     </row>
-    <row r="243" spans="1:23" ht="13.5" customHeight="1">
+    <row r="243" ht="13.5" customHeight="1">
       <c r="A243" s="1"/>
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
@@ -7900,7 +7970,7 @@
       <c r="V243" s="1"/>
       <c r="W243" s="1"/>
     </row>
-    <row r="244" spans="1:23" ht="13.5" customHeight="1">
+    <row r="244" ht="13.5" customHeight="1">
       <c r="A244" s="1"/>
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
@@ -7925,7 +7995,7 @@
       <c r="V244" s="1"/>
       <c r="W244" s="1"/>
     </row>
-    <row r="245" spans="1:23" ht="13.5" customHeight="1">
+    <row r="245" ht="13.5" customHeight="1">
       <c r="A245" s="1"/>
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
@@ -7950,7 +8020,7 @@
       <c r="V245" s="1"/>
       <c r="W245" s="1"/>
     </row>
-    <row r="246" spans="1:23" ht="13.5" customHeight="1">
+    <row r="246" ht="13.5" customHeight="1">
       <c r="A246" s="1"/>
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
@@ -7975,7 +8045,7 @@
       <c r="V246" s="1"/>
       <c r="W246" s="1"/>
     </row>
-    <row r="247" spans="1:23" ht="13.5" customHeight="1">
+    <row r="247" ht="13.5" customHeight="1">
       <c r="A247" s="1"/>
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
@@ -8000,7 +8070,7 @@
       <c r="V247" s="1"/>
       <c r="W247" s="1"/>
     </row>
-    <row r="248" spans="1:23" ht="13.5" customHeight="1">
+    <row r="248" ht="13.5" customHeight="1">
       <c r="A248" s="1"/>
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
@@ -8025,7 +8095,7 @@
       <c r="V248" s="1"/>
       <c r="W248" s="1"/>
     </row>
-    <row r="249" spans="1:23" ht="13.5" customHeight="1">
+    <row r="249" ht="13.5" customHeight="1">
       <c r="A249" s="1"/>
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
@@ -8050,7 +8120,7 @@
       <c r="V249" s="1"/>
       <c r="W249" s="1"/>
     </row>
-    <row r="250" spans="1:23" ht="13.5" customHeight="1">
+    <row r="250" ht="13.5" customHeight="1">
       <c r="A250" s="1"/>
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
@@ -8075,7 +8145,7 @@
       <c r="V250" s="1"/>
       <c r="W250" s="1"/>
     </row>
-    <row r="251" spans="1:23" ht="13.5" customHeight="1">
+    <row r="251" ht="13.5" customHeight="1">
       <c r="A251" s="1"/>
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
@@ -8100,7 +8170,7 @@
       <c r="V251" s="1"/>
       <c r="W251" s="1"/>
     </row>
-    <row r="252" spans="1:23" ht="13.5" customHeight="1">
+    <row r="252" ht="13.5" customHeight="1">
       <c r="A252" s="1"/>
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
@@ -8125,7 +8195,7 @@
       <c r="V252" s="1"/>
       <c r="W252" s="1"/>
     </row>
-    <row r="253" spans="1:23" ht="13.5" customHeight="1">
+    <row r="253" ht="13.5" customHeight="1">
       <c r="A253" s="1"/>
       <c r="B253" s="1"/>
       <c r="C253" s="1"/>
@@ -8150,7 +8220,7 @@
       <c r="V253" s="1"/>
       <c r="W253" s="1"/>
     </row>
-    <row r="254" spans="1:23" ht="13.5" customHeight="1">
+    <row r="254" ht="13.5" customHeight="1">
       <c r="A254" s="1"/>
       <c r="B254" s="1"/>
       <c r="C254" s="1"/>
@@ -8175,7 +8245,7 @@
       <c r="V254" s="1"/>
       <c r="W254" s="1"/>
     </row>
-    <row r="255" spans="1:23" ht="13.5" customHeight="1">
+    <row r="255" ht="13.5" customHeight="1">
       <c r="A255" s="1"/>
       <c r="B255" s="1"/>
       <c r="C255" s="1"/>
@@ -8200,7 +8270,7 @@
       <c r="V255" s="1"/>
       <c r="W255" s="1"/>
     </row>
-    <row r="256" spans="1:23" ht="13.5" customHeight="1">
+    <row r="256" ht="13.5" customHeight="1">
       <c r="A256" s="1"/>
       <c r="B256" s="1"/>
       <c r="C256" s="1"/>
@@ -8225,7 +8295,7 @@
       <c r="V256" s="1"/>
       <c r="W256" s="1"/>
     </row>
-    <row r="257" spans="1:23" ht="13.5" customHeight="1">
+    <row r="257" ht="13.5" customHeight="1">
       <c r="A257" s="1"/>
       <c r="B257" s="1"/>
       <c r="C257" s="1"/>
@@ -8250,7 +8320,7 @@
       <c r="V257" s="1"/>
       <c r="W257" s="1"/>
     </row>
-    <row r="258" spans="1:23" ht="13.5" customHeight="1">
+    <row r="258" ht="13.5" customHeight="1">
       <c r="A258" s="1"/>
       <c r="B258" s="1"/>
       <c r="C258" s="1"/>
@@ -8275,7 +8345,7 @@
       <c r="V258" s="1"/>
       <c r="W258" s="1"/>
     </row>
-    <row r="259" spans="1:23" ht="13.5" customHeight="1">
+    <row r="259" ht="13.5" customHeight="1">
       <c r="A259" s="1"/>
       <c r="B259" s="1"/>
       <c r="C259" s="1"/>
@@ -8300,7 +8370,7 @@
       <c r="V259" s="1"/>
       <c r="W259" s="1"/>
     </row>
-    <row r="260" spans="1:23" ht="13.5" customHeight="1">
+    <row r="260" ht="13.5" customHeight="1">
       <c r="A260" s="1"/>
       <c r="B260" s="1"/>
       <c r="C260" s="1"/>
@@ -8325,7 +8395,7 @@
       <c r="V260" s="1"/>
       <c r="W260" s="1"/>
     </row>
-    <row r="261" spans="1:23" ht="13.5" customHeight="1">
+    <row r="261" ht="13.5" customHeight="1">
       <c r="A261" s="1"/>
       <c r="B261" s="1"/>
       <c r="C261" s="1"/>
@@ -8350,7 +8420,7 @@
       <c r="V261" s="1"/>
       <c r="W261" s="1"/>
     </row>
-    <row r="262" spans="1:23" ht="13.5" customHeight="1">
+    <row r="262" ht="13.5" customHeight="1">
       <c r="A262" s="1"/>
       <c r="B262" s="1"/>
       <c r="C262" s="1"/>
@@ -8375,7 +8445,7 @@
       <c r="V262" s="1"/>
       <c r="W262" s="1"/>
     </row>
-    <row r="263" spans="1:23" ht="13.5" customHeight="1">
+    <row r="263" ht="13.5" customHeight="1">
       <c r="A263" s="1"/>
       <c r="B263" s="1"/>
       <c r="C263" s="1"/>
@@ -8400,7 +8470,7 @@
       <c r="V263" s="1"/>
       <c r="W263" s="1"/>
     </row>
-    <row r="264" spans="1:23" ht="13.5" customHeight="1">
+    <row r="264" ht="13.5" customHeight="1">
       <c r="A264" s="1"/>
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
@@ -8425,7 +8495,7 @@
       <c r="V264" s="1"/>
       <c r="W264" s="1"/>
     </row>
-    <row r="265" spans="1:23" ht="13.5" customHeight="1">
+    <row r="265" ht="13.5" customHeight="1">
       <c r="A265" s="1"/>
       <c r="B265" s="1"/>
       <c r="C265" s="1"/>
@@ -8450,7 +8520,7 @@
       <c r="V265" s="1"/>
       <c r="W265" s="1"/>
     </row>
-    <row r="266" spans="1:23" ht="13.5" customHeight="1">
+    <row r="266" ht="13.5" customHeight="1">
       <c r="A266" s="1"/>
       <c r="B266" s="1"/>
       <c r="C266" s="1"/>
@@ -8475,7 +8545,7 @@
       <c r="V266" s="1"/>
       <c r="W266" s="1"/>
     </row>
-    <row r="267" spans="1:23" ht="13.5" customHeight="1">
+    <row r="267" ht="13.5" customHeight="1">
       <c r="A267" s="1"/>
       <c r="B267" s="1"/>
       <c r="C267" s="1"/>
@@ -8500,7 +8570,7 @@
       <c r="V267" s="1"/>
       <c r="W267" s="1"/>
     </row>
-    <row r="268" spans="1:23" ht="13.5" customHeight="1">
+    <row r="268" ht="13.5" customHeight="1">
       <c r="A268" s="1"/>
       <c r="B268" s="1"/>
       <c r="C268" s="1"/>
@@ -8525,7 +8595,7 @@
       <c r="V268" s="1"/>
       <c r="W268" s="1"/>
     </row>
-    <row r="269" spans="1:23" ht="13.5" customHeight="1">
+    <row r="269" ht="13.5" customHeight="1">
       <c r="A269" s="1"/>
       <c r="B269" s="1"/>
       <c r="C269" s="1"/>
@@ -8550,7 +8620,7 @@
       <c r="V269" s="1"/>
       <c r="W269" s="1"/>
     </row>
-    <row r="270" spans="1:23" ht="13.5" customHeight="1">
+    <row r="270" ht="13.5" customHeight="1">
       <c r="A270" s="1"/>
       <c r="B270" s="1"/>
       <c r="C270" s="1"/>
@@ -8575,7 +8645,7 @@
       <c r="V270" s="1"/>
       <c r="W270" s="1"/>
     </row>
-    <row r="271" spans="1:23" ht="13.5" customHeight="1">
+    <row r="271" ht="13.5" customHeight="1">
       <c r="A271" s="1"/>
       <c r="B271" s="1"/>
       <c r="C271" s="1"/>
@@ -8600,7 +8670,7 @@
       <c r="V271" s="1"/>
       <c r="W271" s="1"/>
     </row>
-    <row r="272" spans="1:23" ht="13.5" customHeight="1">
+    <row r="272" ht="13.5" customHeight="1">
       <c r="A272" s="1"/>
       <c r="B272" s="1"/>
       <c r="C272" s="1"/>
@@ -8625,7 +8695,7 @@
       <c r="V272" s="1"/>
       <c r="W272" s="1"/>
     </row>
-    <row r="273" spans="1:23" ht="13.5" customHeight="1">
+    <row r="273" ht="13.5" customHeight="1">
       <c r="A273" s="1"/>
       <c r="B273" s="1"/>
       <c r="C273" s="1"/>
@@ -8650,7 +8720,7 @@
       <c r="V273" s="1"/>
       <c r="W273" s="1"/>
     </row>
-    <row r="274" spans="1:23" ht="13.5" customHeight="1">
+    <row r="274" ht="13.5" customHeight="1">
       <c r="A274" s="1"/>
       <c r="B274" s="1"/>
       <c r="C274" s="1"/>
@@ -8675,7 +8745,7 @@
       <c r="V274" s="1"/>
       <c r="W274" s="1"/>
     </row>
-    <row r="275" spans="1:23" ht="13.5" customHeight="1">
+    <row r="275" ht="13.5" customHeight="1">
       <c r="A275" s="1"/>
       <c r="B275" s="1"/>
       <c r="C275" s="1"/>
@@ -8700,7 +8770,7 @@
       <c r="V275" s="1"/>
       <c r="W275" s="1"/>
     </row>
-    <row r="276" spans="1:23" ht="13.5" customHeight="1">
+    <row r="276" ht="13.5" customHeight="1">
       <c r="A276" s="1"/>
       <c r="B276" s="1"/>
       <c r="C276" s="1"/>
@@ -8725,7 +8795,7 @@
       <c r="V276" s="1"/>
       <c r="W276" s="1"/>
     </row>
-    <row r="277" spans="1:23" ht="13.5" customHeight="1">
+    <row r="277" ht="13.5" customHeight="1">
       <c r="A277" s="1"/>
       <c r="B277" s="1"/>
       <c r="C277" s="1"/>
@@ -8750,7 +8820,7 @@
       <c r="V277" s="1"/>
       <c r="W277" s="1"/>
     </row>
-    <row r="278" spans="1:23" ht="13.5" customHeight="1">
+    <row r="278" ht="13.5" customHeight="1">
       <c r="A278" s="1"/>
       <c r="B278" s="1"/>
       <c r="C278" s="1"/>
@@ -8775,7 +8845,7 @@
       <c r="V278" s="1"/>
       <c r="W278" s="1"/>
     </row>
-    <row r="279" spans="1:23" ht="13.5" customHeight="1">
+    <row r="279" ht="13.5" customHeight="1">
       <c r="A279" s="1"/>
       <c r="B279" s="1"/>
       <c r="C279" s="1"/>
@@ -8800,7 +8870,7 @@
       <c r="V279" s="1"/>
       <c r="W279" s="1"/>
     </row>
-    <row r="280" spans="1:23" ht="13.5" customHeight="1">
+    <row r="280" ht="13.5" customHeight="1">
       <c r="A280" s="1"/>
       <c r="B280" s="1"/>
       <c r="C280" s="1"/>
@@ -8825,7 +8895,7 @@
       <c r="V280" s="1"/>
       <c r="W280" s="1"/>
     </row>
-    <row r="281" spans="1:23" ht="13.5" customHeight="1">
+    <row r="281" ht="13.5" customHeight="1">
       <c r="A281" s="1"/>
       <c r="B281" s="1"/>
       <c r="C281" s="1"/>
@@ -8850,7 +8920,7 @@
       <c r="V281" s="1"/>
       <c r="W281" s="1"/>
     </row>
-    <row r="282" spans="1:23" ht="13.5" customHeight="1">
+    <row r="282" ht="13.5" customHeight="1">
       <c r="A282" s="1"/>
       <c r="B282" s="1"/>
       <c r="C282" s="1"/>
@@ -8875,7 +8945,7 @@
       <c r="V282" s="1"/>
       <c r="W282" s="1"/>
     </row>
-    <row r="283" spans="1:23" ht="13.5" customHeight="1">
+    <row r="283" ht="13.5" customHeight="1">
       <c r="A283" s="1"/>
       <c r="B283" s="1"/>
       <c r="C283" s="1"/>
@@ -8900,7 +8970,7 @@
       <c r="V283" s="1"/>
       <c r="W283" s="1"/>
     </row>
-    <row r="284" spans="1:23" ht="13.5" customHeight="1">
+    <row r="284" ht="13.5" customHeight="1">
       <c r="A284" s="1"/>
       <c r="B284" s="1"/>
       <c r="C284" s="1"/>
@@ -8925,7 +8995,7 @@
       <c r="V284" s="1"/>
       <c r="W284" s="1"/>
     </row>
-    <row r="285" spans="1:23" ht="13.5" customHeight="1">
+    <row r="285" ht="13.5" customHeight="1">
       <c r="A285" s="1"/>
       <c r="B285" s="1"/>
       <c r="C285" s="1"/>
@@ -8950,7 +9020,7 @@
       <c r="V285" s="1"/>
       <c r="W285" s="1"/>
     </row>
-    <row r="286" spans="1:23" ht="13.5" customHeight="1">
+    <row r="286" ht="13.5" customHeight="1">
       <c r="A286" s="1"/>
       <c r="B286" s="1"/>
       <c r="C286" s="1"/>
@@ -8975,7 +9045,7 @@
       <c r="V286" s="1"/>
       <c r="W286" s="1"/>
     </row>
-    <row r="287" spans="1:23" ht="13.5" customHeight="1">
+    <row r="287" ht="13.5" customHeight="1">
       <c r="A287" s="1"/>
       <c r="B287" s="1"/>
       <c r="C287" s="1"/>
@@ -9000,7 +9070,7 @@
       <c r="V287" s="1"/>
       <c r="W287" s="1"/>
     </row>
-    <row r="288" spans="1:23" ht="13.5" customHeight="1">
+    <row r="288" ht="13.5" customHeight="1">
       <c r="A288" s="1"/>
       <c r="B288" s="1"/>
       <c r="C288" s="1"/>
@@ -9025,7 +9095,7 @@
       <c r="V288" s="1"/>
       <c r="W288" s="1"/>
     </row>
-    <row r="289" spans="1:23" ht="13.5" customHeight="1">
+    <row r="289" ht="13.5" customHeight="1">
       <c r="A289" s="1"/>
       <c r="B289" s="1"/>
       <c r="C289" s="1"/>
@@ -9050,7 +9120,7 @@
       <c r="V289" s="1"/>
       <c r="W289" s="1"/>
     </row>
-    <row r="290" spans="1:23" ht="13.5" customHeight="1">
+    <row r="290" ht="13.5" customHeight="1">
       <c r="A290" s="1"/>
       <c r="B290" s="1"/>
       <c r="C290" s="1"/>
@@ -9075,7 +9145,7 @@
       <c r="V290" s="1"/>
       <c r="W290" s="1"/>
     </row>
-    <row r="291" spans="1:23" ht="13.5" customHeight="1">
+    <row r="291" ht="13.5" customHeight="1">
       <c r="A291" s="1"/>
       <c r="B291" s="1"/>
       <c r="C291" s="1"/>
@@ -9100,7 +9170,7 @@
       <c r="V291" s="1"/>
       <c r="W291" s="1"/>
     </row>
-    <row r="292" spans="1:23" ht="13.5" customHeight="1">
+    <row r="292" ht="13.5" customHeight="1">
       <c r="A292" s="1"/>
       <c r="B292" s="1"/>
       <c r="C292" s="1"/>
@@ -9125,7 +9195,7 @@
       <c r="V292" s="1"/>
       <c r="W292" s="1"/>
     </row>
-    <row r="293" spans="1:23" ht="13.5" customHeight="1">
+    <row r="293" ht="13.5" customHeight="1">
       <c r="A293" s="1"/>
       <c r="B293" s="1"/>
       <c r="C293" s="1"/>
@@ -9150,7 +9220,7 @@
       <c r="V293" s="1"/>
       <c r="W293" s="1"/>
     </row>
-    <row r="294" spans="1:23" ht="13.5" customHeight="1">
+    <row r="294" ht="13.5" customHeight="1">
       <c r="A294" s="1"/>
       <c r="B294" s="1"/>
       <c r="C294" s="1"/>
@@ -9175,7 +9245,7 @@
       <c r="V294" s="1"/>
       <c r="W294" s="1"/>
     </row>
-    <row r="295" spans="1:23" ht="13.5" customHeight="1">
+    <row r="295" ht="13.5" customHeight="1">
       <c r="A295" s="1"/>
       <c r="B295" s="1"/>
       <c r="C295" s="1"/>
@@ -9200,7 +9270,7 @@
       <c r="V295" s="1"/>
       <c r="W295" s="1"/>
     </row>
-    <row r="296" spans="1:23" ht="13.5" customHeight="1">
+    <row r="296" ht="13.5" customHeight="1">
       <c r="A296" s="1"/>
       <c r="B296" s="1"/>
       <c r="C296" s="1"/>
@@ -9225,7 +9295,7 @@
       <c r="V296" s="1"/>
       <c r="W296" s="1"/>
     </row>
-    <row r="297" spans="1:23" ht="13.5" customHeight="1">
+    <row r="297" ht="13.5" customHeight="1">
       <c r="A297" s="1"/>
       <c r="B297" s="1"/>
       <c r="C297" s="1"/>
@@ -9250,7 +9320,7 @@
       <c r="V297" s="1"/>
       <c r="W297" s="1"/>
     </row>
-    <row r="298" spans="1:23" ht="13.5" customHeight="1">
+    <row r="298" ht="13.5" customHeight="1">
       <c r="A298" s="1"/>
       <c r="B298" s="1"/>
       <c r="C298" s="1"/>
@@ -9275,7 +9345,7 @@
       <c r="V298" s="1"/>
       <c r="W298" s="1"/>
     </row>
-    <row r="299" spans="1:23" ht="13.5" customHeight="1">
+    <row r="299" ht="13.5" customHeight="1">
       <c r="A299" s="1"/>
       <c r="B299" s="1"/>
       <c r="C299" s="1"/>
@@ -9300,7 +9370,7 @@
       <c r="V299" s="1"/>
       <c r="W299" s="1"/>
     </row>
-    <row r="300" spans="1:23" ht="13.5" customHeight="1">
+    <row r="300" ht="13.5" customHeight="1">
       <c r="A300" s="1"/>
       <c r="B300" s="1"/>
       <c r="C300" s="1"/>
@@ -9325,7 +9395,7 @@
       <c r="V300" s="1"/>
       <c r="W300" s="1"/>
     </row>
-    <row r="301" spans="1:23" ht="13.5" customHeight="1">
+    <row r="301" ht="13.5" customHeight="1">
       <c r="A301" s="1"/>
       <c r="B301" s="1"/>
       <c r="C301" s="1"/>
@@ -9350,7 +9420,7 @@
       <c r="V301" s="1"/>
       <c r="W301" s="1"/>
     </row>
-    <row r="302" spans="1:23" ht="13.5" customHeight="1">
+    <row r="302" ht="13.5" customHeight="1">
       <c r="A302" s="1"/>
       <c r="B302" s="1"/>
       <c r="C302" s="1"/>
@@ -9375,7 +9445,7 @@
       <c r="V302" s="1"/>
       <c r="W302" s="1"/>
     </row>
-    <row r="303" spans="1:23" ht="13.5" customHeight="1">
+    <row r="303" ht="13.5" customHeight="1">
       <c r="A303" s="1"/>
       <c r="B303" s="1"/>
       <c r="C303" s="1"/>
@@ -9400,7 +9470,7 @@
       <c r="V303" s="1"/>
       <c r="W303" s="1"/>
     </row>
-    <row r="304" spans="1:23" ht="13.5" customHeight="1">
+    <row r="304" ht="13.5" customHeight="1">
       <c r="A304" s="1"/>
       <c r="B304" s="1"/>
       <c r="C304" s="1"/>
@@ -9425,7 +9495,7 @@
       <c r="V304" s="1"/>
       <c r="W304" s="1"/>
     </row>
-    <row r="305" spans="1:23" ht="13.5" customHeight="1">
+    <row r="305" ht="13.5" customHeight="1">
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
       <c r="C305" s="1"/>
@@ -9450,7 +9520,7 @@
       <c r="V305" s="1"/>
       <c r="W305" s="1"/>
     </row>
-    <row r="306" spans="1:23" ht="13.5" customHeight="1">
+    <row r="306" ht="13.5" customHeight="1">
       <c r="A306" s="1"/>
       <c r="B306" s="1"/>
       <c r="C306" s="1"/>
@@ -9475,7 +9545,7 @@
       <c r="V306" s="1"/>
       <c r="W306" s="1"/>
     </row>
-    <row r="307" spans="1:23" ht="13.5" customHeight="1">
+    <row r="307" ht="13.5" customHeight="1">
       <c r="A307" s="1"/>
       <c r="B307" s="1"/>
       <c r="C307" s="1"/>
@@ -9500,7 +9570,7 @@
       <c r="V307" s="1"/>
       <c r="W307" s="1"/>
     </row>
-    <row r="308" spans="1:23" ht="13.5" customHeight="1">
+    <row r="308" ht="13.5" customHeight="1">
       <c r="A308" s="1"/>
       <c r="B308" s="1"/>
       <c r="C308" s="1"/>
@@ -9525,7 +9595,7 @@
       <c r="V308" s="1"/>
       <c r="W308" s="1"/>
     </row>
-    <row r="309" spans="1:23" ht="13.5" customHeight="1">
+    <row r="309" ht="13.5" customHeight="1">
       <c r="A309" s="1"/>
       <c r="B309" s="1"/>
       <c r="C309" s="1"/>
@@ -9550,7 +9620,7 @@
       <c r="V309" s="1"/>
       <c r="W309" s="1"/>
     </row>
-    <row r="310" spans="1:23" ht="13.5" customHeight="1">
+    <row r="310" ht="13.5" customHeight="1">
       <c r="A310" s="1"/>
       <c r="B310" s="1"/>
       <c r="C310" s="1"/>
@@ -9575,7 +9645,7 @@
       <c r="V310" s="1"/>
       <c r="W310" s="1"/>
     </row>
-    <row r="311" spans="1:23" ht="13.5" customHeight="1">
+    <row r="311" ht="13.5" customHeight="1">
       <c r="A311" s="1"/>
       <c r="B311" s="1"/>
       <c r="C311" s="1"/>
@@ -9600,7 +9670,7 @@
       <c r="V311" s="1"/>
       <c r="W311" s="1"/>
     </row>
-    <row r="312" spans="1:23" ht="13.5" customHeight="1">
+    <row r="312" ht="13.5" customHeight="1">
       <c r="A312" s="1"/>
       <c r="B312" s="1"/>
       <c r="C312" s="1"/>
@@ -9625,7 +9695,7 @@
       <c r="V312" s="1"/>
       <c r="W312" s="1"/>
     </row>
-    <row r="313" spans="1:23" ht="13.5" customHeight="1">
+    <row r="313" ht="13.5" customHeight="1">
       <c r="A313" s="1"/>
       <c r="B313" s="1"/>
       <c r="C313" s="1"/>
@@ -9650,7 +9720,7 @@
       <c r="V313" s="1"/>
       <c r="W313" s="1"/>
     </row>
-    <row r="314" spans="1:23" ht="13.5" customHeight="1">
+    <row r="314" ht="13.5" customHeight="1">
       <c r="A314" s="1"/>
       <c r="B314" s="1"/>
       <c r="C314" s="1"/>
@@ -9675,7 +9745,7 @@
       <c r="V314" s="1"/>
       <c r="W314" s="1"/>
     </row>
-    <row r="315" spans="1:23" ht="13.5" customHeight="1">
+    <row r="315" ht="13.5" customHeight="1">
       <c r="A315" s="1"/>
       <c r="B315" s="1"/>
       <c r="C315" s="1"/>
@@ -9700,7 +9770,7 @@
       <c r="V315" s="1"/>
       <c r="W315" s="1"/>
     </row>
-    <row r="316" spans="1:23" ht="13.5" customHeight="1">
+    <row r="316" ht="13.5" customHeight="1">
       <c r="A316" s="1"/>
       <c r="B316" s="1"/>
       <c r="C316" s="1"/>
@@ -9725,7 +9795,7 @@
       <c r="V316" s="1"/>
       <c r="W316" s="1"/>
     </row>
-    <row r="317" spans="1:23" ht="13.5" customHeight="1">
+    <row r="317" ht="13.5" customHeight="1">
       <c r="A317" s="1"/>
       <c r="B317" s="1"/>
       <c r="C317" s="1"/>
@@ -9750,7 +9820,7 @@
       <c r="V317" s="1"/>
       <c r="W317" s="1"/>
     </row>
-    <row r="318" spans="1:23" ht="13.5" customHeight="1">
+    <row r="318" ht="13.5" customHeight="1">
       <c r="A318" s="1"/>
       <c r="B318" s="1"/>
       <c r="C318" s="1"/>
@@ -9775,7 +9845,7 @@
       <c r="V318" s="1"/>
       <c r="W318" s="1"/>
     </row>
-    <row r="319" spans="1:23" ht="13.5" customHeight="1">
+    <row r="319" ht="13.5" customHeight="1">
       <c r="A319" s="1"/>
       <c r="B319" s="1"/>
       <c r="C319" s="1"/>
@@ -9800,7 +9870,7 @@
       <c r="V319" s="1"/>
       <c r="W319" s="1"/>
     </row>
-    <row r="320" spans="1:23" ht="13.5" customHeight="1">
+    <row r="320" ht="13.5" customHeight="1">
       <c r="A320" s="1"/>
       <c r="B320" s="1"/>
       <c r="C320" s="1"/>
@@ -9825,7 +9895,7 @@
       <c r="V320" s="1"/>
       <c r="W320" s="1"/>
     </row>
-    <row r="321" spans="1:23" ht="13.5" customHeight="1">
+    <row r="321" ht="13.5" customHeight="1">
       <c r="A321" s="1"/>
       <c r="B321" s="1"/>
       <c r="C321" s="1"/>
@@ -9850,7 +9920,7 @@
       <c r="V321" s="1"/>
       <c r="W321" s="1"/>
     </row>
-    <row r="322" spans="1:23" ht="13.5" customHeight="1">
+    <row r="322" ht="13.5" customHeight="1">
       <c r="A322" s="1"/>
       <c r="B322" s="1"/>
       <c r="C322" s="1"/>
@@ -9875,7 +9945,7 @@
       <c r="V322" s="1"/>
       <c r="W322" s="1"/>
     </row>
-    <row r="323" spans="1:23" ht="13.5" customHeight="1">
+    <row r="323" ht="13.5" customHeight="1">
       <c r="A323" s="1"/>
       <c r="B323" s="1"/>
       <c r="C323" s="1"/>
@@ -9900,7 +9970,7 @@
       <c r="V323" s="1"/>
       <c r="W323" s="1"/>
     </row>
-    <row r="324" spans="1:23" ht="13.5" customHeight="1">
+    <row r="324" ht="13.5" customHeight="1">
       <c r="A324" s="1"/>
       <c r="B324" s="1"/>
       <c r="C324" s="1"/>
@@ -9925,7 +9995,7 @@
       <c r="V324" s="1"/>
       <c r="W324" s="1"/>
     </row>
-    <row r="325" spans="1:23" ht="13.5" customHeight="1">
+    <row r="325" ht="13.5" customHeight="1">
       <c r="A325" s="1"/>
       <c r="B325" s="1"/>
       <c r="C325" s="1"/>
@@ -9950,7 +10020,7 @@
       <c r="V325" s="1"/>
       <c r="W325" s="1"/>
     </row>
-    <row r="326" spans="1:23" ht="13.5" customHeight="1">
+    <row r="326" ht="13.5" customHeight="1">
       <c r="A326" s="1"/>
       <c r="B326" s="1"/>
       <c r="C326" s="1"/>
@@ -9975,7 +10045,7 @@
       <c r="V326" s="1"/>
       <c r="W326" s="1"/>
     </row>
-    <row r="327" spans="1:23" ht="13.5" customHeight="1">
+    <row r="327" ht="13.5" customHeight="1">
       <c r="A327" s="1"/>
       <c r="B327" s="1"/>
       <c r="C327" s="1"/>
@@ -10000,7 +10070,7 @@
       <c r="V327" s="1"/>
       <c r="W327" s="1"/>
     </row>
-    <row r="328" spans="1:23" ht="13.5" customHeight="1">
+    <row r="328" ht="13.5" customHeight="1">
       <c r="A328" s="1"/>
       <c r="B328" s="1"/>
       <c r="C328" s="1"/>
@@ -10025,7 +10095,7 @@
       <c r="V328" s="1"/>
       <c r="W328" s="1"/>
     </row>
-    <row r="329" spans="1:23" ht="13.5" customHeight="1">
+    <row r="329" ht="13.5" customHeight="1">
       <c r="A329" s="1"/>
       <c r="B329" s="1"/>
       <c r="C329" s="1"/>
@@ -10050,7 +10120,7 @@
       <c r="V329" s="1"/>
       <c r="W329" s="1"/>
     </row>
-    <row r="330" spans="1:23" ht="13.5" customHeight="1">
+    <row r="330" ht="13.5" customHeight="1">
       <c r="A330" s="1"/>
       <c r="B330" s="1"/>
       <c r="C330" s="1"/>
@@ -10075,7 +10145,7 @@
       <c r="V330" s="1"/>
       <c r="W330" s="1"/>
     </row>
-    <row r="331" spans="1:23" ht="13.5" customHeight="1">
+    <row r="331" ht="13.5" customHeight="1">
       <c r="A331" s="1"/>
       <c r="B331" s="1"/>
       <c r="C331" s="1"/>
@@ -10100,7 +10170,7 @@
       <c r="V331" s="1"/>
       <c r="W331" s="1"/>
     </row>
-    <row r="332" spans="1:23" ht="13.5" customHeight="1">
+    <row r="332" ht="13.5" customHeight="1">
       <c r="A332" s="1"/>
       <c r="B332" s="1"/>
       <c r="C332" s="1"/>
@@ -10125,7 +10195,7 @@
       <c r="V332" s="1"/>
       <c r="W332" s="1"/>
     </row>
-    <row r="333" spans="1:23" ht="13.5" customHeight="1">
+    <row r="333" ht="13.5" customHeight="1">
       <c r="A333" s="1"/>
       <c r="B333" s="1"/>
       <c r="C333" s="1"/>
@@ -10150,7 +10220,7 @@
       <c r="V333" s="1"/>
       <c r="W333" s="1"/>
     </row>
-    <row r="334" spans="1:23" ht="13.5" customHeight="1">
+    <row r="334" ht="13.5" customHeight="1">
       <c r="A334" s="1"/>
       <c r="B334" s="1"/>
       <c r="C334" s="1"/>
@@ -10175,7 +10245,7 @@
       <c r="V334" s="1"/>
       <c r="W334" s="1"/>
     </row>
-    <row r="335" spans="1:23" ht="13.5" customHeight="1">
+    <row r="335" ht="13.5" customHeight="1">
       <c r="A335" s="1"/>
       <c r="B335" s="1"/>
       <c r="C335" s="1"/>
@@ -10200,7 +10270,7 @@
       <c r="V335" s="1"/>
       <c r="W335" s="1"/>
     </row>
-    <row r="336" spans="1:23" ht="13.5" customHeight="1">
+    <row r="336" ht="13.5" customHeight="1">
       <c r="A336" s="1"/>
       <c r="B336" s="1"/>
       <c r="C336" s="1"/>
@@ -10225,7 +10295,7 @@
       <c r="V336" s="1"/>
       <c r="W336" s="1"/>
     </row>
-    <row r="337" spans="1:23" ht="13.5" customHeight="1">
+    <row r="337" ht="13.5" customHeight="1">
       <c r="A337" s="1"/>
       <c r="B337" s="1"/>
       <c r="C337" s="1"/>
@@ -10250,7 +10320,7 @@
       <c r="V337" s="1"/>
       <c r="W337" s="1"/>
     </row>
-    <row r="338" spans="1:23" ht="13.5" customHeight="1">
+    <row r="338" ht="13.5" customHeight="1">
       <c r="A338" s="1"/>
       <c r="B338" s="1"/>
       <c r="C338" s="1"/>
@@ -10275,7 +10345,7 @@
       <c r="V338" s="1"/>
       <c r="W338" s="1"/>
     </row>
-    <row r="339" spans="1:23" ht="13.5" customHeight="1">
+    <row r="339" ht="13.5" customHeight="1">
       <c r="A339" s="1"/>
       <c r="B339" s="1"/>
       <c r="C339" s="1"/>
@@ -10300,7 +10370,7 @@
       <c r="V339" s="1"/>
       <c r="W339" s="1"/>
     </row>
-    <row r="340" spans="1:23" ht="13.5" customHeight="1">
+    <row r="340" ht="13.5" customHeight="1">
       <c r="A340" s="1"/>
       <c r="B340" s="1"/>
       <c r="C340" s="1"/>
@@ -10325,7 +10395,7 @@
       <c r="V340" s="1"/>
       <c r="W340" s="1"/>
     </row>
-    <row r="341" spans="1:23" ht="13.5" customHeight="1">
+    <row r="341" ht="13.5" customHeight="1">
       <c r="A341" s="1"/>
       <c r="B341" s="1"/>
       <c r="C341" s="1"/>
@@ -10350,7 +10420,7 @@
       <c r="V341" s="1"/>
       <c r="W341" s="1"/>
     </row>
-    <row r="342" spans="1:23" ht="13.5" customHeight="1">
+    <row r="342" ht="13.5" customHeight="1">
       <c r="A342" s="1"/>
       <c r="B342" s="1"/>
       <c r="C342" s="1"/>
@@ -10375,7 +10445,7 @@
       <c r="V342" s="1"/>
       <c r="W342" s="1"/>
     </row>
-    <row r="343" spans="1:23" ht="13.5" customHeight="1">
+    <row r="343" ht="13.5" customHeight="1">
       <c r="A343" s="1"/>
       <c r="B343" s="1"/>
       <c r="C343" s="1"/>
@@ -10400,7 +10470,7 @@
       <c r="V343" s="1"/>
       <c r="W343" s="1"/>
     </row>
-    <row r="344" spans="1:23" ht="13.5" customHeight="1">
+    <row r="344" ht="13.5" customHeight="1">
       <c r="A344" s="1"/>
       <c r="B344" s="1"/>
       <c r="C344" s="1"/>
@@ -10425,7 +10495,7 @@
       <c r="V344" s="1"/>
       <c r="W344" s="1"/>
     </row>
-    <row r="345" spans="1:23" ht="13.5" customHeight="1">
+    <row r="345" ht="13.5" customHeight="1">
       <c r="A345" s="1"/>
       <c r="B345" s="1"/>
       <c r="C345" s="1"/>
@@ -10450,7 +10520,7 @@
       <c r="V345" s="1"/>
       <c r="W345" s="1"/>
     </row>
-    <row r="346" spans="1:23" ht="13.5" customHeight="1">
+    <row r="346" ht="13.5" customHeight="1">
       <c r="A346" s="1"/>
       <c r="B346" s="1"/>
       <c r="C346" s="1"/>
@@ -10475,7 +10545,7 @@
       <c r="V346" s="1"/>
       <c r="W346" s="1"/>
     </row>
-    <row r="347" spans="1:23" ht="13.5" customHeight="1">
+    <row r="347" ht="13.5" customHeight="1">
       <c r="A347" s="1"/>
       <c r="B347" s="1"/>
       <c r="C347" s="1"/>
@@ -10500,7 +10570,7 @@
       <c r="V347" s="1"/>
       <c r="W347" s="1"/>
     </row>
-    <row r="348" spans="1:23" ht="13.5" customHeight="1">
+    <row r="348" ht="13.5" customHeight="1">
       <c r="A348" s="1"/>
       <c r="B348" s="1"/>
       <c r="C348" s="1"/>
@@ -10525,7 +10595,7 @@
       <c r="V348" s="1"/>
       <c r="W348" s="1"/>
     </row>
-    <row r="349" spans="1:23" ht="13.5" customHeight="1">
+    <row r="349" ht="13.5" customHeight="1">
       <c r="A349" s="1"/>
       <c r="B349" s="1"/>
       <c r="C349" s="1"/>
@@ -10550,7 +10620,7 @@
       <c r="V349" s="1"/>
       <c r="W349" s="1"/>
     </row>
-    <row r="350" spans="1:23" ht="13.5" customHeight="1">
+    <row r="350" ht="13.5" customHeight="1">
       <c r="A350" s="1"/>
       <c r="B350" s="1"/>
       <c r="C350" s="1"/>
@@ -10575,7 +10645,7 @@
       <c r="V350" s="1"/>
       <c r="W350" s="1"/>
     </row>
-    <row r="351" spans="1:23" ht="13.5" customHeight="1">
+    <row r="351" ht="13.5" customHeight="1">
       <c r="A351" s="1"/>
       <c r="B351" s="1"/>
       <c r="C351" s="1"/>
@@ -10600,7 +10670,7 @@
       <c r="V351" s="1"/>
       <c r="W351" s="1"/>
     </row>
-    <row r="352" spans="1:23" ht="13.5" customHeight="1">
+    <row r="352" ht="13.5" customHeight="1">
       <c r="A352" s="1"/>
       <c r="B352" s="1"/>
       <c r="C352" s="1"/>
@@ -11275,16 +11345,18 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="B38" r:id="rId5"/>
-    <hyperlink ref="C38" r:id="rId6"/>
-    <hyperlink ref="B75" r:id="rId7"/>
-    <hyperlink ref="C75" r:id="rId8"/>
+    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink r:id="rId2" ref="C2"/>
+    <hyperlink r:id="rId3" ref="B3"/>
+    <hyperlink r:id="rId4" ref="C3"/>
+    <hyperlink r:id="rId5" ref="B38"/>
+    <hyperlink r:id="rId6" ref="C38"/>
+    <hyperlink r:id="rId7" ref="B75"/>
+    <hyperlink r:id="rId8" ref="C75"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
27-6-2022 Appointments Latest updates.
By,
Patrick
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Patrick-Codoid\Naveen\Appointments_Updated\config\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="MMH" sheetId="1" r:id="rId4"/>
+    <sheet name="MMH" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="247">
   <si>
     <t>KEY</t>
   </si>
@@ -749,78 +757,73 @@
   </si>
   <si>
     <t>daisy@mmh-demo.com</t>
+  </si>
+  <si>
+    <t>APPOINTMENT_DETAILS_FOR_JOIN_VIDEO_CONSULTATION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Verdana"/>
     </font>
     <font>
       <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
@@ -830,7 +833,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -840,7 +843,13 @@
     </fill>
   </fills>
   <borders count="4">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FFCCCCCC"/>
@@ -854,6 +863,7 @@
       <bottom style="medium">
         <color rgb="FFCCCCCC"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -868,6 +878,7 @@
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -882,85 +893,74 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="3" fillId="2" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1150,26 +1150,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="69.57"/>
-    <col customWidth="1" min="2" max="2" width="157.14"/>
-    <col customWidth="1" min="3" max="3" width="125.14"/>
-    <col customWidth="1" min="4" max="23" width="8.86"/>
+    <col min="1" max="1" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="157.140625" customWidth="1"/>
+    <col min="3" max="3" width="125.140625" customWidth="1"/>
+    <col min="4" max="23" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customHeight="1">
+    <row r="1" spans="1:23" ht="13.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1202,7 @@
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
     </row>
-    <row r="2" ht="13.5" customHeight="1">
+    <row r="2" spans="1:23" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1231,7 +1233,7 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
     </row>
-    <row r="3" ht="13.5" customHeight="1">
+    <row r="3" spans="1:23" ht="13.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1262,7 +1264,7 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" ht="13.5" customHeight="1">
+    <row r="4" spans="1:23" ht="13.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1295,7 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
     </row>
-    <row r="5" ht="13.5" customHeight="1">
+    <row r="5" spans="1:23" ht="13.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1324,7 +1326,7 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
     </row>
-    <row r="6" ht="13.5" customHeight="1">
+    <row r="6" spans="1:23" ht="13.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1355,7 +1357,7 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
     </row>
-    <row r="7" ht="13.5" customHeight="1">
+    <row r="7" spans="1:23" ht="13.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1386,7 +1388,7 @@
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
     </row>
-    <row r="8" ht="13.5" customHeight="1">
+    <row r="8" spans="1:23" ht="13.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1415,7 +1417,7 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
     </row>
-    <row r="9" ht="13.5" customHeight="1">
+    <row r="9" spans="1:23" ht="13.5" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1440,7 +1442,7 @@
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
     </row>
-    <row r="10" ht="13.5" customHeight="1">
+    <row r="10" spans="1:23" ht="13.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1471,7 +1473,7 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
     </row>
-    <row r="11" ht="13.5" customHeight="1">
+    <row r="11" spans="1:23" ht="13.5" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1502,7 +1504,7 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
     </row>
-    <row r="12" ht="13.5" customHeight="1">
+    <row r="12" spans="1:23" ht="13.5" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1533,7 +1535,7 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
     </row>
-    <row r="13" ht="13.5" customHeight="1">
+    <row r="13" spans="1:23" ht="13.5" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1562,7 +1564,7 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
     </row>
-    <row r="14" ht="13.5" customHeight="1">
+    <row r="14" spans="1:23" ht="13.5" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1587,7 +1589,7 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" ht="13.5" customHeight="1">
+    <row r="15" spans="1:23" ht="13.5" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1618,7 +1620,7 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" ht="13.5" customHeight="1">
+    <row r="16" spans="1:23" ht="13.5" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -1649,7 +1651,7 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" ht="13.5" customHeight="1">
+    <row r="17" spans="1:23" ht="13.5" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1680,7 +1682,7 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
     </row>
-    <row r="18" ht="13.5" customHeight="1">
+    <row r="18" spans="1:23" ht="13.5" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1709,7 +1711,7 @@
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
     </row>
-    <row r="19" ht="13.5" customHeight="1">
+    <row r="19" spans="1:23" ht="13.5" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1734,7 +1736,7 @@
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
     </row>
-    <row r="20" ht="13.5" customHeight="1">
+    <row r="20" spans="1:23" ht="13.5" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1765,7 +1767,7 @@
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
     </row>
-    <row r="21" ht="13.5" customHeight="1">
+    <row r="21" spans="1:23" ht="13.5" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -1796,7 +1798,7 @@
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
     </row>
-    <row r="22" ht="13.5" customHeight="1">
+    <row r="22" spans="1:23" ht="13.5" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1827,7 +1829,7 @@
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
     </row>
-    <row r="23" ht="13.5" customHeight="1">
+    <row r="23" spans="1:23" ht="13.5" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1856,7 +1858,7 @@
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
     </row>
-    <row r="24" ht="13.5" customHeight="1">
+    <row r="24" spans="1:23" ht="13.5" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1881,7 +1883,7 @@
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
     </row>
-    <row r="25" ht="13.5" customHeight="1">
+    <row r="25" spans="1:23" ht="13.5" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1912,7 +1914,7 @@
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
     </row>
-    <row r="26" ht="13.5" customHeight="1">
+    <row r="26" spans="1:23" ht="13.5" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1943,7 +1945,7 @@
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
     </row>
-    <row r="27" ht="13.5" customHeight="1">
+    <row r="27" spans="1:23" ht="13.5" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -1974,7 +1976,7 @@
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
     </row>
-    <row r="28" ht="13.5" customHeight="1">
+    <row r="28" spans="1:23" ht="13.5" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
@@ -2005,7 +2007,7 @@
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
     </row>
-    <row r="29" ht="13.5" customHeight="1">
+    <row r="29" spans="1:23" ht="13.5" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
@@ -2034,7 +2036,7 @@
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
     </row>
-    <row r="30" ht="13.5" customHeight="1">
+    <row r="30" spans="1:23" ht="13.5" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2059,7 +2061,7 @@
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
     </row>
-    <row r="31" ht="13.5" customHeight="1">
+    <row r="31" spans="1:23" ht="13.5" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -2090,7 +2092,7 @@
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
     </row>
-    <row r="32" ht="13.5" customHeight="1">
+    <row r="32" spans="1:23" ht="13.5" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2121,7 +2123,7 @@
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
     </row>
-    <row r="33" ht="13.5" customHeight="1">
+    <row r="33" spans="1:23" ht="13.5" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2146,7 +2148,7 @@
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
     </row>
-    <row r="34" ht="13.5" customHeight="1">
+    <row r="34" spans="1:23" ht="13.5" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
@@ -2177,7 +2179,7 @@
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
     </row>
-    <row r="35" ht="13.5" customHeight="1">
+    <row r="35" spans="1:23" ht="13.5" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2202,9 +2204,13 @@
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
     </row>
-    <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
+    <row r="36" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A36" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -2227,7 +2233,7 @@
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
     </row>
-    <row r="37" ht="13.5" customHeight="1">
+    <row r="37" spans="1:23" ht="13.5" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2252,14 +2258,14 @@
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
     </row>
-    <row r="38" ht="13.5" customHeight="1">
+    <row r="38" spans="1:23" ht="13.5" customHeight="1">
       <c r="A38" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="18" t="s">
         <v>50</v>
       </c>
       <c r="D38" s="1"/>
@@ -2283,14 +2289,14 @@
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
     </row>
-    <row r="39" ht="13.5" customHeight="1">
+    <row r="39" spans="1:23" ht="13.5" customHeight="1">
       <c r="A39" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="1"/>
@@ -2314,7 +2320,7 @@
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
     </row>
-    <row r="40" ht="13.5" customHeight="1">
+    <row r="40" spans="1:23" ht="13.5" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2339,8 +2345,8 @@
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
     </row>
-    <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" s="8" t="s">
+    <row r="41" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A41" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -2370,8 +2376,8 @@
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
     </row>
-    <row r="42" ht="13.5" customHeight="1">
-      <c r="A42" s="8" t="s">
+    <row r="42" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A42" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -2401,8 +2407,8 @@
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
     </row>
-    <row r="43" ht="13.5" customHeight="1">
-      <c r="A43" s="8" t="s">
+    <row r="43" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A43" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -2432,8 +2438,8 @@
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
     </row>
-    <row r="44" ht="13.5" customHeight="1">
-      <c r="A44" s="8"/>
+    <row r="44" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A44" s="7"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="1"/>
@@ -2457,8 +2463,8 @@
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
     </row>
-    <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="8"/>
+    <row r="45" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A45" s="7"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="1"/>
@@ -2482,8 +2488,8 @@
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
     </row>
-    <row r="46" ht="13.5" customHeight="1">
-      <c r="A46" s="8" t="s">
+    <row r="46" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A46" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -2513,8 +2519,8 @@
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
     </row>
-    <row r="47" ht="13.5" customHeight="1">
-      <c r="A47" s="8" t="s">
+    <row r="47" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A47" s="7" t="s">
         <v>60</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -2544,8 +2550,8 @@
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
     </row>
-    <row r="48" ht="13.5" customHeight="1">
-      <c r="A48" s="8" t="s">
+    <row r="48" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A48" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B48" s="5"/>
@@ -2571,8 +2577,8 @@
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
     </row>
-    <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="8"/>
+    <row r="49" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A49" s="7"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="1"/>
@@ -2596,8 +2602,8 @@
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
     </row>
-    <row r="50" ht="13.5" customHeight="1">
-      <c r="A50" s="8"/>
+    <row r="50" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A50" s="7"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="1"/>
@@ -2621,8 +2627,8 @@
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
     </row>
-    <row r="51" ht="13.5" customHeight="1">
-      <c r="A51" s="8" t="s">
+    <row r="51" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A51" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -2652,8 +2658,8 @@
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
     </row>
-    <row r="52" ht="13.5" customHeight="1">
-      <c r="A52" s="8" t="s">
+    <row r="52" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A52" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -2683,12 +2689,12 @@
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
     </row>
-    <row r="53" ht="13.5" customHeight="1">
-      <c r="A53" s="8" t="s">
+    <row r="53" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A53" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2710,8 +2716,8 @@
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
     </row>
-    <row r="54" ht="13.5" customHeight="1">
-      <c r="A54" s="8"/>
+    <row r="54" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A54" s="7"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="1"/>
@@ -2735,8 +2741,8 @@
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
     </row>
-    <row r="55" ht="13.5" customHeight="1">
-      <c r="A55" s="8"/>
+    <row r="55" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A55" s="7"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="1"/>
@@ -2760,8 +2766,8 @@
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
     </row>
-    <row r="56" ht="13.5" customHeight="1">
-      <c r="A56" s="8" t="s">
+    <row r="56" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A56" s="7" t="s">
         <v>68</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -2791,8 +2797,8 @@
       <c r="V56" s="1"/>
       <c r="W56" s="1"/>
     </row>
-    <row r="57" ht="13.5" customHeight="1">
-      <c r="A57" s="8" t="s">
+    <row r="57" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A57" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -2822,8 +2828,8 @@
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
     </row>
-    <row r="58" ht="13.5" customHeight="1">
-      <c r="A58" s="8" t="s">
+    <row r="58" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A58" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B58" s="5"/>
@@ -2849,8 +2855,8 @@
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
     </row>
-    <row r="59" ht="13.5" customHeight="1">
-      <c r="A59" s="8"/>
+    <row r="59" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A59" s="7"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="1"/>
@@ -2874,8 +2880,8 @@
       <c r="V59" s="1"/>
       <c r="W59" s="1"/>
     </row>
-    <row r="60" ht="13.5" customHeight="1">
-      <c r="A60" s="8"/>
+    <row r="60" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A60" s="7"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="1"/>
@@ -2899,8 +2905,8 @@
       <c r="V60" s="1"/>
       <c r="W60" s="1"/>
     </row>
-    <row r="61" ht="13.5" customHeight="1">
-      <c r="A61" s="8" t="s">
+    <row r="61" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A61" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -2930,8 +2936,8 @@
       <c r="V61" s="1"/>
       <c r="W61" s="1"/>
     </row>
-    <row r="62" ht="13.5" customHeight="1">
-      <c r="A62" s="8" t="s">
+    <row r="62" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A62" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B62" s="5" t="s">
@@ -2961,8 +2967,8 @@
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
     </row>
-    <row r="63" ht="13.5" customHeight="1">
-      <c r="A63" s="8"/>
+    <row r="63" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A63" s="7"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="1"/>
@@ -2986,8 +2992,8 @@
       <c r="V63" s="1"/>
       <c r="W63" s="1"/>
     </row>
-    <row r="64" ht="13.5" customHeight="1">
-      <c r="A64" s="8"/>
+    <row r="64" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A64" s="7"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="1"/>
@@ -3011,8 +3017,8 @@
       <c r="V64" s="1"/>
       <c r="W64" s="1"/>
     </row>
-    <row r="65" ht="13.5" customHeight="1">
-      <c r="A65" s="8" t="s">
+    <row r="65" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A65" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B65" s="5" t="s">
@@ -3042,8 +3048,8 @@
       <c r="V65" s="1"/>
       <c r="W65" s="1"/>
     </row>
-    <row r="66" ht="13.5" customHeight="1">
-      <c r="A66" s="8" t="s">
+    <row r="66" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A66" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B66" s="5" t="s">
@@ -3073,8 +3079,8 @@
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
     </row>
-    <row r="67" ht="13.5" customHeight="1">
-      <c r="A67" s="8"/>
+    <row r="67" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A67" s="7"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="1"/>
@@ -3098,8 +3104,8 @@
       <c r="V67" s="1"/>
       <c r="W67" s="1"/>
     </row>
-    <row r="68" ht="13.5" customHeight="1">
-      <c r="A68" s="8"/>
+    <row r="68" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A68" s="7"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="1"/>
@@ -3123,8 +3129,8 @@
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
     </row>
-    <row r="69" ht="13.5" customHeight="1">
-      <c r="A69" s="8" t="s">
+    <row r="69" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A69" s="7" t="s">
         <v>77</v>
       </c>
       <c r="B69" s="5" t="s">
@@ -3154,8 +3160,8 @@
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
     </row>
-    <row r="70" ht="13.5" customHeight="1">
-      <c r="A70" s="8" t="s">
+    <row r="70" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A70" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B70" s="5" t="s">
@@ -3185,8 +3191,8 @@
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
     </row>
-    <row r="71" ht="13.5" customHeight="1">
-      <c r="A71" s="8" t="s">
+    <row r="71" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A71" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B71" s="5" t="s">
@@ -3216,7 +3222,7 @@
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
     </row>
-    <row r="72" ht="13.5" customHeight="1">
+    <row r="72" spans="1:23" ht="13.5" customHeight="1">
       <c r="A72" s="5" t="s">
         <v>83</v>
       </c>
@@ -3247,7 +3253,7 @@
       <c r="V72" s="1"/>
       <c r="W72" s="1"/>
     </row>
-    <row r="73" ht="13.5" customHeight="1">
+    <row r="73" spans="1:23" ht="13.5" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -3272,7 +3278,7 @@
       <c r="V73" s="1"/>
       <c r="W73" s="1"/>
     </row>
-    <row r="74" ht="13.5" customHeight="1">
+    <row r="74" spans="1:23" ht="13.5" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3297,14 +3303,14 @@
       <c r="V74" s="1"/>
       <c r="W74" s="1"/>
     </row>
-    <row r="75" ht="13.5" customHeight="1">
-      <c r="A75" s="10" t="s">
+    <row r="75" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A75" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C75" s="18" t="s">
         <v>50</v>
       </c>
       <c r="D75" s="1"/>
@@ -3328,14 +3334,14 @@
       <c r="V75" s="1"/>
       <c r="W75" s="1"/>
     </row>
-    <row r="76" ht="13.5" customHeight="1">
-      <c r="A76" s="12" t="s">
+    <row r="76" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A76" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B76" s="13" t="s">
+      <c r="B76" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D76" s="1"/>
@@ -3359,9 +3365,9 @@
       <c r="V76" s="1"/>
       <c r="W76" s="1"/>
     </row>
-    <row r="77" ht="13.5" customHeight="1">
-      <c r="A77" s="14"/>
-      <c r="B77" s="15"/>
+    <row r="77" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A77" s="13"/>
+      <c r="B77" s="14"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -3384,14 +3390,14 @@
       <c r="V77" s="1"/>
       <c r="W77" s="1"/>
     </row>
-    <row r="78" ht="13.5" customHeight="1">
-      <c r="A78" s="15" t="s">
+    <row r="78" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A78" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C78" s="17" t="s">
+      <c r="C78" s="15" t="s">
         <v>88</v>
       </c>
       <c r="D78" s="1"/>
@@ -3415,14 +3421,14 @@
       <c r="V78" s="1"/>
       <c r="W78" s="1"/>
     </row>
-    <row r="79" ht="13.5" customHeight="1">
-      <c r="A79" s="15" t="s">
+    <row r="79" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A79" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C79" s="17" t="s">
+      <c r="C79" s="15" t="s">
         <v>90</v>
       </c>
       <c r="D79" s="1"/>
@@ -3446,14 +3452,14 @@
       <c r="V79" s="1"/>
       <c r="W79" s="1"/>
     </row>
-    <row r="80" ht="13.5" customHeight="1">
-      <c r="A80" s="15" t="s">
+    <row r="80" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A80" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C80" s="17" t="s">
+      <c r="C80" s="15" t="s">
         <v>92</v>
       </c>
       <c r="D80" s="1"/>
@@ -3477,14 +3483,14 @@
       <c r="V80" s="1"/>
       <c r="W80" s="1"/>
     </row>
-    <row r="81" ht="13.5" customHeight="1">
-      <c r="A81" s="15" t="s">
+    <row r="81" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A81" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C81" s="17" t="s">
+      <c r="C81" s="15" t="s">
         <v>94</v>
       </c>
       <c r="D81" s="1"/>
@@ -3508,14 +3514,14 @@
       <c r="V81" s="1"/>
       <c r="W81" s="1"/>
     </row>
-    <row r="82" ht="13.5" customHeight="1">
-      <c r="A82" s="15" t="s">
+    <row r="82" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A82" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B82" s="16" t="s">
+      <c r="B82" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C82" s="17" t="s">
+      <c r="C82" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D82" s="1"/>
@@ -3539,14 +3545,14 @@
       <c r="V82" s="1"/>
       <c r="W82" s="1"/>
     </row>
-    <row r="83" ht="13.5" customHeight="1">
-      <c r="A83" s="15" t="s">
+    <row r="83" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A83" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B83" s="16" t="s">
+      <c r="B83" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C83" s="17" t="s">
+      <c r="C83" s="15" t="s">
         <v>98</v>
       </c>
       <c r="D83" s="1"/>
@@ -3570,14 +3576,14 @@
       <c r="V83" s="1"/>
       <c r="W83" s="1"/>
     </row>
-    <row r="84" ht="13.5" customHeight="1">
-      <c r="A84" s="15" t="s">
+    <row r="84" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A84" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B84" s="15" t="s">
+      <c r="B84" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C84" s="18" t="s">
+      <c r="C84" s="14" t="s">
         <v>100</v>
       </c>
       <c r="D84" s="1"/>
@@ -3601,14 +3607,14 @@
       <c r="V84" s="1"/>
       <c r="W84" s="1"/>
     </row>
-    <row r="85" ht="13.5" customHeight="1">
-      <c r="A85" s="15" t="s">
+    <row r="85" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A85" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B85" s="15" t="s">
+      <c r="B85" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="C85" s="18" t="s">
+      <c r="C85" s="14" t="s">
         <v>102</v>
       </c>
       <c r="D85" s="1"/>
@@ -3632,14 +3638,14 @@
       <c r="V85" s="1"/>
       <c r="W85" s="1"/>
     </row>
-    <row r="86" ht="13.5" customHeight="1">
-      <c r="A86" s="15" t="s">
+    <row r="86" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A86" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B86" s="15" t="s">
+      <c r="B86" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C86" s="18" t="s">
+      <c r="C86" s="14" t="s">
         <v>104</v>
       </c>
       <c r="D86" s="1"/>
@@ -3663,14 +3669,14 @@
       <c r="V86" s="1"/>
       <c r="W86" s="1"/>
     </row>
-    <row r="87" ht="13.5" customHeight="1">
-      <c r="A87" s="15" t="s">
+    <row r="87" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A87" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B87" s="15" t="s">
+      <c r="B87" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C87" s="18" t="s">
+      <c r="C87" s="14" t="s">
         <v>106</v>
       </c>
       <c r="D87" s="1"/>
@@ -3694,14 +3700,14 @@
       <c r="V87" s="1"/>
       <c r="W87" s="1"/>
     </row>
-    <row r="88" ht="13.5" customHeight="1">
-      <c r="A88" s="15" t="s">
+    <row r="88" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A88" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B88" s="15" t="s">
+      <c r="B88" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="C88" s="18" t="s">
+      <c r="C88" s="14" t="s">
         <v>108</v>
       </c>
       <c r="D88" s="1"/>
@@ -3725,14 +3731,14 @@
       <c r="V88" s="1"/>
       <c r="W88" s="1"/>
     </row>
-    <row r="89" ht="13.5" customHeight="1">
-      <c r="A89" s="15" t="s">
+    <row r="89" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A89" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B89" s="16" t="s">
+      <c r="B89" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C89" s="17" t="s">
+      <c r="C89" s="15" t="s">
         <v>110</v>
       </c>
       <c r="D89" s="1"/>
@@ -3756,14 +3762,14 @@
       <c r="V89" s="1"/>
       <c r="W89" s="1"/>
     </row>
-    <row r="90" ht="13.5" customHeight="1">
-      <c r="A90" s="15" t="s">
+    <row r="90" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A90" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B90" s="16" t="s">
+      <c r="B90" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C90" s="17" t="s">
+      <c r="C90" s="15" t="s">
         <v>112</v>
       </c>
       <c r="D90" s="1"/>
@@ -3787,14 +3793,14 @@
       <c r="V90" s="1"/>
       <c r="W90" s="1"/>
     </row>
-    <row r="91" ht="13.5" customHeight="1">
-      <c r="A91" s="15" t="s">
+    <row r="91" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A91" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B91" s="16" t="s">
+      <c r="B91" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C91" s="17" t="s">
+      <c r="C91" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D91" s="1"/>
@@ -3818,14 +3824,14 @@
       <c r="V91" s="1"/>
       <c r="W91" s="1"/>
     </row>
-    <row r="92" ht="13.5" customHeight="1">
-      <c r="A92" s="15" t="s">
+    <row r="92" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A92" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B92" s="16" t="s">
+      <c r="B92" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C92" s="17" t="s">
+      <c r="C92" s="15" t="s">
         <v>116</v>
       </c>
       <c r="D92" s="1"/>
@@ -3849,14 +3855,14 @@
       <c r="V92" s="1"/>
       <c r="W92" s="1"/>
     </row>
-    <row r="93" ht="13.5" customHeight="1">
-      <c r="A93" s="15" t="s">
+    <row r="93" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A93" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="B93" s="16" t="s">
+      <c r="B93" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C93" s="17" t="s">
+      <c r="C93" s="15" t="s">
         <v>118</v>
       </c>
       <c r="D93" s="1"/>
@@ -3880,14 +3886,14 @@
       <c r="V93" s="1"/>
       <c r="W93" s="1"/>
     </row>
-    <row r="94" ht="13.5" customHeight="1">
-      <c r="A94" s="15" t="s">
+    <row r="94" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A94" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B94" s="15" t="s">
+      <c r="B94" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C94" s="18" t="s">
+      <c r="C94" s="14" t="s">
         <v>120</v>
       </c>
       <c r="D94" s="1"/>
@@ -3911,14 +3917,14 @@
       <c r="V94" s="1"/>
       <c r="W94" s="1"/>
     </row>
-    <row r="95" ht="13.5" customHeight="1">
-      <c r="A95" s="15" t="s">
+    <row r="95" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A95" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B95" s="15" t="s">
+      <c r="B95" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C95" s="18" t="s">
+      <c r="C95" s="14" t="s">
         <v>122</v>
       </c>
       <c r="D95" s="1"/>
@@ -3942,14 +3948,14 @@
       <c r="V95" s="1"/>
       <c r="W95" s="1"/>
     </row>
-    <row r="96" ht="13.5" customHeight="1">
-      <c r="A96" s="15" t="s">
+    <row r="96" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A96" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="B96" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="C96" s="18" t="s">
+      <c r="C96" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D96" s="1"/>
@@ -3973,14 +3979,14 @@
       <c r="V96" s="1"/>
       <c r="W96" s="1"/>
     </row>
-    <row r="97" ht="13.5" customHeight="1">
-      <c r="A97" s="15" t="s">
+    <row r="97" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A97" s="14" t="s">
         <v>125</v>
       </c>
       <c r="B97" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C97" s="20" t="s">
+      <c r="C97" s="19" t="s">
         <v>126</v>
       </c>
       <c r="D97" s="1"/>
@@ -4004,14 +4010,14 @@
       <c r="V97" s="1"/>
       <c r="W97" s="1"/>
     </row>
-    <row r="98" ht="13.5" customHeight="1">
-      <c r="A98" s="15" t="s">
+    <row r="98" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A98" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B98" s="15" t="s">
+      <c r="B98" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C98" s="18" t="s">
+      <c r="C98" s="14" t="s">
         <v>128</v>
       </c>
       <c r="D98" s="1"/>
@@ -4035,14 +4041,14 @@
       <c r="V98" s="1"/>
       <c r="W98" s="1"/>
     </row>
-    <row r="99" ht="13.5" customHeight="1">
-      <c r="A99" s="15" t="s">
+    <row r="99" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A99" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="B99" s="15" t="s">
+      <c r="B99" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C99" s="18" t="s">
+      <c r="C99" s="14" t="s">
         <v>130</v>
       </c>
       <c r="D99" s="1"/>
@@ -4066,14 +4072,14 @@
       <c r="V99" s="1"/>
       <c r="W99" s="1"/>
     </row>
-    <row r="100" ht="13.5" customHeight="1">
-      <c r="A100" s="15" t="s">
+    <row r="100" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A100" s="14" t="s">
         <v>131</v>
       </c>
       <c r="B100" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C100" s="20" t="s">
+      <c r="C100" s="19" t="s">
         <v>132</v>
       </c>
       <c r="D100" s="1"/>
@@ -4097,14 +4103,14 @@
       <c r="V100" s="1"/>
       <c r="W100" s="1"/>
     </row>
-    <row r="101" ht="13.5" customHeight="1">
-      <c r="A101" s="15" t="s">
+    <row r="101" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A101" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B101" s="15" t="s">
+      <c r="B101" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C101" s="18" t="s">
+      <c r="C101" s="14" t="s">
         <v>134</v>
       </c>
       <c r="D101" s="1"/>
@@ -4128,14 +4134,14 @@
       <c r="V101" s="1"/>
       <c r="W101" s="1"/>
     </row>
-    <row r="102" ht="13.5" customHeight="1">
-      <c r="A102" s="21" t="s">
+    <row r="102" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A102" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B102" s="16" t="s">
+      <c r="B102" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C102" s="17" t="s">
+      <c r="C102" s="15" t="s">
         <v>136</v>
       </c>
       <c r="D102" s="1"/>
@@ -4159,14 +4165,14 @@
       <c r="V102" s="1"/>
       <c r="W102" s="1"/>
     </row>
-    <row r="103" ht="13.5" customHeight="1">
-      <c r="A103" s="15" t="s">
+    <row r="103" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A103" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B103" s="16" t="s">
+      <c r="B103" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C103" s="17" t="s">
+      <c r="C103" s="15" t="s">
         <v>138</v>
       </c>
       <c r="D103" s="1"/>
@@ -4190,14 +4196,14 @@
       <c r="V103" s="1"/>
       <c r="W103" s="1"/>
     </row>
-    <row r="104" ht="13.5" customHeight="1">
-      <c r="A104" s="21" t="s">
+    <row r="104" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A104" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="B104" s="16" t="s">
+      <c r="B104" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="C104" s="17" t="s">
+      <c r="C104" s="15" t="s">
         <v>140</v>
       </c>
       <c r="D104" s="1"/>
@@ -4221,14 +4227,14 @@
       <c r="V104" s="1"/>
       <c r="W104" s="1"/>
     </row>
-    <row r="105" ht="13.5" customHeight="1">
-      <c r="A105" s="15" t="s">
+    <row r="105" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A105" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B105" s="15" t="s">
+      <c r="B105" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="C105" s="18" t="s">
+      <c r="C105" s="14" t="s">
         <v>142</v>
       </c>
       <c r="D105" s="1"/>
@@ -4252,14 +4258,14 @@
       <c r="V105" s="1"/>
       <c r="W105" s="1"/>
     </row>
-    <row r="106" ht="13.5" customHeight="1">
-      <c r="A106" s="15" t="s">
+    <row r="106" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A106" s="14" t="s">
         <v>143</v>
       </c>
       <c r="B106" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="C106" s="20" t="s">
+      <c r="C106" s="19" t="s">
         <v>144</v>
       </c>
       <c r="D106" s="1"/>
@@ -4283,14 +4289,14 @@
       <c r="V106" s="1"/>
       <c r="W106" s="1"/>
     </row>
-    <row r="107" ht="13.5" customHeight="1">
-      <c r="A107" s="15" t="s">
+    <row r="107" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A107" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B107" s="16" t="s">
+      <c r="B107" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C107" s="17" t="s">
+      <c r="C107" s="15" t="s">
         <v>146</v>
       </c>
       <c r="D107" s="1"/>
@@ -4314,14 +4320,14 @@
       <c r="V107" s="1"/>
       <c r="W107" s="1"/>
     </row>
-    <row r="108" ht="13.5" customHeight="1">
-      <c r="A108" s="15" t="s">
+    <row r="108" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A108" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B108" s="16" t="s">
+      <c r="B108" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="C108" s="17" t="s">
+      <c r="C108" s="15" t="s">
         <v>148</v>
       </c>
       <c r="D108" s="1"/>
@@ -4345,14 +4351,14 @@
       <c r="V108" s="1"/>
       <c r="W108" s="1"/>
     </row>
-    <row r="109" ht="13.5" customHeight="1">
-      <c r="A109" s="15" t="s">
+    <row r="109" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A109" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="B109" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="C109" s="18" t="s">
+      <c r="C109" s="14" t="s">
         <v>150</v>
       </c>
       <c r="D109" s="1"/>
@@ -4376,14 +4382,14 @@
       <c r="V109" s="1"/>
       <c r="W109" s="1"/>
     </row>
-    <row r="110" ht="13.5" customHeight="1">
-      <c r="A110" s="15" t="s">
+    <row r="110" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A110" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="B110" s="15" t="s">
+      <c r="B110" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="C110" s="18" t="s">
+      <c r="C110" s="14" t="s">
         <v>152</v>
       </c>
       <c r="D110" s="1"/>
@@ -4407,14 +4413,14 @@
       <c r="V110" s="1"/>
       <c r="W110" s="1"/>
     </row>
-    <row r="111" ht="13.5" customHeight="1">
-      <c r="A111" s="15" t="s">
+    <row r="111" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A111" s="14" t="s">
         <v>153</v>
       </c>
       <c r="B111" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="C111" s="20" t="s">
+      <c r="C111" s="19" t="s">
         <v>154</v>
       </c>
       <c r="D111" s="1"/>
@@ -4438,14 +4444,14 @@
       <c r="V111" s="1"/>
       <c r="W111" s="1"/>
     </row>
-    <row r="112" ht="13.5" customHeight="1">
-      <c r="A112" s="15" t="s">
+    <row r="112" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A112" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="B112" s="16" t="s">
+      <c r="B112" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="C112" s="17" t="s">
+      <c r="C112" s="15" t="s">
         <v>156</v>
       </c>
       <c r="D112" s="1"/>
@@ -4469,14 +4475,14 @@
       <c r="V112" s="1"/>
       <c r="W112" s="1"/>
     </row>
-    <row r="113" ht="13.5" customHeight="1">
-      <c r="A113" s="15" t="s">
+    <row r="113" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A113" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="B113" s="15" t="s">
+      <c r="B113" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C113" s="18" t="s">
+      <c r="C113" s="14" t="s">
         <v>158</v>
       </c>
       <c r="D113" s="1"/>
@@ -4500,14 +4506,14 @@
       <c r="V113" s="1"/>
       <c r="W113" s="1"/>
     </row>
-    <row r="114" ht="13.5" customHeight="1">
-      <c r="A114" s="15" t="s">
+    <row r="114" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A114" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="B114" s="16" t="s">
+      <c r="B114" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="C114" s="17" t="s">
+      <c r="C114" s="15" t="s">
         <v>160</v>
       </c>
       <c r="D114" s="1"/>
@@ -4531,14 +4537,14 @@
       <c r="V114" s="1"/>
       <c r="W114" s="1"/>
     </row>
-    <row r="115" ht="13.5" customHeight="1">
-      <c r="A115" s="15" t="s">
+    <row r="115" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A115" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="B115" s="15" t="s">
+      <c r="B115" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C115" s="18" t="s">
+      <c r="C115" s="14" t="s">
         <v>163</v>
       </c>
       <c r="D115" s="1"/>
@@ -4562,14 +4568,14 @@
       <c r="V115" s="1"/>
       <c r="W115" s="1"/>
     </row>
-    <row r="116" ht="13.5" customHeight="1">
-      <c r="A116" s="15" t="s">
+    <row r="116" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A116" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="B116" s="16" t="s">
+      <c r="B116" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="C116" s="17" t="s">
+      <c r="C116" s="15" t="s">
         <v>166</v>
       </c>
       <c r="D116" s="1"/>
@@ -4593,14 +4599,14 @@
       <c r="V116" s="1"/>
       <c r="W116" s="1"/>
     </row>
-    <row r="117" ht="13.5" customHeight="1">
-      <c r="A117" s="15" t="s">
+    <row r="117" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A117" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B117" s="15" t="s">
+      <c r="B117" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="C117" s="18" t="s">
+      <c r="C117" s="14" t="s">
         <v>169</v>
       </c>
       <c r="D117" s="1"/>
@@ -4624,14 +4630,14 @@
       <c r="V117" s="1"/>
       <c r="W117" s="1"/>
     </row>
-    <row r="118" ht="13.5" customHeight="1">
-      <c r="A118" s="15" t="s">
+    <row r="118" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A118" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B118" s="16" t="s">
+      <c r="B118" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="C118" s="17" t="s">
+      <c r="C118" s="15" t="s">
         <v>172</v>
       </c>
       <c r="D118" s="1"/>
@@ -4655,14 +4661,14 @@
       <c r="V118" s="1"/>
       <c r="W118" s="1"/>
     </row>
-    <row r="119" ht="13.5" customHeight="1">
-      <c r="A119" s="15" t="s">
+    <row r="119" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A119" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="B119" s="15" t="s">
+      <c r="B119" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="C119" s="18" t="s">
+      <c r="C119" s="14" t="s">
         <v>175</v>
       </c>
       <c r="D119" s="1"/>
@@ -4686,14 +4692,14 @@
       <c r="V119" s="1"/>
       <c r="W119" s="1"/>
     </row>
-    <row r="120" ht="13.5" customHeight="1">
-      <c r="A120" s="15" t="s">
+    <row r="120" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A120" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="B120" s="15" t="s">
+      <c r="B120" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="C120" s="18" t="s">
+      <c r="C120" s="14" t="s">
         <v>178</v>
       </c>
       <c r="D120" s="1"/>
@@ -4717,14 +4723,14 @@
       <c r="V120" s="1"/>
       <c r="W120" s="1"/>
     </row>
-    <row r="121" ht="13.5" customHeight="1">
-      <c r="A121" s="15" t="s">
+    <row r="121" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A121" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="B121" s="15" t="s">
+      <c r="B121" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="C121" s="18" t="s">
+      <c r="C121" s="14" t="s">
         <v>181</v>
       </c>
       <c r="D121" s="1"/>
@@ -4748,10 +4754,10 @@
       <c r="V121" s="1"/>
       <c r="W121" s="1"/>
     </row>
-    <row r="122" ht="13.5" customHeight="1">
-      <c r="A122" s="15"/>
-      <c r="B122" s="15"/>
-      <c r="C122" s="18" t="s">
+    <row r="122" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A122" s="14"/>
+      <c r="B122" s="14"/>
+      <c r="C122" s="14" t="s">
         <v>182</v>
       </c>
       <c r="D122" s="1"/>
@@ -4775,14 +4781,14 @@
       <c r="V122" s="1"/>
       <c r="W122" s="1"/>
     </row>
-    <row r="123" ht="13.5" customHeight="1">
-      <c r="A123" s="15" t="s">
+    <row r="123" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A123" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="B123" s="15" t="s">
+      <c r="B123" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C123" s="18" t="s">
+      <c r="C123" s="14" t="s">
         <v>185</v>
       </c>
       <c r="D123" s="1"/>
@@ -4806,10 +4812,10 @@
       <c r="V123" s="1"/>
       <c r="W123" s="1"/>
     </row>
-    <row r="124" ht="13.5" customHeight="1">
-      <c r="A124" s="15"/>
-      <c r="B124" s="15"/>
-      <c r="C124" s="18" t="s">
+    <row r="124" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A124" s="14"/>
+      <c r="B124" s="14"/>
+      <c r="C124" s="14" t="s">
         <v>186</v>
       </c>
       <c r="D124" s="1"/>
@@ -4833,14 +4839,14 @@
       <c r="V124" s="1"/>
       <c r="W124" s="1"/>
     </row>
-    <row r="125" ht="13.5" customHeight="1">
-      <c r="A125" s="15" t="s">
+    <row r="125" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A125" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="B125" s="15" t="s">
+      <c r="B125" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="C125" s="18" t="s">
+      <c r="C125" s="14" t="s">
         <v>189</v>
       </c>
       <c r="D125" s="1"/>
@@ -4864,14 +4870,14 @@
       <c r="V125" s="1"/>
       <c r="W125" s="1"/>
     </row>
-    <row r="126" ht="13.5" customHeight="1">
-      <c r="A126" s="15" t="s">
+    <row r="126" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A126" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="B126" s="16" t="s">
+      <c r="B126" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="C126" s="17" t="s">
+      <c r="C126" s="15" t="s">
         <v>192</v>
       </c>
       <c r="D126" s="1"/>
@@ -4895,14 +4901,14 @@
       <c r="V126" s="1"/>
       <c r="W126" s="1"/>
     </row>
-    <row r="127" ht="13.5" customHeight="1">
-      <c r="A127" s="15" t="s">
+    <row r="127" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A127" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="B127" s="15" t="s">
+      <c r="B127" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="C127" s="18" t="s">
+      <c r="C127" s="14" t="s">
         <v>195</v>
       </c>
       <c r="D127" s="1"/>
@@ -4926,14 +4932,14 @@
       <c r="V127" s="1"/>
       <c r="W127" s="1"/>
     </row>
-    <row r="128" ht="13.5" customHeight="1">
-      <c r="A128" s="15" t="s">
+    <row r="128" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A128" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="B128" s="15" t="s">
+      <c r="B128" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="C128" s="18" t="s">
+      <c r="C128" s="14" t="s">
         <v>198</v>
       </c>
       <c r="D128" s="1"/>
@@ -4957,14 +4963,14 @@
       <c r="V128" s="1"/>
       <c r="W128" s="1"/>
     </row>
-    <row r="129" ht="13.5" customHeight="1">
-      <c r="A129" s="15" t="s">
+    <row r="129" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A129" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="B129" s="15" t="s">
+      <c r="B129" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="C129" s="18" t="s">
+      <c r="C129" s="14" t="s">
         <v>201</v>
       </c>
       <c r="D129" s="1"/>
@@ -4988,14 +4994,14 @@
       <c r="V129" s="1"/>
       <c r="W129" s="1"/>
     </row>
-    <row r="130" ht="13.5" customHeight="1">
-      <c r="A130" s="15" t="s">
+    <row r="130" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A130" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="B130" s="16" t="s">
+      <c r="B130" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="C130" s="17" t="s">
+      <c r="C130" s="15" t="s">
         <v>204</v>
       </c>
       <c r="D130" s="1"/>
@@ -5019,14 +5025,14 @@
       <c r="V130" s="1"/>
       <c r="W130" s="1"/>
     </row>
-    <row r="131" ht="13.5" customHeight="1">
-      <c r="A131" s="15" t="s">
+    <row r="131" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A131" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="B131" s="15" t="s">
+      <c r="B131" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="C131" s="18" t="s">
+      <c r="C131" s="14" t="s">
         <v>206</v>
       </c>
       <c r="D131" s="1"/>
@@ -5050,14 +5056,14 @@
       <c r="V131" s="1"/>
       <c r="W131" s="1"/>
     </row>
-    <row r="132" ht="13.5" customHeight="1">
-      <c r="A132" s="15" t="s">
+    <row r="132" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A132" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="B132" s="15" t="s">
+      <c r="B132" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="C132" s="18" t="s">
+      <c r="C132" s="14" t="s">
         <v>208</v>
       </c>
       <c r="D132" s="1"/>
@@ -5081,14 +5087,14 @@
       <c r="V132" s="1"/>
       <c r="W132" s="1"/>
     </row>
-    <row r="133" ht="13.5" customHeight="1">
-      <c r="A133" s="15" t="s">
+    <row r="133" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A133" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="B133" s="15" t="s">
+      <c r="B133" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="C133" s="18" t="s">
+      <c r="C133" s="14" t="s">
         <v>210</v>
       </c>
       <c r="D133" s="1"/>
@@ -5112,14 +5118,14 @@
       <c r="V133" s="1"/>
       <c r="W133" s="1"/>
     </row>
-    <row r="134" ht="13.5" customHeight="1">
-      <c r="A134" s="15" t="s">
+    <row r="134" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A134" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="B134" s="15" t="s">
+      <c r="B134" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="C134" s="18" t="s">
+      <c r="C134" s="14" t="s">
         <v>212</v>
       </c>
       <c r="D134" s="1"/>
@@ -5143,14 +5149,14 @@
       <c r="V134" s="1"/>
       <c r="W134" s="1"/>
     </row>
-    <row r="135" ht="13.5" customHeight="1">
-      <c r="A135" s="15" t="s">
+    <row r="135" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A135" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="B135" s="15" t="s">
+      <c r="B135" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="C135" s="18" t="s">
+      <c r="C135" s="14" t="s">
         <v>214</v>
       </c>
       <c r="D135" s="1"/>
@@ -5174,14 +5180,14 @@
       <c r="V135" s="1"/>
       <c r="W135" s="1"/>
     </row>
-    <row r="136" ht="13.5" customHeight="1">
-      <c r="A136" s="15" t="s">
+    <row r="136" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A136" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="B136" s="15" t="s">
+      <c r="B136" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="C136" s="18" t="s">
+      <c r="C136" s="14" t="s">
         <v>216</v>
       </c>
       <c r="D136" s="1"/>
@@ -5205,14 +5211,14 @@
       <c r="V136" s="1"/>
       <c r="W136" s="1"/>
     </row>
-    <row r="137" ht="13.5" customHeight="1">
-      <c r="A137" s="15" t="s">
+    <row r="137" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A137" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="B137" s="15" t="s">
+      <c r="B137" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="C137" s="18" t="s">
+      <c r="C137" s="14" t="s">
         <v>218</v>
       </c>
       <c r="D137" s="1"/>
@@ -5236,10 +5242,10 @@
       <c r="V137" s="1"/>
       <c r="W137" s="1"/>
     </row>
-    <row r="138" ht="13.5" customHeight="1">
-      <c r="A138" s="15"/>
-      <c r="B138" s="15"/>
-      <c r="C138" s="18"/>
+    <row r="138" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A138" s="14"/>
+      <c r="B138" s="14"/>
+      <c r="C138" s="14"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -5261,14 +5267,14 @@
       <c r="V138" s="1"/>
       <c r="W138" s="1"/>
     </row>
-    <row r="139" ht="13.5" customHeight="1">
-      <c r="A139" s="15" t="s">
+    <row r="139" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A139" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="B139" s="15" t="s">
+      <c r="B139" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="C139" s="18" t="s">
+      <c r="C139" s="14" t="s">
         <v>220</v>
       </c>
       <c r="D139" s="1"/>
@@ -5292,14 +5298,14 @@
       <c r="V139" s="1"/>
       <c r="W139" s="1"/>
     </row>
-    <row r="140" ht="13.5" customHeight="1">
-      <c r="A140" s="15" t="s">
+    <row r="140" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A140" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="B140" s="15" t="s">
+      <c r="B140" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="C140" s="18" t="s">
+      <c r="C140" s="14" t="s">
         <v>222</v>
       </c>
       <c r="D140" s="1"/>
@@ -5323,14 +5329,14 @@
       <c r="V140" s="1"/>
       <c r="W140" s="1"/>
     </row>
-    <row r="141" ht="13.5" customHeight="1">
-      <c r="A141" s="15" t="s">
+    <row r="141" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A141" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B141" s="15" t="s">
+      <c r="B141" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="C141" s="18" t="s">
+      <c r="C141" s="14" t="s">
         <v>224</v>
       </c>
       <c r="D141" s="1"/>
@@ -5354,14 +5360,14 @@
       <c r="V141" s="1"/>
       <c r="W141" s="1"/>
     </row>
-    <row r="142" ht="13.5" customHeight="1">
-      <c r="A142" s="15" t="s">
+    <row r="142" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A142" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="B142" s="15" t="s">
+      <c r="B142" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="C142" s="18" t="s">
+      <c r="C142" s="14" t="s">
         <v>226</v>
       </c>
       <c r="D142" s="1"/>
@@ -5385,14 +5391,14 @@
       <c r="V142" s="1"/>
       <c r="W142" s="1"/>
     </row>
-    <row r="143" ht="13.5" customHeight="1">
-      <c r="A143" s="15" t="s">
+    <row r="143" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A143" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="B143" s="15" t="s">
+      <c r="B143" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="C143" s="18" t="s">
+      <c r="C143" s="14" t="s">
         <v>228</v>
       </c>
       <c r="D143" s="1"/>
@@ -5416,14 +5422,14 @@
       <c r="V143" s="1"/>
       <c r="W143" s="1"/>
     </row>
-    <row r="144" ht="13.5" customHeight="1">
-      <c r="A144" s="15" t="s">
+    <row r="144" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A144" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B144" s="15" t="s">
+      <c r="B144" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="C144" s="18" t="s">
+      <c r="C144" s="14" t="s">
         <v>229</v>
       </c>
       <c r="D144" s="1"/>
@@ -5447,14 +5453,14 @@
       <c r="V144" s="1"/>
       <c r="W144" s="1"/>
     </row>
-    <row r="145" ht="13.5" customHeight="1">
-      <c r="A145" s="15" t="s">
+    <row r="145" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A145" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="B145" s="15" t="s">
+      <c r="B145" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="C145" s="18" t="s">
+      <c r="C145" s="14" t="s">
         <v>226</v>
       </c>
       <c r="D145" s="1"/>
@@ -5478,14 +5484,14 @@
       <c r="V145" s="1"/>
       <c r="W145" s="1"/>
     </row>
-    <row r="146" ht="13.5" customHeight="1">
-      <c r="A146" s="15" t="s">
+    <row r="146" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A146" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="B146" s="15" t="s">
+      <c r="B146" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="C146" s="18" t="s">
+      <c r="C146" s="14" t="s">
         <v>228</v>
       </c>
       <c r="D146" s="1"/>
@@ -5509,14 +5515,14 @@
       <c r="V146" s="1"/>
       <c r="W146" s="1"/>
     </row>
-    <row r="147" ht="13.5" customHeight="1">
-      <c r="A147" s="15" t="s">
+    <row r="147" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A147" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="B147" s="15" t="s">
+      <c r="B147" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="C147" s="18" t="s">
+      <c r="C147" s="14" t="s">
         <v>231</v>
       </c>
       <c r="D147" s="1"/>
@@ -5540,14 +5546,14 @@
       <c r="V147" s="1"/>
       <c r="W147" s="1"/>
     </row>
-    <row r="148" ht="13.5" customHeight="1">
-      <c r="A148" s="15" t="s">
+    <row r="148" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A148" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="B148" s="15" t="s">
+      <c r="B148" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="C148" s="18" t="s">
+      <c r="C148" s="14" t="s">
         <v>234</v>
       </c>
       <c r="D148" s="1"/>
@@ -5571,14 +5577,14 @@
       <c r="V148" s="1"/>
       <c r="W148" s="1"/>
     </row>
-    <row r="149" ht="13.5" customHeight="1">
-      <c r="A149" s="15" t="s">
+    <row r="149" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A149" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="B149" s="16" t="s">
+      <c r="B149" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="C149" s="17" t="s">
+      <c r="C149" s="15" t="s">
         <v>237</v>
       </c>
       <c r="D149" s="1"/>
@@ -5602,14 +5608,14 @@
       <c r="V149" s="1"/>
       <c r="W149" s="1"/>
     </row>
-    <row r="150" ht="13.5" customHeight="1">
-      <c r="A150" s="15" t="s">
+    <row r="150" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A150" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="B150" s="15" t="s">
+      <c r="B150" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="C150" s="18" t="s">
+      <c r="C150" s="14" t="s">
         <v>239</v>
       </c>
       <c r="D150" s="1"/>
@@ -5633,14 +5639,14 @@
       <c r="V150" s="1"/>
       <c r="W150" s="1"/>
     </row>
-    <row r="151" ht="13.5" customHeight="1">
-      <c r="A151" s="15" t="s">
+    <row r="151" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A151" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="B151" s="15" t="s">
+      <c r="B151" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="C151" s="18" t="s">
+      <c r="C151" s="14" t="s">
         <v>241</v>
       </c>
       <c r="D151" s="1"/>
@@ -5664,14 +5670,14 @@
       <c r="V151" s="1"/>
       <c r="W151" s="1"/>
     </row>
-    <row r="152" ht="13.5" customHeight="1">
-      <c r="A152" s="15" t="s">
+    <row r="152" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A152" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="B152" s="15" t="s">
+      <c r="B152" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="C152" s="18" t="s">
+      <c r="C152" s="14" t="s">
         <v>243</v>
       </c>
       <c r="D152" s="1"/>
@@ -5695,11 +5701,11 @@
       <c r="V152" s="1"/>
       <c r="W152" s="1"/>
     </row>
-    <row r="153" ht="13.5" customHeight="1">
-      <c r="A153" s="15" t="s">
+    <row r="153" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A153" s="14" t="s">
         <v>244</v>
       </c>
-      <c r="B153" s="22" t="s">
+      <c r="B153" s="17" t="s">
         <v>245</v>
       </c>
       <c r="C153" s="1"/>
@@ -5724,7 +5730,7 @@
       <c r="V153" s="1"/>
       <c r="W153" s="1"/>
     </row>
-    <row r="154" ht="13.5" customHeight="1">
+    <row r="154" spans="1:23" ht="13.5" customHeight="1">
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
@@ -5747,7 +5753,7 @@
       <c r="V154" s="1"/>
       <c r="W154" s="1"/>
     </row>
-    <row r="155" ht="13.5" customHeight="1">
+    <row r="155" spans="1:23" ht="13.5" customHeight="1">
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -5770,7 +5776,7 @@
       <c r="V155" s="1"/>
       <c r="W155" s="1"/>
     </row>
-    <row r="156" ht="13.5" customHeight="1">
+    <row r="156" spans="1:23" ht="13.5" customHeight="1">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -5795,7 +5801,7 @@
       <c r="V156" s="1"/>
       <c r="W156" s="1"/>
     </row>
-    <row r="157" ht="13.5" customHeight="1">
+    <row r="157" spans="1:23" ht="13.5" customHeight="1">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -5820,7 +5826,7 @@
       <c r="V157" s="1"/>
       <c r="W157" s="1"/>
     </row>
-    <row r="158" ht="13.5" customHeight="1">
+    <row r="158" spans="1:23" ht="13.5" customHeight="1">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -5845,7 +5851,7 @@
       <c r="V158" s="1"/>
       <c r="W158" s="1"/>
     </row>
-    <row r="159" ht="13.5" customHeight="1">
+    <row r="159" spans="1:23" ht="13.5" customHeight="1">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -5870,7 +5876,7 @@
       <c r="V159" s="1"/>
       <c r="W159" s="1"/>
     </row>
-    <row r="160" ht="13.5" customHeight="1">
+    <row r="160" spans="1:23" ht="13.5" customHeight="1">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -5895,7 +5901,7 @@
       <c r="V160" s="1"/>
       <c r="W160" s="1"/>
     </row>
-    <row r="161" ht="13.5" customHeight="1">
+    <row r="161" spans="1:23" ht="13.5" customHeight="1">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -5920,7 +5926,7 @@
       <c r="V161" s="1"/>
       <c r="W161" s="1"/>
     </row>
-    <row r="162" ht="13.5" customHeight="1">
+    <row r="162" spans="1:23" ht="13.5" customHeight="1">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -5945,7 +5951,7 @@
       <c r="V162" s="1"/>
       <c r="W162" s="1"/>
     </row>
-    <row r="163" ht="13.5" customHeight="1">
+    <row r="163" spans="1:23" ht="13.5" customHeight="1">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -5970,7 +5976,7 @@
       <c r="V163" s="1"/>
       <c r="W163" s="1"/>
     </row>
-    <row r="164" ht="13.5" customHeight="1">
+    <row r="164" spans="1:23" ht="13.5" customHeight="1">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -5995,7 +6001,7 @@
       <c r="V164" s="1"/>
       <c r="W164" s="1"/>
     </row>
-    <row r="165" ht="13.5" customHeight="1">
+    <row r="165" spans="1:23" ht="13.5" customHeight="1">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -6020,7 +6026,7 @@
       <c r="V165" s="1"/>
       <c r="W165" s="1"/>
     </row>
-    <row r="166" ht="13.5" customHeight="1">
+    <row r="166" spans="1:23" ht="13.5" customHeight="1">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -6045,7 +6051,7 @@
       <c r="V166" s="1"/>
       <c r="W166" s="1"/>
     </row>
-    <row r="167" ht="13.5" customHeight="1">
+    <row r="167" spans="1:23" ht="13.5" customHeight="1">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -6070,7 +6076,7 @@
       <c r="V167" s="1"/>
       <c r="W167" s="1"/>
     </row>
-    <row r="168" ht="13.5" customHeight="1">
+    <row r="168" spans="1:23" ht="13.5" customHeight="1">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -6095,7 +6101,7 @@
       <c r="V168" s="1"/>
       <c r="W168" s="1"/>
     </row>
-    <row r="169" ht="13.5" customHeight="1">
+    <row r="169" spans="1:23" ht="13.5" customHeight="1">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -6120,7 +6126,7 @@
       <c r="V169" s="1"/>
       <c r="W169" s="1"/>
     </row>
-    <row r="170" ht="13.5" customHeight="1">
+    <row r="170" spans="1:23" ht="13.5" customHeight="1">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -6145,7 +6151,7 @@
       <c r="V170" s="1"/>
       <c r="W170" s="1"/>
     </row>
-    <row r="171" ht="13.5" customHeight="1">
+    <row r="171" spans="1:23" ht="13.5" customHeight="1">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -6170,7 +6176,7 @@
       <c r="V171" s="1"/>
       <c r="W171" s="1"/>
     </row>
-    <row r="172" ht="13.5" customHeight="1">
+    <row r="172" spans="1:23" ht="13.5" customHeight="1">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -6195,7 +6201,7 @@
       <c r="V172" s="1"/>
       <c r="W172" s="1"/>
     </row>
-    <row r="173" ht="13.5" customHeight="1">
+    <row r="173" spans="1:23" ht="13.5" customHeight="1">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -6220,7 +6226,7 @@
       <c r="V173" s="1"/>
       <c r="W173" s="1"/>
     </row>
-    <row r="174" ht="13.5" customHeight="1">
+    <row r="174" spans="1:23" ht="13.5" customHeight="1">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -6245,7 +6251,7 @@
       <c r="V174" s="1"/>
       <c r="W174" s="1"/>
     </row>
-    <row r="175" ht="13.5" customHeight="1">
+    <row r="175" spans="1:23" ht="13.5" customHeight="1">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -6270,7 +6276,7 @@
       <c r="V175" s="1"/>
       <c r="W175" s="1"/>
     </row>
-    <row r="176" ht="13.5" customHeight="1">
+    <row r="176" spans="1:23" ht="13.5" customHeight="1">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -6295,7 +6301,7 @@
       <c r="V176" s="1"/>
       <c r="W176" s="1"/>
     </row>
-    <row r="177" ht="13.5" customHeight="1">
+    <row r="177" spans="1:23" ht="13.5" customHeight="1">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -6320,7 +6326,7 @@
       <c r="V177" s="1"/>
       <c r="W177" s="1"/>
     </row>
-    <row r="178" ht="13.5" customHeight="1">
+    <row r="178" spans="1:23" ht="13.5" customHeight="1">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -6345,7 +6351,7 @@
       <c r="V178" s="1"/>
       <c r="W178" s="1"/>
     </row>
-    <row r="179" ht="13.5" customHeight="1">
+    <row r="179" spans="1:23" ht="13.5" customHeight="1">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -6370,7 +6376,7 @@
       <c r="V179" s="1"/>
       <c r="W179" s="1"/>
     </row>
-    <row r="180" ht="13.5" customHeight="1">
+    <row r="180" spans="1:23" ht="13.5" customHeight="1">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -6395,7 +6401,7 @@
       <c r="V180" s="1"/>
       <c r="W180" s="1"/>
     </row>
-    <row r="181" ht="13.5" customHeight="1">
+    <row r="181" spans="1:23" ht="13.5" customHeight="1">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -6420,7 +6426,7 @@
       <c r="V181" s="1"/>
       <c r="W181" s="1"/>
     </row>
-    <row r="182" ht="13.5" customHeight="1">
+    <row r="182" spans="1:23" ht="13.5" customHeight="1">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -6445,7 +6451,7 @@
       <c r="V182" s="1"/>
       <c r="W182" s="1"/>
     </row>
-    <row r="183" ht="13.5" customHeight="1">
+    <row r="183" spans="1:23" ht="13.5" customHeight="1">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -6470,7 +6476,7 @@
       <c r="V183" s="1"/>
       <c r="W183" s="1"/>
     </row>
-    <row r="184" ht="13.5" customHeight="1">
+    <row r="184" spans="1:23" ht="13.5" customHeight="1">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -6495,7 +6501,7 @@
       <c r="V184" s="1"/>
       <c r="W184" s="1"/>
     </row>
-    <row r="185" ht="13.5" customHeight="1">
+    <row r="185" spans="1:23" ht="13.5" customHeight="1">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -6520,7 +6526,7 @@
       <c r="V185" s="1"/>
       <c r="W185" s="1"/>
     </row>
-    <row r="186" ht="13.5" customHeight="1">
+    <row r="186" spans="1:23" ht="13.5" customHeight="1">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -6545,7 +6551,7 @@
       <c r="V186" s="1"/>
       <c r="W186" s="1"/>
     </row>
-    <row r="187" ht="13.5" customHeight="1">
+    <row r="187" spans="1:23" ht="13.5" customHeight="1">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -6570,7 +6576,7 @@
       <c r="V187" s="1"/>
       <c r="W187" s="1"/>
     </row>
-    <row r="188" ht="13.5" customHeight="1">
+    <row r="188" spans="1:23" ht="13.5" customHeight="1">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -6595,7 +6601,7 @@
       <c r="V188" s="1"/>
       <c r="W188" s="1"/>
     </row>
-    <row r="189" ht="13.5" customHeight="1">
+    <row r="189" spans="1:23" ht="13.5" customHeight="1">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -6620,7 +6626,7 @@
       <c r="V189" s="1"/>
       <c r="W189" s="1"/>
     </row>
-    <row r="190" ht="13.5" customHeight="1">
+    <row r="190" spans="1:23" ht="13.5" customHeight="1">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -6645,7 +6651,7 @@
       <c r="V190" s="1"/>
       <c r="W190" s="1"/>
     </row>
-    <row r="191" ht="13.5" customHeight="1">
+    <row r="191" spans="1:23" ht="13.5" customHeight="1">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -6670,7 +6676,7 @@
       <c r="V191" s="1"/>
       <c r="W191" s="1"/>
     </row>
-    <row r="192" ht="13.5" customHeight="1">
+    <row r="192" spans="1:23" ht="13.5" customHeight="1">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -6695,7 +6701,7 @@
       <c r="V192" s="1"/>
       <c r="W192" s="1"/>
     </row>
-    <row r="193" ht="13.5" customHeight="1">
+    <row r="193" spans="1:23" ht="13.5" customHeight="1">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -6720,7 +6726,7 @@
       <c r="V193" s="1"/>
       <c r="W193" s="1"/>
     </row>
-    <row r="194" ht="13.5" customHeight="1">
+    <row r="194" spans="1:23" ht="13.5" customHeight="1">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -6745,7 +6751,7 @@
       <c r="V194" s="1"/>
       <c r="W194" s="1"/>
     </row>
-    <row r="195" ht="13.5" customHeight="1">
+    <row r="195" spans="1:23" ht="13.5" customHeight="1">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -6770,7 +6776,7 @@
       <c r="V195" s="1"/>
       <c r="W195" s="1"/>
     </row>
-    <row r="196" ht="13.5" customHeight="1">
+    <row r="196" spans="1:23" ht="13.5" customHeight="1">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -6795,7 +6801,7 @@
       <c r="V196" s="1"/>
       <c r="W196" s="1"/>
     </row>
-    <row r="197" ht="13.5" customHeight="1">
+    <row r="197" spans="1:23" ht="13.5" customHeight="1">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -6820,7 +6826,7 @@
       <c r="V197" s="1"/>
       <c r="W197" s="1"/>
     </row>
-    <row r="198" ht="13.5" customHeight="1">
+    <row r="198" spans="1:23" ht="13.5" customHeight="1">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -6845,7 +6851,7 @@
       <c r="V198" s="1"/>
       <c r="W198" s="1"/>
     </row>
-    <row r="199" ht="13.5" customHeight="1">
+    <row r="199" spans="1:23" ht="13.5" customHeight="1">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -6870,7 +6876,7 @@
       <c r="V199" s="1"/>
       <c r="W199" s="1"/>
     </row>
-    <row r="200" ht="13.5" customHeight="1">
+    <row r="200" spans="1:23" ht="13.5" customHeight="1">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -6895,7 +6901,7 @@
       <c r="V200" s="1"/>
       <c r="W200" s="1"/>
     </row>
-    <row r="201" ht="13.5" customHeight="1">
+    <row r="201" spans="1:23" ht="13.5" customHeight="1">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -6920,7 +6926,7 @@
       <c r="V201" s="1"/>
       <c r="W201" s="1"/>
     </row>
-    <row r="202" ht="13.5" customHeight="1">
+    <row r="202" spans="1:23" ht="13.5" customHeight="1">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -6945,7 +6951,7 @@
       <c r="V202" s="1"/>
       <c r="W202" s="1"/>
     </row>
-    <row r="203" ht="13.5" customHeight="1">
+    <row r="203" spans="1:23" ht="13.5" customHeight="1">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -6970,7 +6976,7 @@
       <c r="V203" s="1"/>
       <c r="W203" s="1"/>
     </row>
-    <row r="204" ht="13.5" customHeight="1">
+    <row r="204" spans="1:23" ht="13.5" customHeight="1">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -6995,7 +7001,7 @@
       <c r="V204" s="1"/>
       <c r="W204" s="1"/>
     </row>
-    <row r="205" ht="13.5" customHeight="1">
+    <row r="205" spans="1:23" ht="13.5" customHeight="1">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -7020,7 +7026,7 @@
       <c r="V205" s="1"/>
       <c r="W205" s="1"/>
     </row>
-    <row r="206" ht="13.5" customHeight="1">
+    <row r="206" spans="1:23" ht="13.5" customHeight="1">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -7045,7 +7051,7 @@
       <c r="V206" s="1"/>
       <c r="W206" s="1"/>
     </row>
-    <row r="207" ht="13.5" customHeight="1">
+    <row r="207" spans="1:23" ht="13.5" customHeight="1">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -7070,7 +7076,7 @@
       <c r="V207" s="1"/>
       <c r="W207" s="1"/>
     </row>
-    <row r="208" ht="13.5" customHeight="1">
+    <row r="208" spans="1:23" ht="13.5" customHeight="1">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -7095,7 +7101,7 @@
       <c r="V208" s="1"/>
       <c r="W208" s="1"/>
     </row>
-    <row r="209" ht="13.5" customHeight="1">
+    <row r="209" spans="1:23" ht="13.5" customHeight="1">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -7120,7 +7126,7 @@
       <c r="V209" s="1"/>
       <c r="W209" s="1"/>
     </row>
-    <row r="210" ht="13.5" customHeight="1">
+    <row r="210" spans="1:23" ht="13.5" customHeight="1">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -7145,7 +7151,7 @@
       <c r="V210" s="1"/>
       <c r="W210" s="1"/>
     </row>
-    <row r="211" ht="13.5" customHeight="1">
+    <row r="211" spans="1:23" ht="13.5" customHeight="1">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -7170,7 +7176,7 @@
       <c r="V211" s="1"/>
       <c r="W211" s="1"/>
     </row>
-    <row r="212" ht="13.5" customHeight="1">
+    <row r="212" spans="1:23" ht="13.5" customHeight="1">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -7195,7 +7201,7 @@
       <c r="V212" s="1"/>
       <c r="W212" s="1"/>
     </row>
-    <row r="213" ht="13.5" customHeight="1">
+    <row r="213" spans="1:23" ht="13.5" customHeight="1">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -7220,7 +7226,7 @@
       <c r="V213" s="1"/>
       <c r="W213" s="1"/>
     </row>
-    <row r="214" ht="13.5" customHeight="1">
+    <row r="214" spans="1:23" ht="13.5" customHeight="1">
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -7245,7 +7251,7 @@
       <c r="V214" s="1"/>
       <c r="W214" s="1"/>
     </row>
-    <row r="215" ht="13.5" customHeight="1">
+    <row r="215" spans="1:23" ht="13.5" customHeight="1">
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -7270,7 +7276,7 @@
       <c r="V215" s="1"/>
       <c r="W215" s="1"/>
     </row>
-    <row r="216" ht="13.5" customHeight="1">
+    <row r="216" spans="1:23" ht="13.5" customHeight="1">
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -7295,7 +7301,7 @@
       <c r="V216" s="1"/>
       <c r="W216" s="1"/>
     </row>
-    <row r="217" ht="13.5" customHeight="1">
+    <row r="217" spans="1:23" ht="13.5" customHeight="1">
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
@@ -7320,7 +7326,7 @@
       <c r="V217" s="1"/>
       <c r="W217" s="1"/>
     </row>
-    <row r="218" ht="13.5" customHeight="1">
+    <row r="218" spans="1:23" ht="13.5" customHeight="1">
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -7345,7 +7351,7 @@
       <c r="V218" s="1"/>
       <c r="W218" s="1"/>
     </row>
-    <row r="219" ht="13.5" customHeight="1">
+    <row r="219" spans="1:23" ht="13.5" customHeight="1">
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
@@ -7370,7 +7376,7 @@
       <c r="V219" s="1"/>
       <c r="W219" s="1"/>
     </row>
-    <row r="220" ht="13.5" customHeight="1">
+    <row r="220" spans="1:23" ht="13.5" customHeight="1">
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
@@ -7395,7 +7401,7 @@
       <c r="V220" s="1"/>
       <c r="W220" s="1"/>
     </row>
-    <row r="221" ht="13.5" customHeight="1">
+    <row r="221" spans="1:23" ht="13.5" customHeight="1">
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -7420,7 +7426,7 @@
       <c r="V221" s="1"/>
       <c r="W221" s="1"/>
     </row>
-    <row r="222" ht="13.5" customHeight="1">
+    <row r="222" spans="1:23" ht="13.5" customHeight="1">
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -7445,7 +7451,7 @@
       <c r="V222" s="1"/>
       <c r="W222" s="1"/>
     </row>
-    <row r="223" ht="13.5" customHeight="1">
+    <row r="223" spans="1:23" ht="13.5" customHeight="1">
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -7470,7 +7476,7 @@
       <c r="V223" s="1"/>
       <c r="W223" s="1"/>
     </row>
-    <row r="224" ht="13.5" customHeight="1">
+    <row r="224" spans="1:23" ht="13.5" customHeight="1">
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -7495,7 +7501,7 @@
       <c r="V224" s="1"/>
       <c r="W224" s="1"/>
     </row>
-    <row r="225" ht="13.5" customHeight="1">
+    <row r="225" spans="1:23" ht="13.5" customHeight="1">
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
@@ -7520,7 +7526,7 @@
       <c r="V225" s="1"/>
       <c r="W225" s="1"/>
     </row>
-    <row r="226" ht="13.5" customHeight="1">
+    <row r="226" spans="1:23" ht="13.5" customHeight="1">
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
@@ -7545,7 +7551,7 @@
       <c r="V226" s="1"/>
       <c r="W226" s="1"/>
     </row>
-    <row r="227" ht="13.5" customHeight="1">
+    <row r="227" spans="1:23" ht="13.5" customHeight="1">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
@@ -7570,7 +7576,7 @@
       <c r="V227" s="1"/>
       <c r="W227" s="1"/>
     </row>
-    <row r="228" ht="13.5" customHeight="1">
+    <row r="228" spans="1:23" ht="13.5" customHeight="1">
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -7595,7 +7601,7 @@
       <c r="V228" s="1"/>
       <c r="W228" s="1"/>
     </row>
-    <row r="229" ht="13.5" customHeight="1">
+    <row r="229" spans="1:23" ht="13.5" customHeight="1">
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
@@ -7620,7 +7626,7 @@
       <c r="V229" s="1"/>
       <c r="W229" s="1"/>
     </row>
-    <row r="230" ht="13.5" customHeight="1">
+    <row r="230" spans="1:23" ht="13.5" customHeight="1">
       <c r="A230" s="1"/>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
@@ -7645,7 +7651,7 @@
       <c r="V230" s="1"/>
       <c r="W230" s="1"/>
     </row>
-    <row r="231" ht="13.5" customHeight="1">
+    <row r="231" spans="1:23" ht="13.5" customHeight="1">
       <c r="A231" s="1"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
@@ -7670,7 +7676,7 @@
       <c r="V231" s="1"/>
       <c r="W231" s="1"/>
     </row>
-    <row r="232" ht="13.5" customHeight="1">
+    <row r="232" spans="1:23" ht="13.5" customHeight="1">
       <c r="A232" s="1"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
@@ -7695,7 +7701,7 @@
       <c r="V232" s="1"/>
       <c r="W232" s="1"/>
     </row>
-    <row r="233" ht="13.5" customHeight="1">
+    <row r="233" spans="1:23" ht="13.5" customHeight="1">
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
@@ -7720,7 +7726,7 @@
       <c r="V233" s="1"/>
       <c r="W233" s="1"/>
     </row>
-    <row r="234" ht="13.5" customHeight="1">
+    <row r="234" spans="1:23" ht="13.5" customHeight="1">
       <c r="A234" s="1"/>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
@@ -7745,7 +7751,7 @@
       <c r="V234" s="1"/>
       <c r="W234" s="1"/>
     </row>
-    <row r="235" ht="13.5" customHeight="1">
+    <row r="235" spans="1:23" ht="13.5" customHeight="1">
       <c r="A235" s="1"/>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
@@ -7770,7 +7776,7 @@
       <c r="V235" s="1"/>
       <c r="W235" s="1"/>
     </row>
-    <row r="236" ht="13.5" customHeight="1">
+    <row r="236" spans="1:23" ht="13.5" customHeight="1">
       <c r="A236" s="1"/>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
@@ -7795,7 +7801,7 @@
       <c r="V236" s="1"/>
       <c r="W236" s="1"/>
     </row>
-    <row r="237" ht="13.5" customHeight="1">
+    <row r="237" spans="1:23" ht="13.5" customHeight="1">
       <c r="A237" s="1"/>
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
@@ -7820,7 +7826,7 @@
       <c r="V237" s="1"/>
       <c r="W237" s="1"/>
     </row>
-    <row r="238" ht="13.5" customHeight="1">
+    <row r="238" spans="1:23" ht="13.5" customHeight="1">
       <c r="A238" s="1"/>
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
@@ -7845,7 +7851,7 @@
       <c r="V238" s="1"/>
       <c r="W238" s="1"/>
     </row>
-    <row r="239" ht="13.5" customHeight="1">
+    <row r="239" spans="1:23" ht="13.5" customHeight="1">
       <c r="A239" s="1"/>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
@@ -7870,7 +7876,7 @@
       <c r="V239" s="1"/>
       <c r="W239" s="1"/>
     </row>
-    <row r="240" ht="13.5" customHeight="1">
+    <row r="240" spans="1:23" ht="13.5" customHeight="1">
       <c r="A240" s="1"/>
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
@@ -7895,7 +7901,7 @@
       <c r="V240" s="1"/>
       <c r="W240" s="1"/>
     </row>
-    <row r="241" ht="13.5" customHeight="1">
+    <row r="241" spans="1:23" ht="13.5" customHeight="1">
       <c r="A241" s="1"/>
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
@@ -7920,7 +7926,7 @@
       <c r="V241" s="1"/>
       <c r="W241" s="1"/>
     </row>
-    <row r="242" ht="13.5" customHeight="1">
+    <row r="242" spans="1:23" ht="13.5" customHeight="1">
       <c r="A242" s="1"/>
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
@@ -7945,7 +7951,7 @@
       <c r="V242" s="1"/>
       <c r="W242" s="1"/>
     </row>
-    <row r="243" ht="13.5" customHeight="1">
+    <row r="243" spans="1:23" ht="13.5" customHeight="1">
       <c r="A243" s="1"/>
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
@@ -7970,7 +7976,7 @@
       <c r="V243" s="1"/>
       <c r="W243" s="1"/>
     </row>
-    <row r="244" ht="13.5" customHeight="1">
+    <row r="244" spans="1:23" ht="13.5" customHeight="1">
       <c r="A244" s="1"/>
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
@@ -7995,7 +8001,7 @@
       <c r="V244" s="1"/>
       <c r="W244" s="1"/>
     </row>
-    <row r="245" ht="13.5" customHeight="1">
+    <row r="245" spans="1:23" ht="13.5" customHeight="1">
       <c r="A245" s="1"/>
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
@@ -8020,7 +8026,7 @@
       <c r="V245" s="1"/>
       <c r="W245" s="1"/>
     </row>
-    <row r="246" ht="13.5" customHeight="1">
+    <row r="246" spans="1:23" ht="13.5" customHeight="1">
       <c r="A246" s="1"/>
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
@@ -8045,7 +8051,7 @@
       <c r="V246" s="1"/>
       <c r="W246" s="1"/>
     </row>
-    <row r="247" ht="13.5" customHeight="1">
+    <row r="247" spans="1:23" ht="13.5" customHeight="1">
       <c r="A247" s="1"/>
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
@@ -8070,7 +8076,7 @@
       <c r="V247" s="1"/>
       <c r="W247" s="1"/>
     </row>
-    <row r="248" ht="13.5" customHeight="1">
+    <row r="248" spans="1:23" ht="13.5" customHeight="1">
       <c r="A248" s="1"/>
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
@@ -8095,7 +8101,7 @@
       <c r="V248" s="1"/>
       <c r="W248" s="1"/>
     </row>
-    <row r="249" ht="13.5" customHeight="1">
+    <row r="249" spans="1:23" ht="13.5" customHeight="1">
       <c r="A249" s="1"/>
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
@@ -8120,7 +8126,7 @@
       <c r="V249" s="1"/>
       <c r="W249" s="1"/>
     </row>
-    <row r="250" ht="13.5" customHeight="1">
+    <row r="250" spans="1:23" ht="13.5" customHeight="1">
       <c r="A250" s="1"/>
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
@@ -8145,7 +8151,7 @@
       <c r="V250" s="1"/>
       <c r="W250" s="1"/>
     </row>
-    <row r="251" ht="13.5" customHeight="1">
+    <row r="251" spans="1:23" ht="13.5" customHeight="1">
       <c r="A251" s="1"/>
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
@@ -8170,7 +8176,7 @@
       <c r="V251" s="1"/>
       <c r="W251" s="1"/>
     </row>
-    <row r="252" ht="13.5" customHeight="1">
+    <row r="252" spans="1:23" ht="13.5" customHeight="1">
       <c r="A252" s="1"/>
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
@@ -8195,7 +8201,7 @@
       <c r="V252" s="1"/>
       <c r="W252" s="1"/>
     </row>
-    <row r="253" ht="13.5" customHeight="1">
+    <row r="253" spans="1:23" ht="13.5" customHeight="1">
       <c r="A253" s="1"/>
       <c r="B253" s="1"/>
       <c r="C253" s="1"/>
@@ -8220,7 +8226,7 @@
       <c r="V253" s="1"/>
       <c r="W253" s="1"/>
     </row>
-    <row r="254" ht="13.5" customHeight="1">
+    <row r="254" spans="1:23" ht="13.5" customHeight="1">
       <c r="A254" s="1"/>
       <c r="B254" s="1"/>
       <c r="C254" s="1"/>
@@ -8245,7 +8251,7 @@
       <c r="V254" s="1"/>
       <c r="W254" s="1"/>
     </row>
-    <row r="255" ht="13.5" customHeight="1">
+    <row r="255" spans="1:23" ht="13.5" customHeight="1">
       <c r="A255" s="1"/>
       <c r="B255" s="1"/>
       <c r="C255" s="1"/>
@@ -8270,7 +8276,7 @@
       <c r="V255" s="1"/>
       <c r="W255" s="1"/>
     </row>
-    <row r="256" ht="13.5" customHeight="1">
+    <row r="256" spans="1:23" ht="13.5" customHeight="1">
       <c r="A256" s="1"/>
       <c r="B256" s="1"/>
       <c r="C256" s="1"/>
@@ -8295,7 +8301,7 @@
       <c r="V256" s="1"/>
       <c r="W256" s="1"/>
     </row>
-    <row r="257" ht="13.5" customHeight="1">
+    <row r="257" spans="1:23" ht="13.5" customHeight="1">
       <c r="A257" s="1"/>
       <c r="B257" s="1"/>
       <c r="C257" s="1"/>
@@ -8320,7 +8326,7 @@
       <c r="V257" s="1"/>
       <c r="W257" s="1"/>
     </row>
-    <row r="258" ht="13.5" customHeight="1">
+    <row r="258" spans="1:23" ht="13.5" customHeight="1">
       <c r="A258" s="1"/>
       <c r="B258" s="1"/>
       <c r="C258" s="1"/>
@@ -8345,7 +8351,7 @@
       <c r="V258" s="1"/>
       <c r="W258" s="1"/>
     </row>
-    <row r="259" ht="13.5" customHeight="1">
+    <row r="259" spans="1:23" ht="13.5" customHeight="1">
       <c r="A259" s="1"/>
       <c r="B259" s="1"/>
       <c r="C259" s="1"/>
@@ -8370,7 +8376,7 @@
       <c r="V259" s="1"/>
       <c r="W259" s="1"/>
     </row>
-    <row r="260" ht="13.5" customHeight="1">
+    <row r="260" spans="1:23" ht="13.5" customHeight="1">
       <c r="A260" s="1"/>
       <c r="B260" s="1"/>
       <c r="C260" s="1"/>
@@ -8395,7 +8401,7 @@
       <c r="V260" s="1"/>
       <c r="W260" s="1"/>
     </row>
-    <row r="261" ht="13.5" customHeight="1">
+    <row r="261" spans="1:23" ht="13.5" customHeight="1">
       <c r="A261" s="1"/>
       <c r="B261" s="1"/>
       <c r="C261" s="1"/>
@@ -8420,7 +8426,7 @@
       <c r="V261" s="1"/>
       <c r="W261" s="1"/>
     </row>
-    <row r="262" ht="13.5" customHeight="1">
+    <row r="262" spans="1:23" ht="13.5" customHeight="1">
       <c r="A262" s="1"/>
       <c r="B262" s="1"/>
       <c r="C262" s="1"/>
@@ -8445,7 +8451,7 @@
       <c r="V262" s="1"/>
       <c r="W262" s="1"/>
     </row>
-    <row r="263" ht="13.5" customHeight="1">
+    <row r="263" spans="1:23" ht="13.5" customHeight="1">
       <c r="A263" s="1"/>
       <c r="B263" s="1"/>
       <c r="C263" s="1"/>
@@ -8470,7 +8476,7 @@
       <c r="V263" s="1"/>
       <c r="W263" s="1"/>
     </row>
-    <row r="264" ht="13.5" customHeight="1">
+    <row r="264" spans="1:23" ht="13.5" customHeight="1">
       <c r="A264" s="1"/>
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
@@ -8495,7 +8501,7 @@
       <c r="V264" s="1"/>
       <c r="W264" s="1"/>
     </row>
-    <row r="265" ht="13.5" customHeight="1">
+    <row r="265" spans="1:23" ht="13.5" customHeight="1">
       <c r="A265" s="1"/>
       <c r="B265" s="1"/>
       <c r="C265" s="1"/>
@@ -8520,7 +8526,7 @@
       <c r="V265" s="1"/>
       <c r="W265" s="1"/>
     </row>
-    <row r="266" ht="13.5" customHeight="1">
+    <row r="266" spans="1:23" ht="13.5" customHeight="1">
       <c r="A266" s="1"/>
       <c r="B266" s="1"/>
       <c r="C266" s="1"/>
@@ -8545,7 +8551,7 @@
       <c r="V266" s="1"/>
       <c r="W266" s="1"/>
     </row>
-    <row r="267" ht="13.5" customHeight="1">
+    <row r="267" spans="1:23" ht="13.5" customHeight="1">
       <c r="A267" s="1"/>
       <c r="B267" s="1"/>
       <c r="C267" s="1"/>
@@ -8570,7 +8576,7 @@
       <c r="V267" s="1"/>
       <c r="W267" s="1"/>
     </row>
-    <row r="268" ht="13.5" customHeight="1">
+    <row r="268" spans="1:23" ht="13.5" customHeight="1">
       <c r="A268" s="1"/>
       <c r="B268" s="1"/>
       <c r="C268" s="1"/>
@@ -8595,7 +8601,7 @@
       <c r="V268" s="1"/>
       <c r="W268" s="1"/>
     </row>
-    <row r="269" ht="13.5" customHeight="1">
+    <row r="269" spans="1:23" ht="13.5" customHeight="1">
       <c r="A269" s="1"/>
       <c r="B269" s="1"/>
       <c r="C269" s="1"/>
@@ -8620,7 +8626,7 @@
       <c r="V269" s="1"/>
       <c r="W269" s="1"/>
     </row>
-    <row r="270" ht="13.5" customHeight="1">
+    <row r="270" spans="1:23" ht="13.5" customHeight="1">
       <c r="A270" s="1"/>
       <c r="B270" s="1"/>
       <c r="C270" s="1"/>
@@ -8645,7 +8651,7 @@
       <c r="V270" s="1"/>
       <c r="W270" s="1"/>
     </row>
-    <row r="271" ht="13.5" customHeight="1">
+    <row r="271" spans="1:23" ht="13.5" customHeight="1">
       <c r="A271" s="1"/>
       <c r="B271" s="1"/>
       <c r="C271" s="1"/>
@@ -8670,7 +8676,7 @@
       <c r="V271" s="1"/>
       <c r="W271" s="1"/>
     </row>
-    <row r="272" ht="13.5" customHeight="1">
+    <row r="272" spans="1:23" ht="13.5" customHeight="1">
       <c r="A272" s="1"/>
       <c r="B272" s="1"/>
       <c r="C272" s="1"/>
@@ -8695,7 +8701,7 @@
       <c r="V272" s="1"/>
       <c r="W272" s="1"/>
     </row>
-    <row r="273" ht="13.5" customHeight="1">
+    <row r="273" spans="1:23" ht="13.5" customHeight="1">
       <c r="A273" s="1"/>
       <c r="B273" s="1"/>
       <c r="C273" s="1"/>
@@ -8720,7 +8726,7 @@
       <c r="V273" s="1"/>
       <c r="W273" s="1"/>
     </row>
-    <row r="274" ht="13.5" customHeight="1">
+    <row r="274" spans="1:23" ht="13.5" customHeight="1">
       <c r="A274" s="1"/>
       <c r="B274" s="1"/>
       <c r="C274" s="1"/>
@@ -8745,7 +8751,7 @@
       <c r="V274" s="1"/>
       <c r="W274" s="1"/>
     </row>
-    <row r="275" ht="13.5" customHeight="1">
+    <row r="275" spans="1:23" ht="13.5" customHeight="1">
       <c r="A275" s="1"/>
       <c r="B275" s="1"/>
       <c r="C275" s="1"/>
@@ -8770,7 +8776,7 @@
       <c r="V275" s="1"/>
       <c r="W275" s="1"/>
     </row>
-    <row r="276" ht="13.5" customHeight="1">
+    <row r="276" spans="1:23" ht="13.5" customHeight="1">
       <c r="A276" s="1"/>
       <c r="B276" s="1"/>
       <c r="C276" s="1"/>
@@ -8795,7 +8801,7 @@
       <c r="V276" s="1"/>
       <c r="W276" s="1"/>
     </row>
-    <row r="277" ht="13.5" customHeight="1">
+    <row r="277" spans="1:23" ht="13.5" customHeight="1">
       <c r="A277" s="1"/>
       <c r="B277" s="1"/>
       <c r="C277" s="1"/>
@@ -8820,7 +8826,7 @@
       <c r="V277" s="1"/>
       <c r="W277" s="1"/>
     </row>
-    <row r="278" ht="13.5" customHeight="1">
+    <row r="278" spans="1:23" ht="13.5" customHeight="1">
       <c r="A278" s="1"/>
       <c r="B278" s="1"/>
       <c r="C278" s="1"/>
@@ -8845,7 +8851,7 @@
       <c r="V278" s="1"/>
       <c r="W278" s="1"/>
     </row>
-    <row r="279" ht="13.5" customHeight="1">
+    <row r="279" spans="1:23" ht="13.5" customHeight="1">
       <c r="A279" s="1"/>
       <c r="B279" s="1"/>
       <c r="C279" s="1"/>
@@ -8870,7 +8876,7 @@
       <c r="V279" s="1"/>
       <c r="W279" s="1"/>
     </row>
-    <row r="280" ht="13.5" customHeight="1">
+    <row r="280" spans="1:23" ht="13.5" customHeight="1">
       <c r="A280" s="1"/>
       <c r="B280" s="1"/>
       <c r="C280" s="1"/>
@@ -8895,7 +8901,7 @@
       <c r="V280" s="1"/>
       <c r="W280" s="1"/>
     </row>
-    <row r="281" ht="13.5" customHeight="1">
+    <row r="281" spans="1:23" ht="13.5" customHeight="1">
       <c r="A281" s="1"/>
       <c r="B281" s="1"/>
       <c r="C281" s="1"/>
@@ -8920,7 +8926,7 @@
       <c r="V281" s="1"/>
       <c r="W281" s="1"/>
     </row>
-    <row r="282" ht="13.5" customHeight="1">
+    <row r="282" spans="1:23" ht="13.5" customHeight="1">
       <c r="A282" s="1"/>
       <c r="B282" s="1"/>
       <c r="C282" s="1"/>
@@ -8945,7 +8951,7 @@
       <c r="V282" s="1"/>
       <c r="W282" s="1"/>
     </row>
-    <row r="283" ht="13.5" customHeight="1">
+    <row r="283" spans="1:23" ht="13.5" customHeight="1">
       <c r="A283" s="1"/>
       <c r="B283" s="1"/>
       <c r="C283" s="1"/>
@@ -8970,7 +8976,7 @@
       <c r="V283" s="1"/>
       <c r="W283" s="1"/>
     </row>
-    <row r="284" ht="13.5" customHeight="1">
+    <row r="284" spans="1:23" ht="13.5" customHeight="1">
       <c r="A284" s="1"/>
       <c r="B284" s="1"/>
       <c r="C284" s="1"/>
@@ -8995,7 +9001,7 @@
       <c r="V284" s="1"/>
       <c r="W284" s="1"/>
     </row>
-    <row r="285" ht="13.5" customHeight="1">
+    <row r="285" spans="1:23" ht="13.5" customHeight="1">
       <c r="A285" s="1"/>
       <c r="B285" s="1"/>
       <c r="C285" s="1"/>
@@ -9020,7 +9026,7 @@
       <c r="V285" s="1"/>
       <c r="W285" s="1"/>
     </row>
-    <row r="286" ht="13.5" customHeight="1">
+    <row r="286" spans="1:23" ht="13.5" customHeight="1">
       <c r="A286" s="1"/>
       <c r="B286" s="1"/>
       <c r="C286" s="1"/>
@@ -9045,7 +9051,7 @@
       <c r="V286" s="1"/>
       <c r="W286" s="1"/>
     </row>
-    <row r="287" ht="13.5" customHeight="1">
+    <row r="287" spans="1:23" ht="13.5" customHeight="1">
       <c r="A287" s="1"/>
       <c r="B287" s="1"/>
       <c r="C287" s="1"/>
@@ -9070,7 +9076,7 @@
       <c r="V287" s="1"/>
       <c r="W287" s="1"/>
     </row>
-    <row r="288" ht="13.5" customHeight="1">
+    <row r="288" spans="1:23" ht="13.5" customHeight="1">
       <c r="A288" s="1"/>
       <c r="B288" s="1"/>
       <c r="C288" s="1"/>
@@ -9095,7 +9101,7 @@
       <c r="V288" s="1"/>
       <c r="W288" s="1"/>
     </row>
-    <row r="289" ht="13.5" customHeight="1">
+    <row r="289" spans="1:23" ht="13.5" customHeight="1">
       <c r="A289" s="1"/>
       <c r="B289" s="1"/>
       <c r="C289" s="1"/>
@@ -9120,7 +9126,7 @@
       <c r="V289" s="1"/>
       <c r="W289" s="1"/>
     </row>
-    <row r="290" ht="13.5" customHeight="1">
+    <row r="290" spans="1:23" ht="13.5" customHeight="1">
       <c r="A290" s="1"/>
       <c r="B290" s="1"/>
       <c r="C290" s="1"/>
@@ -9145,7 +9151,7 @@
       <c r="V290" s="1"/>
       <c r="W290" s="1"/>
     </row>
-    <row r="291" ht="13.5" customHeight="1">
+    <row r="291" spans="1:23" ht="13.5" customHeight="1">
       <c r="A291" s="1"/>
       <c r="B291" s="1"/>
       <c r="C291" s="1"/>
@@ -9170,7 +9176,7 @@
       <c r="V291" s="1"/>
       <c r="W291" s="1"/>
     </row>
-    <row r="292" ht="13.5" customHeight="1">
+    <row r="292" spans="1:23" ht="13.5" customHeight="1">
       <c r="A292" s="1"/>
       <c r="B292" s="1"/>
       <c r="C292" s="1"/>
@@ -9195,7 +9201,7 @@
       <c r="V292" s="1"/>
       <c r="W292" s="1"/>
     </row>
-    <row r="293" ht="13.5" customHeight="1">
+    <row r="293" spans="1:23" ht="13.5" customHeight="1">
       <c r="A293" s="1"/>
       <c r="B293" s="1"/>
       <c r="C293" s="1"/>
@@ -9220,7 +9226,7 @@
       <c r="V293" s="1"/>
       <c r="W293" s="1"/>
     </row>
-    <row r="294" ht="13.5" customHeight="1">
+    <row r="294" spans="1:23" ht="13.5" customHeight="1">
       <c r="A294" s="1"/>
       <c r="B294" s="1"/>
       <c r="C294" s="1"/>
@@ -9245,7 +9251,7 @@
       <c r="V294" s="1"/>
       <c r="W294" s="1"/>
     </row>
-    <row r="295" ht="13.5" customHeight="1">
+    <row r="295" spans="1:23" ht="13.5" customHeight="1">
       <c r="A295" s="1"/>
       <c r="B295" s="1"/>
       <c r="C295" s="1"/>
@@ -9270,7 +9276,7 @@
       <c r="V295" s="1"/>
       <c r="W295" s="1"/>
     </row>
-    <row r="296" ht="13.5" customHeight="1">
+    <row r="296" spans="1:23" ht="13.5" customHeight="1">
       <c r="A296" s="1"/>
       <c r="B296" s="1"/>
       <c r="C296" s="1"/>
@@ -9295,7 +9301,7 @@
       <c r="V296" s="1"/>
       <c r="W296" s="1"/>
     </row>
-    <row r="297" ht="13.5" customHeight="1">
+    <row r="297" spans="1:23" ht="13.5" customHeight="1">
       <c r="A297" s="1"/>
       <c r="B297" s="1"/>
       <c r="C297" s="1"/>
@@ -9320,7 +9326,7 @@
       <c r="V297" s="1"/>
       <c r="W297" s="1"/>
     </row>
-    <row r="298" ht="13.5" customHeight="1">
+    <row r="298" spans="1:23" ht="13.5" customHeight="1">
       <c r="A298" s="1"/>
       <c r="B298" s="1"/>
       <c r="C298" s="1"/>
@@ -9345,7 +9351,7 @@
       <c r="V298" s="1"/>
       <c r="W298" s="1"/>
     </row>
-    <row r="299" ht="13.5" customHeight="1">
+    <row r="299" spans="1:23" ht="13.5" customHeight="1">
       <c r="A299" s="1"/>
       <c r="B299" s="1"/>
       <c r="C299" s="1"/>
@@ -9370,7 +9376,7 @@
       <c r="V299" s="1"/>
       <c r="W299" s="1"/>
     </row>
-    <row r="300" ht="13.5" customHeight="1">
+    <row r="300" spans="1:23" ht="13.5" customHeight="1">
       <c r="A300" s="1"/>
       <c r="B300" s="1"/>
       <c r="C300" s="1"/>
@@ -9395,7 +9401,7 @@
       <c r="V300" s="1"/>
       <c r="W300" s="1"/>
     </row>
-    <row r="301" ht="13.5" customHeight="1">
+    <row r="301" spans="1:23" ht="13.5" customHeight="1">
       <c r="A301" s="1"/>
       <c r="B301" s="1"/>
       <c r="C301" s="1"/>
@@ -9420,7 +9426,7 @@
       <c r="V301" s="1"/>
       <c r="W301" s="1"/>
     </row>
-    <row r="302" ht="13.5" customHeight="1">
+    <row r="302" spans="1:23" ht="13.5" customHeight="1">
       <c r="A302" s="1"/>
       <c r="B302" s="1"/>
       <c r="C302" s="1"/>
@@ -9445,7 +9451,7 @@
       <c r="V302" s="1"/>
       <c r="W302" s="1"/>
     </row>
-    <row r="303" ht="13.5" customHeight="1">
+    <row r="303" spans="1:23" ht="13.5" customHeight="1">
       <c r="A303" s="1"/>
       <c r="B303" s="1"/>
       <c r="C303" s="1"/>
@@ -9470,7 +9476,7 @@
       <c r="V303" s="1"/>
       <c r="W303" s="1"/>
     </row>
-    <row r="304" ht="13.5" customHeight="1">
+    <row r="304" spans="1:23" ht="13.5" customHeight="1">
       <c r="A304" s="1"/>
       <c r="B304" s="1"/>
       <c r="C304" s="1"/>
@@ -9495,7 +9501,7 @@
       <c r="V304" s="1"/>
       <c r="W304" s="1"/>
     </row>
-    <row r="305" ht="13.5" customHeight="1">
+    <row r="305" spans="1:23" ht="13.5" customHeight="1">
       <c r="A305" s="1"/>
       <c r="B305" s="1"/>
       <c r="C305" s="1"/>
@@ -9520,7 +9526,7 @@
       <c r="V305" s="1"/>
       <c r="W305" s="1"/>
     </row>
-    <row r="306" ht="13.5" customHeight="1">
+    <row r="306" spans="1:23" ht="13.5" customHeight="1">
       <c r="A306" s="1"/>
       <c r="B306" s="1"/>
       <c r="C306" s="1"/>
@@ -9545,7 +9551,7 @@
       <c r="V306" s="1"/>
       <c r="W306" s="1"/>
     </row>
-    <row r="307" ht="13.5" customHeight="1">
+    <row r="307" spans="1:23" ht="13.5" customHeight="1">
       <c r="A307" s="1"/>
       <c r="B307" s="1"/>
       <c r="C307" s="1"/>
@@ -9570,7 +9576,7 @@
       <c r="V307" s="1"/>
       <c r="W307" s="1"/>
     </row>
-    <row r="308" ht="13.5" customHeight="1">
+    <row r="308" spans="1:23" ht="13.5" customHeight="1">
       <c r="A308" s="1"/>
       <c r="B308" s="1"/>
       <c r="C308" s="1"/>
@@ -9595,7 +9601,7 @@
       <c r="V308" s="1"/>
       <c r="W308" s="1"/>
     </row>
-    <row r="309" ht="13.5" customHeight="1">
+    <row r="309" spans="1:23" ht="13.5" customHeight="1">
       <c r="A309" s="1"/>
       <c r="B309" s="1"/>
       <c r="C309" s="1"/>
@@ -9620,7 +9626,7 @@
       <c r="V309" s="1"/>
       <c r="W309" s="1"/>
     </row>
-    <row r="310" ht="13.5" customHeight="1">
+    <row r="310" spans="1:23" ht="13.5" customHeight="1">
       <c r="A310" s="1"/>
       <c r="B310" s="1"/>
       <c r="C310" s="1"/>
@@ -9645,7 +9651,7 @@
       <c r="V310" s="1"/>
       <c r="W310" s="1"/>
     </row>
-    <row r="311" ht="13.5" customHeight="1">
+    <row r="311" spans="1:23" ht="13.5" customHeight="1">
       <c r="A311" s="1"/>
       <c r="B311" s="1"/>
       <c r="C311" s="1"/>
@@ -9670,7 +9676,7 @@
       <c r="V311" s="1"/>
       <c r="W311" s="1"/>
     </row>
-    <row r="312" ht="13.5" customHeight="1">
+    <row r="312" spans="1:23" ht="13.5" customHeight="1">
       <c r="A312" s="1"/>
       <c r="B312" s="1"/>
       <c r="C312" s="1"/>
@@ -9695,7 +9701,7 @@
       <c r="V312" s="1"/>
       <c r="W312" s="1"/>
     </row>
-    <row r="313" ht="13.5" customHeight="1">
+    <row r="313" spans="1:23" ht="13.5" customHeight="1">
       <c r="A313" s="1"/>
       <c r="B313" s="1"/>
       <c r="C313" s="1"/>
@@ -9720,7 +9726,7 @@
       <c r="V313" s="1"/>
       <c r="W313" s="1"/>
     </row>
-    <row r="314" ht="13.5" customHeight="1">
+    <row r="314" spans="1:23" ht="13.5" customHeight="1">
       <c r="A314" s="1"/>
       <c r="B314" s="1"/>
       <c r="C314" s="1"/>
@@ -9745,7 +9751,7 @@
       <c r="V314" s="1"/>
       <c r="W314" s="1"/>
     </row>
-    <row r="315" ht="13.5" customHeight="1">
+    <row r="315" spans="1:23" ht="13.5" customHeight="1">
       <c r="A315" s="1"/>
       <c r="B315" s="1"/>
       <c r="C315" s="1"/>
@@ -9770,7 +9776,7 @@
       <c r="V315" s="1"/>
       <c r="W315" s="1"/>
     </row>
-    <row r="316" ht="13.5" customHeight="1">
+    <row r="316" spans="1:23" ht="13.5" customHeight="1">
       <c r="A316" s="1"/>
       <c r="B316" s="1"/>
       <c r="C316" s="1"/>
@@ -9795,7 +9801,7 @@
       <c r="V316" s="1"/>
       <c r="W316" s="1"/>
     </row>
-    <row r="317" ht="13.5" customHeight="1">
+    <row r="317" spans="1:23" ht="13.5" customHeight="1">
       <c r="A317" s="1"/>
       <c r="B317" s="1"/>
       <c r="C317" s="1"/>
@@ -9820,7 +9826,7 @@
       <c r="V317" s="1"/>
       <c r="W317" s="1"/>
     </row>
-    <row r="318" ht="13.5" customHeight="1">
+    <row r="318" spans="1:23" ht="13.5" customHeight="1">
       <c r="A318" s="1"/>
       <c r="B318" s="1"/>
       <c r="C318" s="1"/>
@@ -9845,7 +9851,7 @@
       <c r="V318" s="1"/>
       <c r="W318" s="1"/>
     </row>
-    <row r="319" ht="13.5" customHeight="1">
+    <row r="319" spans="1:23" ht="13.5" customHeight="1">
       <c r="A319" s="1"/>
       <c r="B319" s="1"/>
       <c r="C319" s="1"/>
@@ -9870,7 +9876,7 @@
       <c r="V319" s="1"/>
       <c r="W319" s="1"/>
     </row>
-    <row r="320" ht="13.5" customHeight="1">
+    <row r="320" spans="1:23" ht="13.5" customHeight="1">
       <c r="A320" s="1"/>
       <c r="B320" s="1"/>
       <c r="C320" s="1"/>
@@ -9895,7 +9901,7 @@
       <c r="V320" s="1"/>
       <c r="W320" s="1"/>
     </row>
-    <row r="321" ht="13.5" customHeight="1">
+    <row r="321" spans="1:23" ht="13.5" customHeight="1">
       <c r="A321" s="1"/>
       <c r="B321" s="1"/>
       <c r="C321" s="1"/>
@@ -9920,7 +9926,7 @@
       <c r="V321" s="1"/>
       <c r="W321" s="1"/>
     </row>
-    <row r="322" ht="13.5" customHeight="1">
+    <row r="322" spans="1:23" ht="13.5" customHeight="1">
       <c r="A322" s="1"/>
       <c r="B322" s="1"/>
       <c r="C322" s="1"/>
@@ -9945,7 +9951,7 @@
       <c r="V322" s="1"/>
       <c r="W322" s="1"/>
     </row>
-    <row r="323" ht="13.5" customHeight="1">
+    <row r="323" spans="1:23" ht="13.5" customHeight="1">
       <c r="A323" s="1"/>
       <c r="B323" s="1"/>
       <c r="C323" s="1"/>
@@ -9970,7 +9976,7 @@
       <c r="V323" s="1"/>
       <c r="W323" s="1"/>
     </row>
-    <row r="324" ht="13.5" customHeight="1">
+    <row r="324" spans="1:23" ht="13.5" customHeight="1">
       <c r="A324" s="1"/>
       <c r="B324" s="1"/>
       <c r="C324" s="1"/>
@@ -9995,7 +10001,7 @@
       <c r="V324" s="1"/>
       <c r="W324" s="1"/>
     </row>
-    <row r="325" ht="13.5" customHeight="1">
+    <row r="325" spans="1:23" ht="13.5" customHeight="1">
       <c r="A325" s="1"/>
       <c r="B325" s="1"/>
       <c r="C325" s="1"/>
@@ -10020,7 +10026,7 @@
       <c r="V325" s="1"/>
       <c r="W325" s="1"/>
     </row>
-    <row r="326" ht="13.5" customHeight="1">
+    <row r="326" spans="1:23" ht="13.5" customHeight="1">
       <c r="A326" s="1"/>
       <c r="B326" s="1"/>
       <c r="C326" s="1"/>
@@ -10045,7 +10051,7 @@
       <c r="V326" s="1"/>
       <c r="W326" s="1"/>
     </row>
-    <row r="327" ht="13.5" customHeight="1">
+    <row r="327" spans="1:23" ht="13.5" customHeight="1">
       <c r="A327" s="1"/>
       <c r="B327" s="1"/>
       <c r="C327" s="1"/>
@@ -10070,7 +10076,7 @@
       <c r="V327" s="1"/>
       <c r="W327" s="1"/>
     </row>
-    <row r="328" ht="13.5" customHeight="1">
+    <row r="328" spans="1:23" ht="13.5" customHeight="1">
       <c r="A328" s="1"/>
       <c r="B328" s="1"/>
       <c r="C328" s="1"/>
@@ -10095,7 +10101,7 @@
       <c r="V328" s="1"/>
       <c r="W328" s="1"/>
     </row>
-    <row r="329" ht="13.5" customHeight="1">
+    <row r="329" spans="1:23" ht="13.5" customHeight="1">
       <c r="A329" s="1"/>
       <c r="B329" s="1"/>
       <c r="C329" s="1"/>
@@ -10120,7 +10126,7 @@
       <c r="V329" s="1"/>
       <c r="W329" s="1"/>
     </row>
-    <row r="330" ht="13.5" customHeight="1">
+    <row r="330" spans="1:23" ht="13.5" customHeight="1">
       <c r="A330" s="1"/>
       <c r="B330" s="1"/>
       <c r="C330" s="1"/>
@@ -10145,7 +10151,7 @@
       <c r="V330" s="1"/>
       <c r="W330" s="1"/>
     </row>
-    <row r="331" ht="13.5" customHeight="1">
+    <row r="331" spans="1:23" ht="13.5" customHeight="1">
       <c r="A331" s="1"/>
       <c r="B331" s="1"/>
       <c r="C331" s="1"/>
@@ -10170,7 +10176,7 @@
       <c r="V331" s="1"/>
       <c r="W331" s="1"/>
     </row>
-    <row r="332" ht="13.5" customHeight="1">
+    <row r="332" spans="1:23" ht="13.5" customHeight="1">
       <c r="A332" s="1"/>
       <c r="B332" s="1"/>
       <c r="C332" s="1"/>
@@ -10195,7 +10201,7 @@
       <c r="V332" s="1"/>
       <c r="W332" s="1"/>
     </row>
-    <row r="333" ht="13.5" customHeight="1">
+    <row r="333" spans="1:23" ht="13.5" customHeight="1">
       <c r="A333" s="1"/>
       <c r="B333" s="1"/>
       <c r="C333" s="1"/>
@@ -10220,7 +10226,7 @@
       <c r="V333" s="1"/>
       <c r="W333" s="1"/>
     </row>
-    <row r="334" ht="13.5" customHeight="1">
+    <row r="334" spans="1:23" ht="13.5" customHeight="1">
       <c r="A334" s="1"/>
       <c r="B334" s="1"/>
       <c r="C334" s="1"/>
@@ -10245,7 +10251,7 @@
       <c r="V334" s="1"/>
       <c r="W334" s="1"/>
     </row>
-    <row r="335" ht="13.5" customHeight="1">
+    <row r="335" spans="1:23" ht="13.5" customHeight="1">
       <c r="A335" s="1"/>
       <c r="B335" s="1"/>
       <c r="C335" s="1"/>
@@ -10270,7 +10276,7 @@
       <c r="V335" s="1"/>
       <c r="W335" s="1"/>
     </row>
-    <row r="336" ht="13.5" customHeight="1">
+    <row r="336" spans="1:23" ht="13.5" customHeight="1">
       <c r="A336" s="1"/>
       <c r="B336" s="1"/>
       <c r="C336" s="1"/>
@@ -10295,7 +10301,7 @@
       <c r="V336" s="1"/>
       <c r="W336" s="1"/>
     </row>
-    <row r="337" ht="13.5" customHeight="1">
+    <row r="337" spans="1:23" ht="13.5" customHeight="1">
       <c r="A337" s="1"/>
       <c r="B337" s="1"/>
       <c r="C337" s="1"/>
@@ -10320,7 +10326,7 @@
       <c r="V337" s="1"/>
       <c r="W337" s="1"/>
     </row>
-    <row r="338" ht="13.5" customHeight="1">
+    <row r="338" spans="1:23" ht="13.5" customHeight="1">
       <c r="A338" s="1"/>
       <c r="B338" s="1"/>
       <c r="C338" s="1"/>
@@ -10345,7 +10351,7 @@
       <c r="V338" s="1"/>
       <c r="W338" s="1"/>
     </row>
-    <row r="339" ht="13.5" customHeight="1">
+    <row r="339" spans="1:23" ht="13.5" customHeight="1">
       <c r="A339" s="1"/>
       <c r="B339" s="1"/>
       <c r="C339" s="1"/>
@@ -10370,7 +10376,7 @@
       <c r="V339" s="1"/>
       <c r="W339" s="1"/>
     </row>
-    <row r="340" ht="13.5" customHeight="1">
+    <row r="340" spans="1:23" ht="13.5" customHeight="1">
       <c r="A340" s="1"/>
       <c r="B340" s="1"/>
       <c r="C340" s="1"/>
@@ -10395,7 +10401,7 @@
       <c r="V340" s="1"/>
       <c r="W340" s="1"/>
     </row>
-    <row r="341" ht="13.5" customHeight="1">
+    <row r="341" spans="1:23" ht="13.5" customHeight="1">
       <c r="A341" s="1"/>
       <c r="B341" s="1"/>
       <c r="C341" s="1"/>
@@ -10420,7 +10426,7 @@
       <c r="V341" s="1"/>
       <c r="W341" s="1"/>
     </row>
-    <row r="342" ht="13.5" customHeight="1">
+    <row r="342" spans="1:23" ht="13.5" customHeight="1">
       <c r="A342" s="1"/>
       <c r="B342" s="1"/>
       <c r="C342" s="1"/>
@@ -10445,7 +10451,7 @@
       <c r="V342" s="1"/>
       <c r="W342" s="1"/>
     </row>
-    <row r="343" ht="13.5" customHeight="1">
+    <row r="343" spans="1:23" ht="13.5" customHeight="1">
       <c r="A343" s="1"/>
       <c r="B343" s="1"/>
       <c r="C343" s="1"/>
@@ -10470,7 +10476,7 @@
       <c r="V343" s="1"/>
       <c r="W343" s="1"/>
     </row>
-    <row r="344" ht="13.5" customHeight="1">
+    <row r="344" spans="1:23" ht="13.5" customHeight="1">
       <c r="A344" s="1"/>
       <c r="B344" s="1"/>
       <c r="C344" s="1"/>
@@ -10495,7 +10501,7 @@
       <c r="V344" s="1"/>
       <c r="W344" s="1"/>
     </row>
-    <row r="345" ht="13.5" customHeight="1">
+    <row r="345" spans="1:23" ht="13.5" customHeight="1">
       <c r="A345" s="1"/>
       <c r="B345" s="1"/>
       <c r="C345" s="1"/>
@@ -10520,7 +10526,7 @@
       <c r="V345" s="1"/>
       <c r="W345" s="1"/>
     </row>
-    <row r="346" ht="13.5" customHeight="1">
+    <row r="346" spans="1:23" ht="13.5" customHeight="1">
       <c r="A346" s="1"/>
       <c r="B346" s="1"/>
       <c r="C346" s="1"/>
@@ -10545,7 +10551,7 @@
       <c r="V346" s="1"/>
       <c r="W346" s="1"/>
     </row>
-    <row r="347" ht="13.5" customHeight="1">
+    <row r="347" spans="1:23" ht="13.5" customHeight="1">
       <c r="A347" s="1"/>
       <c r="B347" s="1"/>
       <c r="C347" s="1"/>
@@ -10570,7 +10576,7 @@
       <c r="V347" s="1"/>
       <c r="W347" s="1"/>
     </row>
-    <row r="348" ht="13.5" customHeight="1">
+    <row r="348" spans="1:23" ht="13.5" customHeight="1">
       <c r="A348" s="1"/>
       <c r="B348" s="1"/>
       <c r="C348" s="1"/>
@@ -10595,7 +10601,7 @@
       <c r="V348" s="1"/>
       <c r="W348" s="1"/>
     </row>
-    <row r="349" ht="13.5" customHeight="1">
+    <row r="349" spans="1:23" ht="13.5" customHeight="1">
       <c r="A349" s="1"/>
       <c r="B349" s="1"/>
       <c r="C349" s="1"/>
@@ -10620,7 +10626,7 @@
       <c r="V349" s="1"/>
       <c r="W349" s="1"/>
     </row>
-    <row r="350" ht="13.5" customHeight="1">
+    <row r="350" spans="1:23" ht="13.5" customHeight="1">
       <c r="A350" s="1"/>
       <c r="B350" s="1"/>
       <c r="C350" s="1"/>
@@ -10645,7 +10651,7 @@
       <c r="V350" s="1"/>
       <c r="W350" s="1"/>
     </row>
-    <row r="351" ht="13.5" customHeight="1">
+    <row r="351" spans="1:23" ht="13.5" customHeight="1">
       <c r="A351" s="1"/>
       <c r="B351" s="1"/>
       <c r="C351" s="1"/>
@@ -10670,7 +10676,7 @@
       <c r="V351" s="1"/>
       <c r="W351" s="1"/>
     </row>
-    <row r="352" ht="13.5" customHeight="1">
+    <row r="352" spans="1:23" ht="13.5" customHeight="1">
       <c r="A352" s="1"/>
       <c r="B352" s="1"/>
       <c r="C352" s="1"/>
@@ -11345,18 +11351,16 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="C2"/>
-    <hyperlink r:id="rId3" ref="B3"/>
-    <hyperlink r:id="rId4" ref="C3"/>
-    <hyperlink r:id="rId5" ref="B38"/>
-    <hyperlink r:id="rId6" ref="C38"/>
-    <hyperlink r:id="rId7" ref="B75"/>
-    <hyperlink r:id="rId8" ref="C75"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="B38" r:id="rId5"/>
+    <hyperlink ref="C38" r:id="rId6"/>
+    <hyperlink ref="B75" r:id="rId7"/>
+    <hyperlink ref="C75" r:id="rId8"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
28-6-2022 Happy Path Pack Setup
By,
Patrick
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -192,9 +192,6 @@
     <t>MORE INFO VERIFICATION DATA FOR PATIENT TO COLLECT PRESCRIPTION</t>
   </si>
   <si>
-    <t>Dr Tim ( VM04Practice );VM04Practice;Patient to Collect Script;Next Day - Fee: NZ$12.00 (Incl. GST);panadol (optizorb) 500mg caplets(paracetamol);Pending</t>
-  </si>
-  <si>
     <t>DATA FOR SENT SCRIPT BY POST</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
     <t>URGENCY PRICE</t>
   </si>
   <si>
-    <t>Urgent/Same day - Fee: NZ$11.00 (Incl. GST);Next Day - Fee: NZ$12.00 (Incl. GST);48 Hours - Fee: NZ$13.00 (Incl. GST);72 Hours - Fee: NZ$14.00 (Incl. GST)</t>
-  </si>
-  <si>
     <t>EMAIL_FOR_HEALTH</t>
   </si>
   <si>
@@ -760,13 +754,19 @@
   </si>
   <si>
     <t>APPOINTMENT_DETAILS_FOR_JOIN_VIDEO_CONSULTATION</t>
+  </si>
+  <si>
+    <t>Dr Tim ( VM04Practice );VM04Practice;Patient to Collect Script;Next Day - Fee: NZ$;panadol (optizorb) 500mg caplets(paracetamol);Pending</t>
+  </si>
+  <si>
+    <t>Urgent/Same day - Fee: NZ$111.00 (Incl. GST);Next Day - Fee: NZ$112.00 (Incl. GST);48 Hours - Fee: NZ$113.00 (Incl. GST);72 Hours - Fee: NZ$0.00 (Incl. GST)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,6 +826,18 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -899,7 +911,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -909,12 +921,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -940,6 +946,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1159,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2206,7 +2221,7 @@
     </row>
     <row r="36" spans="1:23" ht="13.5" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>42</v>
@@ -2262,10 +2277,10 @@
       <c r="A38" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="16" t="s">
         <v>50</v>
       </c>
       <c r="D38" s="1"/>
@@ -2320,7 +2335,7 @@
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
     </row>
-    <row r="40" spans="1:23" ht="13.5" customHeight="1">
+    <row r="40" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2345,14 +2360,14 @@
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
     </row>
-    <row r="41" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A41" s="7" t="s">
+    <row r="41" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A41" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="19" t="s">
         <v>53</v>
       </c>
       <c r="D41" s="1"/>
@@ -2376,14 +2391,14 @@
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
     </row>
-    <row r="42" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A42" s="7" t="s">
+    <row r="42" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A42" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="19" t="s">
         <v>55</v>
       </c>
       <c r="D42" s="1"/>
@@ -2407,15 +2422,15 @@
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
     </row>
-    <row r="43" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A43" s="7" t="s">
+    <row r="43" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A43" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>57</v>
+      <c r="B43" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>245</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -2438,10 +2453,10 @@
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
     </row>
-    <row r="44" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A44" s="7"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
+    <row r="44" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A44" s="18"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2463,10 +2478,10 @@
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
     </row>
-    <row r="45" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A45" s="7"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
+    <row r="45" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A45" s="18"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2488,15 +2503,15 @@
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
     </row>
-    <row r="46" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A46" s="7" t="s">
+    <row r="46" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A46" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>59</v>
+      <c r="C46" s="19" t="s">
+        <v>58</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -2519,15 +2534,15 @@
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
     </row>
-    <row r="47" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A47" s="7" t="s">
+    <row r="47" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A47" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>61</v>
+      <c r="C47" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -2550,12 +2565,12 @@
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
     </row>
-    <row r="48" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A48" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
+    <row r="48" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A48" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2577,10 +2592,10 @@
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
     </row>
-    <row r="49" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A49" s="7"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
+    <row r="49" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A49" s="18"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2602,10 +2617,10 @@
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
     </row>
-    <row r="50" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A50" s="7"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
+    <row r="50" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A50" s="18"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2627,15 +2642,15 @@
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
     </row>
-    <row r="51" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A51" s="7" t="s">
+    <row r="51" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A51" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>64</v>
+      <c r="C51" s="19" t="s">
+        <v>63</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -2658,15 +2673,15 @@
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
     </row>
-    <row r="52" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A52" s="7" t="s">
+    <row r="52" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A52" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>66</v>
+      <c r="C52" s="19" t="s">
+        <v>65</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -2689,12 +2704,12 @@
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
     </row>
-    <row r="53" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A53" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
+    <row r="53" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A53" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2716,10 +2731,10 @@
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
     </row>
-    <row r="54" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A54" s="7"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
+    <row r="54" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A54" s="18"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -2741,10 +2756,10 @@
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
     </row>
-    <row r="55" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A55" s="7"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
+    <row r="55" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A55" s="18"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -2766,15 +2781,15 @@
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
     </row>
-    <row r="56" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A56" s="7" t="s">
+    <row r="56" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A56" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>69</v>
+      <c r="C56" s="19" t="s">
+        <v>68</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2797,15 +2812,15 @@
       <c r="V56" s="1"/>
       <c r="W56" s="1"/>
     </row>
-    <row r="57" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A57" s="7" t="s">
+    <row r="57" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A57" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>71</v>
+      <c r="C57" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -2828,12 +2843,12 @@
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
     </row>
-    <row r="58" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A58" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
+    <row r="58" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A58" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -2855,10 +2870,10 @@
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
     </row>
-    <row r="59" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A59" s="7"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
+    <row r="59" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A59" s="18"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -2880,10 +2895,10 @@
       <c r="V59" s="1"/>
       <c r="W59" s="1"/>
     </row>
-    <row r="60" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A60" s="7"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
+    <row r="60" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A60" s="18"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -2905,15 +2920,15 @@
       <c r="V60" s="1"/>
       <c r="W60" s="1"/>
     </row>
-    <row r="61" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A61" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>69</v>
+    <row r="61" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A61" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61" s="19" t="s">
+        <v>68</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
@@ -2936,15 +2951,15 @@
       <c r="V61" s="1"/>
       <c r="W61" s="1"/>
     </row>
-    <row r="62" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A62" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>71</v>
+    <row r="62" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A62" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -2967,10 +2982,10 @@
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
     </row>
-    <row r="63" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A63" s="7"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
+    <row r="63" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A63" s="18"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -2992,10 +3007,10 @@
       <c r="V63" s="1"/>
       <c r="W63" s="1"/>
     </row>
-    <row r="64" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A64" s="7"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
+    <row r="64" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A64" s="18"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="19"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -3017,15 +3032,15 @@
       <c r="V64" s="1"/>
       <c r="W64" s="1"/>
     </row>
-    <row r="65" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A65" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>69</v>
+    <row r="65" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A65" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>68</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -3048,15 +3063,15 @@
       <c r="V65" s="1"/>
       <c r="W65" s="1"/>
     </row>
-    <row r="66" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A66" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>71</v>
+    <row r="66" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A66" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -3079,10 +3094,10 @@
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
     </row>
-    <row r="67" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A67" s="7"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
+    <row r="67" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A67" s="18"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -3104,10 +3119,10 @@
       <c r="V67" s="1"/>
       <c r="W67" s="1"/>
     </row>
-    <row r="68" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A68" s="7"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
+    <row r="68" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A68" s="18"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="19"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -3129,15 +3144,15 @@
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
     </row>
-    <row r="69" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A69" s="7" t="s">
+    <row r="69" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A69" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>78</v>
+      <c r="C69" s="19" t="s">
+        <v>77</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -3160,15 +3175,15 @@
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
     </row>
-    <row r="70" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A70" s="7" t="s">
+    <row r="70" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A70" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>80</v>
+      <c r="C70" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -3191,15 +3206,15 @@
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
     </row>
-    <row r="71" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A71" s="7" t="s">
+    <row r="71" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A71" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>82</v>
+      <c r="C71" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -3222,15 +3237,15 @@
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
     </row>
-    <row r="72" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A72" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>84</v>
+    <row r="72" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A72" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>246</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -3278,7 +3293,7 @@
       <c r="V73" s="1"/>
       <c r="W73" s="1"/>
     </row>
-    <row r="74" spans="1:23" ht="13.5" customHeight="1">
+    <row r="74" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -3303,14 +3318,14 @@
       <c r="V74" s="1"/>
       <c r="W74" s="1"/>
     </row>
-    <row r="75" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A75" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B75" s="10" t="s">
+    <row r="75" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A75" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C75" s="18" t="s">
+      <c r="C75" s="16" t="s">
         <v>50</v>
       </c>
       <c r="D75" s="1"/>
@@ -3334,11 +3349,11 @@
       <c r="V75" s="1"/>
       <c r="W75" s="1"/>
     </row>
-    <row r="76" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A76" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B76" s="12" t="s">
+    <row r="76" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A76" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B76" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C76" s="6" t="s">
@@ -3366,8 +3381,8 @@
       <c r="W76" s="1"/>
     </row>
     <row r="77" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A77" s="13"/>
-      <c r="B77" s="14"/>
+      <c r="A77" s="11"/>
+      <c r="B77" s="12"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -3391,14 +3406,14 @@
       <c r="W77" s="1"/>
     </row>
     <row r="78" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A78" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B78" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C78" s="15" t="s">
-        <v>88</v>
+      <c r="A78" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>86</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -3422,14 +3437,14 @@
       <c r="W78" s="1"/>
     </row>
     <row r="79" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A79" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B79" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C79" s="15" t="s">
-        <v>90</v>
+      <c r="A79" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C79" s="13" t="s">
+        <v>88</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -3453,14 +3468,14 @@
       <c r="W79" s="1"/>
     </row>
     <row r="80" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A80" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B80" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C80" s="15" t="s">
-        <v>92</v>
+      <c r="A80" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C80" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -3484,14 +3499,14 @@
       <c r="W80" s="1"/>
     </row>
     <row r="81" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A81" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B81" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C81" s="15" t="s">
-        <v>94</v>
+      <c r="A81" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -3515,14 +3530,14 @@
       <c r="W81" s="1"/>
     </row>
     <row r="82" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A82" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>96</v>
+      <c r="A82" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B82" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -3546,14 +3561,14 @@
       <c r="W82" s="1"/>
     </row>
     <row r="83" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A83" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="B83" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>98</v>
+      <c r="A83" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -3577,14 +3592,14 @@
       <c r="W83" s="1"/>
     </row>
     <row r="84" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A84" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C84" s="14" t="s">
-        <v>100</v>
+      <c r="A84" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -3608,14 +3623,14 @@
       <c r="W84" s="1"/>
     </row>
     <row r="85" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A85" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="B85" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>102</v>
+      <c r="A85" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -3639,14 +3654,14 @@
       <c r="W85" s="1"/>
     </row>
     <row r="86" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A86" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="B86" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C86" s="14" t="s">
-        <v>104</v>
+      <c r="A86" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>102</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -3670,14 +3685,14 @@
       <c r="W86" s="1"/>
     </row>
     <row r="87" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A87" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="B87" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C87" s="14" t="s">
-        <v>106</v>
+      <c r="A87" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -3701,14 +3716,14 @@
       <c r="W87" s="1"/>
     </row>
     <row r="88" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A88" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B88" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C88" s="14" t="s">
-        <v>108</v>
+      <c r="A88" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C88" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -3732,14 +3747,14 @@
       <c r="W88" s="1"/>
     </row>
     <row r="89" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A89" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="B89" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>110</v>
+      <c r="A89" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B89" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -3763,14 +3778,14 @@
       <c r="W89" s="1"/>
     </row>
     <row r="90" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A90" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B90" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>112</v>
+      <c r="A90" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>110</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -3794,14 +3809,14 @@
       <c r="W90" s="1"/>
     </row>
     <row r="91" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A91" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B91" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>114</v>
+      <c r="A91" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -3825,14 +3840,14 @@
       <c r="W91" s="1"/>
     </row>
     <row r="92" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A92" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="B92" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>116</v>
+      <c r="A92" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B92" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -3856,14 +3871,14 @@
       <c r="W92" s="1"/>
     </row>
     <row r="93" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A93" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="B93" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C93" s="15" t="s">
-        <v>118</v>
+      <c r="A93" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -3887,14 +3902,14 @@
       <c r="W93" s="1"/>
     </row>
     <row r="94" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A94" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="B94" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C94" s="14" t="s">
-        <v>120</v>
+      <c r="A94" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -3918,14 +3933,14 @@
       <c r="W94" s="1"/>
     </row>
     <row r="95" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A95" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="B95" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="C95" s="14" t="s">
-        <v>122</v>
+      <c r="A95" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C95" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -3949,14 +3964,14 @@
       <c r="W95" s="1"/>
     </row>
     <row r="96" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A96" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="B96" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C96" s="14" t="s">
-        <v>124</v>
+      <c r="A96" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>122</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -3980,14 +3995,14 @@
       <c r="W96" s="1"/>
     </row>
     <row r="97" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A97" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="B97" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C97" s="19" t="s">
-        <v>126</v>
+      <c r="A97" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B97" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C97" s="17" t="s">
+        <v>124</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -4011,14 +4026,14 @@
       <c r="W97" s="1"/>
     </row>
     <row r="98" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A98" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="B98" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="C98" s="14" t="s">
-        <v>128</v>
+      <c r="A98" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C98" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -4042,14 +4057,14 @@
       <c r="W98" s="1"/>
     </row>
     <row r="99" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A99" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="B99" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="C99" s="14" t="s">
-        <v>130</v>
+      <c r="A99" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C99" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -4073,14 +4088,14 @@
       <c r="W99" s="1"/>
     </row>
     <row r="100" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A100" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B100" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="C100" s="19" t="s">
-        <v>132</v>
+      <c r="A100" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C100" s="17" t="s">
+        <v>130</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -4104,14 +4119,14 @@
       <c r="W100" s="1"/>
     </row>
     <row r="101" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A101" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B101" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C101" s="14" t="s">
-        <v>134</v>
+      <c r="A101" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>132</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -4135,14 +4150,14 @@
       <c r="W101" s="1"/>
     </row>
     <row r="102" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A102" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="B102" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C102" s="15" t="s">
-        <v>136</v>
+      <c r="A102" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B102" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>134</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -4166,14 +4181,14 @@
       <c r="W102" s="1"/>
     </row>
     <row r="103" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A103" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="B103" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C103" s="15" t="s">
-        <v>138</v>
+      <c r="A103" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B103" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>136</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
@@ -4197,14 +4212,14 @@
       <c r="W103" s="1"/>
     </row>
     <row r="104" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A104" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B104" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C104" s="15" t="s">
-        <v>140</v>
+      <c r="A104" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B104" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
@@ -4228,14 +4243,14 @@
       <c r="W104" s="1"/>
     </row>
     <row r="105" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A105" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B105" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="C105" s="14" t="s">
-        <v>142</v>
+      <c r="A105" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C105" s="12" t="s">
+        <v>140</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
@@ -4259,14 +4274,14 @@
       <c r="W105" s="1"/>
     </row>
     <row r="106" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A106" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="B106" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="C106" s="19" t="s">
-        <v>144</v>
+      <c r="A106" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B106" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C106" s="17" t="s">
+        <v>142</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
@@ -4290,14 +4305,14 @@
       <c r="W106" s="1"/>
     </row>
     <row r="107" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A107" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="B107" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C107" s="15" t="s">
-        <v>146</v>
+      <c r="A107" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>144</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
@@ -4321,14 +4336,14 @@
       <c r="W107" s="1"/>
     </row>
     <row r="108" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A108" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B108" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C108" s="15" t="s">
-        <v>148</v>
+      <c r="A108" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B108" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C108" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
@@ -4352,14 +4367,14 @@
       <c r="W108" s="1"/>
     </row>
     <row r="109" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A109" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="B109" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="C109" s="14" t="s">
-        <v>150</v>
+      <c r="A109" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B109" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C109" s="12" t="s">
+        <v>148</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
@@ -4383,14 +4398,14 @@
       <c r="W109" s="1"/>
     </row>
     <row r="110" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A110" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="B110" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C110" s="14" t="s">
-        <v>152</v>
+      <c r="A110" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B110" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>150</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
@@ -4414,14 +4429,14 @@
       <c r="W110" s="1"/>
     </row>
     <row r="111" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A111" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="B111" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="C111" s="19" t="s">
-        <v>154</v>
+      <c r="A111" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B111" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C111" s="17" t="s">
+        <v>152</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
@@ -4445,14 +4460,14 @@
       <c r="W111" s="1"/>
     </row>
     <row r="112" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A112" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="B112" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="C112" s="15" t="s">
-        <v>156</v>
+      <c r="A112" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B112" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C112" s="13" t="s">
+        <v>154</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
@@ -4476,14 +4491,14 @@
       <c r="W112" s="1"/>
     </row>
     <row r="113" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A113" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="B113" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="C113" s="14" t="s">
-        <v>158</v>
+      <c r="A113" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B113" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C113" s="12" t="s">
+        <v>156</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
@@ -4507,14 +4522,14 @@
       <c r="W113" s="1"/>
     </row>
     <row r="114" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A114" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="B114" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="C114" s="15" t="s">
-        <v>160</v>
+      <c r="A114" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B114" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C114" s="13" t="s">
+        <v>158</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
@@ -4538,14 +4553,14 @@
       <c r="W114" s="1"/>
     </row>
     <row r="115" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A115" s="14" t="s">
+      <c r="A115" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B115" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C115" s="12" t="s">
         <v>161</v>
-      </c>
-      <c r="B115" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C115" s="14" t="s">
-        <v>163</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
@@ -4569,14 +4584,14 @@
       <c r="W115" s="1"/>
     </row>
     <row r="116" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A116" s="14" t="s">
+      <c r="A116" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B116" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C116" s="13" t="s">
         <v>164</v>
-      </c>
-      <c r="B116" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C116" s="15" t="s">
-        <v>166</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
@@ -4600,14 +4615,14 @@
       <c r="W116" s="1"/>
     </row>
     <row r="117" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A117" s="14" t="s">
+      <c r="A117" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B117" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C117" s="12" t="s">
         <v>167</v>
-      </c>
-      <c r="B117" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="C117" s="14" t="s">
-        <v>169</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
@@ -4631,14 +4646,14 @@
       <c r="W117" s="1"/>
     </row>
     <row r="118" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A118" s="14" t="s">
+      <c r="A118" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B118" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C118" s="13" t="s">
         <v>170</v>
-      </c>
-      <c r="B118" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="C118" s="15" t="s">
-        <v>172</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
@@ -4662,14 +4677,14 @@
       <c r="W118" s="1"/>
     </row>
     <row r="119" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A119" s="14" t="s">
+      <c r="A119" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B119" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C119" s="12" t="s">
         <v>173</v>
-      </c>
-      <c r="B119" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="C119" s="14" t="s">
-        <v>175</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
@@ -4693,14 +4708,14 @@
       <c r="W119" s="1"/>
     </row>
     <row r="120" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A120" s="14" t="s">
+      <c r="A120" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B120" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C120" s="12" t="s">
         <v>176</v>
-      </c>
-      <c r="B120" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="C120" s="14" t="s">
-        <v>178</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
@@ -4724,14 +4739,14 @@
       <c r="W120" s="1"/>
     </row>
     <row r="121" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A121" s="14" t="s">
+      <c r="A121" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B121" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="C121" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="B121" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="C121" s="14" t="s">
-        <v>181</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -4755,10 +4770,10 @@
       <c r="W121" s="1"/>
     </row>
     <row r="122" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A122" s="14"/>
-      <c r="B122" s="14"/>
-      <c r="C122" s="14" t="s">
-        <v>182</v>
+      <c r="A122" s="12"/>
+      <c r="B122" s="12"/>
+      <c r="C122" s="12" t="s">
+        <v>180</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
@@ -4782,14 +4797,14 @@
       <c r="W122" s="1"/>
     </row>
     <row r="123" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A123" s="14" t="s">
+      <c r="A123" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B123" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C123" s="12" t="s">
         <v>183</v>
-      </c>
-      <c r="B123" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C123" s="14" t="s">
-        <v>185</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
@@ -4813,10 +4828,10 @@
       <c r="W123" s="1"/>
     </row>
     <row r="124" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A124" s="14"/>
-      <c r="B124" s="14"/>
-      <c r="C124" s="14" t="s">
-        <v>186</v>
+      <c r="A124" s="12"/>
+      <c r="B124" s="12"/>
+      <c r="C124" s="12" t="s">
+        <v>184</v>
       </c>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
@@ -4840,14 +4855,14 @@
       <c r="W124" s="1"/>
     </row>
     <row r="125" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A125" s="14" t="s">
+      <c r="A125" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B125" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C125" s="12" t="s">
         <v>187</v>
-      </c>
-      <c r="B125" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="C125" s="14" t="s">
-        <v>189</v>
       </c>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
@@ -4871,14 +4886,14 @@
       <c r="W125" s="1"/>
     </row>
     <row r="126" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A126" s="14" t="s">
+      <c r="A126" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B126" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C126" s="13" t="s">
         <v>190</v>
-      </c>
-      <c r="B126" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="C126" s="15" t="s">
-        <v>192</v>
       </c>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
@@ -4902,14 +4917,14 @@
       <c r="W126" s="1"/>
     </row>
     <row r="127" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A127" s="14" t="s">
+      <c r="A127" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B127" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="C127" s="12" t="s">
         <v>193</v>
-      </c>
-      <c r="B127" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="C127" s="14" t="s">
-        <v>195</v>
       </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
@@ -4933,14 +4948,14 @@
       <c r="W127" s="1"/>
     </row>
     <row r="128" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A128" s="14" t="s">
+      <c r="A128" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B128" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C128" s="12" t="s">
         <v>196</v>
-      </c>
-      <c r="B128" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="C128" s="14" t="s">
-        <v>198</v>
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
@@ -4964,14 +4979,14 @@
       <c r="W128" s="1"/>
     </row>
     <row r="129" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A129" s="14" t="s">
+      <c r="A129" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B129" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="C129" s="12" t="s">
         <v>199</v>
-      </c>
-      <c r="B129" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="C129" s="14" t="s">
-        <v>201</v>
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
@@ -4995,14 +5010,14 @@
       <c r="W129" s="1"/>
     </row>
     <row r="130" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A130" s="14" t="s">
+      <c r="A130" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B130" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C130" s="13" t="s">
         <v>202</v>
-      </c>
-      <c r="B130" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="C130" s="15" t="s">
-        <v>204</v>
       </c>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
@@ -5026,14 +5041,14 @@
       <c r="W130" s="1"/>
     </row>
     <row r="131" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A131" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="B131" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="C131" s="14" t="s">
-        <v>206</v>
+      <c r="A131" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="B131" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C131" s="12" t="s">
+        <v>204</v>
       </c>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
@@ -5057,14 +5072,14 @@
       <c r="W131" s="1"/>
     </row>
     <row r="132" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A132" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B132" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="C132" s="14" t="s">
-        <v>208</v>
+      <c r="A132" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B132" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C132" s="12" t="s">
+        <v>206</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
@@ -5088,14 +5103,14 @@
       <c r="W132" s="1"/>
     </row>
     <row r="133" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A133" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="B133" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="C133" s="14" t="s">
-        <v>210</v>
+      <c r="A133" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B133" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C133" s="12" t="s">
+        <v>208</v>
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
@@ -5119,14 +5134,14 @@
       <c r="W133" s="1"/>
     </row>
     <row r="134" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A134" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="B134" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="C134" s="14" t="s">
-        <v>212</v>
+      <c r="A134" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B134" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C134" s="12" t="s">
+        <v>210</v>
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
@@ -5150,14 +5165,14 @@
       <c r="W134" s="1"/>
     </row>
     <row r="135" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A135" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="B135" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="C135" s="14" t="s">
-        <v>214</v>
+      <c r="A135" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B135" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C135" s="12" t="s">
+        <v>212</v>
       </c>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
@@ -5181,14 +5196,14 @@
       <c r="W135" s="1"/>
     </row>
     <row r="136" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A136" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="B136" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="C136" s="14" t="s">
-        <v>216</v>
+      <c r="A136" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="B136" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="C136" s="12" t="s">
+        <v>214</v>
       </c>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
@@ -5212,14 +5227,14 @@
       <c r="W136" s="1"/>
     </row>
     <row r="137" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A137" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="B137" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="C137" s="14" t="s">
-        <v>218</v>
+      <c r="A137" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B137" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C137" s="12" t="s">
+        <v>216</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
@@ -5243,9 +5258,9 @@
       <c r="W137" s="1"/>
     </row>
     <row r="138" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A138" s="14"/>
-      <c r="B138" s="14"/>
-      <c r="C138" s="14"/>
+      <c r="A138" s="12"/>
+      <c r="B138" s="12"/>
+      <c r="C138" s="12"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -5268,14 +5283,14 @@
       <c r="W138" s="1"/>
     </row>
     <row r="139" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A139" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="B139" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="C139" s="14" t="s">
-        <v>220</v>
+      <c r="A139" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="B139" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="C139" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -5299,14 +5314,14 @@
       <c r="W139" s="1"/>
     </row>
     <row r="140" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A140" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="B140" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="C140" s="14" t="s">
-        <v>222</v>
+      <c r="A140" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B140" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>220</v>
       </c>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
@@ -5330,14 +5345,14 @@
       <c r="W140" s="1"/>
     </row>
     <row r="141" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A141" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="B141" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="C141" s="14" t="s">
-        <v>224</v>
+      <c r="A141" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B141" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="C141" s="12" t="s">
+        <v>222</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
@@ -5361,14 +5376,14 @@
       <c r="W141" s="1"/>
     </row>
     <row r="142" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A142" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="B142" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="C142" s="14" t="s">
-        <v>226</v>
+      <c r="A142" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B142" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="C142" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
@@ -5392,14 +5407,14 @@
       <c r="W142" s="1"/>
     </row>
     <row r="143" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A143" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="B143" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="C143" s="14" t="s">
-        <v>228</v>
+      <c r="A143" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B143" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C143" s="12" t="s">
+        <v>226</v>
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
@@ -5423,14 +5438,14 @@
       <c r="W143" s="1"/>
     </row>
     <row r="144" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A144" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="B144" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="C144" s="14" t="s">
-        <v>229</v>
+      <c r="A144" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B144" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C144" s="12" t="s">
+        <v>227</v>
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
@@ -5454,14 +5469,14 @@
       <c r="W144" s="1"/>
     </row>
     <row r="145" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A145" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="B145" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="C145" s="14" t="s">
-        <v>226</v>
+      <c r="A145" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B145" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="C145" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
@@ -5485,14 +5500,14 @@
       <c r="W145" s="1"/>
     </row>
     <row r="146" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A146" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="B146" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="C146" s="14" t="s">
-        <v>228</v>
+      <c r="A146" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B146" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C146" s="12" t="s">
+        <v>226</v>
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
@@ -5516,14 +5531,14 @@
       <c r="W146" s="1"/>
     </row>
     <row r="147" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A147" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="B147" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="C147" s="14" t="s">
-        <v>231</v>
+      <c r="A147" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="B147" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="C147" s="12" t="s">
+        <v>229</v>
       </c>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -5547,14 +5562,14 @@
       <c r="W147" s="1"/>
     </row>
     <row r="148" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A148" s="14" t="s">
+      <c r="A148" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B148" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C148" s="12" t="s">
         <v>232</v>
-      </c>
-      <c r="B148" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="C148" s="14" t="s">
-        <v>234</v>
       </c>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
@@ -5578,14 +5593,14 @@
       <c r="W148" s="1"/>
     </row>
     <row r="149" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A149" s="14" t="s">
+      <c r="A149" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="B149" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="C149" s="13" t="s">
         <v>235</v>
-      </c>
-      <c r="B149" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="C149" s="15" t="s">
-        <v>237</v>
       </c>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
@@ -5609,14 +5624,14 @@
       <c r="W149" s="1"/>
     </row>
     <row r="150" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A150" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="B150" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="C150" s="14" t="s">
-        <v>239</v>
+      <c r="A150" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="B150" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C150" s="12" t="s">
+        <v>237</v>
       </c>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
@@ -5640,14 +5655,14 @@
       <c r="W150" s="1"/>
     </row>
     <row r="151" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A151" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="B151" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="C151" s="14" t="s">
-        <v>241</v>
+      <c r="A151" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B151" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="C151" s="12" t="s">
+        <v>239</v>
       </c>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
@@ -5671,14 +5686,14 @@
       <c r="W151" s="1"/>
     </row>
     <row r="152" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A152" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="B152" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="C152" s="14" t="s">
-        <v>243</v>
+      <c r="A152" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B152" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="C152" s="12" t="s">
+        <v>241</v>
       </c>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
@@ -5702,11 +5717,11 @@
       <c r="W152" s="1"/>
     </row>
     <row r="153" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A153" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="B153" s="17" t="s">
-        <v>245</v>
+      <c r="A153" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B153" s="15" t="s">
+        <v>243</v>
       </c>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
@@ -11357,8 +11372,8 @@
     <hyperlink ref="C3" r:id="rId4"/>
     <hyperlink ref="B38" r:id="rId5"/>
     <hyperlink ref="C38" r:id="rId6"/>
-    <hyperlink ref="B75" r:id="rId7"/>
-    <hyperlink ref="C75" r:id="rId8"/>
+    <hyperlink ref="C75" r:id="rId7"/>
+    <hyperlink ref="B75" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Messages module completed commit by patrick
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Patrick-Codoid\Naveen\Appointments_Updated\config\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Inlogic\clone\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="MMH" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="285">
   <si>
     <t>KEY</t>
   </si>
@@ -760,13 +760,127 @@
   </si>
   <si>
     <t>Urgent/Same day - Fee: NZ$111.00 (Incl. GST);Next Day - Fee: NZ$112.00 (Incl. GST);48 Hours - Fee: NZ$113.00 (Incl. GST);72 Hours - Fee: NZ$0.00 (Incl. GST)</t>
+  </si>
+  <si>
+    <t>MESSAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VM03Location;VM03Location;Lab results enquiry;Clinical Staff;Dr Tim;Lab results enquiry;successfuly;MMHtest.jpg </t>
+  </si>
+  <si>
+    <t>SEND_DATA</t>
+  </si>
+  <si>
+    <t>HARRY HARRY;Dr Tim;Lab results enquiry;Lab results enquiry</t>
+  </si>
+  <si>
+    <t>DRAFT_DATA</t>
+  </si>
+  <si>
+    <t>VM03Location;Lab results enquiry;Clinical Staff;Dr Tim</t>
+  </si>
+  <si>
+    <t>DEV_URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dev.mmh-demo.com/m/Main/Login#info;tim@mmh-demo.com;Manage@123;MMHtest.jpg </t>
+  </si>
+  <si>
+    <t>INBOX_DATA</t>
+  </si>
+  <si>
+    <t>Dr Tim;HARRY HARRY;Lab results enquiry;Lab results enquiry</t>
+  </si>
+  <si>
+    <t>REPLY_DATA</t>
+  </si>
+  <si>
+    <t>GROUP_MESSAGE_DATA</t>
+  </si>
+  <si>
+    <t>VM03Location;Test Group Message -SB</t>
+  </si>
+  <si>
+    <t>EMAIL FOR MESSAGE</t>
+  </si>
+  <si>
+    <t>PASSWORD FOR MESSAGE</t>
+  </si>
+  <si>
+    <t>TIME_OUT_SETTING</t>
+  </si>
+  <si>
+    <t>2 Hour</t>
+  </si>
+  <si>
+    <t>ALERT TYPE</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>SIGNATURE MESSAGE</t>
+  </si>
+  <si>
+    <t>Signature Testing</t>
+  </si>
+  <si>
+    <t>START DATE</t>
+  </si>
+  <si>
+    <t>END DATE</t>
+  </si>
+  <si>
+    <t>OUT OF MESSAGE</t>
+  </si>
+  <si>
+    <t>Out of Office Testing</t>
+  </si>
+  <si>
+    <t>AUTOMATIC REPLY MESSAGE</t>
+  </si>
+  <si>
+    <t>Automatic Reply Message Testing</t>
+  </si>
+  <si>
+    <t>OUT_OF_OFFICE_MESSAGE_DETAILS</t>
+  </si>
+  <si>
+    <t>VM03Location;VM03Location;Patient Communication-S;Patient;Harry Harry;Out of office reply testing;Body : Out of office reply testing</t>
+  </si>
+  <si>
+    <t>HARRY HARRY;Patient Communication-S;Out of Office Testing</t>
+  </si>
+  <si>
+    <t>AUTOMATIC_MESSAGE_DETAILS</t>
+  </si>
+  <si>
+    <t>VM03Location;VM03Location;Patient Communication-S;Patient;Harry Harry;Automatic Reply Message Testing;Body : Automatic reply testing</t>
+  </si>
+  <si>
+    <t>VERIFY_DATA_FOR_ARM</t>
+  </si>
+  <si>
+    <t>HARRY HARRY;Patient Communication-S;Automatic Reply Message Testing</t>
+  </si>
+  <si>
+    <t>EMAIL FOR DOCTOR</t>
+  </si>
+  <si>
+    <t>tim@mmh-demo.com</t>
+  </si>
+  <si>
+    <t>V1 URL</t>
+  </si>
+  <si>
+    <t>PASSWORD FOR DOCTOR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -835,6 +949,39 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF297BDE"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -911,7 +1058,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -957,6 +1104,30 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1172,18 +1343,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="69.5703125" customWidth="1"/>
-    <col min="2" max="2" width="157.140625" customWidth="1"/>
-    <col min="3" max="3" width="125.140625" customWidth="1"/>
-    <col min="4" max="23" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="69.54296875" customWidth="1"/>
+    <col min="2" max="2" width="157.1796875" customWidth="1"/>
+    <col min="3" max="3" width="125.1796875" customWidth="1"/>
+    <col min="4" max="23" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="13.5" customHeight="1">
@@ -5468,7 +5639,7 @@
       <c r="V144" s="1"/>
       <c r="W144" s="1"/>
     </row>
-    <row r="145" spans="1:23" ht="13.5" customHeight="1">
+    <row r="145" spans="1:26" ht="13.5" customHeight="1">
       <c r="A145" s="12" t="s">
         <v>223</v>
       </c>
@@ -5499,7 +5670,7 @@
       <c r="V145" s="1"/>
       <c r="W145" s="1"/>
     </row>
-    <row r="146" spans="1:23" ht="13.5" customHeight="1">
+    <row r="146" spans="1:26" ht="13.5" customHeight="1">
       <c r="A146" s="12" t="s">
         <v>225</v>
       </c>
@@ -5530,7 +5701,7 @@
       <c r="V146" s="1"/>
       <c r="W146" s="1"/>
     </row>
-    <row r="147" spans="1:23" ht="13.5" customHeight="1">
+    <row r="147" spans="1:26" ht="13.5" customHeight="1">
       <c r="A147" s="12" t="s">
         <v>228</v>
       </c>
@@ -5561,7 +5732,7 @@
       <c r="V147" s="1"/>
       <c r="W147" s="1"/>
     </row>
-    <row r="148" spans="1:23" ht="13.5" customHeight="1">
+    <row r="148" spans="1:26" ht="13.5" customHeight="1">
       <c r="A148" s="12" t="s">
         <v>230</v>
       </c>
@@ -5592,7 +5763,7 @@
       <c r="V148" s="1"/>
       <c r="W148" s="1"/>
     </row>
-    <row r="149" spans="1:23" ht="13.5" customHeight="1">
+    <row r="149" spans="1:26" ht="13.5" customHeight="1">
       <c r="A149" s="12" t="s">
         <v>233</v>
       </c>
@@ -5623,7 +5794,7 @@
       <c r="V149" s="1"/>
       <c r="W149" s="1"/>
     </row>
-    <row r="150" spans="1:23" ht="13.5" customHeight="1">
+    <row r="150" spans="1:26" ht="13.5" customHeight="1">
       <c r="A150" s="12" t="s">
         <v>236</v>
       </c>
@@ -5654,7 +5825,7 @@
       <c r="V150" s="1"/>
       <c r="W150" s="1"/>
     </row>
-    <row r="151" spans="1:23" ht="13.5" customHeight="1">
+    <row r="151" spans="1:26" ht="13.5" customHeight="1">
       <c r="A151" s="12" t="s">
         <v>238</v>
       </c>
@@ -5685,7 +5856,7 @@
       <c r="V151" s="1"/>
       <c r="W151" s="1"/>
     </row>
-    <row r="152" spans="1:23" ht="13.5" customHeight="1">
+    <row r="152" spans="1:26" ht="13.5" customHeight="1">
       <c r="A152" s="12" t="s">
         <v>240</v>
       </c>
@@ -5716,7 +5887,7 @@
       <c r="V152" s="1"/>
       <c r="W152" s="1"/>
     </row>
-    <row r="153" spans="1:23" ht="13.5" customHeight="1">
+    <row r="153" spans="1:26" ht="13.5" customHeight="1">
       <c r="A153" s="12" t="s">
         <v>242</v>
       </c>
@@ -5745,7 +5916,7 @@
       <c r="V153" s="1"/>
       <c r="W153" s="1"/>
     </row>
-    <row r="154" spans="1:23" ht="13.5" customHeight="1">
+    <row r="154" spans="1:26" ht="13.5" customHeight="1">
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
@@ -5768,7 +5939,7 @@
       <c r="V154" s="1"/>
       <c r="W154" s="1"/>
     </row>
-    <row r="155" spans="1:23" ht="13.5" customHeight="1">
+    <row r="155" spans="1:26" ht="13.5" customHeight="1">
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -5791,85 +5962,116 @@
       <c r="V155" s="1"/>
       <c r="W155" s="1"/>
     </row>
-    <row r="156" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A156" s="1"/>
-      <c r="B156" s="1"/>
-      <c r="C156" s="1"/>
-      <c r="D156" s="1"/>
-      <c r="E156" s="1"/>
-      <c r="F156" s="1"/>
-      <c r="G156" s="1"/>
-      <c r="H156" s="1"/>
-      <c r="I156" s="1"/>
-      <c r="J156" s="1"/>
-      <c r="K156" s="1"/>
-      <c r="L156" s="1"/>
-      <c r="M156" s="1"/>
-      <c r="N156" s="1"/>
-      <c r="O156" s="1"/>
-      <c r="P156" s="1"/>
-      <c r="Q156" s="1"/>
-      <c r="R156" s="1"/>
-      <c r="S156" s="1"/>
-      <c r="T156" s="1"/>
-      <c r="U156" s="1"/>
-      <c r="V156" s="1"/>
-      <c r="W156" s="1"/>
-    </row>
-    <row r="157" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A157" s="1"/>
-      <c r="B157" s="1"/>
-      <c r="C157" s="1"/>
-      <c r="D157" s="1"/>
-      <c r="E157" s="1"/>
-      <c r="F157" s="1"/>
-      <c r="G157" s="1"/>
-      <c r="H157" s="1"/>
-      <c r="I157" s="1"/>
-      <c r="J157" s="1"/>
-      <c r="K157" s="1"/>
-      <c r="L157" s="1"/>
-      <c r="M157" s="1"/>
-      <c r="N157" s="1"/>
-      <c r="O157" s="1"/>
-      <c r="P157" s="1"/>
-      <c r="Q157" s="1"/>
-      <c r="R157" s="1"/>
-      <c r="S157" s="1"/>
-      <c r="T157" s="1"/>
-      <c r="U157" s="1"/>
-      <c r="V157" s="1"/>
-      <c r="W157" s="1"/>
-    </row>
-    <row r="158" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A158" s="1"/>
-      <c r="B158" s="1"/>
-      <c r="C158" s="1"/>
-      <c r="D158" s="1"/>
-      <c r="E158" s="1"/>
-      <c r="F158" s="1"/>
-      <c r="G158" s="1"/>
-      <c r="H158" s="1"/>
-      <c r="I158" s="1"/>
-      <c r="J158" s="1"/>
-      <c r="K158" s="1"/>
-      <c r="L158" s="1"/>
-      <c r="M158" s="1"/>
-      <c r="N158" s="1"/>
-      <c r="O158" s="1"/>
-      <c r="P158" s="1"/>
-      <c r="Q158" s="1"/>
-      <c r="R158" s="1"/>
-      <c r="S158" s="1"/>
-      <c r="T158" s="1"/>
-      <c r="U158" s="1"/>
-      <c r="V158" s="1"/>
-      <c r="W158" s="1"/>
-    </row>
-    <row r="159" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A159" s="1"/>
-      <c r="B159" s="1"/>
-      <c r="C159" s="1"/>
+    <row r="156" spans="1:26" s="30" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A156" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="B156" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C156" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D156" s="21"/>
+      <c r="E156" s="21"/>
+      <c r="F156" s="21"/>
+      <c r="G156" s="21"/>
+      <c r="H156" s="21"/>
+      <c r="I156" s="21"/>
+      <c r="J156" s="21"/>
+      <c r="K156" s="21"/>
+      <c r="L156" s="21"/>
+      <c r="M156" s="21"/>
+      <c r="N156" s="21"/>
+      <c r="O156" s="21"/>
+      <c r="P156" s="21"/>
+      <c r="Q156" s="21"/>
+      <c r="R156" s="21"/>
+      <c r="S156" s="21"/>
+      <c r="T156" s="21"/>
+      <c r="U156" s="21"/>
+      <c r="V156" s="21"/>
+      <c r="W156" s="21"/>
+      <c r="X156" s="26"/>
+      <c r="Y156" s="26"/>
+      <c r="Z156" s="26"/>
+    </row>
+    <row r="157" spans="1:26" s="30" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A157" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="B157" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="C157" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="D157" s="21"/>
+      <c r="E157" s="21"/>
+      <c r="F157" s="21"/>
+      <c r="G157" s="21"/>
+      <c r="H157" s="21"/>
+      <c r="I157" s="21"/>
+      <c r="J157" s="21"/>
+      <c r="K157" s="21"/>
+      <c r="L157" s="21"/>
+      <c r="M157" s="21"/>
+      <c r="N157" s="21"/>
+      <c r="O157" s="21"/>
+      <c r="P157" s="21"/>
+      <c r="Q157" s="21"/>
+      <c r="R157" s="21"/>
+      <c r="S157" s="21"/>
+      <c r="T157" s="21"/>
+      <c r="U157" s="21"/>
+      <c r="V157" s="21"/>
+      <c r="W157" s="21"/>
+      <c r="X157" s="26"/>
+      <c r="Y157" s="26"/>
+      <c r="Z157" s="26"/>
+    </row>
+    <row r="158" spans="1:26" s="30" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A158" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="B158" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C158" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D158" s="21"/>
+      <c r="E158" s="21"/>
+      <c r="F158" s="21"/>
+      <c r="G158" s="21"/>
+      <c r="H158" s="21"/>
+      <c r="I158" s="21"/>
+      <c r="J158" s="21"/>
+      <c r="K158" s="21"/>
+      <c r="L158" s="21"/>
+      <c r="M158" s="21"/>
+      <c r="N158" s="21"/>
+      <c r="O158" s="21"/>
+      <c r="P158" s="21"/>
+      <c r="Q158" s="21"/>
+      <c r="R158" s="21"/>
+      <c r="S158" s="21"/>
+      <c r="T158" s="21"/>
+      <c r="U158" s="21"/>
+      <c r="V158" s="21"/>
+      <c r="W158" s="21"/>
+      <c r="X158" s="26"/>
+      <c r="Y158" s="26"/>
+      <c r="Z158" s="26"/>
+    </row>
+    <row r="159" spans="1:26" ht="13.5" customHeight="1">
+      <c r="A159" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="B159" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C159" s="21"/>
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
@@ -5891,10 +6093,14 @@
       <c r="V159" s="1"/>
       <c r="W159" s="1"/>
     </row>
-    <row r="160" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A160" s="1"/>
-      <c r="B160" s="1"/>
-      <c r="C160" s="1"/>
+    <row r="160" spans="1:26" ht="13.5" customHeight="1">
+      <c r="A160" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="B160" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="C160" s="21"/>
       <c r="D160" s="1"/>
       <c r="E160" s="1"/>
       <c r="F160" s="1"/>
@@ -5917,9 +6123,13 @@
       <c r="W160" s="1"/>
     </row>
     <row r="161" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A161" s="1"/>
-      <c r="B161" s="1"/>
-      <c r="C161" s="1"/>
+      <c r="A161" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="B161" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C161" s="21"/>
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
@@ -5942,9 +6152,13 @@
       <c r="W161" s="1"/>
     </row>
     <row r="162" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A162" s="1"/>
-      <c r="B162" s="1"/>
-      <c r="C162" s="1"/>
+      <c r="A162" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="B162" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="C162" s="21"/>
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
       <c r="F162" s="1"/>
@@ -5967,9 +6181,13 @@
       <c r="W162" s="1"/>
     </row>
     <row r="163" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A163" s="1"/>
-      <c r="B163" s="1"/>
-      <c r="C163" s="1"/>
+      <c r="A163" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="B163" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="C163" s="21"/>
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
       <c r="F163" s="1"/>
@@ -5992,9 +6210,13 @@
       <c r="W163" s="1"/>
     </row>
     <row r="164" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A164" s="1"/>
-      <c r="B164" s="1"/>
-      <c r="C164" s="1"/>
+      <c r="A164" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="B164" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="C164" s="21"/>
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
       <c r="F164" s="1"/>
@@ -6017,9 +6239,13 @@
       <c r="W164" s="1"/>
     </row>
     <row r="165" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A165" s="1"/>
-      <c r="B165" s="1"/>
-      <c r="C165" s="1"/>
+      <c r="A165" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="B165" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="C165" s="21"/>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
       <c r="F165" s="1"/>
@@ -6042,9 +6268,9 @@
       <c r="W165" s="1"/>
     </row>
     <row r="166" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A166" s="1"/>
-      <c r="B166" s="1"/>
-      <c r="C166" s="1"/>
+      <c r="A166" s="21"/>
+      <c r="B166" s="21"/>
+      <c r="C166" s="21"/>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
       <c r="F166" s="1"/>
@@ -6067,9 +6293,9 @@
       <c r="W166" s="1"/>
     </row>
     <row r="167" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A167" s="1"/>
-      <c r="B167" s="1"/>
-      <c r="C167" s="1"/>
+      <c r="A167" s="21"/>
+      <c r="B167" s="21"/>
+      <c r="C167" s="21"/>
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
       <c r="F167" s="1"/>
@@ -6091,10 +6317,10 @@
       <c r="V167" s="1"/>
       <c r="W167" s="1"/>
     </row>
-    <row r="168" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A168" s="1"/>
-      <c r="B168" s="1"/>
-      <c r="C168" s="1"/>
+    <row r="168" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A168" s="21"/>
+      <c r="B168" s="21"/>
+      <c r="C168" s="21"/>
       <c r="D168" s="1"/>
       <c r="E168" s="1"/>
       <c r="F168" s="1"/>
@@ -6116,10 +6342,16 @@
       <c r="V168" s="1"/>
       <c r="W168" s="1"/>
     </row>
-    <row r="169" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A169" s="1"/>
-      <c r="B169" s="1"/>
-      <c r="C169" s="1"/>
+    <row r="169" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A169" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B169" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C169" s="25" t="s">
+        <v>7</v>
+      </c>
       <c r="D169" s="1"/>
       <c r="E169" s="1"/>
       <c r="F169" s="1"/>
@@ -6141,10 +6373,16 @@
       <c r="V169" s="1"/>
       <c r="W169" s="1"/>
     </row>
-    <row r="170" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A170" s="1"/>
-      <c r="B170" s="1"/>
-      <c r="C170" s="1"/>
+    <row r="170" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A170" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B170" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C170" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="D170" s="1"/>
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
@@ -6167,9 +6405,15 @@
       <c r="W170" s="1"/>
     </row>
     <row r="171" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A171" s="1"/>
-      <c r="B171" s="1"/>
-      <c r="C171" s="1"/>
+      <c r="A171" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="B171" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="C171" s="21" t="s">
+        <v>263</v>
+      </c>
       <c r="D171" s="1"/>
       <c r="E171" s="1"/>
       <c r="F171" s="1"/>
@@ -6192,9 +6436,15 @@
       <c r="W171" s="1"/>
     </row>
     <row r="172" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A172" s="1"/>
-      <c r="B172" s="1"/>
-      <c r="C172" s="1"/>
+      <c r="A172" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="B172" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="C172" s="21" t="s">
+        <v>265</v>
+      </c>
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
       <c r="F172" s="1"/>
@@ -6217,9 +6467,15 @@
       <c r="W172" s="1"/>
     </row>
     <row r="173" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A173" s="1"/>
-      <c r="B173" s="1"/>
-      <c r="C173" s="1"/>
+      <c r="A173" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="B173" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="C173" s="21" t="s">
+        <v>267</v>
+      </c>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
       <c r="F173" s="1"/>
@@ -6242,9 +6498,11 @@
       <c r="W173" s="1"/>
     </row>
     <row r="174" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A174" s="1"/>
-      <c r="B174" s="1"/>
-      <c r="C174" s="1"/>
+      <c r="A174" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="B174" s="21"/>
+      <c r="C174" s="21"/>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
       <c r="F174" s="1"/>
@@ -6267,9 +6525,11 @@
       <c r="W174" s="1"/>
     </row>
     <row r="175" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A175" s="1"/>
-      <c r="B175" s="1"/>
-      <c r="C175" s="1"/>
+      <c r="A175" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="B175" s="21"/>
+      <c r="C175" s="21"/>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
       <c r="F175" s="1"/>
@@ -6292,9 +6552,15 @@
       <c r="W175" s="1"/>
     </row>
     <row r="176" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A176" s="1"/>
-      <c r="B176" s="1"/>
-      <c r="C176" s="1"/>
+      <c r="A176" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="B176" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="C176" s="21" t="s">
+        <v>271</v>
+      </c>
       <c r="D176" s="1"/>
       <c r="E176" s="1"/>
       <c r="F176" s="1"/>
@@ -6317,9 +6583,15 @@
       <c r="W176" s="1"/>
     </row>
     <row r="177" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A177" s="1"/>
-      <c r="B177" s="1"/>
-      <c r="C177" s="1"/>
+      <c r="A177" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="B177" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="C177" s="21" t="s">
+        <v>273</v>
+      </c>
       <c r="D177" s="1"/>
       <c r="E177" s="1"/>
       <c r="F177" s="1"/>
@@ -6342,9 +6614,9 @@
       <c r="W177" s="1"/>
     </row>
     <row r="178" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A178" s="1"/>
-      <c r="B178" s="1"/>
-      <c r="C178" s="1"/>
+      <c r="A178" s="21"/>
+      <c r="B178" s="21"/>
+      <c r="C178" s="21"/>
       <c r="D178" s="1"/>
       <c r="E178" s="1"/>
       <c r="F178" s="1"/>
@@ -6367,9 +6639,15 @@
       <c r="W178" s="1"/>
     </row>
     <row r="179" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A179" s="1"/>
-      <c r="B179" s="1"/>
-      <c r="C179" s="1"/>
+      <c r="A179" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="B179" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="C179" s="21" t="s">
+        <v>275</v>
+      </c>
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
       <c r="F179" s="1"/>
@@ -6392,9 +6670,13 @@
       <c r="W179" s="1"/>
     </row>
     <row r="180" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A180" s="1"/>
-      <c r="B180" s="1"/>
-      <c r="C180" s="1"/>
+      <c r="A180" s="27"/>
+      <c r="B180" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="C180" s="21" t="s">
+        <v>276</v>
+      </c>
       <c r="D180" s="1"/>
       <c r="E180" s="1"/>
       <c r="F180" s="1"/>
@@ -6417,9 +6699,15 @@
       <c r="W180" s="1"/>
     </row>
     <row r="181" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A181" s="1"/>
-      <c r="B181" s="1"/>
-      <c r="C181" s="1"/>
+      <c r="A181" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="B181" s="21" t="s">
+        <v>278</v>
+      </c>
+      <c r="C181" s="21" t="s">
+        <v>278</v>
+      </c>
       <c r="D181" s="1"/>
       <c r="E181" s="1"/>
       <c r="F181" s="1"/>
@@ -6442,9 +6730,15 @@
       <c r="W181" s="1"/>
     </row>
     <row r="182" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A182" s="1"/>
-      <c r="B182" s="1"/>
-      <c r="C182" s="1"/>
+      <c r="A182" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="B182" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="C182" s="21" t="s">
+        <v>280</v>
+      </c>
       <c r="D182" s="1"/>
       <c r="E182" s="1"/>
       <c r="F182" s="1"/>
@@ -6467,9 +6761,13 @@
       <c r="W182" s="1"/>
     </row>
     <row r="183" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A183" s="1"/>
-      <c r="B183" s="1"/>
-      <c r="C183" s="1"/>
+      <c r="A183" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="B183" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="C183" s="21"/>
       <c r="D183" s="1"/>
       <c r="E183" s="1"/>
       <c r="F183" s="1"/>
@@ -6492,9 +6790,9 @@
       <c r="W183" s="1"/>
     </row>
     <row r="184" spans="1:23" ht="13.5" customHeight="1">
-      <c r="A184" s="1"/>
-      <c r="B184" s="1"/>
-      <c r="C184" s="1"/>
+      <c r="A184" s="21"/>
+      <c r="B184" s="21"/>
+      <c r="C184" s="21"/>
       <c r="D184" s="1"/>
       <c r="E184" s="1"/>
       <c r="F184" s="1"/>
@@ -10716,22 +11014,46 @@
       <c r="V352" s="1"/>
       <c r="W352" s="1"/>
     </row>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="353" spans="1:23" ht="13.5" customHeight="1">
+      <c r="A353" s="1"/>
+      <c r="B353" s="1"/>
+      <c r="C353" s="1"/>
+      <c r="D353" s="1"/>
+      <c r="E353" s="1"/>
+      <c r="F353" s="1"/>
+      <c r="G353" s="1"/>
+      <c r="H353" s="1"/>
+      <c r="I353" s="1"/>
+      <c r="J353" s="1"/>
+      <c r="K353" s="1"/>
+      <c r="L353" s="1"/>
+      <c r="M353" s="1"/>
+      <c r="N353" s="1"/>
+      <c r="O353" s="1"/>
+      <c r="P353" s="1"/>
+      <c r="Q353" s="1"/>
+      <c r="R353" s="1"/>
+      <c r="S353" s="1"/>
+      <c r="T353" s="1"/>
+      <c r="U353" s="1"/>
+      <c r="V353" s="1"/>
+      <c r="W353" s="1"/>
+    </row>
+    <row r="354" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="355" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="356" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="357" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="358" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="359" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="360" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="361" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="362" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="363" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="364" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="365" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="366" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="367" spans="1:23" ht="15.75" customHeight="1"/>
+    <row r="368" spans="1:23" ht="15.75" customHeight="1"/>
     <row r="369" ht="15.75" customHeight="1"/>
     <row r="370" ht="15.75" customHeight="1"/>
     <row r="371" ht="15.75" customHeight="1"/>
@@ -11364,6 +11686,7 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
@@ -11374,6 +11697,11 @@
     <hyperlink ref="C38" r:id="rId6"/>
     <hyperlink ref="C75" r:id="rId7"/>
     <hyperlink ref="B75" r:id="rId8"/>
+    <hyperlink ref="B162" r:id="rId9" location="info;tim@mmh-demo.com;Manage@123;MMHtest.jpg"/>
+    <hyperlink ref="B169" r:id="rId10"/>
+    <hyperlink ref="C169" r:id="rId11"/>
+    <hyperlink ref="B156" r:id="rId12"/>
+    <hyperlink ref="C156" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
HappyPath Pack setup. Scenarios Updated for Appointments, Messages.
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Inlogic\clone\config\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\INLOGIC\Complete_Pack\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="MMH" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="283">
   <si>
     <t>KEY</t>
   </si>
@@ -54,9 +54,6 @@
     <t>BOOK_VISIT_APPOINTMENT</t>
   </si>
   <si>
-    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Visit;9:00 AM;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
-  </si>
-  <si>
     <t>VISIT_APPOINTMENT_DETAILS</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>BOOK_VIDEO_APPOINTMENT</t>
   </si>
   <si>
-    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Video;9:00 AM;Book Video Appointment;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
-  </si>
-  <si>
     <t>VIDEO_APPOINTMENT_DETAILS</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>BOOK_VISIT_IN_VIDEO_APPOINTMENT</t>
   </si>
   <si>
-    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Video;9:00 AM;Book Face to Face;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
-  </si>
-  <si>
     <t>VISIT_IN_VIDEO_APPOINTMENT_DETAILS</t>
   </si>
   <si>
@@ -111,9 +102,6 @@
     <t>BOOK_PHONE_APPOINTMENT</t>
   </si>
   <si>
-    <t>VM03Location;VM03Location;Myself (HARRY HARRY);Check me,An existing issue;Phone;9:00 AM;Dr Sam Entwistle;022;784512369;AFTER_THREE_DAYS</t>
-  </si>
-  <si>
     <t>PHONE_APPOINTMENT_DETAILS</t>
   </si>
   <si>
@@ -714,21 +702,9 @@
     <t>DATA_MY_ENTRIES_COVID_IMMUNISATIONS</t>
   </si>
   <si>
-    <t>23 Jun 2022;Comirnaty, COVID-19 mRNA (Pfizer-BioNTech)</t>
-  </si>
-  <si>
-    <t>19 May 2022;Comirnaty, COVID-19 mRNA (Pfizer-BioNTech);</t>
-  </si>
-  <si>
     <t>DATA_MY_ENTRIES_INSIDE_COVID_IMMUNISATIONS</t>
   </si>
   <si>
-    <t>Comirnaty, COVID-19 mRNA (Pfizer-BioNTech);COVID19 Comirnaty - 2;Test123;23 Jun 2022;Show this entry to my doctor;TestClinical</t>
-  </si>
-  <si>
-    <t>Comirnaty, COVID-19 mRNA (Pfizer-BioNTech);COVID19 Comirnaty - 1;123456ghffb;19 May 2022;Show this entry to my doctor;TestEdit</t>
-  </si>
-  <si>
     <t>VACCINE_NAME</t>
   </si>
   <si>
@@ -874,13 +850,31 @@
   </si>
   <si>
     <t>PASSWORD FOR DOCTOR</t>
+  </si>
+  <si>
+    <t>01 Jun 2022;Comirnaty, COVID-19 mRNA (Pfizer-BioNTech)</t>
+  </si>
+  <si>
+    <t>Comirnaty, COVID-19 mRNA (Pfizer-BioNTech);COVID19 Comirnaty - 2;Test123;01 Jun 2022;Show this entry to my doctor;Test02-Additional Information</t>
+  </si>
+  <si>
+    <t>VM03Location;VM03Location;Myself (HARRY HARRY);A new issue,An existing issue;Visit;9:00 AM;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>VM03Location;VM03Location;Myself (HARRY HARRY);A new issue,An existing issue;Video;9:00 AM;Book Video Appointment;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>VM03Location;VM03Location;Myself (HARRY HARRY);A new issue,An existing issue;Video;9:00 AM;Book Face to Face;Dr Sam Entwistle;AFTER_THREE_DAYS</t>
+  </si>
+  <si>
+    <t>VM03Location;VM03Location;Myself (HARRY HARRY);A new issue,An existing issue;Phone;9:00 AM;Dr Sam Entwistle;022;784512369;AFTER_THREE_DAYS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -891,50 +885,59 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -986,8 +989,14 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1000,8 +1009,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1054,11 +1069,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD1D1D1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD1D1D1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD1D1D1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD1D1D1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1128,6 +1158,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1345,16 +1378,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="B154" sqref="B154"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="69.54296875" customWidth="1"/>
-    <col min="2" max="2" width="157.1796875" customWidth="1"/>
-    <col min="3" max="3" width="125.1796875" customWidth="1"/>
-    <col min="4" max="23" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="157.140625" customWidth="1"/>
+    <col min="3" max="3" width="135.140625" customWidth="1"/>
+    <col min="4" max="23" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="13.5" customHeight="1">
@@ -1486,10 +1519,10 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>279</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>279</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1514,13 +1547,13 @@
     </row>
     <row r="6" spans="1:23" ht="13.5" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1545,13 +1578,13 @@
     </row>
     <row r="7" spans="1:23" ht="13.5" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1576,10 +1609,10 @@
     </row>
     <row r="8" spans="1:23" ht="13.5" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1630,13 +1663,13 @@
     </row>
     <row r="10" spans="1:23" ht="13.5" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>280</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>280</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1661,13 +1694,13 @@
     </row>
     <row r="11" spans="1:23" ht="13.5" customHeight="1">
       <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1692,13 +1725,13 @@
     </row>
     <row r="12" spans="1:23" ht="13.5" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1723,10 +1756,10 @@
     </row>
     <row r="13" spans="1:23" ht="13.5" customHeight="1">
       <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1777,13 +1810,13 @@
     </row>
     <row r="15" spans="1:23" ht="13.5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>281</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>281</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1808,13 +1841,13 @@
     </row>
     <row r="16" spans="1:23" ht="13.5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1839,13 +1872,13 @@
     </row>
     <row r="17" spans="1:23" ht="13.5" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1870,10 +1903,10 @@
     </row>
     <row r="18" spans="1:23" ht="13.5" customHeight="1">
       <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1924,13 +1957,13 @@
     </row>
     <row r="20" spans="1:23" ht="13.5" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>282</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>282</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1955,13 +1988,13 @@
     </row>
     <row r="21" spans="1:23" ht="13.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1986,13 +2019,13 @@
     </row>
     <row r="22" spans="1:23" ht="13.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2017,10 +2050,10 @@
     </row>
     <row r="23" spans="1:23" ht="13.5" customHeight="1">
       <c r="A23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2071,13 +2104,13 @@
     </row>
     <row r="25" spans="1:23" ht="13.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>11</v>
+        <v>279</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>11</v>
+        <v>279</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -2102,13 +2135,13 @@
     </row>
     <row r="26" spans="1:23" ht="13.5" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -2133,13 +2166,13 @@
     </row>
     <row r="27" spans="1:23" ht="13.5" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -2164,13 +2197,13 @@
     </row>
     <row r="28" spans="1:23" ht="13.5" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -2195,10 +2228,10 @@
     </row>
     <row r="29" spans="1:23" ht="13.5" customHeight="1">
       <c r="A29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -2249,13 +2282,13 @@
     </row>
     <row r="31" spans="1:23" ht="13.5" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -2280,13 +2313,13 @@
     </row>
     <row r="32" spans="1:23" ht="13.5" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -2336,13 +2369,13 @@
     </row>
     <row r="34" spans="1:23" ht="13.5" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -2392,10 +2425,10 @@
     </row>
     <row r="36" spans="1:23" ht="13.5" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2446,13 +2479,13 @@
     </row>
     <row r="38" spans="1:23" ht="13.5" customHeight="1">
       <c r="A38" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -2477,7 +2510,7 @@
     </row>
     <row r="39" spans="1:23" ht="13.5" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>9</v>
@@ -2533,13 +2566,13 @@
     </row>
     <row r="41" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A41" s="18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -2564,13 +2597,13 @@
     </row>
     <row r="42" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A42" s="18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -2595,13 +2628,13 @@
     </row>
     <row r="43" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A43" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -2676,13 +2709,13 @@
     </row>
     <row r="46" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A46" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -2707,13 +2740,13 @@
     </row>
     <row r="47" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A47" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -2738,7 +2771,7 @@
     </row>
     <row r="48" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A48" s="18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B48" s="19"/>
       <c r="C48" s="19"/>
@@ -2815,13 +2848,13 @@
     </row>
     <row r="51" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A51" s="18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -2846,13 +2879,13 @@
     </row>
     <row r="52" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A52" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -2877,7 +2910,7 @@
     </row>
     <row r="53" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A53" s="18" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
@@ -2954,13 +2987,13 @@
     </row>
     <row r="56" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A56" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2985,13 +3018,13 @@
     </row>
     <row r="57" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A57" s="18" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -3016,7 +3049,7 @@
     </row>
     <row r="58" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A58" s="18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B58" s="19"/>
       <c r="C58" s="19"/>
@@ -3093,13 +3126,13 @@
     </row>
     <row r="61" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A61" s="18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
@@ -3124,13 +3157,13 @@
     </row>
     <row r="62" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A62" s="18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -3205,13 +3238,13 @@
     </row>
     <row r="65" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A65" s="18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -3236,13 +3269,13 @@
     </row>
     <row r="66" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A66" s="18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -3317,13 +3350,13 @@
     </row>
     <row r="69" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A69" s="18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -3348,13 +3381,13 @@
     </row>
     <row r="70" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A70" s="18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -3379,13 +3412,13 @@
     </row>
     <row r="71" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A71" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -3410,13 +3443,13 @@
     </row>
     <row r="72" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A72" s="19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -3491,13 +3524,13 @@
     </row>
     <row r="75" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A75" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -3522,7 +3555,7 @@
     </row>
     <row r="76" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A76" s="9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B76" s="10" t="s">
         <v>9</v>
@@ -3578,13 +3611,13 @@
     </row>
     <row r="78" spans="1:23" ht="13.5" customHeight="1">
       <c r="A78" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -3609,13 +3642,13 @@
     </row>
     <row r="79" spans="1:23" ht="13.5" customHeight="1">
       <c r="A79" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -3640,13 +3673,13 @@
     </row>
     <row r="80" spans="1:23" ht="13.5" customHeight="1">
       <c r="A80" s="12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -3671,13 +3704,13 @@
     </row>
     <row r="81" spans="1:23" ht="13.5" customHeight="1">
       <c r="A81" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -3702,13 +3735,13 @@
     </row>
     <row r="82" spans="1:23" ht="13.5" customHeight="1">
       <c r="A82" s="12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -3733,13 +3766,13 @@
     </row>
     <row r="83" spans="1:23" ht="13.5" customHeight="1">
       <c r="A83" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -3764,13 +3797,13 @@
     </row>
     <row r="84" spans="1:23" ht="13.5" customHeight="1">
       <c r="A84" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -3795,13 +3828,13 @@
     </row>
     <row r="85" spans="1:23" ht="13.5" customHeight="1">
       <c r="A85" s="12" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -3826,13 +3859,13 @@
     </row>
     <row r="86" spans="1:23" ht="13.5" customHeight="1">
       <c r="A86" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -3857,13 +3890,13 @@
     </row>
     <row r="87" spans="1:23" ht="13.5" customHeight="1">
       <c r="A87" s="12" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -3888,13 +3921,13 @@
     </row>
     <row r="88" spans="1:23" ht="13.5" customHeight="1">
       <c r="A88" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -3919,13 +3952,13 @@
     </row>
     <row r="89" spans="1:23" ht="13.5" customHeight="1">
       <c r="A89" s="12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -3950,13 +3983,13 @@
     </row>
     <row r="90" spans="1:23" ht="13.5" customHeight="1">
       <c r="A90" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -3981,13 +4014,13 @@
     </row>
     <row r="91" spans="1:23" ht="13.5" customHeight="1">
       <c r="A91" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -4012,13 +4045,13 @@
     </row>
     <row r="92" spans="1:23" ht="13.5" customHeight="1">
       <c r="A92" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -4043,13 +4076,13 @@
     </row>
     <row r="93" spans="1:23" ht="13.5" customHeight="1">
       <c r="A93" s="12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -4074,13 +4107,13 @@
     </row>
     <row r="94" spans="1:23" ht="13.5" customHeight="1">
       <c r="A94" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -4105,13 +4138,13 @@
     </row>
     <row r="95" spans="1:23" ht="13.5" customHeight="1">
       <c r="A95" s="12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -4136,13 +4169,13 @@
     </row>
     <row r="96" spans="1:23" ht="13.5" customHeight="1">
       <c r="A96" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -4167,13 +4200,13 @@
     </row>
     <row r="97" spans="1:23" ht="13.5" customHeight="1">
       <c r="A97" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -4198,13 +4231,13 @@
     </row>
     <row r="98" spans="1:23" ht="13.5" customHeight="1">
       <c r="A98" s="12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -4229,13 +4262,13 @@
     </row>
     <row r="99" spans="1:23" ht="13.5" customHeight="1">
       <c r="A99" s="12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -4260,13 +4293,13 @@
     </row>
     <row r="100" spans="1:23" ht="13.5" customHeight="1">
       <c r="A100" s="12" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B100" s="17" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -4291,13 +4324,13 @@
     </row>
     <row r="101" spans="1:23" ht="13.5" customHeight="1">
       <c r="A101" s="12" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -4322,13 +4355,13 @@
     </row>
     <row r="102" spans="1:23" ht="13.5" customHeight="1">
       <c r="A102" s="14" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C102" s="13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -4353,13 +4386,13 @@
     </row>
     <row r="103" spans="1:23" ht="13.5" customHeight="1">
       <c r="A103" s="12" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
@@ -4384,13 +4417,13 @@
     </row>
     <row r="104" spans="1:23" ht="13.5" customHeight="1">
       <c r="A104" s="14" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
@@ -4415,13 +4448,13 @@
     </row>
     <row r="105" spans="1:23" ht="13.5" customHeight="1">
       <c r="A105" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
@@ -4446,13 +4479,13 @@
     </row>
     <row r="106" spans="1:23" ht="13.5" customHeight="1">
       <c r="A106" s="12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B106" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C106" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
@@ -4477,13 +4510,13 @@
     </row>
     <row r="107" spans="1:23" ht="13.5" customHeight="1">
       <c r="A107" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
@@ -4508,13 +4541,13 @@
     </row>
     <row r="108" spans="1:23" ht="13.5" customHeight="1">
       <c r="A108" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
@@ -4539,13 +4572,13 @@
     </row>
     <row r="109" spans="1:23" ht="13.5" customHeight="1">
       <c r="A109" s="12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
@@ -4570,13 +4603,13 @@
     </row>
     <row r="110" spans="1:23" ht="13.5" customHeight="1">
       <c r="A110" s="12" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
@@ -4601,13 +4634,13 @@
     </row>
     <row r="111" spans="1:23" ht="13.5" customHeight="1">
       <c r="A111" s="12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B111" s="17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C111" s="17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
@@ -4632,13 +4665,13 @@
     </row>
     <row r="112" spans="1:23" ht="13.5" customHeight="1">
       <c r="A112" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
@@ -4663,13 +4696,13 @@
     </row>
     <row r="113" spans="1:23" ht="13.5" customHeight="1">
       <c r="A113" s="12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
@@ -4694,13 +4727,13 @@
     </row>
     <row r="114" spans="1:23" ht="13.5" customHeight="1">
       <c r="A114" s="12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
@@ -4725,13 +4758,13 @@
     </row>
     <row r="115" spans="1:23" ht="13.5" customHeight="1">
       <c r="A115" s="12" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
@@ -4756,13 +4789,13 @@
     </row>
     <row r="116" spans="1:23" ht="13.5" customHeight="1">
       <c r="A116" s="12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
@@ -4787,13 +4820,13 @@
     </row>
     <row r="117" spans="1:23" ht="13.5" customHeight="1">
       <c r="A117" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
@@ -4818,13 +4851,13 @@
     </row>
     <row r="118" spans="1:23" ht="13.5" customHeight="1">
       <c r="A118" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C118" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
@@ -4849,13 +4882,13 @@
     </row>
     <row r="119" spans="1:23" ht="13.5" customHeight="1">
       <c r="A119" s="12" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
@@ -4880,13 +4913,13 @@
     </row>
     <row r="120" spans="1:23" ht="13.5" customHeight="1">
       <c r="A120" s="12" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
@@ -4911,13 +4944,13 @@
     </row>
     <row r="121" spans="1:23" ht="13.5" customHeight="1">
       <c r="A121" s="12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -4944,7 +4977,7 @@
       <c r="A122" s="12"/>
       <c r="B122" s="12"/>
       <c r="C122" s="12" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
@@ -4969,13 +5002,13 @@
     </row>
     <row r="123" spans="1:23" ht="13.5" customHeight="1">
       <c r="A123" s="12" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B123" s="12" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C123" s="12" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
@@ -5002,7 +5035,7 @@
       <c r="A124" s="12"/>
       <c r="B124" s="12"/>
       <c r="C124" s="12" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
@@ -5027,13 +5060,13 @@
     </row>
     <row r="125" spans="1:23" ht="13.5" customHeight="1">
       <c r="A125" s="12" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C125" s="12" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
@@ -5058,13 +5091,13 @@
     </row>
     <row r="126" spans="1:23" ht="13.5" customHeight="1">
       <c r="A126" s="12" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C126" s="13" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
@@ -5089,13 +5122,13 @@
     </row>
     <row r="127" spans="1:23" ht="13.5" customHeight="1">
       <c r="A127" s="12" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C127" s="12" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
@@ -5120,13 +5153,13 @@
     </row>
     <row r="128" spans="1:23" ht="13.5" customHeight="1">
       <c r="A128" s="12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B128" s="12" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
@@ -5151,13 +5184,13 @@
     </row>
     <row r="129" spans="1:23" ht="13.5" customHeight="1">
       <c r="A129" s="12" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C129" s="12" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
@@ -5182,13 +5215,13 @@
     </row>
     <row r="130" spans="1:23" ht="13.5" customHeight="1">
       <c r="A130" s="12" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C130" s="13" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
@@ -5213,13 +5246,13 @@
     </row>
     <row r="131" spans="1:23" ht="13.5" customHeight="1">
       <c r="A131" s="12" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B131" s="12" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C131" s="12" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
@@ -5244,13 +5277,13 @@
     </row>
     <row r="132" spans="1:23" ht="13.5" customHeight="1">
       <c r="A132" s="12" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B132" s="12" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C132" s="12" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
@@ -5275,13 +5308,13 @@
     </row>
     <row r="133" spans="1:23" ht="13.5" customHeight="1">
       <c r="A133" s="12" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B133" s="12" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C133" s="12" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
@@ -5306,13 +5339,13 @@
     </row>
     <row r="134" spans="1:23" ht="13.5" customHeight="1">
       <c r="A134" s="12" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B134" s="12" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C134" s="12" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
@@ -5337,13 +5370,13 @@
     </row>
     <row r="135" spans="1:23" ht="13.5" customHeight="1">
       <c r="A135" s="12" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B135" s="12" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C135" s="12" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
@@ -5368,13 +5401,13 @@
     </row>
     <row r="136" spans="1:23" ht="13.5" customHeight="1">
       <c r="A136" s="12" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B136" s="12" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C136" s="12" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
@@ -5399,13 +5432,13 @@
     </row>
     <row r="137" spans="1:23" ht="13.5" customHeight="1">
       <c r="A137" s="12" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B137" s="12" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C137" s="12" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
@@ -5455,13 +5488,13 @@
     </row>
     <row r="139" spans="1:23" ht="13.5" customHeight="1">
       <c r="A139" s="12" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B139" s="12" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C139" s="12" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -5486,13 +5519,13 @@
     </row>
     <row r="140" spans="1:23" ht="13.5" customHeight="1">
       <c r="A140" s="12" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B140" s="12" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
@@ -5517,13 +5550,13 @@
     </row>
     <row r="141" spans="1:23" ht="13.5" customHeight="1">
       <c r="A141" s="12" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B141" s="12" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
@@ -5548,13 +5581,13 @@
     </row>
     <row r="142" spans="1:23" ht="13.5" customHeight="1">
       <c r="A142" s="12" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
@@ -5579,13 +5612,13 @@
     </row>
     <row r="143" spans="1:23" ht="13.5" customHeight="1">
       <c r="A143" s="12" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B143" s="12" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
@@ -5610,13 +5643,13 @@
     </row>
     <row r="144" spans="1:23" ht="13.5" customHeight="1">
       <c r="A144" s="12" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B144" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
@@ -5641,13 +5674,13 @@
     </row>
     <row r="145" spans="1:26" ht="13.5" customHeight="1">
       <c r="A145" s="12" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B145" s="12" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
@@ -5672,13 +5705,13 @@
     </row>
     <row r="146" spans="1:26" ht="13.5" customHeight="1">
       <c r="A146" s="12" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B146" s="12" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
@@ -5701,15 +5734,15 @@
       <c r="V146" s="1"/>
       <c r="W146" s="1"/>
     </row>
-    <row r="147" spans="1:26" ht="13.5" customHeight="1">
+    <row r="147" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A147" s="12" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B147" s="12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -5732,15 +5765,15 @@
       <c r="V147" s="1"/>
       <c r="W147" s="1"/>
     </row>
-    <row r="148" spans="1:26" ht="13.5" customHeight="1">
+    <row r="148" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A148" s="12" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="C148" s="12" t="s">
-        <v>232</v>
+        <v>277</v>
+      </c>
+      <c r="C148" s="31" t="s">
+        <v>277</v>
       </c>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
@@ -5765,13 +5798,13 @@
     </row>
     <row r="149" spans="1:26" ht="13.5" customHeight="1">
       <c r="A149" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="B149" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C149" s="13" t="s">
-        <v>235</v>
+        <v>227</v>
+      </c>
+      <c r="B149" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="C149" s="12" t="s">
+        <v>278</v>
       </c>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
@@ -5796,13 +5829,13 @@
     </row>
     <row r="150" spans="1:26" ht="13.5" customHeight="1">
       <c r="A150" s="12" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
@@ -5827,13 +5860,13 @@
     </row>
     <row r="151" spans="1:26" ht="13.5" customHeight="1">
       <c r="A151" s="12" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
@@ -5858,13 +5891,13 @@
     </row>
     <row r="152" spans="1:26" ht="13.5" customHeight="1">
       <c r="A152" s="12" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B152" s="12" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
@@ -5889,10 +5922,10 @@
     </row>
     <row r="153" spans="1:26" ht="13.5" customHeight="1">
       <c r="A153" s="12" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B153" s="15" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
@@ -5964,7 +5997,7 @@
     </row>
     <row r="156" spans="1:26" s="30" customFormat="1" ht="13.5" customHeight="1">
       <c r="A156" s="21" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B156" s="25" t="s">
         <v>4</v>
@@ -5998,13 +6031,13 @@
     </row>
     <row r="157" spans="1:26" s="30" customFormat="1" ht="13.5" customHeight="1">
       <c r="A157" s="29" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B157" s="25" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C157" s="25" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D157" s="21"/>
       <c r="E157" s="21"/>
@@ -6032,7 +6065,7 @@
     </row>
     <row r="158" spans="1:26" s="30" customFormat="1" ht="13.5" customHeight="1">
       <c r="A158" s="29" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B158" s="21" t="s">
         <v>9</v>
@@ -6066,10 +6099,10 @@
     </row>
     <row r="159" spans="1:26" ht="13.5" customHeight="1">
       <c r="A159" s="21" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B159" s="22" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C159" s="21"/>
       <c r="D159" s="1"/>
@@ -6095,10 +6128,10 @@
     </row>
     <row r="160" spans="1:26" ht="13.5" customHeight="1">
       <c r="A160" s="21" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B160" s="23" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C160" s="21"/>
       <c r="D160" s="1"/>
@@ -6124,10 +6157,10 @@
     </row>
     <row r="161" spans="1:23" ht="13.5" customHeight="1">
       <c r="A161" s="21" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B161" s="23" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C161" s="21"/>
       <c r="D161" s="1"/>
@@ -6153,10 +6186,10 @@
     </row>
     <row r="162" spans="1:23" ht="13.5" customHeight="1">
       <c r="A162" s="21" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B162" s="24" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C162" s="21"/>
       <c r="D162" s="1"/>
@@ -6182,10 +6215,10 @@
     </row>
     <row r="163" spans="1:23" ht="13.5" customHeight="1">
       <c r="A163" s="21" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B163" s="23" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C163" s="21"/>
       <c r="D163" s="1"/>
@@ -6211,10 +6244,10 @@
     </row>
     <row r="164" spans="1:23" ht="13.5" customHeight="1">
       <c r="A164" s="21" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B164" s="23" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C164" s="21"/>
       <c r="D164" s="1"/>
@@ -6240,10 +6273,10 @@
     </row>
     <row r="165" spans="1:23" ht="13.5" customHeight="1">
       <c r="A165" s="21" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B165" s="23" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C165" s="21"/>
       <c r="D165" s="1"/>
@@ -6344,7 +6377,7 @@
     </row>
     <row r="169" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A169" s="19" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="B169" s="25" t="s">
         <v>7</v>
@@ -6375,7 +6408,7 @@
     </row>
     <row r="170" spans="1:23" ht="13.5" customHeight="1" thickBot="1">
       <c r="A170" s="19" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B170" s="19" t="s">
         <v>9</v>
@@ -6406,13 +6439,13 @@
     </row>
     <row r="171" spans="1:23" ht="13.5" customHeight="1">
       <c r="A171" s="26" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B171" s="26" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C171" s="21" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D171" s="1"/>
       <c r="E171" s="1"/>
@@ -6437,13 +6470,13 @@
     </row>
     <row r="172" spans="1:23" ht="13.5" customHeight="1">
       <c r="A172" s="21" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B172" s="21" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C172" s="21" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
@@ -6468,13 +6501,13 @@
     </row>
     <row r="173" spans="1:23" ht="13.5" customHeight="1">
       <c r="A173" s="21" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B173" s="21" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C173" s="21" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
@@ -6499,7 +6532,7 @@
     </row>
     <row r="174" spans="1:23" ht="13.5" customHeight="1">
       <c r="A174" s="21" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B174" s="21"/>
       <c r="C174" s="21"/>
@@ -6526,7 +6559,7 @@
     </row>
     <row r="175" spans="1:23" ht="13.5" customHeight="1">
       <c r="A175" s="21" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B175" s="21"/>
       <c r="C175" s="21"/>
@@ -6553,13 +6586,13 @@
     </row>
     <row r="176" spans="1:23" ht="13.5" customHeight="1">
       <c r="A176" s="21" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B176" s="21" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C176" s="21" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="D176" s="1"/>
       <c r="E176" s="1"/>
@@ -6584,13 +6617,13 @@
     </row>
     <row r="177" spans="1:23" ht="13.5" customHeight="1">
       <c r="A177" s="21" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B177" s="21" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C177" s="21" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D177" s="1"/>
       <c r="E177" s="1"/>
@@ -6640,13 +6673,13 @@
     </row>
     <row r="179" spans="1:23" ht="13.5" customHeight="1">
       <c r="A179" s="27" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B179" s="21" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C179" s="21" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
@@ -6672,10 +6705,10 @@
     <row r="180" spans="1:23" ht="13.5" customHeight="1">
       <c r="A180" s="27"/>
       <c r="B180" s="21" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C180" s="21" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D180" s="1"/>
       <c r="E180" s="1"/>
@@ -6700,13 +6733,13 @@
     </row>
     <row r="181" spans="1:23" ht="13.5" customHeight="1">
       <c r="A181" s="27" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B181" s="21" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C181" s="21" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="D181" s="1"/>
       <c r="E181" s="1"/>
@@ -6731,13 +6764,13 @@
     </row>
     <row r="182" spans="1:23" ht="13.5" customHeight="1">
       <c r="A182" s="28" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B182" s="21" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C182" s="21" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D182" s="1"/>
       <c r="E182" s="1"/>
@@ -6762,10 +6795,10 @@
     </row>
     <row r="183" spans="1:23" ht="13.5" customHeight="1">
       <c r="A183" s="27" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B183" s="21" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C183" s="21"/>
       <c r="D183" s="1"/>
@@ -11704,6 +11737,6 @@
     <hyperlink ref="C156" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sanity pack and Mobile Pack setup by Patrick - 08.07.22
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Inlogic\local_Checkout\config\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\local_Checkout\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5220C4-617A-4008-B4AD-9A9F749CF383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MMH" sheetId="1" r:id="rId1"/>
+    <sheet name="MMH_MobileApp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="330">
   <si>
     <t>KEY</t>
   </si>
@@ -997,12 +999,24 @@
   </si>
   <si>
     <t>VM03Location;VM03Location;Patient Communication-S;Patient;Harry Harry;Out of office reply testing;Body : Out of office reply testing_RANDOM</t>
+  </si>
+  <si>
+    <t>VM03Location;Dr Sam Entwistle;AFTER_THREE_DAYS;Follow-up</t>
+  </si>
+  <si>
+    <t>Dr Sam Entwistle;Follow-up</t>
+  </si>
+  <si>
+    <t>Approved;Dr Sam Entwistle;VM03Location;Pay at Health Centre;Follow-up</t>
+  </si>
+  <si>
+    <t>Approved;Phone Appointment;Dr Sam Entwistle;VM03Location;Pay at Health Centre;Follow-up</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1296,10 +1310,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
+    <sheetView topLeftCell="A168" workbookViewId="0">
       <selection activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
@@ -11846,21 +11860,120 @@
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="B38" r:id="rId5"/>
-    <hyperlink ref="C38" r:id="rId6"/>
-    <hyperlink ref="B75" r:id="rId7"/>
-    <hyperlink ref="C75" r:id="rId8"/>
-    <hyperlink ref="B156" r:id="rId9"/>
-    <hyperlink ref="C156" r:id="rId10"/>
-    <hyperlink ref="B162" r:id="rId11" location="info;tim@mmh-demo.com;Manage@123;MMHtest.jpg"/>
-    <hyperlink ref="B169" r:id="rId12"/>
-    <hyperlink ref="C169" r:id="rId13"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B38" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C38" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B75" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C75" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B156" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C156" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B162" r:id="rId11" location="info;tim@mmh-demo.com;Manage@123;MMHtest.jpg" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B169" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C169" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0182EF84-9AAF-4A9D-91E6-D50D70555D4C}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Updated MMH_Appointment feature. - Updated testdata, BaseScreen, DriverUtil, MobileCukes. - Udpated Screen, Steps and DemoScreenContainer related to Appointment Module.
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\local_Checkout\config\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MMH_Framework\MMH_Git_Updated[11-07]\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5220C4-617A-4008-B4AD-9A9F749CF383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198C12C9-C2EA-4918-88CC-66BC04EAF210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="356">
   <si>
     <t>KEY</t>
   </si>
@@ -1011,17 +1011,151 @@
   </si>
   <si>
     <t>Approved;Phone Appointment;Dr Sam Entwistle;VM03Location;Pay at Health Centre;Follow-up</t>
+  </si>
+  <si>
+    <t>Approved;Video Appointment;Dr Sam Entwistle;VM03Location;Pay at Health Centre;Follow-up</t>
+  </si>
+  <si>
+    <t>CONTACT_NUMBER</t>
+  </si>
+  <si>
+    <t>4111111111111111;test;02;24;121</t>
+  </si>
+  <si>
+    <t>VISIT_APPOINTMENT_SUMMARY_USING_CARD_PAYMENT</t>
+  </si>
+  <si>
+    <t>BOOK_PHONE_APPOINTMENT_USING_CARD_PAYMENT</t>
+  </si>
+  <si>
+    <t>PHONE_APPOINTMENT_DETAILS_USING_CARD_PAYMENT</t>
+  </si>
+  <si>
+    <t>PHONE_APPOINTMENT_SUMMARY_USING_CARD_PAYMENT</t>
+  </si>
+  <si>
+    <t>BOOK_VIDEO_APPOINTMENT_USING_CARD_PAYMENT</t>
+  </si>
+  <si>
+    <t>VIDEO_APPOINTMENT_DETAILS_USING_CARD_PAYMENT</t>
+  </si>
+  <si>
+    <t>VIDEO_APPOINTMENT_SUMMARY_USING_CARD_PAYMENT</t>
+  </si>
+  <si>
+    <t>Approved;Phone Appointment;Dr Sam Entwistle;VM03Location;Follow-up</t>
+  </si>
+  <si>
+    <t>Approved;Dr Sam Entwistle;VM03Location;Follow-up</t>
+  </si>
+  <si>
+    <t>BOOK_VISIT_APPOINTMENT_0_AMOUNT</t>
+  </si>
+  <si>
+    <t>VISIT_APPOINTMENT_DETAILS_0_AMOUNT</t>
+  </si>
+  <si>
+    <t>VISIT_APPOINTMENT_SUMMARY_0_AMOUNT</t>
+  </si>
+  <si>
+    <t>VM03Location2;Dr.Neel;AFTER_THREE_DAYS;Follow-up</t>
+  </si>
+  <si>
+    <t>Dr.Neel;Follow-up</t>
+  </si>
+  <si>
+    <t>Approved;Dr.Neel;VM03Location2;Pay at Health Centre;Follow-up</t>
+  </si>
+  <si>
+    <t>BOOK_PHONE_APPOINTMENT_0_AMOUNT</t>
+  </si>
+  <si>
+    <t>PHONE_APPOINTMENT_DETAILS_0_AMOUNT</t>
+  </si>
+  <si>
+    <t>PHONE_APPOINTMENT_SUMMARY_0_AMOUNT</t>
+  </si>
+  <si>
+    <t>Approved;Phone Appointment;Dr.Neel;VM03Location2;Pay at Health Centre;Follow-up</t>
+  </si>
+  <si>
+    <t>Approved;Video Appointment;Dr.Neel;VM03Location2;Pay at Health Centre;Follow-up</t>
+  </si>
+  <si>
+    <t>BOOK_VIDEO_APPOINTMENT_0_AMOUNT</t>
+  </si>
+  <si>
+    <t>VIDEO_APPOINTMENT_DETAILS_0_AMOUNT</t>
+  </si>
+  <si>
+    <t>VIDEO_APPOINTMENT_SUMMARY_0_AMOUNT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1036,6 +1170,21 @@
       <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1064,38 +1213,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1313,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11881,99 +12045,412 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0182EF84-9AAF-4A9D-91E6-D50D70555D4C}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.1796875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" s="15" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" s="15" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" s="15" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" s="15" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" s="15" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="B12" s="24">
+        <v>784512369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" s="15" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" s="15" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="B34" s="24">
+        <v>784512369</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="26" t="s">
+        <v>342</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="B50" s="24">
+        <v>784512369</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="B54" s="27" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="B56" s="27" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{F2EAAA5B-5C00-48F7-B385-AC499BC71E4C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Updated MMH_Appointment feature file. - Added MMH_Health_Records feature file. - Updated Screen, Steps and Base Screen. - Updated testdata.
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MMH_Framework\MMH_Git_Updated[11-07]\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198C12C9-C2EA-4918-88CC-66BC04EAF210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165B4FA5-ACE0-445C-8817-8978B42C408B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="384">
   <si>
     <t>KEY</t>
   </si>
@@ -1089,17 +1089,129 @@
   </si>
   <si>
     <t>VIDEO_APPOINTMENT_SUMMARY_0_AMOUNT</t>
+  </si>
+  <si>
+    <t>TEST_RESULTS_RECORDS</t>
+  </si>
+  <si>
+    <t>TEST_RESULTS_DETAILS</t>
+  </si>
+  <si>
+    <t>Hpicpn_Hl7 Of The Message;02 Jun 2018</t>
+  </si>
+  <si>
+    <t>Amylmetacresol 0.6mg;Dichlorobenzyl Alcohol 1.2mg Lozenges (strawberry);07 Jun 2022</t>
+  </si>
+  <si>
+    <t>Prescribed By;Dr Sam Entwistle;VM03Location;More Information;Item Name: Amylmetacresol 0.6mg;Dichlorobenzyl Alcohol 1.2mg Lozenges (strawberry);Date Given: 07 Jun 2022;Directions: 5, As Required;Period: 0 Days;Dosage: 5;Status: Long Term</t>
+  </si>
+  <si>
+    <t>PRESCRIPTIONS_RECORDS</t>
+  </si>
+  <si>
+    <t>PRESCRIPTIONS_DETAILS</t>
+  </si>
+  <si>
+    <t>Dr Sam Entwistle;VM03Location;Test Results;Patient Details;Patient Name: TEST, Patient;NHI No:;Date of Birth: 26-Jun-1995;Ordered by:Sam Eaves;Laboratory:;Observation date:02-Jun-2018</t>
+  </si>
+  <si>
+    <t>2-aminoethyl dihydrogen phosphate;07 Jun 2022</t>
+  </si>
+  <si>
+    <t>ALLERGIES_RECORDS</t>
+  </si>
+  <si>
+    <t>ALLERGIES_DETAILS</t>
+  </si>
+  <si>
+    <t>Dr Sam Entwistle;VM03Location;Doctor's Note;note1;Type: Drug Class;Date Recorded: 07 Jun 2022</t>
+  </si>
+  <si>
+    <t>Plasma total protein S level;07 Jun 2022</t>
+  </si>
+  <si>
+    <t>Prescribed By;Dr Sam Entwistle;VM03Location;Condition Info;Condition Name: Plasma total protein S level;Date Recorded: 07 Jun 2022;Is Long Term? No;Clinician Notes;note1</t>
+  </si>
+  <si>
+    <t>CONDITIONS_RECORDS</t>
+  </si>
+  <si>
+    <t>CONDITIONS_DETAILS</t>
+  </si>
+  <si>
+    <t>BCG;07 Jun 2022 08:38 PM</t>
+  </si>
+  <si>
+    <t>Dr Sam Entwistle;VM03Location;Doctor's Note;Outcome: Given;Notes: note1;Expiry: 01 Dec 2020 04:06 PM;Batch Number: 2345690;Route: Intra Muscular;Site: Buttock</t>
+  </si>
+  <si>
+    <t>IMMUNISATIONS_RECORDS</t>
+  </si>
+  <si>
+    <t>IMMUNISATIONS_DETAILS</t>
+  </si>
+  <si>
+    <t>Dr Sam Entwistle;07 Jun 2022</t>
+  </si>
+  <si>
+    <t>Dr Sam Entwistle;VM03Location;Visit Information;Visit Type: Consult In Surgery;Visit Date: 07 Jun 2022 08:34 PM;Objective Notes;Test Objective;Subjective Notes;Test Subjective</t>
+  </si>
+  <si>
+    <t>DOCTOR_NOTES_RECORDS</t>
+  </si>
+  <si>
+    <t>DOCTOR_NOTES_DETAILS</t>
+  </si>
+  <si>
+    <t>Body Mass Index;14 Jun 2022</t>
+  </si>
+  <si>
+    <t>Dr Sam Entwistle;VM03Location;Doctor's Note;Note: note1;Due Date: 14 Jun 2022 08:37 PM;Contact information;Is Contacted? Yes;Contacted Date: 07 Jun 2022;Comment: MMH Email</t>
+  </si>
+  <si>
+    <t>RECALLS_RECORDS</t>
+  </si>
+  <si>
+    <t>RECALLS_DETAILS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1213,53 +1325,66 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1477,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:B29"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12045,10 +12170,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0182EF84-9AAF-4A9D-91E6-D50D70555D4C}">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12446,6 +12571,118 @@
         <v>18</v>
       </c>
     </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="28" t="s">
+        <v>356</v>
+      </c>
+      <c r="B59" s="30" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="28" t="s">
+        <v>357</v>
+      </c>
+      <c r="B60" s="31" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="32" t="s">
+        <v>362</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="33" t="s">
+        <v>365</v>
+      </c>
+      <c r="B63" s="34" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A64" s="33" t="s">
+        <v>366</v>
+      </c>
+      <c r="B64" s="34" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="33" t="s">
+        <v>370</v>
+      </c>
+      <c r="B65" s="34" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="33" t="s">
+        <v>371</v>
+      </c>
+      <c r="B66" s="34" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="33" t="s">
+        <v>374</v>
+      </c>
+      <c r="B67" s="34" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="33" t="s">
+        <v>375</v>
+      </c>
+      <c r="B68" s="34" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="33" t="s">
+        <v>378</v>
+      </c>
+      <c r="B69" s="34" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A70" s="33" t="s">
+        <v>379</v>
+      </c>
+      <c r="B70" s="34" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="33" t="s">
+        <v>382</v>
+      </c>
+      <c r="B71" s="34" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A72" s="33" t="s">
+        <v>383</v>
+      </c>
+      <c r="B72" s="34" t="s">
+        <v>381</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{F2EAAA5B-5C00-48F7-B385-AC499BC71E4C}"/>

</xml_diff>

<commit_message>
UAT URL UPDATE & MESSAGE MODULE UPDATE
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\INLOGIC\My Exe\clone\config\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Patrick-Codoid\Mobile_App_Code\URL UPDATE\clone_new\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="383">
   <si>
     <t>KEY</t>
   </si>
@@ -1129,18 +1129,12 @@
     <t>RECALLS_DETAILS</t>
   </si>
   <si>
-    <t>VM03Location;VM03Location;Lab results enquiry;Clinical Staff;Dr Tim;Compose Message_RANDOM;Compose Message Testing_RANDOM;MMHtest.jpg</t>
-  </si>
-  <si>
     <t>COMPOSE_MESSAGE</t>
   </si>
   <si>
     <t>DRAFT_MESSAGE</t>
   </si>
   <si>
-    <t xml:space="preserve">VM03Location;VM03Location;Lab results enquiry;Clinical Staff;Dr Tim;Draft Message_RANDOM;Draft Message Testing_RANDOM;MMHtest.jpg </t>
-  </si>
-  <si>
     <t>https://v2web.mmh-demo.com/home</t>
   </si>
   <si>
@@ -1166,12 +1160,21 @@
   </si>
   <si>
     <t>VM03Location;VM03Location;Patient Communication-S;Patient;Harry Harry;Automatic Reply Message Testing_RANDOM;Body : Automatic reply testing_RANDOM</t>
+  </si>
+  <si>
+    <t>VM03Location;VM03Location;Lab results enquiry;Clinical Staff;Testprovider1;Compose Message_RANDOM;Compose Message Testing_RANDOM;MMHtest.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VM03Location;VM03Location;Lab results enquiry;Clinical Staff;Testprovider1;Draft Message_RANDOM;Draft Message Testing_RANDOM;MMHtest.jpg </t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1627,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A185" sqref="A185"/>
+    <sheetView tabSelected="1" topLeftCell="C145" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C158" sqref="C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1676,10 +1679,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -2517,13 +2520,13 @@
     </row>
     <row r="30" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -6348,10 +6351,10 @@
         <v>225</v>
       </c>
       <c r="B159" s="36" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C159" s="36" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D159" s="7"/>
       <c r="E159" s="7"/>
@@ -6413,13 +6416,13 @@
     </row>
     <row r="161" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="C161" s="7" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
@@ -6475,13 +6478,13 @@
     </row>
     <row r="163" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="34" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="C163" s="7" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
@@ -7061,13 +7064,13 @@
     </row>
     <row r="183" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B183" s="37" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C183" s="37" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D183" s="1"/>
       <c r="E183" s="1"/>
@@ -7126,10 +7129,10 @@
         <v>249</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C185" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D185" s="1"/>
       <c r="E185" s="1"/>
@@ -7157,10 +7160,10 @@
         <v>304</v>
       </c>
       <c r="B186" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C186" s="10" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D186" s="1"/>
       <c r="E186" s="1"/>
@@ -7219,10 +7222,10 @@
         <v>225</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C188" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>

</xml_diff>

<commit_message>
Screenshots for failure scenarios updated.
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Patrick-Codoid\Mobile_App_Code\URL UPDATE\clone_new\config\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Patrick-Codoid\Happy_Path_Framework\Mobile_Response16-08-2022\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>URL</t>
-  </si>
-  <si>
-    <t>https://v2webuat.mmh-demo.com/home</t>
   </si>
   <si>
     <t>https://v2web.mmh-demo.com/home</t>
@@ -1224,12 +1221,15 @@
   <si>
     <t>Dr Sam Entwistle;VM03Location;Doctor's Note;Note: note1;Due Date: 14 Jun 2022 08:37 PM;Contact information;Is Contacted? Yes;Contacted Date: 07 Jun 2022;Comment: MMH Email</t>
   </si>
+  <si>
+    <t>https://v2webfeature.mmh-demo.com/home</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1297,6 +1297,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1328,10 +1335,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1378,8 +1386,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1595,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C142" workbookViewId="0">
-      <selection activeCell="C163" sqref="C163"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1645,11 +1655,11 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="24" t="s">
+        <v>400</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1677,13 +1687,13 @@
     </row>
     <row r="3" spans="1:26" ht="13.5" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1711,13 +1721,13 @@
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1745,13 +1755,13 @@
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1779,13 +1789,13 @@
     </row>
     <row r="6" spans="1:26" ht="13.5" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1813,13 +1823,13 @@
     </row>
     <row r="7" spans="1:26" ht="13.5" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1847,13 +1857,13 @@
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1909,13 +1919,13 @@
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1943,13 +1953,13 @@
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1">
       <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1977,13 +1987,13 @@
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2011,13 +2021,13 @@
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1">
       <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2073,13 +2083,13 @@
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
       <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2107,13 +2117,13 @@
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2141,13 +2151,13 @@
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2175,13 +2185,13 @@
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1">
       <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2237,13 +2247,13 @@
     </row>
     <row r="20" spans="1:26" ht="13.5" customHeight="1">
       <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -2271,13 +2281,13 @@
     </row>
     <row r="21" spans="1:26" ht="13.5" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2305,13 +2315,13 @@
     </row>
     <row r="22" spans="1:26" ht="13.5" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -2339,13 +2349,13 @@
     </row>
     <row r="23" spans="1:26" ht="13.5" customHeight="1">
       <c r="A23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -2401,13 +2411,13 @@
     </row>
     <row r="25" spans="1:26" ht="13.5" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -2435,13 +2445,13 @@
     </row>
     <row r="26" spans="1:26" ht="13.5" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -2469,13 +2479,13 @@
     </row>
     <row r="27" spans="1:26" ht="13.5" customHeight="1">
       <c r="A27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -2503,13 +2513,13 @@
     </row>
     <row r="28" spans="1:26" ht="13.5" customHeight="1">
       <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -2537,13 +2547,13 @@
     </row>
     <row r="29" spans="1:26" ht="13.5" customHeight="1">
       <c r="A29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -2571,13 +2581,13 @@
     </row>
     <row r="30" spans="1:26" ht="13.5" customHeight="1">
       <c r="A30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -2661,13 +2671,13 @@
     </row>
     <row r="33" spans="1:26" ht="13.5" customHeight="1">
       <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -2695,13 +2705,13 @@
     </row>
     <row r="34" spans="1:26" ht="13.5" customHeight="1">
       <c r="A34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -2757,13 +2767,13 @@
     </row>
     <row r="36" spans="1:26" ht="13.5" customHeight="1">
       <c r="A36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -2819,13 +2829,13 @@
     </row>
     <row r="38" spans="1:26" ht="13.5" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -2881,13 +2891,13 @@
     </row>
     <row r="40" spans="1:26" ht="13.5" customHeight="1">
       <c r="A40" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="C40" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -2915,13 +2925,13 @@
     </row>
     <row r="41" spans="1:26" ht="13.5" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -2977,13 +2987,13 @@
     </row>
     <row r="43" spans="1:26" ht="13.5" customHeight="1">
       <c r="A43" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="C43" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -3011,13 +3021,13 @@
     </row>
     <row r="44" spans="1:26" ht="13.5" customHeight="1">
       <c r="A44" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="C44" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -3045,13 +3055,13 @@
     </row>
     <row r="45" spans="1:26" ht="13.5" customHeight="1">
       <c r="A45" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="C45" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -3135,13 +3145,13 @@
     </row>
     <row r="48" spans="1:26" ht="13.5" customHeight="1">
       <c r="A48" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="C48" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -3169,13 +3179,13 @@
     </row>
     <row r="49" spans="1:26" ht="13.5" customHeight="1">
       <c r="A49" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="C49" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -3203,7 +3213,7 @@
     </row>
     <row r="50" spans="1:26" ht="13.5" customHeight="1">
       <c r="A50" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -3289,13 +3299,13 @@
     </row>
     <row r="53" spans="1:26" ht="13.5" customHeight="1">
       <c r="A53" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="C53" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -3323,13 +3333,13 @@
     </row>
     <row r="54" spans="1:26" ht="13.5" customHeight="1">
       <c r="A54" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="C54" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -3357,7 +3367,7 @@
     </row>
     <row r="55" spans="1:26" ht="13.5" customHeight="1">
       <c r="A55" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -3443,13 +3453,13 @@
     </row>
     <row r="58" spans="1:26" ht="13.5" customHeight="1">
       <c r="A58" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="C58" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -3477,13 +3487,13 @@
     </row>
     <row r="59" spans="1:26" ht="13.5" customHeight="1">
       <c r="A59" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="C59" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -3511,7 +3521,7 @@
     </row>
     <row r="60" spans="1:26" ht="13.5" customHeight="1">
       <c r="A60" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -3597,13 +3607,13 @@
     </row>
     <row r="63" spans="1:26" ht="13.5" customHeight="1">
       <c r="A63" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -3631,13 +3641,13 @@
     </row>
     <row r="64" spans="1:26" ht="13.5" customHeight="1">
       <c r="A64" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -3721,13 +3731,13 @@
     </row>
     <row r="67" spans="1:26" ht="13.5" customHeight="1">
       <c r="A67" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -3755,13 +3765,13 @@
     </row>
     <row r="68" spans="1:26" ht="13.5" customHeight="1">
       <c r="A68" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -3845,13 +3855,13 @@
     </row>
     <row r="71" spans="1:26" ht="13.5" customHeight="1">
       <c r="A71" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="C71" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -3879,13 +3889,13 @@
     </row>
     <row r="72" spans="1:26" ht="13.5" customHeight="1">
       <c r="A72" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="C72" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -3913,13 +3923,13 @@
     </row>
     <row r="73" spans="1:26" ht="13.5" customHeight="1">
       <c r="A73" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="C73" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -3947,13 +3957,13 @@
     </row>
     <row r="74" spans="1:26" ht="13.5" customHeight="1">
       <c r="A74" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="C74" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -4037,13 +4047,13 @@
     </row>
     <row r="77" spans="1:26" ht="13.5" customHeight="1">
       <c r="A77" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -4071,13 +4081,13 @@
     </row>
     <row r="78" spans="1:26" ht="13.5" customHeight="1">
       <c r="A78" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -4133,13 +4143,13 @@
     </row>
     <row r="80" spans="1:26" ht="13.5" customHeight="1">
       <c r="A80" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B80" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="C80" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -4167,13 +4177,13 @@
     </row>
     <row r="81" spans="1:26" ht="13.5" customHeight="1">
       <c r="A81" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B81" s="8" t="s">
-        <v>88</v>
-      </c>
       <c r="C81" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -4201,13 +4211,13 @@
     </row>
     <row r="82" spans="1:26" ht="13.5" customHeight="1">
       <c r="A82" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B82" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B82" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="C82" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -4235,13 +4245,13 @@
     </row>
     <row r="83" spans="1:26" ht="13.5" customHeight="1">
       <c r="A83" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B83" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B83" s="8" t="s">
-        <v>92</v>
-      </c>
       <c r="C83" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -4269,13 +4279,13 @@
     </row>
     <row r="84" spans="1:26" ht="13.5" customHeight="1">
       <c r="A84" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B84" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="C84" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -4303,13 +4313,13 @@
     </row>
     <row r="85" spans="1:26" ht="13.5" customHeight="1">
       <c r="A85" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B85" s="8" t="s">
-        <v>96</v>
-      </c>
       <c r="C85" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -4337,13 +4347,13 @@
     </row>
     <row r="86" spans="1:26" ht="13.5" customHeight="1">
       <c r="A86" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="C86" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -4371,13 +4381,13 @@
     </row>
     <row r="87" spans="1:26" ht="13.5" customHeight="1">
       <c r="A87" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="C87" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -4405,13 +4415,13 @@
     </row>
     <row r="88" spans="1:26" ht="13.5" customHeight="1">
       <c r="A88" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="C88" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -4439,13 +4449,13 @@
     </row>
     <row r="89" spans="1:26" ht="13.5" customHeight="1">
       <c r="A89" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="C89" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -4473,13 +4483,13 @@
     </row>
     <row r="90" spans="1:26" ht="13.5" customHeight="1">
       <c r="A90" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="C90" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -4507,13 +4517,13 @@
     </row>
     <row r="91" spans="1:26" ht="13.5" customHeight="1">
       <c r="A91" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B91" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B91" s="8" t="s">
-        <v>108</v>
-      </c>
       <c r="C91" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -4541,13 +4551,13 @@
     </row>
     <row r="92" spans="1:26" ht="13.5" customHeight="1">
       <c r="A92" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B92" s="8" t="s">
-        <v>110</v>
-      </c>
       <c r="C92" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -4575,13 +4585,13 @@
     </row>
     <row r="93" spans="1:26" ht="13.5" customHeight="1">
       <c r="A93" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B93" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B93" s="8" t="s">
-        <v>112</v>
-      </c>
       <c r="C93" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -4609,13 +4619,13 @@
     </row>
     <row r="94" spans="1:26" ht="13.5" customHeight="1">
       <c r="A94" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B94" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>114</v>
-      </c>
       <c r="C94" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -4643,13 +4653,13 @@
     </row>
     <row r="95" spans="1:26" ht="13.5" customHeight="1">
       <c r="A95" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B95" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B95" s="8" t="s">
-        <v>116</v>
-      </c>
       <c r="C95" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -4677,13 +4687,13 @@
     </row>
     <row r="96" spans="1:26" ht="13.5" customHeight="1">
       <c r="A96" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="C96" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -4711,13 +4721,13 @@
     </row>
     <row r="97" spans="1:26" ht="13.5" customHeight="1">
       <c r="A97" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="C97" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -4745,13 +4755,13 @@
     </row>
     <row r="98" spans="1:26" ht="13.5" customHeight="1">
       <c r="A98" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="C98" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -4779,13 +4789,13 @@
     </row>
     <row r="99" spans="1:26" ht="13.5" customHeight="1">
       <c r="A99" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B99" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B99" s="9" t="s">
-        <v>124</v>
-      </c>
       <c r="C99" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -4813,13 +4823,13 @@
     </row>
     <row r="100" spans="1:26" ht="13.5" customHeight="1">
       <c r="A100" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="C100" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -4847,13 +4857,13 @@
     </row>
     <row r="101" spans="1:26" ht="13.5" customHeight="1">
       <c r="A101" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="C101" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -4881,13 +4891,13 @@
     </row>
     <row r="102" spans="1:26" ht="13.5" customHeight="1">
       <c r="A102" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B102" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B102" s="9" t="s">
-        <v>130</v>
-      </c>
       <c r="C102" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -4915,13 +4925,13 @@
     </row>
     <row r="103" spans="1:26" ht="13.5" customHeight="1">
       <c r="A103" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="C103" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
@@ -4949,13 +4959,13 @@
     </row>
     <row r="104" spans="1:26" ht="13.5" customHeight="1">
       <c r="A104" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B104" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="C104" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
@@ -4983,13 +4993,13 @@
     </row>
     <row r="105" spans="1:26" ht="13.5" customHeight="1">
       <c r="A105" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B105" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B105" s="8" t="s">
-        <v>136</v>
-      </c>
       <c r="C105" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
@@ -5017,13 +5027,13 @@
     </row>
     <row r="106" spans="1:26" ht="13.5" customHeight="1">
       <c r="A106" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B106" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B106" s="8" t="s">
-        <v>138</v>
-      </c>
       <c r="C106" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
@@ -5051,13 +5061,13 @@
     </row>
     <row r="107" spans="1:26" ht="13.5" customHeight="1">
       <c r="A107" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="C107" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
@@ -5085,13 +5095,13 @@
     </row>
     <row r="108" spans="1:26" ht="13.5" customHeight="1">
       <c r="A108" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B108" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B108" s="9" t="s">
-        <v>142</v>
-      </c>
       <c r="C108" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
@@ -5119,13 +5129,13 @@
     </row>
     <row r="109" spans="1:26" ht="13.5" customHeight="1">
       <c r="A109" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B109" s="8" t="s">
-        <v>144</v>
-      </c>
       <c r="C109" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
@@ -5153,13 +5163,13 @@
     </row>
     <row r="110" spans="1:26" ht="13.5" customHeight="1">
       <c r="A110" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B110" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B110" s="8" t="s">
-        <v>146</v>
-      </c>
       <c r="C110" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
@@ -5187,13 +5197,13 @@
     </row>
     <row r="111" spans="1:26" ht="13.5" customHeight="1">
       <c r="A111" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="C111" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
@@ -5221,13 +5231,13 @@
     </row>
     <row r="112" spans="1:26" ht="13.5" customHeight="1">
       <c r="A112" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="C112" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
@@ -5255,13 +5265,13 @@
     </row>
     <row r="113" spans="1:26" ht="13.5" customHeight="1">
       <c r="A113" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B113" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B113" s="9" t="s">
-        <v>152</v>
-      </c>
       <c r="C113" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
@@ -5289,13 +5299,13 @@
     </row>
     <row r="114" spans="1:26" ht="13.5" customHeight="1">
       <c r="A114" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B114" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="B114" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="C114" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
@@ -5323,13 +5333,13 @@
     </row>
     <row r="115" spans="1:26" ht="13.5" customHeight="1">
       <c r="A115" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="C115" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
@@ -5357,13 +5367,13 @@
     </row>
     <row r="116" spans="1:26" ht="13.5" customHeight="1">
       <c r="A116" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B116" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B116" s="8" t="s">
-        <v>158</v>
-      </c>
       <c r="C116" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
@@ -5391,13 +5401,13 @@
     </row>
     <row r="117" spans="1:26" ht="13.5" customHeight="1">
       <c r="A117" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="C117" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
@@ -5425,13 +5435,13 @@
     </row>
     <row r="118" spans="1:26" ht="13.5" customHeight="1">
       <c r="A118" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B118" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B118" s="8" t="s">
-        <v>162</v>
-      </c>
       <c r="C118" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
@@ -5459,13 +5469,13 @@
     </row>
     <row r="119" spans="1:26" ht="13.5" customHeight="1">
       <c r="A119" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="C119" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
@@ -5493,13 +5503,13 @@
     </row>
     <row r="120" spans="1:26" ht="13.5" customHeight="1">
       <c r="A120" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B120" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B120" s="8" t="s">
-        <v>166</v>
-      </c>
       <c r="C120" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
@@ -5527,13 +5537,13 @@
     </row>
     <row r="121" spans="1:26" ht="13.5" customHeight="1">
       <c r="A121" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="C121" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -5561,13 +5571,13 @@
     </row>
     <row r="122" spans="1:26" ht="13.5" customHeight="1">
       <c r="A122" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B122" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C122" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
@@ -5595,13 +5605,13 @@
     </row>
     <row r="123" spans="1:26" ht="13.5" customHeight="1">
       <c r="A123" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B123" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="C123" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
@@ -5657,13 +5667,13 @@
     </row>
     <row r="125" spans="1:26" ht="13.5" customHeight="1">
       <c r="A125" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="C125" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
@@ -5719,13 +5729,13 @@
     </row>
     <row r="127" spans="1:26" ht="13.5" customHeight="1">
       <c r="A127" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="C127" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
@@ -5753,13 +5763,13 @@
     </row>
     <row r="128" spans="1:26" ht="13.5" customHeight="1">
       <c r="A128" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B128" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B128" s="8" t="s">
-        <v>178</v>
-      </c>
       <c r="C128" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
@@ -5787,13 +5797,13 @@
     </row>
     <row r="129" spans="1:26" ht="13.5" customHeight="1">
       <c r="A129" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B129" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="B129" s="11" t="s">
-        <v>180</v>
-      </c>
       <c r="C129" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
@@ -5821,13 +5831,13 @@
     </row>
     <row r="130" spans="1:26" ht="13.5" customHeight="1">
       <c r="A130" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B130" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="B130" s="11" t="s">
-        <v>182</v>
-      </c>
       <c r="C130" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
@@ -5855,13 +5865,13 @@
     </row>
     <row r="131" spans="1:26" ht="13.5" customHeight="1">
       <c r="A131" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B131" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B131" s="11" t="s">
-        <v>184</v>
-      </c>
       <c r="C131" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
@@ -5889,13 +5899,13 @@
     </row>
     <row r="132" spans="1:26" ht="13.5" customHeight="1">
       <c r="A132" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B132" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="B132" s="12" t="s">
-        <v>186</v>
-      </c>
       <c r="C132" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
@@ -5923,13 +5933,13 @@
     </row>
     <row r="133" spans="1:26" ht="13.5" customHeight="1">
       <c r="A133" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B133" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="C133" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
@@ -5957,13 +5967,13 @@
     </row>
     <row r="134" spans="1:26" ht="13.5" customHeight="1">
       <c r="A134" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="C134" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
@@ -5991,13 +6001,13 @@
     </row>
     <row r="135" spans="1:26" ht="13.5" customHeight="1">
       <c r="A135" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B135" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="C135" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
@@ -6025,13 +6035,13 @@
     </row>
     <row r="136" spans="1:26" ht="13.5" customHeight="1">
       <c r="A136" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="C136" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
@@ -6059,13 +6069,13 @@
     </row>
     <row r="137" spans="1:26" ht="13.5" customHeight="1">
       <c r="A137" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B137" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="C137" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
@@ -6093,13 +6103,13 @@
     </row>
     <row r="138" spans="1:26" ht="13.5" customHeight="1">
       <c r="A138" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="C138" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
@@ -6127,13 +6137,13 @@
     </row>
     <row r="139" spans="1:26" ht="13.5" customHeight="1">
       <c r="A139" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="C139" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -6189,13 +6199,13 @@
     </row>
     <row r="141" spans="1:26" ht="13.5" customHeight="1">
       <c r="A141" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="C141" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
@@ -6223,13 +6233,13 @@
     </row>
     <row r="142" spans="1:26" ht="13.5" customHeight="1">
       <c r="A142" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B142" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="C142" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
@@ -6257,13 +6267,13 @@
     </row>
     <row r="143" spans="1:26" ht="13.5" customHeight="1">
       <c r="A143" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B143" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="C143" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
@@ -6291,13 +6301,13 @@
     </row>
     <row r="144" spans="1:26" ht="13.5" customHeight="1">
       <c r="A144" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B144" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="C144" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
@@ -6325,13 +6335,13 @@
     </row>
     <row r="145" spans="1:26" ht="13.5" customHeight="1">
       <c r="A145" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B145" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="C145" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
@@ -6359,13 +6369,13 @@
     </row>
     <row r="146" spans="1:26" ht="13.5" customHeight="1">
       <c r="A146" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
@@ -6393,13 +6403,13 @@
     </row>
     <row r="147" spans="1:26" ht="13.5" customHeight="1">
       <c r="A147" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -6427,13 +6437,13 @@
     </row>
     <row r="148" spans="1:26" ht="13.5" customHeight="1">
       <c r="A148" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="C148" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
@@ -6461,13 +6471,13 @@
     </row>
     <row r="149" spans="1:26" ht="13.5" customHeight="1">
       <c r="A149" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="C149" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
@@ -6495,13 +6505,13 @@
     </row>
     <row r="150" spans="1:26" ht="13.5" customHeight="1">
       <c r="A150" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="C150" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
@@ -6529,13 +6539,13 @@
     </row>
     <row r="151" spans="1:26" ht="13.5" customHeight="1">
       <c r="A151" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B151" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="B151" s="8" t="s">
-        <v>218</v>
-      </c>
       <c r="C151" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
@@ -6563,13 +6573,13 @@
     </row>
     <row r="152" spans="1:26" ht="13.5" customHeight="1">
       <c r="A152" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="C152" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
@@ -6597,13 +6607,13 @@
     </row>
     <row r="153" spans="1:26" ht="13.5" customHeight="1">
       <c r="A153" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>222</v>
-      </c>
       <c r="C153" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
@@ -6631,13 +6641,13 @@
     </row>
     <row r="154" spans="1:26" ht="13.5" customHeight="1">
       <c r="A154" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B154" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="C154" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
@@ -6665,13 +6675,13 @@
     </row>
     <row r="155" spans="1:26" ht="13.5" customHeight="1">
       <c r="A155" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B155" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="C155" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -6755,13 +6765,13 @@
     </row>
     <row r="158" spans="1:26" ht="13.5" customHeight="1">
       <c r="A158" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B158" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="B158" s="13" t="s">
-        <v>228</v>
-      </c>
       <c r="C158" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D158" s="8"/>
       <c r="E158" s="8"/>
@@ -6789,13 +6799,13 @@
     </row>
     <row r="159" spans="1:26" ht="13.5" customHeight="1">
       <c r="A159" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B159" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="B159" s="15" t="s">
-        <v>230</v>
-      </c>
       <c r="C159" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D159" s="8"/>
       <c r="E159" s="8"/>
@@ -6823,13 +6833,13 @@
     </row>
     <row r="160" spans="1:26" ht="13.5" customHeight="1">
       <c r="A160" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D160" s="8"/>
       <c r="E160" s="8"/>
@@ -6857,13 +6867,13 @@
     </row>
     <row r="161" spans="1:26" ht="13.5" customHeight="1">
       <c r="A161" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B161" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="B161" s="8" t="s">
-        <v>233</v>
-      </c>
       <c r="C161" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
@@ -6891,13 +6901,13 @@
     </row>
     <row r="162" spans="1:26" ht="13.5" customHeight="1">
       <c r="A162" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B162" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="C162" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
@@ -6925,13 +6935,13 @@
     </row>
     <row r="163" spans="1:26" ht="13.5" customHeight="1">
       <c r="A163" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B163" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="B163" s="8" t="s">
-        <v>237</v>
-      </c>
       <c r="C163" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
@@ -6959,13 +6969,13 @@
     </row>
     <row r="164" spans="1:26" ht="13.5" customHeight="1">
       <c r="A164" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B164" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="B164" s="4" t="s">
-        <v>239</v>
-      </c>
       <c r="C164" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
@@ -6993,13 +7003,13 @@
     </row>
     <row r="165" spans="1:26" ht="13.5" customHeight="1">
       <c r="A165" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B165" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="C165" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
@@ -7027,13 +7037,13 @@
     </row>
     <row r="166" spans="1:26" ht="13.5" customHeight="1">
       <c r="A166" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
@@ -7061,13 +7071,13 @@
     </row>
     <row r="167" spans="1:26" ht="13.5" customHeight="1">
       <c r="A167" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B167" s="1" t="s">
-        <v>244</v>
-      </c>
       <c r="C167" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
@@ -7179,13 +7189,13 @@
     </row>
     <row r="171" spans="1:26" ht="13.5" customHeight="1">
       <c r="A171" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B171" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C171" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D171" s="1"/>
       <c r="E171" s="1"/>
@@ -7213,13 +7223,13 @@
     </row>
     <row r="172" spans="1:26" ht="13.5" customHeight="1">
       <c r="A172" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
@@ -7247,13 +7257,13 @@
     </row>
     <row r="173" spans="1:26" ht="13.5" customHeight="1">
       <c r="A173" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B173" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B173" s="5" t="s">
-        <v>248</v>
-      </c>
       <c r="C173" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
@@ -7281,13 +7291,13 @@
     </row>
     <row r="174" spans="1:26" ht="13.5" customHeight="1">
       <c r="A174" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B174" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="B174" s="8" t="s">
-        <v>250</v>
-      </c>
       <c r="C174" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
@@ -7315,13 +7325,13 @@
     </row>
     <row r="175" spans="1:26" ht="13.5" customHeight="1">
       <c r="A175" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B175" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="B175" s="8" t="s">
-        <v>252</v>
-      </c>
       <c r="C175" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
@@ -7349,7 +7359,7 @@
     </row>
     <row r="176" spans="1:26" ht="13.5" customHeight="1">
       <c r="A176" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
@@ -7379,7 +7389,7 @@
     </row>
     <row r="177" spans="1:26" ht="13.5" customHeight="1">
       <c r="A177" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
@@ -7409,13 +7419,13 @@
     </row>
     <row r="178" spans="1:26" ht="13.5" customHeight="1">
       <c r="A178" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B178" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="B178" s="8" t="s">
-        <v>256</v>
-      </c>
       <c r="C178" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D178" s="1"/>
       <c r="E178" s="1"/>
@@ -7443,13 +7453,13 @@
     </row>
     <row r="179" spans="1:26" ht="13.5" customHeight="1">
       <c r="A179" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B179" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="B179" s="8" t="s">
-        <v>258</v>
-      </c>
       <c r="C179" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
@@ -7505,13 +7515,13 @@
     </row>
     <row r="181" spans="1:26" ht="13.5" customHeight="1">
       <c r="A181" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="B181" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="B181" s="8" t="s">
-        <v>260</v>
-      </c>
       <c r="C181" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D181" s="1"/>
       <c r="E181" s="1"/>
@@ -7540,10 +7550,10 @@
     <row r="182" spans="1:26" ht="13.5" customHeight="1">
       <c r="A182" s="14"/>
       <c r="B182" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D182" s="1"/>
       <c r="E182" s="1"/>
@@ -7571,13 +7581,13 @@
     </row>
     <row r="183" spans="1:26" ht="13.5" customHeight="1">
       <c r="A183" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="B183" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="B183" s="17" t="s">
-        <v>263</v>
-      </c>
       <c r="C183" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D183" s="1"/>
       <c r="E183" s="1"/>
@@ -7605,13 +7615,13 @@
     </row>
     <row r="184" spans="1:26" ht="13.5" customHeight="1">
       <c r="A184" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="B184" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="B184" s="8" t="s">
-        <v>265</v>
-      </c>
       <c r="C184" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D184" s="1"/>
       <c r="E184" s="1"/>
@@ -7639,13 +7649,13 @@
     </row>
     <row r="185" spans="1:26" ht="13.5" customHeight="1">
       <c r="A185" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="B185" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="B185" s="8" t="s">
-        <v>267</v>
-      </c>
       <c r="C185" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D185" s="1"/>
       <c r="E185" s="1"/>
@@ -7673,13 +7683,13 @@
     </row>
     <row r="186" spans="1:26" ht="13.5" customHeight="1">
       <c r="A186" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="B186" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B186" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="C186" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D186" s="1"/>
       <c r="E186" s="1"/>
@@ -7707,13 +7717,13 @@
     </row>
     <row r="187" spans="1:26" ht="13.5" customHeight="1">
       <c r="A187" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B187" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="B187" s="8" t="s">
-        <v>271</v>
-      </c>
       <c r="C187" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D187" s="1"/>
       <c r="E187" s="1"/>
@@ -7741,13 +7751,13 @@
     </row>
     <row r="188" spans="1:26" ht="13.5" customHeight="1">
       <c r="A188" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B188" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="B188" s="8" t="s">
-        <v>230</v>
-      </c>
       <c r="C188" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>
@@ -7803,13 +7813,13 @@
     </row>
     <row r="190" spans="1:26" ht="13.5" customHeight="1">
       <c r="A190" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B190" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="B190" s="8" t="s">
-        <v>273</v>
-      </c>
       <c r="C190" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D190" s="1"/>
       <c r="E190" s="1"/>
@@ -7837,13 +7847,13 @@
     </row>
     <row r="191" spans="1:26" ht="13.5" customHeight="1">
       <c r="A191" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B191" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="B191" s="8" t="s">
-        <v>275</v>
-      </c>
       <c r="C191" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D191" s="1"/>
       <c r="E191" s="1"/>
@@ -7871,13 +7881,13 @@
     </row>
     <row r="192" spans="1:26" ht="13.5" customHeight="1">
       <c r="A192" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B192" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="B192" s="8" t="s">
-        <v>277</v>
-      </c>
       <c r="C192" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D192" s="1"/>
       <c r="E192" s="1"/>
@@ -7905,13 +7915,13 @@
     </row>
     <row r="193" spans="1:26" ht="13.5" customHeight="1">
       <c r="A193" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B193" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B193" s="8" t="s">
-        <v>279</v>
-      </c>
       <c r="C193" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D193" s="1"/>
       <c r="E193" s="1"/>
@@ -7939,13 +7949,13 @@
     </row>
     <row r="194" spans="1:26" ht="13.5" customHeight="1">
       <c r="A194" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B194" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B194" s="1" t="s">
-        <v>281</v>
-      </c>
       <c r="C194" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D194" s="1"/>
       <c r="E194" s="1"/>
@@ -7973,13 +7983,13 @@
     </row>
     <row r="195" spans="1:26" ht="13.5" customHeight="1">
       <c r="A195" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B195" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B195" s="1" t="s">
-        <v>283</v>
-      </c>
       <c r="C195" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D195" s="1"/>
       <c r="E195" s="1"/>
@@ -8007,13 +8017,13 @@
     </row>
     <row r="196" spans="1:26" ht="13.5" customHeight="1">
       <c r="A196" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B196" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B196" s="1" t="s">
-        <v>285</v>
-      </c>
       <c r="C196" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D196" s="1"/>
       <c r="E196" s="1"/>
@@ -8041,13 +8051,13 @@
     </row>
     <row r="197" spans="1:26" ht="13.5" customHeight="1">
       <c r="A197" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B197" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B197" s="1" t="s">
-        <v>287</v>
-      </c>
       <c r="C197" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D197" s="1"/>
       <c r="E197" s="1"/>
@@ -8075,13 +8085,13 @@
     </row>
     <row r="198" spans="1:26" ht="13.5" customHeight="1">
       <c r="A198" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B198" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B198" s="1" t="s">
-        <v>289</v>
-      </c>
       <c r="C198" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D198" s="1"/>
       <c r="E198" s="1"/>
@@ -8109,13 +8119,13 @@
     </row>
     <row r="199" spans="1:26" ht="13.5" customHeight="1">
       <c r="A199" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B199" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B199" s="1" t="s">
-        <v>291</v>
-      </c>
       <c r="C199" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D199" s="1"/>
       <c r="E199" s="1"/>
@@ -8143,13 +8153,13 @@
     </row>
     <row r="200" spans="1:26" ht="13.5" customHeight="1">
       <c r="A200" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B200" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B200" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="C200" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D200" s="1"/>
       <c r="E200" s="1"/>
@@ -8177,13 +8187,13 @@
     </row>
     <row r="201" spans="1:26" ht="13.5" customHeight="1">
       <c r="A201" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B201" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B201" s="1" t="s">
-        <v>295</v>
-      </c>
       <c r="C201" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D201" s="1"/>
       <c r="E201" s="1"/>
@@ -8211,13 +8221,13 @@
     </row>
     <row r="202" spans="1:26" ht="13.5" customHeight="1">
       <c r="A202" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B202" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B202" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="C202" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D202" s="1"/>
       <c r="E202" s="1"/>
@@ -8245,13 +8255,13 @@
     </row>
     <row r="203" spans="1:26" ht="13.5" customHeight="1">
       <c r="A203" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B203" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B203" s="1" t="s">
-        <v>299</v>
-      </c>
       <c r="C203" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D203" s="1"/>
       <c r="E203" s="1"/>
@@ -8279,13 +8289,13 @@
     </row>
     <row r="204" spans="1:26" ht="13.5" customHeight="1">
       <c r="A204" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B204" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B204" s="1" t="s">
-        <v>301</v>
-      </c>
       <c r="C204" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D204" s="1"/>
       <c r="E204" s="1"/>
@@ -8313,13 +8323,13 @@
     </row>
     <row r="205" spans="1:26" ht="13.5" customHeight="1">
       <c r="A205" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B205" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="B205" s="10" t="s">
-        <v>303</v>
-      </c>
       <c r="C205" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D205" s="1"/>
       <c r="E205" s="1"/>
@@ -8347,13 +8357,13 @@
     </row>
     <row r="206" spans="1:26" ht="13.5" customHeight="1">
       <c r="A206" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B206" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B206" s="1" t="s">
-        <v>305</v>
-      </c>
       <c r="C206" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>
@@ -8381,13 +8391,13 @@
     </row>
     <row r="207" spans="1:26" ht="13.5" customHeight="1">
       <c r="A207" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B207" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B207" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="C207" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D207" s="1"/>
       <c r="E207" s="1"/>
@@ -8415,13 +8425,13 @@
     </row>
     <row r="208" spans="1:26" ht="13.5" customHeight="1">
       <c r="A208" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D208" s="1"/>
       <c r="E208" s="1"/>
@@ -8449,13 +8459,13 @@
     </row>
     <row r="209" spans="1:26" ht="13.5" customHeight="1">
       <c r="A209" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B209" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C209" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D209" s="1"/>
       <c r="E209" s="1"/>
@@ -8483,13 +8493,13 @@
     </row>
     <row r="210" spans="1:26" ht="13.5" customHeight="1">
       <c r="A210" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D210" s="1"/>
       <c r="E210" s="1"/>
@@ -8517,13 +8527,13 @@
     </row>
     <row r="211" spans="1:26" ht="13.5" customHeight="1">
       <c r="A211" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B211" s="1" t="s">
-        <v>312</v>
-      </c>
       <c r="C211" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D211" s="1"/>
       <c r="E211" s="1"/>
@@ -8551,13 +8561,13 @@
     </row>
     <row r="212" spans="1:26" ht="13.5" customHeight="1">
       <c r="A212" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B212" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B212" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="C212" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D212" s="1"/>
       <c r="E212" s="1"/>
@@ -8585,13 +8595,13 @@
     </row>
     <row r="213" spans="1:26" ht="13.5" customHeight="1">
       <c r="A213" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B213" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B213" s="1" t="s">
-        <v>316</v>
-      </c>
       <c r="C213" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D213" s="1"/>
       <c r="E213" s="1"/>
@@ -8619,13 +8629,13 @@
     </row>
     <row r="214" spans="1:26" ht="13.5" customHeight="1">
       <c r="A214" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D214" s="1"/>
       <c r="E214" s="1"/>
@@ -8653,13 +8663,13 @@
     </row>
     <row r="215" spans="1:26" ht="13.5" customHeight="1">
       <c r="A215" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B215" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="B215" s="1" t="s">
-        <v>319</v>
-      </c>
       <c r="C215" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D215" s="1"/>
       <c r="E215" s="1"/>
@@ -8687,13 +8697,13 @@
     </row>
     <row r="216" spans="1:26" ht="13.5" customHeight="1">
       <c r="A216" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B216" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="B216" s="11" t="s">
-        <v>321</v>
-      </c>
       <c r="C216" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D216" s="1"/>
       <c r="E216" s="1"/>
@@ -8721,13 +8731,13 @@
     </row>
     <row r="217" spans="1:26" ht="13.5" customHeight="1">
       <c r="A217" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B217" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="B217" s="11" t="s">
-        <v>323</v>
-      </c>
       <c r="C217" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D217" s="1"/>
       <c r="E217" s="1"/>
@@ -8755,13 +8765,13 @@
     </row>
     <row r="218" spans="1:26" ht="13.5" customHeight="1">
       <c r="A218" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B218" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B218" s="1" t="s">
-        <v>325</v>
-      </c>
       <c r="C218" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D218" s="1"/>
       <c r="E218" s="1"/>
@@ -8789,13 +8799,13 @@
     </row>
     <row r="219" spans="1:26" ht="13.5" customHeight="1">
       <c r="A219" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B219" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="B219" s="12" t="s">
-        <v>327</v>
-      </c>
       <c r="C219" s="12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D219" s="1"/>
       <c r="E219" s="1"/>
@@ -8823,13 +8833,13 @@
     </row>
     <row r="220" spans="1:26" ht="13.5" customHeight="1">
       <c r="A220" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B220" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="B220" s="11" t="s">
-        <v>329</v>
-      </c>
       <c r="C220" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D220" s="1"/>
       <c r="E220" s="1"/>
@@ -8857,13 +8867,13 @@
     </row>
     <row r="221" spans="1:26" ht="13.5" customHeight="1">
       <c r="A221" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B221" s="18" t="s">
         <v>330</v>
       </c>
-      <c r="B221" s="18" t="s">
-        <v>331</v>
-      </c>
       <c r="C221" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D221" s="1"/>
       <c r="E221" s="1"/>
@@ -8891,13 +8901,13 @@
     </row>
     <row r="222" spans="1:26" ht="13.5" customHeight="1">
       <c r="A222" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D222" s="1"/>
       <c r="E222" s="1"/>
@@ -8925,13 +8935,13 @@
     </row>
     <row r="223" spans="1:26" ht="13.5" customHeight="1">
       <c r="A223" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B223" s="11" t="s">
         <v>333</v>
       </c>
-      <c r="B223" s="11" t="s">
-        <v>334</v>
-      </c>
       <c r="C223" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D223" s="1"/>
       <c r="E223" s="1"/>
@@ -8959,13 +8969,13 @@
     </row>
     <row r="224" spans="1:26" ht="13.5" customHeight="1">
       <c r="A224" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B224" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B224" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="C224" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D224" s="1"/>
       <c r="E224" s="1"/>
@@ -8993,13 +9003,13 @@
     </row>
     <row r="225" spans="1:26" ht="13.5" customHeight="1">
       <c r="A225" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B225" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="B225" s="12" t="s">
-        <v>338</v>
-      </c>
       <c r="C225" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D225" s="1"/>
       <c r="E225" s="1"/>
@@ -9027,13 +9037,13 @@
     </row>
     <row r="226" spans="1:26" ht="13.5" customHeight="1">
       <c r="A226" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D226" s="1"/>
       <c r="E226" s="1"/>
@@ -9061,13 +9071,13 @@
     </row>
     <row r="227" spans="1:26" ht="13.5" customHeight="1">
       <c r="A227" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B227" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="B227" s="12" t="s">
-        <v>340</v>
-      </c>
       <c r="C227" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D227" s="1"/>
       <c r="E227" s="1"/>
@@ -9095,13 +9105,13 @@
     </row>
     <row r="228" spans="1:26" ht="13.5" customHeight="1">
       <c r="A228" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B228" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C228" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D228" s="1"/>
       <c r="E228" s="1"/>
@@ -9129,13 +9139,13 @@
     </row>
     <row r="229" spans="1:26" ht="13.5" customHeight="1">
       <c r="A229" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B229" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="B229" s="12" t="s">
-        <v>342</v>
-      </c>
       <c r="C229" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D229" s="1"/>
       <c r="E229" s="1"/>
@@ -30821,7 +30831,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -30850,10 +30860,10 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>7</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -30882,10 +30892,10 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>9</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -30914,10 +30924,10 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -30946,10 +30956,10 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -30978,10 +30988,10 @@
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
@@ -31010,10 +31020,10 @@
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -31070,10 +31080,10 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -31102,10 +31112,10 @@
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -31134,7 +31144,7 @@
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B12" s="22">
         <v>784512369</v>
@@ -31166,10 +31176,10 @@
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -31198,10 +31208,10 @@
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -31258,10 +31268,10 @@
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -31290,10 +31300,10 @@
     </row>
     <row r="17" spans="1:26">
       <c r="A17" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -31322,10 +31332,10 @@
     </row>
     <row r="18" spans="1:26">
       <c r="A18" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -31354,10 +31364,10 @@
     </row>
     <row r="19" spans="1:26">
       <c r="A19" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -31414,10 +31424,10 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -31446,10 +31456,10 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -31478,10 +31488,10 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
@@ -31510,10 +31520,10 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
@@ -31570,10 +31580,10 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
@@ -31602,10 +31612,10 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
@@ -31634,10 +31644,10 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>349</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>350</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -31666,10 +31676,10 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
@@ -31698,10 +31708,10 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>16</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>17</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
@@ -31758,10 +31768,10 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -31790,10 +31800,10 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -31822,7 +31832,7 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B34" s="22">
         <v>784512369</v>
@@ -31854,10 +31864,10 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="B35" s="19" t="s">
         <v>354</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>355</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -31886,10 +31896,10 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
@@ -31946,10 +31956,10 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="19" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="19"/>
@@ -31978,10 +31988,10 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -32010,10 +32020,10 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C40" s="19"/>
       <c r="D40" s="19"/>
@@ -32042,10 +32052,10 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
@@ -32102,10 +32112,10 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>359</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>360</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
@@ -32134,10 +32144,10 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="19" t="s">
+        <v>360</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>361</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>362</v>
       </c>
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
@@ -32166,10 +32176,10 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
       <c r="A45" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
@@ -32198,10 +32208,10 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>363</v>
-      </c>
-      <c r="B46" s="19" t="s">
-        <v>364</v>
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
@@ -32258,10 +32268,10 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C48" s="19"/>
       <c r="D48" s="19"/>
@@ -32290,10 +32300,10 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
@@ -32322,7 +32332,7 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B50" s="22">
         <v>784512369</v>
@@ -32354,10 +32364,10 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>367</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>368</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
@@ -32386,10 +32396,10 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1">
       <c r="A52" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C52" s="19"/>
       <c r="D52" s="19"/>
@@ -32446,10 +32456,10 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1">
       <c r="A54" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C54" s="19"/>
       <c r="D54" s="19"/>
@@ -32478,10 +32488,10 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1">
       <c r="A55" s="19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
@@ -32510,10 +32520,10 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1">
       <c r="A56" s="19" t="s">
+        <v>370</v>
+      </c>
+      <c r="B56" s="19" t="s">
         <v>371</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>372</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
@@ -32542,10 +32552,10 @@
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1">
       <c r="A57" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="B57" s="19" t="s">
-        <v>17</v>
       </c>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
@@ -32602,10 +32612,10 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1">
       <c r="A59" s="19" t="s">
+        <v>372</v>
+      </c>
+      <c r="B59" s="19" t="s">
         <v>373</v>
-      </c>
-      <c r="B59" s="19" t="s">
-        <v>374</v>
       </c>
       <c r="C59" s="19"/>
       <c r="D59" s="19"/>
@@ -32634,10 +32644,10 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1">
       <c r="A60" s="19" t="s">
+        <v>374</v>
+      </c>
+      <c r="B60" s="23" t="s">
         <v>375</v>
-      </c>
-      <c r="B60" s="23" t="s">
-        <v>376</v>
       </c>
       <c r="C60" s="19"/>
       <c r="D60" s="19"/>
@@ -32666,10 +32676,10 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1">
       <c r="A61" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="B61" s="23" t="s">
         <v>377</v>
-      </c>
-      <c r="B61" s="23" t="s">
-        <v>378</v>
       </c>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
@@ -32698,10 +32708,10 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1">
       <c r="A62" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="B62" s="23" t="s">
         <v>379</v>
-      </c>
-      <c r="B62" s="23" t="s">
-        <v>380</v>
       </c>
       <c r="C62" s="19"/>
       <c r="D62" s="19"/>
@@ -32730,10 +32740,10 @@
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1">
       <c r="A63" s="19" t="s">
+        <v>380</v>
+      </c>
+      <c r="B63" s="23" t="s">
         <v>381</v>
-      </c>
-      <c r="B63" s="23" t="s">
-        <v>382</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
@@ -32762,10 +32772,10 @@
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1">
       <c r="A64" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="B64" s="23" t="s">
         <v>383</v>
-      </c>
-      <c r="B64" s="23" t="s">
-        <v>384</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
@@ -32794,10 +32804,10 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1">
       <c r="A65" s="19" t="s">
+        <v>384</v>
+      </c>
+      <c r="B65" s="23" t="s">
         <v>385</v>
-      </c>
-      <c r="B65" s="23" t="s">
-        <v>386</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
@@ -32826,10 +32836,10 @@
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1">
       <c r="A66" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="B66" s="23" t="s">
         <v>387</v>
-      </c>
-      <c r="B66" s="23" t="s">
-        <v>388</v>
       </c>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
@@ -32858,10 +32868,10 @@
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1">
       <c r="A67" s="19" t="s">
+        <v>388</v>
+      </c>
+      <c r="B67" s="23" t="s">
         <v>389</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>390</v>
       </c>
       <c r="C67" s="19"/>
       <c r="D67" s="19"/>
@@ -32890,10 +32900,10 @@
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1">
       <c r="A68" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="B68" s="23" t="s">
         <v>391</v>
-      </c>
-      <c r="B68" s="23" t="s">
-        <v>392</v>
       </c>
       <c r="C68" s="19"/>
       <c r="D68" s="19"/>
@@ -32922,10 +32932,10 @@
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1">
       <c r="A69" s="19" t="s">
+        <v>392</v>
+      </c>
+      <c r="B69" s="23" t="s">
         <v>393</v>
-      </c>
-      <c r="B69" s="23" t="s">
-        <v>394</v>
       </c>
       <c r="C69" s="19"/>
       <c r="D69" s="19"/>
@@ -32954,10 +32964,10 @@
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1">
       <c r="A70" s="19" t="s">
+        <v>394</v>
+      </c>
+      <c r="B70" s="23" t="s">
         <v>395</v>
-      </c>
-      <c r="B70" s="23" t="s">
-        <v>396</v>
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="19"/>
@@ -32986,10 +32996,10 @@
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1">
       <c r="A71" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="B71" s="23" t="s">
         <v>397</v>
-      </c>
-      <c r="B71" s="23" t="s">
-        <v>398</v>
       </c>
       <c r="C71" s="19"/>
       <c r="D71" s="19"/>
@@ -33018,10 +33028,10 @@
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1">
       <c r="A72" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="B72" s="23" t="s">
         <v>399</v>
-      </c>
-      <c r="B72" s="23" t="s">
-        <v>400</v>
       </c>
       <c r="C72" s="19"/>
       <c r="D72" s="19"/>

</xml_diff>

<commit_message>
1. Appointments Loading Error fixed. 2. Windows time zone changing script added. 3. RRP Amount is updated.
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -263,9 +263,6 @@
   </si>
   <si>
     <t>URGENCY PRICE</t>
-  </si>
-  <si>
-    <t>Urgent/Same day - Fee: NZ$11.00 (Incl. GST);Next Day - Fee: NZ$12.00 (Incl. GST);48 Hours - Fee: NZ$13.00 (Incl. GST);72 Hours - Fee: NZ$14.00 (Incl. GST)</t>
   </si>
   <si>
     <t>EMAIL_FOR_HEALTH</t>
@@ -1224,6 +1221,9 @@
   <si>
     <t>https://v2webfeature.mmh-demo.com/home</t>
   </si>
+  <si>
+    <t>Urgent/Same day - Fee: NZ$40.01 (Incl. GST);Next Day - Fee: NZ$40.04 (Incl. GST);48 Hours - Fee: NZ$40.07 (Incl. GST);72 Hours - Fee: NZ$50.10 (Incl. GST)</t>
+  </si>
 </sst>
 </file>
 
@@ -1605,15 +1605,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="C55" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="69.5703125" customWidth="1"/>
     <col min="2" max="2" width="161.42578125" customWidth="1"/>
-    <col min="3" max="3" width="148.7109375" customWidth="1"/>
+    <col min="3" max="3" width="161.140625" customWidth="1"/>
     <col min="4" max="23" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1656,7 +1656,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -3960,10 +3960,10 @@
         <v>80</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>81</v>
+        <v>400</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>81</v>
+        <v>400</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -4047,7 +4047,7 @@
     </row>
     <row r="77" spans="1:26" ht="13.5" customHeight="1">
       <c r="A77" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>47</v>
@@ -4081,7 +4081,7 @@
     </row>
     <row r="78" spans="1:26" ht="13.5" customHeight="1">
       <c r="A78" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>8</v>
@@ -4143,13 +4143,13 @@
     </row>
     <row r="80" spans="1:26" ht="13.5" customHeight="1">
       <c r="A80" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B80" s="8" t="s">
-        <v>85</v>
-      </c>
       <c r="C80" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -4177,13 +4177,13 @@
     </row>
     <row r="81" spans="1:26" ht="13.5" customHeight="1">
       <c r="A81" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B81" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="C81" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -4211,13 +4211,13 @@
     </row>
     <row r="82" spans="1:26" ht="13.5" customHeight="1">
       <c r="A82" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B82" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="C82" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -4245,13 +4245,13 @@
     </row>
     <row r="83" spans="1:26" ht="13.5" customHeight="1">
       <c r="A83" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B83" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B83" s="8" t="s">
-        <v>91</v>
-      </c>
       <c r="C83" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -4279,13 +4279,13 @@
     </row>
     <row r="84" spans="1:26" ht="13.5" customHeight="1">
       <c r="A84" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B84" s="8" t="s">
-        <v>93</v>
-      </c>
       <c r="C84" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -4313,13 +4313,13 @@
     </row>
     <row r="85" spans="1:26" ht="13.5" customHeight="1">
       <c r="A85" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B85" s="8" t="s">
-        <v>95</v>
-      </c>
       <c r="C85" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -4347,13 +4347,13 @@
     </row>
     <row r="86" spans="1:26" ht="13.5" customHeight="1">
       <c r="A86" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C86" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -4381,13 +4381,13 @@
     </row>
     <row r="87" spans="1:26" ht="13.5" customHeight="1">
       <c r="A87" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="C87" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -4415,13 +4415,13 @@
     </row>
     <row r="88" spans="1:26" ht="13.5" customHeight="1">
       <c r="A88" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="C88" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -4449,13 +4449,13 @@
     </row>
     <row r="89" spans="1:26" ht="13.5" customHeight="1">
       <c r="A89" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="C89" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -4483,13 +4483,13 @@
     </row>
     <row r="90" spans="1:26" ht="13.5" customHeight="1">
       <c r="A90" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="C90" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -4517,13 +4517,13 @@
     </row>
     <row r="91" spans="1:26" ht="13.5" customHeight="1">
       <c r="A91" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B91" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B91" s="8" t="s">
-        <v>107</v>
-      </c>
       <c r="C91" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -4551,13 +4551,13 @@
     </row>
     <row r="92" spans="1:26" ht="13.5" customHeight="1">
       <c r="A92" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B92" s="8" t="s">
-        <v>109</v>
-      </c>
       <c r="C92" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -4585,13 +4585,13 @@
     </row>
     <row r="93" spans="1:26" ht="13.5" customHeight="1">
       <c r="A93" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B93" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B93" s="8" t="s">
-        <v>111</v>
-      </c>
       <c r="C93" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -4619,13 +4619,13 @@
     </row>
     <row r="94" spans="1:26" ht="13.5" customHeight="1">
       <c r="A94" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B94" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="C94" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -4653,13 +4653,13 @@
     </row>
     <row r="95" spans="1:26" ht="13.5" customHeight="1">
       <c r="A95" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B95" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B95" s="8" t="s">
-        <v>115</v>
-      </c>
       <c r="C95" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -4687,13 +4687,13 @@
     </row>
     <row r="96" spans="1:26" ht="13.5" customHeight="1">
       <c r="A96" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="C96" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -4721,13 +4721,13 @@
     </row>
     <row r="97" spans="1:26" ht="13.5" customHeight="1">
       <c r="A97" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="C97" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -4755,13 +4755,13 @@
     </row>
     <row r="98" spans="1:26" ht="13.5" customHeight="1">
       <c r="A98" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="C98" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -4789,13 +4789,13 @@
     </row>
     <row r="99" spans="1:26" ht="13.5" customHeight="1">
       <c r="A99" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B99" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B99" s="9" t="s">
-        <v>123</v>
-      </c>
       <c r="C99" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -4823,13 +4823,13 @@
     </row>
     <row r="100" spans="1:26" ht="13.5" customHeight="1">
       <c r="A100" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="C100" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -4857,13 +4857,13 @@
     </row>
     <row r="101" spans="1:26" ht="13.5" customHeight="1">
       <c r="A101" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="C101" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -4891,13 +4891,13 @@
     </row>
     <row r="102" spans="1:26" ht="13.5" customHeight="1">
       <c r="A102" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B102" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B102" s="9" t="s">
-        <v>129</v>
-      </c>
       <c r="C102" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -4925,13 +4925,13 @@
     </row>
     <row r="103" spans="1:26" ht="13.5" customHeight="1">
       <c r="A103" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="C103" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
@@ -4959,13 +4959,13 @@
     </row>
     <row r="104" spans="1:26" ht="13.5" customHeight="1">
       <c r="A104" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B104" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="C104" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
@@ -4993,13 +4993,13 @@
     </row>
     <row r="105" spans="1:26" ht="13.5" customHeight="1">
       <c r="A105" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B105" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B105" s="8" t="s">
-        <v>135</v>
-      </c>
       <c r="C105" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
@@ -5027,13 +5027,13 @@
     </row>
     <row r="106" spans="1:26" ht="13.5" customHeight="1">
       <c r="A106" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B106" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B106" s="8" t="s">
-        <v>137</v>
-      </c>
       <c r="C106" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
@@ -5061,13 +5061,13 @@
     </row>
     <row r="107" spans="1:26" ht="13.5" customHeight="1">
       <c r="A107" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="C107" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
@@ -5095,13 +5095,13 @@
     </row>
     <row r="108" spans="1:26" ht="13.5" customHeight="1">
       <c r="A108" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B108" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B108" s="9" t="s">
-        <v>141</v>
-      </c>
       <c r="C108" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
@@ -5129,13 +5129,13 @@
     </row>
     <row r="109" spans="1:26" ht="13.5" customHeight="1">
       <c r="A109" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B109" s="8" t="s">
-        <v>143</v>
-      </c>
       <c r="C109" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
@@ -5163,13 +5163,13 @@
     </row>
     <row r="110" spans="1:26" ht="13.5" customHeight="1">
       <c r="A110" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B110" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B110" s="8" t="s">
-        <v>145</v>
-      </c>
       <c r="C110" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
@@ -5197,13 +5197,13 @@
     </row>
     <row r="111" spans="1:26" ht="13.5" customHeight="1">
       <c r="A111" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="C111" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
@@ -5231,13 +5231,13 @@
     </row>
     <row r="112" spans="1:26" ht="13.5" customHeight="1">
       <c r="A112" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="C112" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
@@ -5265,13 +5265,13 @@
     </row>
     <row r="113" spans="1:26" ht="13.5" customHeight="1">
       <c r="A113" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B113" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B113" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="C113" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
@@ -5299,13 +5299,13 @@
     </row>
     <row r="114" spans="1:26" ht="13.5" customHeight="1">
       <c r="A114" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B114" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B114" s="8" t="s">
-        <v>153</v>
-      </c>
       <c r="C114" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
@@ -5333,13 +5333,13 @@
     </row>
     <row r="115" spans="1:26" ht="13.5" customHeight="1">
       <c r="A115" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="C115" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
@@ -5367,13 +5367,13 @@
     </row>
     <row r="116" spans="1:26" ht="13.5" customHeight="1">
       <c r="A116" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B116" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B116" s="8" t="s">
-        <v>157</v>
-      </c>
       <c r="C116" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
@@ -5401,13 +5401,13 @@
     </row>
     <row r="117" spans="1:26" ht="13.5" customHeight="1">
       <c r="A117" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="C117" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
@@ -5435,13 +5435,13 @@
     </row>
     <row r="118" spans="1:26" ht="13.5" customHeight="1">
       <c r="A118" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B118" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B118" s="8" t="s">
-        <v>161</v>
-      </c>
       <c r="C118" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
@@ -5469,13 +5469,13 @@
     </row>
     <row r="119" spans="1:26" ht="13.5" customHeight="1">
       <c r="A119" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="C119" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
@@ -5503,13 +5503,13 @@
     </row>
     <row r="120" spans="1:26" ht="13.5" customHeight="1">
       <c r="A120" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B120" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B120" s="8" t="s">
-        <v>165</v>
-      </c>
       <c r="C120" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
@@ -5537,13 +5537,13 @@
     </row>
     <row r="121" spans="1:26" ht="13.5" customHeight="1">
       <c r="A121" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="C121" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -5571,13 +5571,13 @@
     </row>
     <row r="122" spans="1:26" ht="13.5" customHeight="1">
       <c r="A122" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B122" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="C122" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
@@ -5605,13 +5605,13 @@
     </row>
     <row r="123" spans="1:26" ht="13.5" customHeight="1">
       <c r="A123" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B123" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="C123" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
@@ -5667,13 +5667,13 @@
     </row>
     <row r="125" spans="1:26" ht="13.5" customHeight="1">
       <c r="A125" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="C125" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
@@ -5729,13 +5729,13 @@
     </row>
     <row r="127" spans="1:26" ht="13.5" customHeight="1">
       <c r="A127" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="C127" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
@@ -5763,13 +5763,13 @@
     </row>
     <row r="128" spans="1:26" ht="13.5" customHeight="1">
       <c r="A128" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B128" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B128" s="8" t="s">
-        <v>177</v>
-      </c>
       <c r="C128" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
@@ -5797,13 +5797,13 @@
     </row>
     <row r="129" spans="1:26" ht="13.5" customHeight="1">
       <c r="A129" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B129" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="B129" s="11" t="s">
-        <v>179</v>
-      </c>
       <c r="C129" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
@@ -5831,13 +5831,13 @@
     </row>
     <row r="130" spans="1:26" ht="13.5" customHeight="1">
       <c r="A130" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B130" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B130" s="11" t="s">
-        <v>181</v>
-      </c>
       <c r="C130" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
@@ -5865,13 +5865,13 @@
     </row>
     <row r="131" spans="1:26" ht="13.5" customHeight="1">
       <c r="A131" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B131" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B131" s="11" t="s">
-        <v>183</v>
-      </c>
       <c r="C131" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
@@ -5899,13 +5899,13 @@
     </row>
     <row r="132" spans="1:26" ht="13.5" customHeight="1">
       <c r="A132" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B132" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="B132" s="12" t="s">
-        <v>185</v>
-      </c>
       <c r="C132" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
@@ -5933,13 +5933,13 @@
     </row>
     <row r="133" spans="1:26" ht="13.5" customHeight="1">
       <c r="A133" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B133" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="C133" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
@@ -5967,13 +5967,13 @@
     </row>
     <row r="134" spans="1:26" ht="13.5" customHeight="1">
       <c r="A134" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="C134" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
@@ -6001,13 +6001,13 @@
     </row>
     <row r="135" spans="1:26" ht="13.5" customHeight="1">
       <c r="A135" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B135" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="C135" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
@@ -6035,13 +6035,13 @@
     </row>
     <row r="136" spans="1:26" ht="13.5" customHeight="1">
       <c r="A136" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="C136" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
@@ -6069,13 +6069,13 @@
     </row>
     <row r="137" spans="1:26" ht="13.5" customHeight="1">
       <c r="A137" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B137" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="C137" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
@@ -6103,13 +6103,13 @@
     </row>
     <row r="138" spans="1:26" ht="13.5" customHeight="1">
       <c r="A138" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="C138" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
@@ -6137,13 +6137,13 @@
     </row>
     <row r="139" spans="1:26" ht="13.5" customHeight="1">
       <c r="A139" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="C139" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -6199,13 +6199,13 @@
     </row>
     <row r="141" spans="1:26" ht="13.5" customHeight="1">
       <c r="A141" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="C141" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
@@ -6233,13 +6233,13 @@
     </row>
     <row r="142" spans="1:26" ht="13.5" customHeight="1">
       <c r="A142" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B142" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="C142" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
@@ -6267,13 +6267,13 @@
     </row>
     <row r="143" spans="1:26" ht="13.5" customHeight="1">
       <c r="A143" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B143" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="C143" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
@@ -6301,13 +6301,13 @@
     </row>
     <row r="144" spans="1:26" ht="13.5" customHeight="1">
       <c r="A144" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B144" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="C144" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
@@ -6335,13 +6335,13 @@
     </row>
     <row r="145" spans="1:26" ht="13.5" customHeight="1">
       <c r="A145" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B145" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="C145" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
@@ -6369,13 +6369,13 @@
     </row>
     <row r="146" spans="1:26" ht="13.5" customHeight="1">
       <c r="A146" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
@@ -6403,13 +6403,13 @@
     </row>
     <row r="147" spans="1:26" ht="13.5" customHeight="1">
       <c r="A147" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -6437,13 +6437,13 @@
     </row>
     <row r="148" spans="1:26" ht="13.5" customHeight="1">
       <c r="A148" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="C148" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
@@ -6471,13 +6471,13 @@
     </row>
     <row r="149" spans="1:26" ht="13.5" customHeight="1">
       <c r="A149" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="C149" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
@@ -6505,13 +6505,13 @@
     </row>
     <row r="150" spans="1:26" ht="13.5" customHeight="1">
       <c r="A150" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="C150" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
@@ -6539,13 +6539,13 @@
     </row>
     <row r="151" spans="1:26" ht="13.5" customHeight="1">
       <c r="A151" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B151" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="B151" s="8" t="s">
-        <v>217</v>
-      </c>
       <c r="C151" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
@@ -6573,13 +6573,13 @@
     </row>
     <row r="152" spans="1:26" ht="13.5" customHeight="1">
       <c r="A152" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="C152" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
@@ -6607,13 +6607,13 @@
     </row>
     <row r="153" spans="1:26" ht="13.5" customHeight="1">
       <c r="A153" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="C153" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
@@ -6641,13 +6641,13 @@
     </row>
     <row r="154" spans="1:26" ht="13.5" customHeight="1">
       <c r="A154" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B154" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="C154" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
@@ -6675,13 +6675,13 @@
     </row>
     <row r="155" spans="1:26" ht="13.5" customHeight="1">
       <c r="A155" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B155" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="C155" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -6765,13 +6765,13 @@
     </row>
     <row r="158" spans="1:26" ht="13.5" customHeight="1">
       <c r="A158" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B158" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="B158" s="13" t="s">
-        <v>227</v>
-      </c>
       <c r="C158" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D158" s="8"/>
       <c r="E158" s="8"/>
@@ -6799,13 +6799,13 @@
     </row>
     <row r="159" spans="1:26" ht="13.5" customHeight="1">
       <c r="A159" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="B159" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="B159" s="15" t="s">
-        <v>229</v>
-      </c>
       <c r="C159" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D159" s="8"/>
       <c r="E159" s="8"/>
@@ -6833,7 +6833,7 @@
     </row>
     <row r="160" spans="1:26" ht="13.5" customHeight="1">
       <c r="A160" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B160" s="8" t="s">
         <v>8</v>
@@ -6867,13 +6867,13 @@
     </row>
     <row r="161" spans="1:26" ht="13.5" customHeight="1">
       <c r="A161" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B161" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="B161" s="8" t="s">
-        <v>232</v>
-      </c>
       <c r="C161" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
@@ -6901,13 +6901,13 @@
     </row>
     <row r="162" spans="1:26" ht="13.5" customHeight="1">
       <c r="A162" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B162" s="1" t="s">
-        <v>234</v>
-      </c>
       <c r="C162" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
@@ -6935,13 +6935,13 @@
     </row>
     <row r="163" spans="1:26" ht="13.5" customHeight="1">
       <c r="A163" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="B163" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="B163" s="8" t="s">
-        <v>236</v>
-      </c>
       <c r="C163" s="12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
@@ -6969,13 +6969,13 @@
     </row>
     <row r="164" spans="1:26" ht="13.5" customHeight="1">
       <c r="A164" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B164" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="B164" s="4" t="s">
-        <v>238</v>
-      </c>
       <c r="C164" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
@@ -7003,13 +7003,13 @@
     </row>
     <row r="165" spans="1:26" ht="13.5" customHeight="1">
       <c r="A165" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B165" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="C165" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
@@ -7037,13 +7037,13 @@
     </row>
     <row r="166" spans="1:26" ht="13.5" customHeight="1">
       <c r="A166" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
@@ -7071,13 +7071,13 @@
     </row>
     <row r="167" spans="1:26" ht="13.5" customHeight="1">
       <c r="A167" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B167" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="C167" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
@@ -7189,7 +7189,7 @@
     </row>
     <row r="171" spans="1:26" ht="13.5" customHeight="1">
       <c r="A171" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B171" s="13" t="s">
         <v>6</v>
@@ -7223,7 +7223,7 @@
     </row>
     <row r="172" spans="1:26" ht="13.5" customHeight="1">
       <c r="A172" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B172" s="5" t="s">
         <v>8</v>
@@ -7257,13 +7257,13 @@
     </row>
     <row r="173" spans="1:26" ht="13.5" customHeight="1">
       <c r="A173" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B173" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="B173" s="5" t="s">
-        <v>247</v>
-      </c>
       <c r="C173" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
@@ -7291,13 +7291,13 @@
     </row>
     <row r="174" spans="1:26" ht="13.5" customHeight="1">
       <c r="A174" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B174" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B174" s="8" t="s">
-        <v>249</v>
-      </c>
       <c r="C174" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
@@ -7325,13 +7325,13 @@
     </row>
     <row r="175" spans="1:26" ht="13.5" customHeight="1">
       <c r="A175" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B175" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B175" s="8" t="s">
-        <v>251</v>
-      </c>
       <c r="C175" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
@@ -7359,7 +7359,7 @@
     </row>
     <row r="176" spans="1:26" ht="13.5" customHeight="1">
       <c r="A176" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
@@ -7389,7 +7389,7 @@
     </row>
     <row r="177" spans="1:26" ht="13.5" customHeight="1">
       <c r="A177" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
@@ -7419,13 +7419,13 @@
     </row>
     <row r="178" spans="1:26" ht="13.5" customHeight="1">
       <c r="A178" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B178" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="B178" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="C178" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D178" s="1"/>
       <c r="E178" s="1"/>
@@ -7453,13 +7453,13 @@
     </row>
     <row r="179" spans="1:26" ht="13.5" customHeight="1">
       <c r="A179" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B179" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="B179" s="8" t="s">
-        <v>257</v>
-      </c>
       <c r="C179" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
@@ -7515,13 +7515,13 @@
     </row>
     <row r="181" spans="1:26" ht="13.5" customHeight="1">
       <c r="A181" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="B181" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="B181" s="8" t="s">
-        <v>259</v>
-      </c>
       <c r="C181" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D181" s="1"/>
       <c r="E181" s="1"/>
@@ -7550,10 +7550,10 @@
     <row r="182" spans="1:26" ht="13.5" customHeight="1">
       <c r="A182" s="14"/>
       <c r="B182" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D182" s="1"/>
       <c r="E182" s="1"/>
@@ -7581,13 +7581,13 @@
     </row>
     <row r="183" spans="1:26" ht="13.5" customHeight="1">
       <c r="A183" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B183" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="B183" s="17" t="s">
-        <v>262</v>
-      </c>
       <c r="C183" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D183" s="1"/>
       <c r="E183" s="1"/>
@@ -7615,13 +7615,13 @@
     </row>
     <row r="184" spans="1:26" ht="13.5" customHeight="1">
       <c r="A184" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="B184" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="B184" s="8" t="s">
-        <v>264</v>
-      </c>
       <c r="C184" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D184" s="1"/>
       <c r="E184" s="1"/>
@@ -7649,13 +7649,13 @@
     </row>
     <row r="185" spans="1:26" ht="13.5" customHeight="1">
       <c r="A185" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="B185" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="B185" s="8" t="s">
-        <v>266</v>
-      </c>
       <c r="C185" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D185" s="1"/>
       <c r="E185" s="1"/>
@@ -7683,13 +7683,13 @@
     </row>
     <row r="186" spans="1:26" ht="13.5" customHeight="1">
       <c r="A186" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="B186" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B186" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="C186" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D186" s="1"/>
       <c r="E186" s="1"/>
@@ -7717,13 +7717,13 @@
     </row>
     <row r="187" spans="1:26" ht="13.5" customHeight="1">
       <c r="A187" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="B187" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="B187" s="8" t="s">
-        <v>270</v>
-      </c>
       <c r="C187" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D187" s="1"/>
       <c r="E187" s="1"/>
@@ -7751,13 +7751,13 @@
     </row>
     <row r="188" spans="1:26" ht="13.5" customHeight="1">
       <c r="A188" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="B188" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="B188" s="8" t="s">
-        <v>229</v>
-      </c>
       <c r="C188" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>
@@ -7813,13 +7813,13 @@
     </row>
     <row r="190" spans="1:26" ht="13.5" customHeight="1">
       <c r="A190" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B190" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="B190" s="8" t="s">
-        <v>272</v>
-      </c>
       <c r="C190" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D190" s="1"/>
       <c r="E190" s="1"/>
@@ -7847,13 +7847,13 @@
     </row>
     <row r="191" spans="1:26" ht="13.5" customHeight="1">
       <c r="A191" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B191" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="B191" s="8" t="s">
-        <v>274</v>
-      </c>
       <c r="C191" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D191" s="1"/>
       <c r="E191" s="1"/>
@@ -7881,13 +7881,13 @@
     </row>
     <row r="192" spans="1:26" ht="13.5" customHeight="1">
       <c r="A192" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B192" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B192" s="8" t="s">
-        <v>276</v>
-      </c>
       <c r="C192" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D192" s="1"/>
       <c r="E192" s="1"/>
@@ -7915,13 +7915,13 @@
     </row>
     <row r="193" spans="1:26" ht="13.5" customHeight="1">
       <c r="A193" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B193" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="B193" s="8" t="s">
-        <v>278</v>
-      </c>
       <c r="C193" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D193" s="1"/>
       <c r="E193" s="1"/>
@@ -7949,13 +7949,13 @@
     </row>
     <row r="194" spans="1:26" ht="13.5" customHeight="1">
       <c r="A194" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B194" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B194" s="1" t="s">
-        <v>280</v>
-      </c>
       <c r="C194" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D194" s="1"/>
       <c r="E194" s="1"/>
@@ -7983,13 +7983,13 @@
     </row>
     <row r="195" spans="1:26" ht="13.5" customHeight="1">
       <c r="A195" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B195" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B195" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="C195" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D195" s="1"/>
       <c r="E195" s="1"/>
@@ -8017,13 +8017,13 @@
     </row>
     <row r="196" spans="1:26" ht="13.5" customHeight="1">
       <c r="A196" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B196" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B196" s="1" t="s">
-        <v>284</v>
-      </c>
       <c r="C196" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D196" s="1"/>
       <c r="E196" s="1"/>
@@ -8051,13 +8051,13 @@
     </row>
     <row r="197" spans="1:26" ht="13.5" customHeight="1">
       <c r="A197" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B197" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B197" s="1" t="s">
-        <v>286</v>
-      </c>
       <c r="C197" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D197" s="1"/>
       <c r="E197" s="1"/>
@@ -8085,13 +8085,13 @@
     </row>
     <row r="198" spans="1:26" ht="13.5" customHeight="1">
       <c r="A198" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B198" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B198" s="1" t="s">
-        <v>288</v>
-      </c>
       <c r="C198" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D198" s="1"/>
       <c r="E198" s="1"/>
@@ -8119,13 +8119,13 @@
     </row>
     <row r="199" spans="1:26" ht="13.5" customHeight="1">
       <c r="A199" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B199" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B199" s="1" t="s">
-        <v>290</v>
-      </c>
       <c r="C199" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D199" s="1"/>
       <c r="E199" s="1"/>
@@ -8153,13 +8153,13 @@
     </row>
     <row r="200" spans="1:26" ht="13.5" customHeight="1">
       <c r="A200" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B200" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="B200" s="1" t="s">
-        <v>292</v>
-      </c>
       <c r="C200" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D200" s="1"/>
       <c r="E200" s="1"/>
@@ -8187,13 +8187,13 @@
     </row>
     <row r="201" spans="1:26" ht="13.5" customHeight="1">
       <c r="A201" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B201" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B201" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="C201" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D201" s="1"/>
       <c r="E201" s="1"/>
@@ -8221,13 +8221,13 @@
     </row>
     <row r="202" spans="1:26" ht="13.5" customHeight="1">
       <c r="A202" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B202" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B202" s="1" t="s">
-        <v>296</v>
-      </c>
       <c r="C202" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D202" s="1"/>
       <c r="E202" s="1"/>
@@ -8255,13 +8255,13 @@
     </row>
     <row r="203" spans="1:26" ht="13.5" customHeight="1">
       <c r="A203" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B203" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B203" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="C203" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D203" s="1"/>
       <c r="E203" s="1"/>
@@ -8289,13 +8289,13 @@
     </row>
     <row r="204" spans="1:26" ht="13.5" customHeight="1">
       <c r="A204" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B204" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="B204" s="1" t="s">
-        <v>300</v>
-      </c>
       <c r="C204" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D204" s="1"/>
       <c r="E204" s="1"/>
@@ -8323,13 +8323,13 @@
     </row>
     <row r="205" spans="1:26" ht="13.5" customHeight="1">
       <c r="A205" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B205" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="B205" s="10" t="s">
-        <v>302</v>
-      </c>
       <c r="C205" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D205" s="1"/>
       <c r="E205" s="1"/>
@@ -8357,13 +8357,13 @@
     </row>
     <row r="206" spans="1:26" ht="13.5" customHeight="1">
       <c r="A206" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B206" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B206" s="1" t="s">
-        <v>304</v>
-      </c>
       <c r="C206" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>
@@ -8391,13 +8391,13 @@
     </row>
     <row r="207" spans="1:26" ht="13.5" customHeight="1">
       <c r="A207" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B207" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B207" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="C207" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D207" s="1"/>
       <c r="E207" s="1"/>
@@ -8425,13 +8425,13 @@
     </row>
     <row r="208" spans="1:26" ht="13.5" customHeight="1">
       <c r="A208" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D208" s="1"/>
       <c r="E208" s="1"/>
@@ -8459,13 +8459,13 @@
     </row>
     <row r="209" spans="1:26" ht="13.5" customHeight="1">
       <c r="A209" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B209" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C209" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D209" s="1"/>
       <c r="E209" s="1"/>
@@ -8493,13 +8493,13 @@
     </row>
     <row r="210" spans="1:26" ht="13.5" customHeight="1">
       <c r="A210" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D210" s="1"/>
       <c r="E210" s="1"/>
@@ -8527,13 +8527,13 @@
     </row>
     <row r="211" spans="1:26" ht="13.5" customHeight="1">
       <c r="A211" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B211" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="C211" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D211" s="1"/>
       <c r="E211" s="1"/>
@@ -8561,13 +8561,13 @@
     </row>
     <row r="212" spans="1:26" ht="13.5" customHeight="1">
       <c r="A212" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B212" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B212" s="1" t="s">
-        <v>313</v>
-      </c>
       <c r="C212" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D212" s="1"/>
       <c r="E212" s="1"/>
@@ -8595,13 +8595,13 @@
     </row>
     <row r="213" spans="1:26" ht="13.5" customHeight="1">
       <c r="A213" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B213" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="B213" s="1" t="s">
-        <v>315</v>
-      </c>
       <c r="C213" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D213" s="1"/>
       <c r="E213" s="1"/>
@@ -8629,13 +8629,13 @@
     </row>
     <row r="214" spans="1:26" ht="13.5" customHeight="1">
       <c r="A214" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D214" s="1"/>
       <c r="E214" s="1"/>
@@ -8663,13 +8663,13 @@
     </row>
     <row r="215" spans="1:26" ht="13.5" customHeight="1">
       <c r="A215" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B215" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B215" s="1" t="s">
-        <v>318</v>
-      </c>
       <c r="C215" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D215" s="1"/>
       <c r="E215" s="1"/>
@@ -8697,13 +8697,13 @@
     </row>
     <row r="216" spans="1:26" ht="13.5" customHeight="1">
       <c r="A216" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B216" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="B216" s="11" t="s">
-        <v>320</v>
-      </c>
       <c r="C216" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D216" s="1"/>
       <c r="E216" s="1"/>
@@ -8731,13 +8731,13 @@
     </row>
     <row r="217" spans="1:26" ht="13.5" customHeight="1">
       <c r="A217" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B217" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="B217" s="11" t="s">
-        <v>322</v>
-      </c>
       <c r="C217" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D217" s="1"/>
       <c r="E217" s="1"/>
@@ -8765,13 +8765,13 @@
     </row>
     <row r="218" spans="1:26" ht="13.5" customHeight="1">
       <c r="A218" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B218" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B218" s="1" t="s">
-        <v>324</v>
-      </c>
       <c r="C218" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D218" s="1"/>
       <c r="E218" s="1"/>
@@ -8799,13 +8799,13 @@
     </row>
     <row r="219" spans="1:26" ht="13.5" customHeight="1">
       <c r="A219" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B219" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="B219" s="12" t="s">
-        <v>326</v>
-      </c>
       <c r="C219" s="12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D219" s="1"/>
       <c r="E219" s="1"/>
@@ -8833,13 +8833,13 @@
     </row>
     <row r="220" spans="1:26" ht="13.5" customHeight="1">
       <c r="A220" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B220" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="B220" s="11" t="s">
-        <v>328</v>
-      </c>
       <c r="C220" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D220" s="1"/>
       <c r="E220" s="1"/>
@@ -8867,13 +8867,13 @@
     </row>
     <row r="221" spans="1:26" ht="13.5" customHeight="1">
       <c r="A221" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B221" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="B221" s="18" t="s">
-        <v>330</v>
-      </c>
       <c r="C221" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D221" s="1"/>
       <c r="E221" s="1"/>
@@ -8901,13 +8901,13 @@
     </row>
     <row r="222" spans="1:26" ht="13.5" customHeight="1">
       <c r="A222" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D222" s="1"/>
       <c r="E222" s="1"/>
@@ -8935,13 +8935,13 @@
     </row>
     <row r="223" spans="1:26" ht="13.5" customHeight="1">
       <c r="A223" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B223" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="B223" s="11" t="s">
-        <v>333</v>
-      </c>
       <c r="C223" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D223" s="1"/>
       <c r="E223" s="1"/>
@@ -8969,13 +8969,13 @@
     </row>
     <row r="224" spans="1:26" ht="13.5" customHeight="1">
       <c r="A224" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B224" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B224" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="C224" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D224" s="1"/>
       <c r="E224" s="1"/>
@@ -9003,13 +9003,13 @@
     </row>
     <row r="225" spans="1:26" ht="13.5" customHeight="1">
       <c r="A225" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B225" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="B225" s="12" t="s">
-        <v>337</v>
-      </c>
       <c r="C225" s="12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D225" s="1"/>
       <c r="E225" s="1"/>
@@ -9037,13 +9037,13 @@
     </row>
     <row r="226" spans="1:26" ht="13.5" customHeight="1">
       <c r="A226" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D226" s="1"/>
       <c r="E226" s="1"/>
@@ -9071,13 +9071,13 @@
     </row>
     <row r="227" spans="1:26" ht="13.5" customHeight="1">
       <c r="A227" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B227" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="B227" s="12" t="s">
-        <v>339</v>
-      </c>
       <c r="C227" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D227" s="1"/>
       <c r="E227" s="1"/>
@@ -9105,13 +9105,13 @@
     </row>
     <row r="228" spans="1:26" ht="13.5" customHeight="1">
       <c r="A228" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B228" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C228" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D228" s="1"/>
       <c r="E228" s="1"/>
@@ -9139,13 +9139,13 @@
     </row>
     <row r="229" spans="1:26" ht="13.5" customHeight="1">
       <c r="A229" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B229" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="B229" s="12" t="s">
-        <v>341</v>
-      </c>
       <c r="C229" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D229" s="1"/>
       <c r="E229" s="1"/>
@@ -30831,7 +30831,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -30927,7 +30927,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -30959,7 +30959,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -31023,7 +31023,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -31083,7 +31083,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -31115,7 +31115,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -31144,7 +31144,7 @@
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B12" s="22">
         <v>784512369</v>
@@ -31179,7 +31179,7 @@
         <v>30</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -31271,7 +31271,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -31303,7 +31303,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -31335,7 +31335,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -31427,7 +31427,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -31459,7 +31459,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -31491,7 +31491,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
@@ -31583,7 +31583,7 @@
         <v>31</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
@@ -31615,7 +31615,7 @@
         <v>32</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
@@ -31644,10 +31644,10 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>348</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>349</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -31679,7 +31679,7 @@
         <v>35</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
@@ -31768,10 +31768,10 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -31800,10 +31800,10 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -31832,7 +31832,7 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B34" s="22">
         <v>784512369</v>
@@ -31864,10 +31864,10 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="B35" s="19" t="s">
         <v>353</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>354</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -31956,10 +31956,10 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="19"/>
@@ -31988,10 +31988,10 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -32020,10 +32020,10 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C40" s="19"/>
       <c r="D40" s="19"/>
@@ -32112,10 +32112,10 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="B43" s="19" t="s">
         <v>358</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>359</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
@@ -32144,10 +32144,10 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="B44" s="19" t="s">
         <v>360</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>361</v>
       </c>
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
@@ -32208,10 +32208,10 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>362</v>
-      </c>
-      <c r="B46" s="19" t="s">
-        <v>363</v>
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
@@ -32268,10 +32268,10 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C48" s="19"/>
       <c r="D48" s="19"/>
@@ -32300,10 +32300,10 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
@@ -32332,7 +32332,7 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B50" s="22">
         <v>784512369</v>
@@ -32364,10 +32364,10 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>366</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>367</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
@@ -32456,10 +32456,10 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1">
       <c r="A54" s="19" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C54" s="19"/>
       <c r="D54" s="19"/>
@@ -32488,10 +32488,10 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1">
       <c r="A55" s="19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
@@ -32520,10 +32520,10 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1">
       <c r="A56" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="B56" s="19" t="s">
         <v>370</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>371</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
@@ -32612,10 +32612,10 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1">
       <c r="A59" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="B59" s="19" t="s">
         <v>372</v>
-      </c>
-      <c r="B59" s="19" t="s">
-        <v>373</v>
       </c>
       <c r="C59" s="19"/>
       <c r="D59" s="19"/>
@@ -32644,10 +32644,10 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1">
       <c r="A60" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="B60" s="23" t="s">
         <v>374</v>
-      </c>
-      <c r="B60" s="23" t="s">
-        <v>375</v>
       </c>
       <c r="C60" s="19"/>
       <c r="D60" s="19"/>
@@ -32676,10 +32676,10 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1">
       <c r="A61" s="19" t="s">
+        <v>375</v>
+      </c>
+      <c r="B61" s="23" t="s">
         <v>376</v>
-      </c>
-      <c r="B61" s="23" t="s">
-        <v>377</v>
       </c>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
@@ -32708,10 +32708,10 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1">
       <c r="A62" s="19" t="s">
+        <v>377</v>
+      </c>
+      <c r="B62" s="23" t="s">
         <v>378</v>
-      </c>
-      <c r="B62" s="23" t="s">
-        <v>379</v>
       </c>
       <c r="C62" s="19"/>
       <c r="D62" s="19"/>
@@ -32740,10 +32740,10 @@
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1">
       <c r="A63" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="B63" s="23" t="s">
         <v>380</v>
-      </c>
-      <c r="B63" s="23" t="s">
-        <v>381</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
@@ -32772,10 +32772,10 @@
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1">
       <c r="A64" s="19" t="s">
+        <v>381</v>
+      </c>
+      <c r="B64" s="23" t="s">
         <v>382</v>
-      </c>
-      <c r="B64" s="23" t="s">
-        <v>383</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
@@ -32804,10 +32804,10 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1">
       <c r="A65" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="B65" s="23" t="s">
         <v>384</v>
-      </c>
-      <c r="B65" s="23" t="s">
-        <v>385</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
@@ -32836,10 +32836,10 @@
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1">
       <c r="A66" s="19" t="s">
+        <v>385</v>
+      </c>
+      <c r="B66" s="23" t="s">
         <v>386</v>
-      </c>
-      <c r="B66" s="23" t="s">
-        <v>387</v>
       </c>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
@@ -32868,10 +32868,10 @@
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1">
       <c r="A67" s="19" t="s">
+        <v>387</v>
+      </c>
+      <c r="B67" s="23" t="s">
         <v>388</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>389</v>
       </c>
       <c r="C67" s="19"/>
       <c r="D67" s="19"/>
@@ -32900,10 +32900,10 @@
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1">
       <c r="A68" s="19" t="s">
+        <v>389</v>
+      </c>
+      <c r="B68" s="23" t="s">
         <v>390</v>
-      </c>
-      <c r="B68" s="23" t="s">
-        <v>391</v>
       </c>
       <c r="C68" s="19"/>
       <c r="D68" s="19"/>
@@ -32932,10 +32932,10 @@
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1">
       <c r="A69" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="B69" s="23" t="s">
         <v>392</v>
-      </c>
-      <c r="B69" s="23" t="s">
-        <v>393</v>
       </c>
       <c r="C69" s="19"/>
       <c r="D69" s="19"/>
@@ -32964,10 +32964,10 @@
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1">
       <c r="A70" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="B70" s="23" t="s">
         <v>394</v>
-      </c>
-      <c r="B70" s="23" t="s">
-        <v>395</v>
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="19"/>
@@ -32996,10 +32996,10 @@
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1">
       <c r="A71" s="19" t="s">
+        <v>395</v>
+      </c>
+      <c r="B71" s="23" t="s">
         <v>396</v>
-      </c>
-      <c r="B71" s="23" t="s">
-        <v>397</v>
       </c>
       <c r="C71" s="19"/>
       <c r="D71" s="19"/>
@@ -33028,10 +33028,10 @@
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1">
       <c r="A72" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="B72" s="23" t="s">
         <v>398</v>
-      </c>
-      <c r="B72" s="23" t="s">
-        <v>399</v>
       </c>
       <c r="C72" s="19"/>
       <c r="D72" s="19"/>

</xml_diff>

<commit_message>
- URGENCY REQUEST UPDATE - Extent Report Update
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -1552,7 +1552,7 @@
     <t>Approved;Dr Sam Entwistle;VM03Location;Follow-up</t>
   </si>
   <si>
-    <t>Urgent/Same day - Fee: NZ$40.01 (Incl. GST);Next Day - Fee: NZ$40.04 (Incl. GST);48 Hours - Fee: NZ$40.07 (Incl. GST);72 Hours - Fee: NZ$50.10 (Incl. GST)</t>
+    <t>Urgent/Same day - Fee: NZ$10.00 (Incl. GST);Next Day - Fee: NZ$20.00 (Incl. GST);48 Hours - Fee: NZ$30.00 (Incl. GST);72 Hours - Fee: NZ$40.00 (Incl. GST)</t>
   </si>
 </sst>
 </file>
@@ -1946,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B50" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="C50" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Beating Module Add for sanity path
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -11,14 +11,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mjTNPQIgH1fu8Aox66rsWlR1raURA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgyDUSv1981ZLFbux8uP7gz+xB2wg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="883">
   <si>
     <t>KEY</t>
   </si>
@@ -2285,7 +2285,7 @@
     <t>HEIGHT_CARD_SURVEY_MY_ENTRIES_DATA</t>
   </si>
   <si>
-    <t>6;TestBMI</t>
+    <t>5;TestBMI</t>
   </si>
   <si>
     <t>HDL_MY_ENTRIES_DATA</t>
@@ -2324,7 +2324,7 @@
     <t>WEIGHT_CARD_SURVEY_MY_ENTRIES_DATA</t>
   </si>
   <si>
-    <t>50;TestWeight</t>
+    <t>50;TestBMI</t>
   </si>
   <si>
     <t>EDIT_WEIGHT_CARD_MY_ENTRIES_DATA</t>
@@ -2658,6 +2658,15 @@
   </si>
   <si>
     <t>Weight;50;TestBMI</t>
+  </si>
+  <si>
+    <t>EMAIL FOR BEATING_THE_BLUES</t>
+  </si>
+  <si>
+    <t>tk1@mmh-demo.com</t>
+  </si>
+  <si>
+    <t>PASSWORD FOR BEATING_THE_BLUES</t>
   </si>
 </sst>
 </file>
@@ -2744,12 +2753,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="9.0"/>
-      <color rgb="FF297BDE"/>
-      <name val="&quot;JetBrains Mono&quot;"/>
-    </font>
-    <font>
       <u/>
       <sz val="11.0"/>
       <color rgb="FF0563C1"/>
@@ -2770,6 +2773,11 @@
       <sz val="9.0"/>
       <color theme="1"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2812,7 +2820,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2872,16 +2880,16 @@
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -2896,14 +2904,20 @@
     <xf borderId="2" fillId="2" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -25537,75 +25551,57 @@
       <c r="C39" s="22"/>
     </row>
     <row r="40">
-      <c r="A40" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>11</v>
-      </c>
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
     </row>
     <row r="41">
-      <c r="A41" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>13</v>
-      </c>
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
     </row>
     <row r="42">
-      <c r="A42" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>15</v>
-      </c>
+      <c r="A42" s="22"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
     </row>
     <row r="43">
-      <c r="A43" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>17</v>
-      </c>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
     </row>
     <row r="44">
       <c r="A44" s="22" t="s">
-        <v>40</v>
+        <v>531</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>41</v>
+        <v>226</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>41</v>
+        <v>226</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>43</v>
+        <v>532</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>533</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
+      <c r="A46" s="22" t="s">
+        <v>534</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>535</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="22"/>
@@ -25614,89 +25610,89 @@
     </row>
     <row r="48">
       <c r="A48" s="22" t="s">
-        <v>18</v>
+        <v>536</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>19</v>
+        <v>537</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>19</v>
+        <v>537</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="22" t="s">
-        <v>20</v>
+        <v>538</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>21</v>
+        <v>539</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>21</v>
+        <v>539</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>15</v>
-      </c>
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="24"/>
     </row>
     <row r="51">
       <c r="A51" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B51" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51" s="22" t="s">
-        <v>41</v>
+        <v>540</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>541</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="22"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
+      <c r="A52" s="22" t="s">
+        <v>542</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>543</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>543</v>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" s="22"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
+      <c r="A53" s="22" t="s">
+        <v>544</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>545</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>545</v>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="B54" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>226</v>
-      </c>
+      <c r="A54" s="22"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
     </row>
     <row r="55">
       <c r="A55" s="22" t="s">
-        <v>532</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>533</v>
-      </c>
-      <c r="C55" s="26" t="s">
-        <v>533</v>
+        <v>546</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>547</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="22" t="s">
-        <v>534</v>
+        <v>548</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>535</v>
+        <v>549</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>535</v>
+        <v>549</v>
       </c>
     </row>
     <row r="57">
@@ -25706,180 +25702,186 @@
     </row>
     <row r="58">
       <c r="A58" s="22" t="s">
-        <v>536</v>
+        <v>550</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>537</v>
+        <v>551</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>537</v>
+        <v>551</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="22" t="s">
-        <v>538</v>
-      </c>
-      <c r="B59" s="22" t="s">
-        <v>539</v>
-      </c>
-      <c r="C59" s="22" t="s">
-        <v>539</v>
-      </c>
+      <c r="A59" s="22"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
     </row>
     <row r="60">
       <c r="A60" s="22"/>
       <c r="B60" s="22"/>
-      <c r="C60" s="24"/>
+      <c r="C60" s="22"/>
     </row>
     <row r="61">
       <c r="A61" s="22" t="s">
-        <v>540</v>
-      </c>
-      <c r="B61" s="24" t="s">
-        <v>541</v>
-      </c>
-      <c r="C61" s="25" t="s">
-        <v>541</v>
+        <v>552</v>
+      </c>
+      <c r="B61" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="22" t="s">
-        <v>542</v>
+        <v>553</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>543</v>
+        <v>9</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>543</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="22" t="s">
-        <v>544</v>
-      </c>
-      <c r="B63" s="22" t="s">
-        <v>545</v>
-      </c>
-      <c r="C63" s="22" t="s">
-        <v>545</v>
-      </c>
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
     </row>
     <row r="64">
-      <c r="A64" s="22"/>
-      <c r="B64" s="22"/>
-      <c r="C64" s="22"/>
+      <c r="A64" s="27" t="s">
+        <v>554</v>
+      </c>
+      <c r="B64" s="22" t="s">
+        <v>555</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" s="22" t="s">
-        <v>546</v>
-      </c>
-      <c r="B65" s="22" t="s">
-        <v>547</v>
-      </c>
-      <c r="C65" s="22" t="s">
-        <v>547</v>
-      </c>
+      <c r="A65" s="22"/>
+      <c r="B65" s="22"/>
+      <c r="C65" s="22"/>
     </row>
     <row r="66">
       <c r="A66" s="22" t="s">
-        <v>548</v>
+        <v>556</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>549</v>
+        <v>48</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>549</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="22"/>
-      <c r="B67" s="22"/>
-      <c r="C67" s="22"/>
+      <c r="A67" s="22" t="s">
+        <v>557</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="68">
-      <c r="A68" s="22" t="s">
-        <v>550</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>551</v>
-      </c>
-      <c r="C68" s="22" t="s">
-        <v>551</v>
-      </c>
+      <c r="A68" s="22"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
     </row>
     <row r="69">
-      <c r="A69" s="22"/>
-      <c r="B69" s="22"/>
-      <c r="C69" s="22"/>
+      <c r="A69" s="22" t="s">
+        <v>558</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="70">
-      <c r="A70" s="22"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
+      <c r="A70" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="71">
-      <c r="A71" s="22" t="s">
-        <v>552</v>
+      <c r="A71" s="27" t="s">
+        <v>560</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>48</v>
+        <v>561</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>48</v>
+        <v>561</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="22" t="s">
-        <v>553</v>
+      <c r="A72" s="27" t="s">
+        <v>562</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>9</v>
+        <v>563</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>9</v>
+        <v>563</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="22"/>
-      <c r="B73" s="22"/>
-      <c r="C73" s="22"/>
+      <c r="A73" s="27" t="s">
+        <v>564</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>565</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="74">
-      <c r="A74" s="27" t="s">
-        <v>554</v>
-      </c>
-      <c r="B74" s="22" t="s">
-        <v>555</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>555</v>
-      </c>
+      <c r="A74" s="22"/>
+      <c r="B74" s="22"/>
+      <c r="C74" s="22"/>
     </row>
     <row r="75">
-      <c r="A75" s="22"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="22"/>
+      <c r="A75" s="27" t="s">
+        <v>566</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>567</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>567</v>
+      </c>
     </row>
     <row r="76">
-      <c r="A76" s="22" t="s">
-        <v>556</v>
+      <c r="A76" s="27" t="s">
+        <v>568</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>48</v>
+        <v>569</v>
       </c>
       <c r="C76" s="22" t="s">
-        <v>48</v>
+        <v>569</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="22" t="s">
-        <v>557</v>
+      <c r="A77" s="27" t="s">
+        <v>570</v>
       </c>
       <c r="B77" s="22" t="s">
-        <v>9</v>
+        <v>571</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>9</v>
+        <v>571</v>
       </c>
     </row>
     <row r="78">
@@ -25888,184 +25890,172 @@
       <c r="C78" s="22"/>
     </row>
     <row r="79">
-      <c r="A79" s="22" t="s">
-        <v>558</v>
-      </c>
-      <c r="B79" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C79" s="22" t="s">
-        <v>9</v>
-      </c>
+      <c r="A79" s="22"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
     </row>
     <row r="80">
-      <c r="A80" s="22" t="s">
-        <v>559</v>
+      <c r="A80" s="27" t="s">
+        <v>572</v>
       </c>
       <c r="B80" s="22" t="s">
-        <v>48</v>
+        <v>573</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>48</v>
+        <v>573</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="27" t="s">
-        <v>560</v>
+        <v>574</v>
       </c>
       <c r="B81" s="22" t="s">
-        <v>561</v>
+        <v>575</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>561</v>
+        <v>575</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="27" t="s">
-        <v>562</v>
+        <v>576</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>563</v>
+        <v>577</v>
       </c>
       <c r="C82" s="22" t="s">
-        <v>563</v>
+        <v>577</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="27" t="s">
-        <v>564</v>
+        <v>578</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>565</v>
+        <v>579</v>
       </c>
       <c r="C83" s="22" t="s">
-        <v>565</v>
+        <v>579</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="22"/>
-      <c r="B84" s="22"/>
-      <c r="C84" s="22"/>
+      <c r="A84" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>581</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="85">
-      <c r="A85" s="27" t="s">
-        <v>566</v>
+      <c r="A85" s="22" t="s">
+        <v>582</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>567</v>
+        <v>583</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>567</v>
+        <v>583</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="27" t="s">
-        <v>568</v>
+      <c r="A86" s="22" t="s">
+        <v>584</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>569</v>
+        <v>585</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>569</v>
+        <v>585</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="27" t="s">
-        <v>570</v>
-      </c>
-      <c r="B87" s="22" t="s">
-        <v>571</v>
-      </c>
-      <c r="C87" s="22" t="s">
-        <v>571</v>
-      </c>
+      <c r="A87" s="22"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="22"/>
     </row>
     <row r="88">
-      <c r="A88" s="22"/>
-      <c r="B88" s="22"/>
-      <c r="C88" s="22"/>
+      <c r="A88" s="22" t="s">
+        <v>586</v>
+      </c>
+      <c r="B88" s="22" t="s">
+        <v>587</v>
+      </c>
+      <c r="C88" s="22" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="89">
-      <c r="A89" s="22"/>
-      <c r="B89" s="22"/>
-      <c r="C89" s="22"/>
+      <c r="A89" s="22" t="s">
+        <v>588</v>
+      </c>
+      <c r="B89" s="22" t="s">
+        <v>589</v>
+      </c>
+      <c r="C89" s="22" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="90">
-      <c r="A90" s="27" t="s">
-        <v>572</v>
+      <c r="A90" s="22" t="s">
+        <v>590</v>
       </c>
       <c r="B90" s="22" t="s">
-        <v>573</v>
+        <v>591</v>
       </c>
       <c r="C90" s="22" t="s">
-        <v>573</v>
+        <v>591</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="27" t="s">
-        <v>574</v>
-      </c>
-      <c r="B91" s="22" t="s">
-        <v>575</v>
-      </c>
-      <c r="C91" s="22" t="s">
-        <v>575</v>
-      </c>
+      <c r="A91" s="22"/>
+      <c r="B91" s="22"/>
+      <c r="C91" s="22"/>
     </row>
     <row r="92">
-      <c r="A92" s="27" t="s">
-        <v>576</v>
+      <c r="A92" s="22" t="s">
+        <v>592</v>
       </c>
       <c r="B92" s="22" t="s">
-        <v>577</v>
+        <v>593</v>
       </c>
       <c r="C92" s="22" t="s">
-        <v>577</v>
+        <v>593</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="27" t="s">
-        <v>578</v>
+      <c r="A93" s="22" t="s">
+        <v>594</v>
       </c>
       <c r="B93" s="22" t="s">
-        <v>579</v>
+        <v>595</v>
       </c>
       <c r="C93" s="22" t="s">
-        <v>579</v>
+        <v>595</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="22" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="B94" s="22" t="s">
-        <v>581</v>
+        <v>597</v>
       </c>
       <c r="C94" s="22" t="s">
-        <v>581</v>
+        <v>597</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="22" t="s">
-        <v>582</v>
-      </c>
-      <c r="B95" s="22" t="s">
-        <v>583</v>
-      </c>
-      <c r="C95" s="22" t="s">
-        <v>583</v>
-      </c>
+      <c r="A95" s="22"/>
+      <c r="B95" s="22"/>
+      <c r="C95" s="22"/>
     </row>
     <row r="96">
-      <c r="A96" s="22" t="s">
-        <v>584</v>
-      </c>
-      <c r="B96" s="22" t="s">
-        <v>585</v>
-      </c>
-      <c r="C96" s="22" t="s">
-        <v>585</v>
-      </c>
+      <c r="A96" s="22"/>
+      <c r="B96" s="22"/>
+      <c r="C96" s="22"/>
     </row>
     <row r="97">
       <c r="A97" s="22"/>
@@ -26073,159 +26063,151 @@
       <c r="C97" s="22"/>
     </row>
     <row r="98">
-      <c r="A98" s="22" t="s">
-        <v>586</v>
-      </c>
-      <c r="B98" s="22" t="s">
-        <v>587</v>
-      </c>
-      <c r="C98" s="22" t="s">
-        <v>587</v>
-      </c>
+      <c r="A98" s="22"/>
+      <c r="B98" s="22"/>
+      <c r="C98" s="22"/>
     </row>
     <row r="99">
-      <c r="A99" s="22" t="s">
-        <v>588</v>
-      </c>
-      <c r="B99" s="22" t="s">
-        <v>589</v>
-      </c>
-      <c r="C99" s="22" t="s">
-        <v>589</v>
-      </c>
+      <c r="A99" s="22"/>
+      <c r="B99" s="22"/>
+      <c r="C99" s="22"/>
     </row>
     <row r="100">
-      <c r="A100" s="22" t="s">
-        <v>590</v>
-      </c>
-      <c r="B100" s="22" t="s">
-        <v>591</v>
-      </c>
-      <c r="C100" s="22" t="s">
-        <v>591</v>
-      </c>
+      <c r="A100" s="22"/>
+      <c r="B100" s="22"/>
+      <c r="C100" s="22"/>
     </row>
     <row r="101">
-      <c r="A101" s="22"/>
-      <c r="B101" s="22"/>
-      <c r="C101" s="22"/>
+      <c r="A101" s="22" t="s">
+        <v>598</v>
+      </c>
+      <c r="B101" s="22" t="s">
+        <v>599</v>
+      </c>
+      <c r="C101" s="22" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="102">
-      <c r="A102" s="22" t="s">
-        <v>592</v>
-      </c>
-      <c r="B102" s="22" t="s">
-        <v>593</v>
-      </c>
-      <c r="C102" s="22" t="s">
-        <v>593</v>
-      </c>
+      <c r="A102" s="22"/>
+      <c r="B102" s="22"/>
+      <c r="C102" s="22"/>
     </row>
     <row r="103">
-      <c r="A103" s="22" t="s">
-        <v>594</v>
-      </c>
-      <c r="B103" s="22" t="s">
-        <v>595</v>
-      </c>
-      <c r="C103" s="22" t="s">
-        <v>595</v>
-      </c>
+      <c r="A103" s="22"/>
+      <c r="B103" s="22"/>
+      <c r="C103" s="22"/>
     </row>
     <row r="104">
-      <c r="A104" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="B104" s="22" t="s">
-        <v>597</v>
-      </c>
-      <c r="C104" s="22" t="s">
-        <v>597</v>
+      <c r="A104" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B104" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C104" s="23" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="22"/>
-      <c r="B105" s="22"/>
-      <c r="C105" s="22"/>
+      <c r="A105" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B105" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C105" s="23" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="106">
-      <c r="A106" s="22"/>
-      <c r="B106" s="22"/>
-      <c r="C106" s="22"/>
+      <c r="A106" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B106" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C106" s="23" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="107">
-      <c r="A107" s="22"/>
-      <c r="B107" s="22"/>
-      <c r="C107" s="22"/>
+      <c r="A107" s="23"/>
+      <c r="B107" s="23"/>
+      <c r="C107" s="23"/>
     </row>
     <row r="108">
-      <c r="A108" s="22"/>
-      <c r="B108" s="22"/>
-      <c r="C108" s="22"/>
+      <c r="A108" s="23"/>
+      <c r="B108" s="23"/>
+      <c r="C108" s="23"/>
     </row>
     <row r="109">
-      <c r="A109" s="22"/>
-      <c r="B109" s="22"/>
-      <c r="C109" s="22"/>
+      <c r="A109" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B109" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C109" s="23" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="110">
-      <c r="A110" s="22"/>
-      <c r="B110" s="22"/>
-      <c r="C110" s="22"/>
+      <c r="A110" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B110" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C110" s="23" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="111">
-      <c r="A111" s="22" t="s">
-        <v>598</v>
-      </c>
-      <c r="B111" s="22" t="s">
-        <v>599</v>
-      </c>
-      <c r="C111" s="22" t="s">
-        <v>599</v>
-      </c>
+      <c r="A111" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B111" s="23"/>
+      <c r="C111" s="23"/>
     </row>
     <row r="112">
-      <c r="A112" s="22"/>
-      <c r="B112" s="22"/>
-      <c r="C112" s="22"/>
+      <c r="A112" s="23"/>
+      <c r="B112" s="23"/>
+      <c r="C112" s="23"/>
     </row>
     <row r="113">
-      <c r="A113" s="22"/>
-      <c r="B113" s="22"/>
-      <c r="C113" s="22"/>
+      <c r="A113" s="23"/>
+      <c r="B113" s="23"/>
+      <c r="C113" s="23"/>
     </row>
     <row r="114">
       <c r="A114" s="23" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B114" s="23" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C114" s="23" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="23" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B115" s="23" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C115" s="23" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B116" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C116" s="23" t="s">
-        <v>55</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B116" s="23"/>
+      <c r="C116" s="23"/>
     </row>
     <row r="117">
       <c r="A117" s="23"/>
@@ -26239,110 +26221,82 @@
     </row>
     <row r="119">
       <c r="A119" s="23" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B119" s="23" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C119" s="23" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="23" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B120" s="23" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C120" s="23" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="23" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B121" s="23"/>
       <c r="C121" s="23"/>
     </row>
     <row r="122">
-      <c r="A122" s="23"/>
-      <c r="B122" s="23"/>
-      <c r="C122" s="23"/>
+      <c r="A122" s="22"/>
+      <c r="B122" s="22"/>
+      <c r="C122" s="22"/>
     </row>
     <row r="123">
-      <c r="A123" s="23"/>
-      <c r="B123" s="23"/>
-      <c r="C123" s="23"/>
+      <c r="A123" s="22"/>
+      <c r="B123" s="22"/>
+      <c r="C123" s="22"/>
     </row>
     <row r="124">
-      <c r="A124" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B124" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C124" s="23" t="s">
-        <v>62</v>
-      </c>
+      <c r="A124" s="22"/>
+      <c r="B124" s="22"/>
+      <c r="C124" s="22"/>
     </row>
     <row r="125">
-      <c r="A125" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B125" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C125" s="23" t="s">
-        <v>64</v>
-      </c>
+      <c r="A125" s="22"/>
+      <c r="B125" s="22"/>
+      <c r="C125" s="22"/>
     </row>
     <row r="126">
-      <c r="A126" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B126" s="23"/>
-      <c r="C126" s="23"/>
+      <c r="A126" s="22"/>
+      <c r="B126" s="22"/>
+      <c r="C126" s="22"/>
     </row>
     <row r="127">
-      <c r="A127" s="23"/>
-      <c r="B127" s="23"/>
-      <c r="C127" s="23"/>
+      <c r="A127" s="22"/>
+      <c r="B127" s="22"/>
+      <c r="C127" s="22"/>
     </row>
     <row r="128">
-      <c r="A128" s="23"/>
-      <c r="B128" s="23"/>
-      <c r="C128" s="23"/>
+      <c r="A128" s="22"/>
+      <c r="B128" s="22"/>
+      <c r="C128" s="22"/>
     </row>
     <row r="129">
-      <c r="A129" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B129" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C129" s="23" t="s">
-        <v>67</v>
-      </c>
+      <c r="A129" s="22"/>
+      <c r="B129" s="22"/>
+      <c r="C129" s="22"/>
     </row>
     <row r="130">
-      <c r="A130" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B130" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C130" s="23" t="s">
-        <v>69</v>
-      </c>
+      <c r="A130" s="22"/>
+      <c r="B130" s="22"/>
+      <c r="C130" s="22"/>
     </row>
     <row r="131">
-      <c r="A131" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B131" s="23"/>
-      <c r="C131" s="23"/>
+      <c r="A131" s="22"/>
+      <c r="B131" s="22"/>
+      <c r="C131" s="22"/>
     </row>
     <row r="132">
       <c r="A132" s="22"/>
@@ -26370,229 +26324,283 @@
       <c r="C136" s="22"/>
     </row>
     <row r="137">
-      <c r="A137" s="22"/>
-      <c r="B137" s="22"/>
-      <c r="C137" s="22"/>
+      <c r="A137" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B137" s="29" t="s">
+        <v>600</v>
+      </c>
+      <c r="C137" s="29" t="s">
+        <v>600</v>
+      </c>
     </row>
     <row r="138">
-      <c r="A138" s="22"/>
-      <c r="B138" s="22"/>
-      <c r="C138" s="22"/>
+      <c r="A138" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B138" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C138" s="30" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="139">
-      <c r="A139" s="22"/>
-      <c r="B139" s="22"/>
-      <c r="C139" s="22"/>
+      <c r="A139" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B139" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139" s="28" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="140">
-      <c r="A140" s="22"/>
-      <c r="B140" s="22"/>
-      <c r="C140" s="22"/>
+      <c r="A140" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B140" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="C140" s="28" t="s">
+        <v>601</v>
+      </c>
     </row>
     <row r="141">
-      <c r="A141" s="22"/>
-      <c r="B141" s="22"/>
-      <c r="C141" s="22"/>
+      <c r="A141" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B141" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C141" s="22" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="142">
-      <c r="A142" s="22"/>
-      <c r="B142" s="22"/>
-      <c r="C142" s="22"/>
+      <c r="A142" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B142" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C142" s="31" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="143">
-      <c r="A143" s="22"/>
-      <c r="B143" s="22"/>
-      <c r="C143" s="22"/>
+      <c r="A143" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="B143" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="C143" s="22" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="144">
-      <c r="A144" s="22"/>
-      <c r="B144" s="22"/>
-      <c r="C144" s="22"/>
+      <c r="A144" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="B144" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="C144" s="28" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="145">
-      <c r="A145" s="22"/>
-      <c r="B145" s="22"/>
-      <c r="C145" s="22"/>
+      <c r="A145" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="B145" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="C145" s="28" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="146">
-      <c r="A146" s="22"/>
-      <c r="B146" s="22"/>
-      <c r="C146" s="22"/>
+      <c r="A146" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="B146" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="C146" s="28" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B147" s="29" t="s">
-        <v>600</v>
-      </c>
-      <c r="C147" s="29" t="s">
-        <v>600</v>
+        <v>209</v>
+      </c>
+      <c r="B147" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="C147" s="28" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B148" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C148" s="30" t="s">
-        <v>48</v>
+        <v>195</v>
+      </c>
+      <c r="B148" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="C148" s="28" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="28" t="s">
-        <v>49</v>
+        <v>284</v>
       </c>
       <c r="B149" s="28" t="s">
-        <v>9</v>
+        <v>285</v>
       </c>
       <c r="C149" s="28" t="s">
-        <v>9</v>
+        <v>285</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="B150" s="28" t="s">
-        <v>601</v>
-      </c>
-      <c r="C150" s="28" t="s">
-        <v>601</v>
+        <v>163</v>
+      </c>
+      <c r="B150" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C150" s="22" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="B151" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C151" s="22" t="s">
-        <v>86</v>
+        <v>165</v>
+      </c>
+      <c r="B151" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="C151" s="31" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="B152" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="C152" s="31" t="s">
-        <v>92</v>
+        <v>282</v>
+      </c>
+      <c r="B152" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="C152" s="22" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="28" t="s">
-        <v>276</v>
-      </c>
-      <c r="B153" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="C153" s="22" t="s">
-        <v>277</v>
-      </c>
+      <c r="A153" s="22"/>
+      <c r="B153" s="22"/>
+      <c r="C153" s="22"/>
     </row>
     <row r="154">
       <c r="A154" s="28" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
       <c r="B154" s="28" t="s">
-        <v>192</v>
+        <v>329</v>
       </c>
       <c r="C154" s="28" t="s">
-        <v>192</v>
+        <v>329</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="B155" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="C155" s="28" t="s">
-        <v>211</v>
+        <v>602</v>
+      </c>
+      <c r="B155" s="31" t="s">
+        <v>603</v>
+      </c>
+      <c r="C155" s="31" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="B156" s="28" t="s">
-        <v>208</v>
-      </c>
-      <c r="C156" s="28" t="s">
-        <v>208</v>
+        <v>332</v>
+      </c>
+      <c r="B156" s="22" t="s">
+        <v>604</v>
+      </c>
+      <c r="C156" s="22" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="28" t="s">
-        <v>209</v>
-      </c>
-      <c r="B157" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="C157" s="28" t="s">
-        <v>210</v>
+        <v>605</v>
+      </c>
+      <c r="B157" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="C157" s="22" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="28" t="s">
-        <v>195</v>
+        <v>127</v>
       </c>
       <c r="B158" s="28" t="s">
-        <v>196</v>
+        <v>128</v>
       </c>
       <c r="C158" s="28" t="s">
-        <v>196</v>
+        <v>128</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="B159" s="28" t="s">
-        <v>285</v>
-      </c>
-      <c r="C159" s="28" t="s">
-        <v>285</v>
+        <v>133</v>
+      </c>
+      <c r="B159" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C159" s="31" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="B160" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="C160" s="22" t="s">
-        <v>164</v>
+        <v>286</v>
+      </c>
+      <c r="B160" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="C160" s="28" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="28" t="s">
-        <v>165</v>
-      </c>
-      <c r="B161" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="C161" s="31" t="s">
-        <v>166</v>
+        <v>201</v>
+      </c>
+      <c r="B161" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="C161" s="28" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="28" t="s">
-        <v>282</v>
-      </c>
-      <c r="B162" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="C162" s="22" t="s">
-        <v>283</v>
+        <v>203</v>
+      </c>
+      <c r="B162" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="C162" s="28" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="163">
@@ -26602,787 +26610,793 @@
     </row>
     <row r="164">
       <c r="A164" s="28" t="s">
-        <v>328</v>
-      </c>
-      <c r="B164" s="28" t="s">
-        <v>329</v>
-      </c>
-      <c r="C164" s="28" t="s">
-        <v>329</v>
+        <v>606</v>
+      </c>
+      <c r="B164" s="31" t="s">
+        <v>607</v>
+      </c>
+      <c r="C164" s="31" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="28" t="s">
-        <v>602</v>
-      </c>
-      <c r="B165" s="31" t="s">
-        <v>603</v>
-      </c>
-      <c r="C165" s="31" t="s">
-        <v>603</v>
+        <v>608</v>
+      </c>
+      <c r="B165" s="22" t="s">
+        <v>609</v>
+      </c>
+      <c r="C165" s="22" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="28" t="s">
-        <v>332</v>
-      </c>
-      <c r="B166" s="22" t="s">
-        <v>604</v>
-      </c>
-      <c r="C166" s="22" t="s">
-        <v>604</v>
+        <v>139</v>
+      </c>
+      <c r="B166" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="C166" s="28" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="28" t="s">
-        <v>605</v>
-      </c>
-      <c r="B167" s="22" t="s">
-        <v>335</v>
-      </c>
-      <c r="C167" s="22" t="s">
-        <v>335</v>
+        <v>143</v>
+      </c>
+      <c r="B167" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="C167" s="31" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="28" t="s">
-        <v>127</v>
+        <v>294</v>
       </c>
       <c r="B168" s="28" t="s">
-        <v>128</v>
+        <v>295</v>
       </c>
       <c r="C168" s="28" t="s">
-        <v>128</v>
+        <v>295</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B169" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="C169" s="31" t="s">
-        <v>134</v>
+        <v>610</v>
+      </c>
+      <c r="B169" s="28" t="s">
+        <v>611</v>
+      </c>
+      <c r="C169" s="28" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="28" t="s">
-        <v>286</v>
+        <v>336</v>
       </c>
       <c r="B170" s="28" t="s">
-        <v>287</v>
+        <v>192</v>
       </c>
       <c r="C170" s="28" t="s">
-        <v>287</v>
+        <v>192</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="28" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="B171" s="28" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="C171" s="28" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="28" t="s">
-        <v>203</v>
+        <v>612</v>
       </c>
       <c r="B172" s="28" t="s">
-        <v>204</v>
+        <v>613</v>
       </c>
       <c r="C172" s="28" t="s">
-        <v>204</v>
+        <v>613</v>
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="22"/>
-      <c r="B173" s="22"/>
-      <c r="C173" s="22"/>
+      <c r="A173" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="B173" s="28" t="s">
+        <v>340</v>
+      </c>
+      <c r="C173" s="28" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="28" t="s">
-        <v>606</v>
+        <v>614</v>
       </c>
       <c r="B174" s="31" t="s">
-        <v>607</v>
+        <v>615</v>
       </c>
       <c r="C174" s="31" t="s">
-        <v>607</v>
+        <v>615</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="28" t="s">
-        <v>608</v>
-      </c>
-      <c r="B175" s="22" t="s">
-        <v>609</v>
-      </c>
-      <c r="C175" s="22" t="s">
-        <v>609</v>
+        <v>219</v>
+      </c>
+      <c r="B175" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="C175" s="28" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="28" t="s">
-        <v>139</v>
+        <v>221</v>
       </c>
       <c r="B176" s="28" t="s">
-        <v>140</v>
+        <v>222</v>
       </c>
       <c r="C176" s="28" t="s">
-        <v>140</v>
+        <v>222</v>
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="B177" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="C177" s="31" t="s">
-        <v>144</v>
-      </c>
+      <c r="A177" s="22"/>
+      <c r="B177" s="22"/>
+      <c r="C177" s="22"/>
     </row>
     <row r="178">
       <c r="A178" s="28" t="s">
-        <v>294</v>
+        <v>223</v>
       </c>
       <c r="B178" s="28" t="s">
-        <v>295</v>
+        <v>224</v>
       </c>
       <c r="C178" s="28" t="s">
-        <v>295</v>
+        <v>224</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="28" t="s">
-        <v>610</v>
+        <v>213</v>
       </c>
       <c r="B179" s="28" t="s">
-        <v>611</v>
+        <v>214</v>
       </c>
       <c r="C179" s="28" t="s">
-        <v>611</v>
+        <v>214</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="28" t="s">
-        <v>336</v>
-      </c>
-      <c r="B180" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="C180" s="28" t="s">
-        <v>192</v>
+        <v>616</v>
+      </c>
+      <c r="B180" s="31" t="s">
+        <v>617</v>
+      </c>
+      <c r="C180" s="31" t="s">
+        <v>617</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="28" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="B181" s="28" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="C181" s="28" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="28" t="s">
-        <v>612</v>
+        <v>175</v>
       </c>
       <c r="B182" s="28" t="s">
-        <v>613</v>
+        <v>192</v>
       </c>
       <c r="C182" s="28" t="s">
-        <v>613</v>
+        <v>192</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="28" t="s">
-        <v>339</v>
-      </c>
-      <c r="B183" s="28" t="s">
-        <v>340</v>
-      </c>
-      <c r="C183" s="28" t="s">
-        <v>340</v>
+        <v>618</v>
+      </c>
+      <c r="B183" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="C183" s="31" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="28" t="s">
-        <v>614</v>
+        <v>620</v>
       </c>
       <c r="B184" s="31" t="s">
-        <v>615</v>
+        <v>621</v>
       </c>
       <c r="C184" s="31" t="s">
-        <v>615</v>
+        <v>621</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="B185" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="C185" s="28" t="s">
-        <v>220</v>
+        <v>115</v>
+      </c>
+      <c r="B185" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C185" s="32" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="B186" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="C186" s="28" t="s">
-        <v>222</v>
+      <c r="A186" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B186" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C186" s="33" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="22"/>
-      <c r="B187" s="22"/>
-      <c r="C187" s="22"/>
+      <c r="A187" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B187" s="32" t="s">
+        <v>622</v>
+      </c>
+      <c r="C187" s="32" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="188">
-      <c r="A188" s="28" t="s">
-        <v>223</v>
-      </c>
-      <c r="B188" s="28" t="s">
-        <v>224</v>
-      </c>
-      <c r="C188" s="28" t="s">
-        <v>224</v>
+      <c r="A188" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B188" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="C188" s="34" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="28" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="B189" s="28" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="C189" s="28" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="28" t="s">
-        <v>616</v>
-      </c>
-      <c r="B190" s="31" t="s">
-        <v>617</v>
-      </c>
-      <c r="C190" s="31" t="s">
-        <v>617</v>
+        <v>97</v>
+      </c>
+      <c r="B190" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C190" s="28" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="B191" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="C191" s="28" t="s">
-        <v>200</v>
+        <v>107</v>
+      </c>
+      <c r="B191" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C191" s="31" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="B192" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="C192" s="28" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="B192" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="C192" s="31" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="28" t="s">
-        <v>618</v>
+        <v>159</v>
       </c>
       <c r="B193" s="31" t="s">
-        <v>619</v>
+        <v>192</v>
       </c>
       <c r="C193" s="31" t="s">
-        <v>619</v>
+        <v>192</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="28" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="B194" s="31" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="C194" s="31" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="B195" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="C195" s="32" t="s">
-        <v>116</v>
+        <v>197</v>
+      </c>
+      <c r="B195" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="C195" s="31" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="196">
-      <c r="A196" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="B196" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="C196" s="33" t="s">
-        <v>122</v>
+      <c r="A196" s="28" t="s">
+        <v>625</v>
+      </c>
+      <c r="B196" s="31" t="s">
+        <v>626</v>
+      </c>
+      <c r="C196" s="31" t="s">
+        <v>626</v>
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B197" s="32" t="s">
-        <v>622</v>
-      </c>
-      <c r="C197" s="32" t="s">
-        <v>622</v>
+      <c r="A197" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="B197" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C197" s="28" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="B198" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="C198" s="34" t="s">
-        <v>154</v>
+      <c r="A198" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="B198" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C198" s="31" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="28" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B199" s="28" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C199" s="28" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="28" t="s">
-        <v>97</v>
+        <v>181</v>
       </c>
       <c r="B200" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C200" s="28" t="s">
-        <v>98</v>
+        <v>182</v>
+      </c>
+      <c r="C200" s="33" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="B201" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="C201" s="31" t="s">
-        <v>108</v>
+        <v>225</v>
+      </c>
+      <c r="B201" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="C201" s="33" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="202">
-      <c r="A202" s="28" t="s">
-        <v>193</v>
-      </c>
-      <c r="B202" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="C202" s="31" t="s">
-        <v>194</v>
+      <c r="A202" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B202" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C202" s="33" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="B203" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="C203" s="31" t="s">
-        <v>192</v>
+      <c r="A203" s="33" t="s">
+        <v>627</v>
+      </c>
+      <c r="B203" s="33" t="s">
+        <v>628</v>
+      </c>
+      <c r="C203" s="33" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="28" t="s">
-        <v>623</v>
-      </c>
-      <c r="B204" s="31" t="s">
-        <v>624</v>
-      </c>
-      <c r="C204" s="31" t="s">
-        <v>624</v>
+        <v>36</v>
+      </c>
+      <c r="B204" s="28" t="s">
+        <v>629</v>
+      </c>
+      <c r="C204" s="28" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="B205" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="C205" s="31" t="s">
-        <v>198</v>
+        <v>630</v>
+      </c>
+      <c r="B205" s="22" t="s">
+        <v>631</v>
+      </c>
+      <c r="C205" s="22" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="28" t="s">
-        <v>625</v>
-      </c>
-      <c r="B206" s="31" t="s">
-        <v>626</v>
-      </c>
-      <c r="C206" s="31" t="s">
-        <v>626</v>
+        <v>632</v>
+      </c>
+      <c r="B206" s="35" t="s">
+        <v>633</v>
+      </c>
+      <c r="C206" s="35" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="28" t="s">
-        <v>183</v>
+        <v>634</v>
       </c>
       <c r="B207" s="28" t="s">
-        <v>184</v>
+        <v>635</v>
       </c>
       <c r="C207" s="28" t="s">
-        <v>184</v>
+        <v>635</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="B208" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="C208" s="31" t="s">
-        <v>186</v>
+        <v>636</v>
+      </c>
+      <c r="B208" s="22" t="s">
+        <v>637</v>
+      </c>
+      <c r="C208" s="22" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="B209" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="C209" s="28" t="s">
-        <v>180</v>
+        <v>638</v>
+      </c>
+      <c r="B209" s="36">
+        <v>120.0</v>
+      </c>
+      <c r="C209" s="36">
+        <v>120.0</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="B210" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="C210" s="33" t="s">
-        <v>182</v>
+        <v>639</v>
+      </c>
+      <c r="B210" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="C210" s="22" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="B211" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="C211" s="33" t="s">
-        <v>226</v>
+        <v>641</v>
+      </c>
+      <c r="B211" s="22" t="s">
+        <v>642</v>
+      </c>
+      <c r="C211" s="22" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="212">
-      <c r="A212" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="B212" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C212" s="33" t="s">
-        <v>9</v>
+      <c r="A212" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B212" s="22" t="s">
+        <v>644</v>
+      </c>
+      <c r="C212" s="22" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="33" t="s">
-        <v>627</v>
-      </c>
-      <c r="B213" s="33" t="s">
-        <v>628</v>
-      </c>
-      <c r="C213" s="33" t="s">
-        <v>628</v>
+      <c r="A213" s="28" t="s">
+        <v>645</v>
+      </c>
+      <c r="B213" s="22" t="s">
+        <v>646</v>
+      </c>
+      <c r="C213" s="22" t="s">
+        <v>646</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B214" s="28" t="s">
-        <v>629</v>
-      </c>
-      <c r="C214" s="28" t="s">
-        <v>629</v>
+        <v>647</v>
+      </c>
+      <c r="B214" s="22" t="s">
+        <v>637</v>
+      </c>
+      <c r="C214" s="22" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="215">
-      <c r="A215" s="28" t="s">
-        <v>630</v>
+      <c r="A215" s="22" t="s">
+        <v>648</v>
       </c>
       <c r="B215" s="22" t="s">
-        <v>631</v>
+        <v>649</v>
       </c>
       <c r="C215" s="22" t="s">
-        <v>631</v>
+        <v>649</v>
       </c>
     </row>
     <row r="216">
-      <c r="A216" s="28" t="s">
-        <v>632</v>
-      </c>
-      <c r="B216" s="35" t="s">
-        <v>633</v>
-      </c>
-      <c r="C216" s="35" t="s">
-        <v>633</v>
+      <c r="A216" s="22" t="s">
+        <v>650</v>
+      </c>
+      <c r="B216" s="36">
+        <v>6.0</v>
+      </c>
+      <c r="C216" s="36">
+        <v>6.0</v>
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="28" t="s">
-        <v>634</v>
-      </c>
-      <c r="B217" s="28" t="s">
-        <v>635</v>
-      </c>
-      <c r="C217" s="28" t="s">
-        <v>635</v>
+      <c r="A217" s="22" t="s">
+        <v>651</v>
+      </c>
+      <c r="B217" s="22" t="s">
+        <v>652</v>
+      </c>
+      <c r="C217" s="22" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="218">
-      <c r="A218" s="28" t="s">
-        <v>636</v>
+      <c r="A218" s="22" t="s">
+        <v>653</v>
       </c>
       <c r="B218" s="22" t="s">
+        <v>654</v>
+      </c>
+      <c r="C218" s="22" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="22" t="s">
+        <v>655</v>
+      </c>
+      <c r="B219" s="22" t="s">
+        <v>656</v>
+      </c>
+      <c r="C219" s="22" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="22" t="s">
+        <v>657</v>
+      </c>
+      <c r="B220" s="22" t="s">
         <v>637</v>
       </c>
-      <c r="C218" s="22" t="s">
+      <c r="C220" s="22" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="219">
-      <c r="A219" s="28" t="s">
-        <v>638</v>
-      </c>
-      <c r="B219" s="36">
-        <v>120.0</v>
-      </c>
-      <c r="C219" s="36">
-        <v>120.0</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" s="28" t="s">
-        <v>639</v>
-      </c>
-      <c r="B220" s="22" t="s">
-        <v>640</v>
-      </c>
-      <c r="C220" s="22" t="s">
-        <v>640</v>
-      </c>
-    </row>
     <row r="221">
-      <c r="A221" s="28" t="s">
-        <v>641</v>
+      <c r="A221" s="22" t="s">
+        <v>658</v>
       </c>
       <c r="B221" s="22" t="s">
-        <v>642</v>
+        <v>659</v>
       </c>
       <c r="C221" s="22" t="s">
-        <v>642</v>
+        <v>659</v>
       </c>
     </row>
     <row r="222">
-      <c r="A222" s="28" t="s">
-        <v>643</v>
-      </c>
-      <c r="B222" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="C222" s="22" t="s">
-        <v>644</v>
+      <c r="A222" s="22" t="s">
+        <v>660</v>
+      </c>
+      <c r="B222" s="37">
+        <v>13.0</v>
+      </c>
+      <c r="C222" s="37">
+        <v>13.0</v>
       </c>
     </row>
     <row r="223">
-      <c r="A223" s="28" t="s">
-        <v>645</v>
+      <c r="A223" s="22" t="s">
+        <v>661</v>
       </c>
       <c r="B223" s="22" t="s">
-        <v>646</v>
+        <v>662</v>
       </c>
       <c r="C223" s="22" t="s">
-        <v>646</v>
+        <v>662</v>
       </c>
     </row>
     <row r="224">
-      <c r="A224" s="28" t="s">
-        <v>647</v>
+      <c r="A224" s="22" t="s">
+        <v>663</v>
       </c>
       <c r="B224" s="22" t="s">
-        <v>637</v>
+        <v>664</v>
       </c>
       <c r="C224" s="22" t="s">
-        <v>637</v>
+        <v>664</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="22" t="s">
-        <v>648</v>
+        <v>665</v>
       </c>
       <c r="B225" s="22" t="s">
-        <v>649</v>
+        <v>666</v>
       </c>
       <c r="C225" s="22" t="s">
-        <v>649</v>
+        <v>666</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="22" t="s">
-        <v>650</v>
-      </c>
-      <c r="B226" s="36">
-        <v>6.0</v>
-      </c>
-      <c r="C226" s="36">
-        <v>6.0</v>
+        <v>667</v>
+      </c>
+      <c r="B226" s="22" t="s">
+        <v>637</v>
+      </c>
+      <c r="C226" s="22" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="22" t="s">
-        <v>651</v>
+        <v>668</v>
       </c>
       <c r="B227" s="22" t="s">
-        <v>652</v>
+        <v>669</v>
       </c>
       <c r="C227" s="22" t="s">
-        <v>652</v>
+        <v>669</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="22" t="s">
-        <v>653</v>
-      </c>
-      <c r="B228" s="22" t="s">
-        <v>654</v>
-      </c>
-      <c r="C228" s="22" t="s">
-        <v>654</v>
+        <v>670</v>
+      </c>
+      <c r="B228" s="36">
+        <v>12.0</v>
+      </c>
+      <c r="C228" s="36">
+        <v>12.0</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="22" t="s">
-        <v>655</v>
+        <v>671</v>
       </c>
       <c r="B229" s="22" t="s">
-        <v>656</v>
+        <v>672</v>
       </c>
       <c r="C229" s="22" t="s">
-        <v>656</v>
+        <v>672</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="22" t="s">
-        <v>657</v>
+        <v>673</v>
       </c>
       <c r="B230" s="22" t="s">
-        <v>637</v>
+        <v>674</v>
       </c>
       <c r="C230" s="22" t="s">
-        <v>637</v>
+        <v>674</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="22" t="s">
-        <v>658</v>
+        <v>675</v>
       </c>
       <c r="B231" s="22" t="s">
-        <v>659</v>
+        <v>637</v>
       </c>
       <c r="C231" s="22" t="s">
-        <v>659</v>
+        <v>637</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="22" t="s">
-        <v>660</v>
-      </c>
-      <c r="B232" s="37">
-        <v>13.0</v>
-      </c>
-      <c r="C232" s="37">
-        <v>13.0</v>
+        <v>676</v>
+      </c>
+      <c r="B232" s="22" t="s">
+        <v>677</v>
+      </c>
+      <c r="C232" s="22" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="22" t="s">
-        <v>661</v>
-      </c>
-      <c r="B233" s="22" t="s">
-        <v>662</v>
-      </c>
-      <c r="C233" s="22" t="s">
-        <v>662</v>
+        <v>678</v>
+      </c>
+      <c r="B233" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="C233" s="36">
+        <v>2.0</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="22" t="s">
-        <v>663</v>
+        <v>679</v>
       </c>
       <c r="B234" s="22" t="s">
-        <v>664</v>
+        <v>680</v>
       </c>
       <c r="C234" s="22" t="s">
-        <v>664</v>
+        <v>680</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="22" t="s">
-        <v>665</v>
+        <v>681</v>
       </c>
       <c r="B235" s="22" t="s">
-        <v>666</v>
+        <v>682</v>
       </c>
       <c r="C235" s="22" t="s">
-        <v>666</v>
+        <v>682</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="22" t="s">
-        <v>667</v>
+        <v>683</v>
       </c>
       <c r="B236" s="22" t="s">
         <v>637</v>
@@ -27393,51 +27407,51 @@
     </row>
     <row r="237">
       <c r="A237" s="22" t="s">
-        <v>668</v>
-      </c>
-      <c r="B237" s="22" t="s">
-        <v>669</v>
-      </c>
-      <c r="C237" s="22" t="s">
-        <v>669</v>
+        <v>684</v>
+      </c>
+      <c r="B237" s="36">
+        <v>7.0</v>
+      </c>
+      <c r="C237" s="36">
+        <v>7.0</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="22" t="s">
-        <v>670</v>
+        <v>685</v>
       </c>
       <c r="B238" s="36">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="C238" s="36">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="22" t="s">
-        <v>671</v>
+        <v>686</v>
       </c>
       <c r="B239" s="22" t="s">
-        <v>672</v>
+        <v>687</v>
       </c>
       <c r="C239" s="22" t="s">
-        <v>672</v>
+        <v>687</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="22" t="s">
-        <v>673</v>
+        <v>688</v>
       </c>
       <c r="B240" s="22" t="s">
-        <v>674</v>
+        <v>689</v>
       </c>
       <c r="C240" s="22" t="s">
-        <v>674</v>
+        <v>689</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="22" t="s">
-        <v>675</v>
+        <v>690</v>
       </c>
       <c r="B241" s="22" t="s">
         <v>637</v>
@@ -27448,51 +27462,51 @@
     </row>
     <row r="242">
       <c r="A242" s="22" t="s">
-        <v>676</v>
+        <v>691</v>
       </c>
       <c r="B242" s="22" t="s">
-        <v>677</v>
-      </c>
-      <c r="C242" s="22" t="s">
-        <v>677</v>
+        <v>692</v>
+      </c>
+      <c r="C242" s="35" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="22" t="s">
-        <v>678</v>
+        <v>693</v>
       </c>
       <c r="B243" s="36">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="C243" s="36">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="22" t="s">
-        <v>679</v>
+        <v>694</v>
       </c>
       <c r="B244" s="22" t="s">
-        <v>680</v>
+        <v>695</v>
       </c>
       <c r="C244" s="22" t="s">
-        <v>680</v>
+        <v>695</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="22" t="s">
-        <v>681</v>
+        <v>696</v>
       </c>
       <c r="B245" s="22" t="s">
-        <v>682</v>
+        <v>697</v>
       </c>
       <c r="C245" s="22" t="s">
-        <v>682</v>
+        <v>697</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="22" t="s">
-        <v>683</v>
+        <v>698</v>
       </c>
       <c r="B246" s="22" t="s">
         <v>637</v>
@@ -27503,51 +27517,51 @@
     </row>
     <row r="247">
       <c r="A247" s="22" t="s">
-        <v>684</v>
+        <v>699</v>
       </c>
       <c r="B247" s="36">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="C247" s="36">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="22" t="s">
-        <v>685</v>
+        <v>700</v>
       </c>
       <c r="B248" s="36">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="C248" s="36">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="22" t="s">
-        <v>686</v>
+        <v>701</v>
       </c>
       <c r="B249" s="22" t="s">
-        <v>687</v>
+        <v>702</v>
       </c>
       <c r="C249" s="22" t="s">
-        <v>687</v>
+        <v>702</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="22" t="s">
-        <v>688</v>
+        <v>703</v>
       </c>
       <c r="B250" s="22" t="s">
-        <v>689</v>
+        <v>702</v>
       </c>
       <c r="C250" s="22" t="s">
-        <v>689</v>
+        <v>702</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="22" t="s">
-        <v>690</v>
+        <v>704</v>
       </c>
       <c r="B251" s="22" t="s">
         <v>637</v>
@@ -27558,51 +27572,51 @@
     </row>
     <row r="252">
       <c r="A252" s="22" t="s">
-        <v>691</v>
-      </c>
-      <c r="B252" s="22" t="s">
-        <v>692</v>
-      </c>
-      <c r="C252" s="35" t="s">
-        <v>692</v>
+        <v>705</v>
+      </c>
+      <c r="B252" s="36">
+        <v>12.0</v>
+      </c>
+      <c r="C252" s="36">
+        <v>12.0</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="22" t="s">
-        <v>693</v>
+        <v>706</v>
       </c>
       <c r="B253" s="36">
-        <v>6.0</v>
+        <v>13.0</v>
       </c>
       <c r="C253" s="36">
-        <v>6.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="22" t="s">
-        <v>694</v>
+        <v>707</v>
       </c>
       <c r="B254" s="22" t="s">
-        <v>695</v>
+        <v>708</v>
       </c>
       <c r="C254" s="22" t="s">
-        <v>695</v>
+        <v>708</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="22" t="s">
-        <v>696</v>
+        <v>709</v>
       </c>
       <c r="B255" s="22" t="s">
-        <v>697</v>
+        <v>710</v>
       </c>
       <c r="C255" s="22" t="s">
-        <v>697</v>
+        <v>710</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="22" t="s">
-        <v>698</v>
+        <v>711</v>
       </c>
       <c r="B256" s="22" t="s">
         <v>637</v>
@@ -27613,51 +27627,51 @@
     </row>
     <row r="257">
       <c r="A257" s="22" t="s">
-        <v>699</v>
-      </c>
-      <c r="B257" s="36">
-        <v>9.0</v>
-      </c>
-      <c r="C257" s="36">
-        <v>9.0</v>
+        <v>712</v>
+      </c>
+      <c r="B257" s="22" t="s">
+        <v>649</v>
+      </c>
+      <c r="C257" s="22" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="22" t="s">
-        <v>700</v>
+        <v>713</v>
       </c>
       <c r="B258" s="36">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
       <c r="C258" s="36">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="22" t="s">
-        <v>701</v>
+        <v>714</v>
       </c>
       <c r="B259" s="22" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="C259" s="22" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="22" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="B260" s="22" t="s">
-        <v>702</v>
+        <v>717</v>
       </c>
       <c r="C260" s="22" t="s">
-        <v>702</v>
+        <v>717</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="22" t="s">
-        <v>704</v>
+        <v>718</v>
       </c>
       <c r="B261" s="22" t="s">
         <v>637</v>
@@ -27668,51 +27682,51 @@
     </row>
     <row r="262">
       <c r="A262" s="22" t="s">
-        <v>705</v>
-      </c>
-      <c r="B262" s="36">
-        <v>12.0</v>
-      </c>
-      <c r="C262" s="36">
-        <v>12.0</v>
+        <v>719</v>
+      </c>
+      <c r="B262" s="22" t="s">
+        <v>720</v>
+      </c>
+      <c r="C262" s="22" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="22" t="s">
-        <v>706</v>
+        <v>721</v>
       </c>
       <c r="B263" s="36">
-        <v>13.0</v>
+        <v>7.0</v>
       </c>
       <c r="C263" s="36">
-        <v>13.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="22" t="s">
-        <v>707</v>
+        <v>722</v>
       </c>
       <c r="B264" s="22" t="s">
-        <v>708</v>
+        <v>723</v>
       </c>
       <c r="C264" s="22" t="s">
-        <v>708</v>
+        <v>723</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="22" t="s">
-        <v>709</v>
+        <v>724</v>
       </c>
       <c r="B265" s="22" t="s">
-        <v>710</v>
+        <v>725</v>
       </c>
       <c r="C265" s="22" t="s">
-        <v>710</v>
+        <v>725</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="22" t="s">
-        <v>711</v>
+        <v>726</v>
       </c>
       <c r="B266" s="22" t="s">
         <v>637</v>
@@ -27723,51 +27737,51 @@
     </row>
     <row r="267">
       <c r="A267" s="22" t="s">
-        <v>712</v>
+        <v>727</v>
       </c>
       <c r="B267" s="22" t="s">
-        <v>649</v>
+        <v>728</v>
       </c>
       <c r="C267" s="22" t="s">
-        <v>649</v>
+        <v>728</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="22" t="s">
-        <v>713</v>
+        <v>729</v>
       </c>
       <c r="B268" s="36">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="C268" s="36">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="22" t="s">
-        <v>714</v>
+        <v>730</v>
       </c>
       <c r="B269" s="22" t="s">
-        <v>715</v>
+        <v>731</v>
       </c>
       <c r="C269" s="22" t="s">
-        <v>715</v>
+        <v>731</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="22" t="s">
-        <v>716</v>
+        <v>732</v>
       </c>
       <c r="B270" s="22" t="s">
-        <v>717</v>
+        <v>733</v>
       </c>
       <c r="C270" s="22" t="s">
-        <v>717</v>
+        <v>733</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="22" t="s">
-        <v>718</v>
+        <v>734</v>
       </c>
       <c r="B271" s="22" t="s">
         <v>637</v>
@@ -27778,51 +27792,51 @@
     </row>
     <row r="272">
       <c r="A272" s="22" t="s">
-        <v>719</v>
+        <v>735</v>
       </c>
       <c r="B272" s="22" t="s">
-        <v>720</v>
+        <v>736</v>
       </c>
       <c r="C272" s="22" t="s">
-        <v>720</v>
+        <v>736</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="22" t="s">
-        <v>721</v>
+        <v>737</v>
       </c>
       <c r="B273" s="36">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="C273" s="36">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="22" t="s">
-        <v>722</v>
+        <v>738</v>
       </c>
       <c r="B274" s="22" t="s">
-        <v>723</v>
+        <v>739</v>
       </c>
       <c r="C274" s="22" t="s">
-        <v>723</v>
+        <v>739</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="22" t="s">
-        <v>724</v>
+        <v>740</v>
       </c>
       <c r="B275" s="22" t="s">
-        <v>725</v>
+        <v>741</v>
       </c>
       <c r="C275" s="22" t="s">
-        <v>725</v>
+        <v>741</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="22" t="s">
-        <v>726</v>
+        <v>742</v>
       </c>
       <c r="B276" s="22" t="s">
         <v>637</v>
@@ -27833,18 +27847,18 @@
     </row>
     <row r="277">
       <c r="A277" s="22" t="s">
-        <v>727</v>
+        <v>743</v>
       </c>
       <c r="B277" s="22" t="s">
-        <v>728</v>
+        <v>744</v>
       </c>
       <c r="C277" s="22" t="s">
-        <v>728</v>
+        <v>744</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="22" t="s">
-        <v>729</v>
+        <v>745</v>
       </c>
       <c r="B278" s="36">
         <v>3.0</v>
@@ -27855,29 +27869,29 @@
     </row>
     <row r="279">
       <c r="A279" s="22" t="s">
-        <v>730</v>
+        <v>746</v>
       </c>
       <c r="B279" s="22" t="s">
-        <v>731</v>
+        <v>747</v>
       </c>
       <c r="C279" s="22" t="s">
-        <v>731</v>
+        <v>747</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="22" t="s">
-        <v>732</v>
+        <v>748</v>
       </c>
       <c r="B280" s="22" t="s">
-        <v>733</v>
+        <v>749</v>
       </c>
       <c r="C280" s="22" t="s">
-        <v>733</v>
+        <v>749</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="22" t="s">
-        <v>734</v>
+        <v>750</v>
       </c>
       <c r="B281" s="22" t="s">
         <v>637</v>
@@ -27888,18 +27902,18 @@
     </row>
     <row r="282">
       <c r="A282" s="22" t="s">
-        <v>735</v>
-      </c>
-      <c r="B282" s="22" t="s">
-        <v>736</v>
-      </c>
-      <c r="C282" s="22" t="s">
-        <v>736</v>
+        <v>751</v>
+      </c>
+      <c r="B282" s="35" t="s">
+        <v>752</v>
+      </c>
+      <c r="C282" s="35" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="22" t="s">
-        <v>737</v>
+        <v>753</v>
       </c>
       <c r="B283" s="36">
         <v>3.0</v>
@@ -27910,84 +27924,84 @@
     </row>
     <row r="284">
       <c r="A284" s="22" t="s">
-        <v>738</v>
-      </c>
-      <c r="B284" s="22" t="s">
-        <v>739</v>
-      </c>
-      <c r="C284" s="22" t="s">
-        <v>739</v>
+        <v>754</v>
+      </c>
+      <c r="B284" s="38" t="s">
+        <v>755</v>
+      </c>
+      <c r="C284" s="38" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="22" t="s">
-        <v>740</v>
+        <v>756</v>
       </c>
       <c r="B285" s="22" t="s">
-        <v>741</v>
+        <v>757</v>
       </c>
       <c r="C285" s="22" t="s">
-        <v>741</v>
+        <v>757</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="22" t="s">
-        <v>742</v>
+        <v>758</v>
       </c>
       <c r="B286" s="22" t="s">
-        <v>637</v>
+        <v>759</v>
       </c>
       <c r="C286" s="22" t="s">
-        <v>637</v>
+        <v>759</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="22" t="s">
-        <v>743</v>
+        <v>760</v>
       </c>
       <c r="B287" s="22" t="s">
-        <v>744</v>
+        <v>637</v>
       </c>
       <c r="C287" s="22" t="s">
-        <v>744</v>
+        <v>637</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="22" t="s">
-        <v>745</v>
-      </c>
-      <c r="B288" s="36">
-        <v>3.0</v>
-      </c>
-      <c r="C288" s="36">
-        <v>3.0</v>
+        <v>761</v>
+      </c>
+      <c r="B288" s="36" t="s">
+        <v>762</v>
+      </c>
+      <c r="C288" s="36" t="s">
+        <v>762</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="22" t="s">
-        <v>746</v>
-      </c>
-      <c r="B289" s="22" t="s">
-        <v>747</v>
-      </c>
-      <c r="C289" s="22" t="s">
-        <v>747</v>
+        <v>763</v>
+      </c>
+      <c r="B289" s="36">
+        <v>6.0</v>
+      </c>
+      <c r="C289" s="36">
+        <v>6.0</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="22" t="s">
-        <v>748</v>
+        <v>764</v>
       </c>
       <c r="B290" s="22" t="s">
-        <v>749</v>
+        <v>765</v>
       </c>
       <c r="C290" s="22" t="s">
-        <v>749</v>
+        <v>765</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="22" t="s">
-        <v>750</v>
+        <v>766</v>
       </c>
       <c r="B291" s="22" t="s">
         <v>637</v>
@@ -27998,785 +28012,692 @@
     </row>
     <row r="292">
       <c r="A292" s="22" t="s">
-        <v>751</v>
-      </c>
-      <c r="B292" s="35" t="s">
-        <v>752</v>
-      </c>
-      <c r="C292" s="35" t="s">
-        <v>752</v>
+        <v>767</v>
+      </c>
+      <c r="B292" s="38" t="s">
+        <v>768</v>
+      </c>
+      <c r="C292" s="38" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="22" t="s">
-        <v>753</v>
+        <v>769</v>
       </c>
       <c r="B293" s="36">
-        <v>3.0</v>
+        <v>50.0</v>
       </c>
       <c r="C293" s="36">
-        <v>3.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="22" t="s">
-        <v>754</v>
-      </c>
-      <c r="B294" s="22" t="s">
-        <v>755</v>
-      </c>
-      <c r="C294" s="22" t="s">
-        <v>755</v>
+        <v>770</v>
+      </c>
+      <c r="B294" s="36">
+        <v>55.0</v>
+      </c>
+      <c r="C294" s="36">
+        <v>55.0</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="22" t="s">
-        <v>756</v>
+        <v>771</v>
       </c>
       <c r="B295" s="22" t="s">
-        <v>757</v>
+        <v>772</v>
       </c>
       <c r="C295" s="22" t="s">
-        <v>757</v>
+        <v>772</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="22" t="s">
-        <v>758</v>
+        <v>773</v>
       </c>
       <c r="B296" s="22" t="s">
-        <v>759</v>
+        <v>774</v>
       </c>
       <c r="C296" s="22" t="s">
-        <v>759</v>
+        <v>774</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="22" t="s">
-        <v>760</v>
+        <v>775</v>
       </c>
       <c r="B297" s="22" t="s">
-        <v>637</v>
+        <v>776</v>
       </c>
       <c r="C297" s="22" t="s">
-        <v>637</v>
+        <v>776</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="22" t="s">
-        <v>761</v>
-      </c>
-      <c r="B298" s="36" t="s">
-        <v>762</v>
-      </c>
-      <c r="C298" s="36" t="s">
-        <v>762</v>
+        <v>777</v>
+      </c>
+      <c r="B298" s="22" t="s">
+        <v>778</v>
+      </c>
+      <c r="C298" s="22" t="s">
+        <v>778</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="22" t="s">
-        <v>763</v>
-      </c>
-      <c r="B299" s="36">
-        <v>6.0</v>
-      </c>
-      <c r="C299" s="36">
-        <v>6.0</v>
+        <v>779</v>
+      </c>
+      <c r="B299" s="22" t="s">
+        <v>778</v>
+      </c>
+      <c r="C299" s="22" t="s">
+        <v>778</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="22" t="s">
-        <v>764</v>
+        <v>780</v>
       </c>
       <c r="B300" s="22" t="s">
-        <v>765</v>
+        <v>781</v>
       </c>
       <c r="C300" s="22" t="s">
-        <v>765</v>
+        <v>781</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="22" t="s">
-        <v>766</v>
+        <v>782</v>
       </c>
       <c r="B301" s="22" t="s">
-        <v>637</v>
+        <v>783</v>
       </c>
       <c r="C301" s="22" t="s">
-        <v>637</v>
+        <v>783</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="22" t="s">
-        <v>767</v>
+        <v>784</v>
       </c>
       <c r="B302" s="22" t="s">
-        <v>768</v>
+        <v>785</v>
       </c>
       <c r="C302" s="22" t="s">
-        <v>768</v>
+        <v>785</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="22" t="s">
-        <v>769</v>
-      </c>
-      <c r="B303" s="36">
-        <v>50.0</v>
-      </c>
-      <c r="C303" s="36">
-        <v>50.0</v>
+        <v>786</v>
+      </c>
+      <c r="B303" s="22" t="s">
+        <v>787</v>
+      </c>
+      <c r="C303" s="22" t="s">
+        <v>787</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="22" t="s">
-        <v>770</v>
-      </c>
-      <c r="B304" s="36">
-        <v>55.0</v>
-      </c>
-      <c r="C304" s="36">
-        <v>55.0</v>
+        <v>788</v>
+      </c>
+      <c r="B304" s="22" t="s">
+        <v>789</v>
+      </c>
+      <c r="C304" s="22" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="22" t="s">
-        <v>771</v>
+        <v>790</v>
       </c>
       <c r="B305" s="22" t="s">
-        <v>772</v>
+        <v>791</v>
       </c>
       <c r="C305" s="22" t="s">
-        <v>772</v>
+        <v>791</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="22" t="s">
-        <v>773</v>
+        <v>792</v>
       </c>
       <c r="B306" s="22" t="s">
-        <v>774</v>
+        <v>793</v>
       </c>
       <c r="C306" s="22" t="s">
-        <v>774</v>
+        <v>793</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="22" t="s">
-        <v>775</v>
+        <v>794</v>
       </c>
       <c r="B307" s="22" t="s">
-        <v>776</v>
+        <v>795</v>
       </c>
       <c r="C307" s="22" t="s">
-        <v>776</v>
+        <v>795</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="22" t="s">
-        <v>777</v>
+        <v>796</v>
       </c>
       <c r="B308" s="22" t="s">
-        <v>778</v>
+        <v>797</v>
       </c>
       <c r="C308" s="22" t="s">
-        <v>778</v>
+        <v>797</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="22" t="s">
-        <v>779</v>
+        <v>798</v>
       </c>
       <c r="B309" s="22" t="s">
-        <v>778</v>
+        <v>799</v>
       </c>
       <c r="C309" s="22" t="s">
-        <v>778</v>
+        <v>799</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="22" t="s">
-        <v>780</v>
+        <v>800</v>
       </c>
       <c r="B310" s="22" t="s">
-        <v>781</v>
+        <v>801</v>
       </c>
       <c r="C310" s="22" t="s">
-        <v>781</v>
+        <v>801</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="22" t="s">
-        <v>782</v>
+        <v>802</v>
       </c>
       <c r="B311" s="22" t="s">
-        <v>783</v>
+        <v>803</v>
       </c>
       <c r="C311" s="22" t="s">
-        <v>783</v>
+        <v>803</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="22" t="s">
-        <v>784</v>
+        <v>804</v>
       </c>
       <c r="B312" s="22" t="s">
-        <v>785</v>
+        <v>805</v>
       </c>
       <c r="C312" s="22" t="s">
-        <v>785</v>
+        <v>805</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="22" t="s">
-        <v>786</v>
+        <v>806</v>
       </c>
       <c r="B313" s="22" t="s">
-        <v>787</v>
+        <v>807</v>
       </c>
       <c r="C313" s="22" t="s">
-        <v>787</v>
+        <v>807</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="22" t="s">
-        <v>788</v>
+        <v>808</v>
       </c>
       <c r="B314" s="22" t="s">
-        <v>789</v>
+        <v>637</v>
       </c>
       <c r="C314" s="22" t="s">
-        <v>789</v>
+        <v>637</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="22" t="s">
-        <v>790</v>
+        <v>809</v>
       </c>
       <c r="B315" s="22" t="s">
-        <v>791</v>
+        <v>810</v>
       </c>
       <c r="C315" s="22" t="s">
-        <v>791</v>
+        <v>810</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="22" t="s">
-        <v>792</v>
+        <v>811</v>
       </c>
       <c r="B316" s="22" t="s">
-        <v>793</v>
+        <v>812</v>
       </c>
       <c r="C316" s="22" t="s">
-        <v>793</v>
+        <v>812</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="22" t="s">
-        <v>794</v>
+        <v>813</v>
       </c>
       <c r="B317" s="22" t="s">
-        <v>795</v>
+        <v>814</v>
       </c>
       <c r="C317" s="22" t="s">
-        <v>795</v>
+        <v>814</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="22" t="s">
-        <v>796</v>
+        <v>815</v>
       </c>
       <c r="B318" s="22" t="s">
-        <v>797</v>
+        <v>816</v>
       </c>
       <c r="C318" s="22" t="s">
-        <v>797</v>
+        <v>816</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="22" t="s">
-        <v>798</v>
+        <v>817</v>
       </c>
       <c r="B319" s="22" t="s">
-        <v>799</v>
+        <v>818</v>
       </c>
       <c r="C319" s="22" t="s">
-        <v>799</v>
+        <v>818</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="22" t="s">
-        <v>800</v>
+        <v>819</v>
       </c>
       <c r="B320" s="22" t="s">
-        <v>801</v>
+        <v>820</v>
       </c>
       <c r="C320" s="22" t="s">
-        <v>801</v>
+        <v>820</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="22" t="s">
-        <v>802</v>
+        <v>821</v>
       </c>
       <c r="B321" s="22" t="s">
-        <v>803</v>
+        <v>822</v>
       </c>
       <c r="C321" s="22" t="s">
-        <v>803</v>
+        <v>822</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="22" t="s">
-        <v>804</v>
+        <v>823</v>
       </c>
       <c r="B322" s="22" t="s">
-        <v>805</v>
+        <v>824</v>
       </c>
       <c r="C322" s="22" t="s">
-        <v>805</v>
+        <v>824</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="22" t="s">
-        <v>806</v>
+        <v>825</v>
       </c>
       <c r="B323" s="22" t="s">
-        <v>807</v>
+        <v>826</v>
       </c>
       <c r="C323" s="22" t="s">
-        <v>807</v>
+        <v>826</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="22" t="s">
-        <v>808</v>
+        <v>827</v>
       </c>
       <c r="B324" s="22" t="s">
-        <v>637</v>
+        <v>828</v>
       </c>
       <c r="C324" s="22" t="s">
-        <v>637</v>
+        <v>828</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="22" t="s">
-        <v>809</v>
+        <v>829</v>
       </c>
       <c r="B325" s="22" t="s">
-        <v>810</v>
+        <v>830</v>
       </c>
       <c r="C325" s="22" t="s">
-        <v>810</v>
+        <v>830</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="22" t="s">
-        <v>811</v>
+        <v>831</v>
       </c>
       <c r="B326" s="22" t="s">
-        <v>812</v>
+        <v>832</v>
       </c>
       <c r="C326" s="22" t="s">
-        <v>812</v>
+        <v>832</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="22" t="s">
-        <v>813</v>
+        <v>833</v>
       </c>
       <c r="B327" s="22" t="s">
-        <v>814</v>
+        <v>834</v>
       </c>
       <c r="C327" s="22" t="s">
-        <v>814</v>
+        <v>834</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="22" t="s">
-        <v>815</v>
+        <v>835</v>
       </c>
       <c r="B328" s="22" t="s">
-        <v>816</v>
+        <v>836</v>
       </c>
       <c r="C328" s="22" t="s">
-        <v>816</v>
+        <v>836</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="22" t="s">
-        <v>817</v>
+        <v>837</v>
       </c>
       <c r="B329" s="22" t="s">
-        <v>818</v>
+        <v>838</v>
       </c>
       <c r="C329" s="22" t="s">
-        <v>818</v>
+        <v>838</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="22" t="s">
-        <v>819</v>
+        <v>839</v>
       </c>
       <c r="B330" s="22" t="s">
-        <v>820</v>
+        <v>840</v>
       </c>
       <c r="C330" s="22" t="s">
-        <v>820</v>
+        <v>840</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="22" t="s">
-        <v>821</v>
+        <v>841</v>
       </c>
       <c r="B331" s="22" t="s">
-        <v>822</v>
+        <v>842</v>
       </c>
       <c r="C331" s="22" t="s">
-        <v>822</v>
+        <v>842</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="22" t="s">
-        <v>823</v>
+        <v>843</v>
       </c>
       <c r="B332" s="22" t="s">
-        <v>824</v>
+        <v>844</v>
       </c>
       <c r="C332" s="22" t="s">
-        <v>824</v>
+        <v>844</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="22" t="s">
-        <v>825</v>
+        <v>845</v>
       </c>
       <c r="B333" s="22" t="s">
-        <v>826</v>
+        <v>846</v>
       </c>
       <c r="C333" s="22" t="s">
-        <v>826</v>
+        <v>846</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="22" t="s">
-        <v>827</v>
+        <v>847</v>
       </c>
       <c r="B334" s="22" t="s">
-        <v>828</v>
+        <v>848</v>
       </c>
       <c r="C334" s="22" t="s">
-        <v>828</v>
+        <v>848</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="22" t="s">
-        <v>829</v>
+        <v>849</v>
       </c>
       <c r="B335" s="22" t="s">
-        <v>830</v>
+        <v>850</v>
       </c>
       <c r="C335" s="22" t="s">
-        <v>830</v>
+        <v>850</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="22" t="s">
-        <v>831</v>
+        <v>851</v>
       </c>
       <c r="B336" s="22" t="s">
-        <v>832</v>
+        <v>682</v>
       </c>
       <c r="C336" s="22" t="s">
-        <v>832</v>
+        <v>682</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="22" t="s">
-        <v>833</v>
+        <v>852</v>
       </c>
       <c r="B337" s="22" t="s">
-        <v>834</v>
+        <v>853</v>
       </c>
       <c r="C337" s="22" t="s">
-        <v>834</v>
+        <v>853</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="22" t="s">
-        <v>835</v>
+        <v>854</v>
       </c>
       <c r="B338" s="22" t="s">
-        <v>836</v>
+        <v>855</v>
       </c>
       <c r="C338" s="22" t="s">
-        <v>836</v>
+        <v>855</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="22" t="s">
-        <v>837</v>
+        <v>856</v>
       </c>
       <c r="B339" s="22" t="s">
-        <v>838</v>
+        <v>697</v>
       </c>
       <c r="C339" s="22" t="s">
-        <v>838</v>
+        <v>697</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="22" t="s">
-        <v>839</v>
+        <v>857</v>
       </c>
       <c r="B340" s="22" t="s">
-        <v>840</v>
+        <v>702</v>
       </c>
       <c r="C340" s="22" t="s">
-        <v>840</v>
+        <v>702</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="22" t="s">
-        <v>841</v>
+        <v>858</v>
       </c>
       <c r="B341" s="22" t="s">
-        <v>842</v>
+        <v>859</v>
       </c>
       <c r="C341" s="22" t="s">
-        <v>842</v>
+        <v>859</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="22" t="s">
-        <v>843</v>
+        <v>860</v>
       </c>
       <c r="B342" s="22" t="s">
-        <v>844</v>
+        <v>861</v>
       </c>
       <c r="C342" s="22" t="s">
-        <v>844</v>
+        <v>861</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="22" t="s">
-        <v>845</v>
+        <v>862</v>
       </c>
       <c r="B343" s="22" t="s">
-        <v>846</v>
+        <v>863</v>
       </c>
       <c r="C343" s="22" t="s">
-        <v>846</v>
+        <v>863</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="22" t="s">
-        <v>847</v>
+        <v>864</v>
       </c>
       <c r="B344" s="22" t="s">
-        <v>848</v>
+        <v>865</v>
       </c>
       <c r="C344" s="22" t="s">
-        <v>848</v>
+        <v>865</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="22" t="s">
-        <v>849</v>
+        <v>866</v>
       </c>
       <c r="B345" s="22" t="s">
-        <v>850</v>
+        <v>867</v>
       </c>
       <c r="C345" s="22" t="s">
-        <v>850</v>
+        <v>867</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="22" t="s">
-        <v>851</v>
+        <v>868</v>
       </c>
       <c r="B346" s="22" t="s">
-        <v>682</v>
+        <v>869</v>
       </c>
       <c r="C346" s="22" t="s">
-        <v>682</v>
+        <v>869</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="22" t="s">
-        <v>852</v>
+        <v>870</v>
       </c>
       <c r="B347" s="22" t="s">
-        <v>853</v>
+        <v>871</v>
       </c>
       <c r="C347" s="22" t="s">
-        <v>853</v>
+        <v>871</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="22" t="s">
-        <v>854</v>
+        <v>872</v>
       </c>
       <c r="B348" s="22" t="s">
-        <v>855</v>
+        <v>873</v>
       </c>
       <c r="C348" s="22" t="s">
-        <v>855</v>
+        <v>873</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="22" t="s">
-        <v>856</v>
+        <v>874</v>
       </c>
       <c r="B349" s="22" t="s">
-        <v>697</v>
+        <v>875</v>
       </c>
       <c r="C349" s="22" t="s">
-        <v>697</v>
+        <v>875</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="22" t="s">
-        <v>857</v>
+        <v>876</v>
       </c>
       <c r="B350" s="22" t="s">
-        <v>702</v>
+        <v>877</v>
       </c>
       <c r="C350" s="22" t="s">
-        <v>702</v>
+        <v>877</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="22" t="s">
-        <v>858</v>
+        <v>878</v>
       </c>
       <c r="B351" s="22" t="s">
-        <v>859</v>
+        <v>879</v>
       </c>
       <c r="C351" s="22" t="s">
-        <v>859</v>
+        <v>879</v>
       </c>
     </row>
     <row r="352">
-      <c r="A352" s="22" t="s">
-        <v>860</v>
-      </c>
-      <c r="B352" s="22" t="s">
-        <v>861</v>
-      </c>
-      <c r="C352" s="22" t="s">
-        <v>861</v>
+      <c r="A352" s="38" t="s">
+        <v>880</v>
+      </c>
+      <c r="B352" s="38" t="s">
+        <v>881</v>
+      </c>
+      <c r="C352" s="38" t="s">
+        <v>881</v>
       </c>
     </row>
     <row r="353">
-      <c r="A353" s="22" t="s">
-        <v>862</v>
-      </c>
-      <c r="B353" s="22" t="s">
-        <v>863</v>
-      </c>
-      <c r="C353" s="22" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="354">
-      <c r="A354" s="22" t="s">
-        <v>864</v>
-      </c>
-      <c r="B354" s="22" t="s">
-        <v>865</v>
-      </c>
-      <c r="C354" s="22" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="355">
-      <c r="A355" s="22" t="s">
-        <v>866</v>
-      </c>
-      <c r="B355" s="22" t="s">
-        <v>867</v>
-      </c>
-      <c r="C355" s="22" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="356">
-      <c r="A356" s="22" t="s">
-        <v>868</v>
-      </c>
-      <c r="B356" s="22" t="s">
-        <v>869</v>
-      </c>
-      <c r="C356" s="22" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="357">
-      <c r="A357" s="22" t="s">
-        <v>870</v>
-      </c>
-      <c r="B357" s="22" t="s">
-        <v>871</v>
-      </c>
-      <c r="C357" s="22" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="358">
-      <c r="A358" s="22" t="s">
-        <v>872</v>
-      </c>
-      <c r="B358" s="22" t="s">
-        <v>873</v>
-      </c>
-      <c r="C358" s="22" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="359">
-      <c r="A359" s="22" t="s">
-        <v>874</v>
-      </c>
-      <c r="B359" s="22" t="s">
-        <v>875</v>
-      </c>
-      <c r="C359" s="22" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="360">
-      <c r="A360" s="22" t="s">
-        <v>876</v>
-      </c>
-      <c r="B360" s="22" t="s">
-        <v>877</v>
-      </c>
-      <c r="C360" s="22" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="361">
-      <c r="A361" s="22" t="s">
-        <v>878</v>
-      </c>
-      <c r="B361" s="22" t="s">
-        <v>879</v>
-      </c>
-      <c r="C361" s="22" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="362">
-      <c r="A362" s="22"/>
-      <c r="B362" s="22"/>
-      <c r="C362" s="22"/>
+      <c r="A353" s="39" t="s">
+        <v>882</v>
+      </c>
+      <c r="B353" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C353" s="39" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B147"/>
-    <hyperlink r:id="rId2" ref="C147"/>
-    <hyperlink r:id="rId3" ref="B148"/>
-    <hyperlink r:id="rId4" ref="C148"/>
+    <hyperlink r:id="rId1" ref="B137"/>
+    <hyperlink r:id="rId2" ref="C137"/>
+    <hyperlink r:id="rId3" ref="B138"/>
+    <hyperlink r:id="rId4" ref="C138"/>
   </hyperlinks>
   <drawing r:id="rId5"/>
 </worksheet>

</xml_diff>

<commit_message>
RRP Ne Changes according to the New Changes
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Patrick-Codoid\Mobile_App_Code\MobileApp_SignOff\config\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Inlogic\Latest_clone_Happy_Path\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="MMH" sheetId="1" r:id="rId1"/>
@@ -200,9 +200,6 @@
   </si>
   <si>
     <t>DATA FOR PRESCRIPTION BY SENT SCRIPT TO PHARMACY</t>
-  </si>
-  <si>
-    <t>VM04Practice;Kevin Peterson;Send Script to Pharmacy;Find a pharmacy;Auckland;Auckland Central;Chemist Warehouse Auckland;48 Hours - Fee: NZ$;Panadol (Optizorb) 500mg Caplets;Repeat Medication Testing for Sent Script by Pharmacy;Chemist Warehouse Auckland</t>
   </si>
   <si>
     <t>VERIFICATION DATA FOR SENT SCRIPT TO PHARMACY</t>
@@ -1552,13 +1549,16 @@
     <t>Approved;Dr Sam Entwistle;VM03Location;Follow-up</t>
   </si>
   <si>
-    <t>Urgent/Same day - Fee: NZ$10.00 (Incl. GST);Next Day - Fee: NZ$20.00 (Incl. GST);48 Hours - Fee: NZ$30.00 (Incl. GST);72 Hours - Fee: NZ$40.00 (Incl. GST)</t>
-  </si>
-  <si>
     <t>REPLY MESSAGE</t>
   </si>
   <si>
     <t>Reply Message_RANDOM;Body:Reply Message_RANDOM;2;3;4;Received Msg Testing_RANDOM</t>
+  </si>
+  <si>
+    <t>VM04Practice;Kevin Peterson;Send Script to Pharmacy;Select from my saved list;Auckland;Auckland Central;Chemist Warehouse Auckland;48 Hours - Fee: NZ$;Panadol (Optizorb) 500mg Caplets;Repeat Medication Testing for Sent Script by Pharmacy;Chemist Warehouse Auckland</t>
+  </si>
+  <si>
+    <t>Urgent/Same day - Fee: NZ$101.00 (Incl. GST);Next Day - Fee: NZ$102.00 (Incl. GST);48 Hours - Fee: NZ$103.00 (Incl. GST);72 Hours - Fee: NZ$104.00 (Incl. GST)</t>
   </si>
 </sst>
 </file>
@@ -1952,16 +1952,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C178" workbookViewId="0">
-      <selection activeCell="C193" sqref="C193"/>
+    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="69.5703125" customWidth="1"/>
-    <col min="2" max="2" width="161.42578125" customWidth="1"/>
-    <col min="3" max="3" width="161.140625" customWidth="1"/>
-    <col min="4" max="23" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="69.54296875" customWidth="1"/>
+    <col min="2" max="2" width="161.453125" customWidth="1"/>
+    <col min="3" max="3" width="161.1796875" customWidth="1"/>
+    <col min="4" max="23" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" customHeight="1">
@@ -2003,10 +2003,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -3649,10 +3649,10 @@
         <v>59</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>60</v>
+        <v>511</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>60</v>
+        <v>511</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -3680,13 +3680,13 @@
     </row>
     <row r="54" spans="1:26" ht="13.5" customHeight="1">
       <c r="A54" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="C54" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -3714,7 +3714,7 @@
     </row>
     <row r="55" spans="1:26" ht="13.5" customHeight="1">
       <c r="A55" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -3800,13 +3800,13 @@
     </row>
     <row r="58" spans="1:26" ht="13.5" customHeight="1">
       <c r="A58" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="C58" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -3834,13 +3834,13 @@
     </row>
     <row r="59" spans="1:26" ht="13.5" customHeight="1">
       <c r="A59" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="C59" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -3868,7 +3868,7 @@
     </row>
     <row r="60" spans="1:26" ht="13.5" customHeight="1">
       <c r="A60" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -3954,13 +3954,13 @@
     </row>
     <row r="63" spans="1:26" ht="13.5" customHeight="1">
       <c r="A63" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -3988,13 +3988,13 @@
     </row>
     <row r="64" spans="1:26" ht="13.5" customHeight="1">
       <c r="A64" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -4078,13 +4078,13 @@
     </row>
     <row r="67" spans="1:26" ht="13.5" customHeight="1">
       <c r="A67" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -4112,13 +4112,13 @@
     </row>
     <row r="68" spans="1:26" ht="13.5" customHeight="1">
       <c r="A68" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -4202,13 +4202,13 @@
     </row>
     <row r="71" spans="1:26" ht="13.5" customHeight="1">
       <c r="A71" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="C71" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -4236,13 +4236,13 @@
     </row>
     <row r="72" spans="1:26" ht="13.5" customHeight="1">
       <c r="A72" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="C72" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -4270,13 +4270,13 @@
     </row>
     <row r="73" spans="1:26" ht="13.5" customHeight="1">
       <c r="A73" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="C73" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -4304,13 +4304,13 @@
     </row>
     <row r="74" spans="1:26" ht="13.5" customHeight="1">
       <c r="A74" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -4394,7 +4394,7 @@
     </row>
     <row r="77" spans="1:26" ht="13.5" customHeight="1">
       <c r="A77" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>46</v>
@@ -4428,7 +4428,7 @@
     </row>
     <row r="78" spans="1:26" ht="13.5" customHeight="1">
       <c r="A78" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>7</v>
@@ -4490,13 +4490,13 @@
     </row>
     <row r="80" spans="1:26" ht="13.5" customHeight="1">
       <c r="A80" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B80" s="8" t="s">
-        <v>83</v>
-      </c>
       <c r="C80" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -4524,13 +4524,13 @@
     </row>
     <row r="81" spans="1:26" ht="13.5" customHeight="1">
       <c r="A81" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B81" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B81" s="8" t="s">
-        <v>85</v>
-      </c>
       <c r="C81" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -4558,13 +4558,13 @@
     </row>
     <row r="82" spans="1:26" ht="13.5" customHeight="1">
       <c r="A82" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B82" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="C82" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -4592,13 +4592,13 @@
     </row>
     <row r="83" spans="1:26" ht="13.5" customHeight="1">
       <c r="A83" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B83" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="C83" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -4626,13 +4626,13 @@
     </row>
     <row r="84" spans="1:26" ht="13.5" customHeight="1">
       <c r="A84" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B84" s="8" t="s">
-        <v>91</v>
-      </c>
       <c r="C84" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -4660,13 +4660,13 @@
     </row>
     <row r="85" spans="1:26" ht="13.5" customHeight="1">
       <c r="A85" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B85" s="8" t="s">
-        <v>93</v>
-      </c>
       <c r="C85" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -4694,13 +4694,13 @@
     </row>
     <row r="86" spans="1:26" ht="13.5" customHeight="1">
       <c r="A86" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="C86" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -4728,13 +4728,13 @@
     </row>
     <row r="87" spans="1:26" ht="13.5" customHeight="1">
       <c r="A87" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C87" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -4762,13 +4762,13 @@
     </row>
     <row r="88" spans="1:26" ht="13.5" customHeight="1">
       <c r="A88" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="C88" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -4796,13 +4796,13 @@
     </row>
     <row r="89" spans="1:26" ht="13.5" customHeight="1">
       <c r="A89" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="C89" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -4830,13 +4830,13 @@
     </row>
     <row r="90" spans="1:26" ht="13.5" customHeight="1">
       <c r="A90" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="C90" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -4864,13 +4864,13 @@
     </row>
     <row r="91" spans="1:26" ht="13.5" customHeight="1">
       <c r="A91" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B91" s="8" t="s">
-        <v>105</v>
-      </c>
       <c r="C91" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -4898,13 +4898,13 @@
     </row>
     <row r="92" spans="1:26" ht="13.5" customHeight="1">
       <c r="A92" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B92" s="8" t="s">
-        <v>107</v>
-      </c>
       <c r="C92" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -4932,13 +4932,13 @@
     </row>
     <row r="93" spans="1:26" ht="13.5" customHeight="1">
       <c r="A93" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B93" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B93" s="8" t="s">
-        <v>109</v>
-      </c>
       <c r="C93" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -4966,13 +4966,13 @@
     </row>
     <row r="94" spans="1:26" ht="13.5" customHeight="1">
       <c r="A94" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B94" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>111</v>
-      </c>
       <c r="C94" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -5000,13 +5000,13 @@
     </row>
     <row r="95" spans="1:26" ht="13.5" customHeight="1">
       <c r="A95" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B95" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B95" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="C95" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -5034,13 +5034,13 @@
     </row>
     <row r="96" spans="1:26" ht="13.5" customHeight="1">
       <c r="A96" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="C96" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -5068,13 +5068,13 @@
     </row>
     <row r="97" spans="1:26" ht="13.5" customHeight="1">
       <c r="A97" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="C97" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -5102,13 +5102,13 @@
     </row>
     <row r="98" spans="1:26" ht="13.5" customHeight="1">
       <c r="A98" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B98" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="C98" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -5136,13 +5136,13 @@
     </row>
     <row r="99" spans="1:26" ht="13.5" customHeight="1">
       <c r="A99" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B99" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B99" s="9" t="s">
-        <v>121</v>
-      </c>
       <c r="C99" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -5170,13 +5170,13 @@
     </row>
     <row r="100" spans="1:26" ht="13.5" customHeight="1">
       <c r="A100" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="C100" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -5204,13 +5204,13 @@
     </row>
     <row r="101" spans="1:26" ht="13.5" customHeight="1">
       <c r="A101" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="C101" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -5238,13 +5238,13 @@
     </row>
     <row r="102" spans="1:26" ht="13.5" customHeight="1">
       <c r="A102" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B102" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B102" s="9" t="s">
-        <v>127</v>
-      </c>
       <c r="C102" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
@@ -5272,13 +5272,13 @@
     </row>
     <row r="103" spans="1:26" ht="13.5" customHeight="1">
       <c r="A103" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="C103" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
@@ -5306,13 +5306,13 @@
     </row>
     <row r="104" spans="1:26" ht="13.5" customHeight="1">
       <c r="A104" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B104" s="8" t="s">
-        <v>131</v>
-      </c>
       <c r="C104" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
@@ -5340,13 +5340,13 @@
     </row>
     <row r="105" spans="1:26" ht="13.5" customHeight="1">
       <c r="A105" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B105" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B105" s="8" t="s">
-        <v>133</v>
-      </c>
       <c r="C105" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
@@ -5374,13 +5374,13 @@
     </row>
     <row r="106" spans="1:26" ht="13.5" customHeight="1">
       <c r="A106" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B106" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B106" s="8" t="s">
-        <v>135</v>
-      </c>
       <c r="C106" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
@@ -5408,13 +5408,13 @@
     </row>
     <row r="107" spans="1:26" ht="13.5" customHeight="1">
       <c r="A107" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B107" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="C107" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
@@ -5442,13 +5442,13 @@
     </row>
     <row r="108" spans="1:26" ht="13.5" customHeight="1">
       <c r="A108" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B108" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B108" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="C108" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
@@ -5476,13 +5476,13 @@
     </row>
     <row r="109" spans="1:26" ht="13.5" customHeight="1">
       <c r="A109" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B109" s="8" t="s">
-        <v>141</v>
-      </c>
       <c r="C109" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
@@ -5510,13 +5510,13 @@
     </row>
     <row r="110" spans="1:26" ht="13.5" customHeight="1">
       <c r="A110" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B110" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B110" s="8" t="s">
-        <v>143</v>
-      </c>
       <c r="C110" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
@@ -5544,13 +5544,13 @@
     </row>
     <row r="111" spans="1:26" ht="13.5" customHeight="1">
       <c r="A111" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="C111" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
@@ -5578,13 +5578,13 @@
     </row>
     <row r="112" spans="1:26" ht="13.5" customHeight="1">
       <c r="A112" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="C112" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
@@ -5612,13 +5612,13 @@
     </row>
     <row r="113" spans="1:26" ht="13.5" customHeight="1">
       <c r="A113" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B113" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B113" s="9" t="s">
-        <v>149</v>
-      </c>
       <c r="C113" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
@@ -5646,13 +5646,13 @@
     </row>
     <row r="114" spans="1:26" ht="13.5" customHeight="1">
       <c r="A114" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B114" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B114" s="8" t="s">
-        <v>151</v>
-      </c>
       <c r="C114" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
@@ -5680,13 +5680,13 @@
     </row>
     <row r="115" spans="1:26" ht="13.5" customHeight="1">
       <c r="A115" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="C115" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
@@ -5714,13 +5714,13 @@
     </row>
     <row r="116" spans="1:26" ht="13.5" customHeight="1">
       <c r="A116" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B116" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B116" s="8" t="s">
-        <v>155</v>
-      </c>
       <c r="C116" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
@@ -5748,13 +5748,13 @@
     </row>
     <row r="117" spans="1:26" ht="13.5" customHeight="1">
       <c r="A117" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B117" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B117" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="C117" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
@@ -5782,13 +5782,13 @@
     </row>
     <row r="118" spans="1:26" ht="13.5" customHeight="1">
       <c r="A118" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B118" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B118" s="8" t="s">
-        <v>159</v>
-      </c>
       <c r="C118" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
@@ -5816,13 +5816,13 @@
     </row>
     <row r="119" spans="1:26" ht="13.5" customHeight="1">
       <c r="A119" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="C119" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
@@ -5850,13 +5850,13 @@
     </row>
     <row r="120" spans="1:26" ht="13.5" customHeight="1">
       <c r="A120" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B120" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B120" s="8" t="s">
-        <v>163</v>
-      </c>
       <c r="C120" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
@@ -5884,13 +5884,13 @@
     </row>
     <row r="121" spans="1:26" ht="13.5" customHeight="1">
       <c r="A121" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="C121" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -5918,13 +5918,13 @@
     </row>
     <row r="122" spans="1:26" ht="13.5" customHeight="1">
       <c r="A122" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B122" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="C122" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
@@ -5952,13 +5952,13 @@
     </row>
     <row r="123" spans="1:26" ht="13.5" customHeight="1">
       <c r="A123" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B123" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="C123" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
@@ -6014,13 +6014,13 @@
     </row>
     <row r="125" spans="1:26" ht="13.5" customHeight="1">
       <c r="A125" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B125" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B125" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="C125" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
@@ -6076,13 +6076,13 @@
     </row>
     <row r="127" spans="1:26" ht="13.5" customHeight="1">
       <c r="A127" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="C127" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
@@ -6110,13 +6110,13 @@
     </row>
     <row r="128" spans="1:26" ht="13.5" customHeight="1">
       <c r="A128" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B128" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B128" s="8" t="s">
-        <v>175</v>
-      </c>
       <c r="C128" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
@@ -6144,13 +6144,13 @@
     </row>
     <row r="129" spans="1:26" ht="13.5" customHeight="1">
       <c r="A129" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B129" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="B129" s="11" t="s">
-        <v>177</v>
-      </c>
       <c r="C129" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
@@ -6178,13 +6178,13 @@
     </row>
     <row r="130" spans="1:26" ht="13.5" customHeight="1">
       <c r="A130" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B130" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="B130" s="11" t="s">
-        <v>179</v>
-      </c>
       <c r="C130" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
@@ -6212,13 +6212,13 @@
     </row>
     <row r="131" spans="1:26" ht="13.5" customHeight="1">
       <c r="A131" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B131" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B131" s="11" t="s">
-        <v>181</v>
-      </c>
       <c r="C131" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
@@ -6246,13 +6246,13 @@
     </row>
     <row r="132" spans="1:26" ht="13.5" customHeight="1">
       <c r="A132" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B132" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B132" s="12" t="s">
-        <v>183</v>
-      </c>
       <c r="C132" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
@@ -6280,13 +6280,13 @@
     </row>
     <row r="133" spans="1:26" ht="13.5" customHeight="1">
       <c r="A133" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B133" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="C133" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
@@ -6314,13 +6314,13 @@
     </row>
     <row r="134" spans="1:26" ht="13.5" customHeight="1">
       <c r="A134" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="C134" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
@@ -6348,13 +6348,13 @@
     </row>
     <row r="135" spans="1:26" ht="13.5" customHeight="1">
       <c r="A135" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B135" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="C135" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
@@ -6382,13 +6382,13 @@
     </row>
     <row r="136" spans="1:26" ht="13.5" customHeight="1">
       <c r="A136" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="C136" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
@@ -6416,13 +6416,13 @@
     </row>
     <row r="137" spans="1:26" ht="13.5" customHeight="1">
       <c r="A137" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B137" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B137" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="C137" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
@@ -6450,13 +6450,13 @@
     </row>
     <row r="138" spans="1:26" ht="13.5" customHeight="1">
       <c r="A138" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="C138" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
@@ -6484,13 +6484,13 @@
     </row>
     <row r="139" spans="1:26" ht="13.5" customHeight="1">
       <c r="A139" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="C139" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
@@ -6546,13 +6546,13 @@
     </row>
     <row r="141" spans="1:26" ht="13.5" customHeight="1">
       <c r="A141" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="C141" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
@@ -6580,13 +6580,13 @@
     </row>
     <row r="142" spans="1:26" ht="13.5" customHeight="1">
       <c r="A142" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B142" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="C142" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
@@ -6614,13 +6614,13 @@
     </row>
     <row r="143" spans="1:26" ht="13.5" customHeight="1">
       <c r="A143" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B143" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="C143" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
@@ -6648,13 +6648,13 @@
     </row>
     <row r="144" spans="1:26" ht="13.5" customHeight="1">
       <c r="A144" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B144" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="C144" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
@@ -6682,13 +6682,13 @@
     </row>
     <row r="145" spans="1:26" ht="13.5" customHeight="1">
       <c r="A145" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B145" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="C145" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
@@ -6716,13 +6716,13 @@
     </row>
     <row r="146" spans="1:26" ht="13.5" customHeight="1">
       <c r="A146" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
@@ -6750,13 +6750,13 @@
     </row>
     <row r="147" spans="1:26" ht="13.5" customHeight="1">
       <c r="A147" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -6784,13 +6784,13 @@
     </row>
     <row r="148" spans="1:26" ht="13.5" customHeight="1">
       <c r="A148" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="C148" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
@@ -6818,13 +6818,13 @@
     </row>
     <row r="149" spans="1:26" ht="13.5" customHeight="1">
       <c r="A149" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="C149" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
@@ -6852,13 +6852,13 @@
     </row>
     <row r="150" spans="1:26" ht="13.5" customHeight="1">
       <c r="A150" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="C150" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
@@ -6886,13 +6886,13 @@
     </row>
     <row r="151" spans="1:26" ht="13.5" customHeight="1">
       <c r="A151" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B151" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="B151" s="8" t="s">
-        <v>215</v>
-      </c>
       <c r="C151" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
@@ -6920,13 +6920,13 @@
     </row>
     <row r="152" spans="1:26" ht="13.5" customHeight="1">
       <c r="A152" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="C152" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
@@ -6954,13 +6954,13 @@
     </row>
     <row r="153" spans="1:26" ht="13.5" customHeight="1">
       <c r="A153" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B153" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="C153" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
@@ -6988,13 +6988,13 @@
     </row>
     <row r="154" spans="1:26" ht="13.5" customHeight="1">
       <c r="A154" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B154" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B154" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="C154" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
@@ -7022,13 +7022,13 @@
     </row>
     <row r="155" spans="1:26" ht="13.5" customHeight="1">
       <c r="A155" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B155" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="C155" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -7112,13 +7112,13 @@
     </row>
     <row r="158" spans="1:26" ht="13.5" customHeight="1">
       <c r="A158" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B158" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="B158" s="13" t="s">
-        <v>225</v>
-      </c>
       <c r="C158" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D158" s="8"/>
       <c r="E158" s="8"/>
@@ -7146,13 +7146,13 @@
     </row>
     <row r="159" spans="1:26" ht="13.5" customHeight="1">
       <c r="A159" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B159" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="B159" s="15" t="s">
-        <v>227</v>
-      </c>
       <c r="C159" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D159" s="8"/>
       <c r="E159" s="8"/>
@@ -7180,7 +7180,7 @@
     </row>
     <row r="160" spans="1:26" ht="13.5" customHeight="1">
       <c r="A160" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B160" s="8" t="s">
         <v>7</v>
@@ -7214,13 +7214,13 @@
     </row>
     <row r="161" spans="1:26" ht="13.5" customHeight="1">
       <c r="A161" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B161" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="B161" s="8" t="s">
-        <v>230</v>
-      </c>
       <c r="C161" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
@@ -7248,13 +7248,13 @@
     </row>
     <row r="162" spans="1:26" ht="13.5" customHeight="1">
       <c r="A162" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B162" s="1" t="s">
-        <v>232</v>
-      </c>
       <c r="C162" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
@@ -7282,13 +7282,13 @@
     </row>
     <row r="163" spans="1:26" ht="13.5" customHeight="1">
       <c r="A163" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="B163" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="B163" s="8" t="s">
-        <v>234</v>
-      </c>
       <c r="C163" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
@@ -7316,13 +7316,13 @@
     </row>
     <row r="164" spans="1:26" ht="13.5" customHeight="1">
       <c r="A164" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B164" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B164" s="4" t="s">
-        <v>236</v>
-      </c>
       <c r="C164" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
@@ -7350,13 +7350,13 @@
     </row>
     <row r="165" spans="1:26" ht="13.5" customHeight="1">
       <c r="A165" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B165" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="C165" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
@@ -7384,13 +7384,13 @@
     </row>
     <row r="166" spans="1:26" ht="13.5" customHeight="1">
       <c r="A166" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
@@ -7418,13 +7418,13 @@
     </row>
     <row r="167" spans="1:26" ht="13.5" customHeight="1">
       <c r="A167" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B167" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="C167" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
@@ -7536,7 +7536,7 @@
     </row>
     <row r="171" spans="1:26" ht="13.5" customHeight="1">
       <c r="A171" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B171" s="13" t="s">
         <v>5</v>
@@ -7570,7 +7570,7 @@
     </row>
     <row r="172" spans="1:26" ht="13.5" customHeight="1">
       <c r="A172" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B172" s="5" t="s">
         <v>7</v>
@@ -7604,13 +7604,13 @@
     </row>
     <row r="173" spans="1:26" ht="13.5" customHeight="1">
       <c r="A173" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B173" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B173" s="5" t="s">
-        <v>245</v>
-      </c>
       <c r="C173" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
@@ -7638,13 +7638,13 @@
     </row>
     <row r="174" spans="1:26" ht="13.5" customHeight="1">
       <c r="A174" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B174" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="B174" s="8" t="s">
-        <v>247</v>
-      </c>
       <c r="C174" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
@@ -7672,13 +7672,13 @@
     </row>
     <row r="175" spans="1:26" ht="13.5" customHeight="1">
       <c r="A175" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B175" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B175" s="8" t="s">
-        <v>249</v>
-      </c>
       <c r="C175" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
@@ -7706,7 +7706,7 @@
     </row>
     <row r="176" spans="1:26" ht="13.5" customHeight="1">
       <c r="A176" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
@@ -7736,7 +7736,7 @@
     </row>
     <row r="177" spans="1:26" ht="13.5" customHeight="1">
       <c r="A177" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
@@ -7766,13 +7766,13 @@
     </row>
     <row r="178" spans="1:26" ht="13.5" customHeight="1">
       <c r="A178" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B178" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="B178" s="8" t="s">
-        <v>253</v>
-      </c>
       <c r="C178" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D178" s="1"/>
       <c r="E178" s="1"/>
@@ -7800,13 +7800,13 @@
     </row>
     <row r="179" spans="1:26" ht="13.5" customHeight="1">
       <c r="A179" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B179" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="B179" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="C179" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
@@ -7862,13 +7862,13 @@
     </row>
     <row r="181" spans="1:26" ht="13.5" customHeight="1">
       <c r="A181" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B181" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="B181" s="8" t="s">
-        <v>257</v>
-      </c>
       <c r="C181" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D181" s="1"/>
       <c r="E181" s="1"/>
@@ -7897,10 +7897,10 @@
     <row r="182" spans="1:26" ht="13.5" customHeight="1">
       <c r="A182" s="14"/>
       <c r="B182" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D182" s="1"/>
       <c r="E182" s="1"/>
@@ -7928,13 +7928,13 @@
     </row>
     <row r="183" spans="1:26" ht="13.5" customHeight="1">
       <c r="A183" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="B183" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="B183" s="17" t="s">
-        <v>260</v>
-      </c>
       <c r="C183" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D183" s="1"/>
       <c r="E183" s="1"/>
@@ -7962,13 +7962,13 @@
     </row>
     <row r="184" spans="1:26" ht="13.5" customHeight="1">
       <c r="A184" s="14" t="s">
+        <v>493</v>
+      </c>
+      <c r="B184" s="8" t="s">
         <v>494</v>
       </c>
-      <c r="B184" s="8" t="s">
-        <v>495</v>
-      </c>
       <c r="C184" s="8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D184" s="1"/>
       <c r="E184" s="1"/>
@@ -7996,13 +7996,13 @@
     </row>
     <row r="185" spans="1:26" ht="13.5" customHeight="1">
       <c r="A185" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B185" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="B185" s="8" t="s">
-        <v>262</v>
-      </c>
       <c r="C185" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D185" s="1"/>
       <c r="E185" s="1"/>
@@ -8030,13 +8030,13 @@
     </row>
     <row r="186" spans="1:26" ht="13.5" customHeight="1">
       <c r="A186" s="14" t="s">
+        <v>495</v>
+      </c>
+      <c r="B186" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="B186" s="1" t="s">
-        <v>497</v>
-      </c>
       <c r="C186" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D186" s="1"/>
       <c r="E186" s="1"/>
@@ -8064,13 +8064,13 @@
     </row>
     <row r="187" spans="1:26" ht="13.5" customHeight="1">
       <c r="A187" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="B187" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="B187" s="8" t="s">
-        <v>264</v>
-      </c>
       <c r="C187" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D187" s="1"/>
       <c r="E187" s="1"/>
@@ -8126,13 +8126,13 @@
     </row>
     <row r="189" spans="1:26" ht="13.5" customHeight="1">
       <c r="A189" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="B189" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="B189" s="8" t="s">
-        <v>499</v>
-      </c>
       <c r="C189" s="8" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D189" s="1"/>
       <c r="E189" s="1"/>
@@ -8160,13 +8160,13 @@
     </row>
     <row r="190" spans="1:26" ht="13.5" customHeight="1">
       <c r="A190" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B190" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="B190" s="8" t="s">
-        <v>266</v>
-      </c>
       <c r="C190" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D190" s="1"/>
       <c r="E190" s="1"/>
@@ -8194,13 +8194,13 @@
     </row>
     <row r="191" spans="1:26" ht="13.5" customHeight="1">
       <c r="A191" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B191" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="B191" s="8" t="s">
-        <v>227</v>
-      </c>
       <c r="C191" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D191" s="1"/>
       <c r="E191" s="1"/>
@@ -8256,13 +8256,13 @@
     </row>
     <row r="193" spans="1:26" ht="13.5" customHeight="1">
       <c r="A193" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B193" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D193" s="1"/>
       <c r="E193" s="1"/>
@@ -8346,13 +8346,13 @@
     </row>
     <row r="196" spans="1:26" ht="13.5" customHeight="1">
       <c r="A196" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B196" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="B196" s="8" t="s">
-        <v>268</v>
-      </c>
       <c r="C196" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D196" s="1"/>
       <c r="E196" s="1"/>
@@ -8380,13 +8380,13 @@
     </row>
     <row r="197" spans="1:26" ht="13.5" customHeight="1">
       <c r="A197" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B197" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B197" s="1" t="s">
-        <v>270</v>
-      </c>
       <c r="C197" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D197" s="1"/>
       <c r="E197" s="1"/>
@@ -8414,13 +8414,13 @@
     </row>
     <row r="198" spans="1:26" ht="13.5" customHeight="1">
       <c r="A198" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B198" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B198" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="C198" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D198" s="1"/>
       <c r="E198" s="1"/>
@@ -8448,13 +8448,13 @@
     </row>
     <row r="199" spans="1:26" ht="13.5" customHeight="1">
       <c r="A199" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B199" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B199" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="C199" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D199" s="1"/>
       <c r="E199" s="1"/>
@@ -8482,13 +8482,13 @@
     </row>
     <row r="200" spans="1:26" ht="13.5" customHeight="1">
       <c r="A200" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B200" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B200" s="1" t="s">
-        <v>276</v>
-      </c>
       <c r="C200" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D200" s="1"/>
       <c r="E200" s="1"/>
@@ -8516,13 +8516,13 @@
     </row>
     <row r="201" spans="1:26" ht="13.5" customHeight="1">
       <c r="A201" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B201" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B201" s="1" t="s">
-        <v>278</v>
-      </c>
       <c r="C201" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D201" s="1"/>
       <c r="E201" s="1"/>
@@ -8550,13 +8550,13 @@
     </row>
     <row r="202" spans="1:26" ht="13.5" customHeight="1">
       <c r="A202" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B202" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B202" s="1" t="s">
-        <v>280</v>
-      </c>
       <c r="C202" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D202" s="1"/>
       <c r="E202" s="1"/>
@@ -8584,13 +8584,13 @@
     </row>
     <row r="203" spans="1:26" ht="13.5" customHeight="1">
       <c r="A203" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B203" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B203" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="C203" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D203" s="1"/>
       <c r="E203" s="1"/>
@@ -8618,13 +8618,13 @@
     </row>
     <row r="204" spans="1:26" ht="13.5" customHeight="1">
       <c r="A204" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B204" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B204" s="1" t="s">
-        <v>284</v>
-      </c>
       <c r="C204" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D204" s="1"/>
       <c r="E204" s="1"/>
@@ -8652,13 +8652,13 @@
     </row>
     <row r="205" spans="1:26" ht="13.5" customHeight="1">
       <c r="A205" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B205" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B205" s="1" t="s">
-        <v>286</v>
-      </c>
       <c r="C205" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D205" s="1"/>
       <c r="E205" s="1"/>
@@ -8686,13 +8686,13 @@
     </row>
     <row r="206" spans="1:26" ht="13.5" customHeight="1">
       <c r="A206" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B206" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B206" s="1" t="s">
-        <v>288</v>
-      </c>
       <c r="C206" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>
@@ -8720,13 +8720,13 @@
     </row>
     <row r="207" spans="1:26" ht="13.5" customHeight="1">
       <c r="A207" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B207" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B207" s="1" t="s">
-        <v>290</v>
-      </c>
       <c r="C207" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D207" s="1"/>
       <c r="E207" s="1"/>
@@ -8754,13 +8754,13 @@
     </row>
     <row r="208" spans="1:26" ht="13.5" customHeight="1">
       <c r="A208" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B208" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="B208" s="10" t="s">
-        <v>292</v>
-      </c>
       <c r="C208" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D208" s="1"/>
       <c r="E208" s="1"/>
@@ -8788,13 +8788,13 @@
     </row>
     <row r="209" spans="1:26" ht="13.5" customHeight="1">
       <c r="A209" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B209" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B209" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="C209" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D209" s="1"/>
       <c r="E209" s="1"/>
@@ -8822,13 +8822,13 @@
     </row>
     <row r="210" spans="1:26" ht="13.5" customHeight="1">
       <c r="A210" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B210" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B210" s="1" t="s">
-        <v>296</v>
-      </c>
       <c r="C210" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D210" s="1"/>
       <c r="E210" s="1"/>
@@ -8856,13 +8856,13 @@
     </row>
     <row r="211" spans="1:26" ht="13.5" customHeight="1">
       <c r="A211" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B211" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B211" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="C211" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D211" s="1"/>
       <c r="E211" s="1"/>
@@ -8890,13 +8890,13 @@
     </row>
     <row r="212" spans="1:26" ht="13.5" customHeight="1">
       <c r="A212" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B212" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="B212" s="10" t="s">
-        <v>300</v>
-      </c>
       <c r="C212" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D212" s="1"/>
       <c r="E212" s="1"/>
@@ -8924,13 +8924,13 @@
     </row>
     <row r="213" spans="1:26" ht="13.5" customHeight="1">
       <c r="A213" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B213" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B213" s="1" t="s">
-        <v>302</v>
-      </c>
       <c r="C213" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D213" s="1"/>
       <c r="E213" s="1"/>
@@ -8958,13 +8958,13 @@
     </row>
     <row r="214" spans="1:26" ht="13.5" customHeight="1">
       <c r="A214" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D214" s="1"/>
       <c r="E214" s="1"/>
@@ -8992,13 +8992,13 @@
     </row>
     <row r="215" spans="1:26" ht="13.5" customHeight="1">
       <c r="A215" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D215" s="1"/>
       <c r="E215" s="1"/>
@@ -9026,13 +9026,13 @@
     </row>
     <row r="216" spans="1:26" ht="13.5" customHeight="1">
       <c r="A216" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D216" s="1"/>
       <c r="E216" s="1"/>
@@ -9060,13 +9060,13 @@
     </row>
     <row r="217" spans="1:26" ht="13.5" customHeight="1">
       <c r="A217" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B217" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="B217" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="C217" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D217" s="1"/>
       <c r="E217" s="1"/>
@@ -9094,13 +9094,13 @@
     </row>
     <row r="218" spans="1:26" ht="13.5" customHeight="1">
       <c r="A218" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B218" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B218" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="C218" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D218" s="1"/>
       <c r="E218" s="1"/>
@@ -9128,13 +9128,13 @@
     </row>
     <row r="219" spans="1:26" ht="13.5" customHeight="1">
       <c r="A219" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B219" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="B219" s="11" t="s">
-        <v>311</v>
-      </c>
       <c r="C219" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D219" s="1"/>
       <c r="E219" s="1"/>
@@ -9162,13 +9162,13 @@
     </row>
     <row r="220" spans="1:26" ht="13.5" customHeight="1">
       <c r="A220" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B220" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C220" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D220" s="1"/>
       <c r="E220" s="1"/>
@@ -9196,13 +9196,13 @@
     </row>
     <row r="221" spans="1:26" ht="13.5" customHeight="1">
       <c r="A221" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B221" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B221" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="C221" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D221" s="1"/>
       <c r="E221" s="1"/>
@@ -9230,13 +9230,13 @@
     </row>
     <row r="222" spans="1:26" ht="13.5" customHeight="1">
       <c r="A222" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B222" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="B222" s="12" t="s">
-        <v>316</v>
-      </c>
       <c r="C222" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D222" s="1"/>
       <c r="E222" s="1"/>
@@ -9264,13 +9264,13 @@
     </row>
     <row r="223" spans="1:26" ht="13.5" customHeight="1">
       <c r="A223" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B223" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="B223" s="11" t="s">
-        <v>318</v>
-      </c>
       <c r="C223" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D223" s="1"/>
       <c r="E223" s="1"/>
@@ -9298,13 +9298,13 @@
     </row>
     <row r="224" spans="1:26" ht="13.5" customHeight="1">
       <c r="A224" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B224" s="18" t="s">
         <v>319</v>
       </c>
-      <c r="B224" s="18" t="s">
-        <v>320</v>
-      </c>
       <c r="C224" s="18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D224" s="1"/>
       <c r="E224" s="1"/>
@@ -9332,13 +9332,13 @@
     </row>
     <row r="225" spans="1:26" ht="13.5" customHeight="1">
       <c r="A225" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B225" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B225" s="1" t="s">
-        <v>322</v>
-      </c>
       <c r="C225" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D225" s="1"/>
       <c r="E225" s="1"/>
@@ -9366,13 +9366,13 @@
     </row>
     <row r="226" spans="1:26" ht="13.5" customHeight="1">
       <c r="A226" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B226" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="B226" s="11" t="s">
-        <v>324</v>
-      </c>
       <c r="C226" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D226" s="1"/>
       <c r="E226" s="1"/>
@@ -9400,13 +9400,13 @@
     </row>
     <row r="227" spans="1:26" ht="13.5" customHeight="1">
       <c r="A227" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B227" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B227" s="1" t="s">
-        <v>326</v>
-      </c>
       <c r="C227" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D227" s="1"/>
       <c r="E227" s="1"/>
@@ -9434,13 +9434,13 @@
     </row>
     <row r="228" spans="1:26" ht="13.5" customHeight="1">
       <c r="A228" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B228" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C228" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D228" s="1"/>
       <c r="E228" s="1"/>
@@ -9468,13 +9468,13 @@
     </row>
     <row r="229" spans="1:26" ht="13.5" customHeight="1">
       <c r="A229" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B229" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="B229" s="1" t="s">
-        <v>329</v>
-      </c>
       <c r="C229" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D229" s="1"/>
       <c r="E229" s="1"/>
@@ -9502,13 +9502,13 @@
     </row>
     <row r="230" spans="1:26" ht="13.5" customHeight="1">
       <c r="A230" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B230" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="B230" s="12" t="s">
-        <v>331</v>
-      </c>
       <c r="C230" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D230" s="1"/>
       <c r="E230" s="1"/>
@@ -9536,13 +9536,13 @@
     </row>
     <row r="231" spans="1:26" ht="13.5" customHeight="1">
       <c r="A231" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B231" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="B231" s="8" t="s">
-        <v>333</v>
-      </c>
       <c r="C231" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D231" s="1"/>
       <c r="E231" s="1"/>
@@ -9570,13 +9570,13 @@
     </row>
     <row r="232" spans="1:26" ht="13.5" customHeight="1">
       <c r="A232" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B232" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C232" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D232" s="1"/>
       <c r="E232" s="1"/>
@@ -9604,13 +9604,13 @@
     </row>
     <row r="233" spans="1:26" ht="13.5" customHeight="1">
       <c r="A233" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B233" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B233" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="C233" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D233" s="1"/>
       <c r="E233" s="1"/>
@@ -9638,13 +9638,13 @@
     </row>
     <row r="234" spans="1:26" ht="13.5" customHeight="1">
       <c r="A234" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D234" s="1"/>
       <c r="E234" s="1"/>
@@ -9672,13 +9672,13 @@
     </row>
     <row r="235" spans="1:26" ht="13.5" customHeight="1">
       <c r="A235" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B235" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B235" s="1" t="s">
-        <v>337</v>
-      </c>
       <c r="C235" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D235" s="1"/>
       <c r="E235" s="1"/>
@@ -31222,14 +31222,14 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="54.140625" customWidth="1"/>
+    <col min="1" max="1" width="54.1796875" customWidth="1"/>
     <col min="2" max="2" width="81" customWidth="1"/>
-    <col min="3" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" ht="14.5">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -31261,12 +31261,12 @@
       <c r="Y1" s="19"/>
       <c r="Z1" s="19"/>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" ht="14.5">
       <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -31293,7 +31293,7 @@
       <c r="Y2" s="19"/>
       <c r="Z2" s="19"/>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" ht="14.5">
       <c r="A3" s="20" t="s">
         <v>4</v>
       </c>
@@ -31325,7 +31325,7 @@
       <c r="Y3" s="19"/>
       <c r="Z3" s="19"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" ht="14.5">
       <c r="A4" s="20" t="s">
         <v>6</v>
       </c>
@@ -31357,12 +31357,12 @@
       <c r="Y4" s="19"/>
       <c r="Z4" s="19"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" ht="14.5">
       <c r="A5" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -31389,12 +31389,12 @@
       <c r="Y5" s="19"/>
       <c r="Z5" s="19"/>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" ht="14.5">
       <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -31421,12 +31421,12 @@
       <c r="Y6" s="19"/>
       <c r="Z6" s="19"/>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" ht="14.5">
       <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
@@ -31453,12 +31453,12 @@
       <c r="Y7" s="19"/>
       <c r="Z7" s="19"/>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" ht="14.5">
       <c r="A8" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -31485,7 +31485,7 @@
       <c r="Y8" s="19"/>
       <c r="Z8" s="19"/>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" ht="14.5">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -31513,12 +31513,12 @@
       <c r="Y9" s="19"/>
       <c r="Z9" s="19"/>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" ht="14.5">
       <c r="A10" s="19" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -31545,12 +31545,12 @@
       <c r="Y10" s="19"/>
       <c r="Z10" s="19"/>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" ht="14.5">
       <c r="A11" s="19" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -31577,9 +31577,9 @@
       <c r="Y11" s="19"/>
       <c r="Z11" s="19"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" ht="14.5">
       <c r="A12" s="19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B12" s="22">
         <v>784512369</v>
@@ -31609,12 +31609,12 @@
       <c r="Y12" s="19"/>
       <c r="Z12" s="19"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" ht="14.5">
       <c r="A13" s="19" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -31641,12 +31641,12 @@
       <c r="Y13" s="19"/>
       <c r="Z13" s="19"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" ht="14.5">
       <c r="A14" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -31673,7 +31673,7 @@
       <c r="Y14" s="19"/>
       <c r="Z14" s="19"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" ht="14.5">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -31701,12 +31701,12 @@
       <c r="Y15" s="19"/>
       <c r="Z15" s="19"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" ht="14.5">
       <c r="A16" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -31733,12 +31733,12 @@
       <c r="Y16" s="19"/>
       <c r="Z16" s="19"/>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" ht="14.5">
       <c r="A17" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -31765,12 +31765,12 @@
       <c r="Y17" s="19"/>
       <c r="Z17" s="19"/>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" ht="14.5">
       <c r="A18" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -31797,12 +31797,12 @@
       <c r="Y18" s="19"/>
       <c r="Z18" s="19"/>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" ht="14.5">
       <c r="A19" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -31829,7 +31829,7 @@
       <c r="Y19" s="19"/>
       <c r="Z19" s="19"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" ht="14.5">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -31862,7 +31862,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -31894,7 +31894,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -31923,10 +31923,10 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
@@ -31958,7 +31958,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
@@ -31987,10 +31987,10 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
@@ -32047,10 +32047,10 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="20" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
@@ -32079,10 +32079,10 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -32111,10 +32111,10 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
@@ -32143,10 +32143,10 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="B30" s="26" t="s">
         <v>347</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>348</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
@@ -32175,10 +32175,10 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="18" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -32235,10 +32235,10 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -32267,10 +32267,10 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
@@ -32299,10 +32299,10 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -32331,7 +32331,7 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="18" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>15</v>
@@ -32391,10 +32391,10 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="B38" s="19" t="s">
         <v>352</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>353</v>
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="19"/>
@@ -32423,10 +32423,10 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>354</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>355</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -32455,7 +32455,7 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B40" s="19" t="s">
         <v>15</v>
@@ -32487,10 +32487,10 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>356</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>357</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
@@ -32547,10 +32547,10 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="19" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
@@ -32579,10 +32579,10 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
@@ -32611,7 +32611,7 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B45" s="19">
         <v>784512369</v>
@@ -32643,10 +32643,10 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="B46" s="19" t="s">
         <v>360</v>
-      </c>
-      <c r="B46" s="19" t="s">
-        <v>361</v>
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
@@ -32675,7 +32675,7 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B47" s="19" t="s">
         <v>15</v>
@@ -32735,10 +32735,10 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
@@ -32767,10 +32767,10 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="19"/>
@@ -32799,10 +32799,10 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1">
       <c r="A51" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>364</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>365</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
@@ -32831,7 +32831,7 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1">
       <c r="A52" s="19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B52" s="19" t="s">
         <v>15</v>
@@ -32891,10 +32891,10 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1">
       <c r="A54" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="B54" s="19" t="s">
         <v>366</v>
-      </c>
-      <c r="B54" s="19" t="s">
-        <v>367</v>
       </c>
       <c r="C54" s="19"/>
       <c r="D54" s="19"/>
@@ -32923,10 +32923,10 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1">
       <c r="A55" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="B55" s="19" t="s">
         <v>368</v>
-      </c>
-      <c r="B55" s="19" t="s">
-        <v>369</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
@@ -32955,10 +32955,10 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1">
       <c r="A56" s="19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
@@ -32987,10 +32987,10 @@
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1">
       <c r="A57" s="19" t="s">
+        <v>370</v>
+      </c>
+      <c r="B57" s="19" t="s">
         <v>371</v>
-      </c>
-      <c r="B57" s="19" t="s">
-        <v>372</v>
       </c>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
@@ -33019,10 +33019,10 @@
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1">
       <c r="A58" s="19" t="s">
+        <v>372</v>
+      </c>
+      <c r="B58" s="19" t="s">
         <v>373</v>
-      </c>
-      <c r="B58" s="19" t="s">
-        <v>374</v>
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="19"/>
@@ -33051,10 +33051,10 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1">
       <c r="A59" s="19" t="s">
+        <v>374</v>
+      </c>
+      <c r="B59" s="19" t="s">
         <v>375</v>
-      </c>
-      <c r="B59" s="19" t="s">
-        <v>376</v>
       </c>
       <c r="C59" s="19"/>
       <c r="D59" s="19"/>
@@ -33083,10 +33083,10 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1">
       <c r="A60" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="B60" s="23" t="s">
         <v>377</v>
-      </c>
-      <c r="B60" s="23" t="s">
-        <v>378</v>
       </c>
       <c r="C60" s="19"/>
       <c r="D60" s="19"/>
@@ -33115,10 +33115,10 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1">
       <c r="A61" s="19" t="s">
+        <v>378</v>
+      </c>
+      <c r="B61" s="23" t="s">
         <v>379</v>
-      </c>
-      <c r="B61" s="23" t="s">
-        <v>380</v>
       </c>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
@@ -33147,10 +33147,10 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1">
       <c r="A62" s="19" t="s">
+        <v>380</v>
+      </c>
+      <c r="B62" s="23" t="s">
         <v>381</v>
-      </c>
-      <c r="B62" s="23" t="s">
-        <v>382</v>
       </c>
       <c r="C62" s="19"/>
       <c r="D62" s="19"/>
@@ -33179,10 +33179,10 @@
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1">
       <c r="A63" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="B63" s="23" t="s">
         <v>383</v>
-      </c>
-      <c r="B63" s="23" t="s">
-        <v>384</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
@@ -33211,10 +33211,10 @@
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1">
       <c r="A64" s="19" t="s">
+        <v>384</v>
+      </c>
+      <c r="B64" s="23" t="s">
         <v>385</v>
-      </c>
-      <c r="B64" s="23" t="s">
-        <v>386</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
@@ -33243,10 +33243,10 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1">
       <c r="A65" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="B65" s="23" t="s">
         <v>387</v>
-      </c>
-      <c r="B65" s="23" t="s">
-        <v>388</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
@@ -33275,10 +33275,10 @@
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1">
       <c r="A66" s="19" t="s">
+        <v>388</v>
+      </c>
+      <c r="B66" s="23" t="s">
         <v>389</v>
-      </c>
-      <c r="B66" s="23" t="s">
-        <v>390</v>
       </c>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
@@ -33307,10 +33307,10 @@
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1">
       <c r="A67" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="B67" s="23" t="s">
         <v>391</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>392</v>
       </c>
       <c r="C67" s="19"/>
       <c r="D67" s="19"/>
@@ -33367,10 +33367,10 @@
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1">
       <c r="A69" s="19" t="s">
+        <v>399</v>
+      </c>
+      <c r="B69" s="23" t="s">
         <v>400</v>
-      </c>
-      <c r="B69" s="23" t="s">
-        <v>401</v>
       </c>
       <c r="C69" s="19"/>
       <c r="D69" s="19"/>
@@ -33399,10 +33399,10 @@
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1">
       <c r="A70" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="B70" s="23" t="s">
         <v>402</v>
-      </c>
-      <c r="B70" s="23" t="s">
-        <v>403</v>
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="19"/>
@@ -33431,10 +33431,10 @@
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1">
       <c r="A71" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="B71" s="23" t="s">
         <v>404</v>
-      </c>
-      <c r="B71" s="23" t="s">
-        <v>405</v>
       </c>
       <c r="C71" s="19"/>
       <c r="D71" s="19"/>
@@ -33463,10 +33463,10 @@
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1">
       <c r="A72" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="B72" s="23" t="s">
         <v>406</v>
-      </c>
-      <c r="B72" s="23" t="s">
-        <v>407</v>
       </c>
       <c r="C72" s="19"/>
       <c r="D72" s="19"/>
@@ -33523,10 +33523,10 @@
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1">
       <c r="A74" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="B74" s="19" t="s">
         <v>408</v>
-      </c>
-      <c r="B74" s="19" t="s">
-        <v>409</v>
       </c>
       <c r="C74" s="19"/>
       <c r="D74" s="19"/>
@@ -33555,10 +33555,10 @@
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1">
       <c r="A75" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="B75" s="19" t="s">
         <v>402</v>
-      </c>
-      <c r="B75" s="19" t="s">
-        <v>403</v>
       </c>
       <c r="C75" s="19"/>
       <c r="D75" s="19"/>
@@ -33587,10 +33587,10 @@
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1">
       <c r="A76" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="B76" s="19" t="s">
         <v>410</v>
-      </c>
-      <c r="B76" s="19" t="s">
-        <v>411</v>
       </c>
       <c r="C76" s="19"/>
       <c r="D76" s="19"/>
@@ -33619,10 +33619,10 @@
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1">
       <c r="A77" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="B77" s="19" t="s">
         <v>412</v>
-      </c>
-      <c r="B77" s="19" t="s">
-        <v>413</v>
       </c>
       <c r="C77" s="19"/>
       <c r="D77" s="19"/>
@@ -33679,10 +33679,10 @@
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1">
       <c r="A79" s="19" t="s">
+        <v>413</v>
+      </c>
+      <c r="B79" s="19" t="s">
         <v>414</v>
-      </c>
-      <c r="B79" s="19" t="s">
-        <v>415</v>
       </c>
       <c r="C79" s="19"/>
       <c r="D79" s="19"/>
@@ -33711,10 +33711,10 @@
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1">
       <c r="A80" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="B80" s="19" t="s">
         <v>402</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>403</v>
       </c>
       <c r="C80" s="19"/>
       <c r="D80" s="19"/>
@@ -33743,10 +33743,10 @@
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1">
       <c r="A81" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="B81" s="19" t="s">
         <v>416</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>417</v>
       </c>
       <c r="C81" s="19"/>
       <c r="D81" s="19"/>
@@ -33775,10 +33775,10 @@
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1">
       <c r="A82" s="19" t="s">
+        <v>417</v>
+      </c>
+      <c r="B82" s="19" t="s">
         <v>418</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>419</v>
       </c>
       <c r="C82" s="19"/>
       <c r="D82" s="19"/>
@@ -33807,10 +33807,10 @@
     </row>
     <row r="83" spans="1:26" ht="15.75" customHeight="1">
       <c r="A83" s="19" t="s">
+        <v>419</v>
+      </c>
+      <c r="B83" s="19" t="s">
         <v>420</v>
-      </c>
-      <c r="B83" s="19" t="s">
-        <v>421</v>
       </c>
       <c r="C83" s="19"/>
       <c r="D83" s="19"/>
@@ -33867,10 +33867,10 @@
     </row>
     <row r="85" spans="1:26" ht="15.75" customHeight="1">
       <c r="A85" s="19" t="s">
+        <v>421</v>
+      </c>
+      <c r="B85" s="19" t="s">
         <v>422</v>
-      </c>
-      <c r="B85" s="19" t="s">
-        <v>423</v>
       </c>
       <c r="C85" s="19"/>
       <c r="D85" s="19"/>
@@ -33899,10 +33899,10 @@
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1">
       <c r="A86" s="19" t="s">
+        <v>423</v>
+      </c>
+      <c r="B86" s="19" t="s">
         <v>424</v>
-      </c>
-      <c r="B86" s="19" t="s">
-        <v>425</v>
       </c>
       <c r="C86" s="19"/>
       <c r="D86" s="19"/>
@@ -33931,10 +33931,10 @@
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1">
       <c r="A87" s="19" t="s">
+        <v>425</v>
+      </c>
+      <c r="B87" s="19" t="s">
         <v>426</v>
-      </c>
-      <c r="B87" s="19" t="s">
-        <v>427</v>
       </c>
       <c r="C87" s="19"/>
       <c r="D87" s="19"/>
@@ -33963,10 +33963,10 @@
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1">
       <c r="A88" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="B88" s="19" t="s">
         <v>402</v>
-      </c>
-      <c r="B88" s="19" t="s">
-        <v>403</v>
       </c>
       <c r="C88" s="19"/>
       <c r="D88" s="19"/>
@@ -33995,10 +33995,10 @@
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1">
       <c r="A89" s="19" t="s">
+        <v>427</v>
+      </c>
+      <c r="B89" s="19" t="s">
         <v>428</v>
-      </c>
-      <c r="B89" s="19" t="s">
-        <v>429</v>
       </c>
       <c r="C89" s="19"/>
       <c r="D89" s="19"/>
@@ -34027,10 +34027,10 @@
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1">
       <c r="A90" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="B90" s="19" t="s">
         <v>430</v>
-      </c>
-      <c r="B90" s="19" t="s">
-        <v>431</v>
       </c>
       <c r="C90" s="19"/>
       <c r="D90" s="19"/>
@@ -34059,10 +34059,10 @@
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1">
       <c r="A91" s="19" t="s">
+        <v>431</v>
+      </c>
+      <c r="B91" s="19" t="s">
         <v>432</v>
-      </c>
-      <c r="B91" s="19" t="s">
-        <v>433</v>
       </c>
       <c r="C91" s="19"/>
       <c r="D91" s="19"/>
@@ -34091,10 +34091,10 @@
     </row>
     <row r="92" spans="1:26" ht="15.75" customHeight="1">
       <c r="A92" s="19" t="s">
+        <v>433</v>
+      </c>
+      <c r="B92" s="19" t="s">
         <v>434</v>
-      </c>
-      <c r="B92" s="19" t="s">
-        <v>435</v>
       </c>
       <c r="C92" s="19"/>
       <c r="D92" s="19"/>
@@ -34123,10 +34123,10 @@
     </row>
     <row r="93" spans="1:26" ht="15.75" customHeight="1">
       <c r="A93" s="19" t="s">
+        <v>435</v>
+      </c>
+      <c r="B93" s="19" t="s">
         <v>436</v>
-      </c>
-      <c r="B93" s="19" t="s">
-        <v>437</v>
       </c>
       <c r="C93" s="19"/>
       <c r="D93" s="19"/>
@@ -34183,10 +34183,10 @@
     </row>
     <row r="95" spans="1:26" ht="15.75" customHeight="1">
       <c r="A95" s="19" t="s">
+        <v>437</v>
+      </c>
+      <c r="B95" s="19" t="s">
         <v>438</v>
-      </c>
-      <c r="B95" s="19" t="s">
-        <v>439</v>
       </c>
       <c r="C95" s="19"/>
       <c r="D95" s="19"/>
@@ -34215,10 +34215,10 @@
     </row>
     <row r="96" spans="1:26" ht="15.75" customHeight="1">
       <c r="A96" s="19" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C96" s="19"/>
       <c r="D96" s="19"/>
@@ -34247,10 +34247,10 @@
     </row>
     <row r="97" spans="1:26" ht="15.75" customHeight="1">
       <c r="A97" s="19" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C97" s="19"/>
       <c r="D97" s="19"/>
@@ -34279,10 +34279,10 @@
     </row>
     <row r="98" spans="1:26" ht="15.75" customHeight="1">
       <c r="A98" s="19" t="s">
+        <v>441</v>
+      </c>
+      <c r="B98" s="19" t="s">
         <v>442</v>
-      </c>
-      <c r="B98" s="19" t="s">
-        <v>443</v>
       </c>
       <c r="C98" s="19"/>
       <c r="D98" s="19"/>
@@ -34311,10 +34311,10 @@
     </row>
     <row r="99" spans="1:26" ht="15.75" customHeight="1">
       <c r="A99" s="19" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C99" s="19"/>
       <c r="D99" s="19"/>
@@ -34343,10 +34343,10 @@
     </row>
     <row r="100" spans="1:26" ht="15.75" customHeight="1">
       <c r="A100" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="B100" s="19" t="s">
         <v>402</v>
-      </c>
-      <c r="B100" s="19" t="s">
-        <v>403</v>
       </c>
       <c r="C100" s="19"/>
       <c r="D100" s="19"/>
@@ -34375,10 +34375,10 @@
     </row>
     <row r="101" spans="1:26" ht="15.75" customHeight="1">
       <c r="A101" s="19" t="s">
+        <v>444</v>
+      </c>
+      <c r="B101" s="19" t="s">
         <v>445</v>
-      </c>
-      <c r="B101" s="19" t="s">
-        <v>446</v>
       </c>
       <c r="C101" s="19"/>
       <c r="D101" s="19"/>
@@ -34407,10 +34407,10 @@
     </row>
     <row r="102" spans="1:26" ht="15.75" customHeight="1">
       <c r="A102" s="19" t="s">
+        <v>446</v>
+      </c>
+      <c r="B102" s="19" t="s">
         <v>447</v>
-      </c>
-      <c r="B102" s="19" t="s">
-        <v>448</v>
       </c>
       <c r="C102" s="19"/>
       <c r="D102" s="19"/>
@@ -34467,10 +34467,10 @@
     </row>
     <row r="104" spans="1:26" ht="15.75" customHeight="1">
       <c r="A104" s="19" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C104" s="19"/>
       <c r="D104" s="19"/>
@@ -34527,10 +34527,10 @@
     </row>
     <row r="106" spans="1:26" ht="15.75" customHeight="1">
       <c r="A106" s="19" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C106" s="19"/>
       <c r="D106" s="19"/>
@@ -34559,10 +34559,10 @@
     </row>
     <row r="107" spans="1:26" ht="15.75" customHeight="1">
       <c r="A107" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="B107" s="19" t="s">
         <v>451</v>
-      </c>
-      <c r="B107" s="19" t="s">
-        <v>452</v>
       </c>
       <c r="C107" s="19"/>
       <c r="D107" s="19"/>
@@ -34591,10 +34591,10 @@
     </row>
     <row r="108" spans="1:26" ht="15.75" customHeight="1">
       <c r="A108" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="B108" s="19" t="s">
         <v>402</v>
-      </c>
-      <c r="B108" s="19" t="s">
-        <v>403</v>
       </c>
       <c r="C108" s="19"/>
       <c r="D108" s="19"/>
@@ -34623,10 +34623,10 @@
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1">
       <c r="A109" s="19" t="s">
+        <v>452</v>
+      </c>
+      <c r="B109" s="19" t="s">
         <v>453</v>
-      </c>
-      <c r="B109" s="19" t="s">
-        <v>454</v>
       </c>
       <c r="C109" s="19"/>
       <c r="D109" s="19"/>
@@ -34655,10 +34655,10 @@
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1">
       <c r="A110" s="19" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C110" s="19"/>
       <c r="D110" s="19"/>
@@ -34743,10 +34743,10 @@
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1">
       <c r="A113" s="19" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C113" s="19"/>
       <c r="D113" s="19"/>
@@ -34775,10 +34775,10 @@
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1">
       <c r="A114" s="19" t="s">
+        <v>456</v>
+      </c>
+      <c r="B114" s="19" t="s">
         <v>457</v>
-      </c>
-      <c r="B114" s="19" t="s">
-        <v>458</v>
       </c>
       <c r="C114" s="19"/>
       <c r="D114" s="19"/>
@@ -34807,10 +34807,10 @@
     </row>
     <row r="115" spans="1:26" ht="15.75" customHeight="1">
       <c r="A115" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="B115" s="19" t="s">
         <v>402</v>
-      </c>
-      <c r="B115" s="19" t="s">
-        <v>403</v>
       </c>
       <c r="C115" s="19"/>
       <c r="D115" s="19"/>
@@ -34839,10 +34839,10 @@
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1">
       <c r="A116" s="19" t="s">
+        <v>458</v>
+      </c>
+      <c r="B116" s="19" t="s">
         <v>459</v>
-      </c>
-      <c r="B116" s="19" t="s">
-        <v>460</v>
       </c>
       <c r="C116" s="19"/>
       <c r="D116" s="19"/>
@@ -34899,10 +34899,10 @@
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1">
       <c r="A118" s="19" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B118" s="19" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C118" s="19"/>
       <c r="D118" s="19"/>
@@ -34931,10 +34931,10 @@
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1">
       <c r="A119" s="19" t="s">
+        <v>461</v>
+      </c>
+      <c r="B119" s="19" t="s">
         <v>462</v>
-      </c>
-      <c r="B119" s="19" t="s">
-        <v>463</v>
       </c>
       <c r="C119" s="19"/>
       <c r="D119" s="19"/>
@@ -34963,10 +34963,10 @@
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1">
       <c r="A120" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="B120" s="19" t="s">
         <v>402</v>
-      </c>
-      <c r="B120" s="19" t="s">
-        <v>403</v>
       </c>
       <c r="C120" s="19"/>
       <c r="D120" s="19"/>
@@ -34995,10 +34995,10 @@
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1">
       <c r="A121" s="19" t="s">
+        <v>463</v>
+      </c>
+      <c r="B121" s="19" t="s">
         <v>464</v>
-      </c>
-      <c r="B121" s="19" t="s">
-        <v>465</v>
       </c>
       <c r="C121" s="19"/>
       <c r="D121" s="19"/>
@@ -35027,10 +35027,10 @@
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1">
       <c r="A122" s="19" t="s">
+        <v>465</v>
+      </c>
+      <c r="B122" s="19" t="s">
         <v>466</v>
-      </c>
-      <c r="B122" s="19" t="s">
-        <v>467</v>
       </c>
       <c r="C122" s="19"/>
       <c r="D122" s="19"/>
@@ -35087,10 +35087,10 @@
     </row>
     <row r="124" spans="1:26" ht="15.75" customHeight="1">
       <c r="A124" s="19" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C124" s="19"/>
       <c r="D124" s="19"/>
@@ -35119,10 +35119,10 @@
     </row>
     <row r="125" spans="1:26" ht="15.75" customHeight="1">
       <c r="A125" s="19" t="s">
+        <v>468</v>
+      </c>
+      <c r="B125" s="19" t="s">
         <v>469</v>
-      </c>
-      <c r="B125" s="19" t="s">
-        <v>470</v>
       </c>
       <c r="C125" s="19"/>
       <c r="D125" s="19"/>
@@ -35151,10 +35151,10 @@
     </row>
     <row r="126" spans="1:26" ht="15.75" customHeight="1">
       <c r="A126" s="19" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C126" s="19"/>
       <c r="D126" s="19"/>
@@ -35211,10 +35211,10 @@
     </row>
     <row r="128" spans="1:26" ht="15.75" customHeight="1">
       <c r="A128" s="19" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B128" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C128" s="19"/>
       <c r="D128" s="19"/>
@@ -35243,7 +35243,7 @@
     </row>
     <row r="129" spans="1:26" ht="15.75" customHeight="1">
       <c r="A129" s="19" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B129" s="19" t="s">
         <v>7</v>
@@ -35275,10 +35275,10 @@
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1">
       <c r="A130" s="19" t="s">
+        <v>473</v>
+      </c>
+      <c r="B130" s="19" t="s">
         <v>474</v>
-      </c>
-      <c r="B130" s="19" t="s">
-        <v>475</v>
       </c>
       <c r="C130" s="19"/>
       <c r="D130" s="19"/>
@@ -35307,10 +35307,10 @@
     </row>
     <row r="131" spans="1:26" ht="15.75" customHeight="1">
       <c r="A131" s="19" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B131" s="19" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C131" s="19"/>
       <c r="D131" s="19"/>
@@ -35339,10 +35339,10 @@
     </row>
     <row r="132" spans="1:26" ht="15.75" customHeight="1">
       <c r="A132" s="19" t="s">
+        <v>476</v>
+      </c>
+      <c r="B132" s="19" t="s">
         <v>477</v>
-      </c>
-      <c r="B132" s="19" t="s">
-        <v>478</v>
       </c>
       <c r="C132" s="19"/>
       <c r="D132" s="19"/>
@@ -35399,10 +35399,10 @@
     </row>
     <row r="134" spans="1:26" ht="15.75" customHeight="1">
       <c r="A134" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="B134" s="19" t="s">
         <v>479</v>
-      </c>
-      <c r="B134" s="19" t="s">
-        <v>480</v>
       </c>
       <c r="C134" s="19"/>
       <c r="D134" s="19"/>
@@ -35431,10 +35431,10 @@
     </row>
     <row r="135" spans="1:26" ht="15.75" customHeight="1">
       <c r="A135" s="19" t="s">
+        <v>480</v>
+      </c>
+      <c r="B135" s="19" t="s">
         <v>481</v>
-      </c>
-      <c r="B135" s="19" t="s">
-        <v>482</v>
       </c>
       <c r="C135" s="19"/>
       <c r="D135" s="19"/>
@@ -35463,10 +35463,10 @@
     </row>
     <row r="136" spans="1:26" ht="15.75" customHeight="1">
       <c r="A136" s="19" t="s">
+        <v>482</v>
+      </c>
+      <c r="B136" s="19" t="s">
         <v>483</v>
-      </c>
-      <c r="B136" s="19" t="s">
-        <v>484</v>
       </c>
       <c r="C136" s="19"/>
       <c r="D136" s="19"/>
@@ -35495,10 +35495,10 @@
     </row>
     <row r="137" spans="1:26" ht="15.75" customHeight="1">
       <c r="A137" s="19" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B137" s="19" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C137" s="19"/>
       <c r="D137" s="19"/>
@@ -35527,10 +35527,10 @@
     </row>
     <row r="138" spans="1:26" ht="15.75" customHeight="1">
       <c r="A138" s="19" t="s">
+        <v>485</v>
+      </c>
+      <c r="B138" s="19" t="s">
         <v>486</v>
-      </c>
-      <c r="B138" s="19" t="s">
-        <v>487</v>
       </c>
       <c r="C138" s="19"/>
       <c r="D138" s="19"/>
@@ -35559,10 +35559,10 @@
     </row>
     <row r="139" spans="1:26" ht="15.75" customHeight="1">
       <c r="A139" s="19" t="s">
+        <v>487</v>
+      </c>
+      <c r="B139" s="19" t="s">
         <v>488</v>
-      </c>
-      <c r="B139" s="19" t="s">
-        <v>489</v>
       </c>
       <c r="C139" s="19"/>
       <c r="D139" s="19"/>
@@ -35619,10 +35619,10 @@
     </row>
     <row r="141" spans="1:26" ht="15.75" customHeight="1">
       <c r="A141" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B141" s="19" t="s">
         <v>261</v>
-      </c>
-      <c r="B141" s="19" t="s">
-        <v>262</v>
       </c>
       <c r="C141" s="19"/>
       <c r="D141" s="19"/>
@@ -35651,10 +35651,10 @@
     </row>
     <row r="142" spans="1:26" ht="15.75" customHeight="1">
       <c r="A142" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="B142" s="19" t="s">
         <v>224</v>
-      </c>
-      <c r="B142" s="19" t="s">
-        <v>225</v>
       </c>
       <c r="C142" s="19"/>
       <c r="D142" s="19"/>
@@ -35683,10 +35683,10 @@
     </row>
     <row r="143" spans="1:26" ht="15.75" customHeight="1">
       <c r="A143" s="19" t="s">
+        <v>489</v>
+      </c>
+      <c r="B143" s="19" t="s">
         <v>490</v>
-      </c>
-      <c r="B143" s="19" t="s">
-        <v>491</v>
       </c>
       <c r="C143" s="19"/>
       <c r="D143" s="19"/>
@@ -35743,10 +35743,10 @@
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1">
       <c r="A145" s="19" t="s">
+        <v>491</v>
+      </c>
+      <c r="B145" s="19" t="s">
         <v>492</v>
-      </c>
-      <c r="B145" s="19" t="s">
-        <v>493</v>
       </c>
       <c r="C145" s="19"/>
       <c r="D145" s="19"/>

</xml_diff>

<commit_message>
xpath changes in healthRecords 12/10/22
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -12,14 +12,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mis+N7J1EYg97C+uHq7LXEBbVLqvA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mi0uSG8z+ZhD5bPtHFHuACRVvBL2w=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="921">
   <si>
     <t>KEY</t>
   </si>
@@ -1894,9 +1894,6 @@
   </si>
   <si>
     <t>VM04Practice;Kevin Peterson;Deliver Meds by Pharmacy;Select from my saved list;ZOOM Pharmacy home delivery;2: 456, demo;48 Hours;Panadol (Optizorb) 500mg Caplets;Repeat Medication Testing for Delivery Meds by Pharmacy;ZOOM Pharmacy home delivery</t>
-  </si>
-  <si>
-    <t>Urgent/Same day  - Std Fee: $56.00 (Incl. GST);Next Day  - Std Fee: $12.00 (Incl. GST);48 Hours  - Std Fee: $13.00 (Incl. GST);72 Hours  - Std Fee: $14.00 (Incl. GST)</t>
   </si>
   <si>
     <t>My Health Records</t>
@@ -2901,7 +2898,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2962,7 +2958,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3061,12 +3057,7 @@
     </xf>
     <xf borderId="1" fillId="4" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="1" fillId="5" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -31053,11 +31044,11 @@
       <c r="A186" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="B186" s="32" t="s">
-        <v>625</v>
-      </c>
-      <c r="C186" s="32" t="s">
-        <v>625</v>
+      <c r="B186" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C186" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="D186" s="23"/>
       <c r="E186" s="23"/>
@@ -31110,7 +31101,7 @@
     </row>
     <row r="188">
       <c r="B188" s="34" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D188" s="23"/>
       <c r="E188" s="23"/>
@@ -31253,10 +31244,10 @@
         <v>3</v>
       </c>
       <c r="B193" s="36" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C193" s="36" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D193" s="23"/>
       <c r="E193" s="23"/>
@@ -31355,10 +31346,10 @@
         <v>105</v>
       </c>
       <c r="B196" s="35" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C196" s="35" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D196" s="23"/>
       <c r="E196" s="23"/>
@@ -31856,13 +31847,13 @@
     </row>
     <row r="211">
       <c r="A211" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="B211" s="38" t="s">
         <v>629</v>
       </c>
-      <c r="B211" s="38" t="s">
-        <v>630</v>
-      </c>
       <c r="C211" s="38" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D211" s="23"/>
       <c r="E211" s="23"/>
@@ -31893,10 +31884,10 @@
         <v>334</v>
       </c>
       <c r="B212" s="23" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C212" s="23" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D212" s="23"/>
       <c r="E212" s="23"/>
@@ -31924,7 +31915,7 @@
     </row>
     <row r="213">
       <c r="A213" s="35" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B213" s="23" t="s">
         <v>337</v>
@@ -32156,13 +32147,13 @@
     </row>
     <row r="220">
       <c r="A220" s="35" t="s">
+        <v>632</v>
+      </c>
+      <c r="B220" s="38" t="s">
         <v>633</v>
       </c>
-      <c r="B220" s="38" t="s">
-        <v>634</v>
-      </c>
       <c r="C220" s="38" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D220" s="23"/>
       <c r="E220" s="23"/>
@@ -32190,13 +32181,13 @@
     </row>
     <row r="221">
       <c r="A221" s="35" t="s">
+        <v>634</v>
+      </c>
+      <c r="B221" s="23" t="s">
         <v>635</v>
       </c>
-      <c r="B221" s="23" t="s">
-        <v>636</v>
-      </c>
       <c r="C221" s="23" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D221" s="23"/>
       <c r="E221" s="23"/>
@@ -32326,13 +32317,13 @@
     </row>
     <row r="225">
       <c r="A225" s="35" t="s">
+        <v>636</v>
+      </c>
+      <c r="B225" s="35" t="s">
         <v>637</v>
       </c>
-      <c r="B225" s="35" t="s">
-        <v>638</v>
-      </c>
       <c r="C225" s="35" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D225" s="23"/>
       <c r="E225" s="23"/>
@@ -32428,13 +32419,13 @@
     </row>
     <row r="228">
       <c r="A228" s="35" t="s">
+        <v>638</v>
+      </c>
+      <c r="B228" s="35" t="s">
         <v>639</v>
       </c>
-      <c r="B228" s="35" t="s">
-        <v>640</v>
-      </c>
       <c r="C228" s="35" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D228" s="23"/>
       <c r="E228" s="23"/>
@@ -32496,13 +32487,13 @@
     </row>
     <row r="230">
       <c r="A230" s="35" t="s">
+        <v>640</v>
+      </c>
+      <c r="B230" s="38" t="s">
         <v>641</v>
       </c>
-      <c r="B230" s="38" t="s">
-        <v>642</v>
-      </c>
       <c r="C230" s="38" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D230" s="23"/>
       <c r="E230" s="23"/>
@@ -32691,13 +32682,13 @@
     </row>
     <row r="236">
       <c r="A236" s="35" t="s">
+        <v>642</v>
+      </c>
+      <c r="B236" s="38" t="s">
         <v>643</v>
       </c>
-      <c r="B236" s="38" t="s">
-        <v>644</v>
-      </c>
       <c r="C236" s="38" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D236" s="23"/>
       <c r="E236" s="23"/>
@@ -32793,13 +32784,13 @@
     </row>
     <row r="239">
       <c r="A239" s="35" t="s">
+        <v>644</v>
+      </c>
+      <c r="B239" s="38" t="s">
         <v>645</v>
       </c>
-      <c r="B239" s="38" t="s">
-        <v>646</v>
-      </c>
       <c r="C239" s="38" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D239" s="23"/>
       <c r="E239" s="23"/>
@@ -32827,13 +32818,13 @@
     </row>
     <row r="240">
       <c r="A240" s="35" t="s">
+        <v>646</v>
+      </c>
+      <c r="B240" s="38" t="s">
         <v>647</v>
       </c>
-      <c r="B240" s="38" t="s">
-        <v>648</v>
-      </c>
       <c r="C240" s="38" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D240" s="23"/>
       <c r="E240" s="23"/>
@@ -32932,10 +32923,10 @@
         <v>147</v>
       </c>
       <c r="B243" s="38" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C243" s="38" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D243" s="23"/>
       <c r="E243" s="23"/>
@@ -33167,13 +33158,13 @@
     </row>
     <row r="250">
       <c r="A250" s="35" t="s">
+        <v>649</v>
+      </c>
+      <c r="B250" s="38" t="s">
         <v>650</v>
       </c>
-      <c r="B250" s="38" t="s">
-        <v>651</v>
-      </c>
       <c r="C250" s="38" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D250" s="23"/>
       <c r="E250" s="23"/>
@@ -33235,13 +33226,13 @@
     </row>
     <row r="252">
       <c r="A252" s="35" t="s">
+        <v>651</v>
+      </c>
+      <c r="B252" s="38" t="s">
         <v>652</v>
       </c>
-      <c r="B252" s="38" t="s">
-        <v>653</v>
-      </c>
       <c r="C252" s="38" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D252" s="23"/>
       <c r="E252" s="23"/>
@@ -33455,7 +33446,7 @@
     </row>
     <row r="259">
       <c r="B259" s="40" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D259" s="23"/>
       <c r="E259" s="23"/>
@@ -33626,13 +33617,13 @@
     </row>
     <row r="265">
       <c r="A265" s="35" t="s">
+        <v>654</v>
+      </c>
+      <c r="B265" s="35" t="s">
         <v>655</v>
       </c>
-      <c r="B265" s="35" t="s">
-        <v>656</v>
-      </c>
       <c r="C265" s="35" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D265" s="23"/>
       <c r="E265" s="23"/>
@@ -33663,10 +33654,10 @@
         <v>36</v>
       </c>
       <c r="B266" s="35" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C266" s="35" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D266" s="23"/>
       <c r="E266" s="23"/>
@@ -33694,13 +33685,13 @@
     </row>
     <row r="267">
       <c r="A267" s="35" t="s">
+        <v>657</v>
+      </c>
+      <c r="B267" s="23" t="s">
         <v>658</v>
       </c>
-      <c r="B267" s="23" t="s">
-        <v>659</v>
-      </c>
       <c r="C267" s="23" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D267" s="23"/>
       <c r="E267" s="23"/>
@@ -33728,13 +33719,13 @@
     </row>
     <row r="268">
       <c r="A268" s="35" t="s">
+        <v>659</v>
+      </c>
+      <c r="B268" s="41" t="s">
         <v>660</v>
       </c>
-      <c r="B268" s="41" t="s">
-        <v>661</v>
-      </c>
       <c r="C268" s="41" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D268" s="23"/>
       <c r="E268" s="23"/>
@@ -33762,13 +33753,13 @@
     </row>
     <row r="269">
       <c r="A269" s="35" t="s">
+        <v>661</v>
+      </c>
+      <c r="B269" s="35" t="s">
         <v>662</v>
       </c>
-      <c r="B269" s="35" t="s">
-        <v>663</v>
-      </c>
       <c r="C269" s="35" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D269" s="23"/>
       <c r="E269" s="23"/>
@@ -33796,13 +33787,13 @@
     </row>
     <row r="270">
       <c r="A270" s="35" t="s">
+        <v>663</v>
+      </c>
+      <c r="B270" s="23" t="s">
         <v>664</v>
       </c>
-      <c r="B270" s="23" t="s">
-        <v>665</v>
-      </c>
       <c r="C270" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D270" s="23"/>
       <c r="E270" s="23"/>
@@ -33830,7 +33821,7 @@
     </row>
     <row r="271">
       <c r="A271" s="35" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B271" s="42">
         <v>120.0</v>
@@ -33864,13 +33855,13 @@
     </row>
     <row r="272">
       <c r="A272" s="35" t="s">
+        <v>666</v>
+      </c>
+      <c r="B272" s="23" t="s">
         <v>667</v>
       </c>
-      <c r="B272" s="23" t="s">
-        <v>668</v>
-      </c>
       <c r="C272" s="23" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D272" s="23"/>
       <c r="E272" s="23"/>
@@ -33898,13 +33889,13 @@
     </row>
     <row r="273">
       <c r="A273" s="35" t="s">
+        <v>668</v>
+      </c>
+      <c r="B273" s="23" t="s">
         <v>669</v>
       </c>
-      <c r="B273" s="23" t="s">
-        <v>670</v>
-      </c>
       <c r="C273" s="23" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D273" s="23"/>
       <c r="E273" s="23"/>
@@ -33932,13 +33923,13 @@
     </row>
     <row r="274">
       <c r="A274" s="35" t="s">
+        <v>670</v>
+      </c>
+      <c r="B274" s="23" t="s">
         <v>671</v>
       </c>
-      <c r="B274" s="23" t="s">
-        <v>672</v>
-      </c>
       <c r="C274" s="23" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D274" s="23"/>
       <c r="E274" s="23"/>
@@ -33966,13 +33957,13 @@
     </row>
     <row r="275">
       <c r="A275" s="35" t="s">
+        <v>672</v>
+      </c>
+      <c r="B275" s="23" t="s">
         <v>673</v>
       </c>
-      <c r="B275" s="23" t="s">
-        <v>674</v>
-      </c>
       <c r="C275" s="23" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D275" s="23"/>
       <c r="E275" s="23"/>
@@ -34000,13 +33991,13 @@
     </row>
     <row r="276">
       <c r="A276" s="35" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B276" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C276" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D276" s="23"/>
       <c r="E276" s="23"/>
@@ -34034,13 +34025,13 @@
     </row>
     <row r="277">
       <c r="A277" s="23" t="s">
+        <v>675</v>
+      </c>
+      <c r="B277" s="23" t="s">
         <v>676</v>
       </c>
-      <c r="B277" s="23" t="s">
-        <v>677</v>
-      </c>
       <c r="C277" s="23" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D277" s="23"/>
       <c r="E277" s="23"/>
@@ -34068,7 +34059,7 @@
     </row>
     <row r="278">
       <c r="A278" s="23" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B278" s="42">
         <v>6.0</v>
@@ -34102,13 +34093,13 @@
     </row>
     <row r="279">
       <c r="A279" s="23" t="s">
+        <v>678</v>
+      </c>
+      <c r="B279" s="23" t="s">
         <v>679</v>
       </c>
-      <c r="B279" s="23" t="s">
-        <v>680</v>
-      </c>
       <c r="C279" s="23" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D279" s="23"/>
       <c r="E279" s="23"/>
@@ -34136,13 +34127,13 @@
     </row>
     <row r="280">
       <c r="A280" s="23" t="s">
+        <v>680</v>
+      </c>
+      <c r="B280" s="23" t="s">
         <v>681</v>
       </c>
-      <c r="B280" s="23" t="s">
-        <v>682</v>
-      </c>
       <c r="C280" s="23" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D280" s="23"/>
       <c r="E280" s="23"/>
@@ -34170,13 +34161,13 @@
     </row>
     <row r="281">
       <c r="A281" s="23" t="s">
+        <v>682</v>
+      </c>
+      <c r="B281" s="23" t="s">
         <v>683</v>
       </c>
-      <c r="B281" s="23" t="s">
-        <v>684</v>
-      </c>
       <c r="C281" s="23" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D281" s="23"/>
       <c r="E281" s="23"/>
@@ -34204,13 +34195,13 @@
     </row>
     <row r="282">
       <c r="A282" s="23" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B282" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C282" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D282" s="23"/>
       <c r="E282" s="23"/>
@@ -34238,13 +34229,13 @@
     </row>
     <row r="283">
       <c r="A283" s="23" t="s">
+        <v>685</v>
+      </c>
+      <c r="B283" s="23" t="s">
         <v>686</v>
       </c>
-      <c r="B283" s="23" t="s">
-        <v>687</v>
-      </c>
       <c r="C283" s="23" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D283" s="23"/>
       <c r="E283" s="23"/>
@@ -34272,7 +34263,7 @@
     </row>
     <row r="284">
       <c r="A284" s="23" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B284" s="43">
         <v>13.0</v>
@@ -34306,13 +34297,13 @@
     </row>
     <row r="285">
       <c r="A285" s="23" t="s">
+        <v>688</v>
+      </c>
+      <c r="B285" s="23" t="s">
         <v>689</v>
       </c>
-      <c r="B285" s="23" t="s">
-        <v>690</v>
-      </c>
       <c r="C285" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D285" s="23"/>
       <c r="E285" s="23"/>
@@ -34340,13 +34331,13 @@
     </row>
     <row r="286">
       <c r="A286" s="23" t="s">
+        <v>690</v>
+      </c>
+      <c r="B286" s="23" t="s">
         <v>691</v>
       </c>
-      <c r="B286" s="23" t="s">
-        <v>692</v>
-      </c>
       <c r="C286" s="23" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D286" s="23"/>
       <c r="E286" s="23"/>
@@ -34374,13 +34365,13 @@
     </row>
     <row r="287">
       <c r="A287" s="23" t="s">
+        <v>692</v>
+      </c>
+      <c r="B287" s="23" t="s">
         <v>693</v>
       </c>
-      <c r="B287" s="23" t="s">
-        <v>694</v>
-      </c>
       <c r="C287" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D287" s="23"/>
       <c r="E287" s="23"/>
@@ -34408,13 +34399,13 @@
     </row>
     <row r="288">
       <c r="A288" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B288" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C288" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D288" s="23"/>
       <c r="E288" s="23"/>
@@ -34442,13 +34433,13 @@
     </row>
     <row r="289">
       <c r="A289" s="23" t="s">
+        <v>695</v>
+      </c>
+      <c r="B289" s="23" t="s">
         <v>696</v>
       </c>
-      <c r="B289" s="23" t="s">
-        <v>697</v>
-      </c>
       <c r="C289" s="23" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D289" s="23"/>
       <c r="E289" s="23"/>
@@ -34476,7 +34467,7 @@
     </row>
     <row r="290">
       <c r="A290" s="23" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B290" s="42">
         <v>12.0</v>
@@ -34510,13 +34501,13 @@
     </row>
     <row r="291">
       <c r="A291" s="23" t="s">
+        <v>698</v>
+      </c>
+      <c r="B291" s="23" t="s">
         <v>699</v>
       </c>
-      <c r="B291" s="23" t="s">
-        <v>700</v>
-      </c>
       <c r="C291" s="23" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D291" s="23"/>
       <c r="E291" s="23"/>
@@ -34544,13 +34535,13 @@
     </row>
     <row r="292">
       <c r="A292" s="23" t="s">
+        <v>700</v>
+      </c>
+      <c r="B292" s="23" t="s">
         <v>701</v>
       </c>
-      <c r="B292" s="23" t="s">
-        <v>702</v>
-      </c>
       <c r="C292" s="23" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D292" s="23"/>
       <c r="E292" s="23"/>
@@ -34578,13 +34569,13 @@
     </row>
     <row r="293">
       <c r="A293" s="23" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B293" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C293" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D293" s="23"/>
       <c r="E293" s="23"/>
@@ -34612,13 +34603,13 @@
     </row>
     <row r="294">
       <c r="A294" s="23" t="s">
+        <v>703</v>
+      </c>
+      <c r="B294" s="23" t="s">
         <v>704</v>
       </c>
-      <c r="B294" s="23" t="s">
-        <v>705</v>
-      </c>
       <c r="C294" s="23" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D294" s="23"/>
       <c r="E294" s="23"/>
@@ -34646,7 +34637,7 @@
     </row>
     <row r="295">
       <c r="A295" s="23" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B295" s="42">
         <v>2.0</v>
@@ -34680,13 +34671,13 @@
     </row>
     <row r="296">
       <c r="A296" s="23" t="s">
+        <v>706</v>
+      </c>
+      <c r="B296" s="23" t="s">
         <v>707</v>
       </c>
-      <c r="B296" s="23" t="s">
-        <v>708</v>
-      </c>
       <c r="C296" s="23" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D296" s="23"/>
       <c r="E296" s="23"/>
@@ -34714,13 +34705,13 @@
     </row>
     <row r="297">
       <c r="A297" s="23" t="s">
+        <v>708</v>
+      </c>
+      <c r="B297" s="23" t="s">
         <v>709</v>
       </c>
-      <c r="B297" s="23" t="s">
-        <v>710</v>
-      </c>
       <c r="C297" s="23" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D297" s="23"/>
       <c r="E297" s="23"/>
@@ -34748,13 +34739,13 @@
     </row>
     <row r="298">
       <c r="A298" s="23" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B298" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C298" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D298" s="23"/>
       <c r="E298" s="23"/>
@@ -34782,7 +34773,7 @@
     </row>
     <row r="299">
       <c r="A299" s="23" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B299" s="42">
         <v>7.0</v>
@@ -34816,7 +34807,7 @@
     </row>
     <row r="300">
       <c r="A300" s="23" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B300" s="42">
         <v>8.0</v>
@@ -34850,13 +34841,13 @@
     </row>
     <row r="301">
       <c r="A301" s="23" t="s">
+        <v>713</v>
+      </c>
+      <c r="B301" s="23" t="s">
         <v>714</v>
       </c>
-      <c r="B301" s="23" t="s">
-        <v>715</v>
-      </c>
       <c r="C301" s="23" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D301" s="23"/>
       <c r="E301" s="23"/>
@@ -34884,13 +34875,13 @@
     </row>
     <row r="302">
       <c r="A302" s="23" t="s">
+        <v>715</v>
+      </c>
+      <c r="B302" s="23" t="s">
         <v>716</v>
       </c>
-      <c r="B302" s="23" t="s">
-        <v>717</v>
-      </c>
       <c r="C302" s="23" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D302" s="23"/>
       <c r="E302" s="23"/>
@@ -34918,13 +34909,13 @@
     </row>
     <row r="303">
       <c r="A303" s="23" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B303" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C303" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D303" s="23"/>
       <c r="E303" s="23"/>
@@ -34952,13 +34943,13 @@
     </row>
     <row r="304">
       <c r="A304" s="23" t="s">
+        <v>718</v>
+      </c>
+      <c r="B304" s="23" t="s">
         <v>719</v>
       </c>
-      <c r="B304" s="23" t="s">
-        <v>720</v>
-      </c>
       <c r="C304" s="41" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D304" s="23"/>
       <c r="E304" s="23"/>
@@ -34986,7 +34977,7 @@
     </row>
     <row r="305">
       <c r="A305" s="23" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B305" s="42">
         <v>6.0</v>
@@ -35020,13 +35011,13 @@
     </row>
     <row r="306">
       <c r="A306" s="23" t="s">
+        <v>721</v>
+      </c>
+      <c r="B306" s="23" t="s">
         <v>722</v>
       </c>
-      <c r="B306" s="23" t="s">
-        <v>723</v>
-      </c>
       <c r="C306" s="23" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D306" s="23"/>
       <c r="E306" s="23"/>
@@ -35054,13 +35045,13 @@
     </row>
     <row r="307">
       <c r="A307" s="23" t="s">
+        <v>723</v>
+      </c>
+      <c r="B307" s="23" t="s">
         <v>724</v>
       </c>
-      <c r="B307" s="23" t="s">
-        <v>725</v>
-      </c>
       <c r="C307" s="23" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D307" s="23"/>
       <c r="E307" s="23"/>
@@ -35088,13 +35079,13 @@
     </row>
     <row r="308">
       <c r="A308" s="23" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B308" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C308" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D308" s="23"/>
       <c r="E308" s="23"/>
@@ -35122,7 +35113,7 @@
     </row>
     <row r="309">
       <c r="A309" s="23" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B309" s="42">
         <v>9.0</v>
@@ -35156,7 +35147,7 @@
     </row>
     <row r="310">
       <c r="A310" s="23" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B310" s="42">
         <v>10.0</v>
@@ -35190,13 +35181,13 @@
     </row>
     <row r="311">
       <c r="A311" s="23" t="s">
+        <v>728</v>
+      </c>
+      <c r="B311" s="23" t="s">
         <v>729</v>
       </c>
-      <c r="B311" s="23" t="s">
-        <v>730</v>
-      </c>
       <c r="C311" s="23" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D311" s="23"/>
       <c r="E311" s="23"/>
@@ -35224,13 +35215,13 @@
     </row>
     <row r="312">
       <c r="A312" s="23" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B312" s="23" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C312" s="23" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D312" s="23"/>
       <c r="E312" s="23"/>
@@ -35258,13 +35249,13 @@
     </row>
     <row r="313">
       <c r="A313" s="23" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B313" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C313" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D313" s="23"/>
       <c r="E313" s="23"/>
@@ -35292,7 +35283,7 @@
     </row>
     <row r="314">
       <c r="A314" s="23" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B314" s="42">
         <v>12.0</v>
@@ -35326,7 +35317,7 @@
     </row>
     <row r="315">
       <c r="A315" s="23" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B315" s="42">
         <v>13.0</v>
@@ -35360,13 +35351,13 @@
     </row>
     <row r="316">
       <c r="A316" s="23" t="s">
+        <v>734</v>
+      </c>
+      <c r="B316" s="23" t="s">
         <v>735</v>
       </c>
-      <c r="B316" s="23" t="s">
-        <v>736</v>
-      </c>
       <c r="C316" s="23" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D316" s="23"/>
       <c r="E316" s="23"/>
@@ -35394,13 +35385,13 @@
     </row>
     <row r="317">
       <c r="A317" s="23" t="s">
+        <v>736</v>
+      </c>
+      <c r="B317" s="23" t="s">
         <v>737</v>
       </c>
-      <c r="B317" s="23" t="s">
-        <v>738</v>
-      </c>
       <c r="C317" s="23" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D317" s="23"/>
       <c r="E317" s="23"/>
@@ -35428,13 +35419,13 @@
     </row>
     <row r="318">
       <c r="A318" s="23" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B318" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C318" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D318" s="23"/>
       <c r="E318" s="23"/>
@@ -35462,13 +35453,13 @@
     </row>
     <row r="319">
       <c r="A319" s="23" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B319" s="23" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C319" s="23" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D319" s="23"/>
       <c r="E319" s="23"/>
@@ -35496,7 +35487,7 @@
     </row>
     <row r="320">
       <c r="A320" s="23" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B320" s="42">
         <v>6.0</v>
@@ -35530,13 +35521,13 @@
     </row>
     <row r="321">
       <c r="A321" s="23" t="s">
+        <v>741</v>
+      </c>
+      <c r="B321" s="23" t="s">
         <v>742</v>
       </c>
-      <c r="B321" s="23" t="s">
-        <v>743</v>
-      </c>
       <c r="C321" s="23" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="D321" s="23"/>
       <c r="E321" s="23"/>
@@ -35564,13 +35555,13 @@
     </row>
     <row r="322">
       <c r="A322" s="23" t="s">
+        <v>743</v>
+      </c>
+      <c r="B322" s="23" t="s">
         <v>744</v>
       </c>
-      <c r="B322" s="23" t="s">
-        <v>745</v>
-      </c>
       <c r="C322" s="23" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D322" s="23"/>
       <c r="E322" s="23"/>
@@ -35598,13 +35589,13 @@
     </row>
     <row r="323">
       <c r="A323" s="23" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B323" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C323" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D323" s="23"/>
       <c r="E323" s="23"/>
@@ -35632,13 +35623,13 @@
     </row>
     <row r="324">
       <c r="A324" s="23" t="s">
+        <v>746</v>
+      </c>
+      <c r="B324" s="23" t="s">
         <v>747</v>
       </c>
-      <c r="B324" s="23" t="s">
-        <v>748</v>
-      </c>
       <c r="C324" s="23" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D324" s="23"/>
       <c r="E324" s="23"/>
@@ -35666,7 +35657,7 @@
     </row>
     <row r="325">
       <c r="A325" s="23" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B325" s="42">
         <v>7.0</v>
@@ -35700,13 +35691,13 @@
     </row>
     <row r="326">
       <c r="A326" s="23" t="s">
+        <v>749</v>
+      </c>
+      <c r="B326" s="23" t="s">
         <v>750</v>
       </c>
-      <c r="B326" s="23" t="s">
-        <v>751</v>
-      </c>
       <c r="C326" s="23" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D326" s="23"/>
       <c r="E326" s="23"/>
@@ -35734,13 +35725,13 @@
     </row>
     <row r="327">
       <c r="A327" s="23" t="s">
+        <v>751</v>
+      </c>
+      <c r="B327" s="23" t="s">
         <v>752</v>
       </c>
-      <c r="B327" s="23" t="s">
-        <v>753</v>
-      </c>
       <c r="C327" s="23" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D327" s="23"/>
       <c r="E327" s="23"/>
@@ -35768,13 +35759,13 @@
     </row>
     <row r="328">
       <c r="A328" s="23" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B328" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C328" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D328" s="23"/>
       <c r="E328" s="23"/>
@@ -35802,13 +35793,13 @@
     </row>
     <row r="329">
       <c r="A329" s="23" t="s">
+        <v>754</v>
+      </c>
+      <c r="B329" s="23" t="s">
         <v>755</v>
       </c>
-      <c r="B329" s="23" t="s">
-        <v>756</v>
-      </c>
       <c r="C329" s="23" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D329" s="23"/>
       <c r="E329" s="23"/>
@@ -35836,7 +35827,7 @@
     </row>
     <row r="330">
       <c r="A330" s="23" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B330" s="42">
         <v>3.0</v>
@@ -35870,13 +35861,13 @@
     </row>
     <row r="331">
       <c r="A331" s="23" t="s">
+        <v>757</v>
+      </c>
+      <c r="B331" s="23" t="s">
         <v>758</v>
       </c>
-      <c r="B331" s="23" t="s">
-        <v>759</v>
-      </c>
       <c r="C331" s="23" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D331" s="23"/>
       <c r="E331" s="23"/>
@@ -35904,13 +35895,13 @@
     </row>
     <row r="332">
       <c r="A332" s="23" t="s">
+        <v>759</v>
+      </c>
+      <c r="B332" s="23" t="s">
         <v>760</v>
       </c>
-      <c r="B332" s="23" t="s">
-        <v>761</v>
-      </c>
       <c r="C332" s="23" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D332" s="23"/>
       <c r="E332" s="23"/>
@@ -35938,13 +35929,13 @@
     </row>
     <row r="333">
       <c r="A333" s="23" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B333" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C333" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D333" s="23"/>
       <c r="E333" s="23"/>
@@ -35972,13 +35963,13 @@
     </row>
     <row r="334">
       <c r="A334" s="23" t="s">
+        <v>762</v>
+      </c>
+      <c r="B334" s="23" t="s">
         <v>763</v>
       </c>
-      <c r="B334" s="23" t="s">
-        <v>764</v>
-      </c>
       <c r="C334" s="23" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D334" s="23"/>
       <c r="E334" s="23"/>
@@ -36006,7 +35997,7 @@
     </row>
     <row r="335">
       <c r="A335" s="23" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B335" s="42">
         <v>3.0</v>
@@ -36040,13 +36031,13 @@
     </row>
     <row r="336">
       <c r="A336" s="23" t="s">
+        <v>765</v>
+      </c>
+      <c r="B336" s="23" t="s">
         <v>766</v>
       </c>
-      <c r="B336" s="23" t="s">
-        <v>767</v>
-      </c>
       <c r="C336" s="23" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D336" s="23"/>
       <c r="E336" s="23"/>
@@ -36074,13 +36065,13 @@
     </row>
     <row r="337">
       <c r="A337" s="23" t="s">
+        <v>767</v>
+      </c>
+      <c r="B337" s="23" t="s">
         <v>768</v>
       </c>
-      <c r="B337" s="23" t="s">
-        <v>769</v>
-      </c>
       <c r="C337" s="23" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D337" s="23"/>
       <c r="E337" s="23"/>
@@ -36108,13 +36099,13 @@
     </row>
     <row r="338">
       <c r="A338" s="23" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B338" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C338" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D338" s="23"/>
       <c r="E338" s="23"/>
@@ -36142,13 +36133,13 @@
     </row>
     <row r="339">
       <c r="A339" s="23" t="s">
+        <v>770</v>
+      </c>
+      <c r="B339" s="23" t="s">
         <v>771</v>
       </c>
-      <c r="B339" s="23" t="s">
-        <v>772</v>
-      </c>
       <c r="C339" s="23" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D339" s="23"/>
       <c r="E339" s="23"/>
@@ -36176,7 +36167,7 @@
     </row>
     <row r="340">
       <c r="A340" s="23" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B340" s="42">
         <v>3.0</v>
@@ -36210,13 +36201,13 @@
     </row>
     <row r="341">
       <c r="A341" s="23" t="s">
+        <v>773</v>
+      </c>
+      <c r="B341" s="23" t="s">
         <v>774</v>
       </c>
-      <c r="B341" s="23" t="s">
-        <v>775</v>
-      </c>
       <c r="C341" s="23" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D341" s="23"/>
       <c r="E341" s="23"/>
@@ -36244,13 +36235,13 @@
     </row>
     <row r="342">
       <c r="A342" s="23" t="s">
+        <v>775</v>
+      </c>
+      <c r="B342" s="23" t="s">
         <v>776</v>
       </c>
-      <c r="B342" s="23" t="s">
-        <v>777</v>
-      </c>
       <c r="C342" s="23" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D342" s="23"/>
       <c r="E342" s="23"/>
@@ -36278,13 +36269,13 @@
     </row>
     <row r="343">
       <c r="A343" s="23" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B343" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C343" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D343" s="23"/>
       <c r="E343" s="23"/>
@@ -36312,13 +36303,13 @@
     </row>
     <row r="344">
       <c r="A344" s="23" t="s">
+        <v>778</v>
+      </c>
+      <c r="B344" s="41" t="s">
         <v>779</v>
       </c>
-      <c r="B344" s="41" t="s">
-        <v>780</v>
-      </c>
       <c r="C344" s="41" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D344" s="23"/>
       <c r="E344" s="23"/>
@@ -36346,7 +36337,7 @@
     </row>
     <row r="345">
       <c r="A345" s="23" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B345" s="42">
         <v>3.0</v>
@@ -36380,13 +36371,13 @@
     </row>
     <row r="346">
       <c r="A346" s="23" t="s">
+        <v>781</v>
+      </c>
+      <c r="B346" s="23" t="s">
         <v>782</v>
       </c>
-      <c r="B346" s="23" t="s">
-        <v>783</v>
-      </c>
       <c r="C346" s="23" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D346" s="23"/>
       <c r="E346" s="23"/>
@@ -36414,13 +36405,13 @@
     </row>
     <row r="347">
       <c r="A347" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="B347" s="23" t="s">
         <v>784</v>
       </c>
-      <c r="B347" s="23" t="s">
-        <v>785</v>
-      </c>
       <c r="C347" s="23" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D347" s="23"/>
       <c r="E347" s="23"/>
@@ -36448,13 +36439,13 @@
     </row>
     <row r="348">
       <c r="A348" s="23" t="s">
+        <v>785</v>
+      </c>
+      <c r="B348" s="23" t="s">
         <v>786</v>
       </c>
-      <c r="B348" s="23" t="s">
-        <v>787</v>
-      </c>
       <c r="C348" s="23" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D348" s="23"/>
       <c r="E348" s="23"/>
@@ -36482,13 +36473,13 @@
     </row>
     <row r="349">
       <c r="A349" s="23" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B349" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C349" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D349" s="23"/>
       <c r="E349" s="23"/>
@@ -36516,13 +36507,13 @@
     </row>
     <row r="350">
       <c r="A350" s="23" t="s">
+        <v>788</v>
+      </c>
+      <c r="B350" s="42" t="s">
         <v>789</v>
       </c>
-      <c r="B350" s="42" t="s">
-        <v>790</v>
-      </c>
       <c r="C350" s="42" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D350" s="23"/>
       <c r="E350" s="23"/>
@@ -36550,7 +36541,7 @@
     </row>
     <row r="351">
       <c r="A351" s="23" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B351" s="42">
         <v>6.0</v>
@@ -36584,13 +36575,13 @@
     </row>
     <row r="352">
       <c r="A352" s="23" t="s">
+        <v>791</v>
+      </c>
+      <c r="B352" s="23" t="s">
         <v>792</v>
       </c>
-      <c r="B352" s="23" t="s">
-        <v>793</v>
-      </c>
       <c r="C352" s="23" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D352" s="23"/>
       <c r="E352" s="23"/>
@@ -36618,13 +36609,13 @@
     </row>
     <row r="353">
       <c r="A353" s="23" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B353" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C353" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D353" s="23"/>
       <c r="E353" s="23"/>
@@ -36652,13 +36643,13 @@
     </row>
     <row r="354">
       <c r="A354" s="23" t="s">
+        <v>794</v>
+      </c>
+      <c r="B354" s="23" t="s">
         <v>795</v>
       </c>
-      <c r="B354" s="23" t="s">
-        <v>796</v>
-      </c>
       <c r="C354" s="23" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D354" s="23"/>
       <c r="E354" s="23"/>
@@ -36686,7 +36677,7 @@
     </row>
     <row r="355">
       <c r="A355" s="23" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B355" s="42">
         <v>50.0</v>
@@ -36720,7 +36711,7 @@
     </row>
     <row r="356">
       <c r="A356" s="23" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B356" s="42">
         <v>55.0</v>
@@ -36754,13 +36745,13 @@
     </row>
     <row r="357">
       <c r="A357" s="23" t="s">
+        <v>798</v>
+      </c>
+      <c r="B357" s="23" t="s">
         <v>799</v>
       </c>
-      <c r="B357" s="23" t="s">
-        <v>800</v>
-      </c>
       <c r="C357" s="23" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D357" s="23"/>
       <c r="E357" s="23"/>
@@ -36788,13 +36779,13 @@
     </row>
     <row r="358">
       <c r="A358" s="23" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B358" s="23" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C358" s="23" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D358" s="23"/>
       <c r="E358" s="23"/>
@@ -36822,13 +36813,13 @@
     </row>
     <row r="359">
       <c r="A359" s="23" t="s">
+        <v>801</v>
+      </c>
+      <c r="B359" s="23" t="s">
         <v>802</v>
       </c>
-      <c r="B359" s="23" t="s">
-        <v>803</v>
-      </c>
       <c r="C359" s="23" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D359" s="23"/>
       <c r="E359" s="23"/>
@@ -36856,13 +36847,13 @@
     </row>
     <row r="360">
       <c r="A360" s="23" t="s">
+        <v>803</v>
+      </c>
+      <c r="B360" s="23" t="s">
         <v>804</v>
       </c>
-      <c r="B360" s="23" t="s">
-        <v>805</v>
-      </c>
       <c r="C360" s="23" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D360" s="23"/>
       <c r="E360" s="23"/>
@@ -36890,13 +36881,13 @@
     </row>
     <row r="361">
       <c r="A361" s="23" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B361" s="23" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C361" s="23" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D361" s="23"/>
       <c r="E361" s="23"/>
@@ -36924,13 +36915,13 @@
     </row>
     <row r="362">
       <c r="A362" s="23" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B362" s="23" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C362" s="23" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D362" s="23"/>
       <c r="E362" s="23"/>
@@ -36958,13 +36949,13 @@
     </row>
     <row r="363">
       <c r="A363" s="23" t="s">
+        <v>807</v>
+      </c>
+      <c r="B363" s="23" t="s">
         <v>808</v>
       </c>
-      <c r="B363" s="23" t="s">
-        <v>809</v>
-      </c>
       <c r="C363" s="23" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D363" s="23"/>
       <c r="E363" s="23"/>
@@ -36992,13 +36983,13 @@
     </row>
     <row r="364">
       <c r="A364" s="23" t="s">
+        <v>809</v>
+      </c>
+      <c r="B364" s="23" t="s">
         <v>810</v>
       </c>
-      <c r="B364" s="23" t="s">
-        <v>811</v>
-      </c>
       <c r="C364" s="23" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D364" s="23"/>
       <c r="E364" s="23"/>
@@ -37026,13 +37017,13 @@
     </row>
     <row r="365">
       <c r="A365" s="23" t="s">
+        <v>811</v>
+      </c>
+      <c r="B365" s="23" t="s">
         <v>812</v>
       </c>
-      <c r="B365" s="23" t="s">
-        <v>813</v>
-      </c>
       <c r="C365" s="23" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D365" s="23"/>
       <c r="E365" s="23"/>
@@ -37060,13 +37051,13 @@
     </row>
     <row r="366">
       <c r="A366" s="23" t="s">
+        <v>813</v>
+      </c>
+      <c r="B366" s="23" t="s">
         <v>814</v>
       </c>
-      <c r="B366" s="23" t="s">
-        <v>815</v>
-      </c>
       <c r="C366" s="23" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D366" s="23"/>
       <c r="E366" s="23"/>
@@ -37094,13 +37085,13 @@
     </row>
     <row r="367">
       <c r="A367" s="23" t="s">
+        <v>815</v>
+      </c>
+      <c r="B367" s="23" t="s">
         <v>816</v>
       </c>
-      <c r="B367" s="23" t="s">
-        <v>817</v>
-      </c>
       <c r="C367" s="23" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D367" s="23"/>
       <c r="E367" s="23"/>
@@ -37128,13 +37119,13 @@
     </row>
     <row r="368">
       <c r="A368" s="23" t="s">
+        <v>817</v>
+      </c>
+      <c r="B368" s="23" t="s">
         <v>818</v>
       </c>
-      <c r="B368" s="23" t="s">
-        <v>819</v>
-      </c>
       <c r="C368" s="23" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D368" s="23"/>
       <c r="E368" s="23"/>
@@ -37162,13 +37153,13 @@
     </row>
     <row r="369">
       <c r="A369" s="23" t="s">
+        <v>819</v>
+      </c>
+      <c r="B369" s="23" t="s">
         <v>820</v>
       </c>
-      <c r="B369" s="23" t="s">
-        <v>821</v>
-      </c>
       <c r="C369" s="23" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D369" s="23"/>
       <c r="E369" s="23"/>
@@ -37196,13 +37187,13 @@
     </row>
     <row r="370">
       <c r="A370" s="23" t="s">
+        <v>821</v>
+      </c>
+      <c r="B370" s="23" t="s">
         <v>822</v>
       </c>
-      <c r="B370" s="23" t="s">
-        <v>823</v>
-      </c>
       <c r="C370" s="23" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D370" s="23"/>
       <c r="E370" s="23"/>
@@ -37230,13 +37221,13 @@
     </row>
     <row r="371">
       <c r="A371" s="23" t="s">
+        <v>823</v>
+      </c>
+      <c r="B371" s="23" t="s">
         <v>824</v>
       </c>
-      <c r="B371" s="23" t="s">
-        <v>825</v>
-      </c>
       <c r="C371" s="23" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D371" s="23"/>
       <c r="E371" s="23"/>
@@ -37264,13 +37255,13 @@
     </row>
     <row r="372">
       <c r="A372" s="23" t="s">
+        <v>825</v>
+      </c>
+      <c r="B372" s="23" t="s">
         <v>826</v>
       </c>
-      <c r="B372" s="23" t="s">
-        <v>827</v>
-      </c>
       <c r="C372" s="23" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D372" s="23"/>
       <c r="E372" s="23"/>
@@ -37298,13 +37289,13 @@
     </row>
     <row r="373">
       <c r="A373" s="23" t="s">
+        <v>827</v>
+      </c>
+      <c r="B373" s="23" t="s">
         <v>828</v>
       </c>
-      <c r="B373" s="23" t="s">
-        <v>829</v>
-      </c>
       <c r="C373" s="23" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D373" s="23"/>
       <c r="E373" s="23"/>
@@ -37457,7 +37448,7 @@
     </row>
     <row r="379">
       <c r="B379" s="34" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D379" s="23"/>
       <c r="E379" s="23"/>
@@ -37560,13 +37551,13 @@
     </row>
     <row r="383">
       <c r="A383" s="23" t="s">
+        <v>830</v>
+      </c>
+      <c r="B383" s="23" t="s">
         <v>831</v>
       </c>
-      <c r="B383" s="23" t="s">
-        <v>832</v>
-      </c>
       <c r="C383" s="23" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D383" s="23"/>
       <c r="E383" s="23"/>
@@ -37594,13 +37585,13 @@
     </row>
     <row r="384">
       <c r="A384" s="23" t="s">
+        <v>832</v>
+      </c>
+      <c r="B384" s="23" t="s">
         <v>833</v>
       </c>
-      <c r="B384" s="23" t="s">
-        <v>834</v>
-      </c>
       <c r="C384" s="23" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D384" s="23"/>
       <c r="E384" s="23"/>
@@ -37628,13 +37619,13 @@
     </row>
     <row r="385">
       <c r="A385" s="23" t="s">
+        <v>834</v>
+      </c>
+      <c r="B385" s="23" t="s">
         <v>835</v>
       </c>
-      <c r="B385" s="23" t="s">
-        <v>836</v>
-      </c>
       <c r="C385" s="23" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D385" s="23"/>
       <c r="E385" s="23"/>
@@ -37662,13 +37653,13 @@
     </row>
     <row r="386">
       <c r="A386" s="23" t="s">
+        <v>836</v>
+      </c>
+      <c r="B386" s="23" t="s">
         <v>837</v>
       </c>
-      <c r="B386" s="23" t="s">
-        <v>838</v>
-      </c>
       <c r="C386" s="23" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D386" s="23"/>
       <c r="E386" s="23"/>
@@ -37696,13 +37687,13 @@
     </row>
     <row r="387">
       <c r="A387" s="23" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B387" s="23" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C387" s="23" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D387" s="23"/>
       <c r="E387" s="23"/>
@@ -37730,13 +37721,13 @@
     </row>
     <row r="388">
       <c r="A388" s="23" t="s">
+        <v>839</v>
+      </c>
+      <c r="B388" s="23" t="s">
         <v>840</v>
       </c>
-      <c r="B388" s="23" t="s">
-        <v>841</v>
-      </c>
       <c r="C388" s="23" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D388" s="23"/>
       <c r="E388" s="23"/>
@@ -37789,7 +37780,7 @@
     </row>
     <row r="390">
       <c r="B390" s="34" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D390" s="23"/>
       <c r="E390" s="23"/>
@@ -37867,13 +37858,13 @@
     </row>
     <row r="393">
       <c r="A393" s="23" t="s">
+        <v>842</v>
+      </c>
+      <c r="B393" s="23" t="s">
         <v>843</v>
       </c>
-      <c r="B393" s="23" t="s">
-        <v>844</v>
-      </c>
       <c r="C393" s="23" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D393" s="23"/>
       <c r="E393" s="23"/>
@@ -37901,13 +37892,13 @@
     </row>
     <row r="394">
       <c r="A394" s="23" t="s">
+        <v>844</v>
+      </c>
+      <c r="B394" s="23" t="s">
         <v>845</v>
       </c>
-      <c r="B394" s="23" t="s">
-        <v>846</v>
-      </c>
       <c r="C394" s="23" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D394" s="23"/>
       <c r="E394" s="23"/>
@@ -37935,13 +37926,13 @@
     </row>
     <row r="395">
       <c r="A395" s="23" t="s">
+        <v>846</v>
+      </c>
+      <c r="B395" s="23" t="s">
         <v>847</v>
       </c>
-      <c r="B395" s="23" t="s">
-        <v>848</v>
-      </c>
       <c r="C395" s="23" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D395" s="23"/>
       <c r="E395" s="23"/>
@@ -37969,13 +37960,13 @@
     </row>
     <row r="396">
       <c r="A396" s="23" t="s">
+        <v>848</v>
+      </c>
+      <c r="B396" s="23" t="s">
         <v>849</v>
       </c>
-      <c r="B396" s="23" t="s">
-        <v>850</v>
-      </c>
       <c r="C396" s="23" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D396" s="23"/>
       <c r="E396" s="23"/>
@@ -38003,13 +37994,13 @@
     </row>
     <row r="397">
       <c r="A397" s="23" t="s">
+        <v>850</v>
+      </c>
+      <c r="B397" s="23" t="s">
         <v>851</v>
       </c>
-      <c r="B397" s="23" t="s">
-        <v>852</v>
-      </c>
       <c r="C397" s="23" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="D397" s="23"/>
       <c r="E397" s="23"/>
@@ -38037,13 +38028,13 @@
     </row>
     <row r="398">
       <c r="A398" s="23" t="s">
+        <v>852</v>
+      </c>
+      <c r="B398" s="23" t="s">
         <v>853</v>
       </c>
-      <c r="B398" s="23" t="s">
-        <v>854</v>
-      </c>
       <c r="C398" s="23" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D398" s="23"/>
       <c r="E398" s="23"/>
@@ -38071,13 +38062,13 @@
     </row>
     <row r="399">
       <c r="A399" s="23" t="s">
+        <v>854</v>
+      </c>
+      <c r="B399" s="23" t="s">
         <v>855</v>
       </c>
-      <c r="B399" s="23" t="s">
-        <v>856</v>
-      </c>
       <c r="C399" s="23" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D399" s="23"/>
       <c r="E399" s="23"/>
@@ -38105,13 +38096,13 @@
     </row>
     <row r="400">
       <c r="A400" s="23" t="s">
+        <v>856</v>
+      </c>
+      <c r="B400" s="23" t="s">
         <v>857</v>
       </c>
-      <c r="B400" s="23" t="s">
-        <v>858</v>
-      </c>
       <c r="C400" s="23" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D400" s="23"/>
       <c r="E400" s="23"/>
@@ -38139,13 +38130,13 @@
     </row>
     <row r="401">
       <c r="A401" s="23" t="s">
+        <v>858</v>
+      </c>
+      <c r="B401" s="23" t="s">
         <v>859</v>
       </c>
-      <c r="B401" s="23" t="s">
-        <v>860</v>
-      </c>
       <c r="C401" s="23" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D401" s="23"/>
       <c r="E401" s="23"/>
@@ -38173,13 +38164,13 @@
     </row>
     <row r="402">
       <c r="A402" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="B402" s="23" t="s">
         <v>861</v>
       </c>
-      <c r="B402" s="23" t="s">
-        <v>862</v>
-      </c>
       <c r="C402" s="23" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D402" s="23"/>
       <c r="E402" s="23"/>
@@ -38207,13 +38198,13 @@
     </row>
     <row r="403">
       <c r="A403" s="23" t="s">
+        <v>862</v>
+      </c>
+      <c r="B403" s="23" t="s">
         <v>863</v>
       </c>
-      <c r="B403" s="23" t="s">
-        <v>864</v>
-      </c>
       <c r="C403" s="23" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D403" s="23"/>
       <c r="E403" s="23"/>
@@ -38241,13 +38232,13 @@
     </row>
     <row r="404">
       <c r="A404" s="23" t="s">
+        <v>864</v>
+      </c>
+      <c r="B404" s="23" t="s">
         <v>865</v>
       </c>
-      <c r="B404" s="23" t="s">
-        <v>866</v>
-      </c>
       <c r="C404" s="23" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D404" s="23"/>
       <c r="E404" s="23"/>
@@ -38275,13 +38266,13 @@
     </row>
     <row r="405">
       <c r="A405" s="23" t="s">
+        <v>866</v>
+      </c>
+      <c r="B405" s="23" t="s">
         <v>867</v>
       </c>
-      <c r="B405" s="23" t="s">
-        <v>868</v>
-      </c>
       <c r="C405" s="23" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D405" s="23"/>
       <c r="E405" s="23"/>
@@ -38309,13 +38300,13 @@
     </row>
     <row r="406">
       <c r="A406" s="23" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B406" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C406" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D406" s="23"/>
       <c r="E406" s="23"/>
@@ -38343,13 +38334,13 @@
     </row>
     <row r="407">
       <c r="A407" s="23" t="s">
+        <v>869</v>
+      </c>
+      <c r="B407" s="23" t="s">
         <v>870</v>
       </c>
-      <c r="B407" s="23" t="s">
-        <v>871</v>
-      </c>
       <c r="C407" s="23" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D407" s="23"/>
       <c r="E407" s="23"/>
@@ -38377,13 +38368,13 @@
     </row>
     <row r="408">
       <c r="A408" s="23" t="s">
+        <v>871</v>
+      </c>
+      <c r="B408" s="23" t="s">
         <v>872</v>
       </c>
-      <c r="B408" s="23" t="s">
-        <v>873</v>
-      </c>
       <c r="C408" s="23" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="D408" s="23"/>
       <c r="E408" s="23"/>
@@ -38411,13 +38402,13 @@
     </row>
     <row r="409">
       <c r="A409" s="23" t="s">
+        <v>873</v>
+      </c>
+      <c r="B409" s="23" t="s">
         <v>874</v>
       </c>
-      <c r="B409" s="23" t="s">
-        <v>875</v>
-      </c>
       <c r="C409" s="23" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="D409" s="23"/>
       <c r="E409" s="23"/>
@@ -38445,13 +38436,13 @@
     </row>
     <row r="410">
       <c r="A410" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="B410" s="23" t="s">
         <v>876</v>
       </c>
-      <c r="B410" s="23" t="s">
-        <v>877</v>
-      </c>
       <c r="C410" s="23" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D410" s="23"/>
       <c r="E410" s="23"/>
@@ -38479,13 +38470,13 @@
     </row>
     <row r="411">
       <c r="A411" s="23" t="s">
+        <v>877</v>
+      </c>
+      <c r="B411" s="23" t="s">
         <v>878</v>
       </c>
-      <c r="B411" s="23" t="s">
-        <v>879</v>
-      </c>
       <c r="C411" s="23" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D411" s="23"/>
       <c r="E411" s="23"/>
@@ -38513,13 +38504,13 @@
     </row>
     <row r="412">
       <c r="A412" s="23" t="s">
+        <v>879</v>
+      </c>
+      <c r="B412" s="23" t="s">
         <v>880</v>
       </c>
-      <c r="B412" s="23" t="s">
-        <v>881</v>
-      </c>
       <c r="C412" s="23" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="D412" s="23"/>
       <c r="E412" s="23"/>
@@ -38547,13 +38538,13 @@
     </row>
     <row r="413">
       <c r="A413" s="23" t="s">
+        <v>881</v>
+      </c>
+      <c r="B413" s="23" t="s">
         <v>882</v>
       </c>
-      <c r="B413" s="23" t="s">
-        <v>883</v>
-      </c>
       <c r="C413" s="23" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D413" s="23"/>
       <c r="E413" s="23"/>
@@ -38581,13 +38572,13 @@
     </row>
     <row r="414">
       <c r="A414" s="23" t="s">
+        <v>883</v>
+      </c>
+      <c r="B414" s="23" t="s">
         <v>884</v>
       </c>
-      <c r="B414" s="23" t="s">
-        <v>885</v>
-      </c>
       <c r="C414" s="23" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D414" s="23"/>
       <c r="E414" s="23"/>
@@ -38615,13 +38606,13 @@
     </row>
     <row r="415">
       <c r="A415" s="23" t="s">
+        <v>885</v>
+      </c>
+      <c r="B415" s="23" t="s">
         <v>886</v>
       </c>
-      <c r="B415" s="23" t="s">
-        <v>887</v>
-      </c>
       <c r="C415" s="23" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D415" s="23"/>
       <c r="E415" s="23"/>
@@ -38649,13 +38640,13 @@
     </row>
     <row r="416">
       <c r="A416" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="B416" s="23" t="s">
         <v>888</v>
       </c>
-      <c r="B416" s="23" t="s">
-        <v>889</v>
-      </c>
       <c r="C416" s="23" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D416" s="23"/>
       <c r="E416" s="23"/>
@@ -38683,13 +38674,13 @@
     </row>
     <row r="417">
       <c r="A417" s="23" t="s">
+        <v>889</v>
+      </c>
+      <c r="B417" s="23" t="s">
         <v>890</v>
       </c>
-      <c r="B417" s="23" t="s">
-        <v>891</v>
-      </c>
       <c r="C417" s="23" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D417" s="23"/>
       <c r="E417" s="23"/>
@@ -38717,13 +38708,13 @@
     </row>
     <row r="418">
       <c r="A418" s="23" t="s">
+        <v>891</v>
+      </c>
+      <c r="B418" s="23" t="s">
         <v>892</v>
       </c>
-      <c r="B418" s="23" t="s">
-        <v>893</v>
-      </c>
       <c r="C418" s="23" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D418" s="23"/>
       <c r="E418" s="23"/>
@@ -38751,13 +38742,13 @@
     </row>
     <row r="419">
       <c r="A419" s="23" t="s">
+        <v>893</v>
+      </c>
+      <c r="B419" s="23" t="s">
         <v>894</v>
       </c>
-      <c r="B419" s="23" t="s">
-        <v>895</v>
-      </c>
       <c r="C419" s="23" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D419" s="23"/>
       <c r="E419" s="23"/>
@@ -38785,13 +38776,13 @@
     </row>
     <row r="420">
       <c r="A420" s="23" t="s">
+        <v>895</v>
+      </c>
+      <c r="B420" s="23" t="s">
         <v>896</v>
       </c>
-      <c r="B420" s="23" t="s">
-        <v>897</v>
-      </c>
       <c r="C420" s="23" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="D420" s="23"/>
       <c r="E420" s="23"/>
@@ -38819,13 +38810,13 @@
     </row>
     <row r="421">
       <c r="A421" s="23" t="s">
+        <v>897</v>
+      </c>
+      <c r="B421" s="23" t="s">
         <v>898</v>
       </c>
-      <c r="B421" s="23" t="s">
-        <v>899</v>
-      </c>
       <c r="C421" s="23" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D421" s="23"/>
       <c r="E421" s="23"/>
@@ -38853,13 +38844,13 @@
     </row>
     <row r="422">
       <c r="A422" s="23" t="s">
+        <v>899</v>
+      </c>
+      <c r="B422" s="23" t="s">
         <v>900</v>
       </c>
-      <c r="B422" s="23" t="s">
-        <v>901</v>
-      </c>
       <c r="C422" s="23" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D422" s="23"/>
       <c r="E422" s="23"/>
@@ -38887,13 +38878,13 @@
     </row>
     <row r="423">
       <c r="A423" s="23" t="s">
+        <v>901</v>
+      </c>
+      <c r="B423" s="23" t="s">
         <v>902</v>
       </c>
-      <c r="B423" s="23" t="s">
-        <v>903</v>
-      </c>
       <c r="C423" s="23" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D423" s="23"/>
       <c r="E423" s="23"/>
@@ -38921,13 +38912,13 @@
     </row>
     <row r="424">
       <c r="A424" s="23" t="s">
+        <v>903</v>
+      </c>
+      <c r="B424" s="23" t="s">
         <v>904</v>
       </c>
-      <c r="B424" s="23" t="s">
-        <v>905</v>
-      </c>
       <c r="C424" s="23" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D424" s="23"/>
       <c r="E424" s="23"/>
@@ -38955,13 +38946,13 @@
     </row>
     <row r="425">
       <c r="A425" s="23" t="s">
+        <v>905</v>
+      </c>
+      <c r="B425" s="23" t="s">
         <v>906</v>
       </c>
-      <c r="B425" s="23" t="s">
-        <v>907</v>
-      </c>
       <c r="C425" s="23" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D425" s="23"/>
       <c r="E425" s="23"/>
@@ -38989,13 +38980,13 @@
     </row>
     <row r="426">
       <c r="A426" s="23" t="s">
+        <v>907</v>
+      </c>
+      <c r="B426" s="23" t="s">
         <v>908</v>
       </c>
-      <c r="B426" s="23" t="s">
-        <v>909</v>
-      </c>
       <c r="C426" s="23" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D426" s="23"/>
       <c r="E426" s="23"/>
@@ -39048,7 +39039,7 @@
     </row>
     <row r="428">
       <c r="B428" s="34" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D428" s="23"/>
       <c r="E428" s="23"/>
@@ -39126,13 +39117,13 @@
     </row>
     <row r="431">
       <c r="A431" s="23" t="s">
+        <v>910</v>
+      </c>
+      <c r="B431" s="23" t="s">
         <v>911</v>
       </c>
-      <c r="B431" s="23" t="s">
-        <v>912</v>
-      </c>
       <c r="C431" s="23" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D431" s="23"/>
       <c r="E431" s="23"/>
@@ -39160,7 +39151,7 @@
     </row>
     <row r="432">
       <c r="A432" s="23" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B432" s="23" t="s">
         <v>9</v>
@@ -54835,10 +54826,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="3">
@@ -54846,10 +54837,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="4">
@@ -54866,7 +54857,7 @@
     <row r="6">
       <c r="A6" s="45"/>
       <c r="B6" s="45" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C6" s="45"/>
     </row>
@@ -54877,13 +54868,13 @@
     </row>
     <row r="8">
       <c r="A8" s="16" t="s">
+        <v>916</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>917</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>918</v>
-      </c>
       <c r="C8" s="16" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="9">
@@ -54898,8 +54889,8 @@
     </row>
     <row r="11">
       <c r="A11" s="45"/>
-      <c r="B11" s="46" t="s">
-        <v>919</v>
+      <c r="B11" s="45" t="s">
+        <v>918</v>
       </c>
       <c r="C11" s="45"/>
     </row>
@@ -54909,14 +54900,14 @@
       <c r="C12" s="16"/>
     </row>
     <row r="13">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="46" t="s">
+        <v>919</v>
+      </c>
+      <c r="B13" s="46" t="s">
         <v>920</v>
       </c>
-      <c r="B13" s="47" t="s">
-        <v>921</v>
-      </c>
-      <c r="C13" s="47" t="s">
-        <v>921</v>
+      <c r="C13" s="46" t="s">
+        <v>920</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xpath changes in health Indicators 13/10/22
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sanity_Clone_12_10_22\config\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8D3221-01DC-492F-9DAA-5A1348594627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9851C56-C0F5-4CC4-853C-9DB80FF92A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25305,8 +25305,8 @@
   </sheetPr>
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C68" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -25920,7 +25920,7 @@
       <c r="A76" s="22" t="s">
         <v>531</v>
       </c>
-      <c r="B76" s="29" t="s">
+      <c r="B76" s="48" t="s">
         <v>9</v>
       </c>
       <c r="C76" s="29" t="s">
@@ -29698,6 +29698,7 @@
     <hyperlink ref="C194" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
     <hyperlink ref="B77" r:id="rId6" xr:uid="{EF79774B-5E55-4254-93AB-697AF9EED9F8}"/>
     <hyperlink ref="C77" r:id="rId7" xr:uid="{3D3F534D-FB08-44A7-9645-ADDBC7CC15F1}"/>
+    <hyperlink ref="B76" r:id="rId8" xr:uid="{E20CB28C-6D32-4752-A0B9-EEC98C54D3E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
happy path xpath changes for the messages module 18/10/22
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -10,7 +10,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7miT7rtLTRt44S4b1wiI8V3Fb4qWIg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mi3VpcCn/1peu4J6BbD/OfinyPjGA=="/>
     </ext>
   </extLst>
 </workbook>
@@ -184,7 +184,7 @@
     <t>MORE INFO VERIFICATION DATA FOR PATIENT TO COLLECT PRESCRIPTION</t>
   </si>
   <si>
-    <t>Dr Tim ( VM04Practice );VM04Practice;Patient to Collect Script;Next Day - Fee: NZ$;panadol (optizorb) 500mg caplets(paracetamol);Pending</t>
+    <t>Dr Tim ( VM04Practice );VM04Practice;Patient to Collect Script;Next Day;panadol (optizorb) 500mg caplets(paracetamol);Pending</t>
   </si>
   <si>
     <t>DATA FOR SENT SCRIPT BY POST</t>
@@ -211,7 +211,7 @@
     <t>VERIFICATION DATA FOR SENT SCRIPT TO PHARMACY</t>
   </si>
   <si>
-    <t>VM04Practice;panadol (optizorb) 500mg caplets(paracetamol);pending;Chemist Warehouse Auckland - Lower Queen St;48 Hours - Fee: NZ$21.00 (Incl. GST);Kevin Peterson</t>
+    <t>VM04Practice;panadol (optizorb) 500mg caplets(paracetamol);pending;Chemist Warehouse Auckland - Lower Queen St;48 Hours;Kevin Peterson</t>
   </si>
   <si>
     <t>MORE INFO DATA FOR PRESCRIPTION BY SENT SCRIPT TO PHARMACY</t>
@@ -226,7 +226,7 @@
     <t>VERIFICATION DATA FOR DELIVERY MEDS BY PHARMACY</t>
   </si>
   <si>
-    <t>VM04Practice;panadol (optizorb) 500mg caplets(paracetamol);pending;ZOOM Pharmacy home delivery;48 Hours - Fee: NZ$25.00 (Incl. GST);Kevin Peterson</t>
+    <t>VM04Practice;panadol (optizorb) 500mg caplets(paracetamol);pending;ZOOM Pharmacy home delivery;48 Hours;Kevin Peterson</t>
   </si>
   <si>
     <t>MORE INFO DATA FOR DELIVERY MEDS BY PHARMACY</t>
@@ -265,7 +265,7 @@
     <t>URGENCY PRICE</t>
   </si>
   <si>
-    <t>Urgent/Same day  - Fee: $1.00 (Incl. GST);Next Day  -Fee: $2.00 (Incl. GST);48 Hours  - Fee: $3.00 (Incl. GST);72 Hours  - Fee: $4.00 (Incl. GST)</t>
+    <t>Urgent/Same day;Next Day;48 Hours;72 Hours</t>
   </si>
   <si>
     <t>EMAIL_FOR_HEALTH</t>
@@ -1688,10 +1688,10 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3258,10 +3258,10 @@
       <c r="A45" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D45" s="1"/>
@@ -3495,10 +3495,10 @@
       <c r="A54" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="7" t="s">
         <v>64</v>
       </c>
       <c r="D54" s="1"/>
@@ -3626,10 +3626,10 @@
       <c r="A59" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="7" t="s">
         <v>69</v>
       </c>
       <c r="D59" s="1"/>
@@ -3701,9 +3701,9 @@
       <c r="W61" s="1"/>
     </row>
     <row r="62" ht="13.5" customHeight="1">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -3760,10 +3760,10 @@
       <c r="A64" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="7" t="s">
         <v>69</v>
       </c>
       <c r="D64" s="1"/>
@@ -3866,10 +3866,10 @@
       <c r="A68" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="7" t="s">
         <v>69</v>
       </c>
       <c r="D68" s="1"/>
@@ -4034,10 +4034,10 @@
       <c r="A74" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="7" t="s">
         <v>82</v>
       </c>
       <c r="D74" s="1"/>

</xml_diff>

<commit_message>
safari fix For HappyPath (01/12/22)
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -12,7 +12,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mgyC/811pWS+pkQvkFcasU//uwJQw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mj8QzBXTqWXON1UIif699cO9DG7lA=="/>
     </ext>
   </extLst>
 </workbook>
@@ -1617,10 +1617,10 @@
     <t>PASSWORD_FOR_PROFILE</t>
   </si>
   <si>
+    <t>NEW_PASSWORD_FOR_PROFILE</t>
+  </si>
+  <si>
     <t>Manage@1234</t>
-  </si>
-  <si>
-    <t>NEW_PASSWORD_FOR_PROFILE</t>
   </si>
   <si>
     <t>ADDRESS_FOR_PROFILE</t>
@@ -3118,7 +3118,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3196,9 +3196,6 @@
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="15" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
@@ -26049,21 +26046,21 @@
         <v>531</v>
       </c>
       <c r="B76" s="28" t="s">
-        <v>532</v>
+        <v>9</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>532</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" ht="15.0" customHeight="1">
       <c r="A77" s="22" t="s">
+        <v>532</v>
+      </c>
+      <c r="B77" s="28" t="s">
         <v>533</v>
       </c>
-      <c r="B77" s="28" t="s">
-        <v>9</v>
-      </c>
       <c r="C77" s="28" t="s">
-        <v>9</v>
+        <v>533</v>
       </c>
     </row>
     <row r="79">
@@ -26640,10 +26637,10 @@
       <c r="A157" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B157" s="34" t="s">
+      <c r="B157" s="32" t="s">
         <v>620</v>
       </c>
-      <c r="C157" s="34" t="s">
+      <c r="C157" s="32" t="s">
         <v>620</v>
       </c>
     </row>
@@ -26817,56 +26814,56 @@
       </c>
     </row>
     <row r="188">
-      <c r="B188" s="35" t="s">
+      <c r="B188" s="34" t="s">
         <v>624</v>
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="36" t="s">
+      <c r="A193" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B193" s="37" t="s">
+      <c r="B193" s="36" t="s">
         <v>625</v>
       </c>
-      <c r="C193" s="37" t="s">
+      <c r="C193" s="36" t="s">
         <v>625</v>
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="36" t="s">
+      <c r="A194" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B194" s="38" t="s">
+      <c r="B194" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="C194" s="38" t="s">
+      <c r="C194" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="195">
-      <c r="A195" s="36" t="s">
+      <c r="A195" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B195" s="36" t="s">
+      <c r="B195" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C195" s="36" t="s">
+      <c r="C195" s="35" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="196">
-      <c r="A196" s="36" t="s">
+      <c r="A196" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="B196" s="36" t="s">
+      <c r="B196" s="35" t="s">
         <v>626</v>
       </c>
-      <c r="C196" s="36" t="s">
+      <c r="C196" s="35" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="36" t="s">
+      <c r="A197" s="35" t="s">
         <v>85</v>
       </c>
       <c r="B197" s="23" t="s">
@@ -26877,18 +26874,18 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="36" t="s">
+      <c r="A198" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="B198" s="39" t="s">
+      <c r="B198" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C198" s="39" t="s">
+      <c r="C198" s="38" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="36" t="s">
+      <c r="A199" s="35" t="s">
         <v>278</v>
       </c>
       <c r="B199" s="23" t="s">
@@ -26899,73 +26896,73 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" s="36" t="s">
+      <c r="A200" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="B200" s="36" t="s">
+      <c r="B200" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="C200" s="36" t="s">
+      <c r="C200" s="35" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="36" t="s">
+      <c r="A201" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="B201" s="36" t="s">
+      <c r="B201" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="C201" s="36" t="s">
+      <c r="C201" s="35" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="202">
-      <c r="A202" s="36" t="s">
+      <c r="A202" s="35" t="s">
         <v>207</v>
       </c>
-      <c r="B202" s="36" t="s">
+      <c r="B202" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="C202" s="36" t="s">
+      <c r="C202" s="35" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="36" t="s">
+      <c r="A203" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="B203" s="36" t="s">
+      <c r="B203" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="C203" s="36" t="s">
+      <c r="C203" s="35" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="36" t="s">
+      <c r="A204" s="35" t="s">
         <v>195</v>
       </c>
-      <c r="B204" s="36" t="s">
+      <c r="B204" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="C204" s="36" t="s">
+      <c r="C204" s="35" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="36" t="s">
+      <c r="A205" s="35" t="s">
         <v>286</v>
       </c>
-      <c r="B205" s="36" t="s">
+      <c r="B205" s="35" t="s">
         <v>287</v>
       </c>
-      <c r="C205" s="36" t="s">
+      <c r="C205" s="35" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="206">
-      <c r="A206" s="36" t="s">
+      <c r="A206" s="35" t="s">
         <v>163</v>
       </c>
       <c r="B206" s="23" t="s">
@@ -26976,18 +26973,18 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" s="36" t="s">
+      <c r="A207" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="B207" s="39" t="s">
+      <c r="B207" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="C207" s="39" t="s">
+      <c r="C207" s="38" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="208">
-      <c r="A208" s="36" t="s">
+      <c r="A208" s="35" t="s">
         <v>284</v>
       </c>
       <c r="B208" s="23" t="s">
@@ -26998,29 +26995,29 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" s="36" t="s">
+      <c r="A210" s="35" t="s">
         <v>330</v>
       </c>
-      <c r="B210" s="36" t="s">
+      <c r="B210" s="35" t="s">
         <v>331</v>
       </c>
-      <c r="C210" s="36" t="s">
+      <c r="C210" s="35" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="211">
-      <c r="A211" s="36" t="s">
+      <c r="A211" s="35" t="s">
         <v>627</v>
       </c>
-      <c r="B211" s="39" t="s">
+      <c r="B211" s="38" t="s">
         <v>628</v>
       </c>
-      <c r="C211" s="39" t="s">
+      <c r="C211" s="38" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="212">
-      <c r="A212" s="36" t="s">
+      <c r="A212" s="35" t="s">
         <v>334</v>
       </c>
       <c r="B212" s="23" t="s">
@@ -27031,7 +27028,7 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="36" t="s">
+      <c r="A213" s="35" t="s">
         <v>630</v>
       </c>
       <c r="B213" s="23" t="s">
@@ -27042,73 +27039,73 @@
       </c>
     </row>
     <row r="214">
-      <c r="A214" s="36" t="s">
+      <c r="A214" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="B214" s="36" t="s">
+      <c r="B214" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="C214" s="36" t="s">
+      <c r="C214" s="35" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="215">
-      <c r="A215" s="36" t="s">
+      <c r="A215" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="B215" s="39" t="s">
+      <c r="B215" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="C215" s="39" t="s">
+      <c r="C215" s="38" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="216">
-      <c r="A216" s="36" t="s">
+      <c r="A216" s="35" t="s">
         <v>288</v>
       </c>
-      <c r="B216" s="36" t="s">
+      <c r="B216" s="35" t="s">
         <v>289</v>
       </c>
-      <c r="C216" s="36" t="s">
+      <c r="C216" s="35" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="36" t="s">
+      <c r="A217" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="B217" s="36" t="s">
+      <c r="B217" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="C217" s="36" t="s">
+      <c r="C217" s="35" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="218">
-      <c r="A218" s="36" t="s">
+      <c r="A218" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="B218" s="36" t="s">
+      <c r="B218" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="C218" s="36" t="s">
+      <c r="C218" s="35" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="36" t="s">
+      <c r="A220" s="35" t="s">
         <v>631</v>
       </c>
-      <c r="B220" s="39" t="s">
+      <c r="B220" s="38" t="s">
         <v>632</v>
       </c>
-      <c r="C220" s="39" t="s">
+      <c r="C220" s="38" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="221">
-      <c r="A221" s="36" t="s">
+      <c r="A221" s="35" t="s">
         <v>633</v>
       </c>
       <c r="B221" s="23" t="s">
@@ -27119,430 +27116,430 @@
       </c>
     </row>
     <row r="222">
-      <c r="A222" s="36" t="s">
+      <c r="A222" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="B222" s="36" t="s">
+      <c r="B222" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="C222" s="36" t="s">
+      <c r="C222" s="35" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="223">
-      <c r="A223" s="36" t="s">
+      <c r="A223" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="B223" s="39" t="s">
+      <c r="B223" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="C223" s="39" t="s">
+      <c r="C223" s="38" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="224">
-      <c r="A224" s="36" t="s">
+      <c r="A224" s="35" t="s">
         <v>296</v>
       </c>
-      <c r="B224" s="36" t="s">
+      <c r="B224" s="35" t="s">
         <v>297</v>
       </c>
-      <c r="C224" s="36" t="s">
+      <c r="C224" s="35" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="36" t="s">
+      <c r="A225" s="35" t="s">
         <v>635</v>
       </c>
-      <c r="B225" s="36" t="s">
+      <c r="B225" s="35" t="s">
         <v>636</v>
       </c>
-      <c r="C225" s="36" t="s">
+      <c r="C225" s="35" t="s">
         <v>636</v>
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="36" t="s">
+      <c r="A226" s="35" t="s">
         <v>338</v>
       </c>
-      <c r="B226" s="36" t="s">
+      <c r="B226" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="C226" s="36" t="s">
+      <c r="C226" s="35" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="36" t="s">
+      <c r="A227" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="B227" s="36" t="s">
+      <c r="B227" s="35" t="s">
         <v>214</v>
       </c>
-      <c r="C227" s="36" t="s">
+      <c r="C227" s="35" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="228">
-      <c r="A228" s="36" t="s">
+      <c r="A228" s="35" t="s">
         <v>637</v>
       </c>
-      <c r="B228" s="36" t="s">
+      <c r="B228" s="35" t="s">
         <v>638</v>
       </c>
-      <c r="C228" s="36" t="s">
+      <c r="C228" s="35" t="s">
         <v>638</v>
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="36" t="s">
+      <c r="A229" s="35" t="s">
         <v>341</v>
       </c>
-      <c r="B229" s="36" t="s">
+      <c r="B229" s="35" t="s">
         <v>342</v>
       </c>
-      <c r="C229" s="36" t="s">
+      <c r="C229" s="35" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="36" t="s">
+      <c r="A230" s="35" t="s">
         <v>639</v>
       </c>
-      <c r="B230" s="39" t="s">
+      <c r="B230" s="38" t="s">
         <v>640</v>
       </c>
-      <c r="C230" s="39" t="s">
+      <c r="C230" s="38" t="s">
         <v>640</v>
       </c>
     </row>
     <row r="231">
-      <c r="A231" s="36" t="s">
+      <c r="A231" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B231" s="36" t="s">
+      <c r="B231" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="C231" s="36" t="s">
+      <c r="C231" s="35" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="232">
-      <c r="A232" s="36" t="s">
+      <c r="A232" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="B232" s="36" t="s">
+      <c r="B232" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="C232" s="36" t="s">
+      <c r="C232" s="35" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="234">
-      <c r="A234" s="36" t="s">
+      <c r="A234" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="B234" s="36" t="s">
+      <c r="B234" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="C234" s="36" t="s">
+      <c r="C234" s="35" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="235">
-      <c r="A235" s="36" t="s">
+      <c r="A235" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="B235" s="36" t="s">
+      <c r="B235" s="35" t="s">
         <v>214</v>
       </c>
-      <c r="C235" s="36" t="s">
+      <c r="C235" s="35" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="236">
-      <c r="A236" s="36" t="s">
+      <c r="A236" s="35" t="s">
         <v>641</v>
       </c>
-      <c r="B236" s="39" t="s">
+      <c r="B236" s="38" t="s">
         <v>642</v>
       </c>
-      <c r="C236" s="39" t="s">
+      <c r="C236" s="38" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="237">
-      <c r="A237" s="36" t="s">
+      <c r="A237" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="B237" s="36" t="s">
+      <c r="B237" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="C237" s="36" t="s">
+      <c r="C237" s="35" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="238">
-      <c r="A238" s="36" t="s">
+      <c r="A238" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="B238" s="36" t="s">
+      <c r="B238" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="C238" s="36" t="s">
+      <c r="C238" s="35" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="239">
-      <c r="A239" s="36" t="s">
+      <c r="A239" s="35" t="s">
         <v>643</v>
       </c>
-      <c r="B239" s="39" t="s">
+      <c r="B239" s="38" t="s">
         <v>644</v>
       </c>
-      <c r="C239" s="39" t="s">
+      <c r="C239" s="38" t="s">
         <v>644</v>
       </c>
     </row>
     <row r="240">
-      <c r="A240" s="36" t="s">
+      <c r="A240" s="35" t="s">
         <v>645</v>
       </c>
-      <c r="B240" s="39" t="s">
+      <c r="B240" s="38" t="s">
         <v>646</v>
       </c>
-      <c r="C240" s="39" t="s">
+      <c r="C240" s="38" t="s">
         <v>646</v>
       </c>
     </row>
     <row r="241">
-      <c r="A241" s="36" t="s">
+      <c r="A241" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="B241" s="39" t="s">
+      <c r="B241" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="C241" s="39" t="s">
+      <c r="C241" s="38" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="242">
-      <c r="A242" s="36" t="s">
+      <c r="A242" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="B242" s="36" t="s">
+      <c r="B242" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="C242" s="36" t="s">
+      <c r="C242" s="35" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="243">
-      <c r="A243" s="36" t="s">
+      <c r="A243" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="B243" s="39" t="s">
+      <c r="B243" s="38" t="s">
         <v>647</v>
       </c>
-      <c r="C243" s="39" t="s">
+      <c r="C243" s="38" t="s">
         <v>647</v>
       </c>
     </row>
     <row r="244">
-      <c r="A244" s="36" t="s">
+      <c r="A244" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="B244" s="40" t="s">
+      <c r="B244" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="C244" s="40" t="s">
+      <c r="C244" s="39" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="245">
-      <c r="A245" s="36" t="s">
+      <c r="A245" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="B245" s="36" t="s">
+      <c r="B245" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="C245" s="36" t="s">
+      <c r="C245" s="35" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="246">
-      <c r="A246" s="36" t="s">
+      <c r="A246" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="B246" s="36" t="s">
+      <c r="B246" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="C246" s="36" t="s">
+      <c r="C246" s="35" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="247">
-      <c r="A247" s="36" t="s">
+      <c r="A247" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B247" s="39" t="s">
+      <c r="B247" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="C247" s="39" t="s">
+      <c r="C247" s="38" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="248">
-      <c r="A248" s="36" t="s">
+      <c r="A248" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="B248" s="39" t="s">
+      <c r="B248" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="C248" s="39" t="s">
+      <c r="C248" s="38" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="249">
-      <c r="A249" s="36" t="s">
+      <c r="A249" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="B249" s="39" t="s">
+      <c r="B249" s="38" t="s">
         <v>192</v>
       </c>
-      <c r="C249" s="39" t="s">
+      <c r="C249" s="38" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="250">
-      <c r="A250" s="36" t="s">
+      <c r="A250" s="35" t="s">
         <v>648</v>
       </c>
-      <c r="B250" s="39" t="s">
+      <c r="B250" s="38" t="s">
         <v>649</v>
       </c>
-      <c r="C250" s="39" t="s">
+      <c r="C250" s="38" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="251">
-      <c r="A251" s="36" t="s">
+      <c r="A251" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="B251" s="39" t="s">
+      <c r="B251" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="C251" s="39" t="s">
+      <c r="C251" s="38" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="252">
-      <c r="A252" s="36" t="s">
+      <c r="A252" s="35" t="s">
         <v>650</v>
       </c>
-      <c r="B252" s="39" t="s">
+      <c r="B252" s="38" t="s">
         <v>651</v>
       </c>
-      <c r="C252" s="39" t="s">
+      <c r="C252" s="38" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="253">
-      <c r="A253" s="36" t="s">
+      <c r="A253" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="B253" s="36" t="s">
+      <c r="B253" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="C253" s="36" t="s">
+      <c r="C253" s="35" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="254">
-      <c r="A254" s="36" t="s">
+      <c r="A254" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="B254" s="39" t="s">
+      <c r="B254" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="C254" s="39" t="s">
+      <c r="C254" s="38" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="255">
-      <c r="A255" s="36" t="s">
+      <c r="A255" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="B255" s="36" t="s">
+      <c r="B255" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="C255" s="36" t="s">
+      <c r="C255" s="35" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="256">
-      <c r="A256" s="36" t="s">
+      <c r="A256" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="B256" s="36" t="s">
+      <c r="B256" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="C256" s="36" t="s">
+      <c r="C256" s="35" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="259">
-      <c r="B259" s="41" t="s">
+      <c r="B259" s="40" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="263">
-      <c r="A263" s="36" t="s">
+      <c r="A263" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="B263" s="36" t="s">
+      <c r="B263" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="C263" s="36" t="s">
+      <c r="C263" s="35" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="264">
-      <c r="A264" s="36" t="s">
+      <c r="A264" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="B264" s="36" t="s">
+      <c r="B264" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C264" s="36" t="s">
+      <c r="C264" s="35" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="265">
-      <c r="A265" s="36" t="s">
+      <c r="A265" s="35" t="s">
         <v>653</v>
       </c>
-      <c r="B265" s="36" t="s">
+      <c r="B265" s="35" t="s">
         <v>654</v>
       </c>
-      <c r="C265" s="36" t="s">
+      <c r="C265" s="35" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="266">
-      <c r="A266" s="36" t="s">
+      <c r="A266" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B266" s="36" t="s">
+      <c r="B266" s="35" t="s">
         <v>655</v>
       </c>
-      <c r="C266" s="36" t="s">
+      <c r="C266" s="35" t="s">
         <v>655</v>
       </c>
     </row>
     <row r="267">
-      <c r="A267" s="36" t="s">
+      <c r="A267" s="35" t="s">
         <v>656</v>
       </c>
       <c r="B267" s="23" t="s">
@@ -27553,29 +27550,29 @@
       </c>
     </row>
     <row r="268">
-      <c r="A268" s="36" t="s">
+      <c r="A268" s="35" t="s">
         <v>658</v>
       </c>
-      <c r="B268" s="42" t="s">
+      <c r="B268" s="41" t="s">
         <v>659</v>
       </c>
-      <c r="C268" s="42" t="s">
+      <c r="C268" s="41" t="s">
         <v>659</v>
       </c>
     </row>
     <row r="269">
-      <c r="A269" s="36" t="s">
+      <c r="A269" s="35" t="s">
         <v>660</v>
       </c>
-      <c r="B269" s="36" t="s">
+      <c r="B269" s="35" t="s">
         <v>661</v>
       </c>
-      <c r="C269" s="36" t="s">
+      <c r="C269" s="35" t="s">
         <v>661</v>
       </c>
     </row>
     <row r="270">
-      <c r="A270" s="36" t="s">
+      <c r="A270" s="35" t="s">
         <v>662</v>
       </c>
       <c r="B270" s="23" t="s">
@@ -27586,18 +27583,18 @@
       </c>
     </row>
     <row r="271">
-      <c r="A271" s="36" t="s">
+      <c r="A271" s="35" t="s">
         <v>664</v>
       </c>
-      <c r="B271" s="43">
+      <c r="B271" s="42">
         <v>120.0</v>
       </c>
-      <c r="C271" s="43">
+      <c r="C271" s="42">
         <v>120.0</v>
       </c>
     </row>
     <row r="272">
-      <c r="A272" s="36" t="s">
+      <c r="A272" s="35" t="s">
         <v>665</v>
       </c>
       <c r="B272" s="23" t="s">
@@ -27608,7 +27605,7 @@
       </c>
     </row>
     <row r="273">
-      <c r="A273" s="36" t="s">
+      <c r="A273" s="35" t="s">
         <v>667</v>
       </c>
       <c r="B273" s="23" t="s">
@@ -27619,7 +27616,7 @@
       </c>
     </row>
     <row r="274">
-      <c r="A274" s="36" t="s">
+      <c r="A274" s="35" t="s">
         <v>669</v>
       </c>
       <c r="B274" s="23" t="s">
@@ -27630,7 +27627,7 @@
       </c>
     </row>
     <row r="275">
-      <c r="A275" s="36" t="s">
+      <c r="A275" s="35" t="s">
         <v>671</v>
       </c>
       <c r="B275" s="23" t="s">
@@ -27641,7 +27638,7 @@
       </c>
     </row>
     <row r="276">
-      <c r="A276" s="36" t="s">
+      <c r="A276" s="35" t="s">
         <v>673</v>
       </c>
       <c r="B276" s="23" t="s">
@@ -27666,10 +27663,10 @@
       <c r="A278" s="23" t="s">
         <v>676</v>
       </c>
-      <c r="B278" s="43">
+      <c r="B278" s="42">
         <v>6.0</v>
       </c>
-      <c r="C278" s="43">
+      <c r="C278" s="42">
         <v>6.0</v>
       </c>
     </row>
@@ -27732,10 +27729,10 @@
       <c r="A284" s="23" t="s">
         <v>686</v>
       </c>
-      <c r="B284" s="44">
+      <c r="B284" s="43">
         <v>13.0</v>
       </c>
-      <c r="C284" s="44">
+      <c r="C284" s="43">
         <v>13.0</v>
       </c>
     </row>
@@ -27798,10 +27795,10 @@
       <c r="A290" s="23" t="s">
         <v>696</v>
       </c>
-      <c r="B290" s="43">
+      <c r="B290" s="42">
         <v>12.0</v>
       </c>
-      <c r="C290" s="43">
+      <c r="C290" s="42">
         <v>12.0</v>
       </c>
     </row>
@@ -27853,10 +27850,10 @@
       <c r="A295" s="23" t="s">
         <v>704</v>
       </c>
-      <c r="B295" s="43">
+      <c r="B295" s="42">
         <v>2.0</v>
       </c>
-      <c r="C295" s="43">
+      <c r="C295" s="42">
         <v>2.0</v>
       </c>
     </row>
@@ -27897,10 +27894,10 @@
       <c r="A299" s="23" t="s">
         <v>710</v>
       </c>
-      <c r="B299" s="43">
+      <c r="B299" s="42">
         <v>7.0</v>
       </c>
-      <c r="C299" s="43">
+      <c r="C299" s="42">
         <v>7.0</v>
       </c>
     </row>
@@ -27908,10 +27905,10 @@
       <c r="A300" s="23" t="s">
         <v>711</v>
       </c>
-      <c r="B300" s="43">
+      <c r="B300" s="42">
         <v>8.0</v>
       </c>
-      <c r="C300" s="43">
+      <c r="C300" s="42">
         <v>8.0</v>
       </c>
     </row>
@@ -27955,7 +27952,7 @@
       <c r="B304" s="23" t="s">
         <v>718</v>
       </c>
-      <c r="C304" s="42" t="s">
+      <c r="C304" s="41" t="s">
         <v>718</v>
       </c>
     </row>
@@ -27963,10 +27960,10 @@
       <c r="A305" s="23" t="s">
         <v>719</v>
       </c>
-      <c r="B305" s="43">
+      <c r="B305" s="42">
         <v>6.0</v>
       </c>
-      <c r="C305" s="43">
+      <c r="C305" s="42">
         <v>6.0</v>
       </c>
     </row>
@@ -28007,10 +28004,10 @@
       <c r="A309" s="23" t="s">
         <v>725</v>
       </c>
-      <c r="B309" s="43">
+      <c r="B309" s="42">
         <v>9.0</v>
       </c>
-      <c r="C309" s="43">
+      <c r="C309" s="42">
         <v>9.0</v>
       </c>
     </row>
@@ -28018,10 +28015,10 @@
       <c r="A310" s="23" t="s">
         <v>726</v>
       </c>
-      <c r="B310" s="43">
+      <c r="B310" s="42">
         <v>10.0</v>
       </c>
-      <c r="C310" s="43">
+      <c r="C310" s="42">
         <v>10.0</v>
       </c>
     </row>
@@ -28062,10 +28059,10 @@
       <c r="A314" s="23" t="s">
         <v>731</v>
       </c>
-      <c r="B314" s="43">
+      <c r="B314" s="42">
         <v>12.0</v>
       </c>
-      <c r="C314" s="43">
+      <c r="C314" s="42">
         <v>12.0</v>
       </c>
     </row>
@@ -28073,10 +28070,10 @@
       <c r="A315" s="23" t="s">
         <v>732</v>
       </c>
-      <c r="B315" s="43">
+      <c r="B315" s="42">
         <v>13.0</v>
       </c>
-      <c r="C315" s="43">
+      <c r="C315" s="42">
         <v>13.0</v>
       </c>
     </row>
@@ -28128,10 +28125,10 @@
       <c r="A320" s="23" t="s">
         <v>739</v>
       </c>
-      <c r="B320" s="43">
+      <c r="B320" s="42">
         <v>6.0</v>
       </c>
-      <c r="C320" s="43">
+      <c r="C320" s="42">
         <v>6.0</v>
       </c>
     </row>
@@ -28183,10 +28180,10 @@
       <c r="A325" s="23" t="s">
         <v>747</v>
       </c>
-      <c r="B325" s="43">
+      <c r="B325" s="42">
         <v>7.0</v>
       </c>
-      <c r="C325" s="43">
+      <c r="C325" s="42">
         <v>7.0</v>
       </c>
     </row>
@@ -28238,10 +28235,10 @@
       <c r="A330" s="23" t="s">
         <v>755</v>
       </c>
-      <c r="B330" s="43">
+      <c r="B330" s="42">
         <v>3.0</v>
       </c>
-      <c r="C330" s="43">
+      <c r="C330" s="42">
         <v>3.0</v>
       </c>
     </row>
@@ -28293,10 +28290,10 @@
       <c r="A335" s="23" t="s">
         <v>763</v>
       </c>
-      <c r="B335" s="43">
+      <c r="B335" s="42">
         <v>3.0</v>
       </c>
-      <c r="C335" s="43">
+      <c r="C335" s="42">
         <v>3.0</v>
       </c>
     </row>
@@ -28348,10 +28345,10 @@
       <c r="A340" s="23" t="s">
         <v>771</v>
       </c>
-      <c r="B340" s="43">
+      <c r="B340" s="42">
         <v>3.0</v>
       </c>
-      <c r="C340" s="43">
+      <c r="C340" s="42">
         <v>3.0</v>
       </c>
     </row>
@@ -28392,10 +28389,10 @@
       <c r="A344" s="23" t="s">
         <v>777</v>
       </c>
-      <c r="B344" s="42" t="s">
+      <c r="B344" s="41" t="s">
         <v>778</v>
       </c>
-      <c r="C344" s="42" t="s">
+      <c r="C344" s="41" t="s">
         <v>778</v>
       </c>
     </row>
@@ -28403,10 +28400,10 @@
       <c r="A345" s="23" t="s">
         <v>779</v>
       </c>
-      <c r="B345" s="43">
+      <c r="B345" s="42">
         <v>3.0</v>
       </c>
-      <c r="C345" s="43">
+      <c r="C345" s="42">
         <v>3.0</v>
       </c>
     </row>
@@ -28458,10 +28455,10 @@
       <c r="A350" s="23" t="s">
         <v>787</v>
       </c>
-      <c r="B350" s="43" t="s">
+      <c r="B350" s="42" t="s">
         <v>788</v>
       </c>
-      <c r="C350" s="43" t="s">
+      <c r="C350" s="42" t="s">
         <v>788</v>
       </c>
     </row>
@@ -28469,10 +28466,10 @@
       <c r="A351" s="23" t="s">
         <v>789</v>
       </c>
-      <c r="B351" s="43">
+      <c r="B351" s="42">
         <v>6.0</v>
       </c>
-      <c r="C351" s="43">
+      <c r="C351" s="42">
         <v>6.0</v>
       </c>
     </row>
@@ -28513,10 +28510,10 @@
       <c r="A355" s="23" t="s">
         <v>795</v>
       </c>
-      <c r="B355" s="43">
+      <c r="B355" s="42">
         <v>50.0</v>
       </c>
-      <c r="C355" s="43">
+      <c r="C355" s="42">
         <v>50.0</v>
       </c>
     </row>
@@ -28524,10 +28521,10 @@
       <c r="A356" s="23" t="s">
         <v>796</v>
       </c>
-      <c r="B356" s="43">
+      <c r="B356" s="42">
         <v>55.0</v>
       </c>
-      <c r="C356" s="43">
+      <c r="C356" s="42">
         <v>55.0</v>
       </c>
     </row>
@@ -28719,7 +28716,7 @@
       </c>
     </row>
     <row r="379">
-      <c r="B379" s="35" t="s">
+      <c r="B379" s="34" t="s">
         <v>828</v>
       </c>
     </row>
@@ -28790,7 +28787,7 @@
       </c>
     </row>
     <row r="390">
-      <c r="B390" s="35" t="s">
+      <c r="B390" s="34" t="s">
         <v>840</v>
       </c>
     </row>
@@ -29290,7 +29287,7 @@
       </c>
     </row>
     <row r="440">
-      <c r="B440" s="35" t="s">
+      <c r="B440" s="34" t="s">
         <v>930</v>
       </c>
     </row>
@@ -29347,13 +29344,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
     </row>
@@ -29391,11 +29388,11 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="45" t="s">
         <v>936</v>
       </c>
-      <c r="C6" s="46"/>
+      <c r="C6" s="45"/>
     </row>
     <row r="7">
       <c r="A7" s="16"/>
@@ -29430,20 +29427,20 @@
       <c r="C10" s="16"/>
     </row>
     <row r="11">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46" t="s">
+      <c r="A11" s="45"/>
+      <c r="B11" s="45" t="s">
         <v>941</v>
       </c>
-      <c r="C11" s="46"/>
+      <c r="C11" s="45"/>
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
         <v>942</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="46" t="s">
         <v>625</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="46" t="s">
         <v>625</v>
       </c>
     </row>
@@ -29556,8 +29553,8 @@
     </row>
     <row r="28">
       <c r="A28" s="16"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
     </row>
     <row r="29">
       <c r="A29" s="16" t="s">
@@ -29572,17 +29569,17 @@
     </row>
     <row r="30">
       <c r="A30" s="16"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
     </row>
     <row r="31">
       <c r="A31" s="16" t="s">
         <v>942</v>
       </c>
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="46" t="s">
         <v>514</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="46" t="s">
         <v>514</v>
       </c>
     </row>
@@ -29590,10 +29587,10 @@
       <c r="A32" s="16" t="s">
         <v>952</v>
       </c>
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="46" t="s">
         <v>7</v>
       </c>
     </row>
@@ -29601,10 +29598,10 @@
       <c r="A33" s="16" t="s">
         <v>953</v>
       </c>
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="48" t="s">
+      <c r="C33" s="47" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sanity Pack Update for V4.1.1(31/01/23)
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -3243,7 +3243,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3322,9 +3322,6 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -28019,7 +28016,7 @@
         <v>607</v>
       </c>
       <c r="B76" s="36" t="s">
-        <v>608</v>
+        <v>8</v>
       </c>
       <c r="C76" s="36" t="s">
         <v>608</v>
@@ -28029,11 +28026,11 @@
       <c r="A77" s="28" t="s">
         <v>609</v>
       </c>
-      <c r="B77" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" s="37" t="s">
-        <v>8</v>
+      <c r="B77" s="36" t="s">
+        <v>608</v>
+      </c>
+      <c r="C77" s="36" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1"/>
@@ -28130,7 +28127,7 @@
     </row>
     <row r="90" ht="15.75" customHeight="1"/>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="38" t="s">
+      <c r="A91" s="37" t="s">
         <v>626</v>
       </c>
       <c r="B91" s="28" t="s">
@@ -28141,7 +28138,7 @@
       </c>
     </row>
     <row r="92" ht="15.0" customHeight="1">
-      <c r="A92" s="38" t="s">
+      <c r="A92" s="37" t="s">
         <v>628</v>
       </c>
       <c r="B92" s="28" t="s">
@@ -28184,7 +28181,7 @@
     </row>
     <row r="100" ht="15.75" customHeight="1"/>
     <row r="101" ht="15.0" customHeight="1">
-      <c r="A101" s="39" t="s">
+      <c r="A101" s="38" t="s">
         <v>633</v>
       </c>
       <c r="B101" s="28" t="s">
@@ -28196,7 +28193,7 @@
     </row>
     <row r="102" ht="15.75" customHeight="1"/>
     <row r="103" ht="15.0" customHeight="1">
-      <c r="A103" s="38" t="s">
+      <c r="A103" s="37" t="s">
         <v>634</v>
       </c>
       <c r="B103" s="28" t="s">
@@ -28207,7 +28204,7 @@
       </c>
     </row>
     <row r="104" ht="15.0" customHeight="1">
-      <c r="A104" s="38" t="s">
+      <c r="A104" s="37" t="s">
         <v>636</v>
       </c>
       <c r="B104" s="28" t="s">
@@ -28271,7 +28268,7 @@
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="39" t="s">
+      <c r="A114" s="38" t="s">
         <v>643</v>
       </c>
       <c r="B114" s="28" t="s">
@@ -28282,7 +28279,7 @@
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="39" t="s">
+      <c r="A115" s="38" t="s">
         <v>645</v>
       </c>
       <c r="B115" s="28" t="s">
@@ -28293,7 +28290,7 @@
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="39" t="s">
+      <c r="A116" s="38" t="s">
         <v>647</v>
       </c>
       <c r="B116" s="28" t="s">
@@ -28305,7 +28302,7 @@
     </row>
     <row r="117" ht="15.75" customHeight="1"/>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="39" t="s">
+      <c r="A118" s="38" t="s">
         <v>649</v>
       </c>
       <c r="B118" s="28" t="s">
@@ -28316,7 +28313,7 @@
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="39" t="s">
+      <c r="A119" s="38" t="s">
         <v>651</v>
       </c>
       <c r="B119" s="28" t="s">
@@ -28327,7 +28324,7 @@
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="39" t="s">
+      <c r="A120" s="38" t="s">
         <v>653</v>
       </c>
       <c r="B120" s="28" t="s">
@@ -28368,7 +28365,7 @@
     <row r="125" ht="15.75" customHeight="1"/>
     <row r="126" ht="15.75" customHeight="1"/>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="39" t="s">
+      <c r="A127" s="38" t="s">
         <v>658</v>
       </c>
       <c r="B127" s="28" t="s">
@@ -28379,7 +28376,7 @@
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="39" t="s">
+      <c r="A128" s="38" t="s">
         <v>660</v>
       </c>
       <c r="B128" s="28" t="s">
@@ -28390,7 +28387,7 @@
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="39" t="s">
+      <c r="A129" s="38" t="s">
         <v>662</v>
       </c>
       <c r="B129" s="28" t="s">
@@ -28401,7 +28398,7 @@
       </c>
     </row>
     <row r="130" ht="15.0" customHeight="1">
-      <c r="A130" s="39" t="s">
+      <c r="A130" s="38" t="s">
         <v>664</v>
       </c>
       <c r="B130" s="28" t="s">
@@ -28526,7 +28523,7 @@
     </row>
     <row r="144" ht="15.75" customHeight="1"/>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="40" t="s">
+      <c r="A145" s="39" t="s">
         <v>686</v>
       </c>
       <c r="B145" s="34" t="s">
@@ -28537,7 +28534,7 @@
       </c>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="40" t="s">
+      <c r="A146" s="39" t="s">
         <v>688</v>
       </c>
       <c r="B146" s="34" t="s">
@@ -28548,7 +28545,7 @@
       </c>
     </row>
     <row r="147" ht="15.0" customHeight="1">
-      <c r="A147" s="40" t="s">
+      <c r="A147" s="39" t="s">
         <v>689</v>
       </c>
       <c r="B147" s="34" t="s">
@@ -28576,13 +28573,13 @@
       </c>
     </row>
     <row r="151" ht="15.0" customHeight="1">
-      <c r="A151" s="40" t="s">
+      <c r="A151" s="39" t="s">
         <v>693</v>
       </c>
-      <c r="B151" s="41" t="s">
+      <c r="B151" s="40" t="s">
         <v>694</v>
       </c>
-      <c r="C151" s="41" t="s">
+      <c r="C151" s="40" t="s">
         <v>694</v>
       </c>
     </row>
@@ -28610,222 +28607,222 @@
     </row>
     <row r="154" ht="15.75" customHeight="1"/>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="42" t="s">
+      <c r="A155" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="B155" s="41" t="s">
+      <c r="B155" s="40" t="s">
         <v>692</v>
       </c>
-      <c r="C155" s="41" t="s">
+      <c r="C155" s="40" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="156" ht="15.0" customHeight="1">
-      <c r="A156" s="42" t="s">
+      <c r="A156" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B156" s="41" t="s">
+      <c r="B156" s="40" t="s">
         <v>694</v>
       </c>
-      <c r="C156" s="41" t="s">
+      <c r="C156" s="40" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="157" ht="15.0" customHeight="1">
-      <c r="A157" s="42" t="s">
+      <c r="A157" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B157" s="41" t="s">
+      <c r="B157" s="40" t="s">
         <v>695</v>
       </c>
-      <c r="C157" s="41" t="s">
+      <c r="C157" s="40" t="s">
         <v>695</v>
       </c>
     </row>
     <row r="158" ht="15.75" customHeight="1"/>
     <row r="159" ht="15.75" customHeight="1"/>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="42" t="s">
+      <c r="A160" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B160" s="41" t="s">
+      <c r="B160" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="C160" s="41" t="s">
+      <c r="C160" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="161" ht="15.0" customHeight="1">
-      <c r="A161" s="42" t="s">
+      <c r="A161" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="B161" s="41" t="s">
+      <c r="B161" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C161" s="41" t="s">
+      <c r="C161" s="40" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="162" ht="15.0" customHeight="1">
-      <c r="A162" s="42" t="s">
+      <c r="A162" s="41" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="163" ht="15.75" customHeight="1"/>
     <row r="164" ht="15.75" customHeight="1"/>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="42" t="s">
+      <c r="A165" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="B165" s="41" t="s">
+      <c r="B165" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C165" s="41" t="s">
+      <c r="C165" s="40" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="166" ht="15.0" customHeight="1">
-      <c r="A166" s="42" t="s">
+      <c r="A166" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="B166" s="41" t="s">
+      <c r="B166" s="40" t="s">
         <v>696</v>
       </c>
-      <c r="C166" s="41" t="s">
+      <c r="C166" s="40" t="s">
         <v>696</v>
       </c>
     </row>
     <row r="167" ht="15.0" customHeight="1">
-      <c r="A167" s="42" t="s">
+      <c r="A167" s="41" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="168" ht="15.75" customHeight="1"/>
     <row r="169" ht="15.75" customHeight="1"/>
     <row r="170" ht="15.0" customHeight="1">
-      <c r="A170" s="42" t="s">
+      <c r="A170" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="B170" s="41" t="s">
+      <c r="B170" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C170" s="41" t="s">
+      <c r="C170" s="40" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="171" ht="15.0" customHeight="1">
-      <c r="A171" s="42" t="s">
+      <c r="A171" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="B171" s="41" t="s">
+      <c r="B171" s="40" t="s">
         <v>697</v>
       </c>
-      <c r="C171" s="41" t="s">
+      <c r="C171" s="40" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="42" t="s">
+      <c r="A172" s="41" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="173" ht="15.75" customHeight="1"/>
     <row r="174" ht="15.75" customHeight="1"/>
     <row r="175" ht="15.0" customHeight="1">
-      <c r="A175" s="42" t="s">
+      <c r="A175" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="B175" s="41" t="s">
+      <c r="B175" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C175" s="41" t="s">
+      <c r="C175" s="40" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="42" t="s">
+      <c r="A176" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="B176" s="41" t="s">
+      <c r="B176" s="40" t="s">
         <v>697</v>
       </c>
-      <c r="C176" s="41" t="s">
+      <c r="C176" s="40" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="177" ht="15.75" customHeight="1"/>
     <row r="178" ht="15.75" customHeight="1"/>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="42" t="s">
+      <c r="A179" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="B179" s="41" t="s">
+      <c r="B179" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C179" s="41" t="s">
+      <c r="C179" s="40" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="42" t="s">
+      <c r="A180" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="B180" s="41" t="s">
+      <c r="B180" s="40" t="s">
         <v>697</v>
       </c>
-      <c r="C180" s="41" t="s">
+      <c r="C180" s="40" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="181" ht="15.75" customHeight="1"/>
     <row r="182" ht="15.75" customHeight="1"/>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="42" t="s">
+      <c r="A183" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="B183" s="41" t="s">
+      <c r="B183" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="C183" s="41" t="s">
+      <c r="C183" s="40" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="42" t="s">
+      <c r="A184" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="B184" s="41" t="s">
+      <c r="B184" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="C184" s="41" t="s">
+      <c r="C184" s="40" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="42" t="s">
+      <c r="A185" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="B185" s="41" t="s">
+      <c r="B185" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="C185" s="41" t="s">
+      <c r="C185" s="40" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="41" t="s">
+      <c r="A186" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="B186" s="41" t="s">
+      <c r="B186" s="40" t="s">
         <v>698</v>
       </c>
-      <c r="C186" s="41" t="s">
+      <c r="C186" s="40" t="s">
         <v>698</v>
       </c>
     </row>
     <row r="187" ht="15.75" customHeight="1"/>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="B188" s="43" t="s">
+      <c r="B188" s="42" t="s">
         <v>699</v>
       </c>
     </row>
@@ -28834,7 +28831,7 @@
     <row r="191" ht="15.75" customHeight="1"/>
     <row r="192" ht="15.75" customHeight="1"/>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="44" t="s">
+      <c r="A193" s="43" t="s">
         <v>3</v>
       </c>
       <c r="B193" s="2" t="s">
@@ -28845,40 +28842,40 @@
       </c>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="44" t="s">
+      <c r="A194" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="B194" s="45" t="s">
+      <c r="B194" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C194" s="45" t="s">
+      <c r="C194" s="44" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="44" t="s">
+      <c r="A195" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B195" s="44" t="s">
+      <c r="B195" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C195" s="44" t="s">
+      <c r="C195" s="43" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="44" t="s">
+      <c r="A196" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="B196" s="44" t="s">
+      <c r="B196" s="43" t="s">
         <v>700</v>
       </c>
-      <c r="C196" s="44" t="s">
+      <c r="C196" s="43" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="44" t="s">
+      <c r="A197" s="43" t="s">
         <v>87</v>
       </c>
       <c r="B197" s="30" t="s">
@@ -28889,18 +28886,18 @@
       </c>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="44" t="s">
+      <c r="A198" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="B198" s="46" t="s">
+      <c r="B198" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="C198" s="46" t="s">
+      <c r="C198" s="45" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="44" t="s">
+      <c r="A199" s="43" t="s">
         <v>279</v>
       </c>
       <c r="B199" s="30" t="s">
@@ -28911,73 +28908,73 @@
       </c>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="44" t="s">
+      <c r="A200" s="43" t="s">
         <v>193</v>
       </c>
-      <c r="B200" s="44" t="s">
+      <c r="B200" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="C200" s="44" t="s">
+      <c r="C200" s="43" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="44" t="s">
+      <c r="A201" s="43" t="s">
         <v>207</v>
       </c>
-      <c r="B201" s="44" t="s">
+      <c r="B201" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="C201" s="44" t="s">
+      <c r="C201" s="43" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="44" t="s">
+      <c r="A202" s="43" t="s">
         <v>209</v>
       </c>
-      <c r="B202" s="44" t="s">
+      <c r="B202" s="43" t="s">
         <v>210</v>
       </c>
-      <c r="C202" s="44" t="s">
+      <c r="C202" s="43" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="44" t="s">
+      <c r="A203" s="43" t="s">
         <v>211</v>
       </c>
-      <c r="B203" s="44" t="s">
+      <c r="B203" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="C203" s="44" t="s">
+      <c r="C203" s="43" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="44" t="s">
+      <c r="A204" s="43" t="s">
         <v>197</v>
       </c>
-      <c r="B204" s="44" t="s">
+      <c r="B204" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="C204" s="44" t="s">
+      <c r="C204" s="43" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="44" t="s">
+      <c r="A205" s="43" t="s">
         <v>287</v>
       </c>
-      <c r="B205" s="44" t="s">
+      <c r="B205" s="43" t="s">
         <v>288</v>
       </c>
-      <c r="C205" s="44" t="s">
+      <c r="C205" s="43" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="44" t="s">
+      <c r="A206" s="43" t="s">
         <v>165</v>
       </c>
       <c r="B206" s="30" t="s">
@@ -28988,18 +28985,18 @@
       </c>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="44" t="s">
+      <c r="A207" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="B207" s="46" t="s">
+      <c r="B207" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="C207" s="46" t="s">
+      <c r="C207" s="45" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="44" t="s">
+      <c r="A208" s="43" t="s">
         <v>285</v>
       </c>
       <c r="B208" s="30" t="s">
@@ -29011,29 +29008,29 @@
     </row>
     <row r="209" ht="15.75" customHeight="1"/>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="44" t="s">
+      <c r="A210" s="43" t="s">
         <v>333</v>
       </c>
-      <c r="B210" s="44" t="s">
+      <c r="B210" s="43" t="s">
         <v>334</v>
       </c>
-      <c r="C210" s="44" t="s">
+      <c r="C210" s="43" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="44" t="s">
+      <c r="A211" s="43" t="s">
         <v>701</v>
       </c>
-      <c r="B211" s="46" t="s">
+      <c r="B211" s="45" t="s">
         <v>702</v>
       </c>
-      <c r="C211" s="46" t="s">
+      <c r="C211" s="45" t="s">
         <v>702</v>
       </c>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="44" t="s">
+      <c r="A212" s="43" t="s">
         <v>337</v>
       </c>
       <c r="B212" s="30" t="s">
@@ -29044,7 +29041,7 @@
       </c>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="44" t="s">
+      <c r="A213" s="43" t="s">
         <v>704</v>
       </c>
       <c r="B213" s="30" t="s">
@@ -29055,74 +29052,74 @@
       </c>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="44" t="s">
+      <c r="A214" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="B214" s="44" t="s">
+      <c r="B214" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="C214" s="44" t="s">
+      <c r="C214" s="43" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="44" t="s">
+      <c r="A215" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="B215" s="46" t="s">
+      <c r="B215" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="C215" s="46" t="s">
+      <c r="C215" s="45" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="44" t="s">
+      <c r="A216" s="43" t="s">
         <v>289</v>
       </c>
-      <c r="B216" s="44" t="s">
+      <c r="B216" s="43" t="s">
         <v>290</v>
       </c>
-      <c r="C216" s="44" t="s">
+      <c r="C216" s="43" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="44" t="s">
+      <c r="A217" s="43" t="s">
         <v>203</v>
       </c>
-      <c r="B217" s="44" t="s">
+      <c r="B217" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="C217" s="44" t="s">
+      <c r="C217" s="43" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="44" t="s">
+      <c r="A218" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="B218" s="44" t="s">
+      <c r="B218" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="C218" s="44" t="s">
+      <c r="C218" s="43" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="219" ht="15.75" customHeight="1"/>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="44" t="s">
+      <c r="A220" s="43" t="s">
         <v>705</v>
       </c>
-      <c r="B220" s="46" t="s">
+      <c r="B220" s="45" t="s">
         <v>706</v>
       </c>
-      <c r="C220" s="46" t="s">
+      <c r="C220" s="45" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="44" t="s">
+      <c r="A221" s="43" t="s">
         <v>707</v>
       </c>
       <c r="B221" s="30" t="s">
@@ -29133,384 +29130,384 @@
       </c>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="44" t="s">
+      <c r="A222" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="B222" s="44" t="s">
+      <c r="B222" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="C222" s="44" t="s">
+      <c r="C222" s="43" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="44" t="s">
+      <c r="A223" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="B223" s="46" t="s">
+      <c r="B223" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="C223" s="46" t="s">
+      <c r="C223" s="45" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="44" t="s">
+      <c r="A224" s="43" t="s">
         <v>297</v>
       </c>
-      <c r="B224" s="44" t="s">
+      <c r="B224" s="43" t="s">
         <v>298</v>
       </c>
-      <c r="C224" s="44" t="s">
+      <c r="C224" s="43" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="44" t="s">
+      <c r="A225" s="43" t="s">
         <v>709</v>
       </c>
-      <c r="B225" s="44" t="s">
+      <c r="B225" s="43" t="s">
         <v>710</v>
       </c>
-      <c r="C225" s="44" t="s">
+      <c r="C225" s="43" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="44" t="s">
+      <c r="A226" s="43" t="s">
         <v>341</v>
       </c>
-      <c r="B226" s="44" t="s">
+      <c r="B226" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="C226" s="44" t="s">
+      <c r="C226" s="43" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="44" t="s">
+      <c r="A227" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="B227" s="44" t="s">
+      <c r="B227" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="C227" s="44" t="s">
+      <c r="C227" s="43" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="A228" s="44" t="s">
+      <c r="A228" s="43" t="s">
         <v>711</v>
       </c>
-      <c r="B228" s="44" t="s">
+      <c r="B228" s="43" t="s">
         <v>712</v>
       </c>
-      <c r="C228" s="44" t="s">
+      <c r="C228" s="43" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="A229" s="44" t="s">
+      <c r="A229" s="43" t="s">
         <v>344</v>
       </c>
-      <c r="B229" s="44" t="s">
+      <c r="B229" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="C229" s="44" t="s">
+      <c r="C229" s="43" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="A230" s="44" t="s">
+      <c r="A230" s="43" t="s">
         <v>713</v>
       </c>
-      <c r="B230" s="46" t="s">
+      <c r="B230" s="45" t="s">
         <v>714</v>
       </c>
-      <c r="C230" s="46" t="s">
+      <c r="C230" s="45" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="A231" s="44" t="s">
+      <c r="A231" s="43" t="s">
         <v>221</v>
       </c>
-      <c r="B231" s="44" t="s">
+      <c r="B231" s="43" t="s">
         <v>715</v>
       </c>
-      <c r="C231" s="44" t="s">
+      <c r="C231" s="43" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="44" t="s">
+      <c r="A232" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="B232" s="44" t="s">
+      <c r="B232" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="C232" s="44" t="s">
+      <c r="C232" s="43" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="233" ht="15.75" customHeight="1"/>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="A234" s="44" t="s">
+      <c r="A234" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="B234" s="44" t="s">
+      <c r="B234" s="43" t="s">
         <v>226</v>
       </c>
-      <c r="C234" s="44" t="s">
+      <c r="C234" s="43" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="A235" s="44" t="s">
+      <c r="A235" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="B235" s="44" t="s">
+      <c r="B235" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="C235" s="44" t="s">
+      <c r="C235" s="43" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="A236" s="44" t="s">
+      <c r="A236" s="43" t="s">
         <v>716</v>
       </c>
-      <c r="B236" s="46" t="s">
+      <c r="B236" s="45" t="s">
         <v>717</v>
       </c>
-      <c r="C236" s="46" t="s">
+      <c r="C236" s="45" t="s">
         <v>717</v>
       </c>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="44" t="s">
+      <c r="A237" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="B237" s="44" t="s">
+      <c r="B237" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="C237" s="44" t="s">
+      <c r="C237" s="43" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="A238" s="44" t="s">
+      <c r="A238" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="B238" s="44" t="s">
+      <c r="B238" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="C238" s="44" t="s">
+      <c r="C238" s="43" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="A239" s="44" t="s">
+      <c r="A239" s="43" t="s">
         <v>718</v>
       </c>
-      <c r="B239" s="46" t="s">
+      <c r="B239" s="45" t="s">
         <v>719</v>
       </c>
-      <c r="C239" s="46" t="s">
+      <c r="C239" s="45" t="s">
         <v>719</v>
       </c>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="A240" s="44" t="s">
+      <c r="A240" s="43" t="s">
         <v>720</v>
       </c>
-      <c r="B240" s="46" t="s">
+      <c r="B240" s="45" t="s">
         <v>721</v>
       </c>
-      <c r="C240" s="46" t="s">
+      <c r="C240" s="45" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="A241" s="44" t="s">
+      <c r="A241" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B241" s="46" t="s">
+      <c r="B241" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="C241" s="46" t="s">
+      <c r="C241" s="45" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="A242" s="44" t="s">
+      <c r="A242" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="B242" s="44" t="s">
+      <c r="B242" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="C242" s="44" t="s">
+      <c r="C242" s="43" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="A243" s="44" t="s">
+      <c r="A243" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="B243" s="46" t="s">
+      <c r="B243" s="45" t="s">
         <v>722</v>
       </c>
-      <c r="C243" s="46" t="s">
+      <c r="C243" s="45" t="s">
         <v>722</v>
       </c>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="A244" s="44" t="s">
+      <c r="A244" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="B244" s="47" t="s">
+      <c r="B244" s="46" t="s">
         <v>156</v>
       </c>
-      <c r="C244" s="47" t="s">
+      <c r="C244" s="46" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="A245" s="44" t="s">
+      <c r="A245" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="B245" s="44" t="s">
+      <c r="B245" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="C245" s="44" t="s">
+      <c r="C245" s="43" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="A246" s="44" t="s">
+      <c r="A246" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="B246" s="44" t="s">
+      <c r="B246" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="C246" s="44" t="s">
+      <c r="C246" s="43" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="A247" s="44" t="s">
+      <c r="A247" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="B247" s="46" t="s">
+      <c r="B247" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="C247" s="46" t="s">
+      <c r="C247" s="45" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="A248" s="44" t="s">
+      <c r="A248" s="43" t="s">
         <v>195</v>
       </c>
-      <c r="B248" s="46" t="s">
+      <c r="B248" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="C248" s="46" t="s">
+      <c r="C248" s="45" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="A249" s="44" t="s">
+      <c r="A249" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="B249" s="46" t="s">
+      <c r="B249" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="C249" s="46" t="s">
+      <c r="C249" s="45" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="A250" s="44" t="s">
+      <c r="A250" s="43" t="s">
         <v>723</v>
       </c>
-      <c r="B250" s="46" t="s">
+      <c r="B250" s="45" t="s">
         <v>724</v>
       </c>
-      <c r="C250" s="46" t="s">
+      <c r="C250" s="45" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="A251" s="44" t="s">
+      <c r="A251" s="43" t="s">
         <v>199</v>
       </c>
-      <c r="B251" s="46" t="s">
+      <c r="B251" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="C251" s="46" t="s">
+      <c r="C251" s="45" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="A252" s="44" t="s">
+      <c r="A252" s="43" t="s">
         <v>725</v>
       </c>
-      <c r="B252" s="46" t="s">
+      <c r="B252" s="45" t="s">
         <v>726</v>
       </c>
-      <c r="C252" s="46" t="s">
+      <c r="C252" s="45" t="s">
         <v>726</v>
       </c>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="A253" s="44" t="s">
+      <c r="A253" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="B253" s="44" t="s">
+      <c r="B253" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="C253" s="44" t="s">
+      <c r="C253" s="43" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="A254" s="44" t="s">
+      <c r="A254" s="43" t="s">
         <v>187</v>
       </c>
-      <c r="B254" s="46" t="s">
+      <c r="B254" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="C254" s="46" t="s">
+      <c r="C254" s="45" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="A255" s="44" t="s">
+      <c r="A255" s="43" t="s">
         <v>181</v>
       </c>
-      <c r="B255" s="44" t="s">
+      <c r="B255" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="C255" s="44" t="s">
+      <c r="C255" s="43" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="A256" s="44" t="s">
+      <c r="A256" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="B256" s="44" t="s">
+      <c r="B256" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="C256" s="44" t="s">
+      <c r="C256" s="43" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="257" ht="15.75" customHeight="1"/>
     <row r="258" ht="15.75" customHeight="1"/>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="B259" s="48" t="s">
+      <c r="B259" s="47" t="s">
         <v>727</v>
       </c>
     </row>
@@ -29518,51 +29515,51 @@
     <row r="261" ht="15.75" customHeight="1"/>
     <row r="262" ht="15.75" customHeight="1"/>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="A263" s="44" t="s">
+      <c r="A263" s="43" t="s">
         <v>227</v>
       </c>
-      <c r="B263" s="44" t="s">
+      <c r="B263" s="43" t="s">
         <v>228</v>
       </c>
-      <c r="C263" s="44" t="s">
+      <c r="C263" s="43" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="A264" s="44" t="s">
+      <c r="A264" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="B264" s="44" t="s">
+      <c r="B264" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="C264" s="44" t="s">
+      <c r="C264" s="43" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="A265" s="44" t="s">
+      <c r="A265" s="43" t="s">
         <v>728</v>
       </c>
-      <c r="B265" s="44" t="s">
+      <c r="B265" s="43" t="s">
         <v>729</v>
       </c>
-      <c r="C265" s="44" t="s">
+      <c r="C265" s="43" t="s">
         <v>729</v>
       </c>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="A266" s="44" t="s">
+      <c r="A266" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="B266" s="44" t="s">
+      <c r="B266" s="43" t="s">
         <v>730</v>
       </c>
-      <c r="C266" s="44" t="s">
+      <c r="C266" s="43" t="s">
         <v>730</v>
       </c>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="A267" s="44" t="s">
+      <c r="A267" s="43" t="s">
         <v>731</v>
       </c>
       <c r="B267" s="30" t="s">
@@ -29573,29 +29570,29 @@
       </c>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="A268" s="44" t="s">
+      <c r="A268" s="43" t="s">
         <v>733</v>
       </c>
-      <c r="B268" s="49" t="s">
+      <c r="B268" s="48" t="s">
         <v>734</v>
       </c>
-      <c r="C268" s="49" t="s">
+      <c r="C268" s="48" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="A269" s="44" t="s">
+      <c r="A269" s="43" t="s">
         <v>735</v>
       </c>
-      <c r="B269" s="44" t="s">
+      <c r="B269" s="43" t="s">
         <v>736</v>
       </c>
-      <c r="C269" s="44" t="s">
+      <c r="C269" s="43" t="s">
         <v>736</v>
       </c>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="A270" s="44" t="s">
+      <c r="A270" s="43" t="s">
         <v>737</v>
       </c>
       <c r="B270" s="30" t="s">
@@ -29606,18 +29603,18 @@
       </c>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="A271" s="44" t="s">
+      <c r="A271" s="43" t="s">
         <v>739</v>
       </c>
-      <c r="B271" s="50">
+      <c r="B271" s="49">
         <v>120.0</v>
       </c>
-      <c r="C271" s="50">
+      <c r="C271" s="49">
         <v>120.0</v>
       </c>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="A272" s="44" t="s">
+      <c r="A272" s="43" t="s">
         <v>740</v>
       </c>
       <c r="B272" s="30" t="s">
@@ -29628,7 +29625,7 @@
       </c>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="A273" s="44" t="s">
+      <c r="A273" s="43" t="s">
         <v>742</v>
       </c>
       <c r="B273" s="30" t="s">
@@ -29639,7 +29636,7 @@
       </c>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="A274" s="44" t="s">
+      <c r="A274" s="43" t="s">
         <v>744</v>
       </c>
       <c r="B274" s="30" t="s">
@@ -29650,7 +29647,7 @@
       </c>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="A275" s="44" t="s">
+      <c r="A275" s="43" t="s">
         <v>746</v>
       </c>
       <c r="B275" s="30" t="s">
@@ -29661,7 +29658,7 @@
       </c>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="A276" s="44" t="s">
+      <c r="A276" s="43" t="s">
         <v>748</v>
       </c>
       <c r="B276" s="30" t="s">
@@ -29686,10 +29683,10 @@
       <c r="A278" s="30" t="s">
         <v>751</v>
       </c>
-      <c r="B278" s="50">
+      <c r="B278" s="49">
         <v>6.0</v>
       </c>
-      <c r="C278" s="50">
+      <c r="C278" s="49">
         <v>6.0</v>
       </c>
     </row>
@@ -29752,10 +29749,10 @@
       <c r="A284" s="30" t="s">
         <v>761</v>
       </c>
-      <c r="B284" s="51">
+      <c r="B284" s="50">
         <v>13.0</v>
       </c>
-      <c r="C284" s="51">
+      <c r="C284" s="50">
         <v>13.0</v>
       </c>
     </row>
@@ -29818,10 +29815,10 @@
       <c r="A290" s="30" t="s">
         <v>771</v>
       </c>
-      <c r="B290" s="50">
+      <c r="B290" s="49">
         <v>12.0</v>
       </c>
-      <c r="C290" s="50">
+      <c r="C290" s="49">
         <v>12.0</v>
       </c>
     </row>
@@ -29873,10 +29870,10 @@
       <c r="A295" s="30" t="s">
         <v>779</v>
       </c>
-      <c r="B295" s="50">
+      <c r="B295" s="49">
         <v>2.0</v>
       </c>
-      <c r="C295" s="50">
+      <c r="C295" s="49">
         <v>2.0</v>
       </c>
     </row>
@@ -29917,10 +29914,10 @@
       <c r="A299" s="30" t="s">
         <v>785</v>
       </c>
-      <c r="B299" s="50">
+      <c r="B299" s="49">
         <v>7.0</v>
       </c>
-      <c r="C299" s="50">
+      <c r="C299" s="49">
         <v>7.0</v>
       </c>
     </row>
@@ -29928,10 +29925,10 @@
       <c r="A300" s="30" t="s">
         <v>786</v>
       </c>
-      <c r="B300" s="50">
+      <c r="B300" s="49">
         <v>8.0</v>
       </c>
-      <c r="C300" s="50">
+      <c r="C300" s="49">
         <v>8.0</v>
       </c>
     </row>
@@ -29975,7 +29972,7 @@
       <c r="B304" s="30" t="s">
         <v>793</v>
       </c>
-      <c r="C304" s="49" t="s">
+      <c r="C304" s="48" t="s">
         <v>793</v>
       </c>
     </row>
@@ -29983,10 +29980,10 @@
       <c r="A305" s="30" t="s">
         <v>794</v>
       </c>
-      <c r="B305" s="50">
+      <c r="B305" s="49">
         <v>6.0</v>
       </c>
-      <c r="C305" s="50">
+      <c r="C305" s="49">
         <v>6.0</v>
       </c>
     </row>
@@ -30027,10 +30024,10 @@
       <c r="A309" s="30" t="s">
         <v>800</v>
       </c>
-      <c r="B309" s="50">
+      <c r="B309" s="49">
         <v>9.0</v>
       </c>
-      <c r="C309" s="50">
+      <c r="C309" s="49">
         <v>9.0</v>
       </c>
     </row>
@@ -30038,10 +30035,10 @@
       <c r="A310" s="30" t="s">
         <v>801</v>
       </c>
-      <c r="B310" s="50">
+      <c r="B310" s="49">
         <v>10.0</v>
       </c>
-      <c r="C310" s="50">
+      <c r="C310" s="49">
         <v>10.0</v>
       </c>
     </row>
@@ -30082,10 +30079,10 @@
       <c r="A314" s="30" t="s">
         <v>806</v>
       </c>
-      <c r="B314" s="50">
+      <c r="B314" s="49">
         <v>12.0</v>
       </c>
-      <c r="C314" s="50">
+      <c r="C314" s="49">
         <v>12.0</v>
       </c>
     </row>
@@ -30093,10 +30090,10 @@
       <c r="A315" s="30" t="s">
         <v>807</v>
       </c>
-      <c r="B315" s="50">
+      <c r="B315" s="49">
         <v>13.0</v>
       </c>
-      <c r="C315" s="50">
+      <c r="C315" s="49">
         <v>13.0</v>
       </c>
     </row>
@@ -30148,10 +30145,10 @@
       <c r="A320" s="30" t="s">
         <v>814</v>
       </c>
-      <c r="B320" s="50">
+      <c r="B320" s="49">
         <v>6.0</v>
       </c>
-      <c r="C320" s="50">
+      <c r="C320" s="49">
         <v>6.0</v>
       </c>
     </row>
@@ -30203,10 +30200,10 @@
       <c r="A325" s="30" t="s">
         <v>822</v>
       </c>
-      <c r="B325" s="50">
+      <c r="B325" s="49">
         <v>7.0</v>
       </c>
-      <c r="C325" s="50">
+      <c r="C325" s="49">
         <v>7.0</v>
       </c>
     </row>
@@ -30258,10 +30255,10 @@
       <c r="A330" s="30" t="s">
         <v>830</v>
       </c>
-      <c r="B330" s="50">
+      <c r="B330" s="49">
         <v>3.0</v>
       </c>
-      <c r="C330" s="50">
+      <c r="C330" s="49">
         <v>3.0</v>
       </c>
     </row>
@@ -30313,10 +30310,10 @@
       <c r="A335" s="30" t="s">
         <v>838</v>
       </c>
-      <c r="B335" s="50">
+      <c r="B335" s="49">
         <v>3.0</v>
       </c>
-      <c r="C335" s="50">
+      <c r="C335" s="49">
         <v>3.0</v>
       </c>
     </row>
@@ -30368,10 +30365,10 @@
       <c r="A340" s="30" t="s">
         <v>846</v>
       </c>
-      <c r="B340" s="50">
+      <c r="B340" s="49">
         <v>3.0</v>
       </c>
-      <c r="C340" s="50">
+      <c r="C340" s="49">
         <v>3.0</v>
       </c>
     </row>
@@ -30412,10 +30409,10 @@
       <c r="A344" s="30" t="s">
         <v>852</v>
       </c>
-      <c r="B344" s="49" t="s">
+      <c r="B344" s="48" t="s">
         <v>853</v>
       </c>
-      <c r="C344" s="49" t="s">
+      <c r="C344" s="48" t="s">
         <v>853</v>
       </c>
     </row>
@@ -30423,10 +30420,10 @@
       <c r="A345" s="30" t="s">
         <v>854</v>
       </c>
-      <c r="B345" s="50">
+      <c r="B345" s="49">
         <v>3.0</v>
       </c>
-      <c r="C345" s="50">
+      <c r="C345" s="49">
         <v>3.0</v>
       </c>
     </row>
@@ -30478,10 +30475,10 @@
       <c r="A350" s="30" t="s">
         <v>862</v>
       </c>
-      <c r="B350" s="50" t="s">
+      <c r="B350" s="49" t="s">
         <v>863</v>
       </c>
-      <c r="C350" s="50" t="s">
+      <c r="C350" s="49" t="s">
         <v>863</v>
       </c>
     </row>
@@ -30489,10 +30486,10 @@
       <c r="A351" s="30" t="s">
         <v>864</v>
       </c>
-      <c r="B351" s="50">
+      <c r="B351" s="49">
         <v>6.0</v>
       </c>
-      <c r="C351" s="50">
+      <c r="C351" s="49">
         <v>6.0</v>
       </c>
     </row>
@@ -30533,10 +30530,10 @@
       <c r="A355" s="30" t="s">
         <v>870</v>
       </c>
-      <c r="B355" s="50">
+      <c r="B355" s="49">
         <v>50.0</v>
       </c>
-      <c r="C355" s="50">
+      <c r="C355" s="49">
         <v>50.0</v>
       </c>
     </row>
@@ -30544,10 +30541,10 @@
       <c r="A356" s="30" t="s">
         <v>871</v>
       </c>
-      <c r="B356" s="50">
+      <c r="B356" s="49">
         <v>55.0</v>
       </c>
-      <c r="C356" s="50">
+      <c r="C356" s="49">
         <v>55.0</v>
       </c>
     </row>
@@ -30744,7 +30741,7 @@
     <row r="377" ht="15.75" customHeight="1"/>
     <row r="378" ht="15.75" customHeight="1"/>
     <row r="379" ht="15.75" customHeight="1">
-      <c r="B379" s="43" t="s">
+      <c r="B379" s="42" t="s">
         <v>903</v>
       </c>
     </row>
@@ -30819,7 +30816,7 @@
     </row>
     <row r="389" ht="15.75" customHeight="1"/>
     <row r="390" ht="15.75" customHeight="1">
-      <c r="B390" s="43" t="s">
+      <c r="B390" s="42" t="s">
         <v>915</v>
       </c>
     </row>
@@ -31323,7 +31320,7 @@
       </c>
     </row>
     <row r="440" ht="15.75" customHeight="1">
-      <c r="B440" s="43" t="s">
+      <c r="B440" s="42" t="s">
         <v>1005</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Push For HappyPath(13/02/23)
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -27413,8 +27413,8 @@
   </sheetPr>
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -29479,10 +29479,10 @@
         <v>607</v>
       </c>
       <c r="B76" s="51" t="s">
-        <v>608</v>
+        <v>8</v>
       </c>
       <c r="C76" s="51" t="s">
-        <v>608</v>
+        <v>8</v>
       </c>
       <c r="D76"/>
       <c r="E76"/>
@@ -29510,10 +29510,10 @@
         <v>609</v>
       </c>
       <c r="B77" s="51" t="s">
-        <v>608</v>
+        <v>8</v>
       </c>
       <c r="C77" s="51" t="s">
-        <v>608</v>
+        <v>8</v>
       </c>
       <c r="D77"/>
       <c r="E77"/>

</xml_diff>

<commit_message>
Jenkis test for Sanity (23/02/23)
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1973" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="1008">
   <si>
     <t>KEY</t>
   </si>
@@ -3052,7 +3052,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -3123,6 +3123,11 @@
     </font>
     <font>
       <b/>
+      <color rgb="FF297BDE"/>
+      <name val="&quot;JetBrains Mono&quot;"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11.0"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
@@ -3160,7 +3165,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3183,6 +3188,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA8D08D"/>
         <bgColor rgb="FFA8D08D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2B2B2B"/>
+        <bgColor rgb="FF2B2B2B"/>
       </patternFill>
     </fill>
     <fill>
@@ -3234,7 +3245,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3288,20 +3299,23 @@
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="6" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3322,23 +3336,23 @@
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="15" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="6" fontId="13" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="16" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="15" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="16" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="15" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="2" fontId="16" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="12" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="2" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="6" fontId="13" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="2" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -26476,7 +26490,17 @@
         <v>257</v>
       </c>
     </row>
-    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1">
+      <c r="A112" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
     <row r="113" ht="15.75" customHeight="1"/>
     <row r="114" ht="15.75" customHeight="1"/>
     <row r="115" ht="15.75" customHeight="1"/>
@@ -27409,26 +27433,26 @@
       <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
     </row>
     <row r="2">
       <c r="A2" s="26" t="s">
@@ -27464,7 +27488,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="29" t="s">
         <v>589</v>
       </c>
     </row>
@@ -27635,7 +27659,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.0" customHeight="1">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="30" t="s">
         <v>256</v>
       </c>
       <c r="B27" s="26" t="s">
@@ -27647,7 +27671,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="31" t="s">
         <v>597</v>
       </c>
     </row>
@@ -27675,296 +27699,296 @@
     </row>
     <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="32" t="s">
         <v>600</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="32" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="32" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="36" ht="13.5" customHeight="1">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C36" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="37" ht="13.5" customHeight="1"/>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="32" t="s">
         <v>601</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="32" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="39" ht="13.5" customHeight="1">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="31" t="s">
+      <c r="C39" s="32" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="40" ht="13.5" customHeight="1">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="C40" s="32" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="41" ht="13.5" customHeight="1">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="31" t="s">
+      <c r="C41" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="42" ht="13.5" customHeight="1"/>
     <row r="43" ht="13.5" customHeight="1">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="32" t="s">
         <v>602</v>
       </c>
-      <c r="C43" s="31" t="s">
+      <c r="C43" s="32" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="44" ht="13.5" customHeight="1">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="31" t="s">
+      <c r="C44" s="32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="45" ht="13.5" customHeight="1">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="31" t="s">
+      <c r="C45" s="32" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="46" ht="13.5" customHeight="1">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C46" s="31" t="s">
+      <c r="C46" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="47" ht="13.5" customHeight="1"/>
     <row r="48" ht="13.5" customHeight="1">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="32" t="s">
         <v>603</v>
       </c>
-      <c r="C48" s="31" t="s">
+      <c r="C48" s="32" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="49" ht="13.5" customHeight="1">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="31" t="s">
+      <c r="C49" s="32" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="50" ht="13.5" customHeight="1">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="31" t="s">
+      <c r="C50" s="32" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="51" ht="13.5" customHeight="1">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C51" s="31" t="s">
+      <c r="C51" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="52" ht="13.5" customHeight="1"/>
     <row r="53" ht="13.5" customHeight="1">
-      <c r="A53" s="31" t="s">
+      <c r="A53" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B53" s="31" t="s">
+      <c r="B53" s="32" t="s">
         <v>600</v>
       </c>
-      <c r="C53" s="31" t="s">
+      <c r="C53" s="32" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="54" ht="13.5" customHeight="1">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="31" t="s">
+      <c r="B54" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C54" s="31" t="s">
+      <c r="C54" s="32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="55" ht="13.5" customHeight="1">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B55" s="31" t="s">
+      <c r="B55" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="31" t="s">
+      <c r="C55" s="32" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="56" ht="13.5" customHeight="1">
-      <c r="A56" s="31" t="s">
+      <c r="A56" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="31" t="s">
+      <c r="B56" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="31" t="s">
+      <c r="C56" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="57" ht="13.5" customHeight="1">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="31" t="s">
+      <c r="B57" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="31" t="s">
+      <c r="C57" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="58" ht="13.5" customHeight="1">
-      <c r="A58" s="31" t="s">
+      <c r="A58" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="32" t="s">
         <v>604</v>
       </c>
-      <c r="C58" s="31" t="s">
+      <c r="C58" s="32" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="59" ht="13.5" customHeight="1"/>
     <row r="60" ht="13.5" customHeight="1"/>
     <row r="61" ht="13.5" customHeight="1">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B61" s="31" t="s">
+      <c r="B61" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C61" s="31" t="s">
+      <c r="C61" s="32" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="62" ht="13.5" customHeight="1">
-      <c r="A62" s="31" t="s">
+      <c r="A62" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B62" s="31" t="s">
+      <c r="B62" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C62" s="31" t="s">
+      <c r="C62" s="32" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="63" ht="13.5" customHeight="1"/>
     <row r="64" ht="13.5" customHeight="1">
-      <c r="A64" s="31" t="s">
+      <c r="A64" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B64" s="31" t="s">
+      <c r="B64" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C64" s="31" t="s">
+      <c r="C64" s="32" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="65" ht="13.5" customHeight="1"/>
     <row r="66" ht="13.5" customHeight="1">
-      <c r="A66" s="31" t="s">
+      <c r="A66" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B66" s="31" t="s">
+      <c r="B66" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C66" s="31" t="s">
+      <c r="C66" s="32" t="s">
         <v>40</v>
       </c>
     </row>
@@ -27975,7 +27999,7 @@
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1"/>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="B73" s="28" t="s">
+      <c r="B73" s="29" t="s">
         <v>605</v>
       </c>
     </row>
@@ -27987,7 +28011,7 @@
       <c r="B75" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="C75" s="32" t="s">
+      <c r="C75" s="33" t="s">
         <v>228</v>
       </c>
     </row>
@@ -27995,10 +28019,10 @@
       <c r="A76" s="26" t="s">
         <v>607</v>
       </c>
-      <c r="B76" s="33" t="s">
+      <c r="B76" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C76" s="33" t="s">
+      <c r="C76" s="34" t="s">
         <v>8</v>
       </c>
     </row>
@@ -28006,10 +28030,10 @@
       <c r="A77" s="26" t="s">
         <v>608</v>
       </c>
-      <c r="B77" s="33" t="s">
+      <c r="B77" s="34" t="s">
         <v>609</v>
       </c>
-      <c r="C77" s="33" t="s">
+      <c r="C77" s="34" t="s">
         <v>609</v>
       </c>
     </row>
@@ -28107,7 +28131,7 @@
     </row>
     <row r="90" ht="15.75" customHeight="1"/>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="34" t="s">
+      <c r="A91" s="35" t="s">
         <v>626</v>
       </c>
       <c r="B91" s="26" t="s">
@@ -28118,7 +28142,7 @@
       </c>
     </row>
     <row r="92" ht="15.0" customHeight="1">
-      <c r="A92" s="34" t="s">
+      <c r="A92" s="35" t="s">
         <v>628</v>
       </c>
       <c r="B92" s="26" t="s">
@@ -28131,7 +28155,7 @@
     <row r="93" ht="15.75" customHeight="1"/>
     <row r="94" ht="15.75" customHeight="1"/>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="B95" s="28" t="s">
+      <c r="B95" s="29" t="s">
         <v>630</v>
       </c>
     </row>
@@ -28161,7 +28185,7 @@
     </row>
     <row r="100" ht="15.75" customHeight="1"/>
     <row r="101" ht="15.0" customHeight="1">
-      <c r="A101" s="35" t="s">
+      <c r="A101" s="36" t="s">
         <v>633</v>
       </c>
       <c r="B101" s="26" t="s">
@@ -28173,7 +28197,7 @@
     </row>
     <row r="102" ht="15.75" customHeight="1"/>
     <row r="103" ht="15.0" customHeight="1">
-      <c r="A103" s="34" t="s">
+      <c r="A103" s="35" t="s">
         <v>634</v>
       </c>
       <c r="B103" s="26" t="s">
@@ -28184,7 +28208,7 @@
       </c>
     </row>
     <row r="104" ht="15.0" customHeight="1">
-      <c r="A104" s="34" t="s">
+      <c r="A104" s="35" t="s">
         <v>636</v>
       </c>
       <c r="B104" s="26" t="s">
@@ -28196,7 +28220,7 @@
     </row>
     <row r="105" ht="15.75" customHeight="1"/>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="B106" s="28" t="s">
+      <c r="B106" s="29" t="s">
         <v>638</v>
       </c>
     </row>
@@ -28248,7 +28272,7 @@
       </c>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="35" t="s">
+      <c r="A114" s="36" t="s">
         <v>643</v>
       </c>
       <c r="B114" s="26" t="s">
@@ -28259,7 +28283,7 @@
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="35" t="s">
+      <c r="A115" s="36" t="s">
         <v>645</v>
       </c>
       <c r="B115" s="26" t="s">
@@ -28270,7 +28294,7 @@
       </c>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="35" t="s">
+      <c r="A116" s="36" t="s">
         <v>647</v>
       </c>
       <c r="B116" s="26" t="s">
@@ -28282,7 +28306,7 @@
     </row>
     <row r="117" ht="15.75" customHeight="1"/>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="35" t="s">
+      <c r="A118" s="36" t="s">
         <v>649</v>
       </c>
       <c r="B118" s="26" t="s">
@@ -28293,7 +28317,7 @@
       </c>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="35" t="s">
+      <c r="A119" s="36" t="s">
         <v>651</v>
       </c>
       <c r="B119" s="26" t="s">
@@ -28304,7 +28328,7 @@
       </c>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="35" t="s">
+      <c r="A120" s="36" t="s">
         <v>653</v>
       </c>
       <c r="B120" s="26" t="s">
@@ -28316,7 +28340,7 @@
     </row>
     <row r="121" ht="15.75" customHeight="1"/>
     <row r="122" ht="15.0" customHeight="1">
-      <c r="B122" s="28" t="s">
+      <c r="B122" s="29" t="s">
         <v>655</v>
       </c>
     </row>
@@ -28345,7 +28369,7 @@
     <row r="125" ht="15.75" customHeight="1"/>
     <row r="126" ht="15.75" customHeight="1"/>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="35" t="s">
+      <c r="A127" s="36" t="s">
         <v>658</v>
       </c>
       <c r="B127" s="26" t="s">
@@ -28356,7 +28380,7 @@
       </c>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="35" t="s">
+      <c r="A128" s="36" t="s">
         <v>660</v>
       </c>
       <c r="B128" s="26" t="s">
@@ -28367,7 +28391,7 @@
       </c>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="35" t="s">
+      <c r="A129" s="36" t="s">
         <v>662</v>
       </c>
       <c r="B129" s="26" t="s">
@@ -28378,7 +28402,7 @@
       </c>
     </row>
     <row r="130" ht="15.0" customHeight="1">
-      <c r="A130" s="35" t="s">
+      <c r="A130" s="36" t="s">
         <v>664</v>
       </c>
       <c r="B130" s="26" t="s">
@@ -28503,41 +28527,41 @@
     </row>
     <row r="144" ht="15.75" customHeight="1"/>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="36" t="s">
+      <c r="A145" s="37" t="s">
         <v>686</v>
       </c>
-      <c r="B145" s="31" t="s">
+      <c r="B145" s="32" t="s">
         <v>687</v>
       </c>
-      <c r="C145" s="31" t="s">
+      <c r="C145" s="32" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="36" t="s">
+      <c r="A146" s="37" t="s">
         <v>688</v>
       </c>
-      <c r="B146" s="31" t="s">
+      <c r="B146" s="32" t="s">
         <v>687</v>
       </c>
-      <c r="C146" s="31" t="s">
+      <c r="C146" s="32" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="147" ht="15.0" customHeight="1">
-      <c r="A147" s="36" t="s">
+      <c r="A147" s="37" t="s">
         <v>689</v>
       </c>
-      <c r="B147" s="31" t="s">
+      <c r="B147" s="32" t="s">
         <v>687</v>
       </c>
-      <c r="C147" s="31" t="s">
+      <c r="C147" s="32" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="148" ht="15.75" customHeight="1"/>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="B149" s="28" t="s">
+      <c r="B149" s="29" t="s">
         <v>690</v>
       </c>
     </row>
@@ -28553,13 +28577,13 @@
       </c>
     </row>
     <row r="151" ht="15.0" customHeight="1">
-      <c r="A151" s="36" t="s">
+      <c r="A151" s="37" t="s">
         <v>693</v>
       </c>
-      <c r="B151" s="37" t="s">
+      <c r="B151" s="38" t="s">
         <v>694</v>
       </c>
-      <c r="C151" s="37" t="s">
+      <c r="C151" s="38" t="s">
         <v>694</v>
       </c>
     </row>
@@ -28587,222 +28611,222 @@
     </row>
     <row r="154" ht="15.75" customHeight="1"/>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="38" t="s">
+      <c r="A155" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B155" s="37" t="s">
+      <c r="B155" s="38" t="s">
         <v>692</v>
       </c>
-      <c r="C155" s="37" t="s">
+      <c r="C155" s="38" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="156" ht="15.0" customHeight="1">
-      <c r="A156" s="38" t="s">
+      <c r="A156" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B156" s="37" t="s">
+      <c r="B156" s="38" t="s">
         <v>694</v>
       </c>
-      <c r="C156" s="37" t="s">
+      <c r="C156" s="38" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="157" ht="15.0" customHeight="1">
-      <c r="A157" s="38" t="s">
+      <c r="A157" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B157" s="37" t="s">
+      <c r="B157" s="38" t="s">
         <v>695</v>
       </c>
-      <c r="C157" s="37" t="s">
+      <c r="C157" s="38" t="s">
         <v>695</v>
       </c>
     </row>
     <row r="158" ht="15.75" customHeight="1"/>
     <row r="159" ht="15.75" customHeight="1"/>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="38" t="s">
+      <c r="A160" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B160" s="37" t="s">
+      <c r="B160" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C160" s="37" t="s">
+      <c r="C160" s="38" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="161" ht="15.0" customHeight="1">
-      <c r="A161" s="38" t="s">
+      <c r="A161" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B161" s="37" t="s">
+      <c r="B161" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C161" s="37" t="s">
+      <c r="C161" s="38" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="162" ht="15.0" customHeight="1">
-      <c r="A162" s="38" t="s">
+      <c r="A162" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="163" ht="15.75" customHeight="1"/>
     <row r="164" ht="15.75" customHeight="1"/>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="38" t="s">
+      <c r="A165" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B165" s="37" t="s">
+      <c r="B165" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C165" s="37" t="s">
+      <c r="C165" s="38" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="166" ht="15.0" customHeight="1">
-      <c r="A166" s="38" t="s">
+      <c r="A166" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="B166" s="37" t="s">
+      <c r="B166" s="38" t="s">
         <v>696</v>
       </c>
-      <c r="C166" s="37" t="s">
+      <c r="C166" s="38" t="s">
         <v>696</v>
       </c>
     </row>
     <row r="167" ht="15.0" customHeight="1">
-      <c r="A167" s="38" t="s">
+      <c r="A167" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="168" ht="15.75" customHeight="1"/>
     <row r="169" ht="15.75" customHeight="1"/>
     <row r="170" ht="15.0" customHeight="1">
-      <c r="A170" s="38" t="s">
+      <c r="A170" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="B170" s="37" t="s">
+      <c r="B170" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="C170" s="37" t="s">
+      <c r="C170" s="38" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="171" ht="15.0" customHeight="1">
-      <c r="A171" s="38" t="s">
+      <c r="A171" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="B171" s="37" t="s">
+      <c r="B171" s="38" t="s">
         <v>697</v>
       </c>
-      <c r="C171" s="37" t="s">
+      <c r="C171" s="38" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="38" t="s">
+      <c r="A172" s="39" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="173" ht="15.75" customHeight="1"/>
     <row r="174" ht="15.75" customHeight="1"/>
     <row r="175" ht="15.0" customHeight="1">
-      <c r="A175" s="38" t="s">
+      <c r="A175" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="B175" s="37" t="s">
+      <c r="B175" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="C175" s="37" t="s">
+      <c r="C175" s="38" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="38" t="s">
+      <c r="A176" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B176" s="37" t="s">
+      <c r="B176" s="38" t="s">
         <v>697</v>
       </c>
-      <c r="C176" s="37" t="s">
+      <c r="C176" s="38" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="177" ht="15.75" customHeight="1"/>
     <row r="178" ht="15.75" customHeight="1"/>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="38" t="s">
+      <c r="A179" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="B179" s="37" t="s">
+      <c r="B179" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="C179" s="37" t="s">
+      <c r="C179" s="38" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="38" t="s">
+      <c r="A180" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="B180" s="37" t="s">
+      <c r="B180" s="38" t="s">
         <v>697</v>
       </c>
-      <c r="C180" s="37" t="s">
+      <c r="C180" s="38" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="181" ht="15.75" customHeight="1"/>
     <row r="182" ht="15.75" customHeight="1"/>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="38" t="s">
+      <c r="A183" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="B183" s="37" t="s">
+      <c r="B183" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C183" s="37" t="s">
+      <c r="C183" s="38" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="38" t="s">
+      <c r="A184" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="B184" s="37" t="s">
+      <c r="B184" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="C184" s="37" t="s">
+      <c r="C184" s="38" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="38" t="s">
+      <c r="A185" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="B185" s="37" t="s">
+      <c r="B185" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C185" s="37" t="s">
+      <c r="C185" s="38" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="37" t="s">
+      <c r="A186" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="B186" s="37" t="s">
+      <c r="B186" s="38" t="s">
         <v>698</v>
       </c>
-      <c r="C186" s="37" t="s">
+      <c r="C186" s="38" t="s">
         <v>698</v>
       </c>
     </row>
     <row r="187" ht="15.75" customHeight="1"/>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="B188" s="39" t="s">
+      <c r="B188" s="40" t="s">
         <v>699</v>
       </c>
     </row>
@@ -28811,7 +28835,7 @@
     <row r="191" ht="15.75" customHeight="1"/>
     <row r="192" ht="15.75" customHeight="1"/>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="40" t="s">
+      <c r="A193" s="41" t="s">
         <v>3</v>
       </c>
       <c r="B193" s="2" t="s">
@@ -28822,672 +28846,672 @@
       </c>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="40" t="s">
+      <c r="A194" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B194" s="41" t="s">
+      <c r="B194" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="C194" s="41" t="s">
+      <c r="C194" s="42" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="40" t="s">
+      <c r="A195" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B195" s="40" t="s">
+      <c r="B195" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C195" s="40" t="s">
+      <c r="C195" s="41" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="40" t="s">
+      <c r="A196" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="B196" s="40" t="s">
+      <c r="B196" s="41" t="s">
         <v>700</v>
       </c>
-      <c r="C196" s="40" t="s">
+      <c r="C196" s="41" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="40" t="s">
+      <c r="A197" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="B197" s="27" t="s">
+      <c r="B197" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C197" s="27" t="s">
+      <c r="C197" s="28" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="40" t="s">
+      <c r="A198" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="B198" s="42" t="s">
+      <c r="B198" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="C198" s="42" t="s">
+      <c r="C198" s="43" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="40" t="s">
+      <c r="A199" s="41" t="s">
         <v>279</v>
       </c>
-      <c r="B199" s="27" t="s">
+      <c r="B199" s="28" t="s">
         <v>280</v>
       </c>
-      <c r="C199" s="27" t="s">
+      <c r="C199" s="28" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="40" t="s">
+      <c r="A200" s="41" t="s">
         <v>193</v>
       </c>
-      <c r="B200" s="40" t="s">
+      <c r="B200" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="C200" s="40" t="s">
+      <c r="C200" s="41" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="40" t="s">
+      <c r="A201" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="B201" s="40" t="s">
+      <c r="B201" s="41" t="s">
         <v>213</v>
       </c>
-      <c r="C201" s="40" t="s">
+      <c r="C201" s="41" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="40" t="s">
+      <c r="A202" s="41" t="s">
         <v>209</v>
       </c>
-      <c r="B202" s="40" t="s">
+      <c r="B202" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="C202" s="40" t="s">
+      <c r="C202" s="41" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="40" t="s">
+      <c r="A203" s="41" t="s">
         <v>211</v>
       </c>
-      <c r="B203" s="40" t="s">
+      <c r="B203" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="C203" s="40" t="s">
+      <c r="C203" s="41" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="40" t="s">
+      <c r="A204" s="41" t="s">
         <v>197</v>
       </c>
-      <c r="B204" s="40" t="s">
+      <c r="B204" s="41" t="s">
         <v>198</v>
       </c>
-      <c r="C204" s="40" t="s">
+      <c r="C204" s="41" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="40" t="s">
+      <c r="A205" s="41" t="s">
         <v>287</v>
       </c>
-      <c r="B205" s="40" t="s">
+      <c r="B205" s="41" t="s">
         <v>288</v>
       </c>
-      <c r="C205" s="40" t="s">
+      <c r="C205" s="41" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="40" t="s">
+      <c r="A206" s="41" t="s">
         <v>165</v>
       </c>
-      <c r="B206" s="27" t="s">
+      <c r="B206" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="C206" s="27" t="s">
+      <c r="C206" s="28" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="40" t="s">
+      <c r="A207" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="B207" s="42" t="s">
+      <c r="B207" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="C207" s="42" t="s">
+      <c r="C207" s="43" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="40" t="s">
+      <c r="A208" s="41" t="s">
         <v>285</v>
       </c>
-      <c r="B208" s="27" t="s">
+      <c r="B208" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="C208" s="27" t="s">
+      <c r="C208" s="28" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="209" ht="15.75" customHeight="1"/>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="40" t="s">
+      <c r="A210" s="41" t="s">
         <v>333</v>
       </c>
-      <c r="B210" s="40" t="s">
+      <c r="B210" s="41" t="s">
         <v>334</v>
       </c>
-      <c r="C210" s="40" t="s">
+      <c r="C210" s="41" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="40" t="s">
+      <c r="A211" s="41" t="s">
         <v>701</v>
       </c>
-      <c r="B211" s="42" t="s">
+      <c r="B211" s="43" t="s">
         <v>702</v>
       </c>
-      <c r="C211" s="42" t="s">
+      <c r="C211" s="43" t="s">
         <v>702</v>
       </c>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="40" t="s">
+      <c r="A212" s="41" t="s">
         <v>337</v>
       </c>
-      <c r="B212" s="27" t="s">
+      <c r="B212" s="28" t="s">
         <v>703</v>
       </c>
-      <c r="C212" s="27" t="s">
+      <c r="C212" s="28" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="40" t="s">
+      <c r="A213" s="41" t="s">
         <v>704</v>
       </c>
-      <c r="B213" s="27" t="s">
+      <c r="B213" s="28" t="s">
         <v>340</v>
       </c>
-      <c r="C213" s="27" t="s">
+      <c r="C213" s="28" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="40" t="s">
+      <c r="A214" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="B214" s="40" t="s">
+      <c r="B214" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="C214" s="40" t="s">
+      <c r="C214" s="41" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="40" t="s">
+      <c r="A215" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="B215" s="42" t="s">
+      <c r="B215" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="C215" s="42" t="s">
+      <c r="C215" s="43" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="40" t="s">
+      <c r="A216" s="41" t="s">
         <v>289</v>
       </c>
-      <c r="B216" s="40" t="s">
+      <c r="B216" s="41" t="s">
         <v>290</v>
       </c>
-      <c r="C216" s="40" t="s">
+      <c r="C216" s="41" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="40" t="s">
+      <c r="A217" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="B217" s="40" t="s">
+      <c r="B217" s="41" t="s">
         <v>204</v>
       </c>
-      <c r="C217" s="40" t="s">
+      <c r="C217" s="41" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="40" t="s">
+      <c r="A218" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="B218" s="40" t="s">
+      <c r="B218" s="41" t="s">
         <v>206</v>
       </c>
-      <c r="C218" s="40" t="s">
+      <c r="C218" s="41" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="219" ht="15.75" customHeight="1"/>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="40" t="s">
+      <c r="A220" s="41" t="s">
         <v>705</v>
       </c>
-      <c r="B220" s="42" t="s">
+      <c r="B220" s="43" t="s">
         <v>706</v>
       </c>
-      <c r="C220" s="42" t="s">
+      <c r="C220" s="43" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="40" t="s">
+      <c r="A221" s="41" t="s">
         <v>707</v>
       </c>
-      <c r="B221" s="27" t="s">
+      <c r="B221" s="28" t="s">
         <v>708</v>
       </c>
-      <c r="C221" s="27" t="s">
+      <c r="C221" s="28" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="40" t="s">
+      <c r="A222" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="B222" s="40" t="s">
+      <c r="B222" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="C222" s="40" t="s">
+      <c r="C222" s="41" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="40" t="s">
+      <c r="A223" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="B223" s="42" t="s">
+      <c r="B223" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="C223" s="42" t="s">
+      <c r="C223" s="43" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="40" t="s">
+      <c r="A224" s="41" t="s">
         <v>297</v>
       </c>
-      <c r="B224" s="40" t="s">
+      <c r="B224" s="41" t="s">
         <v>298</v>
       </c>
-      <c r="C224" s="40" t="s">
+      <c r="C224" s="41" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="40" t="s">
+      <c r="A225" s="41" t="s">
         <v>709</v>
       </c>
-      <c r="B225" s="40" t="s">
+      <c r="B225" s="41" t="s">
         <v>710</v>
       </c>
-      <c r="C225" s="40" t="s">
+      <c r="C225" s="41" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="40" t="s">
+      <c r="A226" s="41" t="s">
         <v>341</v>
       </c>
-      <c r="B226" s="40" t="s">
+      <c r="B226" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="C226" s="40" t="s">
+      <c r="C226" s="41" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="40" t="s">
+      <c r="A227" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="B227" s="40" t="s">
+      <c r="B227" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="C227" s="40" t="s">
+      <c r="C227" s="41" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="A228" s="40" t="s">
+      <c r="A228" s="41" t="s">
         <v>711</v>
       </c>
-      <c r="B228" s="40" t="s">
+      <c r="B228" s="41" t="s">
         <v>712</v>
       </c>
-      <c r="C228" s="40" t="s">
+      <c r="C228" s="41" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="A229" s="40" t="s">
+      <c r="A229" s="41" t="s">
         <v>344</v>
       </c>
-      <c r="B229" s="40" t="s">
+      <c r="B229" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="C229" s="40" t="s">
+      <c r="C229" s="41" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="A230" s="40" t="s">
+      <c r="A230" s="41" t="s">
         <v>713</v>
       </c>
-      <c r="B230" s="42" t="s">
+      <c r="B230" s="43" t="s">
         <v>714</v>
       </c>
-      <c r="C230" s="42" t="s">
+      <c r="C230" s="43" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="A231" s="40" t="s">
+      <c r="A231" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="B231" s="40" t="s">
+      <c r="B231" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="C231" s="40" t="s">
+      <c r="C231" s="41" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="40" t="s">
+      <c r="A232" s="41" t="s">
         <v>223</v>
       </c>
-      <c r="B232" s="40" t="s">
+      <c r="B232" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="C232" s="40" t="s">
+      <c r="C232" s="41" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="233" ht="15.75" customHeight="1"/>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="A234" s="40" t="s">
+      <c r="A234" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="B234" s="40" t="s">
+      <c r="B234" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="C234" s="40" t="s">
+      <c r="C234" s="41" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="A235" s="40" t="s">
+      <c r="A235" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="B235" s="40" t="s">
+      <c r="B235" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="C235" s="40" t="s">
+      <c r="C235" s="41" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="A236" s="40" t="s">
+      <c r="A236" s="41" t="s">
         <v>715</v>
       </c>
-      <c r="B236" s="42" t="s">
+      <c r="B236" s="43" t="s">
         <v>716</v>
       </c>
-      <c r="C236" s="42" t="s">
+      <c r="C236" s="43" t="s">
         <v>716</v>
       </c>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="40" t="s">
+      <c r="A237" s="41" t="s">
         <v>201</v>
       </c>
-      <c r="B237" s="40" t="s">
+      <c r="B237" s="41" t="s">
         <v>202</v>
       </c>
-      <c r="C237" s="40" t="s">
+      <c r="C237" s="41" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="A238" s="40" t="s">
+      <c r="A238" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="B238" s="40" t="s">
+      <c r="B238" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="C238" s="40" t="s">
+      <c r="C238" s="41" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="A239" s="40" t="s">
+      <c r="A239" s="41" t="s">
         <v>717</v>
       </c>
-      <c r="B239" s="42" t="s">
+      <c r="B239" s="43" t="s">
         <v>718</v>
       </c>
-      <c r="C239" s="42" t="s">
+      <c r="C239" s="43" t="s">
         <v>718</v>
       </c>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="A240" s="40" t="s">
+      <c r="A240" s="41" t="s">
         <v>719</v>
       </c>
-      <c r="B240" s="42" t="s">
+      <c r="B240" s="43" t="s">
         <v>720</v>
       </c>
-      <c r="C240" s="42" t="s">
+      <c r="C240" s="43" t="s">
         <v>720</v>
       </c>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="A241" s="40" t="s">
+      <c r="A241" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="B241" s="42" t="s">
+      <c r="B241" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="C241" s="42" t="s">
+      <c r="C241" s="43" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="A242" s="40" t="s">
+      <c r="A242" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="B242" s="40" t="s">
+      <c r="B242" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="C242" s="40" t="s">
+      <c r="C242" s="41" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="A243" s="40" t="s">
+      <c r="A243" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="B243" s="42" t="s">
+      <c r="B243" s="43" t="s">
         <v>721</v>
       </c>
-      <c r="C243" s="42" t="s">
+      <c r="C243" s="43" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="A244" s="40" t="s">
+      <c r="A244" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="B244" s="43" t="s">
+      <c r="B244" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="C244" s="43" t="s">
+      <c r="C244" s="44" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="A245" s="40" t="s">
+      <c r="A245" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="B245" s="40" t="s">
+      <c r="B245" s="41" t="s">
         <v>192</v>
       </c>
-      <c r="C245" s="40" t="s">
+      <c r="C245" s="41" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="A246" s="40" t="s">
+      <c r="A246" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="B246" s="40" t="s">
+      <c r="B246" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="C246" s="40" t="s">
+      <c r="C246" s="41" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="A247" s="40" t="s">
+      <c r="A247" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="B247" s="42" t="s">
+      <c r="B247" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="C247" s="42" t="s">
+      <c r="C247" s="43" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="A248" s="40" t="s">
+      <c r="A248" s="41" t="s">
         <v>195</v>
       </c>
-      <c r="B248" s="42" t="s">
+      <c r="B248" s="43" t="s">
         <v>196</v>
       </c>
-      <c r="C248" s="42" t="s">
+      <c r="C248" s="43" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="A249" s="40" t="s">
+      <c r="A249" s="41" t="s">
         <v>161</v>
       </c>
-      <c r="B249" s="42" t="s">
+      <c r="B249" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="C249" s="42" t="s">
+      <c r="C249" s="43" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="A250" s="40" t="s">
+      <c r="A250" s="41" t="s">
         <v>722</v>
       </c>
-      <c r="B250" s="42" t="s">
+      <c r="B250" s="43" t="s">
         <v>723</v>
       </c>
-      <c r="C250" s="42" t="s">
+      <c r="C250" s="43" t="s">
         <v>723</v>
       </c>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="A251" s="40" t="s">
+      <c r="A251" s="41" t="s">
         <v>199</v>
       </c>
-      <c r="B251" s="42" t="s">
+      <c r="B251" s="43" t="s">
         <v>200</v>
       </c>
-      <c r="C251" s="42" t="s">
+      <c r="C251" s="43" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="A252" s="40" t="s">
+      <c r="A252" s="41" t="s">
         <v>724</v>
       </c>
-      <c r="B252" s="42" t="s">
+      <c r="B252" s="43" t="s">
         <v>725</v>
       </c>
-      <c r="C252" s="42" t="s">
+      <c r="C252" s="43" t="s">
         <v>725</v>
       </c>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="A253" s="40" t="s">
+      <c r="A253" s="41" t="s">
         <v>185</v>
       </c>
-      <c r="B253" s="40" t="s">
+      <c r="B253" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="C253" s="40" t="s">
+      <c r="C253" s="41" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="A254" s="40" t="s">
+      <c r="A254" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="B254" s="42" t="s">
+      <c r="B254" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="C254" s="42" t="s">
+      <c r="C254" s="43" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="A255" s="40" t="s">
+      <c r="A255" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="B255" s="40" t="s">
+      <c r="B255" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="C255" s="40" t="s">
+      <c r="C255" s="41" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="A256" s="40" t="s">
+      <c r="A256" s="41" t="s">
         <v>183</v>
       </c>
-      <c r="B256" s="40" t="s">
+      <c r="B256" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="C256" s="40" t="s">
+      <c r="C256" s="41" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="257" ht="15.75" customHeight="1"/>
     <row r="258" ht="15.75" customHeight="1"/>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="B259" s="44" t="s">
+      <c r="B259" s="45" t="s">
         <v>726</v>
       </c>
     </row>
@@ -29495,1223 +29519,1223 @@
     <row r="261" ht="15.75" customHeight="1"/>
     <row r="262" ht="15.75" customHeight="1"/>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="A263" s="40" t="s">
+      <c r="A263" s="41" t="s">
         <v>227</v>
       </c>
-      <c r="B263" s="40" t="s">
+      <c r="B263" s="41" t="s">
         <v>228</v>
       </c>
-      <c r="C263" s="40" t="s">
+      <c r="C263" s="41" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="A264" s="40" t="s">
+      <c r="A264" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="B264" s="40" t="s">
+      <c r="B264" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C264" s="40" t="s">
+      <c r="C264" s="41" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="A265" s="40" t="s">
+      <c r="A265" s="41" t="s">
         <v>727</v>
       </c>
-      <c r="B265" s="40" t="s">
+      <c r="B265" s="41" t="s">
         <v>728</v>
       </c>
-      <c r="C265" s="40" t="s">
+      <c r="C265" s="41" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="A266" s="40" t="s">
+      <c r="A266" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B266" s="40" t="s">
+      <c r="B266" s="41" t="s">
         <v>729</v>
       </c>
-      <c r="C266" s="40" t="s">
+      <c r="C266" s="41" t="s">
         <v>729</v>
       </c>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="A267" s="40" t="s">
+      <c r="A267" s="41" t="s">
         <v>730</v>
       </c>
-      <c r="B267" s="27" t="s">
+      <c r="B267" s="28" t="s">
         <v>731</v>
       </c>
-      <c r="C267" s="27" t="s">
+      <c r="C267" s="28" t="s">
         <v>731</v>
       </c>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="A268" s="40" t="s">
+      <c r="A268" s="41" t="s">
         <v>732</v>
       </c>
-      <c r="B268" s="45" t="s">
+      <c r="B268" s="46" t="s">
         <v>733</v>
       </c>
-      <c r="C268" s="45" t="s">
+      <c r="C268" s="46" t="s">
         <v>733</v>
       </c>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="A269" s="40" t="s">
+      <c r="A269" s="41" t="s">
         <v>734</v>
       </c>
-      <c r="B269" s="40" t="s">
+      <c r="B269" s="41" t="s">
         <v>735</v>
       </c>
-      <c r="C269" s="40" t="s">
+      <c r="C269" s="41" t="s">
         <v>735</v>
       </c>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="A270" s="40" t="s">
+      <c r="A270" s="41" t="s">
         <v>736</v>
       </c>
-      <c r="B270" s="27" t="s">
+      <c r="B270" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C270" s="27" t="s">
+      <c r="C270" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="A271" s="40" t="s">
+      <c r="A271" s="41" t="s">
         <v>738</v>
       </c>
-      <c r="B271" s="46">
+      <c r="B271" s="47">
         <v>120.0</v>
       </c>
-      <c r="C271" s="46">
+      <c r="C271" s="47">
         <v>120.0</v>
       </c>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="A272" s="40" t="s">
+      <c r="A272" s="41" t="s">
         <v>739</v>
       </c>
-      <c r="B272" s="27" t="s">
+      <c r="B272" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="C272" s="27" t="s">
+      <c r="C272" s="28" t="s">
         <v>740</v>
       </c>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="A273" s="40" t="s">
+      <c r="A273" s="41" t="s">
         <v>741</v>
       </c>
-      <c r="B273" s="27" t="s">
+      <c r="B273" s="28" t="s">
         <v>742</v>
       </c>
-      <c r="C273" s="27" t="s">
+      <c r="C273" s="28" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="A274" s="40" t="s">
+      <c r="A274" s="41" t="s">
         <v>743</v>
       </c>
-      <c r="B274" s="27" t="s">
+      <c r="B274" s="28" t="s">
         <v>744</v>
       </c>
-      <c r="C274" s="27" t="s">
+      <c r="C274" s="28" t="s">
         <v>744</v>
       </c>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="A275" s="40" t="s">
+      <c r="A275" s="41" t="s">
         <v>745</v>
       </c>
-      <c r="B275" s="27" t="s">
+      <c r="B275" s="28" t="s">
         <v>746</v>
       </c>
-      <c r="C275" s="27" t="s">
+      <c r="C275" s="28" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="A276" s="40" t="s">
+      <c r="A276" s="41" t="s">
         <v>747</v>
       </c>
-      <c r="B276" s="27" t="s">
+      <c r="B276" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C276" s="27" t="s">
+      <c r="C276" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="277" ht="15.75" customHeight="1">
-      <c r="A277" s="27" t="s">
+      <c r="A277" s="28" t="s">
         <v>748</v>
       </c>
-      <c r="B277" s="27" t="s">
+      <c r="B277" s="28" t="s">
         <v>749</v>
       </c>
-      <c r="C277" s="27" t="s">
+      <c r="C277" s="28" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="A278" s="27" t="s">
+      <c r="A278" s="28" t="s">
         <v>750</v>
       </c>
-      <c r="B278" s="46">
+      <c r="B278" s="47">
         <v>6.0</v>
       </c>
-      <c r="C278" s="46">
+      <c r="C278" s="47">
         <v>6.0</v>
       </c>
     </row>
     <row r="279" ht="15.75" customHeight="1">
-      <c r="A279" s="27" t="s">
+      <c r="A279" s="28" t="s">
         <v>751</v>
       </c>
-      <c r="B279" s="27" t="s">
+      <c r="B279" s="28" t="s">
         <v>752</v>
       </c>
-      <c r="C279" s="27" t="s">
+      <c r="C279" s="28" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="280" ht="15.75" customHeight="1">
-      <c r="A280" s="27" t="s">
+      <c r="A280" s="28" t="s">
         <v>753</v>
       </c>
-      <c r="B280" s="27" t="s">
+      <c r="B280" s="28" t="s">
         <v>754</v>
       </c>
-      <c r="C280" s="27" t="s">
+      <c r="C280" s="28" t="s">
         <v>754</v>
       </c>
     </row>
     <row r="281" ht="15.75" customHeight="1">
-      <c r="A281" s="27" t="s">
+      <c r="A281" s="28" t="s">
         <v>755</v>
       </c>
-      <c r="B281" s="27" t="s">
+      <c r="B281" s="28" t="s">
         <v>756</v>
       </c>
-      <c r="C281" s="27" t="s">
+      <c r="C281" s="28" t="s">
         <v>756</v>
       </c>
     </row>
     <row r="282" ht="15.75" customHeight="1">
-      <c r="A282" s="27" t="s">
+      <c r="A282" s="28" t="s">
         <v>757</v>
       </c>
-      <c r="B282" s="27" t="s">
+      <c r="B282" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C282" s="27" t="s">
+      <c r="C282" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="283" ht="15.75" customHeight="1">
-      <c r="A283" s="27" t="s">
+      <c r="A283" s="28" t="s">
         <v>758</v>
       </c>
-      <c r="B283" s="27" t="s">
+      <c r="B283" s="28" t="s">
         <v>759</v>
       </c>
-      <c r="C283" s="27" t="s">
+      <c r="C283" s="28" t="s">
         <v>759</v>
       </c>
     </row>
     <row r="284" ht="15.75" customHeight="1">
-      <c r="A284" s="27" t="s">
+      <c r="A284" s="28" t="s">
         <v>760</v>
       </c>
-      <c r="B284" s="47">
+      <c r="B284" s="48">
         <v>13.0</v>
       </c>
-      <c r="C284" s="47">
+      <c r="C284" s="48">
         <v>13.0</v>
       </c>
     </row>
     <row r="285" ht="15.75" customHeight="1">
-      <c r="A285" s="27" t="s">
+      <c r="A285" s="28" t="s">
         <v>761</v>
       </c>
-      <c r="B285" s="27" t="s">
+      <c r="B285" s="28" t="s">
         <v>762</v>
       </c>
-      <c r="C285" s="27" t="s">
+      <c r="C285" s="28" t="s">
         <v>762</v>
       </c>
     </row>
     <row r="286" ht="15.75" customHeight="1">
-      <c r="A286" s="27" t="s">
+      <c r="A286" s="28" t="s">
         <v>763</v>
       </c>
-      <c r="B286" s="27" t="s">
+      <c r="B286" s="28" t="s">
         <v>764</v>
       </c>
-      <c r="C286" s="27" t="s">
+      <c r="C286" s="28" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="287" ht="15.75" customHeight="1">
-      <c r="A287" s="27" t="s">
+      <c r="A287" s="28" t="s">
         <v>765</v>
       </c>
-      <c r="B287" s="27" t="s">
+      <c r="B287" s="28" t="s">
         <v>766</v>
       </c>
-      <c r="C287" s="27" t="s">
+      <c r="C287" s="28" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="A288" s="27" t="s">
+      <c r="A288" s="28" t="s">
         <v>767</v>
       </c>
-      <c r="B288" s="27" t="s">
+      <c r="B288" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C288" s="27" t="s">
+      <c r="C288" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="289" ht="15.75" customHeight="1">
-      <c r="A289" s="27" t="s">
+      <c r="A289" s="28" t="s">
         <v>768</v>
       </c>
-      <c r="B289" s="27" t="s">
+      <c r="B289" s="28" t="s">
         <v>769</v>
       </c>
-      <c r="C289" s="27" t="s">
+      <c r="C289" s="28" t="s">
         <v>769</v>
       </c>
     </row>
     <row r="290" ht="15.75" customHeight="1">
-      <c r="A290" s="27" t="s">
+      <c r="A290" s="28" t="s">
         <v>770</v>
       </c>
-      <c r="B290" s="46">
+      <c r="B290" s="47">
         <v>12.0</v>
       </c>
-      <c r="C290" s="46">
+      <c r="C290" s="47">
         <v>12.0</v>
       </c>
     </row>
     <row r="291" ht="15.75" customHeight="1">
-      <c r="A291" s="27" t="s">
+      <c r="A291" s="28" t="s">
         <v>771</v>
       </c>
-      <c r="B291" s="27" t="s">
+      <c r="B291" s="28" t="s">
         <v>772</v>
       </c>
-      <c r="C291" s="27" t="s">
+      <c r="C291" s="28" t="s">
         <v>772</v>
       </c>
     </row>
     <row r="292" ht="15.75" customHeight="1">
-      <c r="A292" s="27" t="s">
+      <c r="A292" s="28" t="s">
         <v>773</v>
       </c>
-      <c r="B292" s="27" t="s">
+      <c r="B292" s="28" t="s">
         <v>774</v>
       </c>
-      <c r="C292" s="27" t="s">
+      <c r="C292" s="28" t="s">
         <v>774</v>
       </c>
     </row>
     <row r="293" ht="15.75" customHeight="1">
-      <c r="A293" s="27" t="s">
+      <c r="A293" s="28" t="s">
         <v>775</v>
       </c>
-      <c r="B293" s="27" t="s">
+      <c r="B293" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C293" s="27" t="s">
+      <c r="C293" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="294" ht="15.75" customHeight="1">
-      <c r="A294" s="27" t="s">
+      <c r="A294" s="28" t="s">
         <v>776</v>
       </c>
-      <c r="B294" s="27" t="s">
+      <c r="B294" s="28" t="s">
         <v>777</v>
       </c>
-      <c r="C294" s="27" t="s">
+      <c r="C294" s="28" t="s">
         <v>777</v>
       </c>
     </row>
     <row r="295" ht="15.75" customHeight="1">
-      <c r="A295" s="27" t="s">
+      <c r="A295" s="28" t="s">
         <v>778</v>
       </c>
-      <c r="B295" s="46">
+      <c r="B295" s="47">
         <v>2.0</v>
       </c>
-      <c r="C295" s="46">
+      <c r="C295" s="47">
         <v>2.0</v>
       </c>
     </row>
     <row r="296" ht="15.75" customHeight="1">
-      <c r="A296" s="27" t="s">
+      <c r="A296" s="28" t="s">
         <v>779</v>
       </c>
-      <c r="B296" s="27" t="s">
+      <c r="B296" s="28" t="s">
         <v>780</v>
       </c>
-      <c r="C296" s="27" t="s">
+      <c r="C296" s="28" t="s">
         <v>780</v>
       </c>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="A297" s="27" t="s">
+      <c r="A297" s="28" t="s">
         <v>781</v>
       </c>
-      <c r="B297" s="27" t="s">
+      <c r="B297" s="28" t="s">
         <v>782</v>
       </c>
-      <c r="C297" s="27" t="s">
+      <c r="C297" s="28" t="s">
         <v>782</v>
       </c>
     </row>
     <row r="298" ht="15.75" customHeight="1">
-      <c r="A298" s="27" t="s">
+      <c r="A298" s="28" t="s">
         <v>783</v>
       </c>
-      <c r="B298" s="27" t="s">
+      <c r="B298" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C298" s="27" t="s">
+      <c r="C298" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="299" ht="15.75" customHeight="1">
-      <c r="A299" s="27" t="s">
+      <c r="A299" s="28" t="s">
         <v>784</v>
       </c>
-      <c r="B299" s="46">
+      <c r="B299" s="47">
         <v>7.0</v>
       </c>
-      <c r="C299" s="46">
+      <c r="C299" s="47">
         <v>7.0</v>
       </c>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="A300" s="27" t="s">
+      <c r="A300" s="28" t="s">
         <v>785</v>
       </c>
-      <c r="B300" s="46">
+      <c r="B300" s="47">
         <v>8.0</v>
       </c>
-      <c r="C300" s="46">
+      <c r="C300" s="47">
         <v>8.0</v>
       </c>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="A301" s="27" t="s">
+      <c r="A301" s="28" t="s">
         <v>786</v>
       </c>
-      <c r="B301" s="27" t="s">
+      <c r="B301" s="28" t="s">
         <v>787</v>
       </c>
-      <c r="C301" s="27" t="s">
+      <c r="C301" s="28" t="s">
         <v>787</v>
       </c>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="A302" s="27" t="s">
+      <c r="A302" s="28" t="s">
         <v>788</v>
       </c>
-      <c r="B302" s="27" t="s">
+      <c r="B302" s="28" t="s">
         <v>789</v>
       </c>
-      <c r="C302" s="27" t="s">
+      <c r="C302" s="28" t="s">
         <v>789</v>
       </c>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="A303" s="27" t="s">
+      <c r="A303" s="28" t="s">
         <v>790</v>
       </c>
-      <c r="B303" s="27" t="s">
+      <c r="B303" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C303" s="27" t="s">
+      <c r="C303" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="A304" s="27" t="s">
+      <c r="A304" s="28" t="s">
         <v>791</v>
       </c>
-      <c r="B304" s="27" t="s">
+      <c r="B304" s="28" t="s">
         <v>792</v>
       </c>
-      <c r="C304" s="45" t="s">
+      <c r="C304" s="46" t="s">
         <v>792</v>
       </c>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="A305" s="27" t="s">
+      <c r="A305" s="28" t="s">
         <v>793</v>
       </c>
-      <c r="B305" s="46">
+      <c r="B305" s="47">
         <v>6.0</v>
       </c>
-      <c r="C305" s="46">
+      <c r="C305" s="47">
         <v>6.0</v>
       </c>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="A306" s="27" t="s">
+      <c r="A306" s="28" t="s">
         <v>794</v>
       </c>
-      <c r="B306" s="27" t="s">
+      <c r="B306" s="28" t="s">
         <v>795</v>
       </c>
-      <c r="C306" s="27" t="s">
+      <c r="C306" s="28" t="s">
         <v>795</v>
       </c>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="A307" s="27" t="s">
+      <c r="A307" s="28" t="s">
         <v>796</v>
       </c>
-      <c r="B307" s="27" t="s">
+      <c r="B307" s="28" t="s">
         <v>797</v>
       </c>
-      <c r="C307" s="27" t="s">
+      <c r="C307" s="28" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="A308" s="27" t="s">
+      <c r="A308" s="28" t="s">
         <v>798</v>
       </c>
-      <c r="B308" s="27" t="s">
+      <c r="B308" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C308" s="27" t="s">
+      <c r="C308" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="A309" s="27" t="s">
+      <c r="A309" s="28" t="s">
         <v>799</v>
       </c>
-      <c r="B309" s="46">
+      <c r="B309" s="47">
         <v>9.0</v>
       </c>
-      <c r="C309" s="46">
+      <c r="C309" s="47">
         <v>9.0</v>
       </c>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="A310" s="27" t="s">
+      <c r="A310" s="28" t="s">
         <v>800</v>
       </c>
-      <c r="B310" s="46">
+      <c r="B310" s="47">
         <v>10.0</v>
       </c>
-      <c r="C310" s="46">
+      <c r="C310" s="47">
         <v>10.0</v>
       </c>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="A311" s="27" t="s">
+      <c r="A311" s="28" t="s">
         <v>801</v>
       </c>
-      <c r="B311" s="27" t="s">
+      <c r="B311" s="28" t="s">
         <v>802</v>
       </c>
-      <c r="C311" s="27" t="s">
+      <c r="C311" s="28" t="s">
         <v>802</v>
       </c>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="A312" s="27" t="s">
+      <c r="A312" s="28" t="s">
         <v>803</v>
       </c>
-      <c r="B312" s="27" t="s">
+      <c r="B312" s="28" t="s">
         <v>802</v>
       </c>
-      <c r="C312" s="27" t="s">
+      <c r="C312" s="28" t="s">
         <v>802</v>
       </c>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="A313" s="27" t="s">
+      <c r="A313" s="28" t="s">
         <v>804</v>
       </c>
-      <c r="B313" s="27" t="s">
+      <c r="B313" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C313" s="27" t="s">
+      <c r="C313" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="A314" s="27" t="s">
+      <c r="A314" s="28" t="s">
         <v>805</v>
       </c>
-      <c r="B314" s="46">
+      <c r="B314" s="47">
         <v>12.0</v>
       </c>
-      <c r="C314" s="46">
+      <c r="C314" s="47">
         <v>12.0</v>
       </c>
     </row>
     <row r="315" ht="15.75" customHeight="1">
-      <c r="A315" s="27" t="s">
+      <c r="A315" s="28" t="s">
         <v>806</v>
       </c>
-      <c r="B315" s="46">
+      <c r="B315" s="47">
         <v>13.0</v>
       </c>
-      <c r="C315" s="46">
+      <c r="C315" s="47">
         <v>13.0</v>
       </c>
     </row>
     <row r="316" ht="15.75" customHeight="1">
-      <c r="A316" s="27" t="s">
+      <c r="A316" s="28" t="s">
         <v>807</v>
       </c>
-      <c r="B316" s="27" t="s">
+      <c r="B316" s="28" t="s">
         <v>808</v>
       </c>
-      <c r="C316" s="27" t="s">
+      <c r="C316" s="28" t="s">
         <v>808</v>
       </c>
     </row>
     <row r="317" ht="15.75" customHeight="1">
-      <c r="A317" s="27" t="s">
+      <c r="A317" s="28" t="s">
         <v>809</v>
       </c>
-      <c r="B317" s="27" t="s">
+      <c r="B317" s="28" t="s">
         <v>810</v>
       </c>
-      <c r="C317" s="27" t="s">
+      <c r="C317" s="28" t="s">
         <v>810</v>
       </c>
     </row>
     <row r="318" ht="15.75" customHeight="1">
-      <c r="A318" s="27" t="s">
+      <c r="A318" s="28" t="s">
         <v>811</v>
       </c>
-      <c r="B318" s="27" t="s">
+      <c r="B318" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C318" s="27" t="s">
+      <c r="C318" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="319" ht="15.75" customHeight="1">
-      <c r="A319" s="27" t="s">
+      <c r="A319" s="28" t="s">
         <v>812</v>
       </c>
-      <c r="B319" s="27" t="s">
+      <c r="B319" s="28" t="s">
         <v>749</v>
       </c>
-      <c r="C319" s="27" t="s">
+      <c r="C319" s="28" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="320" ht="15.75" customHeight="1">
-      <c r="A320" s="27" t="s">
+      <c r="A320" s="28" t="s">
         <v>813</v>
       </c>
-      <c r="B320" s="46">
+      <c r="B320" s="47">
         <v>6.0</v>
       </c>
-      <c r="C320" s="46">
+      <c r="C320" s="47">
         <v>6.0</v>
       </c>
     </row>
     <row r="321" ht="15.75" customHeight="1">
-      <c r="A321" s="27" t="s">
+      <c r="A321" s="28" t="s">
         <v>814</v>
       </c>
-      <c r="B321" s="27" t="s">
+      <c r="B321" s="28" t="s">
         <v>815</v>
       </c>
-      <c r="C321" s="27" t="s">
+      <c r="C321" s="28" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="322" ht="15.75" customHeight="1">
-      <c r="A322" s="27" t="s">
+      <c r="A322" s="28" t="s">
         <v>816</v>
       </c>
-      <c r="B322" s="27" t="s">
+      <c r="B322" s="28" t="s">
         <v>817</v>
       </c>
-      <c r="C322" s="27" t="s">
+      <c r="C322" s="28" t="s">
         <v>817</v>
       </c>
     </row>
     <row r="323" ht="15.75" customHeight="1">
-      <c r="A323" s="27" t="s">
+      <c r="A323" s="28" t="s">
         <v>818</v>
       </c>
-      <c r="B323" s="27" t="s">
+      <c r="B323" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C323" s="27" t="s">
+      <c r="C323" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="324" ht="15.75" customHeight="1">
-      <c r="A324" s="27" t="s">
+      <c r="A324" s="28" t="s">
         <v>819</v>
       </c>
-      <c r="B324" s="27" t="s">
+      <c r="B324" s="28" t="s">
         <v>820</v>
       </c>
-      <c r="C324" s="27" t="s">
+      <c r="C324" s="28" t="s">
         <v>820</v>
       </c>
     </row>
     <row r="325" ht="15.75" customHeight="1">
-      <c r="A325" s="27" t="s">
+      <c r="A325" s="28" t="s">
         <v>821</v>
       </c>
-      <c r="B325" s="46">
+      <c r="B325" s="47">
         <v>7.0</v>
       </c>
-      <c r="C325" s="46">
+      <c r="C325" s="47">
         <v>7.0</v>
       </c>
     </row>
     <row r="326" ht="15.75" customHeight="1">
-      <c r="A326" s="27" t="s">
+      <c r="A326" s="28" t="s">
         <v>822</v>
       </c>
-      <c r="B326" s="27" t="s">
+      <c r="B326" s="28" t="s">
         <v>823</v>
       </c>
-      <c r="C326" s="27" t="s">
+      <c r="C326" s="28" t="s">
         <v>823</v>
       </c>
     </row>
     <row r="327" ht="15.75" customHeight="1">
-      <c r="A327" s="27" t="s">
+      <c r="A327" s="28" t="s">
         <v>824</v>
       </c>
-      <c r="B327" s="27" t="s">
+      <c r="B327" s="28" t="s">
         <v>825</v>
       </c>
-      <c r="C327" s="27" t="s">
+      <c r="C327" s="28" t="s">
         <v>825</v>
       </c>
     </row>
     <row r="328" ht="15.75" customHeight="1">
-      <c r="A328" s="27" t="s">
+      <c r="A328" s="28" t="s">
         <v>826</v>
       </c>
-      <c r="B328" s="27" t="s">
+      <c r="B328" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C328" s="27" t="s">
+      <c r="C328" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="329" ht="15.75" customHeight="1">
-      <c r="A329" s="27" t="s">
+      <c r="A329" s="28" t="s">
         <v>827</v>
       </c>
-      <c r="B329" s="27" t="s">
+      <c r="B329" s="28" t="s">
         <v>828</v>
       </c>
-      <c r="C329" s="27" t="s">
+      <c r="C329" s="28" t="s">
         <v>828</v>
       </c>
     </row>
     <row r="330" ht="15.75" customHeight="1">
-      <c r="A330" s="27" t="s">
+      <c r="A330" s="28" t="s">
         <v>829</v>
       </c>
-      <c r="B330" s="46">
+      <c r="B330" s="47">
         <v>3.0</v>
       </c>
-      <c r="C330" s="46">
+      <c r="C330" s="47">
         <v>3.0</v>
       </c>
     </row>
     <row r="331" ht="15.75" customHeight="1">
-      <c r="A331" s="27" t="s">
+      <c r="A331" s="28" t="s">
         <v>830</v>
       </c>
-      <c r="B331" s="27" t="s">
+      <c r="B331" s="28" t="s">
         <v>831</v>
       </c>
-      <c r="C331" s="27" t="s">
+      <c r="C331" s="28" t="s">
         <v>831</v>
       </c>
     </row>
     <row r="332" ht="15.75" customHeight="1">
-      <c r="A332" s="27" t="s">
+      <c r="A332" s="28" t="s">
         <v>832</v>
       </c>
-      <c r="B332" s="27" t="s">
+      <c r="B332" s="28" t="s">
         <v>833</v>
       </c>
-      <c r="C332" s="27" t="s">
+      <c r="C332" s="28" t="s">
         <v>833</v>
       </c>
     </row>
     <row r="333" ht="15.75" customHeight="1">
-      <c r="A333" s="27" t="s">
+      <c r="A333" s="28" t="s">
         <v>834</v>
       </c>
-      <c r="B333" s="27" t="s">
+      <c r="B333" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C333" s="27" t="s">
+      <c r="C333" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="334" ht="15.75" customHeight="1">
-      <c r="A334" s="27" t="s">
+      <c r="A334" s="28" t="s">
         <v>835</v>
       </c>
-      <c r="B334" s="27" t="s">
+      <c r="B334" s="28" t="s">
         <v>836</v>
       </c>
-      <c r="C334" s="27" t="s">
+      <c r="C334" s="28" t="s">
         <v>836</v>
       </c>
     </row>
     <row r="335" ht="15.75" customHeight="1">
-      <c r="A335" s="27" t="s">
+      <c r="A335" s="28" t="s">
         <v>837</v>
       </c>
-      <c r="B335" s="46">
+      <c r="B335" s="47">
         <v>3.0</v>
       </c>
-      <c r="C335" s="46">
+      <c r="C335" s="47">
         <v>3.0</v>
       </c>
     </row>
     <row r="336" ht="15.75" customHeight="1">
-      <c r="A336" s="27" t="s">
+      <c r="A336" s="28" t="s">
         <v>838</v>
       </c>
-      <c r="B336" s="27" t="s">
+      <c r="B336" s="28" t="s">
         <v>839</v>
       </c>
-      <c r="C336" s="27" t="s">
+      <c r="C336" s="28" t="s">
         <v>839</v>
       </c>
     </row>
     <row r="337" ht="15.75" customHeight="1">
-      <c r="A337" s="27" t="s">
+      <c r="A337" s="28" t="s">
         <v>840</v>
       </c>
-      <c r="B337" s="27" t="s">
+      <c r="B337" s="28" t="s">
         <v>841</v>
       </c>
-      <c r="C337" s="27" t="s">
+      <c r="C337" s="28" t="s">
         <v>841</v>
       </c>
     </row>
     <row r="338" ht="15.75" customHeight="1">
-      <c r="A338" s="27" t="s">
+      <c r="A338" s="28" t="s">
         <v>842</v>
       </c>
-      <c r="B338" s="27" t="s">
+      <c r="B338" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C338" s="27" t="s">
+      <c r="C338" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="339" ht="15.75" customHeight="1">
-      <c r="A339" s="27" t="s">
+      <c r="A339" s="28" t="s">
         <v>843</v>
       </c>
-      <c r="B339" s="27" t="s">
+      <c r="B339" s="28" t="s">
         <v>844</v>
       </c>
-      <c r="C339" s="27" t="s">
+      <c r="C339" s="28" t="s">
         <v>844</v>
       </c>
     </row>
     <row r="340" ht="15.75" customHeight="1">
-      <c r="A340" s="27" t="s">
+      <c r="A340" s="28" t="s">
         <v>845</v>
       </c>
-      <c r="B340" s="46">
+      <c r="B340" s="47">
         <v>3.0</v>
       </c>
-      <c r="C340" s="46">
+      <c r="C340" s="47">
         <v>3.0</v>
       </c>
     </row>
     <row r="341" ht="15.75" customHeight="1">
-      <c r="A341" s="27" t="s">
+      <c r="A341" s="28" t="s">
         <v>846</v>
       </c>
-      <c r="B341" s="27" t="s">
+      <c r="B341" s="28" t="s">
         <v>847</v>
       </c>
-      <c r="C341" s="27" t="s">
+      <c r="C341" s="28" t="s">
         <v>847</v>
       </c>
     </row>
     <row r="342" ht="15.75" customHeight="1">
-      <c r="A342" s="27" t="s">
+      <c r="A342" s="28" t="s">
         <v>848</v>
       </c>
-      <c r="B342" s="27" t="s">
+      <c r="B342" s="28" t="s">
         <v>849</v>
       </c>
-      <c r="C342" s="27" t="s">
+      <c r="C342" s="28" t="s">
         <v>849</v>
       </c>
     </row>
     <row r="343" ht="15.75" customHeight="1">
-      <c r="A343" s="27" t="s">
+      <c r="A343" s="28" t="s">
         <v>850</v>
       </c>
-      <c r="B343" s="27" t="s">
+      <c r="B343" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C343" s="27" t="s">
+      <c r="C343" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="344" ht="15.75" customHeight="1">
-      <c r="A344" s="27" t="s">
+      <c r="A344" s="28" t="s">
         <v>851</v>
       </c>
-      <c r="B344" s="45" t="s">
+      <c r="B344" s="46" t="s">
         <v>852</v>
       </c>
-      <c r="C344" s="45" t="s">
+      <c r="C344" s="46" t="s">
         <v>852</v>
       </c>
     </row>
     <row r="345" ht="15.75" customHeight="1">
-      <c r="A345" s="27" t="s">
+      <c r="A345" s="28" t="s">
         <v>853</v>
       </c>
-      <c r="B345" s="46">
+      <c r="B345" s="47">
         <v>3.0</v>
       </c>
-      <c r="C345" s="46">
+      <c r="C345" s="47">
         <v>3.0</v>
       </c>
     </row>
     <row r="346" ht="15.75" customHeight="1">
-      <c r="A346" s="27" t="s">
+      <c r="A346" s="28" t="s">
         <v>854</v>
       </c>
-      <c r="B346" s="27" t="s">
+      <c r="B346" s="28" t="s">
         <v>855</v>
       </c>
-      <c r="C346" s="27" t="s">
+      <c r="C346" s="28" t="s">
         <v>855</v>
       </c>
     </row>
     <row r="347" ht="15.75" customHeight="1">
-      <c r="A347" s="27" t="s">
+      <c r="A347" s="28" t="s">
         <v>856</v>
       </c>
-      <c r="B347" s="27" t="s">
+      <c r="B347" s="28" t="s">
         <v>857</v>
       </c>
-      <c r="C347" s="27" t="s">
+      <c r="C347" s="28" t="s">
         <v>857</v>
       </c>
     </row>
     <row r="348" ht="15.75" customHeight="1">
-      <c r="A348" s="27" t="s">
+      <c r="A348" s="28" t="s">
         <v>858</v>
       </c>
-      <c r="B348" s="27" t="s">
+      <c r="B348" s="28" t="s">
         <v>859</v>
       </c>
-      <c r="C348" s="27" t="s">
+      <c r="C348" s="28" t="s">
         <v>859</v>
       </c>
     </row>
     <row r="349" ht="15.75" customHeight="1">
-      <c r="A349" s="27" t="s">
+      <c r="A349" s="28" t="s">
         <v>860</v>
       </c>
-      <c r="B349" s="27" t="s">
+      <c r="B349" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C349" s="27" t="s">
+      <c r="C349" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="350" ht="15.75" customHeight="1">
-      <c r="A350" s="27" t="s">
+      <c r="A350" s="28" t="s">
         <v>861</v>
       </c>
-      <c r="B350" s="46" t="s">
+      <c r="B350" s="47" t="s">
         <v>862</v>
       </c>
-      <c r="C350" s="46" t="s">
+      <c r="C350" s="47" t="s">
         <v>862</v>
       </c>
     </row>
     <row r="351" ht="15.75" customHeight="1">
-      <c r="A351" s="27" t="s">
+      <c r="A351" s="28" t="s">
         <v>863</v>
       </c>
-      <c r="B351" s="46">
+      <c r="B351" s="47">
         <v>6.0</v>
       </c>
-      <c r="C351" s="46">
+      <c r="C351" s="47">
         <v>6.0</v>
       </c>
     </row>
     <row r="352" ht="15.75" customHeight="1">
-      <c r="A352" s="27" t="s">
+      <c r="A352" s="28" t="s">
         <v>864</v>
       </c>
-      <c r="B352" s="27" t="s">
+      <c r="B352" s="28" t="s">
         <v>865</v>
       </c>
-      <c r="C352" s="27" t="s">
+      <c r="C352" s="28" t="s">
         <v>865</v>
       </c>
     </row>
     <row r="353" ht="15.75" customHeight="1">
-      <c r="A353" s="27" t="s">
+      <c r="A353" s="28" t="s">
         <v>866</v>
       </c>
-      <c r="B353" s="27" t="s">
+      <c r="B353" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C353" s="27" t="s">
+      <c r="C353" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="354" ht="15.75" customHeight="1">
-      <c r="A354" s="27" t="s">
+      <c r="A354" s="28" t="s">
         <v>867</v>
       </c>
-      <c r="B354" s="27" t="s">
+      <c r="B354" s="28" t="s">
         <v>868</v>
       </c>
-      <c r="C354" s="27" t="s">
+      <c r="C354" s="28" t="s">
         <v>868</v>
       </c>
     </row>
     <row r="355" ht="15.75" customHeight="1">
-      <c r="A355" s="27" t="s">
+      <c r="A355" s="28" t="s">
         <v>869</v>
       </c>
-      <c r="B355" s="46">
+      <c r="B355" s="47">
         <v>50.0</v>
       </c>
-      <c r="C355" s="46">
+      <c r="C355" s="47">
         <v>50.0</v>
       </c>
     </row>
     <row r="356" ht="15.75" customHeight="1">
-      <c r="A356" s="27" t="s">
+      <c r="A356" s="28" t="s">
         <v>870</v>
       </c>
-      <c r="B356" s="46">
+      <c r="B356" s="47">
         <v>55.0</v>
       </c>
-      <c r="C356" s="46">
+      <c r="C356" s="47">
         <v>55.0</v>
       </c>
     </row>
     <row r="357" ht="15.75" customHeight="1">
-      <c r="A357" s="27" t="s">
+      <c r="A357" s="28" t="s">
         <v>871</v>
       </c>
-      <c r="B357" s="27" t="s">
+      <c r="B357" s="28" t="s">
         <v>872</v>
       </c>
-      <c r="C357" s="27" t="s">
+      <c r="C357" s="28" t="s">
         <v>872</v>
       </c>
     </row>
     <row r="358" ht="15.75" customHeight="1">
-      <c r="A358" s="27" t="s">
+      <c r="A358" s="28" t="s">
         <v>873</v>
       </c>
-      <c r="B358" s="27" t="s">
+      <c r="B358" s="28" t="s">
         <v>782</v>
       </c>
-      <c r="C358" s="27" t="s">
+      <c r="C358" s="28" t="s">
         <v>782</v>
       </c>
     </row>
     <row r="359" ht="15.75" customHeight="1">
-      <c r="A359" s="27" t="s">
+      <c r="A359" s="28" t="s">
         <v>874</v>
       </c>
-      <c r="B359" s="27" t="s">
+      <c r="B359" s="28" t="s">
         <v>875</v>
       </c>
-      <c r="C359" s="27" t="s">
+      <c r="C359" s="28" t="s">
         <v>875</v>
       </c>
     </row>
     <row r="360" ht="15.75" customHeight="1">
-      <c r="A360" s="27" t="s">
+      <c r="A360" s="28" t="s">
         <v>876</v>
       </c>
-      <c r="B360" s="27" t="s">
+      <c r="B360" s="28" t="s">
         <v>877</v>
       </c>
-      <c r="C360" s="27" t="s">
+      <c r="C360" s="28" t="s">
         <v>877</v>
       </c>
     </row>
     <row r="361" ht="15.75" customHeight="1">
-      <c r="A361" s="27" t="s">
+      <c r="A361" s="28" t="s">
         <v>878</v>
       </c>
-      <c r="B361" s="27" t="s">
+      <c r="B361" s="28" t="s">
         <v>797</v>
       </c>
-      <c r="C361" s="27" t="s">
+      <c r="C361" s="28" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="362" ht="15.75" customHeight="1">
-      <c r="A362" s="27" t="s">
+      <c r="A362" s="28" t="s">
         <v>879</v>
       </c>
-      <c r="B362" s="27" t="s">
+      <c r="B362" s="28" t="s">
         <v>802</v>
       </c>
-      <c r="C362" s="27" t="s">
+      <c r="C362" s="28" t="s">
         <v>802</v>
       </c>
     </row>
     <row r="363" ht="15.75" customHeight="1">
-      <c r="A363" s="27" t="s">
+      <c r="A363" s="28" t="s">
         <v>880</v>
       </c>
-      <c r="B363" s="27" t="s">
+      <c r="B363" s="28" t="s">
         <v>881</v>
       </c>
-      <c r="C363" s="27" t="s">
+      <c r="C363" s="28" t="s">
         <v>881</v>
       </c>
     </row>
     <row r="364" ht="15.75" customHeight="1">
-      <c r="A364" s="27" t="s">
+      <c r="A364" s="28" t="s">
         <v>882</v>
       </c>
-      <c r="B364" s="27" t="s">
+      <c r="B364" s="28" t="s">
         <v>883</v>
       </c>
-      <c r="C364" s="27" t="s">
+      <c r="C364" s="28" t="s">
         <v>883</v>
       </c>
     </row>
     <row r="365" ht="15.75" customHeight="1">
-      <c r="A365" s="27" t="s">
+      <c r="A365" s="28" t="s">
         <v>884</v>
       </c>
-      <c r="B365" s="27" t="s">
+      <c r="B365" s="28" t="s">
         <v>885</v>
       </c>
-      <c r="C365" s="27" t="s">
+      <c r="C365" s="28" t="s">
         <v>885</v>
       </c>
     </row>
     <row r="366" ht="15.75" customHeight="1">
-      <c r="A366" s="27" t="s">
+      <c r="A366" s="28" t="s">
         <v>886</v>
       </c>
-      <c r="B366" s="27" t="s">
+      <c r="B366" s="28" t="s">
         <v>887</v>
       </c>
-      <c r="C366" s="27" t="s">
+      <c r="C366" s="28" t="s">
         <v>887</v>
       </c>
     </row>
     <row r="367" ht="15.75" customHeight="1">
-      <c r="A367" s="27" t="s">
+      <c r="A367" s="28" t="s">
         <v>888</v>
       </c>
-      <c r="B367" s="27" t="s">
+      <c r="B367" s="28" t="s">
         <v>889</v>
       </c>
-      <c r="C367" s="27" t="s">
+      <c r="C367" s="28" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="368" ht="15.75" customHeight="1">
-      <c r="A368" s="27" t="s">
+      <c r="A368" s="28" t="s">
         <v>890</v>
       </c>
-      <c r="B368" s="27" t="s">
+      <c r="B368" s="28" t="s">
         <v>891</v>
       </c>
-      <c r="C368" s="27" t="s">
+      <c r="C368" s="28" t="s">
         <v>891</v>
       </c>
     </row>
     <row r="369" ht="15.75" customHeight="1">
-      <c r="A369" s="27" t="s">
+      <c r="A369" s="28" t="s">
         <v>892</v>
       </c>
-      <c r="B369" s="27" t="s">
+      <c r="B369" s="28" t="s">
         <v>893</v>
       </c>
-      <c r="C369" s="27" t="s">
+      <c r="C369" s="28" t="s">
         <v>893</v>
       </c>
     </row>
     <row r="370" ht="15.75" customHeight="1">
-      <c r="A370" s="27" t="s">
+      <c r="A370" s="28" t="s">
         <v>894</v>
       </c>
-      <c r="B370" s="27" t="s">
+      <c r="B370" s="28" t="s">
         <v>895</v>
       </c>
-      <c r="C370" s="27" t="s">
+      <c r="C370" s="28" t="s">
         <v>895</v>
       </c>
     </row>
     <row r="371" ht="15.75" customHeight="1">
-      <c r="A371" s="27" t="s">
+      <c r="A371" s="28" t="s">
         <v>896</v>
       </c>
-      <c r="B371" s="27" t="s">
+      <c r="B371" s="28" t="s">
         <v>897</v>
       </c>
-      <c r="C371" s="27" t="s">
+      <c r="C371" s="28" t="s">
         <v>897</v>
       </c>
     </row>
     <row r="372" ht="15.75" customHeight="1">
-      <c r="A372" s="27" t="s">
+      <c r="A372" s="28" t="s">
         <v>898</v>
       </c>
-      <c r="B372" s="27" t="s">
+      <c r="B372" s="28" t="s">
         <v>899</v>
       </c>
-      <c r="C372" s="27" t="s">
+      <c r="C372" s="28" t="s">
         <v>899</v>
       </c>
     </row>
     <row r="373" ht="15.75" customHeight="1">
-      <c r="A373" s="27" t="s">
+      <c r="A373" s="28" t="s">
         <v>900</v>
       </c>
-      <c r="B373" s="27" t="s">
+      <c r="B373" s="28" t="s">
         <v>901</v>
       </c>
-      <c r="C373" s="27" t="s">
+      <c r="C373" s="28" t="s">
         <v>901</v>
       </c>
     </row>
@@ -30721,7 +30745,7 @@
     <row r="377" ht="15.75" customHeight="1"/>
     <row r="378" ht="15.75" customHeight="1"/>
     <row r="379" ht="15.75" customHeight="1">
-      <c r="B379" s="39" t="s">
+      <c r="B379" s="40" t="s">
         <v>902</v>
       </c>
     </row>
@@ -30729,439 +30753,439 @@
     <row r="381" ht="15.75" customHeight="1"/>
     <row r="382" ht="15.75" customHeight="1"/>
     <row r="383" ht="15.75" customHeight="1">
-      <c r="A383" s="27" t="s">
+      <c r="A383" s="28" t="s">
         <v>903</v>
       </c>
-      <c r="B383" s="27" t="s">
+      <c r="B383" s="28" t="s">
         <v>904</v>
       </c>
-      <c r="C383" s="27" t="s">
+      <c r="C383" s="28" t="s">
         <v>904</v>
       </c>
     </row>
     <row r="384" ht="15.75" customHeight="1">
-      <c r="A384" s="27" t="s">
+      <c r="A384" s="28" t="s">
         <v>905</v>
       </c>
-      <c r="B384" s="27" t="s">
+      <c r="B384" s="28" t="s">
         <v>906</v>
       </c>
-      <c r="C384" s="27" t="s">
+      <c r="C384" s="28" t="s">
         <v>906</v>
       </c>
     </row>
     <row r="385" ht="15.75" customHeight="1">
-      <c r="A385" s="27" t="s">
+      <c r="A385" s="28" t="s">
         <v>907</v>
       </c>
-      <c r="B385" s="27" t="s">
+      <c r="B385" s="28" t="s">
         <v>908</v>
       </c>
-      <c r="C385" s="27" t="s">
+      <c r="C385" s="28" t="s">
         <v>908</v>
       </c>
     </row>
     <row r="386" ht="15.75" customHeight="1">
-      <c r="A386" s="27" t="s">
+      <c r="A386" s="28" t="s">
         <v>909</v>
       </c>
-      <c r="B386" s="27" t="s">
+      <c r="B386" s="28" t="s">
         <v>910</v>
       </c>
-      <c r="C386" s="27" t="s">
+      <c r="C386" s="28" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="387" ht="15.75" customHeight="1">
-      <c r="A387" s="27" t="s">
+      <c r="A387" s="28" t="s">
         <v>911</v>
       </c>
-      <c r="B387" s="27" t="s">
+      <c r="B387" s="28" t="s">
         <v>910</v>
       </c>
-      <c r="C387" s="27" t="s">
+      <c r="C387" s="28" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="388" ht="15.75" customHeight="1">
-      <c r="A388" s="27" t="s">
+      <c r="A388" s="28" t="s">
         <v>912</v>
       </c>
-      <c r="B388" s="27" t="s">
+      <c r="B388" s="28" t="s">
         <v>913</v>
       </c>
-      <c r="C388" s="27" t="s">
+      <c r="C388" s="28" t="s">
         <v>913</v>
       </c>
     </row>
     <row r="389" ht="15.75" customHeight="1"/>
     <row r="390" ht="15.75" customHeight="1">
-      <c r="B390" s="39" t="s">
+      <c r="B390" s="40" t="s">
         <v>914</v>
       </c>
     </row>
     <row r="391" ht="15.75" customHeight="1"/>
     <row r="392" ht="15.75" customHeight="1"/>
     <row r="393" ht="15.75" customHeight="1">
-      <c r="A393" s="27" t="s">
+      <c r="A393" s="28" t="s">
         <v>915</v>
       </c>
-      <c r="B393" s="27" t="s">
+      <c r="B393" s="28" t="s">
         <v>916</v>
       </c>
-      <c r="C393" s="27" t="s">
+      <c r="C393" s="28" t="s">
         <v>916</v>
       </c>
     </row>
     <row r="394" ht="15.75" customHeight="1">
-      <c r="A394" s="27" t="s">
+      <c r="A394" s="28" t="s">
         <v>917</v>
       </c>
-      <c r="B394" s="27" t="s">
+      <c r="B394" s="28" t="s">
         <v>918</v>
       </c>
-      <c r="C394" s="27" t="s">
+      <c r="C394" s="28" t="s">
         <v>918</v>
       </c>
     </row>
     <row r="395" ht="15.75" customHeight="1">
-      <c r="A395" s="27" t="s">
+      <c r="A395" s="28" t="s">
         <v>919</v>
       </c>
-      <c r="B395" s="27" t="s">
+      <c r="B395" s="28" t="s">
         <v>920</v>
       </c>
-      <c r="C395" s="27" t="s">
+      <c r="C395" s="28" t="s">
         <v>920</v>
       </c>
     </row>
     <row r="396" ht="15.75" customHeight="1">
-      <c r="A396" s="27" t="s">
+      <c r="A396" s="28" t="s">
         <v>921</v>
       </c>
-      <c r="B396" s="27" t="s">
+      <c r="B396" s="28" t="s">
         <v>922</v>
       </c>
-      <c r="C396" s="27" t="s">
+      <c r="C396" s="28" t="s">
         <v>922</v>
       </c>
     </row>
     <row r="397" ht="15.75" customHeight="1">
-      <c r="A397" s="27" t="s">
+      <c r="A397" s="28" t="s">
         <v>923</v>
       </c>
-      <c r="B397" s="27" t="s">
+      <c r="B397" s="28" t="s">
         <v>924</v>
       </c>
-      <c r="C397" s="27" t="s">
+      <c r="C397" s="28" t="s">
         <v>924</v>
       </c>
     </row>
     <row r="398" ht="15.75" customHeight="1">
-      <c r="A398" s="27" t="s">
+      <c r="A398" s="28" t="s">
         <v>925</v>
       </c>
-      <c r="B398" s="27" t="s">
+      <c r="B398" s="28" t="s">
         <v>926</v>
       </c>
-      <c r="C398" s="27" t="s">
+      <c r="C398" s="28" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="399" ht="15.75" customHeight="1">
-      <c r="A399" s="27" t="s">
+      <c r="A399" s="28" t="s">
         <v>927</v>
       </c>
-      <c r="B399" s="27" t="s">
+      <c r="B399" s="28" t="s">
         <v>928</v>
       </c>
-      <c r="C399" s="27" t="s">
+      <c r="C399" s="28" t="s">
         <v>928</v>
       </c>
     </row>
     <row r="400" ht="15.75" customHeight="1">
-      <c r="A400" s="27" t="s">
+      <c r="A400" s="28" t="s">
         <v>929</v>
       </c>
-      <c r="B400" s="27" t="s">
+      <c r="B400" s="28" t="s">
         <v>930</v>
       </c>
-      <c r="C400" s="27" t="s">
+      <c r="C400" s="28" t="s">
         <v>930</v>
       </c>
     </row>
     <row r="401" ht="15.75" customHeight="1">
-      <c r="A401" s="27" t="s">
+      <c r="A401" s="28" t="s">
         <v>931</v>
       </c>
-      <c r="B401" s="27" t="s">
+      <c r="B401" s="28" t="s">
         <v>932</v>
       </c>
-      <c r="C401" s="27" t="s">
+      <c r="C401" s="28" t="s">
         <v>932</v>
       </c>
     </row>
     <row r="402" ht="15.75" customHeight="1">
-      <c r="A402" s="27" t="s">
+      <c r="A402" s="28" t="s">
         <v>933</v>
       </c>
-      <c r="B402" s="27" t="s">
+      <c r="B402" s="28" t="s">
         <v>934</v>
       </c>
-      <c r="C402" s="27" t="s">
+      <c r="C402" s="28" t="s">
         <v>934</v>
       </c>
     </row>
     <row r="403" ht="15.75" customHeight="1">
-      <c r="A403" s="27" t="s">
+      <c r="A403" s="28" t="s">
         <v>935</v>
       </c>
-      <c r="B403" s="27" t="s">
+      <c r="B403" s="28" t="s">
         <v>936</v>
       </c>
-      <c r="C403" s="27" t="s">
+      <c r="C403" s="28" t="s">
         <v>936</v>
       </c>
     </row>
     <row r="404" ht="15.75" customHeight="1">
-      <c r="A404" s="27" t="s">
+      <c r="A404" s="28" t="s">
         <v>937</v>
       </c>
-      <c r="B404" s="27" t="s">
+      <c r="B404" s="28" t="s">
         <v>938</v>
       </c>
-      <c r="C404" s="27" t="s">
+      <c r="C404" s="28" t="s">
         <v>938</v>
       </c>
     </row>
     <row r="405" ht="15.75" customHeight="1">
-      <c r="A405" s="27" t="s">
+      <c r="A405" s="28" t="s">
         <v>939</v>
       </c>
-      <c r="B405" s="27" t="s">
+      <c r="B405" s="28" t="s">
         <v>940</v>
       </c>
-      <c r="C405" s="27" t="s">
+      <c r="C405" s="28" t="s">
         <v>940</v>
       </c>
     </row>
     <row r="406" ht="15.75" customHeight="1">
-      <c r="A406" s="27" t="s">
+      <c r="A406" s="28" t="s">
         <v>941</v>
       </c>
-      <c r="B406" s="27" t="s">
+      <c r="B406" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="C406" s="27" t="s">
+      <c r="C406" s="28" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="407" ht="15.75" customHeight="1">
-      <c r="A407" s="27" t="s">
+      <c r="A407" s="28" t="s">
         <v>942</v>
       </c>
-      <c r="B407" s="27" t="s">
+      <c r="B407" s="28" t="s">
         <v>943</v>
       </c>
-      <c r="C407" s="27" t="s">
+      <c r="C407" s="28" t="s">
         <v>943</v>
       </c>
     </row>
     <row r="408" ht="15.75" customHeight="1">
-      <c r="A408" s="27" t="s">
+      <c r="A408" s="28" t="s">
         <v>944</v>
       </c>
-      <c r="B408" s="27" t="s">
+      <c r="B408" s="28" t="s">
         <v>945</v>
       </c>
-      <c r="C408" s="27" t="s">
+      <c r="C408" s="28" t="s">
         <v>945</v>
       </c>
     </row>
     <row r="409" ht="15.75" customHeight="1">
-      <c r="A409" s="27" t="s">
+      <c r="A409" s="28" t="s">
         <v>946</v>
       </c>
-      <c r="B409" s="27" t="s">
+      <c r="B409" s="28" t="s">
         <v>947</v>
       </c>
-      <c r="C409" s="27" t="s">
+      <c r="C409" s="28" t="s">
         <v>947</v>
       </c>
     </row>
     <row r="410" ht="15.75" customHeight="1">
-      <c r="A410" s="27" t="s">
+      <c r="A410" s="28" t="s">
         <v>948</v>
       </c>
-      <c r="B410" s="27" t="s">
+      <c r="B410" s="28" t="s">
         <v>949</v>
       </c>
-      <c r="C410" s="27" t="s">
+      <c r="C410" s="28" t="s">
         <v>949</v>
       </c>
     </row>
     <row r="411" ht="15.75" customHeight="1">
-      <c r="A411" s="27" t="s">
+      <c r="A411" s="28" t="s">
         <v>950</v>
       </c>
-      <c r="B411" s="27" t="s">
+      <c r="B411" s="28" t="s">
         <v>951</v>
       </c>
-      <c r="C411" s="27" t="s">
+      <c r="C411" s="28" t="s">
         <v>951</v>
       </c>
     </row>
     <row r="412" ht="15.75" customHeight="1">
-      <c r="A412" s="27" t="s">
+      <c r="A412" s="28" t="s">
         <v>952</v>
       </c>
-      <c r="B412" s="27" t="s">
+      <c r="B412" s="28" t="s">
         <v>953</v>
       </c>
-      <c r="C412" s="27" t="s">
+      <c r="C412" s="28" t="s">
         <v>953</v>
       </c>
     </row>
     <row r="413" ht="15.75" customHeight="1">
-      <c r="A413" s="27" t="s">
+      <c r="A413" s="28" t="s">
         <v>954</v>
       </c>
-      <c r="B413" s="27" t="s">
+      <c r="B413" s="28" t="s">
         <v>955</v>
       </c>
-      <c r="C413" s="27" t="s">
+      <c r="C413" s="28" t="s">
         <v>955</v>
       </c>
     </row>
     <row r="414" ht="15.75" customHeight="1">
-      <c r="A414" s="27" t="s">
+      <c r="A414" s="28" t="s">
         <v>956</v>
       </c>
-      <c r="B414" s="27" t="s">
+      <c r="B414" s="28" t="s">
         <v>957</v>
       </c>
-      <c r="C414" s="27" t="s">
+      <c r="C414" s="28" t="s">
         <v>957</v>
       </c>
     </row>
     <row r="415" ht="15.75" customHeight="1">
-      <c r="A415" s="27" t="s">
+      <c r="A415" s="28" t="s">
         <v>958</v>
       </c>
-      <c r="B415" s="27" t="s">
+      <c r="B415" s="28" t="s">
         <v>959</v>
       </c>
-      <c r="C415" s="27" t="s">
+      <c r="C415" s="28" t="s">
         <v>959</v>
       </c>
     </row>
     <row r="416" ht="15.75" customHeight="1">
-      <c r="A416" s="27" t="s">
+      <c r="A416" s="28" t="s">
         <v>960</v>
       </c>
-      <c r="B416" s="27" t="s">
+      <c r="B416" s="28" t="s">
         <v>961</v>
       </c>
-      <c r="C416" s="27" t="s">
+      <c r="C416" s="28" t="s">
         <v>961</v>
       </c>
     </row>
     <row r="417" ht="15.75" customHeight="1">
-      <c r="A417" s="27" t="s">
+      <c r="A417" s="28" t="s">
         <v>962</v>
       </c>
-      <c r="B417" s="27" t="s">
+      <c r="B417" s="28" t="s">
         <v>963</v>
       </c>
-      <c r="C417" s="27" t="s">
+      <c r="C417" s="28" t="s">
         <v>963</v>
       </c>
     </row>
     <row r="418" ht="15.75" customHeight="1">
-      <c r="A418" s="27" t="s">
+      <c r="A418" s="28" t="s">
         <v>964</v>
       </c>
-      <c r="B418" s="27" t="s">
+      <c r="B418" s="28" t="s">
         <v>965</v>
       </c>
-      <c r="C418" s="27" t="s">
+      <c r="C418" s="28" t="s">
         <v>965</v>
       </c>
     </row>
     <row r="419" ht="15.75" customHeight="1">
-      <c r="A419" s="27" t="s">
+      <c r="A419" s="28" t="s">
         <v>966</v>
       </c>
-      <c r="B419" s="27" t="s">
+      <c r="B419" s="28" t="s">
         <v>967</v>
       </c>
-      <c r="C419" s="27" t="s">
+      <c r="C419" s="28" t="s">
         <v>967</v>
       </c>
     </row>
     <row r="420" ht="15.75" customHeight="1">
-      <c r="A420" s="27" t="s">
+      <c r="A420" s="28" t="s">
         <v>968</v>
       </c>
-      <c r="B420" s="27" t="s">
+      <c r="B420" s="28" t="s">
         <v>969</v>
       </c>
-      <c r="C420" s="27" t="s">
+      <c r="C420" s="28" t="s">
         <v>969</v>
       </c>
     </row>
     <row r="421" ht="15.75" customHeight="1">
-      <c r="A421" s="27" t="s">
+      <c r="A421" s="28" t="s">
         <v>970</v>
       </c>
-      <c r="B421" s="27" t="s">
+      <c r="B421" s="28" t="s">
         <v>971</v>
       </c>
-      <c r="C421" s="27" t="s">
+      <c r="C421" s="28" t="s">
         <v>971</v>
       </c>
     </row>
     <row r="422" ht="15.75" customHeight="1">
-      <c r="A422" s="27" t="s">
+      <c r="A422" s="28" t="s">
         <v>972</v>
       </c>
-      <c r="B422" s="27" t="s">
+      <c r="B422" s="28" t="s">
         <v>973</v>
       </c>
-      <c r="C422" s="27" t="s">
+      <c r="C422" s="28" t="s">
         <v>973</v>
       </c>
     </row>
     <row r="423" ht="15.75" customHeight="1">
-      <c r="A423" s="27" t="s">
+      <c r="A423" s="28" t="s">
         <v>974</v>
       </c>
-      <c r="B423" s="27" t="s">
+      <c r="B423" s="28" t="s">
         <v>975</v>
       </c>
-      <c r="C423" s="27" t="s">
+      <c r="C423" s="28" t="s">
         <v>975</v>
       </c>
     </row>
     <row r="424" ht="15.75" customHeight="1">
-      <c r="A424" s="27" t="s">
+      <c r="A424" s="28" t="s">
         <v>976</v>
       </c>
-      <c r="B424" s="27" t="s">
+      <c r="B424" s="28" t="s">
         <v>977</v>
       </c>
-      <c r="C424" s="27" t="s">
+      <c r="C424" s="28" t="s">
         <v>977</v>
       </c>
     </row>
     <row r="425" ht="15.75" customHeight="1">
-      <c r="A425" s="27" t="s">
+      <c r="A425" s="28" t="s">
         <v>978</v>
       </c>
-      <c r="B425" s="27" t="s">
+      <c r="B425" s="28" t="s">
         <v>979</v>
       </c>
-      <c r="C425" s="27" t="s">
+      <c r="C425" s="28" t="s">
         <v>979</v>
       </c>
     </row>
@@ -31178,51 +31202,51 @@
     </row>
     <row r="427" ht="15.75" customHeight="1"/>
     <row r="428" ht="15.75" customHeight="1">
-      <c r="A428" s="27" t="s">
+      <c r="A428" s="28" t="s">
         <v>982</v>
       </c>
-      <c r="B428" s="27" t="s">
+      <c r="B428" s="28" t="s">
         <v>983</v>
       </c>
-      <c r="C428" s="27" t="s">
+      <c r="C428" s="28" t="s">
         <v>983</v>
       </c>
     </row>
     <row r="429" ht="15.75" customHeight="1">
-      <c r="A429" s="27" t="s">
+      <c r="A429" s="28" t="s">
         <v>984</v>
       </c>
-      <c r="B429" s="27" t="s">
+      <c r="B429" s="28" t="s">
         <v>985</v>
       </c>
-      <c r="C429" s="27" t="s">
+      <c r="C429" s="28" t="s">
         <v>985</v>
       </c>
     </row>
     <row r="430" ht="15.75" customHeight="1">
-      <c r="A430" s="27" t="s">
+      <c r="A430" s="28" t="s">
         <v>986</v>
       </c>
-      <c r="B430" s="27" t="s">
+      <c r="B430" s="28" t="s">
         <v>987</v>
       </c>
-      <c r="C430" s="27" t="s">
+      <c r="C430" s="28" t="s">
         <v>987</v>
       </c>
     </row>
     <row r="431" ht="15.75" customHeight="1">
-      <c r="A431" s="27" t="s">
+      <c r="A431" s="28" t="s">
         <v>988</v>
       </c>
-      <c r="B431" s="27" t="s">
+      <c r="B431" s="28" t="s">
         <v>989</v>
       </c>
-      <c r="C431" s="27" t="s">
+      <c r="C431" s="28" t="s">
         <v>989</v>
       </c>
     </row>
     <row r="432" ht="15.75" customHeight="1">
-      <c r="A432" s="27" t="s">
+      <c r="A432" s="28" t="s">
         <v>990</v>
       </c>
       <c r="B432" s="12" t="s">
@@ -31234,57 +31258,57 @@
     </row>
     <row r="433" ht="15.75" customHeight="1"/>
     <row r="434" ht="15.75" customHeight="1">
-      <c r="A434" s="27" t="s">
+      <c r="A434" s="28" t="s">
         <v>992</v>
       </c>
-      <c r="B434" s="27" t="s">
+      <c r="B434" s="28" t="s">
         <v>993</v>
       </c>
-      <c r="C434" s="27" t="s">
+      <c r="C434" s="28" t="s">
         <v>993</v>
       </c>
     </row>
     <row r="435" ht="15.75" customHeight="1">
-      <c r="A435" s="27" t="s">
+      <c r="A435" s="28" t="s">
         <v>994</v>
       </c>
-      <c r="B435" s="27" t="s">
+      <c r="B435" s="28" t="s">
         <v>995</v>
       </c>
-      <c r="C435" s="27" t="s">
+      <c r="C435" s="28" t="s">
         <v>995</v>
       </c>
     </row>
     <row r="436" ht="15.75" customHeight="1">
-      <c r="A436" s="27" t="s">
+      <c r="A436" s="28" t="s">
         <v>996</v>
       </c>
-      <c r="B436" s="27" t="s">
+      <c r="B436" s="28" t="s">
         <v>997</v>
       </c>
-      <c r="C436" s="27" t="s">
+      <c r="C436" s="28" t="s">
         <v>997</v>
       </c>
     </row>
     <row r="437" ht="15.75" customHeight="1">
-      <c r="A437" s="27" t="s">
+      <c r="A437" s="28" t="s">
         <v>998</v>
       </c>
-      <c r="B437" s="27" t="s">
+      <c r="B437" s="28" t="s">
         <v>999</v>
       </c>
-      <c r="C437" s="27" t="s">
+      <c r="C437" s="28" t="s">
         <v>999</v>
       </c>
     </row>
     <row r="438" ht="15.75" customHeight="1">
-      <c r="A438" s="27" t="s">
+      <c r="A438" s="28" t="s">
         <v>1000</v>
       </c>
-      <c r="B438" s="27" t="s">
+      <c r="B438" s="28" t="s">
         <v>1001</v>
       </c>
-      <c r="C438" s="27" t="s">
+      <c r="C438" s="28" t="s">
         <v>1001</v>
       </c>
     </row>
@@ -31300,31 +31324,31 @@
       </c>
     </row>
     <row r="440" ht="15.75" customHeight="1">
-      <c r="B440" s="39" t="s">
+      <c r="B440" s="40" t="s">
         <v>1004</v>
       </c>
     </row>
     <row r="441" ht="15.75" customHeight="1"/>
     <row r="442" ht="15.75" customHeight="1"/>
     <row r="443" ht="15.75" customHeight="1">
-      <c r="A443" s="27" t="s">
+      <c r="A443" s="28" t="s">
         <v>1005</v>
       </c>
-      <c r="B443" s="27" t="s">
+      <c r="B443" s="28" t="s">
         <v>1006</v>
       </c>
-      <c r="C443" s="27" t="s">
+      <c r="C443" s="28" t="s">
         <v>1006</v>
       </c>
     </row>
     <row r="444" ht="15.75" customHeight="1">
-      <c r="A444" s="27" t="s">
+      <c r="A444" s="28" t="s">
         <v>1007</v>
       </c>
-      <c r="B444" s="27" t="s">
+      <c r="B444" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C444" s="27" t="s">
+      <c r="C444" s="28" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update code provider portal
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -1848,10 +1848,10 @@
     <t>PASSWORD_FOR_PROFILE</t>
   </si>
   <si>
+    <t>Manage@1234</t>
+  </si>
+  <si>
     <t>NEW_PASSWORD_FOR_PROFILE</t>
-  </si>
-  <si>
-    <t>Manage@1234</t>
   </si>
   <si>
     <t>ADDRESS_FOR_PROFILE</t>
@@ -3124,7 +3124,7 @@
     <font>
       <b/>
       <color rgb="FF297BDE"/>
-      <name val="&quot;JetBrains Mono&quot;"/>
+      <name val="JetBrains Mono"/>
     </font>
     <font>
       <b/>
@@ -3299,9 +3299,7 @@
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -28020,21 +28018,21 @@
         <v>607</v>
       </c>
       <c r="B76" s="34" t="s">
-        <v>8</v>
+        <v>608</v>
       </c>
       <c r="C76" s="34" t="s">
-        <v>8</v>
+        <v>608</v>
       </c>
     </row>
     <row r="77" ht="15.0" customHeight="1">
       <c r="A77" s="26" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B77" s="34" t="s">
-        <v>609</v>
+        <v>8</v>
       </c>
       <c r="C77" s="34" t="s">
-        <v>609</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
SanityPathWeb Stable For V4.2.13 (18/04/23)
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="1158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="1159">
   <si>
     <t>KEY</t>
   </si>
@@ -2495,6 +2495,9 @@
   </si>
   <si>
     <t>5-HT3 receptor antagonists;07 Mar 2023 11:11 PM;07 Mar 2023</t>
+  </si>
+  <si>
+    <t>Acetylaspartic acid;28 Mar 2023 10:26 PM;28 Mar 2023</t>
   </si>
   <si>
     <t>VERIFY_DASHBOARD_HEALTH_RECORD_2</t>
@@ -3725,7 +3728,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3830,6 +3833,9 @@
     </xf>
     <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
@@ -29264,104 +29270,104 @@
       <c r="B139" s="29" t="s">
         <v>825</v>
       </c>
-      <c r="C139" s="29" t="s">
-        <v>825</v>
+      <c r="C139" s="49" t="s">
+        <v>826</v>
       </c>
     </row>
     <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="29" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B140" s="29" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C140" s="29" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="29" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B141" s="29" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C141" s="29" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="142" ht="15.75" customHeight="1"/>
     <row r="143" ht="15.0" customHeight="1">
       <c r="A143" s="29" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B143" s="29" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C143" s="29" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="144" ht="15.75" customHeight="1"/>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="49" t="s">
-        <v>832</v>
+      <c r="A145" s="50" t="s">
+        <v>833</v>
       </c>
       <c r="B145" s="44" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C145" s="44" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="49" t="s">
+      <c r="A146" s="50" t="s">
+        <v>835</v>
+      </c>
+      <c r="B146" s="44" t="s">
         <v>834</v>
       </c>
-      <c r="B146" s="44" t="s">
-        <v>833</v>
-      </c>
       <c r="C146" s="44" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="147" ht="15.0" customHeight="1">
-      <c r="A147" s="49" t="s">
-        <v>835</v>
+      <c r="A147" s="50" t="s">
+        <v>836</v>
       </c>
       <c r="B147" s="44" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C147" s="44" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="148" ht="15.75" customHeight="1"/>
     <row r="149" ht="15.75" customHeight="1">
       <c r="B149" s="41" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
     </row>
     <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="29" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="B150" s="29" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="C150" s="29" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="151" ht="15.0" customHeight="1">
-      <c r="A151" s="49" t="s">
-        <v>839</v>
-      </c>
-      <c r="B151" s="50" t="s">
+      <c r="A151" s="50" t="s">
         <v>840</v>
       </c>
-      <c r="C151" s="50" t="s">
-        <v>840</v>
+      <c r="B151" s="51" t="s">
+        <v>841</v>
+      </c>
+      <c r="C151" s="51" t="s">
+        <v>841</v>
       </c>
     </row>
     <row r="152" ht="15.0" customHeight="1">
@@ -29388,223 +29394,223 @@
     </row>
     <row r="154" ht="15.75" customHeight="1"/>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="51" t="s">
+      <c r="A155" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="B155" s="50" t="s">
-        <v>838</v>
-      </c>
-      <c r="C155" s="50" t="s">
-        <v>838</v>
+      <c r="B155" s="51" t="s">
+        <v>839</v>
+      </c>
+      <c r="C155" s="51" t="s">
+        <v>839</v>
       </c>
     </row>
     <row r="156" ht="15.0" customHeight="1">
-      <c r="A156" s="51" t="s">
+      <c r="A156" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="B156" s="50" t="s">
-        <v>840</v>
-      </c>
-      <c r="C156" s="50" t="s">
-        <v>840</v>
+      <c r="B156" s="51" t="s">
+        <v>841</v>
+      </c>
+      <c r="C156" s="51" t="s">
+        <v>841</v>
       </c>
     </row>
     <row r="157" ht="15.0" customHeight="1">
-      <c r="A157" s="51" t="s">
+      <c r="A157" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="B157" s="50" t="s">
-        <v>841</v>
-      </c>
-      <c r="C157" s="50" t="s">
-        <v>841</v>
+      <c r="B157" s="51" t="s">
+        <v>842</v>
+      </c>
+      <c r="C157" s="51" t="s">
+        <v>842</v>
       </c>
     </row>
     <row r="158" ht="15.75" customHeight="1"/>
     <row r="159" ht="15.75" customHeight="1"/>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="51" t="s">
+      <c r="A160" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="B160" s="50" t="s">
+      <c r="B160" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="C160" s="50" t="s">
+      <c r="C160" s="51" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="161" ht="15.0" customHeight="1">
-      <c r="A161" s="51" t="s">
+      <c r="A161" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="B161" s="50" t="s">
+      <c r="B161" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="C161" s="50" t="s">
+      <c r="C161" s="51" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="162" ht="15.0" customHeight="1">
-      <c r="A162" s="51" t="s">
+      <c r="A162" s="52" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="163" ht="15.75" customHeight="1"/>
     <row r="164" ht="15.75" customHeight="1"/>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="51" t="s">
+      <c r="A165" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="B165" s="50" t="s">
+      <c r="B165" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="C165" s="50" t="s">
+      <c r="C165" s="51" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="166" ht="15.0" customHeight="1">
-      <c r="A166" s="51" t="s">
+      <c r="A166" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="B166" s="50" t="s">
-        <v>842</v>
-      </c>
-      <c r="C166" s="50" t="s">
-        <v>842</v>
+      <c r="B166" s="51" t="s">
+        <v>843</v>
+      </c>
+      <c r="C166" s="51" t="s">
+        <v>843</v>
       </c>
     </row>
     <row r="167" ht="15.0" customHeight="1">
-      <c r="A167" s="51" t="s">
+      <c r="A167" s="52" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="168" ht="15.75" customHeight="1"/>
     <row r="169" ht="15.75" customHeight="1"/>
     <row r="170" ht="15.0" customHeight="1">
-      <c r="A170" s="51" t="s">
+      <c r="A170" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="B170" s="50" t="s">
+      <c r="B170" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="C170" s="50" t="s">
+      <c r="C170" s="51" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="171" ht="15.0" customHeight="1">
-      <c r="A171" s="51" t="s">
+      <c r="A171" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="B171" s="50" t="s">
-        <v>843</v>
-      </c>
-      <c r="C171" s="50" t="s">
-        <v>843</v>
+      <c r="B171" s="51" t="s">
+        <v>844</v>
+      </c>
+      <c r="C171" s="51" t="s">
+        <v>844</v>
       </c>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="51" t="s">
+      <c r="A172" s="52" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="173" ht="15.75" customHeight="1"/>
     <row r="174" ht="15.75" customHeight="1"/>
     <row r="175" ht="15.0" customHeight="1">
-      <c r="A175" s="51" t="s">
+      <c r="A175" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="B175" s="50" t="s">
+      <c r="B175" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="C175" s="50" t="s">
+      <c r="C175" s="51" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="51" t="s">
+      <c r="A176" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="B176" s="50" t="s">
-        <v>843</v>
-      </c>
-      <c r="C176" s="50" t="s">
-        <v>843</v>
+      <c r="B176" s="51" t="s">
+        <v>844</v>
+      </c>
+      <c r="C176" s="51" t="s">
+        <v>844</v>
       </c>
     </row>
     <row r="177" ht="15.75" customHeight="1"/>
     <row r="178" ht="15.75" customHeight="1"/>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="51" t="s">
+      <c r="A179" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="B179" s="50" t="s">
+      <c r="B179" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="C179" s="50" t="s">
+      <c r="C179" s="51" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="51" t="s">
+      <c r="A180" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="B180" s="50" t="s">
-        <v>843</v>
-      </c>
-      <c r="C180" s="50" t="s">
-        <v>843</v>
+      <c r="B180" s="51" t="s">
+        <v>844</v>
+      </c>
+      <c r="C180" s="51" t="s">
+        <v>844</v>
       </c>
     </row>
     <row r="181" ht="15.75" customHeight="1"/>
     <row r="182" ht="15.75" customHeight="1"/>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="51" t="s">
+      <c r="A183" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="B183" s="50" t="s">
+      <c r="B183" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="C183" s="50" t="s">
+      <c r="C183" s="51" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="51" t="s">
+      <c r="A184" s="52" t="s">
         <v>105</v>
       </c>
-      <c r="B184" s="50" t="s">
+      <c r="B184" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="C184" s="50" t="s">
+      <c r="C184" s="51" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="51" t="s">
+      <c r="A185" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="B185" s="50" t="s">
+      <c r="B185" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="C185" s="50" t="s">
+      <c r="C185" s="51" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="50" t="s">
+      <c r="A186" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="B186" s="50" t="s">
-        <v>844</v>
-      </c>
-      <c r="C186" s="50" t="s">
-        <v>844</v>
+      <c r="B186" s="51" t="s">
+        <v>845</v>
+      </c>
+      <c r="C186" s="51" t="s">
+        <v>845</v>
       </c>
     </row>
     <row r="187" ht="15.75" customHeight="1"/>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="B188" s="52" t="s">
-        <v>845</v>
+      <c r="B188" s="53" t="s">
+        <v>846</v>
       </c>
     </row>
     <row r="189" ht="15.75" customHeight="1"/>
@@ -29612,7 +29618,7 @@
     <row r="191" ht="15.75" customHeight="1"/>
     <row r="192" ht="15.75" customHeight="1"/>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="53" t="s">
+      <c r="A193" s="54" t="s">
         <v>3</v>
       </c>
       <c r="B193" s="3" t="s">
@@ -29623,40 +29629,40 @@
       </c>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="53" t="s">
+      <c r="A194" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="B194" s="54" t="s">
+      <c r="B194" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="C194" s="54" t="s">
+      <c r="C194" s="55" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="53" t="s">
+      <c r="A195" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="B195" s="53" t="s">
+      <c r="B195" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C195" s="53" t="s">
+      <c r="C195" s="54" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="53" t="s">
+      <c r="A196" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="B196" s="53" t="s">
-        <v>846</v>
-      </c>
-      <c r="C196" s="53" t="s">
-        <v>846</v>
+      <c r="B196" s="54" t="s">
+        <v>847</v>
+      </c>
+      <c r="C196" s="54" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="53" t="s">
+      <c r="A197" s="54" t="s">
         <v>113</v>
       </c>
       <c r="B197" s="40" t="s">
@@ -29667,18 +29673,18 @@
       </c>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="53" t="s">
+      <c r="A198" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="B198" s="55" t="s">
+      <c r="B198" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="C198" s="55" t="s">
+      <c r="C198" s="56" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="53" t="s">
+      <c r="A199" s="54" t="s">
         <v>358</v>
       </c>
       <c r="B199" s="40" t="s">
@@ -29689,73 +29695,73 @@
       </c>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="53" t="s">
+      <c r="A200" s="54" t="s">
         <v>261</v>
       </c>
-      <c r="B200" s="53" t="s">
+      <c r="B200" s="54" t="s">
         <v>262</v>
       </c>
-      <c r="C200" s="53" t="s">
+      <c r="C200" s="54" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="53" t="s">
+      <c r="A201" s="54" t="s">
         <v>275</v>
       </c>
-      <c r="B201" s="53" t="s">
+      <c r="B201" s="54" t="s">
         <v>281</v>
       </c>
-      <c r="C201" s="53" t="s">
+      <c r="C201" s="54" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="53" t="s">
+      <c r="A202" s="54" t="s">
         <v>277</v>
       </c>
-      <c r="B202" s="53" t="s">
+      <c r="B202" s="54" t="s">
         <v>278</v>
       </c>
-      <c r="C202" s="53" t="s">
+      <c r="C202" s="54" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="53" t="s">
+      <c r="A203" s="54" t="s">
         <v>279</v>
       </c>
-      <c r="B203" s="53" t="s">
+      <c r="B203" s="54" t="s">
         <v>280</v>
       </c>
-      <c r="C203" s="53" t="s">
+      <c r="C203" s="54" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="53" t="s">
+      <c r="A204" s="54" t="s">
         <v>265</v>
       </c>
-      <c r="B204" s="53" t="s">
+      <c r="B204" s="54" t="s">
         <v>266</v>
       </c>
-      <c r="C204" s="53" t="s">
+      <c r="C204" s="54" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="53" t="s">
+      <c r="A205" s="54" t="s">
         <v>366</v>
       </c>
-      <c r="B205" s="53" t="s">
+      <c r="B205" s="54" t="s">
         <v>367</v>
       </c>
-      <c r="C205" s="53" t="s">
+      <c r="C205" s="54" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="53" t="s">
+      <c r="A206" s="54" t="s">
         <v>227</v>
       </c>
       <c r="B206" s="40" t="s">
@@ -29766,18 +29772,18 @@
       </c>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="53" t="s">
+      <c r="A207" s="54" t="s">
         <v>229</v>
       </c>
-      <c r="B207" s="55" t="s">
+      <c r="B207" s="56" t="s">
         <v>230</v>
       </c>
-      <c r="C207" s="55" t="s">
+      <c r="C207" s="56" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="53" t="s">
+      <c r="A208" s="54" t="s">
         <v>364</v>
       </c>
       <c r="B208" s="40" t="s">
@@ -29789,41 +29795,41 @@
     </row>
     <row r="209" ht="15.75" customHeight="1"/>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="53" t="s">
+      <c r="A210" s="54" t="s">
         <v>412</v>
       </c>
-      <c r="B210" s="53" t="s">
+      <c r="B210" s="54" t="s">
         <v>413</v>
       </c>
-      <c r="C210" s="53" t="s">
+      <c r="C210" s="54" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="53" t="s">
-        <v>847</v>
-      </c>
-      <c r="B211" s="55" t="s">
+      <c r="A211" s="54" t="s">
         <v>848</v>
       </c>
-      <c r="C211" s="55" t="s">
-        <v>848</v>
+      <c r="B211" s="56" t="s">
+        <v>849</v>
+      </c>
+      <c r="C211" s="56" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="53" t="s">
+      <c r="A212" s="54" t="s">
         <v>416</v>
       </c>
       <c r="B212" s="40" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C212" s="40" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="53" t="s">
-        <v>850</v>
+      <c r="A213" s="54" t="s">
+        <v>851</v>
       </c>
       <c r="B213" s="40" t="s">
         <v>419</v>
@@ -29833,1687 +29839,1687 @@
       </c>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="53" t="s">
+      <c r="A214" s="54" t="s">
         <v>175</v>
       </c>
-      <c r="B214" s="53" t="s">
+      <c r="B214" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="C214" s="53" t="s">
+      <c r="C214" s="54" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="53" t="s">
+      <c r="A215" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="B215" s="55" t="s">
+      <c r="B215" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="C215" s="55" t="s">
+      <c r="C215" s="56" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="53" t="s">
+      <c r="A216" s="54" t="s">
         <v>368</v>
       </c>
-      <c r="B216" s="53" t="s">
+      <c r="B216" s="54" t="s">
         <v>369</v>
       </c>
-      <c r="C216" s="53" t="s">
+      <c r="C216" s="54" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="53" t="s">
+      <c r="A217" s="54" t="s">
         <v>271</v>
       </c>
-      <c r="B217" s="53" t="s">
+      <c r="B217" s="54" t="s">
         <v>272</v>
       </c>
-      <c r="C217" s="53" t="s">
+      <c r="C217" s="54" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="53" t="s">
+      <c r="A218" s="54" t="s">
         <v>273</v>
       </c>
-      <c r="B218" s="53" t="s">
+      <c r="B218" s="54" t="s">
         <v>274</v>
       </c>
-      <c r="C218" s="53" t="s">
+      <c r="C218" s="54" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="219" ht="15.75" customHeight="1"/>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="53" t="s">
-        <v>851</v>
-      </c>
-      <c r="B220" s="55" t="s">
+      <c r="A220" s="54" t="s">
         <v>852</v>
       </c>
-      <c r="C220" s="55" t="s">
-        <v>852</v>
+      <c r="B220" s="56" t="s">
+        <v>853</v>
+      </c>
+      <c r="C220" s="56" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="53" t="s">
-        <v>853</v>
+      <c r="A221" s="54" t="s">
+        <v>854</v>
       </c>
       <c r="B221" s="40" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C221" s="40" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="53" t="s">
+      <c r="A222" s="54" t="s">
         <v>193</v>
       </c>
-      <c r="B222" s="53" t="s">
+      <c r="B222" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="C222" s="53" t="s">
+      <c r="C222" s="54" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="53" t="s">
+      <c r="A223" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="B223" s="55" t="s">
+      <c r="B223" s="56" t="s">
         <v>201</v>
       </c>
-      <c r="C223" s="55" t="s">
+      <c r="C223" s="56" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="53" t="s">
+      <c r="A224" s="54" t="s">
         <v>376</v>
       </c>
-      <c r="B224" s="53" t="s">
+      <c r="B224" s="54" t="s">
         <v>377</v>
       </c>
-      <c r="C224" s="53" t="s">
+      <c r="C224" s="54" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="53" t="s">
-        <v>855</v>
-      </c>
-      <c r="B225" s="53" t="s">
+      <c r="A225" s="54" t="s">
         <v>856</v>
       </c>
-      <c r="C225" s="53" t="s">
-        <v>856</v>
+      <c r="B225" s="54" t="s">
+        <v>857</v>
+      </c>
+      <c r="C225" s="54" t="s">
+        <v>857</v>
       </c>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="53" t="s">
+      <c r="A226" s="54" t="s">
         <v>420</v>
       </c>
-      <c r="B226" s="53" t="s">
+      <c r="B226" s="54" t="s">
         <v>262</v>
       </c>
-      <c r="C226" s="53" t="s">
+      <c r="C226" s="54" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="53" t="s">
+      <c r="A227" s="54" t="s">
         <v>283</v>
       </c>
-      <c r="B227" s="53" t="s">
+      <c r="B227" s="54" t="s">
         <v>284</v>
       </c>
-      <c r="C227" s="53" t="s">
+      <c r="C227" s="54" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="A228" s="53" t="s">
-        <v>857</v>
-      </c>
-      <c r="B228" s="53" t="s">
+      <c r="A228" s="54" t="s">
         <v>858</v>
       </c>
-      <c r="C228" s="53" t="s">
-        <v>858</v>
+      <c r="B228" s="54" t="s">
+        <v>859</v>
+      </c>
+      <c r="C228" s="54" t="s">
+        <v>859</v>
       </c>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="A229" s="53" t="s">
+      <c r="A229" s="54" t="s">
         <v>423</v>
       </c>
-      <c r="B229" s="53" t="s">
+      <c r="B229" s="54" t="s">
         <v>290</v>
       </c>
-      <c r="C229" s="53" t="s">
+      <c r="C229" s="54" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="A230" s="53" t="s">
-        <v>859</v>
-      </c>
-      <c r="B230" s="55" t="s">
+      <c r="A230" s="54" t="s">
         <v>860</v>
       </c>
-      <c r="C230" s="55" t="s">
-        <v>860</v>
+      <c r="B230" s="56" t="s">
+        <v>861</v>
+      </c>
+      <c r="C230" s="56" t="s">
+        <v>861</v>
       </c>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="A231" s="53" t="s">
+      <c r="A231" s="54" t="s">
         <v>289</v>
       </c>
-      <c r="B231" s="53" t="s">
+      <c r="B231" s="54" t="s">
         <v>290</v>
       </c>
-      <c r="C231" s="53" t="s">
+      <c r="C231" s="54" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="53" t="s">
+      <c r="A232" s="54" t="s">
         <v>291</v>
       </c>
-      <c r="B232" s="53" t="s">
+      <c r="B232" s="54" t="s">
         <v>292</v>
       </c>
-      <c r="C232" s="53" t="s">
+      <c r="C232" s="54" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="233" ht="15.75" customHeight="1"/>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="A234" s="53" t="s">
+      <c r="A234" s="54" t="s">
         <v>293</v>
       </c>
-      <c r="B234" s="53" t="s">
+      <c r="B234" s="54" t="s">
         <v>294</v>
       </c>
-      <c r="C234" s="53" t="s">
+      <c r="C234" s="54" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="A235" s="53" t="s">
+      <c r="A235" s="54" t="s">
         <v>283</v>
       </c>
-      <c r="B235" s="53" t="s">
+      <c r="B235" s="54" t="s">
         <v>284</v>
       </c>
-      <c r="C235" s="53" t="s">
+      <c r="C235" s="54" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="A236" s="53" t="s">
-        <v>861</v>
-      </c>
-      <c r="B236" s="55" t="s">
+      <c r="A236" s="54" t="s">
         <v>862</v>
       </c>
-      <c r="C236" s="55" t="s">
-        <v>862</v>
+      <c r="B236" s="56" t="s">
+        <v>863</v>
+      </c>
+      <c r="C236" s="56" t="s">
+        <v>863</v>
       </c>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="53" t="s">
+      <c r="A237" s="54" t="s">
         <v>269</v>
       </c>
-      <c r="B237" s="53" t="s">
+      <c r="B237" s="54" t="s">
         <v>270</v>
       </c>
-      <c r="C237" s="53" t="s">
+      <c r="C237" s="54" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="A238" s="53" t="s">
+      <c r="A238" s="54" t="s">
         <v>239</v>
       </c>
-      <c r="B238" s="53" t="s">
+      <c r="B238" s="54" t="s">
         <v>262</v>
       </c>
-      <c r="C238" s="53" t="s">
+      <c r="C238" s="54" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="A239" s="53" t="s">
-        <v>863</v>
-      </c>
-      <c r="B239" s="55" t="s">
+      <c r="A239" s="54" t="s">
         <v>864</v>
       </c>
-      <c r="C239" s="55" t="s">
-        <v>864</v>
+      <c r="B239" s="56" t="s">
+        <v>865</v>
+      </c>
+      <c r="C239" s="56" t="s">
+        <v>865</v>
       </c>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="A240" s="53" t="s">
-        <v>865</v>
-      </c>
-      <c r="B240" s="55" t="s">
+      <c r="A240" s="54" t="s">
         <v>866</v>
       </c>
-      <c r="C240" s="55" t="s">
-        <v>866</v>
+      <c r="B240" s="56" t="s">
+        <v>867</v>
+      </c>
+      <c r="C240" s="56" t="s">
+        <v>867</v>
       </c>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="A241" s="53" t="s">
+      <c r="A241" s="54" t="s">
         <v>157</v>
       </c>
-      <c r="B241" s="55" t="s">
+      <c r="B241" s="56" t="s">
         <v>159</v>
       </c>
-      <c r="C241" s="55" t="s">
+      <c r="C241" s="56" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="A242" s="53" t="s">
+      <c r="A242" s="54" t="s">
         <v>166</v>
       </c>
-      <c r="B242" s="53" t="s">
+      <c r="B242" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="C242" s="53" t="s">
+      <c r="C242" s="54" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="A243" s="53" t="s">
+      <c r="A243" s="54" t="s">
         <v>205</v>
       </c>
-      <c r="B243" s="55" t="s">
-        <v>867</v>
-      </c>
-      <c r="C243" s="55" t="s">
-        <v>867</v>
+      <c r="B243" s="56" t="s">
+        <v>868</v>
+      </c>
+      <c r="C243" s="56" t="s">
+        <v>868</v>
       </c>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="A244" s="53" t="s">
+      <c r="A244" s="54" t="s">
         <v>211</v>
       </c>
-      <c r="B244" s="56" t="s">
+      <c r="B244" s="57" t="s">
         <v>216</v>
       </c>
-      <c r="C244" s="56" t="s">
+      <c r="C244" s="57" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="A245" s="53" t="s">
+      <c r="A245" s="54" t="s">
         <v>255</v>
       </c>
-      <c r="B245" s="53" t="s">
+      <c r="B245" s="54" t="s">
         <v>260</v>
       </c>
-      <c r="C245" s="53" t="s">
+      <c r="C245" s="54" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="A246" s="53" t="s">
+      <c r="A246" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="B246" s="53" t="s">
+      <c r="B246" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="C246" s="53" t="s">
+      <c r="C246" s="54" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="A247" s="53" t="s">
+      <c r="A247" s="54" t="s">
         <v>145</v>
       </c>
-      <c r="B247" s="55" t="s">
+      <c r="B247" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="C247" s="55" t="s">
+      <c r="C247" s="56" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="A248" s="53" t="s">
+      <c r="A248" s="54" t="s">
         <v>263</v>
       </c>
-      <c r="B248" s="55" t="s">
+      <c r="B248" s="56" t="s">
         <v>264</v>
       </c>
-      <c r="C248" s="55" t="s">
+      <c r="C248" s="56" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="A249" s="53" t="s">
+      <c r="A249" s="54" t="s">
         <v>223</v>
       </c>
-      <c r="B249" s="55" t="s">
+      <c r="B249" s="56" t="s">
         <v>262</v>
       </c>
-      <c r="C249" s="55" t="s">
+      <c r="C249" s="56" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="A250" s="53" t="s">
-        <v>868</v>
-      </c>
-      <c r="B250" s="55" t="s">
+      <c r="A250" s="54" t="s">
         <v>869</v>
       </c>
-      <c r="C250" s="55" t="s">
-        <v>869</v>
+      <c r="B250" s="56" t="s">
+        <v>870</v>
+      </c>
+      <c r="C250" s="56" t="s">
+        <v>870</v>
       </c>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="A251" s="53" t="s">
+      <c r="A251" s="54" t="s">
         <v>267</v>
       </c>
-      <c r="B251" s="55" t="s">
+      <c r="B251" s="56" t="s">
         <v>268</v>
       </c>
-      <c r="C251" s="55" t="s">
+      <c r="C251" s="56" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="A252" s="53" t="s">
-        <v>870</v>
-      </c>
-      <c r="B252" s="55" t="s">
+      <c r="A252" s="54" t="s">
         <v>871</v>
       </c>
-      <c r="C252" s="55" t="s">
-        <v>871</v>
+      <c r="B252" s="56" t="s">
+        <v>872</v>
+      </c>
+      <c r="C252" s="56" t="s">
+        <v>872</v>
       </c>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="A253" s="53" t="s">
+      <c r="A253" s="54" t="s">
         <v>249</v>
       </c>
-      <c r="B253" s="53" t="s">
-        <v>872</v>
-      </c>
-      <c r="C253" s="53" t="s">
-        <v>872</v>
+      <c r="B253" s="54" t="s">
+        <v>873</v>
+      </c>
+      <c r="C253" s="54" t="s">
+        <v>873</v>
       </c>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="A254" s="53" t="s">
+      <c r="A254" s="54" t="s">
         <v>252</v>
       </c>
-      <c r="B254" s="55" t="s">
-        <v>873</v>
-      </c>
-      <c r="C254" s="55" t="s">
-        <v>873</v>
+      <c r="B254" s="56" t="s">
+        <v>874</v>
+      </c>
+      <c r="C254" s="56" t="s">
+        <v>874</v>
       </c>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="A255" s="53" t="s">
+      <c r="A255" s="54" t="s">
         <v>243</v>
       </c>
-      <c r="B255" s="53" t="s">
-        <v>874</v>
-      </c>
-      <c r="C255" s="53" t="s">
-        <v>874</v>
+      <c r="B255" s="54" t="s">
+        <v>875</v>
+      </c>
+      <c r="C255" s="54" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="A256" s="53" t="s">
+      <c r="A256" s="54" t="s">
         <v>246</v>
       </c>
-      <c r="B256" s="53" t="s">
-        <v>875</v>
-      </c>
-      <c r="C256" s="53" t="s">
-        <v>875</v>
+      <c r="B256" s="54" t="s">
+        <v>876</v>
+      </c>
+      <c r="C256" s="54" t="s">
+        <v>876</v>
       </c>
     </row>
     <row r="257" ht="15.75" customHeight="1"/>
     <row r="258" ht="15.75" customHeight="1"/>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="B259" s="57" t="s">
-        <v>876</v>
+      <c r="B259" s="58" t="s">
+        <v>877</v>
       </c>
     </row>
     <row r="260" ht="15.75" customHeight="1"/>
     <row r="261" ht="15.75" customHeight="1"/>
     <row r="262" ht="15.75" customHeight="1"/>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="A263" s="53" t="s">
+      <c r="A263" s="54" t="s">
         <v>295</v>
       </c>
-      <c r="B263" s="53" t="s">
+      <c r="B263" s="54" t="s">
         <v>296</v>
       </c>
-      <c r="C263" s="53" t="s">
+      <c r="C263" s="54" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="A264" s="53" t="s">
+      <c r="A264" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="B264" s="53" t="s">
+      <c r="B264" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C264" s="53" t="s">
+      <c r="C264" s="54" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="A265" s="53" t="s">
-        <v>877</v>
-      </c>
-      <c r="B265" s="53" t="s">
+      <c r="A265" s="54" t="s">
         <v>878</v>
       </c>
-      <c r="C265" s="53" t="s">
-        <v>878</v>
+      <c r="B265" s="54" t="s">
+        <v>879</v>
+      </c>
+      <c r="C265" s="54" t="s">
+        <v>879</v>
       </c>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="A266" s="53" t="s">
+      <c r="A266" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="B266" s="53" t="s">
-        <v>879</v>
-      </c>
-      <c r="C266" s="53" t="s">
-        <v>879</v>
+      <c r="B266" s="54" t="s">
+        <v>880</v>
+      </c>
+      <c r="C266" s="54" t="s">
+        <v>880</v>
       </c>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="A267" s="53" t="s">
-        <v>880</v>
+      <c r="A267" s="54" t="s">
+        <v>881</v>
       </c>
       <c r="B267" s="40" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="C267" s="40" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="A268" s="53" t="s">
-        <v>882</v>
-      </c>
-      <c r="B268" s="58" t="s">
+      <c r="A268" s="54" t="s">
         <v>883</v>
       </c>
-      <c r="C268" s="58" t="s">
-        <v>883</v>
+      <c r="B268" s="59" t="s">
+        <v>884</v>
+      </c>
+      <c r="C268" s="59" t="s">
+        <v>884</v>
       </c>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="A269" s="53" t="s">
-        <v>884</v>
-      </c>
-      <c r="B269" s="53" t="s">
+      <c r="A269" s="54" t="s">
         <v>885</v>
       </c>
-      <c r="C269" s="53" t="s">
-        <v>885</v>
+      <c r="B269" s="54" t="s">
+        <v>886</v>
+      </c>
+      <c r="C269" s="54" t="s">
+        <v>886</v>
       </c>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="A270" s="53" t="s">
-        <v>886</v>
+      <c r="A270" s="54" t="s">
+        <v>887</v>
       </c>
       <c r="B270" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C270" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="A271" s="53" t="s">
+      <c r="A271" s="54" t="s">
+        <v>889</v>
+      </c>
+      <c r="B271" s="60">
+        <v>120.0</v>
+      </c>
+      <c r="C271" s="60">
+        <v>120.0</v>
+      </c>
+    </row>
+    <row r="272" ht="15.75" customHeight="1">
+      <c r="A272" s="54" t="s">
+        <v>890</v>
+      </c>
+      <c r="B272" s="40" t="s">
+        <v>891</v>
+      </c>
+      <c r="C272" s="40" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="273" ht="15.75" customHeight="1">
+      <c r="A273" s="54" t="s">
+        <v>892</v>
+      </c>
+      <c r="B273" s="40" t="s">
+        <v>893</v>
+      </c>
+      <c r="C273" s="40" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="274" ht="15.75" customHeight="1">
+      <c r="A274" s="54" t="s">
+        <v>894</v>
+      </c>
+      <c r="B274" s="40" t="s">
+        <v>895</v>
+      </c>
+      <c r="C274" s="40" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="275" ht="15.75" customHeight="1">
+      <c r="A275" s="54" t="s">
+        <v>896</v>
+      </c>
+      <c r="B275" s="40" t="s">
+        <v>897</v>
+      </c>
+      <c r="C275" s="40" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="276" ht="15.75" customHeight="1">
+      <c r="A276" s="54" t="s">
+        <v>898</v>
+      </c>
+      <c r="B276" s="40" t="s">
         <v>888</v>
       </c>
-      <c r="B271" s="59">
-        <v>120.0</v>
-      </c>
-      <c r="C271" s="59">
-        <v>120.0</v>
-      </c>
-    </row>
-    <row r="272" ht="15.75" customHeight="1">
-      <c r="A272" s="53" t="s">
-        <v>889</v>
-      </c>
-      <c r="B272" s="40" t="s">
-        <v>890</v>
-      </c>
-      <c r="C272" s="40" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="273" ht="15.75" customHeight="1">
-      <c r="A273" s="53" t="s">
-        <v>891</v>
-      </c>
-      <c r="B273" s="40" t="s">
-        <v>892</v>
-      </c>
-      <c r="C273" s="40" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="274" ht="15.75" customHeight="1">
-      <c r="A274" s="53" t="s">
-        <v>893</v>
-      </c>
-      <c r="B274" s="40" t="s">
-        <v>894</v>
-      </c>
-      <c r="C274" s="40" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="275" ht="15.75" customHeight="1">
-      <c r="A275" s="53" t="s">
-        <v>895</v>
-      </c>
-      <c r="B275" s="40" t="s">
-        <v>896</v>
-      </c>
-      <c r="C275" s="40" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="276" ht="15.75" customHeight="1">
-      <c r="A276" s="53" t="s">
-        <v>897</v>
-      </c>
-      <c r="B276" s="40" t="s">
-        <v>887</v>
-      </c>
       <c r="C276" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="277" ht="15.75" customHeight="1">
       <c r="A277" s="40" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="B277" s="40" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C277" s="40" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
     </row>
     <row r="278" ht="15.75" customHeight="1">
       <c r="A278" s="40" t="s">
-        <v>900</v>
-      </c>
-      <c r="B278" s="59">
+        <v>901</v>
+      </c>
+      <c r="B278" s="60">
         <v>6.0</v>
       </c>
-      <c r="C278" s="59">
+      <c r="C278" s="60">
         <v>6.0</v>
       </c>
     </row>
     <row r="279" ht="15.75" customHeight="1">
       <c r="A279" s="40" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="B279" s="40" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C279" s="40" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="280" ht="15.75" customHeight="1">
       <c r="A280" s="40" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="B280" s="40" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="C280" s="40" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row r="281" ht="15.75" customHeight="1">
       <c r="A281" s="40" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B281" s="40" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="C281" s="40" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
     </row>
     <row r="282" ht="15.75" customHeight="1">
       <c r="A282" s="40" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="B282" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C282" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="283" ht="15.75" customHeight="1">
       <c r="A283" s="40" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B283" s="40" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="C283" s="40" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
     </row>
     <row r="284" ht="15.75" customHeight="1">
       <c r="A284" s="40" t="s">
-        <v>910</v>
-      </c>
-      <c r="B284" s="60">
+        <v>911</v>
+      </c>
+      <c r="B284" s="61">
         <v>13.0</v>
       </c>
-      <c r="C284" s="60">
+      <c r="C284" s="61">
         <v>13.0</v>
       </c>
     </row>
     <row r="285" ht="15.75" customHeight="1">
       <c r="A285" s="40" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="B285" s="40" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="C285" s="40" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
     </row>
     <row r="286" ht="15.75" customHeight="1">
       <c r="A286" s="40" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B286" s="40" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="C286" s="40" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
     </row>
     <row r="287" ht="15.75" customHeight="1">
       <c r="A287" s="40" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B287" s="40" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C287" s="40" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
     </row>
     <row r="288" ht="15.75" customHeight="1">
       <c r="A288" s="40" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="B288" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C288" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="289" ht="15.75" customHeight="1">
       <c r="A289" s="40" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="B289" s="40" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="C289" s="40" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
     </row>
     <row r="290" ht="15.75" customHeight="1">
       <c r="A290" s="40" t="s">
-        <v>920</v>
-      </c>
-      <c r="B290" s="59">
+        <v>921</v>
+      </c>
+      <c r="B290" s="60">
         <v>12.0</v>
       </c>
-      <c r="C290" s="59">
+      <c r="C290" s="60">
         <v>12.0</v>
       </c>
     </row>
     <row r="291" ht="15.75" customHeight="1">
       <c r="A291" s="40" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="B291" s="40" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="C291" s="40" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
     </row>
     <row r="292" ht="15.75" customHeight="1">
       <c r="A292" s="40" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B292" s="40" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="C292" s="40" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
     </row>
     <row r="293" ht="15.75" customHeight="1">
       <c r="A293" s="40" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="B293" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C293" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="294" ht="15.75" customHeight="1">
       <c r="A294" s="40" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B294" s="40" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="C294" s="40" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
     </row>
     <row r="295" ht="15.75" customHeight="1">
       <c r="A295" s="40" t="s">
-        <v>928</v>
-      </c>
-      <c r="B295" s="59">
+        <v>929</v>
+      </c>
+      <c r="B295" s="60">
         <v>2.0</v>
       </c>
-      <c r="C295" s="59">
+      <c r="C295" s="60">
         <v>2.0</v>
       </c>
     </row>
     <row r="296" ht="15.75" customHeight="1">
       <c r="A296" s="40" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B296" s="40" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="C296" s="40" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
     </row>
     <row r="297" ht="15.75" customHeight="1">
       <c r="A297" s="40" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B297" s="40" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C297" s="40" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
     </row>
     <row r="298" ht="15.75" customHeight="1">
       <c r="A298" s="40" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B298" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C298" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="299" ht="15.75" customHeight="1">
       <c r="A299" s="40" t="s">
-        <v>934</v>
-      </c>
-      <c r="B299" s="59">
+        <v>935</v>
+      </c>
+      <c r="B299" s="60">
         <v>7.0</v>
       </c>
-      <c r="C299" s="59">
+      <c r="C299" s="60">
         <v>7.0</v>
       </c>
     </row>
     <row r="300" ht="15.75" customHeight="1">
       <c r="A300" s="40" t="s">
-        <v>935</v>
-      </c>
-      <c r="B300" s="59">
+        <v>936</v>
+      </c>
+      <c r="B300" s="60">
         <v>8.0</v>
       </c>
-      <c r="C300" s="59">
+      <c r="C300" s="60">
         <v>8.0</v>
       </c>
     </row>
     <row r="301" ht="15.75" customHeight="1">
       <c r="A301" s="40" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="B301" s="40" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C301" s="40" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
     </row>
     <row r="302" ht="15.75" customHeight="1">
       <c r="A302" s="40" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="B302" s="40" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C302" s="40" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
     </row>
     <row r="303" ht="15.75" customHeight="1">
       <c r="A303" s="40" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="B303" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C303" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="304" ht="15.75" customHeight="1">
       <c r="A304" s="40" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B304" s="40" t="s">
-        <v>942</v>
-      </c>
-      <c r="C304" s="58" t="s">
-        <v>942</v>
+        <v>943</v>
+      </c>
+      <c r="C304" s="59" t="s">
+        <v>943</v>
       </c>
     </row>
     <row r="305" ht="15.75" customHeight="1">
       <c r="A305" s="40" t="s">
-        <v>943</v>
-      </c>
-      <c r="B305" s="59">
+        <v>944</v>
+      </c>
+      <c r="B305" s="60">
         <v>6.0</v>
       </c>
-      <c r="C305" s="59">
+      <c r="C305" s="60">
         <v>6.0</v>
       </c>
     </row>
     <row r="306" ht="15.75" customHeight="1">
       <c r="A306" s="40" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="B306" s="40" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="C306" s="40" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row r="307" ht="15.75" customHeight="1">
       <c r="A307" s="40" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B307" s="40" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C307" s="40" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
     <row r="308" ht="15.75" customHeight="1">
       <c r="A308" s="40" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="B308" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C308" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="309" ht="15.75" customHeight="1">
       <c r="A309" s="40" t="s">
-        <v>949</v>
-      </c>
-      <c r="B309" s="59">
+        <v>950</v>
+      </c>
+      <c r="B309" s="60">
         <v>9.0</v>
       </c>
-      <c r="C309" s="59">
+      <c r="C309" s="60">
         <v>9.0</v>
       </c>
     </row>
     <row r="310" ht="15.75" customHeight="1">
       <c r="A310" s="40" t="s">
-        <v>950</v>
-      </c>
-      <c r="B310" s="59">
+        <v>951</v>
+      </c>
+      <c r="B310" s="60">
         <v>10.0</v>
       </c>
-      <c r="C310" s="59">
+      <c r="C310" s="60">
         <v>10.0</v>
       </c>
     </row>
     <row r="311" ht="15.75" customHeight="1">
       <c r="A311" s="40" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B311" s="40" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C311" s="40" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
     </row>
     <row r="312" ht="15.75" customHeight="1">
       <c r="A312" s="40" t="s">
+        <v>954</v>
+      </c>
+      <c r="B312" s="40" t="s">
         <v>953</v>
       </c>
-      <c r="B312" s="40" t="s">
-        <v>952</v>
-      </c>
       <c r="C312" s="40" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
     </row>
     <row r="313" ht="15.75" customHeight="1">
       <c r="A313" s="40" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B313" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C313" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="314" ht="15.75" customHeight="1">
       <c r="A314" s="40" t="s">
-        <v>955</v>
-      </c>
-      <c r="B314" s="59">
+        <v>956</v>
+      </c>
+      <c r="B314" s="60">
         <v>12.0</v>
       </c>
-      <c r="C314" s="59">
+      <c r="C314" s="60">
         <v>12.0</v>
       </c>
     </row>
     <row r="315" ht="15.75" customHeight="1">
       <c r="A315" s="40" t="s">
-        <v>956</v>
-      </c>
-      <c r="B315" s="59">
+        <v>957</v>
+      </c>
+      <c r="B315" s="60">
         <v>13.0</v>
       </c>
-      <c r="C315" s="59">
+      <c r="C315" s="60">
         <v>13.0</v>
       </c>
     </row>
     <row r="316" ht="15.75" customHeight="1">
       <c r="A316" s="40" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B316" s="40" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C316" s="40" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="317" ht="15.75" customHeight="1">
       <c r="A317" s="40" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="B317" s="40" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="C317" s="40" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
     </row>
     <row r="318" ht="15.75" customHeight="1">
       <c r="A318" s="40" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B318" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C318" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="319" ht="15.75" customHeight="1">
       <c r="A319" s="40" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B319" s="40" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C319" s="40" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
     </row>
     <row r="320" ht="15.75" customHeight="1">
       <c r="A320" s="40" t="s">
-        <v>963</v>
-      </c>
-      <c r="B320" s="59">
+        <v>964</v>
+      </c>
+      <c r="B320" s="60">
         <v>6.0</v>
       </c>
-      <c r="C320" s="59">
+      <c r="C320" s="60">
         <v>6.0</v>
       </c>
     </row>
     <row r="321" ht="15.75" customHeight="1">
       <c r="A321" s="40" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="B321" s="40" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="C321" s="40" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="322" ht="15.75" customHeight="1">
       <c r="A322" s="40" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="B322" s="40" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="C322" s="40" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row r="323" ht="15.75" customHeight="1">
       <c r="A323" s="40" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B323" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C323" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="324" ht="15.75" customHeight="1">
       <c r="A324" s="40" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="B324" s="40" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="C324" s="40" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="325" ht="15.75" customHeight="1">
       <c r="A325" s="40" t="s">
-        <v>971</v>
-      </c>
-      <c r="B325" s="59">
+        <v>972</v>
+      </c>
+      <c r="B325" s="60">
         <v>7.0</v>
       </c>
-      <c r="C325" s="59">
+      <c r="C325" s="60">
         <v>7.0</v>
       </c>
     </row>
     <row r="326" ht="15.75" customHeight="1">
       <c r="A326" s="40" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B326" s="40" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C326" s="40" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
     </row>
     <row r="327" ht="15.75" customHeight="1">
       <c r="A327" s="40" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="B327" s="40" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="C327" s="40" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
     </row>
     <row r="328" ht="15.75" customHeight="1">
       <c r="A328" s="40" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="B328" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C328" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="329" ht="15.75" customHeight="1">
       <c r="A329" s="40" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="B329" s="40" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="C329" s="40" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
     </row>
     <row r="330" ht="15.75" customHeight="1">
       <c r="A330" s="40" t="s">
-        <v>979</v>
-      </c>
-      <c r="B330" s="59">
+        <v>980</v>
+      </c>
+      <c r="B330" s="60">
         <v>3.0</v>
       </c>
-      <c r="C330" s="59">
+      <c r="C330" s="60">
         <v>3.0</v>
       </c>
     </row>
     <row r="331" ht="15.75" customHeight="1">
       <c r="A331" s="40" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="B331" s="40" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="C331" s="40" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
     </row>
     <row r="332" ht="15.75" customHeight="1">
       <c r="A332" s="40" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B332" s="40" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="C332" s="40" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
     </row>
     <row r="333" ht="15.75" customHeight="1">
       <c r="A333" s="40" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="B333" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C333" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="334" ht="15.75" customHeight="1">
       <c r="A334" s="40" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="B334" s="40" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="C334" s="40" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
     </row>
     <row r="335" ht="15.75" customHeight="1">
       <c r="A335" s="40" t="s">
-        <v>987</v>
-      </c>
-      <c r="B335" s="59">
+        <v>988</v>
+      </c>
+      <c r="B335" s="60">
         <v>3.0</v>
       </c>
-      <c r="C335" s="59">
+      <c r="C335" s="60">
         <v>3.0</v>
       </c>
     </row>
     <row r="336" ht="15.75" customHeight="1">
       <c r="A336" s="40" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B336" s="40" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C336" s="40" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
     </row>
     <row r="337" ht="15.75" customHeight="1">
       <c r="A337" s="40" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="B337" s="40" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="C337" s="40" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
     </row>
     <row r="338" ht="15.75" customHeight="1">
       <c r="A338" s="40" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B338" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C338" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="339" ht="15.75" customHeight="1">
       <c r="A339" s="40" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B339" s="40" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C339" s="40" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
     </row>
     <row r="340" ht="15.75" customHeight="1">
       <c r="A340" s="40" t="s">
-        <v>995</v>
-      </c>
-      <c r="B340" s="59">
+        <v>996</v>
+      </c>
+      <c r="B340" s="60">
         <v>3.0</v>
       </c>
-      <c r="C340" s="59">
+      <c r="C340" s="60">
         <v>3.0</v>
       </c>
     </row>
     <row r="341" ht="15.75" customHeight="1">
       <c r="A341" s="40" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B341" s="40" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="C341" s="40" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
     </row>
     <row r="342" ht="15.75" customHeight="1">
       <c r="A342" s="40" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B342" s="40" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C342" s="40" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="343" ht="15.75" customHeight="1">
       <c r="A343" s="40" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="B343" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C343" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="344" ht="15.75" customHeight="1">
       <c r="A344" s="40" t="s">
-        <v>1001</v>
-      </c>
-      <c r="B344" s="58" t="s">
         <v>1002</v>
       </c>
-      <c r="C344" s="58" t="s">
-        <v>1002</v>
+      <c r="B344" s="59" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C344" s="59" t="s">
+        <v>1003</v>
       </c>
     </row>
     <row r="345" ht="15.75" customHeight="1">
       <c r="A345" s="40" t="s">
-        <v>1003</v>
-      </c>
-      <c r="B345" s="59">
+        <v>1004</v>
+      </c>
+      <c r="B345" s="60">
         <v>3.0</v>
       </c>
-      <c r="C345" s="59">
+      <c r="C345" s="60">
         <v>3.0</v>
       </c>
     </row>
     <row r="346" ht="15.75" customHeight="1">
       <c r="A346" s="40" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B346" s="40" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C346" s="40" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="347" ht="15.75" customHeight="1">
       <c r="A347" s="40" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="B347" s="40" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="C347" s="40" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="348" ht="15.75" customHeight="1">
       <c r="A348" s="40" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B348" s="40" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="C348" s="40" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="349" ht="15.75" customHeight="1">
       <c r="A349" s="40" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B349" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C349" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="350" ht="15.75" customHeight="1">
       <c r="A350" s="40" t="s">
-        <v>1011</v>
-      </c>
-      <c r="B350" s="59" t="s">
         <v>1012</v>
       </c>
-      <c r="C350" s="59" t="s">
-        <v>1012</v>
+      <c r="B350" s="60" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C350" s="60" t="s">
+        <v>1013</v>
       </c>
     </row>
     <row r="351" ht="15.75" customHeight="1">
       <c r="A351" s="40" t="s">
-        <v>1013</v>
-      </c>
-      <c r="B351" s="59">
+        <v>1014</v>
+      </c>
+      <c r="B351" s="60">
         <v>6.0</v>
       </c>
-      <c r="C351" s="59">
+      <c r="C351" s="60">
         <v>6.0</v>
       </c>
     </row>
     <row r="352" ht="15.75" customHeight="1">
       <c r="A352" s="40" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B352" s="40" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C352" s="40" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="353" ht="15.75" customHeight="1">
       <c r="A353" s="40" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B353" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C353" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="354" ht="15.75" customHeight="1">
       <c r="A354" s="40" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B354" s="40" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="C354" s="40" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="355" ht="15.75" customHeight="1">
       <c r="A355" s="40" t="s">
-        <v>1019</v>
-      </c>
-      <c r="B355" s="59">
+        <v>1020</v>
+      </c>
+      <c r="B355" s="60">
         <v>50.0</v>
       </c>
-      <c r="C355" s="59">
+      <c r="C355" s="60">
         <v>50.0</v>
       </c>
     </row>
     <row r="356" ht="15.75" customHeight="1">
       <c r="A356" s="40" t="s">
-        <v>1020</v>
-      </c>
-      <c r="B356" s="59">
+        <v>1021</v>
+      </c>
+      <c r="B356" s="60">
         <v>55.0</v>
       </c>
-      <c r="C356" s="59">
+      <c r="C356" s="60">
         <v>55.0</v>
       </c>
     </row>
     <row r="357" ht="15.75" customHeight="1">
       <c r="A357" s="40" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B357" s="40" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="C357" s="40" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="358" ht="15.75" customHeight="1">
       <c r="A358" s="40" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B358" s="40" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C358" s="40" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
     </row>
     <row r="359" ht="15.75" customHeight="1">
       <c r="A359" s="40" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B359" s="40" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C359" s="40" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="360" ht="15.75" customHeight="1">
       <c r="A360" s="40" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B360" s="40" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="C360" s="40" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="361" ht="15.75" customHeight="1">
       <c r="A361" s="40" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B361" s="40" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C361" s="40" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
     <row r="362" ht="15.75" customHeight="1">
       <c r="A362" s="40" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B362" s="40" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C362" s="40" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
     </row>
     <row r="363" ht="15.75" customHeight="1">
       <c r="A363" s="40" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B363" s="40" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="C363" s="40" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="364" ht="15.75" customHeight="1">
       <c r="A364" s="40" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B364" s="40" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C364" s="40" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="365" ht="15.75" customHeight="1">
       <c r="A365" s="40" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B365" s="40" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="C365" s="40" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="366" ht="15.75" customHeight="1">
       <c r="A366" s="40" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B366" s="40" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="C366" s="40" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="367" ht="15.75" customHeight="1">
       <c r="A367" s="40" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B367" s="40" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="C367" s="40" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="368" ht="15.75" customHeight="1">
       <c r="A368" s="40" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B368" s="40" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="C368" s="40" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="369" ht="15.75" customHeight="1">
       <c r="A369" s="40" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B369" s="40" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="C369" s="40" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="370" ht="15.75" customHeight="1">
       <c r="A370" s="40" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="B370" s="40" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="C370" s="40" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="371" ht="15.75" customHeight="1">
       <c r="A371" s="40" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="B371" s="40" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="C371" s="40" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="372" ht="15.75" customHeight="1">
       <c r="A372" s="40" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="B372" s="40" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="C372" s="40" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="373" ht="15.75" customHeight="1">
       <c r="A373" s="40" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="B373" s="40" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="C373" s="40" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="374" ht="15.75" customHeight="1"/>
@@ -31522,8 +31528,8 @@
     <row r="377" ht="15.75" customHeight="1"/>
     <row r="378" ht="15.75" customHeight="1"/>
     <row r="379" ht="15.75" customHeight="1">
-      <c r="B379" s="52" t="s">
-        <v>1052</v>
+      <c r="B379" s="53" t="s">
+        <v>1053</v>
       </c>
     </row>
     <row r="380" ht="15.75" customHeight="1"/>
@@ -31531,596 +31537,596 @@
     <row r="382" ht="15.75" customHeight="1"/>
     <row r="383" ht="15.75" customHeight="1">
       <c r="A383" s="40" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="B383" s="40" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="C383" s="40" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="384" ht="15.75" customHeight="1">
       <c r="A384" s="40" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B384" s="40" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="C384" s="40" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="385" ht="15.75" customHeight="1">
       <c r="A385" s="40" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B385" s="40" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="C385" s="40" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="386" ht="15.75" customHeight="1">
       <c r="A386" s="40" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="B386" s="40" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="C386" s="40" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="387" ht="15.75" customHeight="1">
       <c r="A387" s="40" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B387" s="40" t="s">
         <v>1061</v>
       </c>
-      <c r="B387" s="40" t="s">
-        <v>1060</v>
-      </c>
       <c r="C387" s="40" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="388" ht="15.75" customHeight="1">
       <c r="A388" s="40" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="B388" s="40" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="C388" s="40" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="389" ht="15.75" customHeight="1"/>
     <row r="390" ht="15.75" customHeight="1">
-      <c r="B390" s="52" t="s">
-        <v>1064</v>
+      <c r="B390" s="53" t="s">
+        <v>1065</v>
       </c>
     </row>
     <row r="391" ht="15.75" customHeight="1"/>
     <row r="392" ht="15.75" customHeight="1"/>
     <row r="393" ht="15.75" customHeight="1">
       <c r="A393" s="40" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="B393" s="40" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="C393" s="40" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="394" ht="15.75" customHeight="1">
       <c r="A394" s="40" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="B394" s="40" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="C394" s="40" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="395" ht="15.75" customHeight="1">
       <c r="A395" s="40" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="B395" s="40" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="C395" s="40" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="396" ht="15.75" customHeight="1">
       <c r="A396" s="40" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="B396" s="40" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="C396" s="40" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="397" ht="15.75" customHeight="1">
       <c r="A397" s="40" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B397" s="40" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="C397" s="40" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="398" ht="15.75" customHeight="1">
       <c r="A398" s="40" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B398" s="40" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="C398" s="40" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="399" ht="15.75" customHeight="1">
       <c r="A399" s="40" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B399" s="40" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="C399" s="40" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="400" ht="15.75" customHeight="1">
       <c r="A400" s="40" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="B400" s="40" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="C400" s="40" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="401" ht="15.75" customHeight="1">
       <c r="A401" s="40" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="B401" s="40" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="C401" s="40" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="402" ht="15.75" customHeight="1">
       <c r="A402" s="40" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="B402" s="40" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="C402" s="40" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="403" ht="15.75" customHeight="1">
       <c r="A403" s="40" t="s">
-        <v>1085</v>
+        <v>1086</v>
       </c>
       <c r="B403" s="40" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
       <c r="C403" s="40" t="s">
-        <v>1086</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="404" ht="15.75" customHeight="1">
       <c r="A404" s="40" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B404" s="40" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="C404" s="40" t="s">
-        <v>1088</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="405" ht="15.75" customHeight="1">
       <c r="A405" s="40" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B405" s="40" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="C405" s="40" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="406" ht="15.75" customHeight="1">
       <c r="A406" s="40" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B406" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C406" s="40" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="407" ht="15.75" customHeight="1">
       <c r="A407" s="40" t="s">
-        <v>1092</v>
+        <v>1093</v>
       </c>
       <c r="B407" s="40" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="C407" s="40" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="408" ht="15.75" customHeight="1">
       <c r="A408" s="40" t="s">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="B408" s="40" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="C408" s="40" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="409" ht="15.75" customHeight="1">
       <c r="A409" s="40" t="s">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="B409" s="40" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="C409" s="40" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="410" ht="15.75" customHeight="1">
       <c r="A410" s="40" t="s">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="B410" s="40" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="C410" s="40" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="411" ht="15.75" customHeight="1">
       <c r="A411" s="40" t="s">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B411" s="40" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="C411" s="40" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="412" ht="15.75" customHeight="1">
       <c r="A412" s="40" t="s">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B412" s="40" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="C412" s="40" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="413" ht="15.75" customHeight="1">
       <c r="A413" s="40" t="s">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="B413" s="40" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="C413" s="40" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="414" ht="15.75" customHeight="1">
       <c r="A414" s="40" t="s">
-        <v>1106</v>
+        <v>1107</v>
       </c>
       <c r="B414" s="40" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="C414" s="40" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="415" ht="15.75" customHeight="1">
       <c r="A415" s="40" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
       <c r="B415" s="40" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="C415" s="40" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="416" ht="15.75" customHeight="1">
       <c r="A416" s="40" t="s">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="B416" s="40" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="C416" s="40" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="417" ht="15.75" customHeight="1">
       <c r="A417" s="40" t="s">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="B417" s="40" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="C417" s="40" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="418" ht="15.75" customHeight="1">
       <c r="A418" s="40" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="B418" s="40" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="C418" s="40" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="419" ht="15.75" customHeight="1">
       <c r="A419" s="40" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="B419" s="40" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="C419" s="40" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="420" ht="15.75" customHeight="1">
       <c r="A420" s="40" t="s">
-        <v>1118</v>
+        <v>1119</v>
       </c>
       <c r="B420" s="40" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="C420" s="40" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="421" ht="15.75" customHeight="1">
       <c r="A421" s="40" t="s">
-        <v>1120</v>
+        <v>1121</v>
       </c>
       <c r="B421" s="40" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="C421" s="40" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="422" ht="15.75" customHeight="1">
       <c r="A422" s="40" t="s">
-        <v>1122</v>
+        <v>1123</v>
       </c>
       <c r="B422" s="40" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="C422" s="40" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="423" ht="15.75" customHeight="1">
       <c r="A423" s="40" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="B423" s="40" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="C423" s="40" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="424" ht="15.75" customHeight="1">
       <c r="A424" s="40" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="B424" s="40" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="C424" s="40" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="425" ht="15.75" customHeight="1">
       <c r="A425" s="40" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="B425" s="40" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
       <c r="C425" s="40" t="s">
-        <v>1129</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="426" ht="15.75" customHeight="1">
       <c r="A426" s="13" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="C426" s="13" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="427" ht="15.75" customHeight="1"/>
     <row r="428" ht="15.75" customHeight="1">
       <c r="A428" s="40" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="B428" s="40" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="C428" s="40" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="429" ht="15.75" customHeight="1">
       <c r="A429" s="40" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="B429" s="40" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="C429" s="40" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="430" ht="15.75" customHeight="1">
       <c r="A430" s="40" t="s">
-        <v>1136</v>
+        <v>1137</v>
       </c>
       <c r="B430" s="40" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="C430" s="40" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="431" ht="15.75" customHeight="1">
       <c r="A431" s="40" t="s">
-        <v>1138</v>
+        <v>1139</v>
       </c>
       <c r="B431" s="40" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="C431" s="40" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="432" ht="15.75" customHeight="1">
       <c r="A432" s="40" t="s">
-        <v>1140</v>
+        <v>1141</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
       <c r="C432" s="13" t="s">
-        <v>1141</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="433" ht="15.75" customHeight="1"/>
     <row r="434" ht="15.75" customHeight="1">
       <c r="A434" s="40" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="B434" s="40" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="C434" s="40" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="435" ht="15.75" customHeight="1">
       <c r="A435" s="40" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="B435" s="40" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="C435" s="40" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="436" ht="15.75" customHeight="1">
       <c r="A436" s="40" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="B436" s="40" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="C436" s="40" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="437" ht="15.75" customHeight="1">
       <c r="A437" s="40" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="B437" s="40" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="C437" s="40" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="438" ht="15.75" customHeight="1">
       <c r="A438" s="40" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="B438" s="40" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="C438" s="40" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="439" ht="15.75" customHeight="1">
       <c r="A439" s="13" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="B439" s="13" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="C439" s="13" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="440" ht="15.75" customHeight="1">
-      <c r="B440" s="52" t="s">
-        <v>1154</v>
+      <c r="B440" s="53" t="s">
+        <v>1155</v>
       </c>
     </row>
     <row r="441" ht="15.75" customHeight="1"/>
     <row r="442" ht="15.75" customHeight="1"/>
     <row r="443" ht="15.75" customHeight="1">
       <c r="A443" s="40" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="B443" s="40" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="C443" s="40" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="444" ht="15.75" customHeight="1">
       <c r="A444" s="40" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="B444" s="40" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Repeat Script Settings script update(12/05/23)
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Provider_Script_28_02_23\config\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B64AF8-213E-4761-A612-EA495F7E35AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Happy_Path_Patient_Web_and_MR" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="1113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="1113">
   <si>
     <t>KEY</t>
   </si>
@@ -3364,7 +3370,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="30">
     <font>
       <sz val="11"/>
@@ -3962,11 +3968,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -16307,11 +16313,11 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C132" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
-    <hyperlink ref="B132" r:id="rId4"/>
-    <hyperlink ref="B138" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C132" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B132" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B138" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -16319,7 +16325,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -25752,7 +25758,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B128" r:id="rId1"/>
+    <hyperlink ref="B128" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -25760,14 +25766,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -27022,23 +27028,43 @@
       </c>
     </row>
     <row r="143" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="144" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="144" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A144" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A145" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="147" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="148" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="149" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="150" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="151" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="152" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="153" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="154" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="155" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="156" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="157" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="158" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="159" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="160" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="161" ht="15.75" customHeight="1"/>
     <row r="162" ht="15.75" customHeight="1"/>
     <row r="163" ht="15.75" customHeight="1"/>
@@ -27881,13 +27907,13 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="B31" r:id="rId3"/>
-    <hyperlink ref="C31" r:id="rId4"/>
-    <hyperlink ref="B46" r:id="rId5"/>
-    <hyperlink ref="C46" r:id="rId6"/>
-    <hyperlink ref="C47" r:id="rId7"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B31" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="C31" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B46" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="C46" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="C47" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId8"/>
@@ -27895,7 +27921,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -32400,15 +32426,15 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="B20" r:id="rId3"/>
-    <hyperlink ref="C20" r:id="rId4"/>
-    <hyperlink ref="C75" r:id="rId5"/>
-    <hyperlink ref="B193" r:id="rId6"/>
-    <hyperlink ref="C193" r:id="rId7"/>
-    <hyperlink ref="B194" r:id="rId8"/>
-    <hyperlink ref="C194" r:id="rId9"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="B20" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="C20" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="C75" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="B193" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="C193" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="B194" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="C194" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
HappyPath_MR&Web and Sanity Pack Stable for V4.4.8(14/06/23)
</commit_message>
<xml_diff>
--- a/config/testdata/testdata.xlsx
+++ b/config/testdata/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23190" windowHeight="10230"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23190" windowHeight="10230" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Happy_Path_Patient_Web_and_MR" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="1145">
   <si>
     <t>KEY</t>
   </si>
@@ -2134,27 +2134,18 @@
     <t>VERIFY_DASHBOARD_MESSAGE_1</t>
   </si>
   <si>
-    <t>, Dr Tim;Dashboard Msg Testing1_RANDOM</t>
-  </si>
-  <si>
     <t>Dr Tim;Dashboard Msg Testing1_RANDOM</t>
   </si>
   <si>
     <t>VERIFY_DASHBOARD_MESSAGE_2</t>
   </si>
   <si>
-    <t>, Dr Tim;Dashboard Msg Testing2_RANDOM</t>
-  </si>
-  <si>
     <t>Dr Tim;Dashboard Msg Testing2_RANDOM</t>
   </si>
   <si>
     <t>VERIFY_DASHBOARD_MESSAGE_3</t>
   </si>
   <si>
-    <t>, Dr Tim;Dashboard Msg Testing3_RANDOM</t>
-  </si>
-  <si>
     <t>Dr Tim;Dashboard Msg Testing3_RANDOM</t>
   </si>
   <si>
@@ -3169,9 +3160,6 @@
     <t>AstraZ/Covishield -1;10/05/2023 12:08:54 AM;Given Elsewhere NZ;test;Intra Muscular;Left Arm;GP1;Automation_Practice1_Loc1</t>
   </si>
   <si>
-    <t>10 May 2023;Skin/subcutaneous tissu diseas;zskin problem;Yes;Automation_Practice1_Loc1;10 May 2023 12:08:43 AM</t>
-  </si>
-  <si>
     <t>09 May 2023;Consult In Surgery;GP1;Automation_Practice1_Loc1;09 May 2023 06:48:16 PM</t>
   </si>
   <si>
@@ -3370,12 +3358,6 @@
     <t>Skin/subcutaneous tissu diseas;10/05/2023 06:08:13 PM;Yes;GP1;Automation_Practice1_Loc1</t>
   </si>
   <si>
-    <t>Automation_Practice1_Loc1;lanoxin pg 62.5mcg tab(digoxin);pending;ZOOM Pharmacy home delivery;48 Hours;48 Hours;</t>
-  </si>
-  <si>
-    <t>Automation_Practice1_Loc1;lanoxin pg 62.5mcg tab(digoxin);pending;ZOOM Pharmacy home delivery;48 Hours;48 Hours</t>
-  </si>
-  <si>
     <t>1 tabs, Once Daily, 2 weeks;14;14;1;System Administrator;Automation_Practice1_Loc1</t>
   </si>
   <si>
@@ -3395,13 +3377,91 @@
   </si>
   <si>
     <t>Blood Pressure;GP1;Automation_Practice1_Loc1</t>
+  </si>
+  <si>
+    <t>Automation_Practice1_Loc1; lanoxin pg 62.5mcg tab(digoxin);pending;Next Day;GP1</t>
+  </si>
+  <si>
+    <t>10 May 2023;Skin/subcutaneous tissu diseas;zskin problem;Yes;Automation_Practice1_Loc1;10 May 2023 06:08:13 PM</t>
+  </si>
+  <si>
+    <t>Manage@1234</t>
+  </si>
+  <si>
+    <t>8508250222;9095337244;9862512345</t>
+  </si>
+  <si>
+    <t>8508250222;9862512345;9977612345;Companion</t>
+  </si>
+  <si>
+    <t>Automation_Practice1_Loc1;First Name Last Name;Auto Pat1</t>
+  </si>
+  <si>
+    <t>Automation_Practice1_Loc1</t>
+  </si>
+  <si>
+    <t>Automation_Practice1_Loc1;Post to notice board;Post Header;Notice Board Tesing_RANDOM</t>
+  </si>
+  <si>
+    <t>Test_RANDOM;Consent Form;MMHtest.jpg;AUTO PAT1</t>
+  </si>
+  <si>
+    <t>Test_RANDOM;Consent Form;MMHtest.jpg;AUTO PAT1;QA Testing For keep this Private</t>
+  </si>
+  <si>
+    <t>Test_RANDOM;Discharge Letter;MMHtest.jpg;AUTO PAT1;Test_RANDOM;Show this entry to my care providers</t>
+  </si>
+  <si>
+    <t>Test_RANDOM;Discharge Letter;MMHtest.jpg;AUTO PAT1;QA Testing For Share with Provider</t>
+  </si>
+  <si>
+    <t>GP1;Dashboard Msg Testing1_RANDOM</t>
+  </si>
+  <si>
+    <t>GP1;Dashboard Msg Testing3_RANDOM</t>
+  </si>
+  <si>
+    <t>GP1;Dashboard Msg Testing2_RANDOM</t>
+  </si>
+  <si>
+    <t>Lab Result1;10 May 2023 6:10 PM;10 May 2023</t>
+  </si>
+  <si>
+    <t>Consult In Surgery;10 May 2023 6:08 PM;10 May 2023</t>
+  </si>
+  <si>
+    <t>Skin/subcutaneous tissu diseas;10 May 2023 6:08 PM;10 May 2023</t>
+  </si>
+  <si>
+    <t>Automation_Practice1_Loc1;Pending</t>
+  </si>
+  <si>
+    <t>AFTER_THREE_DAYS;GP1</t>
+  </si>
+  <si>
+    <t>Automation_Practice1_Loc1;Automation_Practice1_Loc1;Automation_Practice1_Loc1</t>
+  </si>
+  <si>
+    <t>Automation_Practice1_Loc1;Automation_Practice1_Loc1;Internal Communication;Patient;Auto Pat1;Received Msg Testing_RANDOM;Body : Received Message Testing_RANDOM;MMHtest.jpg</t>
+  </si>
+  <si>
+    <t>Automation_Practice1_Loc1;Automation_Practice1_Loc1;Internal Communication;Patient;Auto Pat1;Automatic Reply Message Testing_RANDOM;Body : Automatic Reply Message Testing_RANDOM;MMHtest.jpg</t>
+  </si>
+  <si>
+    <t>Automation_Practice1_Loc1;Automation_Practice1_Loc1;Internal Communication;Patient;Auto Pat1;Dashboard Msg Testing1_RANDOM;Body : Dashboard Message Testing1_RANDOM;MMHtest.jpg</t>
+  </si>
+  <si>
+    <t>Automation_Practice1_Loc1;Automation_Practice1_Loc1;Internal Communication;Patient;Auto Pat1;Dashboard Msg Testing2_RANDOM;Body : Dashboard Message Testing2_RANDOM;MMHtest.jpg</t>
+  </si>
+  <si>
+    <t>Automation_Practice1_Loc1;Automation_Practice1_Loc1;Internal Communication;Patient;Auto Pat1;Dashboard Msg Testing3_RANDOM;Body : Dashboard Message Testing3_RANDOM;MMHtest.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3596,6 +3656,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -3688,10 +3754,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3812,8 +3882,12 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4029,8 +4103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B190" workbookViewId="0">
-      <selection activeCell="B195" sqref="B195"/>
+    <sheetView topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104:B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4108,7 +4182,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -4170,7 +4244,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -4201,7 +4275,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -4232,7 +4306,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -4319,7 +4393,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -4350,7 +4424,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>20</v>
@@ -4381,7 +4455,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
@@ -4468,7 +4542,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>23</v>
@@ -4499,7 +4573,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
@@ -4530,7 +4604,7 @@
         <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>14</v>
@@ -4617,7 +4691,7 @@
         <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>27</v>
@@ -4648,7 +4722,7 @@
         <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>29</v>
@@ -4681,7 +4755,7 @@
         <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>14</v>
@@ -4770,7 +4844,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>10</v>
@@ -4801,7 +4875,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>12</v>
@@ -4925,7 +4999,7 @@
         <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>38</v>
@@ -5006,7 +5080,7 @@
         <v>39</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>40</v>
@@ -5037,7 +5111,7 @@
         <v>41</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>42</v>
@@ -5149,7 +5223,7 @@
         <v>45</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>40</v>
@@ -5205,7 +5279,7 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>47</v>
@@ -5292,7 +5366,7 @@
         <v>49</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>50</v>
@@ -5323,7 +5397,7 @@
         <v>51</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>1113</v>
+        <v>1119</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>52</v>
@@ -5354,7 +5428,7 @@
         <v>53</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>54</v>
@@ -5435,7 +5509,7 @@
         <v>55</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>56</v>
@@ -5466,7 +5540,7 @@
         <v>57</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>58</v>
@@ -5497,7 +5571,7 @@
         <v>59</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>1069</v>
+        <v>1065</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>60</v>
@@ -5577,7 +5651,7 @@
         <v>61</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>62</v>
@@ -5608,7 +5682,7 @@
         <v>63</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>64</v>
@@ -5639,7 +5713,7 @@
         <v>65</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>66</v>
@@ -5720,7 +5794,7 @@
         <v>67</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>68</v>
@@ -5751,7 +5825,7 @@
         <v>69</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>1116</v>
+        <v>1054</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>70</v>
@@ -5782,7 +5856,7 @@
         <v>71</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>72</v>
@@ -5863,7 +5937,7 @@
         <v>73</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>68</v>
@@ -5894,7 +5968,7 @@
         <v>74</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>1117</v>
+        <v>1054</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>70</v>
@@ -5975,7 +6049,7 @@
         <v>75</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>68</v>
@@ -6006,7 +6080,7 @@
         <v>76</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>1117</v>
+        <v>1054</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>70</v>
@@ -6149,7 +6223,7 @@
         <v>81</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>82</v>
@@ -6211,7 +6285,7 @@
         <v>85</v>
       </c>
       <c r="B75" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>47</v>
@@ -6273,7 +6347,7 @@
         <v>87</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>88</v>
@@ -6304,7 +6378,7 @@
         <v>89</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>90</v>
@@ -6335,7 +6409,7 @@
         <v>91</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>92</v>
@@ -6397,7 +6471,7 @@
         <v>95</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>96</v>
@@ -6425,7 +6499,7 @@
         <v>97</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>1049</v>
+        <v>1120</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>98</v>
@@ -6450,7 +6524,7 @@
         <v>99</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>100</v>
@@ -6478,7 +6552,7 @@
         <v>101</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>102</v>
@@ -6503,7 +6577,7 @@
         <v>103</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>104</v>
@@ -6531,7 +6605,7 @@
         <v>105</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>106</v>
@@ -6562,7 +6636,7 @@
         <v>107</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>108</v>
@@ -6590,7 +6664,7 @@
         <v>109</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>110</v>
@@ -6637,7 +6711,7 @@
         <v>111</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>112</v>
@@ -7100,7 +7174,7 @@
         <v>146</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>147</v>
@@ -7128,7 +7202,7 @@
         <v>148</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>149</v>
@@ -7159,7 +7233,7 @@
         <v>150</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>151</v>
@@ -7898,7 +7972,7 @@
         <v>190</v>
       </c>
       <c r="B133" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="C133" s="12" t="s">
         <v>191</v>
@@ -7960,7 +8034,7 @@
         <v>193</v>
       </c>
       <c r="B135" s="7" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>194</v>
@@ -7991,7 +8065,7 @@
         <v>195</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>196</v>
@@ -8022,7 +8096,7 @@
         <v>197</v>
       </c>
       <c r="B137" s="7" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
       <c r="C137" s="7" t="s">
         <v>198</v>
@@ -8084,7 +8158,7 @@
         <v>201</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>202</v>
@@ -8115,7 +8189,7 @@
         <v>203</v>
       </c>
       <c r="B140" s="14" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>196</v>
@@ -8252,7 +8326,7 @@
         <v>207</v>
       </c>
       <c r="B145" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="C145" s="15" t="s">
         <v>6</v>
@@ -8492,7 +8566,7 @@
         <v>219</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>220</v>
@@ -8608,7 +8682,7 @@
         <v>225</v>
       </c>
       <c r="B157" s="16" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="C157" s="16" t="s">
         <v>226</v>
@@ -8670,7 +8744,7 @@
         <v>229</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="C159" s="7" t="s">
         <v>230</v>
@@ -8732,7 +8806,7 @@
         <v>233</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="C161" s="7" t="s">
         <v>234</v>
@@ -8850,7 +8924,7 @@
         <v>190</v>
       </c>
       <c r="B165" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="C165" s="12" t="s">
         <v>191</v>
@@ -8937,7 +9011,7 @@
         <v>241</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>1118</v>
+        <v>1112</v>
       </c>
       <c r="C168" s="7" t="s">
         <v>242</v>
@@ -9092,7 +9166,7 @@
         <v>251</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>1119</v>
+        <v>1113</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>252</v>
@@ -9216,7 +9290,7 @@
         <v>259</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>1120</v>
+        <v>1114</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>260</v>
@@ -9371,7 +9445,7 @@
         <v>269</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>1121</v>
+        <v>1115</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>270</v>
@@ -9495,7 +9569,7 @@
         <v>277</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>1122</v>
+        <v>1116</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>278</v>
@@ -9557,7 +9631,7 @@
         <v>280</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>151</v>
@@ -9619,7 +9693,7 @@
         <v>282</v>
       </c>
       <c r="B190" s="7" t="s">
-        <v>1123</v>
+        <v>1117</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>283</v>
@@ -9774,7 +9848,7 @@
         <v>291</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>1124</v>
+        <v>1118</v>
       </c>
       <c r="C195" s="7" t="s">
         <v>292</v>
@@ -25869,7 +25943,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>191</v>
@@ -25903,7 +25977,7 @@
         <v>488</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>489</v>
@@ -25914,7 +25988,7 @@
         <v>490</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>491</v>
@@ -25925,7 +25999,7 @@
         <v>492</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>493</v>
@@ -25936,7 +26010,7 @@
         <v>494</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>495</v>
@@ -25947,7 +26021,7 @@
         <v>496</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>497</v>
@@ -25958,7 +26032,7 @@
         <v>498</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="C13" s="21" t="s">
         <v>499</v>
@@ -25969,7 +26043,7 @@
         <v>500</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>501</v>
@@ -26002,7 +26076,7 @@
         <v>506</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>507</v>
@@ -26013,7 +26087,7 @@
         <v>508</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>509</v>
@@ -26024,7 +26098,7 @@
         <v>510</v>
       </c>
       <c r="B19" s="60" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>511</v>
@@ -26046,7 +26120,7 @@
         <v>514</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="C21" s="21" t="s">
         <v>515</v>
@@ -26073,7 +26147,7 @@
         <v>315</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>316</v>
@@ -26089,7 +26163,7 @@
         <v>317</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>318</v>
@@ -26133,7 +26207,7 @@
         <v>520</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>521</v>
@@ -26144,7 +26218,7 @@
         <v>522</v>
       </c>
       <c r="B33" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="C33" s="27" t="s">
         <v>47</v>
@@ -26155,7 +26229,7 @@
         <v>49</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>523</v>
@@ -26166,7 +26240,7 @@
         <v>51</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>52</v>
@@ -26202,7 +26276,7 @@
         <v>67</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>68</v>
@@ -26216,7 +26290,7 @@
         <v>69</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>70</v>
@@ -26241,7 +26315,7 @@
         <v>526</v>
       </c>
       <c r="B44" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>6</v>
@@ -26268,7 +26342,7 @@
         <v>527</v>
       </c>
       <c r="B47" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>6</v>
@@ -26497,7 +26571,7 @@
         <v>556</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>557</v>
@@ -26633,21 +26707,21 @@
     <row r="88" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="89" spans="1:3" ht="15.75" customHeight="1">
       <c r="A89" s="12" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
       <c r="B89" s="21" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
       <c r="C89" s="21" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15.75" customHeight="1">
       <c r="A90" s="12" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>578</v>
@@ -26683,7 +26757,7 @@
         <v>582</v>
       </c>
       <c r="B96" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="C96" s="33" t="s">
         <v>6</v>
@@ -26710,7 +26784,7 @@
         <v>583</v>
       </c>
       <c r="B99" s="32" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="C99" s="32" t="s">
         <v>584</v>
@@ -26721,7 +26795,7 @@
         <v>585</v>
       </c>
       <c r="B100" s="32" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="C100" s="32" t="s">
         <v>586</v>
@@ -26737,7 +26811,7 @@
         <v>587</v>
       </c>
       <c r="B102" s="32" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
       <c r="C102" s="32" t="s">
         <v>588</v>
@@ -26759,7 +26833,7 @@
         <v>590</v>
       </c>
       <c r="B104" s="32" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="C104" s="32" t="s">
         <v>591</v>
@@ -26873,7 +26947,7 @@
         <v>9</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="C118" s="12" t="s">
         <v>10</v>
@@ -27002,7 +27076,7 @@
         <v>11</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>12</v>
@@ -27024,7 +27098,7 @@
         <v>13</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="C137" s="32" t="s">
         <v>14</v>
@@ -27035,7 +27109,7 @@
         <v>39</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="C138" s="37" t="s">
         <v>40</v>
@@ -27046,10 +27120,10 @@
         <v>620</v>
       </c>
       <c r="B139" s="37" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="C139" s="37" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="15.75" customHeight="1">
@@ -27113,7 +27187,7 @@
         <v>61</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>62</v>
@@ -27125,7 +27199,7 @@
         <v>55</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>56</v>
@@ -28005,8 +28079,8 @@
   </sheetPr>
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A313" sqref="A313"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -28063,8 +28137,8 @@
       <c r="A3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>6</v>
+      <c r="B3" t="s">
+        <v>1039</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>6</v>
@@ -28090,8 +28164,8 @@
       <c r="A10" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>47</v>
+      <c r="B10" t="s">
+        <v>1039</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>47</v>
@@ -28108,23 +28182,23 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="30">
+    <row r="13" spans="1:23" ht="26.25">
       <c r="A13" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="B13" s="27" t="s">
-        <v>622</v>
+      <c r="B13" s="7" t="s">
+        <v>1058</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="30">
+    <row r="14" spans="1:23" ht="26.25">
       <c r="A14" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="B14" s="27" t="s">
-        <v>623</v>
+      <c r="B14" s="7" t="s">
+        <v>1060</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>623</v>
@@ -28135,7 +28209,7 @@
         <v>624</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>623</v>
+        <v>1060</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>623</v>
@@ -28145,8 +28219,8 @@
       <c r="A16" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="B16" s="27" t="s">
-        <v>196</v>
+      <c r="B16" s="1" t="s">
+        <v>1059</v>
       </c>
       <c r="C16" s="27" t="s">
         <v>196</v>
@@ -28157,7 +28231,7 @@
         <v>462</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>625</v>
+        <v>1140</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>625</v>
@@ -28167,8 +28241,8 @@
       <c r="A18" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>191</v>
+      <c r="B18" t="s">
+        <v>1057</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>191</v>
@@ -28201,7 +28275,7 @@
         <v>229</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>626</v>
+        <v>1062</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>626</v>
@@ -28222,8 +28296,8 @@
       <c r="A23" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="B23" s="27" t="s">
-        <v>220</v>
+      <c r="B23" s="7" t="s">
+        <v>1063</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>220</v>
@@ -28234,7 +28308,7 @@
         <v>233</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>627</v>
+        <v>1141</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>627</v>
@@ -28273,8 +28347,8 @@
       <c r="A30" s="27" t="s">
         <v>630</v>
       </c>
-      <c r="B30" s="27" t="s">
-        <v>47</v>
+      <c r="B30" t="s">
+        <v>1039</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>47</v>
@@ -28296,8 +28370,8 @@
       <c r="A33" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="42" t="s">
-        <v>632</v>
+      <c r="B33" s="1" t="s">
+        <v>1070</v>
       </c>
       <c r="C33" s="42" t="s">
         <v>632</v>
@@ -28307,8 +28381,8 @@
       <c r="A34" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="42" t="s">
-        <v>12</v>
+      <c r="B34" s="1" t="s">
+        <v>1071</v>
       </c>
       <c r="C34" s="42" t="s">
         <v>12</v>
@@ -28318,8 +28392,8 @@
       <c r="A35" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="42" t="s">
-        <v>14</v>
+      <c r="B35" s="1" t="s">
+        <v>1072</v>
       </c>
       <c r="C35" s="42" t="s">
         <v>14</v>
@@ -28329,7 +28403,7 @@
       <c r="A36" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C36" s="42" t="s">
@@ -28341,8 +28415,8 @@
       <c r="A38" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B38" s="42" t="s">
-        <v>633</v>
+      <c r="B38" s="1" t="s">
+        <v>1073</v>
       </c>
       <c r="C38" s="42" t="s">
         <v>633</v>
@@ -28352,8 +28426,8 @@
       <c r="A39" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="42" t="s">
-        <v>20</v>
+      <c r="B39" s="1" t="s">
+        <v>1074</v>
       </c>
       <c r="C39" s="42" t="s">
         <v>20</v>
@@ -28363,8 +28437,8 @@
       <c r="A40" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="42" t="s">
-        <v>14</v>
+      <c r="B40" s="1" t="s">
+        <v>1072</v>
       </c>
       <c r="C40" s="42" t="s">
         <v>14</v>
@@ -28374,7 +28448,7 @@
       <c r="A41" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="42" t="s">
+      <c r="B41" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C41" s="42" t="s">
@@ -28386,8 +28460,8 @@
       <c r="A43" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="42" t="s">
-        <v>634</v>
+      <c r="B43" s="1" t="s">
+        <v>1075</v>
       </c>
       <c r="C43" s="42" t="s">
         <v>634</v>
@@ -28397,8 +28471,8 @@
       <c r="A44" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B44" s="42" t="s">
-        <v>12</v>
+      <c r="B44" s="1" t="s">
+        <v>1071</v>
       </c>
       <c r="C44" s="42" t="s">
         <v>12</v>
@@ -28408,8 +28482,8 @@
       <c r="A45" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B45" s="42" t="s">
-        <v>14</v>
+      <c r="B45" s="1" t="s">
+        <v>1072</v>
       </c>
       <c r="C45" s="42" t="s">
         <v>14</v>
@@ -28419,7 +28493,7 @@
       <c r="A46" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="42" t="s">
+      <c r="B46" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C46" s="42" t="s">
@@ -28431,8 +28505,8 @@
       <c r="A48" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="42" t="s">
-        <v>635</v>
+      <c r="B48" s="1" t="s">
+        <v>1076</v>
       </c>
       <c r="C48" s="42" t="s">
         <v>635</v>
@@ -28442,8 +28516,8 @@
       <c r="A49" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="42" t="s">
-        <v>29</v>
+      <c r="B49" s="1" t="s">
+        <v>1077</v>
       </c>
       <c r="C49" s="42" t="s">
         <v>29</v>
@@ -28453,8 +28527,8 @@
       <c r="A50" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B50" s="42" t="s">
-        <v>14</v>
+      <c r="B50" s="1" t="s">
+        <v>1072</v>
       </c>
       <c r="C50" s="42" t="s">
         <v>14</v>
@@ -28464,7 +28538,7 @@
       <c r="A51" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C51" s="42" t="s">
@@ -28476,8 +28550,8 @@
       <c r="A53" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B53" s="42" t="s">
-        <v>632</v>
+      <c r="B53" s="1" t="s">
+        <v>1070</v>
       </c>
       <c r="C53" s="42" t="s">
         <v>632</v>
@@ -28487,8 +28561,8 @@
       <c r="A54" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B54" s="42" t="s">
-        <v>12</v>
+      <c r="B54" s="1" t="s">
+        <v>1071</v>
       </c>
       <c r="C54" s="42" t="s">
         <v>12</v>
@@ -28498,7 +28572,7 @@
       <c r="A55" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B55" s="42" t="s">
+      <c r="B55" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C55" s="42" t="s">
@@ -28509,7 +28583,7 @@
       <c r="A56" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="42" t="s">
+      <c r="B56" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C56" s="42" t="s">
@@ -28520,7 +28594,7 @@
       <c r="A57" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C57" s="42" t="s">
@@ -28531,8 +28605,8 @@
       <c r="A58" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B58" s="42" t="s">
-        <v>636</v>
+      <c r="B58" s="1" t="s">
+        <v>1078</v>
       </c>
       <c r="C58" s="42" t="s">
         <v>636</v>
@@ -28544,8 +28618,8 @@
       <c r="A61" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="B61" s="42" t="s">
-        <v>40</v>
+      <c r="B61" s="1" t="s">
+        <v>1079</v>
       </c>
       <c r="C61" s="42" t="s">
         <v>40</v>
@@ -28555,8 +28629,8 @@
       <c r="A62" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="B62" s="42" t="s">
-        <v>42</v>
+      <c r="B62" s="1" t="s">
+        <v>1080</v>
       </c>
       <c r="C62" s="42" t="s">
         <v>42</v>
@@ -28579,8 +28653,8 @@
       <c r="A66" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="B66" s="42" t="s">
-        <v>40</v>
+      <c r="B66" s="1" t="s">
+        <v>1079</v>
       </c>
       <c r="C66" s="42" t="s">
         <v>40</v>
@@ -28614,21 +28688,21 @@
         <v>639</v>
       </c>
       <c r="B76" s="44" t="s">
-        <v>8</v>
+        <v>1121</v>
       </c>
       <c r="C76" s="44" t="s">
-        <v>8</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15" customHeight="1">
       <c r="A77" s="27" t="s">
         <v>640</v>
       </c>
-      <c r="B77" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" s="44" t="s">
-        <v>8</v>
+      <c r="B77" s="62" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C77" s="62" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1"/>
@@ -28648,7 +28722,7 @@
         <v>643</v>
       </c>
       <c r="B80" s="27" t="s">
-        <v>644</v>
+        <v>1122</v>
       </c>
       <c r="C80" s="27" t="s">
         <v>644</v>
@@ -28682,7 +28756,7 @@
         <v>649</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>650</v>
+        <v>1123</v>
       </c>
       <c r="C84" s="27" t="s">
         <v>650</v>
@@ -28729,7 +28803,7 @@
         <v>657</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>658</v>
+        <v>1124</v>
       </c>
       <c r="C91" s="27" t="s">
         <v>658</v>
@@ -28759,8 +28833,8 @@
       <c r="A98" s="27" t="s">
         <v>662</v>
       </c>
-      <c r="B98" s="27" t="s">
-        <v>47</v>
+      <c r="B98" t="s">
+        <v>1039</v>
       </c>
       <c r="C98" s="27" t="s">
         <v>47</v>
@@ -28783,7 +28857,7 @@
         <v>664</v>
       </c>
       <c r="B101" s="27" t="s">
-        <v>538</v>
+        <v>1125</v>
       </c>
       <c r="C101" s="27" t="s">
         <v>538</v>
@@ -28795,7 +28869,7 @@
         <v>665</v>
       </c>
       <c r="B103" s="27" t="s">
-        <v>666</v>
+        <v>1126</v>
       </c>
       <c r="C103" s="27" t="s">
         <v>666</v>
@@ -28824,8 +28898,8 @@
       <c r="A109" s="27" t="s">
         <v>670</v>
       </c>
-      <c r="B109" s="27" t="s">
-        <v>47</v>
+      <c r="B109" t="s">
+        <v>1039</v>
       </c>
       <c r="C109" s="27" t="s">
         <v>47</v>
@@ -28858,8 +28932,8 @@
       <c r="A113" s="27" t="s">
         <v>673</v>
       </c>
-      <c r="B113" s="27" t="s">
-        <v>47</v>
+      <c r="B113" t="s">
+        <v>1039</v>
       </c>
       <c r="C113" s="27" t="s">
         <v>47</v>
@@ -28881,7 +28955,7 @@
         <v>676</v>
       </c>
       <c r="B115" s="27" t="s">
-        <v>677</v>
+        <v>1127</v>
       </c>
       <c r="C115" s="27" t="s">
         <v>677</v>
@@ -28892,7 +28966,7 @@
         <v>678</v>
       </c>
       <c r="B116" s="27" t="s">
-        <v>679</v>
+        <v>1128</v>
       </c>
       <c r="C116" s="27" t="s">
         <v>679</v>
@@ -28915,7 +28989,7 @@
         <v>682</v>
       </c>
       <c r="B119" s="27" t="s">
-        <v>683</v>
+        <v>1129</v>
       </c>
       <c r="C119" s="27" t="s">
         <v>683</v>
@@ -28926,7 +29000,7 @@
         <v>684</v>
       </c>
       <c r="B120" s="27" t="s">
-        <v>685</v>
+        <v>1130</v>
       </c>
       <c r="C120" s="27" t="s">
         <v>685</v>
@@ -28942,8 +29016,8 @@
       <c r="A123" s="27" t="s">
         <v>687</v>
       </c>
-      <c r="B123" s="27" t="s">
-        <v>6</v>
+      <c r="B123" t="s">
+        <v>1039</v>
       </c>
       <c r="C123" s="27" t="s">
         <v>6</v>
@@ -29000,7 +29074,7 @@
         <v>695</v>
       </c>
       <c r="B130" s="27" t="s">
-        <v>696</v>
+        <v>1139</v>
       </c>
       <c r="C130" s="27" t="s">
         <v>696</v>
@@ -29011,7 +29085,7 @@
         <v>697</v>
       </c>
       <c r="B131" s="27" t="s">
-        <v>698</v>
+        <v>1142</v>
       </c>
       <c r="C131" s="27" t="s">
         <v>698</v>
@@ -29022,7 +29096,7 @@
         <v>699</v>
       </c>
       <c r="B132" s="27" t="s">
-        <v>700</v>
+        <v>1143</v>
       </c>
       <c r="C132" s="27" t="s">
         <v>700</v>
@@ -29033,7 +29107,7 @@
         <v>701</v>
       </c>
       <c r="B133" s="27" t="s">
-        <v>702</v>
+        <v>1144</v>
       </c>
       <c r="C133" s="27" t="s">
         <v>702</v>
@@ -29045,148 +29119,148 @@
         <v>703</v>
       </c>
       <c r="B135" s="27" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C135" s="27" t="s">
         <v>704</v>
-      </c>
-      <c r="C135" s="27" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="15.75" customHeight="1">
       <c r="A136" s="27" t="s">
+        <v>705</v>
+      </c>
+      <c r="B136" s="27" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C136" s="27" t="s">
         <v>706</v>
-      </c>
-      <c r="B136" s="27" t="s">
-        <v>707</v>
-      </c>
-      <c r="C136" s="27" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="15.75" customHeight="1">
       <c r="A137" s="27" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B137" s="27" t="s">
-        <v>710</v>
+        <v>1132</v>
       </c>
       <c r="C137" s="27" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="139" spans="1:3" ht="15.75" customHeight="1">
       <c r="A139" s="27" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="B139" s="27" t="s">
-        <v>713</v>
+        <v>1134</v>
       </c>
       <c r="C139" s="27" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="15.75" customHeight="1">
       <c r="A140" s="27" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="B140" s="27" t="s">
-        <v>713</v>
+        <v>1135</v>
       </c>
       <c r="C140" s="27" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="15.75" customHeight="1">
       <c r="A141" s="27" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="B141" s="27" t="s">
-        <v>716</v>
+        <v>1136</v>
       </c>
       <c r="C141" s="27" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="143" spans="1:3" ht="15" customHeight="1">
       <c r="A143" s="27" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="B143" s="27" t="s">
-        <v>718</v>
+        <v>1137</v>
       </c>
       <c r="C143" s="27" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="145" spans="1:3" ht="15.75" customHeight="1">
       <c r="A145" s="47" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="B145" s="42" t="s">
-        <v>720</v>
+        <v>1138</v>
       </c>
       <c r="C145" s="42" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="15.75" customHeight="1">
       <c r="A146" s="47" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="B146" s="42" t="s">
-        <v>720</v>
+        <v>1138</v>
       </c>
       <c r="C146" s="42" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="15" customHeight="1">
       <c r="A147" s="47" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="B147" s="42" t="s">
-        <v>720</v>
+        <v>1138</v>
       </c>
       <c r="C147" s="42" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="149" spans="1:3" ht="15.75" customHeight="1">
       <c r="B149" s="39" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="15.75" customHeight="1">
       <c r="A150" s="27" t="s">
-        <v>724</v>
-      </c>
-      <c r="B150" s="27" t="s">
-        <v>725</v>
+        <v>721</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>1051</v>
       </c>
       <c r="C150" s="27" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="15" customHeight="1">
       <c r="A151" s="47" t="s">
-        <v>726</v>
-      </c>
-      <c r="B151" s="48" t="s">
-        <v>727</v>
+        <v>723</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>1119</v>
       </c>
       <c r="C151" s="48" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="15" customHeight="1">
       <c r="A152" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B152" s="27" t="s">
-        <v>47</v>
+      <c r="B152" t="s">
+        <v>1039</v>
       </c>
       <c r="C152" s="27" t="s">
         <v>47</v>
@@ -29208,33 +29282,33 @@
       <c r="A155" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B155" s="48" t="s">
-        <v>725</v>
+      <c r="B155" s="4" t="s">
+        <v>1051</v>
       </c>
       <c r="C155" s="48" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="15" customHeight="1">
       <c r="A156" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="B156" s="48" t="s">
-        <v>727</v>
+      <c r="B156" s="4" t="s">
+        <v>1119</v>
       </c>
       <c r="C156" s="48" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="15" customHeight="1">
       <c r="A157" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="B157" s="48" t="s">
-        <v>728</v>
+      <c r="B157" s="4" t="s">
+        <v>1050</v>
       </c>
       <c r="C157" s="48" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="15.75" customHeight="1"/>
@@ -29243,8 +29317,8 @@
       <c r="A160" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B160" s="48" t="s">
-        <v>56</v>
+      <c r="B160" s="4" t="s">
+        <v>1052</v>
       </c>
       <c r="C160" s="48" t="s">
         <v>56</v>
@@ -29254,8 +29328,8 @@
       <c r="A161" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B161" s="48" t="s">
-        <v>58</v>
+      <c r="B161" s="4" t="s">
+        <v>1068</v>
       </c>
       <c r="C161" s="48" t="s">
         <v>58</v>
@@ -29264,6 +29338,9 @@
     <row r="162" spans="1:3" ht="15" customHeight="1">
       <c r="A162" s="49" t="s">
         <v>59</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>1065</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="15.75" customHeight="1"/>
@@ -29272,8 +29349,8 @@
       <c r="A165" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B165" s="48" t="s">
-        <v>62</v>
+      <c r="B165" s="4" t="s">
+        <v>1056</v>
       </c>
       <c r="C165" s="48" t="s">
         <v>62</v>
@@ -29283,16 +29360,19 @@
       <c r="A166" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B166" s="48" t="s">
-        <v>729</v>
+      <c r="B166" s="4" t="s">
+        <v>1069</v>
       </c>
       <c r="C166" s="48" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="15" customHeight="1">
       <c r="A167" s="49" t="s">
         <v>65</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>1066</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="15.75" customHeight="1"/>
@@ -29301,8 +29381,8 @@
       <c r="A170" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="B170" s="48" t="s">
-        <v>68</v>
+      <c r="B170" s="4" t="s">
+        <v>1053</v>
       </c>
       <c r="C170" s="48" t="s">
         <v>68</v>
@@ -29312,16 +29392,19 @@
       <c r="A171" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="B171" s="48" t="s">
-        <v>730</v>
+      <c r="B171" s="4" t="s">
+        <v>1054</v>
       </c>
       <c r="C171" s="48" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="15.75" customHeight="1">
       <c r="A172" s="49" t="s">
         <v>71</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>1055</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="15.75" customHeight="1"/>
@@ -29330,8 +29413,8 @@
       <c r="A175" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="B175" s="48" t="s">
-        <v>68</v>
+      <c r="B175" s="4" t="s">
+        <v>1053</v>
       </c>
       <c r="C175" s="48" t="s">
         <v>68</v>
@@ -29341,11 +29424,11 @@
       <c r="A176" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="B176" s="48" t="s">
-        <v>730</v>
+      <c r="B176" s="4" t="s">
+        <v>1054</v>
       </c>
       <c r="C176" s="48" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="15.75" customHeight="1"/>
@@ -29354,8 +29437,8 @@
       <c r="A179" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="B179" s="48" t="s">
-        <v>68</v>
+      <c r="B179" s="4" t="s">
+        <v>1053</v>
       </c>
       <c r="C179" s="48" t="s">
         <v>68</v>
@@ -29365,11 +29448,11 @@
       <c r="A180" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B180" s="48" t="s">
-        <v>730</v>
+      <c r="B180" s="4" t="s">
+        <v>1054</v>
       </c>
       <c r="C180" s="48" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="15.75" customHeight="1"/>
@@ -29378,7 +29461,7 @@
       <c r="A183" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="B183" s="48" t="s">
+      <c r="B183" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C183" s="48" t="s">
@@ -29389,7 +29472,7 @@
       <c r="A184" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="B184" s="48" t="s">
+      <c r="B184" s="4" t="s">
         <v>80</v>
       </c>
       <c r="C184" s="48" t="s">
@@ -29400,8 +29483,8 @@
       <c r="A185" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="B185" s="48" t="s">
-        <v>82</v>
+      <c r="B185" s="4" t="s">
+        <v>1067</v>
       </c>
       <c r="C185" s="48" t="s">
         <v>82</v>
@@ -29411,17 +29494,17 @@
       <c r="A186" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="B186" s="48" t="s">
-        <v>731</v>
+      <c r="B186" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="C186" s="48" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="188" spans="1:3" ht="15.75" customHeight="1">
       <c r="B188" s="50" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="15.75" customHeight="1"/>
@@ -29443,8 +29526,8 @@
       <c r="A194" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="B194" s="52" t="s">
-        <v>47</v>
+      <c r="B194" t="s">
+        <v>1039</v>
       </c>
       <c r="C194" s="52" t="s">
         <v>47</v>
@@ -29466,18 +29549,18 @@
         <v>93</v>
       </c>
       <c r="B196" s="51" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="C196" s="51" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="15.75" customHeight="1">
       <c r="A197" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="B197" s="38" t="s">
-        <v>88</v>
+      <c r="B197" s="7" t="s">
+        <v>1040</v>
       </c>
       <c r="C197" s="38" t="s">
         <v>88</v>
@@ -29487,8 +29570,8 @@
       <c r="A198" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="B198" s="53" t="s">
-        <v>90</v>
+      <c r="B198" s="7" t="s">
+        <v>1041</v>
       </c>
       <c r="C198" s="53" t="s">
         <v>90</v>
@@ -29618,13 +29701,13 @@
     </row>
     <row r="211" spans="1:3" ht="15.75" customHeight="1">
       <c r="A211" s="51" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="B211" s="53" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="C211" s="53" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="15.75" customHeight="1">
@@ -29632,15 +29715,15 @@
         <v>299</v>
       </c>
       <c r="B212" s="38" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="C212" s="38" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="213" spans="1:3" ht="15.75" customHeight="1">
       <c r="A213" s="51" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="B213" s="38" t="s">
         <v>302</v>
@@ -29653,8 +29736,8 @@
       <c r="A214" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="B214" s="51" t="s">
-        <v>102</v>
+      <c r="B214" s="1" t="s">
+        <v>1042</v>
       </c>
       <c r="C214" s="51" t="s">
         <v>102</v>
@@ -29664,8 +29747,8 @@
       <c r="A215" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="B215" s="53" t="s">
-        <v>104</v>
+      <c r="B215" s="7" t="s">
+        <v>1043</v>
       </c>
       <c r="C215" s="53" t="s">
         <v>104</v>
@@ -29707,32 +29790,32 @@
     <row r="219" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="220" spans="1:3" ht="15.75" customHeight="1">
       <c r="A220" s="51" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="B220" s="53" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="C220" s="53" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="15.75" customHeight="1">
       <c r="A221" s="51" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="B221" s="38" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="C221" s="38" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="15.75" customHeight="1">
       <c r="A222" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="B222" s="51" t="s">
-        <v>106</v>
+      <c r="B222" s="1" t="s">
+        <v>1044</v>
       </c>
       <c r="C222" s="51" t="s">
         <v>106</v>
@@ -29742,8 +29825,8 @@
       <c r="A223" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="B223" s="53" t="s">
-        <v>108</v>
+      <c r="B223" s="7" t="s">
+        <v>1045</v>
       </c>
       <c r="C223" s="53" t="s">
         <v>108</v>
@@ -29762,13 +29845,13 @@
     </row>
     <row r="225" spans="1:3" ht="15.75" customHeight="1">
       <c r="A225" s="51" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="B225" s="51" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="C225" s="51" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="15.75" customHeight="1">
@@ -29795,13 +29878,13 @@
     </row>
     <row r="228" spans="1:3" ht="15.75" customHeight="1">
       <c r="A228" s="51" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="B228" s="51" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="C228" s="51" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="15.75" customHeight="1">
@@ -29817,13 +29900,13 @@
     </row>
     <row r="230" spans="1:3" ht="15.75" customHeight="1">
       <c r="A230" s="51" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="B230" s="53" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="C230" s="53" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="15.75" customHeight="1">
@@ -29873,13 +29956,13 @@
     </row>
     <row r="236" spans="1:3" ht="15.75" customHeight="1">
       <c r="A236" s="51" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="B236" s="53" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C236" s="53" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="237" spans="1:3" ht="15.75" customHeight="1">
@@ -29906,32 +29989,32 @@
     </row>
     <row r="239" spans="1:3" ht="15.75" customHeight="1">
       <c r="A239" s="51" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="B239" s="53" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="C239" s="53" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="15.75" customHeight="1">
       <c r="A240" s="51" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="B240" s="53" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="C240" s="53" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="241" spans="1:3" ht="15.75" customHeight="1">
       <c r="A241" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="B241" s="53" t="s">
-        <v>98</v>
+      <c r="B241" s="7" t="s">
+        <v>1120</v>
       </c>
       <c r="C241" s="53" t="s">
         <v>98</v>
@@ -29941,8 +30024,8 @@
       <c r="A242" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="B242" s="51" t="s">
-        <v>100</v>
+      <c r="B242" s="1" t="s">
+        <v>1111</v>
       </c>
       <c r="C242" s="51" t="s">
         <v>100</v>
@@ -29952,19 +30035,19 @@
       <c r="A243" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="B243" s="53" t="s">
-        <v>754</v>
+      <c r="B243" s="1" t="s">
+        <v>1083</v>
       </c>
       <c r="C243" s="53" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="244" spans="1:3" ht="15.75" customHeight="1">
       <c r="A244" s="51" t="s">
         <v>111</v>
       </c>
-      <c r="B244" s="54" t="s">
-        <v>113</v>
+      <c r="B244" s="8" t="s">
+        <v>1081</v>
       </c>
       <c r="C244" s="54" t="s">
         <v>113</v>
@@ -29974,8 +30057,8 @@
       <c r="A245" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="B245" s="51" t="s">
-        <v>152</v>
+      <c r="B245" s="1" t="s">
+        <v>1082</v>
       </c>
       <c r="C245" s="51" t="s">
         <v>152</v>
@@ -29985,8 +30068,8 @@
       <c r="A246" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="B246" s="51" t="s">
-        <v>92</v>
+      <c r="B246" s="1" t="s">
+        <v>1046</v>
       </c>
       <c r="C246" s="51" t="s">
         <v>92</v>
@@ -29996,8 +30079,8 @@
       <c r="A247" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="B247" s="53" t="s">
-        <v>96</v>
+      <c r="B247" s="7" t="s">
+        <v>1047</v>
       </c>
       <c r="C247" s="53" t="s">
         <v>96</v>
@@ -30027,13 +30110,13 @@
     </row>
     <row r="250" spans="1:3" ht="15.75" customHeight="1">
       <c r="A250" s="51" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B250" s="53" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="C250" s="53" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="251" spans="1:3" ht="15.75" customHeight="1">
@@ -30049,21 +30132,21 @@
     </row>
     <row r="252" spans="1:3" ht="15.75" customHeight="1">
       <c r="A252" s="51" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="B252" s="53" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="C252" s="53" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="15.75" customHeight="1">
       <c r="A253" s="51" t="s">
         <v>146</v>
       </c>
-      <c r="B253" s="51" t="s">
-        <v>147</v>
+      <c r="B253" s="1" t="s">
+        <v>1048</v>
       </c>
       <c r="C253" s="51" t="s">
         <v>147</v>
@@ -30073,8 +30156,8 @@
       <c r="A254" s="51" t="s">
         <v>148</v>
       </c>
-      <c r="B254" s="53" t="s">
-        <v>149</v>
+      <c r="B254" s="1" t="s">
+        <v>1049</v>
       </c>
       <c r="C254" s="53" t="s">
         <v>149</v>
@@ -30084,8 +30167,8 @@
       <c r="A255" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="B255" s="51" t="s">
-        <v>142</v>
+      <c r="B255" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="C255" s="51" t="s">
         <v>142</v>
@@ -30095,8 +30178,8 @@
       <c r="A256" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="B256" s="51" t="s">
-        <v>145</v>
+      <c r="B256" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="C256" s="51" t="s">
         <v>145</v>
@@ -30106,7 +30189,7 @@
     <row r="258" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="259" spans="1:3" ht="15.75" customHeight="1">
       <c r="B259" s="55" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
     </row>
     <row r="260" spans="1:3" ht="15.75" customHeight="1"/>
@@ -30116,8 +30199,8 @@
       <c r="A263" s="51" t="s">
         <v>187</v>
       </c>
-      <c r="B263" s="51" t="s">
-        <v>188</v>
+      <c r="B263" s="52" t="s">
+        <v>47</v>
       </c>
       <c r="C263" s="51" t="s">
         <v>188</v>
@@ -30136,13 +30219,13 @@
     </row>
     <row r="265" spans="1:3" ht="15.75" customHeight="1">
       <c r="A265" s="51" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="B265" s="51" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="C265" s="51" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="266" spans="1:3" ht="15.75" customHeight="1">
@@ -30150,59 +30233,59 @@
         <v>35</v>
       </c>
       <c r="B266" s="51" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="C266" s="51" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="267" spans="1:3" ht="15.75" customHeight="1">
       <c r="A267" s="51" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="B267" s="38" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="C267" s="38" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
     </row>
     <row r="268" spans="1:3" ht="15.75" customHeight="1">
       <c r="A268" s="51" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="B268" s="56" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="C268" s="56" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="15.75" customHeight="1">
       <c r="A269" s="51" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="B269" s="51" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C269" s="51" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="270" spans="1:3" ht="15.75" customHeight="1">
       <c r="A270" s="51" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="B270" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C270" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="271" spans="1:3" ht="15.75" customHeight="1">
       <c r="A271" s="51" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="B271" s="57">
         <v>120</v>
@@ -30213,73 +30296,73 @@
     </row>
     <row r="272" spans="1:3" ht="15.75" customHeight="1">
       <c r="A272" s="51" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="B272" s="38" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="C272" s="38" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="273" spans="1:3" ht="15.75" customHeight="1">
       <c r="A273" s="51" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="B273" s="38" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="C273" s="38" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
     </row>
     <row r="274" spans="1:3" ht="15.75" customHeight="1">
       <c r="A274" s="51" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="B274" s="38" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="C274" s="38" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="275" spans="1:3" ht="15.75" customHeight="1">
       <c r="A275" s="51" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="B275" s="38" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="C275" s="38" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="15.75" customHeight="1">
       <c r="A276" s="51" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="B276" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C276" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="277" spans="1:3" ht="15.75" customHeight="1">
       <c r="A277" s="38" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="B277" s="38" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C277" s="38" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
     </row>
     <row r="278" spans="1:3" ht="15.75" customHeight="1">
       <c r="A278" s="38" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="B278" s="57">
         <v>6</v>
@@ -30290,62 +30373,62 @@
     </row>
     <row r="279" spans="1:3" ht="15.75" customHeight="1">
       <c r="A279" s="38" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="B279" s="38" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="C279" s="38" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
     </row>
     <row r="280" spans="1:3" ht="15.75" customHeight="1">
       <c r="A280" s="38" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="B280" s="38" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="C280" s="38" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
     </row>
     <row r="281" spans="1:3" ht="15.75" customHeight="1">
       <c r="A281" s="38" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="B281" s="38" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C281" s="38" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
     </row>
     <row r="282" spans="1:3" ht="15.75" customHeight="1">
       <c r="A282" s="38" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="B282" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C282" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="15.75" customHeight="1">
       <c r="A283" s="38" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="B283" s="38" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C283" s="38" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
     </row>
     <row r="284" spans="1:3" ht="15.75" customHeight="1">
       <c r="A284" s="38" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="B284" s="58">
         <v>13</v>
@@ -30356,62 +30439,62 @@
     </row>
     <row r="285" spans="1:3" ht="15.75" customHeight="1">
       <c r="A285" s="38" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="B285" s="38" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C285" s="38" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
     </row>
     <row r="286" spans="1:3" ht="15.75" customHeight="1">
       <c r="A286" s="38" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="B286" s="38" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="C286" s="38" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="287" spans="1:3" ht="15.75" customHeight="1">
       <c r="A287" s="38" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="B287" s="38" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="C287" s="38" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
     </row>
     <row r="288" spans="1:3" ht="15.75" customHeight="1">
       <c r="A288" s="38" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="B288" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C288" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="289" spans="1:3" ht="15.75" customHeight="1">
       <c r="A289" s="38" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="B289" s="38" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="C289" s="38" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
     </row>
     <row r="290" spans="1:3" ht="15.75" customHeight="1">
       <c r="A290" s="38" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="B290" s="57">
         <v>12</v>
@@ -30422,51 +30505,51 @@
     </row>
     <row r="291" spans="1:3" ht="15.75" customHeight="1">
       <c r="A291" s="38" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="B291" s="38" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="C291" s="38" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
     </row>
     <row r="292" spans="1:3" ht="15.75" customHeight="1">
       <c r="A292" s="38" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="B292" s="38" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="C292" s="38" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
     </row>
     <row r="293" spans="1:3" ht="15.75" customHeight="1">
       <c r="A293" s="38" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="B293" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C293" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="294" spans="1:3" ht="15.75" customHeight="1">
       <c r="A294" s="38" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="B294" s="38" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="C294" s="38" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
     </row>
     <row r="295" spans="1:3" ht="15.75" customHeight="1">
       <c r="A295" s="38" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="B295" s="57">
         <v>2</v>
@@ -30477,40 +30560,40 @@
     </row>
     <row r="296" spans="1:3" ht="15.75" customHeight="1">
       <c r="A296" s="38" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="B296" s="38" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="C296" s="38" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="15.75" customHeight="1">
       <c r="A297" s="38" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="B297" s="38" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C297" s="38" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="15.75" customHeight="1">
       <c r="A298" s="38" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="B298" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C298" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="15.75" customHeight="1">
       <c r="A299" s="38" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="B299" s="57">
         <v>7</v>
@@ -30521,7 +30604,7 @@
     </row>
     <row r="300" spans="1:3" ht="15.75" customHeight="1">
       <c r="A300" s="38" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="B300" s="57">
         <v>8</v>
@@ -30532,51 +30615,51 @@
     </row>
     <row r="301" spans="1:3" ht="15.75" customHeight="1">
       <c r="A301" s="38" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="B301" s="38" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="C301" s="38" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="302" spans="1:3" ht="15.75" customHeight="1">
       <c r="A302" s="38" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="B302" s="38" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="C302" s="38" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="15.75" customHeight="1">
       <c r="A303" s="38" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="B303" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C303" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="304" spans="1:3" ht="15.75" customHeight="1">
       <c r="A304" s="38" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="B304" s="38" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="C304" s="56" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
     </row>
     <row r="305" spans="1:3" ht="15.75" customHeight="1">
       <c r="A305" s="38" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="B305" s="57">
         <v>6</v>
@@ -30587,40 +30670,40 @@
     </row>
     <row r="306" spans="1:3" ht="15.75" customHeight="1">
       <c r="A306" s="38" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="B306" s="38" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="C306" s="38" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
     </row>
     <row r="307" spans="1:3" ht="15.75" customHeight="1">
       <c r="A307" s="38" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="B307" s="38" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="C307" s="38" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="15.75" customHeight="1">
       <c r="A308" s="38" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="B308" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C308" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="309" spans="1:3" ht="15.75" customHeight="1">
       <c r="A309" s="38" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="B309" s="57">
         <v>9</v>
@@ -30631,7 +30714,7 @@
     </row>
     <row r="310" spans="1:3" ht="15.75" customHeight="1">
       <c r="A310" s="38" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="B310" s="57">
         <v>10</v>
@@ -30642,40 +30725,40 @@
     </row>
     <row r="311" spans="1:3" ht="15.75" customHeight="1">
       <c r="A311" s="38" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="B311" s="38" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="C311" s="38" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
     </row>
     <row r="312" spans="1:3" ht="15.75" customHeight="1">
       <c r="A312" s="38" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="B312" s="38" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="C312" s="38" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="15.75" customHeight="1">
       <c r="A313" s="38" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="B313" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C313" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="314" spans="1:3" ht="15.75" customHeight="1">
       <c r="A314" s="38" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="B314" s="57">
         <v>12</v>
@@ -30686,7 +30769,7 @@
     </row>
     <row r="315" spans="1:3" ht="15.75" customHeight="1">
       <c r="A315" s="38" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="B315" s="57">
         <v>13</v>
@@ -30697,51 +30780,51 @@
     </row>
     <row r="316" spans="1:3" ht="15.75" customHeight="1">
       <c r="A316" s="38" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="B316" s="38" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C316" s="38" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
     </row>
     <row r="317" spans="1:3" ht="15.75" customHeight="1">
       <c r="A317" s="38" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="B317" s="38" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="C317" s="38" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="15.75" customHeight="1">
       <c r="A318" s="38" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="B318" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C318" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="319" spans="1:3" ht="15.75" customHeight="1">
       <c r="A319" s="38" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="B319" s="38" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C319" s="38" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
     </row>
     <row r="320" spans="1:3" ht="15.75" customHeight="1">
       <c r="A320" s="38" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B320" s="57">
         <v>6</v>
@@ -30752,51 +30835,51 @@
     </row>
     <row r="321" spans="1:3" ht="15.75" customHeight="1">
       <c r="A321" s="38" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="B321" s="38" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="C321" s="38" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
     <row r="322" spans="1:3" ht="15.75" customHeight="1">
       <c r="A322" s="38" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="B322" s="38" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="C322" s="38" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="15.75" customHeight="1">
       <c r="A323" s="38" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="B323" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C323" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="15.75" customHeight="1">
       <c r="A324" s="38" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="B324" s="38" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="C324" s="38" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
     </row>
     <row r="325" spans="1:3" ht="15.75" customHeight="1">
       <c r="A325" s="38" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="B325" s="57">
         <v>7</v>
@@ -30807,51 +30890,51 @@
     </row>
     <row r="326" spans="1:3" ht="15.75" customHeight="1">
       <c r="A326" s="38" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="B326" s="38" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="C326" s="38" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
     </row>
     <row r="327" spans="1:3" ht="15.75" customHeight="1">
       <c r="A327" s="38" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="B327" s="38" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="C327" s="38" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
     </row>
     <row r="328" spans="1:3" ht="15.75" customHeight="1">
       <c r="A328" s="38" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="B328" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C328" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="329" spans="1:3" ht="15.75" customHeight="1">
       <c r="A329" s="38" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="B329" s="38" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="C329" s="38" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
     </row>
     <row r="330" spans="1:3" ht="15.75" customHeight="1">
       <c r="A330" s="38" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="B330" s="57">
         <v>3</v>
@@ -30862,51 +30945,51 @@
     </row>
     <row r="331" spans="1:3" ht="15.75" customHeight="1">
       <c r="A331" s="38" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="B331" s="38" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="C331" s="38" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
     </row>
     <row r="332" spans="1:3" ht="15.75" customHeight="1">
       <c r="A332" s="38" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="B332" s="38" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C332" s="38" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
     </row>
     <row r="333" spans="1:3" ht="15.75" customHeight="1">
       <c r="A333" s="38" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B333" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C333" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="334" spans="1:3" ht="15.75" customHeight="1">
       <c r="A334" s="38" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="B334" s="38" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="C334" s="38" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
     </row>
     <row r="335" spans="1:3" ht="15.75" customHeight="1">
       <c r="A335" s="38" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="B335" s="57">
         <v>3</v>
@@ -30917,51 +31000,51 @@
     </row>
     <row r="336" spans="1:3" ht="15.75" customHeight="1">
       <c r="A336" s="38" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="B336" s="38" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="C336" s="38" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
     </row>
     <row r="337" spans="1:3" ht="15.75" customHeight="1">
       <c r="A337" s="38" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="B337" s="38" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="C337" s="38" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
     </row>
     <row r="338" spans="1:3" ht="15.75" customHeight="1">
       <c r="A338" s="38" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="B338" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C338" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="15.75" customHeight="1">
       <c r="A339" s="38" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="B339" s="38" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="C339" s="38" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
     </row>
     <row r="340" spans="1:3" ht="15.75" customHeight="1">
       <c r="A340" s="38" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="B340" s="57">
         <v>3</v>
@@ -30972,51 +31055,51 @@
     </row>
     <row r="341" spans="1:3" ht="15.75" customHeight="1">
       <c r="A341" s="38" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="B341" s="38" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="C341" s="38" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
     </row>
     <row r="342" spans="1:3" ht="15.75" customHeight="1">
       <c r="A342" s="38" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="B342" s="38" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="C342" s="38" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
     </row>
     <row r="343" spans="1:3" ht="15.75" customHeight="1">
       <c r="A343" s="38" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="B343" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C343" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="344" spans="1:3" ht="15.75" customHeight="1">
       <c r="A344" s="38" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="B344" s="56" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="C344" s="56" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
     </row>
     <row r="345" spans="1:3" ht="15.75" customHeight="1">
       <c r="A345" s="38" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="B345" s="57">
         <v>3</v>
@@ -31027,62 +31110,62 @@
     </row>
     <row r="346" spans="1:3" ht="15.75" customHeight="1">
       <c r="A346" s="38" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="B346" s="38" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="C346" s="38" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
     </row>
     <row r="347" spans="1:3" ht="15.75" customHeight="1">
       <c r="A347" s="38" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="B347" s="38" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="C347" s="38" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
     </row>
     <row r="348" spans="1:3" ht="15.75" customHeight="1">
       <c r="A348" s="38" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="B348" s="38" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="C348" s="38" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
     </row>
     <row r="349" spans="1:3" ht="15.75" customHeight="1">
       <c r="A349" s="38" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="B349" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C349" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="350" spans="1:3" ht="15.75" customHeight="1">
       <c r="A350" s="38" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="B350" s="57" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="C350" s="57" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
     </row>
     <row r="351" spans="1:3" ht="15.75" customHeight="1">
       <c r="A351" s="38" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="B351" s="57">
         <v>6</v>
@@ -31093,40 +31176,40 @@
     </row>
     <row r="352" spans="1:3" ht="15.75" customHeight="1">
       <c r="A352" s="38" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="B352" s="38" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="C352" s="38" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
     </row>
     <row r="353" spans="1:3" ht="15.75" customHeight="1">
       <c r="A353" s="38" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="B353" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C353" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="354" spans="1:3" ht="15.75" customHeight="1">
       <c r="A354" s="38" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="B354" s="38" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="C354" s="38" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
     </row>
     <row r="355" spans="1:3" ht="15.75" customHeight="1">
       <c r="A355" s="38" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="B355" s="57">
         <v>50</v>
@@ -31137,7 +31220,7 @@
     </row>
     <row r="356" spans="1:3" ht="15.75" customHeight="1">
       <c r="A356" s="38" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="B356" s="57">
         <v>55</v>
@@ -31148,189 +31231,189 @@
     </row>
     <row r="357" spans="1:3" ht="15.75" customHeight="1">
       <c r="A357" s="38" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="B357" s="38" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="C357" s="38" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="15.75" customHeight="1">
       <c r="A358" s="38" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="B358" s="38" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="C358" s="38" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
     </row>
     <row r="359" spans="1:3" ht="15.75" customHeight="1">
       <c r="A359" s="38" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="B359" s="38" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="C359" s="38" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
     </row>
     <row r="360" spans="1:3" ht="15.75" customHeight="1">
       <c r="A360" s="38" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="B360" s="38" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="C360" s="38" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
     </row>
     <row r="361" spans="1:3" ht="15.75" customHeight="1">
       <c r="A361" s="38" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="B361" s="38" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="C361" s="38" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
     </row>
     <row r="362" spans="1:3" ht="15.75" customHeight="1">
       <c r="A362" s="38" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="B362" s="38" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="C362" s="38" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
     </row>
     <row r="363" spans="1:3" ht="15.75" customHeight="1">
       <c r="A363" s="38" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="B363" s="38" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="C363" s="38" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
     </row>
     <row r="364" spans="1:3" ht="15.75" customHeight="1">
       <c r="A364" s="38" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="B364" s="38" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="C364" s="38" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
     </row>
     <row r="365" spans="1:3" ht="15.75" customHeight="1">
       <c r="A365" s="38" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="B365" s="38" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="C365" s="38" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
     </row>
     <row r="366" spans="1:3" ht="15.75" customHeight="1">
       <c r="A366" s="38" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="B366" s="38" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="C366" s="38" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
     </row>
     <row r="367" spans="1:3" ht="15.75" customHeight="1">
       <c r="A367" s="38" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="B367" s="38" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="C367" s="38" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
     </row>
     <row r="368" spans="1:3" ht="15.75" customHeight="1">
       <c r="A368" s="38" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="B368" s="38" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="C368" s="38" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
     </row>
     <row r="369" spans="1:3" ht="15.75" customHeight="1">
       <c r="A369" s="38" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="B369" s="38" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="C369" s="38" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
     </row>
     <row r="370" spans="1:3" ht="15.75" customHeight="1">
       <c r="A370" s="38" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="B370" s="38" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="C370" s="38" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
     </row>
     <row r="371" spans="1:3" ht="15.75" customHeight="1">
       <c r="A371" s="38" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="B371" s="38" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="C371" s="38" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
     </row>
     <row r="372" spans="1:3" ht="15.75" customHeight="1">
       <c r="A372" s="38" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="B372" s="38" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="C372" s="38" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
     </row>
     <row r="373" spans="1:3" ht="15.75" customHeight="1">
       <c r="A373" s="38" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="B373" s="38" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="C373" s="38" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
     </row>
     <row r="374" spans="1:3" ht="15.75" customHeight="1"/>
@@ -31340,7 +31423,7 @@
     <row r="378" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="379" spans="1:3" ht="15.75" customHeight="1">
       <c r="B379" s="50" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
     </row>
     <row r="380" spans="1:3" ht="15.75" customHeight="1"/>
@@ -31348,596 +31431,596 @@
     <row r="382" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="383" spans="1:3" ht="15.75" customHeight="1">
       <c r="A383" s="38" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="B383" s="38" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="C383" s="38" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
     </row>
     <row r="384" spans="1:3" ht="15.75" customHeight="1">
       <c r="A384" s="38" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="B384" s="38" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="C384" s="38" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
     </row>
     <row r="385" spans="1:3" ht="15.75" customHeight="1">
       <c r="A385" s="38" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="B385" s="38" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="C385" s="38" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
     </row>
     <row r="386" spans="1:3" ht="15.75" customHeight="1">
       <c r="A386" s="38" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="B386" s="38" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="C386" s="38" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
     </row>
     <row r="387" spans="1:3" ht="15.75" customHeight="1">
       <c r="A387" s="38" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="B387" s="38" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="C387" s="38" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
     </row>
     <row r="388" spans="1:3" ht="15.75" customHeight="1">
       <c r="A388" s="38" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="B388" s="38" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="C388" s="38" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
     </row>
     <row r="389" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="390" spans="1:3" ht="15.75" customHeight="1">
       <c r="B390" s="50" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
     </row>
     <row r="391" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="392" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="393" spans="1:3" ht="15.75" customHeight="1">
       <c r="A393" s="38" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="B393" s="38" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="C393" s="38" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
     </row>
     <row r="394" spans="1:3" ht="15.75" customHeight="1">
       <c r="A394" s="38" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="B394" s="38" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="C394" s="38" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
     </row>
     <row r="395" spans="1:3" ht="15.75" customHeight="1">
       <c r="A395" s="38" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="B395" s="38" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="C395" s="38" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
     </row>
     <row r="396" spans="1:3" ht="15.75" customHeight="1">
       <c r="A396" s="38" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="B396" s="38" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="C396" s="38" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
     </row>
     <row r="397" spans="1:3" ht="15.75" customHeight="1">
       <c r="A397" s="38" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="B397" s="38" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="C397" s="38" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
     </row>
     <row r="398" spans="1:3" ht="15.75" customHeight="1">
       <c r="A398" s="38" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="B398" s="38" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="C398" s="38" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
     </row>
     <row r="399" spans="1:3" ht="15.75" customHeight="1">
       <c r="A399" s="38" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="B399" s="38" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="C399" s="38" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
     </row>
     <row r="400" spans="1:3" ht="15.75" customHeight="1">
       <c r="A400" s="38" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="B400" s="38" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="C400" s="38" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
     </row>
     <row r="401" spans="1:3" ht="15.75" customHeight="1">
       <c r="A401" s="38" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="B401" s="38" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="C401" s="38" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
     </row>
     <row r="402" spans="1:3" ht="15.75" customHeight="1">
       <c r="A402" s="38" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="B402" s="38" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="C402" s="38" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
     </row>
     <row r="403" spans="1:3" ht="15.75" customHeight="1">
       <c r="A403" s="38" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="B403" s="38" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="C403" s="38" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="15.75" customHeight="1">
       <c r="A404" s="38" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="B404" s="38" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="C404" s="38" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
     </row>
     <row r="405" spans="1:3" ht="15.75" customHeight="1">
       <c r="A405" s="38" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="B405" s="38" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="C405" s="38" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
     </row>
     <row r="406" spans="1:3" ht="15.75" customHeight="1">
       <c r="A406" s="38" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="B406" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C406" s="38" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="407" spans="1:3" ht="15.75" customHeight="1">
       <c r="A407" s="38" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="B407" s="38" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="C407" s="38" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
     </row>
     <row r="408" spans="1:3" ht="15.75" customHeight="1">
       <c r="A408" s="38" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="B408" s="38" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="C408" s="38" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
     </row>
     <row r="409" spans="1:3" ht="15.75" customHeight="1">
       <c r="A409" s="38" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="B409" s="38" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="C409" s="38" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
     </row>
     <row r="410" spans="1:3" ht="15.75" customHeight="1">
       <c r="A410" s="38" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="B410" s="38" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="C410" s="38" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="15.75" customHeight="1">
       <c r="A411" s="38" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B411" s="38" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="C411" s="38" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="15.75" customHeight="1">
       <c r="A412" s="38" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="B412" s="38" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C412" s="38" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="15.75" customHeight="1">
       <c r="A413" s="38" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="B413" s="38" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="C413" s="38" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
     </row>
     <row r="414" spans="1:3" ht="15.75" customHeight="1">
       <c r="A414" s="38" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="B414" s="38" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="C414" s="38" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
     </row>
     <row r="415" spans="1:3" ht="15.75" customHeight="1">
       <c r="A415" s="38" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="B415" s="38" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="C415" s="38" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
     </row>
     <row r="416" spans="1:3" ht="15.75" customHeight="1">
       <c r="A416" s="38" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="B416" s="38" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="C416" s="38" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="417" spans="1:3" ht="15.75" customHeight="1">
       <c r="A417" s="38" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="B417" s="38" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="C417" s="38" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
     </row>
     <row r="418" spans="1:3" ht="15.75" customHeight="1">
       <c r="A418" s="38" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="B418" s="38" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="C418" s="38" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
     </row>
     <row r="419" spans="1:3" ht="15.75" customHeight="1">
       <c r="A419" s="38" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="B419" s="38" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="C419" s="38" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
     </row>
     <row r="420" spans="1:3" ht="15.75" customHeight="1">
       <c r="A420" s="38" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="B420" s="38" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="C420" s="38" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
     </row>
     <row r="421" spans="1:3" ht="15.75" customHeight="1">
       <c r="A421" s="38" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="B421" s="38" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="C421" s="38" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="422" spans="1:3" ht="15.75" customHeight="1">
       <c r="A422" s="38" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="B422" s="38" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="C422" s="38" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="423" spans="1:3" ht="15.75" customHeight="1">
       <c r="A423" s="38" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="B423" s="38" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="C423" s="38" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="424" spans="1:3" ht="15.75" customHeight="1">
       <c r="A424" s="38" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="B424" s="38" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="C424" s="38" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="425" spans="1:3" ht="15.75" customHeight="1">
       <c r="A425" s="38" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="B425" s="38" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="C425" s="38" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="426" spans="1:3" ht="15.75" customHeight="1">
       <c r="A426" s="12" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="B426" s="12" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="C426" s="12" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="427" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="428" spans="1:3" ht="15.75" customHeight="1">
       <c r="A428" s="38" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="B428" s="38" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="C428" s="38" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="429" spans="1:3" ht="15.75" customHeight="1">
       <c r="A429" s="38" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="B429" s="38" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="C429" s="38" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="430" spans="1:3" ht="15.75" customHeight="1">
       <c r="A430" s="38" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B430" s="38" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="C430" s="38" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="431" spans="1:3" ht="15.75" customHeight="1">
       <c r="A431" s="38" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="B431" s="38" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="C431" s="38" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="432" spans="1:3" ht="15.75" customHeight="1">
       <c r="A432" s="38" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="B432" s="12" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="C432" s="12" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="433" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="434" spans="1:3" ht="15.75" customHeight="1">
       <c r="A434" s="38" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="B434" s="38" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="C434" s="38" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="435" spans="1:3" ht="15.75" customHeight="1">
       <c r="A435" s="38" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="B435" s="38" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="C435" s="38" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="436" spans="1:3" ht="15.75" customHeight="1">
       <c r="A436" s="38" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="B436" s="38" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="C436" s="38" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="437" spans="1:3" ht="15.75" customHeight="1">
       <c r="A437" s="38" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="B437" s="38" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="C437" s="38" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="438" spans="1:3" ht="15.75" customHeight="1">
       <c r="A438" s="38" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="B438" s="38" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C438" s="38" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="439" spans="1:3" ht="15.75" customHeight="1">
       <c r="A439" s="12" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="B439" s="12" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="C439" s="12" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="440" spans="1:3" ht="15.75" customHeight="1">
       <c r="B440" s="50" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="441" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="442" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="443" spans="1:3" ht="15.75" customHeight="1">
       <c r="A443" s="38" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="B443" s="38" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="C443" s="38" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="444" spans="1:3" ht="15.75" customHeight="1">
       <c r="A444" s="38" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="B444" s="38" t="s">
         <v>8</v>
@@ -32511,10 +32594,12 @@
     <hyperlink ref="C75" r:id="rId5"/>
     <hyperlink ref="B193" r:id="rId6"/>
     <hyperlink ref="C193" r:id="rId7"/>
-    <hyperlink ref="B194" r:id="rId8"/>
-    <hyperlink ref="C194" r:id="rId9"/>
+    <hyperlink ref="C194" r:id="rId8"/>
+    <hyperlink ref="B77" r:id="rId9"/>
+    <hyperlink ref="C77" r:id="rId10"/>
+    <hyperlink ref="B263" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>